<commit_message>
Fixed warscore to use only wars where the player could have entered
</commit_message>
<xml_diff>
--- a/docs/data/memberstats.xlsx
+++ b/docs/data/memberstats.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="133">
   <si>
     <t>tag</t>
   </si>
@@ -74,12 +74,12 @@
     <t>arena</t>
   </si>
   <si>
+    <t>age</t>
+  </si>
+  <si>
     <t>joined</t>
   </si>
   <si>
-    <t>age</t>
-  </si>
-  <si>
     <t>#200CGV9QP</t>
   </si>
   <si>
@@ -113,6 +113,9 @@
     <t>#2GP9VYY98</t>
   </si>
   <si>
+    <t>#2J2PPYGLC</t>
+  </si>
+  <si>
     <t>#2JU82PCJ</t>
   </si>
   <si>
@@ -260,6 +263,9 @@
     <t>Tabo da amarela</t>
   </si>
   <si>
+    <t>pedro</t>
+  </si>
+  <si>
     <t>☆ Di♡g♡</t>
   </si>
   <si>
@@ -392,10 +398,10 @@
     <t>League 1</t>
   </si>
   <si>
+    <t>Arena 11</t>
+  </si>
+  <si>
     <t>Arena 12</t>
-  </si>
-  <si>
-    <t>Arena 11</t>
   </si>
   <si>
     <t>League 2</t>
@@ -532,7 +538,7 @@
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C2" t="n">
         <v>11.0</v>
@@ -544,16 +550,16 @@
         <v>4622.0</v>
       </c>
       <c r="F2" t="n">
-        <v>2224.0</v>
+        <v>2225.0</v>
       </c>
       <c r="G2" t="n">
-        <v>2068.0</v>
+        <v>2069.0</v>
       </c>
       <c r="H2" t="n">
-        <v>6916.0</v>
+        <v>6928.0</v>
       </c>
       <c r="I2" t="n">
-        <v>1138.0</v>
+        <v>1140.0</v>
       </c>
       <c r="J2" t="n">
         <v>2661.0</v>
@@ -568,31 +574,31 @@
         <v>7.0</v>
       </c>
       <c r="N2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="O2" t="n">
-        <v>156.0</v>
+        <v>268.0</v>
       </c>
       <c r="P2" t="n">
-        <v>90.0</v>
+        <v>170.0</v>
       </c>
       <c r="Q2" t="n">
-        <v>26914.0</v>
+        <v>27026.0</v>
       </c>
       <c r="R2" t="n">
-        <v>39.0</v>
+        <v>40.0</v>
       </c>
       <c r="S2" t="n">
-        <v>74460.0</v>
+        <v>75580.0</v>
       </c>
       <c r="T2" t="s">
-        <v>124</v>
-      </c>
-      <c r="U2" t="n" s="2">
+        <v>126</v>
+      </c>
+      <c r="U2" t="n">
+        <v>102.0</v>
+      </c>
+      <c r="V2" t="n" s="2">
         <v>43302.0</v>
-      </c>
-      <c r="V2" t="n">
-        <v>101.0</v>
       </c>
     </row>
     <row r="3">
@@ -600,7 +606,7 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C3" t="n">
         <v>10.0</v>
@@ -612,16 +618,16 @@
         <v>4077.0</v>
       </c>
       <c r="F3" t="n">
-        <v>1644.0</v>
+        <v>1648.0</v>
       </c>
       <c r="G3" t="n">
-        <v>1429.0</v>
+        <v>1431.0</v>
       </c>
       <c r="H3" t="n">
-        <v>4268.0</v>
+        <v>4278.0</v>
       </c>
       <c r="I3" t="n">
-        <v>821.0</v>
+        <v>823.0</v>
       </c>
       <c r="J3" t="n">
         <v>2388.0</v>
@@ -636,31 +642,31 @@
         <v>2.0</v>
       </c>
       <c r="N3" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="O3" t="n">
-        <v>118.0</v>
+        <v>196.0</v>
       </c>
       <c r="P3" t="n">
-        <v>40.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q3" t="n">
-        <v>17619.0</v>
+        <v>17697.0</v>
       </c>
       <c r="R3" t="n">
         <v>13.0</v>
       </c>
       <c r="S3" t="n">
-        <v>24160.0</v>
+        <v>25280.0</v>
       </c>
       <c r="T3" t="s">
-        <v>125</v>
-      </c>
-      <c r="U3" t="n" s="2">
+        <v>127</v>
+      </c>
+      <c r="U3" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="V3" t="n" s="2">
         <v>43372.0</v>
-      </c>
-      <c r="V3" t="n">
-        <v>31.0</v>
       </c>
     </row>
     <row r="4">
@@ -668,31 +674,31 @@
         <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C4" t="n">
         <v>11.0</v>
       </c>
       <c r="D4" t="n">
-        <v>3917.0</v>
+        <v>4138.0</v>
       </c>
       <c r="E4" t="n">
-        <v>4196.0</v>
+        <v>4219.0</v>
       </c>
       <c r="F4" t="n">
-        <v>2501.0</v>
+        <v>2527.0</v>
       </c>
       <c r="G4" t="n">
-        <v>2545.0</v>
+        <v>2566.0</v>
       </c>
       <c r="H4" t="n">
-        <v>6021.0</v>
+        <v>6071.0</v>
       </c>
       <c r="I4" t="n">
-        <v>1054.0</v>
+        <v>1056.0</v>
       </c>
       <c r="J4" t="n">
-        <v>1641.0</v>
+        <v>1649.0</v>
       </c>
       <c r="K4" t="n">
         <v>12.0</v>
@@ -704,31 +710,31 @@
         <v>9.0</v>
       </c>
       <c r="N4" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="O4" t="n">
-        <v>10.0</v>
+        <v>46.0</v>
       </c>
       <c r="P4" t="n">
-        <v>120.0</v>
+        <v>200.0</v>
       </c>
       <c r="Q4" t="n">
-        <v>8816.0</v>
+        <v>8852.0</v>
       </c>
       <c r="R4" t="n">
-        <v>38.0</v>
+        <v>39.0</v>
       </c>
       <c r="S4" t="n">
-        <v>53597.0</v>
+        <v>54997.0</v>
       </c>
       <c r="T4" t="s">
-        <v>126</v>
-      </c>
-      <c r="U4" t="n" s="2">
+        <v>127</v>
+      </c>
+      <c r="U4" t="n">
+        <v>322.0</v>
+      </c>
+      <c r="V4" t="n" s="2">
         <v>43082.0</v>
-      </c>
-      <c r="V4" t="n">
-        <v>321.0</v>
       </c>
     </row>
     <row r="5">
@@ -736,31 +742,31 @@
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C5" t="n">
         <v>10.0</v>
       </c>
       <c r="D5" t="n">
-        <v>3639.0</v>
+        <v>3698.0</v>
       </c>
       <c r="E5" t="n">
         <v>3764.0</v>
       </c>
       <c r="F5" t="n">
-        <v>684.0</v>
+        <v>690.0</v>
       </c>
       <c r="G5" t="n">
-        <v>632.0</v>
+        <v>636.0</v>
       </c>
       <c r="H5" t="n">
-        <v>1914.0</v>
+        <v>1929.0</v>
       </c>
       <c r="I5" t="n">
-        <v>379.0</v>
+        <v>381.0</v>
       </c>
       <c r="J5" t="n">
-        <v>1416.0</v>
+        <v>1428.0</v>
       </c>
       <c r="K5" t="n">
         <v>10.0</v>
@@ -772,31 +778,31 @@
         <v>4.0</v>
       </c>
       <c r="N5" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="O5" t="n">
-        <v>165.0</v>
+        <v>390.0</v>
       </c>
       <c r="P5" t="n">
-        <v>80.0</v>
+        <v>160.0</v>
       </c>
       <c r="Q5" t="n">
-        <v>15629.0</v>
+        <v>15875.0</v>
       </c>
       <c r="R5" t="n">
         <v>3.0</v>
       </c>
       <c r="S5" t="n">
-        <v>4760.0</v>
+        <v>5985.0</v>
       </c>
       <c r="T5" t="s">
-        <v>127</v>
-      </c>
-      <c r="U5" t="n" s="2">
+        <v>128</v>
+      </c>
+      <c r="U5" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="V5" t="n" s="2">
         <v>43397.0</v>
-      </c>
-      <c r="V5" t="n">
-        <v>6.0</v>
       </c>
     </row>
     <row r="6">
@@ -804,7 +810,7 @@
         <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C6" t="n">
         <v>10.0</v>
@@ -816,19 +822,19 @@
         <v>4142.0</v>
       </c>
       <c r="F6" t="n">
-        <v>1208.0</v>
+        <v>1209.0</v>
       </c>
       <c r="G6" t="n">
-        <v>1235.0</v>
+        <v>1238.0</v>
       </c>
       <c r="H6" t="n">
-        <v>3086.0</v>
+        <v>3103.0</v>
       </c>
       <c r="I6" t="n">
-        <v>494.0</v>
+        <v>495.0</v>
       </c>
       <c r="J6" t="n">
-        <v>307.0</v>
+        <v>310.0</v>
       </c>
       <c r="K6" t="n">
         <v>10.0</v>
@@ -840,31 +846,31 @@
         <v>0.0</v>
       </c>
       <c r="N6" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="O6" t="n">
-        <v>164.0</v>
+        <v>237.0</v>
       </c>
       <c r="P6" t="n">
-        <v>40.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q6" t="n">
-        <v>14711.0</v>
+        <v>14784.0</v>
       </c>
       <c r="R6" t="n">
-        <v>27.0</v>
+        <v>28.0</v>
       </c>
       <c r="S6" t="n">
         <v>36066.0</v>
       </c>
       <c r="T6" t="s">
-        <v>126</v>
-      </c>
-      <c r="U6" t="n" s="2">
+        <v>129</v>
+      </c>
+      <c r="U6" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="V6" t="n" s="2">
         <v>43356.0</v>
-      </c>
-      <c r="V6" t="n">
-        <v>47.0</v>
       </c>
     </row>
     <row r="7">
@@ -872,31 +878,31 @@
         <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C7" t="n">
         <v>11.0</v>
       </c>
       <c r="D7" t="n">
-        <v>4234.0</v>
+        <v>4263.0</v>
       </c>
       <c r="E7" t="n">
         <v>4418.0</v>
       </c>
       <c r="F7" t="n">
-        <v>2931.0</v>
+        <v>2938.0</v>
       </c>
       <c r="G7" t="n">
-        <v>2644.0</v>
+        <v>2646.0</v>
       </c>
       <c r="H7" t="n">
-        <v>6959.0</v>
+        <v>6971.0</v>
       </c>
       <c r="I7" t="n">
         <v>681.0</v>
       </c>
       <c r="J7" t="n">
-        <v>4126.0</v>
+        <v>4151.0</v>
       </c>
       <c r="K7" t="n">
         <v>10.0</v>
@@ -908,13 +914,13 @@
         <v>166.0</v>
       </c>
       <c r="N7" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="O7" t="n">
         <v>50.0</v>
       </c>
       <c r="P7" t="n">
-        <v>80.0</v>
+        <v>160.0</v>
       </c>
       <c r="Q7" t="n">
         <v>2125.0</v>
@@ -923,16 +929,16 @@
         <v>37.0</v>
       </c>
       <c r="S7" t="n">
-        <v>50080.0</v>
+        <v>51480.0</v>
       </c>
       <c r="T7" t="s">
-        <v>125</v>
-      </c>
-      <c r="U7" t="n" s="2">
+        <v>127</v>
+      </c>
+      <c r="U7" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="V7" t="n" s="2">
         <v>43364.0</v>
-      </c>
-      <c r="V7" t="n">
-        <v>39.0</v>
       </c>
     </row>
     <row r="8">
@@ -940,7 +946,7 @@
         <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C8" t="n">
         <v>11.0</v>
@@ -952,19 +958,19 @@
         <v>4455.0</v>
       </c>
       <c r="F8" t="n">
-        <v>1883.0</v>
+        <v>1888.0</v>
       </c>
       <c r="G8" t="n">
-        <v>1788.0</v>
+        <v>1790.0</v>
       </c>
       <c r="H8" t="n">
-        <v>7434.0</v>
+        <v>7463.0</v>
       </c>
       <c r="I8" t="n">
-        <v>1107.0</v>
+        <v>1108.0</v>
       </c>
       <c r="J8" t="n">
-        <v>1367.0</v>
+        <v>1384.0</v>
       </c>
       <c r="K8" t="n">
         <v>10.0</v>
@@ -976,31 +982,31 @@
         <v>0.0</v>
       </c>
       <c r="N8" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="O8" t="n">
-        <v>28.0</v>
+        <v>84.0</v>
       </c>
       <c r="P8" t="n">
-        <v>130.0</v>
+        <v>210.0</v>
       </c>
       <c r="Q8" t="n">
-        <v>24729.0</v>
+        <v>24785.0</v>
       </c>
       <c r="R8" t="n">
         <v>55.0</v>
       </c>
       <c r="S8" t="n">
-        <v>63955.0</v>
+        <v>64795.0</v>
       </c>
       <c r="T8" t="s">
-        <v>128</v>
-      </c>
-      <c r="U8" t="n" s="2">
+        <v>130</v>
+      </c>
+      <c r="U8" t="n">
+        <v>346.0</v>
+      </c>
+      <c r="V8" t="n" s="2">
         <v>43058.0</v>
-      </c>
-      <c r="V8" t="n">
-        <v>345.0</v>
       </c>
     </row>
     <row r="9">
@@ -1008,31 +1014,31 @@
         <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C9" t="n">
         <v>11.0</v>
       </c>
       <c r="D9" t="n">
-        <v>4290.0</v>
+        <v>4320.0</v>
       </c>
       <c r="E9" t="n">
         <v>4365.0</v>
       </c>
       <c r="F9" t="n">
-        <v>2305.0</v>
+        <v>2311.0</v>
       </c>
       <c r="G9" t="n">
-        <v>2238.0</v>
+        <v>2242.0</v>
       </c>
       <c r="H9" t="n">
-        <v>5068.0</v>
+        <v>5081.0</v>
       </c>
       <c r="I9" t="n">
-        <v>888.0</v>
+        <v>890.0</v>
       </c>
       <c r="J9" t="n">
-        <v>1610.0</v>
+        <v>1622.0</v>
       </c>
       <c r="K9" t="n">
         <v>10.0</v>
@@ -1044,31 +1050,31 @@
         <v>3.0</v>
       </c>
       <c r="N9" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="O9" t="n">
-        <v>76.0</v>
+        <v>121.0</v>
       </c>
       <c r="P9" t="n">
-        <v>120.0</v>
+        <v>200.0</v>
       </c>
       <c r="Q9" t="n">
-        <v>24451.0</v>
+        <v>24496.0</v>
       </c>
       <c r="R9" t="n">
         <v>12.0</v>
       </c>
       <c r="S9" t="n">
-        <v>45952.0</v>
+        <v>47352.0</v>
       </c>
       <c r="T9" t="s">
-        <v>125</v>
-      </c>
-      <c r="U9" t="n" s="2">
+        <v>130</v>
+      </c>
+      <c r="U9" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="V9" t="n" s="2">
         <v>43390.0</v>
-      </c>
-      <c r="V9" t="n">
-        <v>13.0</v>
       </c>
     </row>
     <row r="10">
@@ -1076,7 +1082,7 @@
         <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C10" t="n">
         <v>11.0</v>
@@ -1088,13 +1094,13 @@
         <v>3656.0</v>
       </c>
       <c r="F10" t="n">
-        <v>1095.0</v>
+        <v>1096.0</v>
       </c>
       <c r="G10" t="n">
         <v>1149.0</v>
       </c>
       <c r="H10" t="n">
-        <v>4616.0</v>
+        <v>4617.0</v>
       </c>
       <c r="I10" t="n">
         <v>1229.0</v>
@@ -1112,16 +1118,16 @@
         <v>18.0</v>
       </c>
       <c r="N10" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="O10" t="n">
-        <v>18.0</v>
+        <v>36.0</v>
       </c>
       <c r="P10" t="n">
-        <v>40.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q10" t="n">
-        <v>28763.0</v>
+        <v>28781.0</v>
       </c>
       <c r="R10" t="n">
         <v>7.0</v>
@@ -1130,13 +1136,13 @@
         <v>11970.0</v>
       </c>
       <c r="T10" t="s">
-        <v>127</v>
-      </c>
-      <c r="U10" t="n" s="2">
+        <v>128</v>
+      </c>
+      <c r="U10" t="n">
+        <v>281.0</v>
+      </c>
+      <c r="V10" t="n" s="2">
         <v>43123.0</v>
-      </c>
-      <c r="V10" t="n">
-        <v>280.0</v>
       </c>
     </row>
     <row r="11">
@@ -1144,31 +1150,31 @@
         <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C11" t="n">
         <v>11.0</v>
       </c>
       <c r="D11" t="n">
-        <v>4490.0</v>
+        <v>4461.0</v>
       </c>
       <c r="E11" t="n">
         <v>4490.0</v>
       </c>
       <c r="F11" t="n">
-        <v>2305.0</v>
+        <v>2309.0</v>
       </c>
       <c r="G11" t="n">
-        <v>2138.0</v>
+        <v>2144.0</v>
       </c>
       <c r="H11" t="n">
-        <v>10380.0</v>
+        <v>10407.0</v>
       </c>
       <c r="I11" t="n">
-        <v>2323.0</v>
+        <v>2328.0</v>
       </c>
       <c r="J11" t="n">
-        <v>1896.0</v>
+        <v>1906.0</v>
       </c>
       <c r="K11" t="n">
         <v>11.0</v>
@@ -1180,31 +1186,31 @@
         <v>0.0</v>
       </c>
       <c r="N11" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="O11" t="n">
-        <v>10.0</v>
+        <v>40.0</v>
       </c>
       <c r="P11" t="n">
-        <v>160.0</v>
+        <v>240.0</v>
       </c>
       <c r="Q11" t="n">
-        <v>3052.0</v>
+        <v>3082.0</v>
       </c>
       <c r="R11" t="n">
-        <v>52.0</v>
+        <v>53.0</v>
       </c>
       <c r="S11" t="n">
-        <v>72070.0</v>
+        <v>73190.0</v>
       </c>
       <c r="T11" t="s">
-        <v>128</v>
-      </c>
-      <c r="U11" t="n" s="2">
+        <v>130</v>
+      </c>
+      <c r="U11" t="n">
+        <v>281.0</v>
+      </c>
+      <c r="V11" t="n" s="2">
         <v>43123.0</v>
-      </c>
-      <c r="V11" t="n">
-        <v>280.0</v>
       </c>
     </row>
     <row r="12">
@@ -1212,7 +1218,7 @@
         <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C12" t="n">
         <v>12.0</v>
@@ -1224,19 +1230,19 @@
         <v>4617.0</v>
       </c>
       <c r="F12" t="n">
-        <v>2222.0</v>
+        <v>2229.0</v>
       </c>
       <c r="G12" t="n">
-        <v>1743.0</v>
+        <v>1747.0</v>
       </c>
       <c r="H12" t="n">
-        <v>9291.0</v>
+        <v>9311.0</v>
       </c>
       <c r="I12" t="n">
-        <v>1355.0</v>
+        <v>1357.0</v>
       </c>
       <c r="J12" t="n">
-        <v>4171.0</v>
+        <v>4199.0</v>
       </c>
       <c r="K12" t="n">
         <v>10.0</v>
@@ -1248,31 +1254,31 @@
         <v>7.0</v>
       </c>
       <c r="N12" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="O12" t="n">
-        <v>281.0</v>
+        <v>525.0</v>
       </c>
       <c r="P12" t="n">
-        <v>160.0</v>
+        <v>280.0</v>
       </c>
       <c r="Q12" t="n">
-        <v>87218.0</v>
+        <v>87462.0</v>
       </c>
       <c r="R12" t="n">
-        <v>70.0</v>
+        <v>71.0</v>
       </c>
       <c r="S12" t="n">
         <v>66720.0</v>
       </c>
       <c r="T12" t="s">
-        <v>124</v>
-      </c>
-      <c r="U12" t="n" s="2">
+        <v>126</v>
+      </c>
+      <c r="U12" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="V12" t="n" s="2">
         <v>43397.0</v>
-      </c>
-      <c r="V12" t="n">
-        <v>6.0</v>
       </c>
     </row>
     <row r="13">
@@ -1280,67 +1286,67 @@
         <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C13" t="n">
         <v>11.0</v>
       </c>
       <c r="D13" t="n">
-        <v>4330.0</v>
+        <v>4069.0</v>
       </c>
       <c r="E13" t="n">
-        <v>4371.0</v>
+        <v>4163.0</v>
       </c>
       <c r="F13" t="n">
-        <v>1331.0</v>
+        <v>3141.0</v>
       </c>
       <c r="G13" t="n">
-        <v>1184.0</v>
+        <v>3311.0</v>
       </c>
       <c r="H13" t="n">
-        <v>5388.0</v>
+        <v>8534.0</v>
       </c>
       <c r="I13" t="n">
-        <v>745.0</v>
+        <v>1336.0</v>
       </c>
       <c r="J13" t="n">
-        <v>1187.0</v>
+        <v>1906.0</v>
       </c>
       <c r="K13" t="n">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="L13" t="n">
         <v>0.0</v>
       </c>
       <c r="M13" t="n">
-        <v>11.0</v>
+        <v>0.0</v>
       </c>
       <c r="N13" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="O13" t="n">
-        <v>110.0</v>
+        <v>0.0</v>
       </c>
       <c r="P13" t="n">
-        <v>153.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q13" t="n">
-        <v>36577.0</v>
+        <v>14123.0</v>
       </c>
       <c r="R13" t="n">
-        <v>56.0</v>
+        <v>17.0</v>
       </c>
       <c r="S13" t="n">
-        <v>67440.0</v>
+        <v>25640.0</v>
       </c>
       <c r="T13" t="s">
-        <v>128</v>
-      </c>
-      <c r="U13" t="n" s="2">
+        <v>127</v>
+      </c>
+      <c r="U13" t="n">
+        <v>186.0</v>
+      </c>
+      <c r="V13" t="n" s="2">
         <v>43218.0</v>
-      </c>
-      <c r="V13" t="n">
-        <v>185.0</v>
       </c>
     </row>
     <row r="14">
@@ -1348,67 +1354,67 @@
         <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C14" t="n">
-        <v>12.0</v>
+        <v>11.0</v>
       </c>
       <c r="D14" t="n">
-        <v>4273.0</v>
+        <v>4362.0</v>
       </c>
       <c r="E14" t="n">
-        <v>4521.0</v>
+        <v>4389.0</v>
       </c>
       <c r="F14" t="n">
-        <v>4537.0</v>
+        <v>1334.0</v>
       </c>
       <c r="G14" t="n">
-        <v>4946.0</v>
+        <v>1186.0</v>
       </c>
       <c r="H14" t="n">
-        <v>10505.0</v>
+        <v>5404.0</v>
       </c>
       <c r="I14" t="n">
-        <v>2031.0</v>
+        <v>748.0</v>
       </c>
       <c r="J14" t="n">
-        <v>1821.0</v>
+        <v>1187.0</v>
       </c>
       <c r="K14" t="n">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="L14" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="M14" t="n">
-        <v>15.0</v>
+        <v>11.0</v>
       </c>
       <c r="N14" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="O14" t="n">
-        <v>352.0</v>
+        <v>218.0</v>
       </c>
       <c r="P14" t="n">
-        <v>130.0</v>
+        <v>240.0</v>
       </c>
       <c r="Q14" t="n">
-        <v>50999.0</v>
+        <v>36685.0</v>
       </c>
       <c r="R14" t="n">
-        <v>28.0</v>
+        <v>57.0</v>
       </c>
       <c r="S14" t="n">
-        <v>73570.0</v>
+        <v>68560.0</v>
       </c>
       <c r="T14" t="s">
-        <v>125</v>
-      </c>
-      <c r="U14" t="n" s="2">
-        <v>43390.0</v>
-      </c>
-      <c r="V14" t="n">
-        <v>13.0</v>
+        <v>130</v>
+      </c>
+      <c r="U14" t="n">
+        <v>186.0</v>
+      </c>
+      <c r="V14" t="n" s="2">
+        <v>43218.0</v>
       </c>
     </row>
     <row r="15">
@@ -1416,67 +1422,67 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C15" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="D15" t="n">
-        <v>4295.0</v>
+        <v>4310.0</v>
       </c>
       <c r="E15" t="n">
-        <v>4416.0</v>
+        <v>4521.0</v>
       </c>
       <c r="F15" t="n">
-        <v>2251.0</v>
+        <v>4549.0</v>
       </c>
       <c r="G15" t="n">
-        <v>2050.0</v>
+        <v>4962.0</v>
       </c>
       <c r="H15" t="n">
-        <v>6640.0</v>
+        <v>10536.0</v>
       </c>
       <c r="I15" t="n">
-        <v>1062.0</v>
+        <v>2036.0</v>
       </c>
       <c r="J15" t="n">
-        <v>3622.0</v>
+        <v>1842.0</v>
       </c>
       <c r="K15" t="n">
-        <v>12.0</v>
+        <v>10.0</v>
       </c>
       <c r="L15" t="n">
-        <v>1200.0</v>
+        <v>4.0</v>
       </c>
       <c r="M15" t="n">
-        <v>11.0</v>
+        <v>15.0</v>
       </c>
       <c r="N15" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="O15" t="n">
-        <v>22.0</v>
+        <v>612.0</v>
       </c>
       <c r="P15" t="n">
-        <v>80.0</v>
+        <v>240.0</v>
       </c>
       <c r="Q15" t="n">
-        <v>20315.0</v>
+        <v>51259.0</v>
       </c>
       <c r="R15" t="n">
-        <v>42.0</v>
+        <v>28.0</v>
       </c>
       <c r="S15" t="n">
-        <v>45101.0</v>
+        <v>74970.0</v>
       </c>
       <c r="T15" t="s">
-        <v>125</v>
-      </c>
-      <c r="U15" t="n" s="2">
-        <v>43275.0</v>
-      </c>
-      <c r="V15" t="n">
-        <v>128.0</v>
+        <v>130</v>
+      </c>
+      <c r="U15" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="V15" t="n" s="2">
+        <v>43390.0</v>
       </c>
     </row>
     <row r="16">
@@ -1484,67 +1490,67 @@
         <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C16" t="n">
         <v>11.0</v>
       </c>
       <c r="D16" t="n">
-        <v>4028.0</v>
+        <v>4355.0</v>
       </c>
       <c r="E16" t="n">
-        <v>4076.0</v>
+        <v>4416.0</v>
       </c>
       <c r="F16" t="n">
-        <v>1528.0</v>
+        <v>2253.0</v>
       </c>
       <c r="G16" t="n">
-        <v>1451.0</v>
+        <v>2050.0</v>
       </c>
       <c r="H16" t="n">
-        <v>3598.0</v>
+        <v>6643.0</v>
       </c>
       <c r="I16" t="n">
-        <v>995.0</v>
+        <v>1063.0</v>
       </c>
       <c r="J16" t="n">
-        <v>2611.0</v>
+        <v>3622.0</v>
       </c>
       <c r="K16" t="n">
-        <v>10.0</v>
+        <v>12.0</v>
       </c>
       <c r="L16" t="n">
-        <v>33.0</v>
+        <v>1200.0</v>
       </c>
       <c r="M16" t="n">
-        <v>34.0</v>
+        <v>11.0</v>
       </c>
       <c r="N16" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="O16" t="n">
-        <v>59.0</v>
+        <v>22.0</v>
       </c>
       <c r="P16" t="n">
-        <v>40.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q16" t="n">
-        <v>30050.0</v>
+        <v>20315.0</v>
       </c>
       <c r="R16" t="n">
-        <v>11.0</v>
+        <v>42.0</v>
       </c>
       <c r="S16" t="n">
-        <v>20738.0</v>
+        <v>45101.0</v>
       </c>
       <c r="T16" t="s">
-        <v>125</v>
-      </c>
-      <c r="U16" t="n" s="2">
-        <v>43220.0</v>
-      </c>
-      <c r="V16" t="n">
-        <v>183.0</v>
+        <v>130</v>
+      </c>
+      <c r="U16" t="n">
+        <v>129.0</v>
+      </c>
+      <c r="V16" t="n" s="2">
+        <v>43275.0</v>
       </c>
     </row>
     <row r="17">
@@ -1552,67 +1558,67 @@
         <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C17" t="n">
         <v>11.0</v>
       </c>
       <c r="D17" t="n">
-        <v>4423.0</v>
+        <v>4028.0</v>
       </c>
       <c r="E17" t="n">
-        <v>4521.0</v>
+        <v>4076.0</v>
       </c>
       <c r="F17" t="n">
-        <v>2718.0</v>
+        <v>1528.0</v>
       </c>
       <c r="G17" t="n">
-        <v>2487.0</v>
+        <v>1451.0</v>
       </c>
       <c r="H17" t="n">
-        <v>6464.0</v>
+        <v>3598.0</v>
       </c>
       <c r="I17" t="n">
-        <v>696.0</v>
+        <v>995.0</v>
       </c>
       <c r="J17" t="n">
-        <v>3583.0</v>
+        <v>2611.0</v>
       </c>
       <c r="K17" t="n">
         <v>10.0</v>
       </c>
       <c r="L17" t="n">
-        <v>0.0</v>
+        <v>33.0</v>
       </c>
       <c r="M17" t="n">
-        <v>0.0</v>
+        <v>34.0</v>
       </c>
       <c r="N17" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="O17" t="n">
-        <v>53.0</v>
+        <v>59.0</v>
       </c>
       <c r="P17" t="n">
-        <v>120.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q17" t="n">
-        <v>21532.0</v>
+        <v>30050.0</v>
       </c>
       <c r="R17" t="n">
-        <v>44.0</v>
+        <v>11.0</v>
       </c>
       <c r="S17" t="n">
-        <v>68905.0</v>
+        <v>20738.0</v>
       </c>
       <c r="T17" t="s">
-        <v>128</v>
-      </c>
-      <c r="U17" t="n" s="2">
-        <v>43058.0</v>
-      </c>
-      <c r="V17" t="n">
-        <v>345.0</v>
+        <v>127</v>
+      </c>
+      <c r="U17" t="n">
+        <v>184.0</v>
+      </c>
+      <c r="V17" t="n" s="2">
+        <v>43220.0</v>
       </c>
     </row>
     <row r="18">
@@ -1620,67 +1626,67 @@
         <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C18" t="n">
-        <v>12.0</v>
+        <v>11.0</v>
       </c>
       <c r="D18" t="n">
-        <v>4344.0</v>
+        <v>4397.0</v>
       </c>
       <c r="E18" t="n">
-        <v>4512.0</v>
+        <v>4521.0</v>
       </c>
       <c r="F18" t="n">
-        <v>2955.0</v>
+        <v>2722.0</v>
       </c>
       <c r="G18" t="n">
-        <v>2843.0</v>
+        <v>2491.0</v>
       </c>
       <c r="H18" t="n">
-        <v>6697.0</v>
+        <v>6475.0</v>
       </c>
       <c r="I18" t="n">
-        <v>1228.0</v>
+        <v>698.0</v>
       </c>
       <c r="J18" t="n">
-        <v>2092.0</v>
+        <v>3595.0</v>
       </c>
       <c r="K18" t="n">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="L18" t="n">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
       <c r="M18" t="n">
-        <v>51.0</v>
+        <v>0.0</v>
       </c>
       <c r="N18" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="O18" t="n">
-        <v>68.0</v>
+        <v>69.0</v>
       </c>
       <c r="P18" t="n">
-        <v>120.0</v>
+        <v>200.0</v>
       </c>
       <c r="Q18" t="n">
-        <v>44835.0</v>
+        <v>21548.0</v>
       </c>
       <c r="R18" t="n">
-        <v>31.0</v>
+        <v>45.0</v>
       </c>
       <c r="S18" t="n">
-        <v>44715.0</v>
+        <v>70585.0</v>
       </c>
       <c r="T18" t="s">
-        <v>128</v>
-      </c>
-      <c r="U18" t="n" s="2">
-        <v>43312.0</v>
-      </c>
-      <c r="V18" t="n">
-        <v>91.0</v>
+        <v>130</v>
+      </c>
+      <c r="U18" t="n">
+        <v>346.0</v>
+      </c>
+      <c r="V18" t="n" s="2">
+        <v>43058.0</v>
       </c>
     </row>
     <row r="19">
@@ -1688,67 +1694,67 @@
         <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C19" t="n">
         <v>12.0</v>
       </c>
       <c r="D19" t="n">
-        <v>4714.0</v>
+        <v>4293.0</v>
       </c>
       <c r="E19" t="n">
-        <v>4732.0</v>
+        <v>4512.0</v>
       </c>
       <c r="F19" t="n">
-        <v>6623.0</v>
+        <v>2956.0</v>
       </c>
       <c r="G19" t="n">
-        <v>6582.0</v>
+        <v>2846.0</v>
       </c>
       <c r="H19" t="n">
-        <v>23235.0</v>
+        <v>6711.0</v>
       </c>
       <c r="I19" t="n">
-        <v>2733.0</v>
+        <v>1231.0</v>
       </c>
       <c r="J19" t="n">
-        <v>2558.0</v>
+        <v>2092.0</v>
       </c>
       <c r="K19" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="L19" t="n">
-        <v>433.0</v>
+        <v>8.0</v>
       </c>
       <c r="M19" t="n">
-        <v>2438.0</v>
+        <v>51.0</v>
       </c>
       <c r="N19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O19" t="n">
-        <v>94.0</v>
+        <v>151.0</v>
       </c>
       <c r="P19" t="n">
-        <v>160.0</v>
+        <v>190.0</v>
       </c>
       <c r="Q19" t="n">
-        <v>66087.0</v>
+        <v>44918.0</v>
       </c>
       <c r="R19" t="n">
-        <v>82.0</v>
+        <v>31.0</v>
       </c>
       <c r="S19" t="n">
-        <v>76295.0</v>
+        <v>45835.0</v>
       </c>
       <c r="T19" t="s">
-        <v>124</v>
-      </c>
-      <c r="U19" t="n" s="2">
-        <v>42705.0</v>
-      </c>
-      <c r="V19" t="n">
-        <v>698.0</v>
+        <v>127</v>
+      </c>
+      <c r="U19" t="n">
+        <v>92.0</v>
+      </c>
+      <c r="V19" t="n" s="2">
+        <v>43312.0</v>
       </c>
     </row>
     <row r="20">
@@ -1756,67 +1762,67 @@
         <v>40</v>
       </c>
       <c r="B20" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C20" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="D20" t="n">
-        <v>3091.0</v>
+        <v>4578.0</v>
       </c>
       <c r="E20" t="n">
-        <v>3170.0</v>
+        <v>4741.0</v>
       </c>
       <c r="F20" t="n">
-        <v>3220.0</v>
+        <v>6633.0</v>
       </c>
       <c r="G20" t="n">
-        <v>4501.0</v>
+        <v>6594.0</v>
       </c>
       <c r="H20" t="n">
-        <v>9017.0</v>
+        <v>23280.0</v>
       </c>
       <c r="I20" t="n">
-        <v>2905.0</v>
+        <v>2736.0</v>
       </c>
       <c r="J20" t="n">
-        <v>444.0</v>
+        <v>2558.0</v>
       </c>
       <c r="K20" t="n">
         <v>10.0</v>
       </c>
       <c r="L20" t="n">
-        <v>0.0</v>
+        <v>433.0</v>
       </c>
       <c r="M20" t="n">
-        <v>0.0</v>
+        <v>2443.0</v>
       </c>
       <c r="N20" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="O20" t="n">
-        <v>30.0</v>
+        <v>212.0</v>
       </c>
       <c r="P20" t="n">
-        <v>40.0</v>
+        <v>280.0</v>
       </c>
       <c r="Q20" t="n">
-        <v>36889.0</v>
+        <v>66205.0</v>
       </c>
       <c r="R20" t="n">
-        <v>25.0</v>
+        <v>84.0</v>
       </c>
       <c r="S20" t="n">
-        <v>41010.0</v>
+        <v>77135.0</v>
       </c>
       <c r="T20" t="s">
-        <v>129</v>
-      </c>
-      <c r="U20" t="n" s="2">
-        <v>43151.0</v>
-      </c>
-      <c r="V20" t="n">
-        <v>252.0</v>
+        <v>130</v>
+      </c>
+      <c r="U20" t="n">
+        <v>699.0</v>
+      </c>
+      <c r="V20" t="n" s="2">
+        <v>42705.0</v>
       </c>
     </row>
     <row r="21">
@@ -1824,31 +1830,31 @@
         <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C21" t="n">
         <v>11.0</v>
       </c>
       <c r="D21" t="n">
-        <v>4113.0</v>
+        <v>3091.0</v>
       </c>
       <c r="E21" t="n">
-        <v>4253.0</v>
+        <v>3170.0</v>
       </c>
       <c r="F21" t="n">
-        <v>1320.0</v>
+        <v>3220.0</v>
       </c>
       <c r="G21" t="n">
-        <v>1380.0</v>
+        <v>4501.0</v>
       </c>
       <c r="H21" t="n">
-        <v>4536.0</v>
+        <v>9017.0</v>
       </c>
       <c r="I21" t="n">
-        <v>867.0</v>
+        <v>2905.0</v>
       </c>
       <c r="J21" t="n">
-        <v>505.0</v>
+        <v>444.0</v>
       </c>
       <c r="K21" t="n">
         <v>10.0</v>
@@ -1860,31 +1866,31 @@
         <v>0.0</v>
       </c>
       <c r="N21" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="O21" t="n">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
       <c r="P21" t="n">
-        <v>0.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q21" t="n">
-        <v>21472.0</v>
+        <v>36889.0</v>
       </c>
       <c r="R21" t="n">
         <v>25.0</v>
       </c>
       <c r="S21" t="n">
-        <v>44781.0</v>
+        <v>41010.0</v>
       </c>
       <c r="T21" t="s">
-        <v>125</v>
-      </c>
-      <c r="U21" t="n" s="2">
-        <v>43254.0</v>
-      </c>
-      <c r="V21" t="n">
-        <v>149.0</v>
+        <v>131</v>
+      </c>
+      <c r="U21" t="n">
+        <v>253.0</v>
+      </c>
+      <c r="V21" t="n" s="2">
+        <v>43151.0</v>
       </c>
     </row>
     <row r="22">
@@ -1892,67 +1898,67 @@
         <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C22" t="n">
         <v>11.0</v>
       </c>
       <c r="D22" t="n">
-        <v>4345.0</v>
+        <v>4119.0</v>
       </c>
       <c r="E22" t="n">
-        <v>4345.0</v>
+        <v>4253.0</v>
       </c>
       <c r="F22" t="n">
-        <v>1883.0</v>
+        <v>1322.0</v>
       </c>
       <c r="G22" t="n">
-        <v>1791.0</v>
+        <v>1382.0</v>
       </c>
       <c r="H22" t="n">
-        <v>7939.0</v>
+        <v>4540.0</v>
       </c>
       <c r="I22" t="n">
-        <v>2040.0</v>
+        <v>868.0</v>
       </c>
       <c r="J22" t="n">
-        <v>1562.0</v>
+        <v>505.0</v>
       </c>
       <c r="K22" t="n">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="L22" t="n">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="M22" t="n">
-        <v>11.0</v>
+        <v>0.0</v>
       </c>
       <c r="N22" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="O22" t="n">
-        <v>124.0</v>
+        <v>0.0</v>
       </c>
       <c r="P22" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>21472.0</v>
+      </c>
+      <c r="R22" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="S22" t="n">
+        <v>44781.0</v>
+      </c>
+      <c r="T22" t="s">
+        <v>127</v>
+      </c>
+      <c r="U22" t="n">
         <v>150.0</v>
       </c>
-      <c r="Q22" t="n">
-        <v>55317.0</v>
-      </c>
-      <c r="R22" t="n">
-        <v>27.0</v>
-      </c>
-      <c r="S22" t="n">
-        <v>61500.0</v>
-      </c>
-      <c r="T22" t="s">
-        <v>128</v>
-      </c>
-      <c r="U22" t="n" s="2">
-        <v>43380.0</v>
-      </c>
-      <c r="V22" t="n">
-        <v>23.0</v>
+      <c r="V22" t="n" s="2">
+        <v>43254.0</v>
       </c>
     </row>
     <row r="23">
@@ -1960,67 +1966,67 @@
         <v>43</v>
       </c>
       <c r="B23" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C23" t="n">
-        <v>12.0</v>
+        <v>11.0</v>
       </c>
       <c r="D23" t="n">
-        <v>4235.0</v>
+        <v>4345.0</v>
       </c>
       <c r="E23" t="n">
-        <v>4280.0</v>
+        <v>4345.0</v>
       </c>
       <c r="F23" t="n">
-        <v>4392.0</v>
+        <v>1883.0</v>
       </c>
       <c r="G23" t="n">
-        <v>4355.0</v>
+        <v>1791.0</v>
       </c>
       <c r="H23" t="n">
-        <v>18254.0</v>
+        <v>7943.0</v>
       </c>
       <c r="I23" t="n">
-        <v>2910.0</v>
+        <v>2041.0</v>
       </c>
       <c r="J23" t="n">
-        <v>2740.0</v>
+        <v>1562.0</v>
       </c>
       <c r="K23" t="n">
         <v>11.0</v>
       </c>
       <c r="L23" t="n">
-        <v>2641.0</v>
+        <v>10.0</v>
       </c>
       <c r="M23" t="n">
-        <v>15427.0</v>
+        <v>11.0</v>
       </c>
       <c r="N23" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O23" t="n">
-        <v>8.0</v>
+        <v>154.0</v>
       </c>
       <c r="P23" t="n">
-        <v>120.0</v>
+        <v>200.0</v>
       </c>
       <c r="Q23" t="n">
-        <v>6192.0</v>
+        <v>55347.0</v>
       </c>
       <c r="R23" t="n">
-        <v>74.0</v>
+        <v>28.0</v>
       </c>
       <c r="S23" t="n">
-        <v>73265.0</v>
+        <v>61500.0</v>
       </c>
       <c r="T23" t="s">
-        <v>125</v>
-      </c>
-      <c r="U23" t="n" s="2">
-        <v>42614.0</v>
-      </c>
-      <c r="V23" t="n">
-        <v>789.0</v>
+        <v>130</v>
+      </c>
+      <c r="U23" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="V23" t="n" s="2">
+        <v>43380.0</v>
       </c>
     </row>
     <row r="24">
@@ -2028,67 +2034,67 @@
         <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C24" t="n">
-        <v>10.0</v>
+        <v>12.0</v>
       </c>
       <c r="D24" t="n">
-        <v>3935.0</v>
+        <v>4235.0</v>
       </c>
       <c r="E24" t="n">
-        <v>4008.0</v>
+        <v>4280.0</v>
       </c>
       <c r="F24" t="n">
-        <v>1357.0</v>
+        <v>4392.0</v>
       </c>
       <c r="G24" t="n">
-        <v>1373.0</v>
+        <v>4355.0</v>
       </c>
       <c r="H24" t="n">
-        <v>3922.0</v>
+        <v>18278.0</v>
       </c>
       <c r="I24" t="n">
-        <v>642.0</v>
+        <v>2912.0</v>
       </c>
       <c r="J24" t="n">
-        <v>793.0</v>
+        <v>2740.0</v>
       </c>
       <c r="K24" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="L24" t="n">
-        <v>0.0</v>
+        <v>2641.0</v>
       </c>
       <c r="M24" t="n">
-        <v>0.0</v>
+        <v>15473.0</v>
       </c>
       <c r="N24" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="O24" t="n">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="P24" t="n">
-        <v>0.0</v>
+        <v>240.0</v>
       </c>
       <c r="Q24" t="n">
-        <v>9576.0</v>
+        <v>6192.0</v>
       </c>
       <c r="R24" t="n">
-        <v>11.0</v>
+        <v>75.0</v>
       </c>
       <c r="S24" t="n">
-        <v>21293.0</v>
+        <v>74105.0</v>
       </c>
       <c r="T24" t="s">
-        <v>126</v>
-      </c>
-      <c r="U24" t="n" s="2">
-        <v>43400.0</v>
-      </c>
-      <c r="V24" t="n">
-        <v>3.0</v>
+        <v>127</v>
+      </c>
+      <c r="U24" t="n">
+        <v>790.0</v>
+      </c>
+      <c r="V24" t="n" s="2">
+        <v>42614.0</v>
       </c>
     </row>
     <row r="25">
@@ -2096,31 +2102,31 @@
         <v>45</v>
       </c>
       <c r="B25" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C25" t="n">
-        <v>12.0</v>
+        <v>10.0</v>
       </c>
       <c r="D25" t="n">
-        <v>4100.0</v>
+        <v>3940.0</v>
       </c>
       <c r="E25" t="n">
-        <v>4210.0</v>
+        <v>4008.0</v>
       </c>
       <c r="F25" t="n">
-        <v>3279.0</v>
+        <v>1358.0</v>
       </c>
       <c r="G25" t="n">
-        <v>3474.0</v>
+        <v>1374.0</v>
       </c>
       <c r="H25" t="n">
-        <v>12054.0</v>
+        <v>3926.0</v>
       </c>
       <c r="I25" t="n">
-        <v>1669.0</v>
+        <v>642.0</v>
       </c>
       <c r="J25" t="n">
-        <v>2752.0</v>
+        <v>793.0</v>
       </c>
       <c r="K25" t="n">
         <v>10.0</v>
@@ -2132,31 +2138,31 @@
         <v>0.0</v>
       </c>
       <c r="N25" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="O25" t="n">
-        <v>246.0</v>
+        <v>44.0</v>
       </c>
       <c r="P25" t="n">
-        <v>160.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q25" t="n">
-        <v>40614.0</v>
+        <v>9620.0</v>
       </c>
       <c r="R25" t="n">
-        <v>61.0</v>
+        <v>11.0</v>
       </c>
       <c r="S25" t="n">
-        <v>66123.0</v>
+        <v>21555.0</v>
       </c>
       <c r="T25" t="s">
-        <v>125</v>
-      </c>
-      <c r="U25" t="n" s="2">
-        <v>43214.0</v>
-      </c>
-      <c r="V25" t="n">
-        <v>189.0</v>
+        <v>129</v>
+      </c>
+      <c r="U25" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="V25" t="n" s="2">
+        <v>43400.0</v>
       </c>
     </row>
     <row r="26">
@@ -2164,67 +2170,67 @@
         <v>46</v>
       </c>
       <c r="B26" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C26" t="n">
         <v>12.0</v>
       </c>
       <c r="D26" t="n">
-        <v>4425.0</v>
+        <v>4100.0</v>
       </c>
       <c r="E26" t="n">
-        <v>4653.0</v>
+        <v>4210.0</v>
       </c>
       <c r="F26" t="n">
-        <v>3677.0</v>
+        <v>3281.0</v>
       </c>
       <c r="G26" t="n">
-        <v>3402.0</v>
+        <v>3477.0</v>
       </c>
       <c r="H26" t="n">
-        <v>11286.0</v>
+        <v>12068.0</v>
       </c>
       <c r="I26" t="n">
-        <v>1542.0</v>
+        <v>1669.0</v>
       </c>
       <c r="J26" t="n">
-        <v>3038.0</v>
+        <v>2757.0</v>
       </c>
       <c r="K26" t="n">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="L26" t="n">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="M26" t="n">
-        <v>192.0</v>
+        <v>0.0</v>
       </c>
       <c r="N26" t="s">
         <v>122</v>
       </c>
       <c r="O26" t="n">
-        <v>0.0</v>
+        <v>340.0</v>
       </c>
       <c r="P26" t="n">
-        <v>0.0</v>
+        <v>240.0</v>
       </c>
       <c r="Q26" t="n">
-        <v>32419.0</v>
+        <v>40708.0</v>
       </c>
       <c r="R26" t="n">
-        <v>57.0</v>
+        <v>61.0</v>
       </c>
       <c r="S26" t="n">
-        <v>68355.0</v>
+        <v>66963.0</v>
       </c>
       <c r="T26" t="s">
-        <v>128</v>
-      </c>
-      <c r="U26" t="n" s="2">
-        <v>42614.0</v>
-      </c>
-      <c r="V26" t="n">
-        <v>789.0</v>
+        <v>127</v>
+      </c>
+      <c r="U26" t="n">
+        <v>190.0</v>
+      </c>
+      <c r="V26" t="n" s="2">
+        <v>43214.0</v>
       </c>
     </row>
     <row r="27">
@@ -2232,43 +2238,43 @@
         <v>47</v>
       </c>
       <c r="B27" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C27" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="D27" t="n">
+        <v>4399.0</v>
+      </c>
+      <c r="E27" t="n">
+        <v>4653.0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>3677.0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>3403.0</v>
+      </c>
+      <c r="H27" t="n">
+        <v>11290.0</v>
+      </c>
+      <c r="I27" t="n">
+        <v>1542.0</v>
+      </c>
+      <c r="J27" t="n">
+        <v>3038.0</v>
+      </c>
+      <c r="K27" t="n">
         <v>11.0</v>
       </c>
-      <c r="D27" t="n">
-        <v>4199.0</v>
-      </c>
-      <c r="E27" t="n">
-        <v>4420.0</v>
-      </c>
-      <c r="F27" t="n">
-        <v>3093.0</v>
-      </c>
-      <c r="G27" t="n">
-        <v>3059.0</v>
-      </c>
-      <c r="H27" t="n">
-        <v>7768.0</v>
-      </c>
-      <c r="I27" t="n">
-        <v>873.0</v>
-      </c>
-      <c r="J27" t="n">
-        <v>2712.0</v>
-      </c>
-      <c r="K27" t="n">
-        <v>10.0</v>
-      </c>
       <c r="L27" t="n">
-        <v>0.0</v>
+        <v>100.0</v>
       </c>
       <c r="M27" t="n">
-        <v>0.0</v>
+        <v>192.0</v>
       </c>
       <c r="N27" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="O27" t="n">
         <v>0.0</v>
@@ -2277,22 +2283,22 @@
         <v>0.0</v>
       </c>
       <c r="Q27" t="n">
-        <v>12600.0</v>
+        <v>32419.0</v>
       </c>
       <c r="R27" t="n">
-        <v>65.0</v>
+        <v>57.0</v>
       </c>
       <c r="S27" t="n">
-        <v>67441.0</v>
+        <v>69755.0</v>
       </c>
       <c r="T27" t="s">
-        <v>125</v>
-      </c>
-      <c r="U27" t="n" s="2">
-        <v>43254.0</v>
-      </c>
-      <c r="V27" t="n">
-        <v>149.0</v>
+        <v>130</v>
+      </c>
+      <c r="U27" t="n">
+        <v>790.0</v>
+      </c>
+      <c r="V27" t="n" s="2">
+        <v>42614.0</v>
       </c>
     </row>
     <row r="28">
@@ -2300,67 +2306,67 @@
         <v>48</v>
       </c>
       <c r="B28" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C28" t="n">
-        <v>12.0</v>
+        <v>11.0</v>
       </c>
       <c r="D28" t="n">
-        <v>4022.0</v>
+        <v>4233.0</v>
       </c>
       <c r="E28" t="n">
-        <v>4052.0</v>
+        <v>4420.0</v>
       </c>
       <c r="F28" t="n">
-        <v>3536.0</v>
+        <v>3096.0</v>
       </c>
       <c r="G28" t="n">
-        <v>3377.0</v>
+        <v>3061.0</v>
       </c>
       <c r="H28" t="n">
-        <v>9124.0</v>
+        <v>7776.0</v>
       </c>
       <c r="I28" t="n">
-        <v>954.0</v>
+        <v>874.0</v>
       </c>
       <c r="J28" t="n">
-        <v>1745.0</v>
+        <v>2712.0</v>
       </c>
       <c r="K28" t="n">
         <v>10.0</v>
       </c>
       <c r="L28" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N28" t="s">
+        <v>122</v>
+      </c>
+      <c r="O28" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P28" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>12600.0</v>
+      </c>
+      <c r="R28" t="n">
         <v>65.0</v>
       </c>
-      <c r="M28" t="n">
-        <v>91.0</v>
-      </c>
-      <c r="N28" t="s">
-        <v>121</v>
-      </c>
-      <c r="O28" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="P28" t="n">
-        <v>80.0</v>
-      </c>
-      <c r="Q28" t="n">
-        <v>51388.0</v>
-      </c>
-      <c r="R28" t="n">
-        <v>3.0</v>
-      </c>
       <c r="S28" t="n">
-        <v>3940.0</v>
+        <v>68841.0</v>
       </c>
       <c r="T28" t="s">
-        <v>125</v>
-      </c>
-      <c r="U28" t="n" s="2">
-        <v>43402.0</v>
-      </c>
-      <c r="V28" t="n">
-        <v>1.0</v>
+        <v>127</v>
+      </c>
+      <c r="U28" t="n">
+        <v>150.0</v>
+      </c>
+      <c r="V28" t="n" s="2">
+        <v>43254.0</v>
       </c>
     </row>
     <row r="29">
@@ -2368,67 +2374,67 @@
         <v>49</v>
       </c>
       <c r="B29" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C29" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="D29" t="n">
-        <v>4067.0</v>
+        <v>4022.0</v>
       </c>
       <c r="E29" t="n">
-        <v>4258.0</v>
+        <v>4052.0</v>
       </c>
       <c r="F29" t="n">
-        <v>1331.0</v>
+        <v>3536.0</v>
       </c>
       <c r="G29" t="n">
-        <v>1101.0</v>
+        <v>3377.0</v>
       </c>
       <c r="H29" t="n">
-        <v>6396.0</v>
+        <v>9124.0</v>
       </c>
       <c r="I29" t="n">
-        <v>1412.0</v>
+        <v>954.0</v>
       </c>
       <c r="J29" t="n">
-        <v>1856.0</v>
+        <v>1745.0</v>
       </c>
       <c r="K29" t="n">
         <v>10.0</v>
       </c>
       <c r="L29" t="n">
-        <v>14.0</v>
+        <v>65.0</v>
       </c>
       <c r="M29" t="n">
-        <v>21.0</v>
+        <v>91.0</v>
       </c>
       <c r="N29" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="O29" t="n">
-        <v>187.0</v>
+        <v>40.0</v>
       </c>
       <c r="P29" t="n">
-        <v>140.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q29" t="n">
-        <v>11530.0</v>
+        <v>51388.0</v>
       </c>
       <c r="R29" t="n">
-        <v>54.0</v>
+        <v>3.0</v>
       </c>
       <c r="S29" t="n">
-        <v>67262.0</v>
+        <v>3940.0</v>
       </c>
       <c r="T29" t="s">
-        <v>125</v>
-      </c>
-      <c r="U29" t="n" s="2">
-        <v>43058.0</v>
-      </c>
-      <c r="V29" t="n">
-        <v>345.0</v>
+        <v>127</v>
+      </c>
+      <c r="U29" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="V29" t="n" s="2">
+        <v>43402.0</v>
       </c>
     </row>
     <row r="30">
@@ -2436,67 +2442,67 @@
         <v>50</v>
       </c>
       <c r="B30" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C30" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="D30" t="n">
-        <v>3827.0</v>
+        <v>4127.0</v>
       </c>
       <c r="E30" t="n">
-        <v>3977.0</v>
+        <v>4258.0</v>
       </c>
       <c r="F30" t="n">
-        <v>658.0</v>
+        <v>1334.0</v>
       </c>
       <c r="G30" t="n">
-        <v>531.0</v>
+        <v>1101.0</v>
       </c>
       <c r="H30" t="n">
-        <v>3305.0</v>
+        <v>6410.0</v>
       </c>
       <c r="I30" t="n">
-        <v>731.0</v>
+        <v>1418.0</v>
       </c>
       <c r="J30" t="n">
-        <v>836.0</v>
+        <v>1856.0</v>
       </c>
       <c r="K30" t="n">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="L30" t="n">
-        <v>0.0</v>
+        <v>14.0</v>
       </c>
       <c r="M30" t="n">
-        <v>0.0</v>
+        <v>21.0</v>
       </c>
       <c r="N30" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="O30" t="n">
-        <v>0.0</v>
+        <v>289.0</v>
       </c>
       <c r="P30" t="n">
-        <v>40.0</v>
+        <v>220.0</v>
       </c>
       <c r="Q30" t="n">
-        <v>4603.0</v>
+        <v>11632.0</v>
       </c>
       <c r="R30" t="n">
-        <v>48.0</v>
+        <v>54.0</v>
       </c>
       <c r="S30" t="n">
-        <v>60281.0</v>
+        <v>67822.0</v>
       </c>
       <c r="T30" t="s">
-        <v>126</v>
-      </c>
-      <c r="U30" t="n" s="2">
-        <v>43138.0</v>
-      </c>
-      <c r="V30" t="n">
-        <v>265.0</v>
+        <v>127</v>
+      </c>
+      <c r="U30" t="n">
+        <v>346.0</v>
+      </c>
+      <c r="V30" t="n" s="2">
+        <v>43058.0</v>
       </c>
     </row>
     <row r="31">
@@ -2504,67 +2510,67 @@
         <v>51</v>
       </c>
       <c r="B31" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C31" t="n">
-        <v>12.0</v>
+        <v>10.0</v>
       </c>
       <c r="D31" t="n">
-        <v>4045.0</v>
+        <v>3827.0</v>
       </c>
       <c r="E31" t="n">
-        <v>4140.0</v>
+        <v>3977.0</v>
       </c>
       <c r="F31" t="n">
-        <v>2114.0</v>
+        <v>658.0</v>
       </c>
       <c r="G31" t="n">
-        <v>2165.0</v>
+        <v>531.0</v>
       </c>
       <c r="H31" t="n">
-        <v>6847.0</v>
+        <v>3313.0</v>
       </c>
       <c r="I31" t="n">
-        <v>1543.0</v>
+        <v>731.0</v>
       </c>
       <c r="J31" t="n">
-        <v>1474.0</v>
+        <v>836.0</v>
       </c>
       <c r="K31" t="n">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="L31" t="n">
         <v>0.0</v>
       </c>
       <c r="M31" t="n">
-        <v>41.0</v>
+        <v>0.0</v>
       </c>
       <c r="N31" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="O31" t="n">
-        <v>21.0</v>
+        <v>10.0</v>
       </c>
       <c r="P31" t="n">
-        <v>40.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q31" t="n">
-        <v>41690.0</v>
+        <v>4613.0</v>
       </c>
       <c r="R31" t="n">
-        <v>35.0</v>
+        <v>48.0</v>
       </c>
       <c r="S31" t="n">
-        <v>65287.0</v>
+        <v>61593.0</v>
       </c>
       <c r="T31" t="s">
-        <v>125</v>
-      </c>
-      <c r="U31" t="n" s="2">
-        <v>42920.0</v>
-      </c>
-      <c r="V31" t="n">
-        <v>483.0</v>
+        <v>129</v>
+      </c>
+      <c r="U31" t="n">
+        <v>266.0</v>
+      </c>
+      <c r="V31" t="n" s="2">
+        <v>43138.0</v>
       </c>
     </row>
     <row r="32">
@@ -2572,67 +2578,67 @@
         <v>52</v>
       </c>
       <c r="B32" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C32" t="n">
         <v>12.0</v>
       </c>
       <c r="D32" t="n">
-        <v>4578.0</v>
+        <v>4018.0</v>
       </c>
       <c r="E32" t="n">
-        <v>4798.0</v>
+        <v>4140.0</v>
       </c>
       <c r="F32" t="n">
-        <v>5067.0</v>
+        <v>2114.0</v>
       </c>
       <c r="G32" t="n">
-        <v>5187.0</v>
+        <v>2166.0</v>
       </c>
       <c r="H32" t="n">
-        <v>12164.0</v>
+        <v>6849.0</v>
       </c>
       <c r="I32" t="n">
-        <v>2219.0</v>
+        <v>1543.0</v>
       </c>
       <c r="J32" t="n">
-        <v>1703.0</v>
+        <v>1474.0</v>
       </c>
       <c r="K32" t="n">
         <v>10.0</v>
       </c>
       <c r="L32" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M32" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="N32" t="s">
+        <v>122</v>
+      </c>
+      <c r="O32" t="n">
         <v>31.0</v>
       </c>
-      <c r="M32" t="n">
-        <v>43.0</v>
-      </c>
-      <c r="N32" t="s">
-        <v>120</v>
-      </c>
-      <c r="O32" t="n">
-        <v>0.0</v>
-      </c>
       <c r="P32" t="n">
-        <v>0.0</v>
+        <v>60.0</v>
       </c>
       <c r="Q32" t="n">
-        <v>58372.0</v>
+        <v>41700.0</v>
       </c>
       <c r="R32" t="n">
-        <v>29.0</v>
+        <v>35.0</v>
       </c>
       <c r="S32" t="n">
-        <v>71230.0</v>
+        <v>65567.0</v>
       </c>
       <c r="T32" t="s">
-        <v>128</v>
-      </c>
-      <c r="U32" t="n" s="2">
-        <v>43058.0</v>
-      </c>
-      <c r="V32" t="n">
-        <v>345.0</v>
+        <v>127</v>
+      </c>
+      <c r="U32" t="n">
+        <v>484.0</v>
+      </c>
+      <c r="V32" t="n" s="2">
+        <v>42920.0</v>
       </c>
     </row>
     <row r="33">
@@ -2640,67 +2646,67 @@
         <v>53</v>
       </c>
       <c r="B33" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C33" t="n">
-        <v>10.0</v>
+        <v>12.0</v>
       </c>
       <c r="D33" t="n">
-        <v>4112.0</v>
+        <v>4529.0</v>
       </c>
       <c r="E33" t="n">
-        <v>4165.0</v>
+        <v>4798.0</v>
       </c>
       <c r="F33" t="n">
-        <v>899.0</v>
+        <v>5076.0</v>
       </c>
       <c r="G33" t="n">
-        <v>750.0</v>
+        <v>5194.0</v>
       </c>
       <c r="H33" t="n">
-        <v>3648.0</v>
+        <v>12184.0</v>
       </c>
       <c r="I33" t="n">
-        <v>783.0</v>
+        <v>2220.0</v>
       </c>
       <c r="J33" t="n">
-        <v>846.0</v>
+        <v>1728.0</v>
       </c>
       <c r="K33" t="n">
-        <v>8.0</v>
+        <v>10.0</v>
       </c>
       <c r="L33" t="n">
-        <v>0.0</v>
+        <v>31.0</v>
       </c>
       <c r="M33" t="n">
-        <v>1.0</v>
+        <v>43.0</v>
       </c>
       <c r="N33" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="O33" t="n">
-        <v>0.0</v>
+        <v>40.0</v>
       </c>
       <c r="P33" t="n">
-        <v>0.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q33" t="n">
-        <v>21863.0</v>
+        <v>58412.0</v>
       </c>
       <c r="R33" t="n">
-        <v>24.0</v>
+        <v>29.0</v>
       </c>
       <c r="S33" t="n">
-        <v>38022.0</v>
+        <v>72350.0</v>
       </c>
       <c r="T33" t="s">
-        <v>125</v>
-      </c>
-      <c r="U33" t="n" s="2">
-        <v>43302.0</v>
-      </c>
-      <c r="V33" t="n">
-        <v>101.0</v>
+        <v>130</v>
+      </c>
+      <c r="U33" t="n">
+        <v>346.0</v>
+      </c>
+      <c r="V33" t="n" s="2">
+        <v>43058.0</v>
       </c>
     </row>
     <row r="34">
@@ -2708,43 +2714,43 @@
         <v>54</v>
       </c>
       <c r="B34" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C34" t="n">
         <v>10.0</v>
       </c>
       <c r="D34" t="n">
-        <v>3882.0</v>
+        <v>4112.0</v>
       </c>
       <c r="E34" t="n">
-        <v>3907.0</v>
+        <v>4165.0</v>
       </c>
       <c r="F34" t="n">
-        <v>929.0</v>
+        <v>899.0</v>
       </c>
       <c r="G34" t="n">
-        <v>954.0</v>
+        <v>750.0</v>
       </c>
       <c r="H34" t="n">
-        <v>4120.0</v>
+        <v>3648.0</v>
       </c>
       <c r="I34" t="n">
-        <v>979.0</v>
+        <v>783.0</v>
       </c>
       <c r="J34" t="n">
-        <v>278.0</v>
+        <v>846.0</v>
       </c>
       <c r="K34" t="n">
-        <v>6.0</v>
+        <v>8.0</v>
       </c>
       <c r="L34" t="n">
         <v>0.0</v>
       </c>
       <c r="M34" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="N34" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="O34" t="n">
         <v>0.0</v>
@@ -2753,22 +2759,22 @@
         <v>0.0</v>
       </c>
       <c r="Q34" t="n">
-        <v>8193.0</v>
+        <v>21863.0</v>
       </c>
       <c r="R34" t="n">
         <v>24.0</v>
       </c>
       <c r="S34" t="n">
-        <v>56403.0</v>
+        <v>38022.0</v>
       </c>
       <c r="T34" t="s">
-        <v>126</v>
-      </c>
-      <c r="U34" t="n" s="2">
-        <v>43312.0</v>
-      </c>
-      <c r="V34" t="n">
-        <v>91.0</v>
+        <v>127</v>
+      </c>
+      <c r="U34" t="n">
+        <v>102.0</v>
+      </c>
+      <c r="V34" t="n" s="2">
+        <v>43302.0</v>
       </c>
     </row>
     <row r="35">
@@ -2776,34 +2782,34 @@
         <v>55</v>
       </c>
       <c r="B35" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C35" t="n">
         <v>10.0</v>
       </c>
       <c r="D35" t="n">
-        <v>3826.0</v>
+        <v>3882.0</v>
       </c>
       <c r="E35" t="n">
-        <v>4007.0</v>
+        <v>3907.0</v>
       </c>
       <c r="F35" t="n">
-        <v>532.0</v>
+        <v>929.0</v>
       </c>
       <c r="G35" t="n">
-        <v>460.0</v>
+        <v>954.0</v>
       </c>
       <c r="H35" t="n">
-        <v>3248.0</v>
+        <v>4121.0</v>
       </c>
       <c r="I35" t="n">
-        <v>682.0</v>
+        <v>979.0</v>
       </c>
       <c r="J35" t="n">
         <v>278.0</v>
       </c>
       <c r="K35" t="n">
-        <v>9.0</v>
+        <v>6.0</v>
       </c>
       <c r="L35" t="n">
         <v>0.0</v>
@@ -2812,31 +2818,31 @@
         <v>0.0</v>
       </c>
       <c r="N35" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="O35" t="n">
-        <v>70.0</v>
+        <v>0.0</v>
       </c>
       <c r="P35" t="n">
-        <v>81.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q35" t="n">
-        <v>16252.0</v>
+        <v>8193.0</v>
       </c>
       <c r="R35" t="n">
-        <v>21.0</v>
+        <v>25.0</v>
       </c>
       <c r="S35" t="n">
-        <v>55280.0</v>
+        <v>56403.0</v>
       </c>
       <c r="T35" t="s">
-        <v>126</v>
-      </c>
-      <c r="U35" t="n" s="2">
-        <v>43274.0</v>
-      </c>
-      <c r="V35" t="n">
-        <v>129.0</v>
+        <v>129</v>
+      </c>
+      <c r="U35" t="n">
+        <v>92.0</v>
+      </c>
+      <c r="V35" t="n" s="2">
+        <v>43312.0</v>
       </c>
     </row>
     <row r="36">
@@ -2844,34 +2850,34 @@
         <v>56</v>
       </c>
       <c r="B36" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C36" t="n">
         <v>10.0</v>
       </c>
       <c r="D36" t="n">
-        <v>3938.0</v>
+        <v>3776.0</v>
       </c>
       <c r="E36" t="n">
-        <v>4017.0</v>
+        <v>4007.0</v>
       </c>
       <c r="F36" t="n">
-        <v>3283.0</v>
+        <v>533.0</v>
       </c>
       <c r="G36" t="n">
-        <v>3830.0</v>
+        <v>463.0</v>
       </c>
       <c r="H36" t="n">
-        <v>9132.0</v>
+        <v>3255.0</v>
       </c>
       <c r="I36" t="n">
-        <v>1697.0</v>
+        <v>683.0</v>
       </c>
       <c r="J36" t="n">
-        <v>222.0</v>
+        <v>278.0</v>
       </c>
       <c r="K36" t="n">
-        <v>4.0</v>
+        <v>9.0</v>
       </c>
       <c r="L36" t="n">
         <v>0.0</v>
@@ -2880,31 +2886,31 @@
         <v>0.0</v>
       </c>
       <c r="N36" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="O36" t="n">
-        <v>31.0</v>
+        <v>90.0</v>
       </c>
       <c r="P36" t="n">
-        <v>40.0</v>
+        <v>160.0</v>
       </c>
       <c r="Q36" t="n">
-        <v>13970.0</v>
+        <v>16272.0</v>
       </c>
       <c r="R36" t="n">
-        <v>34.0</v>
+        <v>22.0</v>
       </c>
       <c r="S36" t="n">
-        <v>62347.0</v>
+        <v>55525.0</v>
       </c>
       <c r="T36" t="s">
-        <v>126</v>
-      </c>
-      <c r="U36" t="n" s="2">
-        <v>43280.0</v>
-      </c>
-      <c r="V36" t="n">
-        <v>123.0</v>
+        <v>128</v>
+      </c>
+      <c r="U36" t="n">
+        <v>130.0</v>
+      </c>
+      <c r="V36" t="n" s="2">
+        <v>43274.0</v>
       </c>
     </row>
     <row r="37">
@@ -2912,34 +2918,34 @@
         <v>57</v>
       </c>
       <c r="B37" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C37" t="n">
-        <v>8.0</v>
+        <v>10.0</v>
       </c>
       <c r="D37" t="n">
-        <v>3431.0</v>
+        <v>3975.0</v>
       </c>
       <c r="E37" t="n">
-        <v>3497.0</v>
+        <v>4017.0</v>
       </c>
       <c r="F37" t="n">
-        <v>275.0</v>
+        <v>3294.0</v>
       </c>
       <c r="G37" t="n">
-        <v>150.0</v>
+        <v>3844.0</v>
       </c>
       <c r="H37" t="n">
-        <v>525.0</v>
+        <v>9161.0</v>
       </c>
       <c r="I37" t="n">
-        <v>98.0</v>
+        <v>1701.0</v>
       </c>
       <c r="J37" t="n">
-        <v>348.0</v>
+        <v>224.0</v>
       </c>
       <c r="K37" t="n">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="L37" t="n">
         <v>0.0</v>
@@ -2948,31 +2954,31 @@
         <v>0.0</v>
       </c>
       <c r="N37" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="O37" t="n">
-        <v>92.0</v>
+        <v>105.0</v>
       </c>
       <c r="P37" t="n">
-        <v>70.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q37" t="n">
-        <v>2003.0</v>
+        <v>14044.0</v>
       </c>
       <c r="R37" t="n">
-        <v>1.0</v>
+        <v>34.0</v>
       </c>
       <c r="S37" t="n">
-        <v>5301.0</v>
+        <v>63134.0</v>
       </c>
       <c r="T37" t="s">
-        <v>127</v>
-      </c>
-      <c r="U37" t="n" s="2">
-        <v>43360.0</v>
-      </c>
-      <c r="V37" t="n">
-        <v>43.0</v>
+        <v>129</v>
+      </c>
+      <c r="U37" t="n">
+        <v>124.0</v>
+      </c>
+      <c r="V37" t="n" s="2">
+        <v>43280.0</v>
       </c>
     </row>
     <row r="38">
@@ -2980,67 +2986,67 @@
         <v>58</v>
       </c>
       <c r="B38" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C38" t="n">
-        <v>11.0</v>
+        <v>8.0</v>
       </c>
       <c r="D38" t="n">
-        <v>4315.0</v>
+        <v>3460.0</v>
       </c>
       <c r="E38" t="n">
-        <v>4315.0</v>
+        <v>3497.0</v>
       </c>
       <c r="F38" t="n">
-        <v>1092.0</v>
+        <v>281.0</v>
       </c>
       <c r="G38" t="n">
-        <v>946.0</v>
+        <v>151.0</v>
       </c>
       <c r="H38" t="n">
-        <v>4191.0</v>
+        <v>533.0</v>
       </c>
       <c r="I38" t="n">
-        <v>436.0</v>
+        <v>101.0</v>
       </c>
       <c r="J38" t="n">
-        <v>2178.0</v>
+        <v>373.0</v>
       </c>
       <c r="K38" t="n">
-        <v>8.0</v>
+        <v>6.0</v>
       </c>
       <c r="L38" t="n">
-        <v>81.0</v>
+        <v>0.0</v>
       </c>
       <c r="M38" t="n">
-        <v>202.0</v>
+        <v>0.0</v>
       </c>
       <c r="N38" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="O38" t="n">
-        <v>257.0</v>
+        <v>142.0</v>
       </c>
       <c r="P38" t="n">
-        <v>180.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q38" t="n">
-        <v>23938.0</v>
+        <v>2053.0</v>
       </c>
       <c r="R38" t="n">
-        <v>34.0</v>
+        <v>1.0</v>
       </c>
       <c r="S38" t="n">
-        <v>67786.0</v>
+        <v>5791.0</v>
       </c>
       <c r="T38" t="s">
         <v>128</v>
       </c>
-      <c r="U38" t="n" s="2">
-        <v>43284.0</v>
-      </c>
-      <c r="V38" t="n">
-        <v>119.0</v>
+      <c r="U38" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="V38" t="n" s="2">
+        <v>43360.0</v>
       </c>
     </row>
     <row r="39">
@@ -3048,67 +3054,67 @@
         <v>59</v>
       </c>
       <c r="B39" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C39" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="D39" t="n">
-        <v>4365.0</v>
+        <v>4315.0</v>
       </c>
       <c r="E39" t="n">
-        <v>4405.0</v>
+        <v>4315.0</v>
       </c>
       <c r="F39" t="n">
-        <v>1091.0</v>
+        <v>1101.0</v>
       </c>
       <c r="G39" t="n">
-        <v>990.0</v>
+        <v>951.0</v>
       </c>
       <c r="H39" t="n">
-        <v>3112.0</v>
+        <v>4221.0</v>
       </c>
       <c r="I39" t="n">
-        <v>650.0</v>
+        <v>442.0</v>
       </c>
       <c r="J39" t="n">
-        <v>1700.0</v>
+        <v>2215.0</v>
       </c>
       <c r="K39" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="L39" t="n">
-        <v>0.0</v>
+        <v>81.0</v>
       </c>
       <c r="M39" t="n">
-        <v>1.0</v>
+        <v>202.0</v>
       </c>
       <c r="N39" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="O39" t="n">
-        <v>70.0</v>
+        <v>443.0</v>
       </c>
       <c r="P39" t="n">
-        <v>80.0</v>
+        <v>290.0</v>
       </c>
       <c r="Q39" t="n">
-        <v>19512.0</v>
+        <v>24124.0</v>
       </c>
       <c r="R39" t="n">
-        <v>14.0</v>
+        <v>35.0</v>
       </c>
       <c r="S39" t="n">
-        <v>46360.0</v>
+        <v>69186.0</v>
       </c>
       <c r="T39" t="s">
-        <v>128</v>
-      </c>
-      <c r="U39" t="n" s="2">
-        <v>43352.0</v>
-      </c>
-      <c r="V39" t="n">
-        <v>51.0</v>
+        <v>130</v>
+      </c>
+      <c r="U39" t="n">
+        <v>120.0</v>
+      </c>
+      <c r="V39" t="n" s="2">
+        <v>43284.0</v>
       </c>
     </row>
     <row r="40">
@@ -3116,67 +3122,67 @@
         <v>60</v>
       </c>
       <c r="B40" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C40" t="n">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="D40" t="n">
-        <v>4527.0</v>
+        <v>4365.0</v>
       </c>
       <c r="E40" t="n">
-        <v>4542.0</v>
+        <v>4405.0</v>
       </c>
       <c r="F40" t="n">
-        <v>4633.0</v>
+        <v>1091.0</v>
       </c>
       <c r="G40" t="n">
-        <v>4693.0</v>
+        <v>990.0</v>
       </c>
       <c r="H40" t="n">
-        <v>26240.0</v>
+        <v>3112.0</v>
       </c>
       <c r="I40" t="n">
-        <v>3571.0</v>
+        <v>650.0</v>
       </c>
       <c r="J40" t="n">
-        <v>2006.0</v>
+        <v>1700.0</v>
       </c>
       <c r="K40" t="n">
-        <v>11.0</v>
+        <v>7.0</v>
       </c>
       <c r="L40" t="n">
         <v>0.0</v>
       </c>
       <c r="M40" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="N40" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="O40" t="n">
-        <v>4.0</v>
+        <v>88.0</v>
       </c>
       <c r="P40" t="n">
-        <v>80.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q40" t="n">
-        <v>7097.0</v>
+        <v>19530.0</v>
       </c>
       <c r="R40" t="n">
-        <v>54.0</v>
+        <v>14.0</v>
       </c>
       <c r="S40" t="n">
-        <v>65915.0</v>
+        <v>46360.0</v>
       </c>
       <c r="T40" t="s">
-        <v>128</v>
-      </c>
-      <c r="U40" t="n" s="2">
-        <v>43252.0</v>
-      </c>
-      <c r="V40" t="n">
-        <v>151.0</v>
+        <v>130</v>
+      </c>
+      <c r="U40" t="n">
+        <v>52.0</v>
+      </c>
+      <c r="V40" t="n" s="2">
+        <v>43352.0</v>
       </c>
     </row>
     <row r="41">
@@ -3184,31 +3190,31 @@
         <v>61</v>
       </c>
       <c r="B41" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C41" t="n">
         <v>11.0</v>
       </c>
       <c r="D41" t="n">
-        <v>4199.0</v>
+        <v>4527.0</v>
       </c>
       <c r="E41" t="n">
-        <v>4323.0</v>
+        <v>4542.0</v>
       </c>
       <c r="F41" t="n">
-        <v>2353.0</v>
+        <v>4633.0</v>
       </c>
       <c r="G41" t="n">
-        <v>2279.0</v>
+        <v>4693.0</v>
       </c>
       <c r="H41" t="n">
-        <v>5897.0</v>
+        <v>26295.0</v>
       </c>
       <c r="I41" t="n">
-        <v>1166.0</v>
+        <v>3579.0</v>
       </c>
       <c r="J41" t="n">
-        <v>2789.0</v>
+        <v>2006.0</v>
       </c>
       <c r="K41" t="n">
         <v>11.0</v>
@@ -3220,31 +3226,31 @@
         <v>0.0</v>
       </c>
       <c r="N41" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="O41" t="n">
-        <v>0.0</v>
+        <v>12.0</v>
       </c>
       <c r="P41" t="n">
-        <v>40.0</v>
+        <v>160.0</v>
       </c>
       <c r="Q41" t="n">
-        <v>20727.0</v>
+        <v>7105.0</v>
       </c>
       <c r="R41" t="n">
-        <v>15.0</v>
+        <v>55.0</v>
       </c>
       <c r="S41" t="n">
-        <v>25052.0</v>
+        <v>67035.0</v>
       </c>
       <c r="T41" t="s">
-        <v>125</v>
-      </c>
-      <c r="U41" t="n" s="2">
-        <v>43370.0</v>
-      </c>
-      <c r="V41" t="n">
-        <v>33.0</v>
+        <v>130</v>
+      </c>
+      <c r="U41" t="n">
+        <v>152.0</v>
+      </c>
+      <c r="V41" t="n" s="2">
+        <v>43252.0</v>
       </c>
     </row>
     <row r="42">
@@ -3252,34 +3258,34 @@
         <v>62</v>
       </c>
       <c r="B42" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C42" t="n">
-        <v>12.0</v>
+        <v>11.0</v>
       </c>
       <c r="D42" t="n">
-        <v>4211.0</v>
+        <v>4201.0</v>
       </c>
       <c r="E42" t="n">
-        <v>4211.0</v>
+        <v>4323.0</v>
       </c>
       <c r="F42" t="n">
-        <v>2709.0</v>
+        <v>2354.0</v>
       </c>
       <c r="G42" t="n">
-        <v>2641.0</v>
+        <v>2280.0</v>
       </c>
       <c r="H42" t="n">
-        <v>7679.0</v>
+        <v>5907.0</v>
       </c>
       <c r="I42" t="n">
-        <v>2237.0</v>
+        <v>1166.0</v>
       </c>
       <c r="J42" t="n">
-        <v>2287.0</v>
+        <v>2789.0</v>
       </c>
       <c r="K42" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="L42" t="n">
         <v>0.0</v>
@@ -3288,31 +3294,31 @@
         <v>0.0</v>
       </c>
       <c r="N42" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="O42" t="n">
-        <v>60.0</v>
+        <v>26.0</v>
       </c>
       <c r="P42" t="n">
         <v>80.0</v>
       </c>
       <c r="Q42" t="n">
-        <v>30990.0</v>
+        <v>20753.0</v>
       </c>
       <c r="R42" t="n">
-        <v>19.0</v>
+        <v>15.0</v>
       </c>
       <c r="S42" t="n">
-        <v>18335.0</v>
+        <v>26452.0</v>
       </c>
       <c r="T42" t="s">
-        <v>125</v>
-      </c>
-      <c r="U42" t="n" s="2">
-        <v>43382.0</v>
-      </c>
-      <c r="V42" t="n">
-        <v>21.0</v>
+        <v>127</v>
+      </c>
+      <c r="U42" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="V42" t="n" s="2">
+        <v>43370.0</v>
       </c>
     </row>
     <row r="43">
@@ -3320,67 +3326,67 @@
         <v>63</v>
       </c>
       <c r="B43" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C43" t="n">
-        <v>10.0</v>
+        <v>12.0</v>
       </c>
       <c r="D43" t="n">
-        <v>4210.0</v>
+        <v>4211.0</v>
       </c>
       <c r="E43" t="n">
-        <v>4318.0</v>
+        <v>4211.0</v>
       </c>
       <c r="F43" t="n">
-        <v>3766.0</v>
+        <v>2713.0</v>
       </c>
       <c r="G43" t="n">
-        <v>4077.0</v>
+        <v>2643.0</v>
       </c>
       <c r="H43" t="n">
-        <v>8547.0</v>
+        <v>7688.0</v>
       </c>
       <c r="I43" t="n">
-        <v>2006.0</v>
+        <v>2239.0</v>
       </c>
       <c r="J43" t="n">
-        <v>1328.0</v>
+        <v>2287.0</v>
       </c>
       <c r="K43" t="n">
         <v>10.0</v>
       </c>
       <c r="L43" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="M43" t="n">
         <v>0.0</v>
       </c>
       <c r="N43" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="O43" t="n">
-        <v>134.0</v>
+        <v>76.0</v>
       </c>
       <c r="P43" t="n">
-        <v>100.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q43" t="n">
-        <v>20447.0</v>
+        <v>31006.0</v>
       </c>
       <c r="R43" t="n">
-        <v>18.0</v>
+        <v>19.0</v>
       </c>
       <c r="S43" t="n">
-        <v>64732.0</v>
+        <v>18615.0</v>
       </c>
       <c r="T43" t="s">
-        <v>125</v>
-      </c>
-      <c r="U43" t="n" s="2">
-        <v>43390.0</v>
-      </c>
-      <c r="V43" t="n">
-        <v>13.0</v>
+        <v>127</v>
+      </c>
+      <c r="U43" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="V43" t="n" s="2">
+        <v>43382.0</v>
       </c>
     </row>
     <row r="44">
@@ -3388,67 +3394,67 @@
         <v>64</v>
       </c>
       <c r="B44" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C44" t="n">
-        <v>12.0</v>
+        <v>10.0</v>
       </c>
       <c r="D44" t="n">
-        <v>4417.0</v>
+        <v>4210.0</v>
       </c>
       <c r="E44" t="n">
-        <v>4473.0</v>
+        <v>4318.0</v>
       </c>
       <c r="F44" t="n">
-        <v>2625.0</v>
+        <v>3767.0</v>
       </c>
       <c r="G44" t="n">
-        <v>2570.0</v>
+        <v>4079.0</v>
       </c>
       <c r="H44" t="n">
-        <v>7170.0</v>
+        <v>8551.0</v>
       </c>
       <c r="I44" t="n">
-        <v>1372.0</v>
+        <v>2006.0</v>
       </c>
       <c r="J44" t="n">
-        <v>3495.0</v>
+        <v>1328.0</v>
       </c>
       <c r="K44" t="n">
         <v>10.0</v>
       </c>
       <c r="L44" t="n">
-        <v>106.0</v>
+        <v>4.0</v>
       </c>
       <c r="M44" t="n">
-        <v>144.0</v>
+        <v>0.0</v>
       </c>
       <c r="N44" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="O44" t="n">
-        <v>50.0</v>
+        <v>212.0</v>
       </c>
       <c r="P44" t="n">
-        <v>40.0</v>
+        <v>140.0</v>
       </c>
       <c r="Q44" t="n">
-        <v>48401.0</v>
+        <v>20525.0</v>
       </c>
       <c r="R44" t="n">
-        <v>29.0</v>
+        <v>18.0</v>
       </c>
       <c r="S44" t="n">
-        <v>36645.0</v>
+        <v>64732.0</v>
       </c>
       <c r="T44" t="s">
-        <v>128</v>
-      </c>
-      <c r="U44" t="n" s="2">
+        <v>127</v>
+      </c>
+      <c r="U44" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="V44" t="n" s="2">
         <v>43390.0</v>
-      </c>
-      <c r="V44" t="n">
-        <v>13.0</v>
       </c>
     </row>
     <row r="45">
@@ -3456,67 +3462,67 @@
         <v>65</v>
       </c>
       <c r="B45" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C45" t="n">
-        <v>7.0</v>
+        <v>12.0</v>
       </c>
       <c r="D45" t="n">
-        <v>2203.0</v>
+        <v>4417.0</v>
       </c>
       <c r="E45" t="n">
-        <v>2203.0</v>
+        <v>4473.0</v>
       </c>
       <c r="F45" t="n">
-        <v>146.0</v>
+        <v>2625.0</v>
       </c>
       <c r="G45" t="n">
-        <v>71.0</v>
+        <v>2570.0</v>
       </c>
       <c r="H45" t="n">
-        <v>256.0</v>
+        <v>7170.0</v>
       </c>
       <c r="I45" t="n">
-        <v>68.0</v>
+        <v>1372.0</v>
       </c>
       <c r="J45" t="n">
-        <v>0.0</v>
+        <v>3495.0</v>
       </c>
       <c r="K45" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="L45" t="n">
-        <v>0.0</v>
+        <v>106.0</v>
       </c>
       <c r="M45" t="n">
-        <v>0.0</v>
+        <v>144.0</v>
       </c>
       <c r="N45" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="O45" t="n">
-        <v>58.0</v>
+        <v>113.0</v>
       </c>
       <c r="P45" t="n">
-        <v>30.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q45" t="n">
-        <v>824.0</v>
+        <v>48464.0</v>
       </c>
       <c r="R45" t="n">
-        <v>0.0</v>
+        <v>29.0</v>
       </c>
       <c r="S45" t="n">
-        <v>0.0</v>
+        <v>36645.0</v>
       </c>
       <c r="T45" t="s">
         <v>130</v>
       </c>
-      <c r="U45" t="n" s="2">
-        <v>43376.0</v>
-      </c>
-      <c r="V45" t="n">
-        <v>27.0</v>
+      <c r="U45" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="V45" t="n" s="2">
+        <v>43390.0</v>
       </c>
     </row>
     <row r="46">
@@ -3524,67 +3530,67 @@
         <v>66</v>
       </c>
       <c r="B46" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C46" t="n">
-        <v>12.0</v>
+        <v>7.0</v>
       </c>
       <c r="D46" t="n">
-        <v>4506.0</v>
+        <v>2229.0</v>
       </c>
       <c r="E46" t="n">
-        <v>4829.0</v>
+        <v>2297.0</v>
       </c>
       <c r="F46" t="n">
-        <v>10666.0</v>
+        <v>150.0</v>
       </c>
       <c r="G46" t="n">
-        <v>11383.0</v>
+        <v>75.0</v>
       </c>
       <c r="H46" t="n">
-        <v>25450.0</v>
+        <v>265.0</v>
       </c>
       <c r="I46" t="n">
-        <v>8774.0</v>
+        <v>70.0</v>
       </c>
       <c r="J46" t="n">
-        <v>2193.0</v>
+        <v>0.0</v>
       </c>
       <c r="K46" t="n">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="L46" t="n">
         <v>0.0</v>
       </c>
       <c r="M46" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="N46" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="O46" t="n">
-        <v>124.0</v>
+        <v>101.0</v>
       </c>
       <c r="P46" t="n">
-        <v>120.0</v>
+        <v>90.0</v>
       </c>
       <c r="Q46" t="n">
-        <v>72595.0</v>
+        <v>867.0</v>
       </c>
       <c r="R46" t="n">
-        <v>19.0</v>
+        <v>0.0</v>
       </c>
       <c r="S46" t="n">
-        <v>74510.0</v>
+        <v>0.0</v>
       </c>
       <c r="T46" t="s">
-        <v>128</v>
-      </c>
-      <c r="U46" t="n" s="2">
-        <v>43390.0</v>
-      </c>
-      <c r="V46" t="n">
-        <v>13.0</v>
+        <v>132</v>
+      </c>
+      <c r="U46" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="V46" t="n" s="2">
+        <v>43376.0</v>
       </c>
     </row>
     <row r="47">
@@ -3592,67 +3598,67 @@
         <v>67</v>
       </c>
       <c r="B47" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C47" t="n">
         <v>12.0</v>
       </c>
       <c r="D47" t="n">
-        <v>4059.0</v>
+        <v>4529.0</v>
       </c>
       <c r="E47" t="n">
-        <v>4059.0</v>
+        <v>4829.0</v>
       </c>
       <c r="F47" t="n">
-        <v>3009.0</v>
+        <v>10687.0</v>
       </c>
       <c r="G47" t="n">
-        <v>3025.0</v>
+        <v>11404.0</v>
       </c>
       <c r="H47" t="n">
-        <v>15298.0</v>
+        <v>25495.0</v>
       </c>
       <c r="I47" t="n">
-        <v>3251.0</v>
+        <v>8788.0</v>
       </c>
       <c r="J47" t="n">
-        <v>1884.0</v>
+        <v>2193.0</v>
       </c>
       <c r="K47" t="n">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="L47" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M47" t="n">
         <v>4.0</v>
       </c>
-      <c r="M47" t="n">
-        <v>26.0</v>
-      </c>
       <c r="N47" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="O47" t="n">
-        <v>158.0</v>
+        <v>330.0</v>
       </c>
       <c r="P47" t="n">
-        <v>160.0</v>
+        <v>240.0</v>
       </c>
       <c r="Q47" t="n">
-        <v>31978.0</v>
+        <v>72801.0</v>
       </c>
       <c r="R47" t="n">
-        <v>34.0</v>
+        <v>19.0</v>
       </c>
       <c r="S47" t="n">
-        <v>61615.0</v>
+        <v>75070.0</v>
       </c>
       <c r="T47" t="s">
-        <v>125</v>
-      </c>
-      <c r="U47" t="n" s="2">
-        <v>43230.0</v>
-      </c>
-      <c r="V47" t="n">
-        <v>173.0</v>
+        <v>130</v>
+      </c>
+      <c r="U47" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="V47" t="n" s="2">
+        <v>43390.0</v>
       </c>
     </row>
     <row r="48">
@@ -3660,67 +3666,67 @@
         <v>68</v>
       </c>
       <c r="B48" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C48" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="D48" t="n">
+        <v>4059.0</v>
+      </c>
+      <c r="E48" t="n">
+        <v>4059.0</v>
+      </c>
+      <c r="F48" t="n">
+        <v>3010.0</v>
+      </c>
+      <c r="G48" t="n">
+        <v>3026.0</v>
+      </c>
+      <c r="H48" t="n">
+        <v>15316.0</v>
+      </c>
+      <c r="I48" t="n">
+        <v>3254.0</v>
+      </c>
+      <c r="J48" t="n">
+        <v>1884.0</v>
+      </c>
+      <c r="K48" t="n">
         <v>11.0</v>
       </c>
-      <c r="D48" t="n">
-        <v>4100.0</v>
-      </c>
-      <c r="E48" t="n">
-        <v>4304.0</v>
-      </c>
-      <c r="F48" t="n">
-        <v>6322.0</v>
-      </c>
-      <c r="G48" t="n">
-        <v>6576.0</v>
-      </c>
-      <c r="H48" t="n">
-        <v>18078.0</v>
-      </c>
-      <c r="I48" t="n">
-        <v>3744.0</v>
-      </c>
-      <c r="J48" t="n">
-        <v>4356.0</v>
-      </c>
-      <c r="K48" t="n">
-        <v>10.0</v>
-      </c>
       <c r="L48" t="n">
-        <v>47.0</v>
+        <v>4.0</v>
       </c>
       <c r="M48" t="n">
-        <v>459.0</v>
+        <v>26.0</v>
       </c>
       <c r="N48" t="s">
         <v>122</v>
       </c>
       <c r="O48" t="n">
-        <v>63.0</v>
+        <v>216.0</v>
       </c>
       <c r="P48" t="n">
-        <v>80.0</v>
+        <v>280.0</v>
       </c>
       <c r="Q48" t="n">
-        <v>20515.0</v>
+        <v>32036.0</v>
       </c>
       <c r="R48" t="n">
-        <v>55.0</v>
+        <v>34.0</v>
       </c>
       <c r="S48" t="n">
-        <v>69037.0</v>
+        <v>61615.0</v>
       </c>
       <c r="T48" t="s">
-        <v>125</v>
-      </c>
-      <c r="U48" t="n" s="2">
-        <v>43184.0</v>
-      </c>
-      <c r="V48" t="n">
-        <v>219.0</v>
+        <v>127</v>
+      </c>
+      <c r="U48" t="n">
+        <v>174.0</v>
+      </c>
+      <c r="V48" t="n" s="2">
+        <v>43230.0</v>
       </c>
     </row>
     <row r="49">
@@ -3728,67 +3734,67 @@
         <v>69</v>
       </c>
       <c r="B49" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C49" t="n">
-        <v>12.0</v>
+        <v>11.0</v>
       </c>
       <c r="D49" t="n">
-        <v>4214.0</v>
+        <v>4105.0</v>
       </c>
       <c r="E49" t="n">
-        <v>4619.0</v>
+        <v>4304.0</v>
       </c>
       <c r="F49" t="n">
-        <v>6320.0</v>
+        <v>6324.0</v>
       </c>
       <c r="G49" t="n">
-        <v>6116.0</v>
+        <v>6578.0</v>
       </c>
       <c r="H49" t="n">
-        <v>13956.0</v>
+        <v>18088.0</v>
       </c>
       <c r="I49" t="n">
-        <v>2639.0</v>
+        <v>3745.0</v>
       </c>
       <c r="J49" t="n">
-        <v>6499.0</v>
+        <v>4356.0</v>
       </c>
       <c r="K49" t="n">
         <v>10.0</v>
       </c>
       <c r="L49" t="n">
-        <v>60.0</v>
+        <v>47.0</v>
       </c>
       <c r="M49" t="n">
-        <v>93.0</v>
+        <v>459.0</v>
       </c>
       <c r="N49" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="O49" t="n">
-        <v>0.0</v>
+        <v>71.0</v>
       </c>
       <c r="P49" t="n">
-        <v>40.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q49" t="n">
-        <v>46865.0</v>
+        <v>20523.0</v>
       </c>
       <c r="R49" t="n">
-        <v>26.0</v>
+        <v>55.0</v>
       </c>
       <c r="S49" t="n">
-        <v>37560.0</v>
+        <v>70437.0</v>
       </c>
       <c r="T49" t="s">
-        <v>125</v>
-      </c>
-      <c r="U49" t="n" s="2">
-        <v>43314.0</v>
-      </c>
-      <c r="V49" t="n">
-        <v>89.0</v>
+        <v>127</v>
+      </c>
+      <c r="U49" t="n">
+        <v>220.0</v>
+      </c>
+      <c r="V49" t="n" s="2">
+        <v>43184.0</v>
       </c>
     </row>
     <row r="50">
@@ -3796,67 +3802,135 @@
         <v>70</v>
       </c>
       <c r="B50" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C50" t="n">
-        <v>10.0</v>
+        <v>12.0</v>
       </c>
       <c r="D50" t="n">
-        <v>3901.0</v>
+        <v>4214.0</v>
       </c>
       <c r="E50" t="n">
-        <v>3901.0</v>
+        <v>4619.0</v>
       </c>
       <c r="F50" t="n">
-        <v>853.0</v>
+        <v>6320.0</v>
       </c>
       <c r="G50" t="n">
-        <v>729.0</v>
+        <v>6116.0</v>
       </c>
       <c r="H50" t="n">
-        <v>3866.0</v>
+        <v>13956.0</v>
       </c>
       <c r="I50" t="n">
-        <v>892.0</v>
+        <v>2639.0</v>
       </c>
       <c r="J50" t="n">
-        <v>533.0</v>
+        <v>6499.0</v>
       </c>
       <c r="K50" t="n">
         <v>10.0</v>
       </c>
       <c r="L50" t="n">
-        <v>0.0</v>
+        <v>60.0</v>
       </c>
       <c r="M50" t="n">
-        <v>0.0</v>
+        <v>93.0</v>
       </c>
       <c r="N50" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="O50" t="n">
-        <v>48.0</v>
+        <v>0.0</v>
       </c>
       <c r="P50" t="n">
         <v>40.0</v>
       </c>
       <c r="Q50" t="n">
-        <v>24290.0</v>
+        <v>46865.0</v>
       </c>
       <c r="R50" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="S50" t="n">
+        <v>37560.0</v>
+      </c>
+      <c r="T50" t="s">
+        <v>127</v>
+      </c>
+      <c r="U50" t="n">
+        <v>90.0</v>
+      </c>
+      <c r="V50" t="n" s="2">
+        <v>43314.0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>71</v>
+      </c>
+      <c r="B51" t="s">
+        <v>121</v>
+      </c>
+      <c r="C51" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="D51" t="n">
+        <v>3901.0</v>
+      </c>
+      <c r="E51" t="n">
+        <v>3901.0</v>
+      </c>
+      <c r="F51" t="n">
+        <v>853.0</v>
+      </c>
+      <c r="G51" t="n">
+        <v>729.0</v>
+      </c>
+      <c r="H51" t="n">
+        <v>3867.0</v>
+      </c>
+      <c r="I51" t="n">
+        <v>892.0</v>
+      </c>
+      <c r="J51" t="n">
+        <v>533.0</v>
+      </c>
+      <c r="K51" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="L51" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M51" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N51" t="s">
+        <v>123</v>
+      </c>
+      <c r="O51" t="n">
+        <v>78.0</v>
+      </c>
+      <c r="P51" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="Q51" t="n">
+        <v>24320.0</v>
+      </c>
+      <c r="R51" t="n">
         <v>15.0</v>
       </c>
-      <c r="S50" t="n">
+      <c r="S51" t="n">
         <v>13894.0</v>
       </c>
-      <c r="T50" t="s">
-        <v>126</v>
-      </c>
-      <c r="U50" t="n" s="2">
+      <c r="T51" t="s">
+        <v>129</v>
+      </c>
+      <c r="U51" t="n">
+        <v>150.0</v>
+      </c>
+      <c r="V51" t="n" s="2">
         <v>43254.0</v>
-      </c>
-      <c r="V50" t="n">
-        <v>149.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Evolution map: first version
</commit_message>
<xml_diff>
--- a/docs/data/memberstats.xlsx
+++ b/docs/data/memberstats.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="131">
   <si>
     <t>tag</t>
   </si>
@@ -80,331 +80,328 @@
     <t>age</t>
   </si>
   <si>
+    <t>#200CGV9QP</t>
+  </si>
+  <si>
+    <t>#208LL8JU</t>
+  </si>
+  <si>
+    <t>#20LPVLY9J</t>
+  </si>
+  <si>
+    <t>#28QLVJ00U</t>
+  </si>
+  <si>
+    <t>#28VVQUJ</t>
+  </si>
+  <si>
+    <t>#28VY80Q2Q</t>
+  </si>
+  <si>
+    <t>#2C9Y02QGJ</t>
+  </si>
+  <si>
+    <t>#2CQLJCV8R</t>
+  </si>
+  <si>
+    <t>#2G8QRCQJQ</t>
+  </si>
+  <si>
+    <t>#2G8YCGGUL</t>
+  </si>
+  <si>
+    <t>#2GP9VYY98</t>
+  </si>
+  <si>
+    <t>#2J2PPYGLC</t>
+  </si>
+  <si>
+    <t>#2JU82PCJ</t>
+  </si>
+  <si>
+    <t>#2L90UUCCY</t>
+  </si>
+  <si>
+    <t>#2PGU9R00C</t>
+  </si>
+  <si>
+    <t>#2PUJ8JLGJ</t>
+  </si>
+  <si>
+    <t>#2Q9PULLCQ</t>
+  </si>
+  <si>
+    <t>#2R8V8PPR</t>
+  </si>
+  <si>
+    <t>#2UVYQPG2J</t>
+  </si>
+  <si>
+    <t>#2V80YRPPV</t>
+  </si>
+  <si>
+    <t>#2VG98LGRL</t>
+  </si>
+  <si>
+    <t>#2VLYP9PP8</t>
+  </si>
+  <si>
+    <t>#2VQPQJGCU</t>
+  </si>
+  <si>
+    <t>#80URYGRY8</t>
+  </si>
+  <si>
+    <t>#828L2V0QV</t>
+  </si>
+  <si>
+    <t>#828Q2QRQ</t>
+  </si>
+  <si>
+    <t>#82R099R2Y</t>
+  </si>
+  <si>
+    <t>#89RYPQL0G</t>
+  </si>
+  <si>
+    <t>#8J9QYYPY8</t>
+  </si>
+  <si>
+    <t>#8R8VUC8G</t>
+  </si>
+  <si>
+    <t>#8RR920URY</t>
+  </si>
+  <si>
+    <t>#92GRP8YP8</t>
+  </si>
+  <si>
+    <t>#98RGLLP2V</t>
+  </si>
+  <si>
+    <t>#99JULCPYJ</t>
+  </si>
+  <si>
+    <t>#9CVC8RJRL</t>
+  </si>
+  <si>
+    <t>#9LU9PL9V0</t>
+  </si>
+  <si>
+    <t>#9R2VQVG0J</t>
+  </si>
+  <si>
+    <t>#9ULVGQLC</t>
+  </si>
+  <si>
+    <t>#CP8RJ000</t>
+  </si>
+  <si>
+    <t>#G82QPLV8</t>
+  </si>
+  <si>
+    <t>#GYUPYYL</t>
+  </si>
+  <si>
+    <t>#L8RYLJRC</t>
+  </si>
+  <si>
+    <t>#LGURPQV8</t>
+  </si>
+  <si>
+    <t>#P0YVL928U</t>
+  </si>
+  <si>
     <t>#QP0RYPG2</t>
   </si>
   <si>
-    <t>#2UVYQPG2J</t>
-  </si>
-  <si>
-    <t>#2GP9VYY98</t>
-  </si>
-  <si>
-    <t>#8RR920URY</t>
-  </si>
-  <si>
-    <t>#CP8RJ000</t>
-  </si>
-  <si>
-    <t>#828Q2QRQ</t>
-  </si>
-  <si>
-    <t>#2G8YCGGUL</t>
-  </si>
-  <si>
-    <t>#200CGV9QP</t>
-  </si>
-  <si>
-    <t>#28VY80Q2Q</t>
-  </si>
-  <si>
-    <t>#2C9Y02QGJ</t>
-  </si>
-  <si>
-    <t>#2JU82PCJ</t>
+    <t>#R9VJL9YQ</t>
+  </si>
+  <si>
+    <t>#RCQ99GPJ</t>
   </si>
   <si>
     <t>#VP0YL88</t>
   </si>
   <si>
-    <t>#828L2V0QV</t>
-  </si>
-  <si>
-    <t>#2CQLJCV8R</t>
-  </si>
-  <si>
-    <t>#2R8V8PPR</t>
-  </si>
-  <si>
-    <t>#L8RYLJRC</t>
-  </si>
-  <si>
-    <t>#9R2VQVG0J</t>
-  </si>
-  <si>
-    <t>#2VQPQJGCU</t>
-  </si>
-  <si>
-    <t>#G82QPLV8</t>
-  </si>
-  <si>
-    <t>#2PGU9R00C</t>
-  </si>
-  <si>
-    <t>#RCQ99GPJ</t>
-  </si>
-  <si>
-    <t>#R9VJL9YQ</t>
-  </si>
-  <si>
-    <t>#89RYPQL0G</t>
-  </si>
-  <si>
-    <t>#2VG98LGRL</t>
-  </si>
-  <si>
-    <t>#LGURPQV8</t>
-  </si>
-  <si>
-    <t>#2Q9PULLCQ</t>
-  </si>
-  <si>
-    <t>#9ULVGQLC</t>
-  </si>
-  <si>
-    <t>#2VLYP9PP8</t>
-  </si>
-  <si>
-    <t>#2L90UUCCY</t>
-  </si>
-  <si>
-    <t>#GYUPYYL</t>
-  </si>
-  <si>
-    <t>#20LPVLY9J</t>
-  </si>
-  <si>
-    <t>#8R8VUC8G</t>
-  </si>
-  <si>
-    <t>#82R099R2Y</t>
-  </si>
-  <si>
-    <t>#208LL8JU</t>
-  </si>
-  <si>
-    <t>#2J2PPYGLC</t>
-  </si>
-  <si>
-    <t>#2PUJ8JLGJ</t>
-  </si>
-  <si>
-    <t>#28VVQUJ</t>
-  </si>
-  <si>
-    <t>#8J9QYYPY8</t>
-  </si>
-  <si>
-    <t>#98RGLLP2V</t>
-  </si>
-  <si>
     <t>#YQLCCYY2</t>
   </si>
   <si>
-    <t>#9CVC8RJRL</t>
-  </si>
-  <si>
-    <t>#80URYGRY8</t>
-  </si>
-  <si>
-    <t>#28QLVJ00U</t>
-  </si>
-  <si>
-    <t>#99JULCPYJ</t>
-  </si>
-  <si>
-    <t>#2G8QRCQJQ</t>
-  </si>
-  <si>
-    <t>#9LU9PL9V0</t>
-  </si>
-  <si>
-    <t>#92GRP8YP8</t>
-  </si>
-  <si>
-    <t>#2V80YRPPV</t>
-  </si>
-  <si>
-    <t>#P0YVL928U</t>
+    <t>zau</t>
+  </si>
+  <si>
+    <t>Pikaya</t>
+  </si>
+  <si>
+    <t>KryptoNnN</t>
+  </si>
+  <si>
+    <t>NOVA I MIGUEL☉</t>
+  </si>
+  <si>
+    <t>fglopes</t>
+  </si>
+  <si>
+    <t>TheKingJK</t>
+  </si>
+  <si>
+    <t>pjp</t>
+  </si>
+  <si>
+    <t>mounir</t>
+  </si>
+  <si>
+    <t>Doomesticador</t>
+  </si>
+  <si>
+    <t>Goblyn</t>
+  </si>
+  <si>
+    <t>Tabo da amarela</t>
+  </si>
+  <si>
+    <t>pedro</t>
+  </si>
+  <si>
+    <t>☆ Di♡g♡</t>
+  </si>
+  <si>
+    <t>Matilde Pires</t>
+  </si>
+  <si>
+    <t>Wut</t>
+  </si>
+  <si>
+    <t>supercell</t>
+  </si>
+  <si>
+    <t>Madnasty</t>
+  </si>
+  <si>
+    <t>unb</t>
+  </si>
+  <si>
+    <t>bascenso</t>
+  </si>
+  <si>
+    <t>Manu</t>
+  </si>
+  <si>
+    <t>Sra. Clash</t>
+  </si>
+  <si>
+    <t>YOSHINZ</t>
+  </si>
+  <si>
+    <t>thunder</t>
+  </si>
+  <si>
+    <t>Jonas 705</t>
+  </si>
+  <si>
+    <t>Fabíola</t>
+  </si>
+  <si>
+    <t>King Bonixe</t>
+  </si>
+  <si>
+    <t>Robb Stark</t>
+  </si>
+  <si>
+    <t>snowkids</t>
+  </si>
+  <si>
+    <t>Ricky</t>
+  </si>
+  <si>
+    <t>qzt</t>
+  </si>
+  <si>
+    <t>filipe</t>
+  </si>
+  <si>
+    <t>SELFIE</t>
+  </si>
+  <si>
+    <t>carmen</t>
+  </si>
+  <si>
+    <t>metamox</t>
+  </si>
+  <si>
+    <t>faneca</t>
+  </si>
+  <si>
+    <t>MASTER PT</t>
+  </si>
+  <si>
+    <t>John Rambo</t>
+  </si>
+  <si>
+    <t>Welton</t>
+  </si>
+  <si>
+    <t>leal</t>
+  </si>
+  <si>
+    <t>Sergas</t>
+  </si>
+  <si>
+    <t>Savler</t>
+  </si>
+  <si>
+    <t>hugo</t>
+  </si>
+  <si>
+    <t>Marcelo</t>
+  </si>
+  <si>
+    <t>EBAERV_</t>
   </si>
   <si>
     <t>LCINORC</t>
   </si>
   <si>
-    <t>bascenso</t>
-  </si>
-  <si>
-    <t>Tabo da amarela</t>
-  </si>
-  <si>
-    <t>filipe</t>
-  </si>
-  <si>
-    <t>leal</t>
-  </si>
-  <si>
-    <t>King Bonixe</t>
-  </si>
-  <si>
-    <t>Goblyn</t>
-  </si>
-  <si>
-    <t>zau</t>
-  </si>
-  <si>
-    <t>TheKingJK</t>
-  </si>
-  <si>
-    <t>pjp</t>
-  </si>
-  <si>
-    <t>☆ Di♡g♡</t>
+    <t>Tio João</t>
+  </si>
+  <si>
+    <t>Inferno</t>
   </si>
   <si>
     <t>topdosl33ts</t>
   </si>
   <si>
-    <t>Fabíola</t>
-  </si>
-  <si>
-    <t>mounir</t>
-  </si>
-  <si>
-    <t>unb</t>
-  </si>
-  <si>
-    <t>hugo</t>
-  </si>
-  <si>
-    <t>John Rambo</t>
-  </si>
-  <si>
-    <t>thunder</t>
-  </si>
-  <si>
-    <t>Sergas</t>
-  </si>
-  <si>
-    <t>Wut</t>
-  </si>
-  <si>
-    <t>Inferno</t>
-  </si>
-  <si>
-    <t>Tio João</t>
-  </si>
-  <si>
-    <t>snowkids</t>
-  </si>
-  <si>
-    <t>Sra. Clash</t>
-  </si>
-  <si>
-    <t>Marcelo</t>
-  </si>
-  <si>
-    <t>Madnasty</t>
-  </si>
-  <si>
-    <t>Welton</t>
-  </si>
-  <si>
-    <t>YOSHINZ</t>
-  </si>
-  <si>
-    <t>Matilde Pires</t>
-  </si>
-  <si>
-    <t>Savler</t>
-  </si>
-  <si>
-    <t>KryptoNnN</t>
-  </si>
-  <si>
-    <t>qzt</t>
-  </si>
-  <si>
-    <t>Robb Stark</t>
-  </si>
-  <si>
-    <t>Pikaya</t>
-  </si>
-  <si>
-    <t>pedro</t>
-  </si>
-  <si>
-    <t>supercell</t>
-  </si>
-  <si>
-    <t>fglopes</t>
-  </si>
-  <si>
-    <t>Ricky</t>
-  </si>
-  <si>
-    <t>carmen</t>
-  </si>
-  <si>
     <t>Bruno Lopez</t>
   </si>
   <si>
-    <t>faneca</t>
-  </si>
-  <si>
-    <t>Jonas 705</t>
-  </si>
-  <si>
-    <t>NOVA I MIGUEL☉</t>
-  </si>
-  <si>
-    <t>metamox</t>
-  </si>
-  <si>
-    <t>Doomesticador</t>
-  </si>
-  <si>
-    <t>MASTER PT</t>
-  </si>
-  <si>
-    <t>SELFIE</t>
-  </si>
-  <si>
-    <t>Manu</t>
-  </si>
-  <si>
-    <t>EBAERV_</t>
+    <t>elder</t>
   </si>
   <si>
     <t>member</t>
   </si>
   <si>
+    <t>coLeader</t>
+  </si>
+  <si>
     <t>leader</t>
   </si>
   <si>
-    <t>elder</t>
-  </si>
-  <si>
-    <t>coLeader</t>
-  </si>
-  <si>
-    <t>League 4</t>
+    <t>League 1</t>
+  </si>
+  <si>
+    <t>Arena 11</t>
+  </si>
+  <si>
+    <t>Arena 12</t>
   </si>
   <si>
     <t>League 2</t>
   </si>
   <si>
-    <t>League 1</t>
-  </si>
-  <si>
-    <t>Arena 12</t>
-  </si>
-  <si>
-    <t>Arena 11</t>
+    <t>Arena 9</t>
   </si>
   <si>
     <t>Arena 10</t>
-  </si>
-  <si>
-    <t>Arena 9</t>
   </si>
   <si>
     <t>Arena 7</t>
@@ -538,64 +535,64 @@
         <v>71</v>
       </c>
       <c r="C2" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>4270.0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>4653.0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>2227.0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>2074.0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>6970.0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1146.0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>2664.0</v>
+      </c>
+      <c r="K2" t="n">
         <v>12.0</v>
       </c>
-      <c r="D2" t="n">
-        <v>4919.0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>4919.0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>10796.0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>11504.0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>25742.0</v>
-      </c>
-      <c r="I2" t="n">
-        <v>8871.0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>2205.0</v>
-      </c>
-      <c r="K2" t="n">
-        <v>10.0</v>
-      </c>
       <c r="L2" t="n">
         <v>0.0</v>
       </c>
       <c r="M2" t="n">
-        <v>4.0</v>
+        <v>7.0</v>
       </c>
       <c r="N2" t="s">
         <v>120</v>
       </c>
       <c r="O2" t="n">
-        <v>94.0</v>
+        <v>132.0</v>
       </c>
       <c r="P2" t="n">
-        <v>20.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q2" t="n">
-        <v>73770.0</v>
+        <v>27482.0</v>
       </c>
       <c r="R2" t="n">
-        <v>20.0</v>
+        <v>41.0</v>
       </c>
       <c r="S2" t="n">
-        <v>77870.0</v>
+        <v>78380.0</v>
       </c>
       <c r="T2" t="s">
         <v>124</v>
       </c>
       <c r="U2" t="n" s="2">
-        <v>43390.0</v>
+        <v>43302.0</v>
       </c>
       <c r="V2" t="n">
-        <v>19.0</v>
+        <v>107.0</v>
       </c>
     </row>
     <row r="3">
@@ -606,64 +603,64 @@
         <v>72</v>
       </c>
       <c r="C3" t="n">
-        <v>12.0</v>
+        <v>10.0</v>
       </c>
       <c r="D3" t="n">
-        <v>4359.0</v>
+        <v>4023.0</v>
       </c>
       <c r="E3" t="n">
-        <v>4767.0</v>
+        <v>4077.0</v>
       </c>
       <c r="F3" t="n">
-        <v>6660.0</v>
+        <v>1648.0</v>
       </c>
       <c r="G3" t="n">
-        <v>6615.0</v>
+        <v>1431.0</v>
       </c>
       <c r="H3" t="n">
-        <v>23463.0</v>
+        <v>4285.0</v>
       </c>
       <c r="I3" t="n">
-        <v>2753.0</v>
+        <v>827.0</v>
       </c>
       <c r="J3" t="n">
-        <v>2570.0</v>
+        <v>2400.0</v>
       </c>
       <c r="K3" t="n">
         <v>10.0</v>
       </c>
       <c r="L3" t="n">
-        <v>433.0</v>
+        <v>0.0</v>
       </c>
       <c r="M3" t="n">
-        <v>2512.0</v>
+        <v>2.0</v>
       </c>
       <c r="N3" t="s">
         <v>121</v>
       </c>
       <c r="O3" t="n">
-        <v>36.0</v>
+        <v>0.0</v>
       </c>
       <c r="P3" t="n">
-        <v>40.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q3" t="n">
-        <v>66965.0</v>
+        <v>17819.0</v>
       </c>
       <c r="R3" t="n">
-        <v>85.0</v>
+        <v>14.0</v>
       </c>
       <c r="S3" t="n">
-        <v>79935.0</v>
+        <v>26960.0</v>
       </c>
       <c r="T3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U3" t="n" s="2">
-        <v>42705.0</v>
+        <v>43372.0</v>
       </c>
       <c r="V3" t="n">
-        <v>704.0</v>
+        <v>37.0</v>
       </c>
     </row>
     <row r="4">
@@ -674,64 +671,64 @@
         <v>73</v>
       </c>
       <c r="C4" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>4148.0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>4254.0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2570.0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2613.0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>6173.0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1063.0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1649.0</v>
+      </c>
+      <c r="K4" t="n">
         <v>12.0</v>
       </c>
-      <c r="D4" t="n">
-        <v>4353.0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>4731.0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>2237.0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>1752.0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>9362.0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>1358.0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>4199.0</v>
-      </c>
-      <c r="K4" t="n">
-        <v>10.0</v>
-      </c>
       <c r="L4" t="n">
         <v>0.0</v>
       </c>
       <c r="M4" t="n">
-        <v>7.0</v>
+        <v>9.0</v>
       </c>
       <c r="N4" t="s">
         <v>120</v>
       </c>
       <c r="O4" t="n">
-        <v>80.0</v>
+        <v>0.0</v>
       </c>
       <c r="P4" t="n">
         <v>40.0</v>
       </c>
       <c r="Q4" t="n">
-        <v>88477.0</v>
+        <v>8910.0</v>
       </c>
       <c r="R4" t="n">
-        <v>72.0</v>
+        <v>41.0</v>
       </c>
       <c r="S4" t="n">
-        <v>70640.0</v>
+        <v>57166.0</v>
       </c>
       <c r="T4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U4" t="n" s="2">
-        <v>43397.0</v>
+        <v>43082.0</v>
       </c>
       <c r="V4" t="n">
-        <v>12.0</v>
+        <v>327.0</v>
       </c>
     </row>
     <row r="5">
@@ -742,64 +739,64 @@
         <v>74</v>
       </c>
       <c r="C5" t="n">
-        <v>12.0</v>
+        <v>10.0</v>
       </c>
       <c r="D5" t="n">
-        <v>4351.0</v>
+        <v>3640.0</v>
       </c>
       <c r="E5" t="n">
-        <v>4798.0</v>
+        <v>3764.0</v>
       </c>
       <c r="F5" t="n">
-        <v>5098.0</v>
+        <v>694.0</v>
       </c>
       <c r="G5" t="n">
-        <v>5211.0</v>
+        <v>644.0</v>
       </c>
       <c r="H5" t="n">
-        <v>12231.0</v>
+        <v>1958.0</v>
       </c>
       <c r="I5" t="n">
-        <v>2230.0</v>
+        <v>381.0</v>
       </c>
       <c r="J5" t="n">
-        <v>1728.0</v>
+        <v>1428.0</v>
       </c>
       <c r="K5" t="n">
         <v>10.0</v>
       </c>
       <c r="L5" t="n">
-        <v>31.0</v>
+        <v>0.0</v>
       </c>
       <c r="M5" t="n">
-        <v>43.0</v>
+        <v>4.0</v>
       </c>
       <c r="N5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O5" t="n">
-        <v>86.0</v>
+        <v>80.0</v>
       </c>
       <c r="P5" t="n">
         <v>40.0</v>
       </c>
       <c r="Q5" t="n">
-        <v>58823.0</v>
+        <v>16416.0</v>
       </c>
       <c r="R5" t="n">
-        <v>30.0</v>
+        <v>4.0</v>
       </c>
       <c r="S5" t="n">
-        <v>74870.0</v>
+        <v>8680.0</v>
       </c>
       <c r="T5" t="s">
         <v>125</v>
       </c>
       <c r="U5" t="n" s="2">
-        <v>43058.0</v>
+        <v>43397.0</v>
       </c>
       <c r="V5" t="n">
-        <v>351.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="6">
@@ -810,31 +807,31 @@
         <v>75</v>
       </c>
       <c r="C6" t="n">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="D6" t="n">
-        <v>4306.0</v>
+        <v>3956.0</v>
       </c>
       <c r="E6" t="n">
-        <v>4553.0</v>
+        <v>4142.0</v>
       </c>
       <c r="F6" t="n">
-        <v>4635.0</v>
+        <v>1221.0</v>
       </c>
       <c r="G6" t="n">
-        <v>4693.0</v>
+        <v>1252.0</v>
       </c>
       <c r="H6" t="n">
-        <v>26509.0</v>
+        <v>3143.0</v>
       </c>
       <c r="I6" t="n">
-        <v>3609.0</v>
+        <v>496.0</v>
       </c>
       <c r="J6" t="n">
-        <v>2006.0</v>
+        <v>310.0</v>
       </c>
       <c r="K6" t="n">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="L6" t="n">
         <v>0.0</v>
@@ -843,31 +840,31 @@
         <v>0.0</v>
       </c>
       <c r="N6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O6" t="n">
-        <v>0.0</v>
+        <v>122.0</v>
       </c>
       <c r="P6" t="n">
-        <v>40.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q6" t="n">
-        <v>7112.0</v>
+        <v>15380.0</v>
       </c>
       <c r="R6" t="n">
-        <v>57.0</v>
+        <v>28.0</v>
       </c>
       <c r="S6" t="n">
-        <v>69835.0</v>
+        <v>38427.0</v>
       </c>
       <c r="T6" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="U6" t="n" s="2">
-        <v>43252.0</v>
+        <v>43356.0</v>
       </c>
       <c r="V6" t="n">
-        <v>157.0</v>
+        <v>53.0</v>
       </c>
     </row>
     <row r="7">
@@ -878,64 +875,64 @@
         <v>76</v>
       </c>
       <c r="C7" t="n">
-        <v>12.0</v>
+        <v>11.0</v>
       </c>
       <c r="D7" t="n">
-        <v>4304.0</v>
+        <v>4231.0</v>
       </c>
       <c r="E7" t="n">
-        <v>4653.0</v>
+        <v>4489.0</v>
       </c>
       <c r="F7" t="n">
-        <v>3686.0</v>
+        <v>2955.0</v>
       </c>
       <c r="G7" t="n">
-        <v>3405.0</v>
+        <v>2657.0</v>
       </c>
       <c r="H7" t="n">
-        <v>11315.0</v>
+        <v>7007.0</v>
       </c>
       <c r="I7" t="n">
-        <v>1547.0</v>
+        <v>681.0</v>
       </c>
       <c r="J7" t="n">
-        <v>3040.0</v>
+        <v>4151.0</v>
       </c>
       <c r="K7" t="n">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="L7" t="n">
-        <v>100.0</v>
+        <v>52.0</v>
       </c>
       <c r="M7" t="n">
-        <v>195.0</v>
+        <v>166.0</v>
       </c>
       <c r="N7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="O7" t="n">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="P7" t="n">
         <v>40.0</v>
       </c>
       <c r="Q7" t="n">
-        <v>32533.0</v>
+        <v>2125.0</v>
       </c>
       <c r="R7" t="n">
-        <v>59.0</v>
+        <v>38.0</v>
       </c>
       <c r="S7" t="n">
-        <v>72275.0</v>
+        <v>53720.0</v>
       </c>
       <c r="T7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U7" t="n" s="2">
-        <v>42614.0</v>
+        <v>43364.0</v>
       </c>
       <c r="V7" t="n">
-        <v>795.0</v>
+        <v>45.0</v>
       </c>
     </row>
     <row r="8">
@@ -949,28 +946,28 @@
         <v>11.0</v>
       </c>
       <c r="D8" t="n">
-        <v>4294.0</v>
+        <v>4223.0</v>
       </c>
       <c r="E8" t="n">
-        <v>4501.0</v>
+        <v>4497.0</v>
       </c>
       <c r="F8" t="n">
-        <v>2319.0</v>
+        <v>1894.0</v>
       </c>
       <c r="G8" t="n">
-        <v>2152.0</v>
+        <v>1797.0</v>
       </c>
       <c r="H8" t="n">
-        <v>10499.0</v>
+        <v>7525.0</v>
       </c>
       <c r="I8" t="n">
-        <v>2346.0</v>
+        <v>1110.0</v>
       </c>
       <c r="J8" t="n">
-        <v>1906.0</v>
+        <v>1384.0</v>
       </c>
       <c r="K8" t="n">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="L8" t="n">
         <v>0.0</v>
@@ -979,31 +976,31 @@
         <v>0.0</v>
       </c>
       <c r="N8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O8" t="n">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="P8" t="n">
         <v>40.0</v>
       </c>
       <c r="Q8" t="n">
-        <v>3132.0</v>
+        <v>24903.0</v>
       </c>
       <c r="R8" t="n">
-        <v>54.0</v>
+        <v>55.0</v>
       </c>
       <c r="S8" t="n">
-        <v>75150.0</v>
+        <v>67035.0</v>
       </c>
       <c r="T8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="U8" t="n" s="2">
-        <v>43123.0</v>
+        <v>43058.0</v>
       </c>
       <c r="V8" t="n">
-        <v>286.0</v>
+        <v>351.0</v>
       </c>
     </row>
     <row r="9">
@@ -1017,61 +1014,61 @@
         <v>11.0</v>
       </c>
       <c r="D9" t="n">
-        <v>4270.0</v>
+        <v>4168.0</v>
       </c>
       <c r="E9" t="n">
-        <v>4653.0</v>
+        <v>4496.0</v>
       </c>
       <c r="F9" t="n">
-        <v>2227.0</v>
+        <v>2318.0</v>
       </c>
       <c r="G9" t="n">
-        <v>2074.0</v>
+        <v>2248.0</v>
       </c>
       <c r="H9" t="n">
-        <v>6970.0</v>
+        <v>5101.0</v>
       </c>
       <c r="I9" t="n">
-        <v>1146.0</v>
+        <v>892.0</v>
       </c>
       <c r="J9" t="n">
-        <v>2664.0</v>
+        <v>1622.0</v>
       </c>
       <c r="K9" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="N9" t="s">
+        <v>121</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>24651.0</v>
+      </c>
+      <c r="R9" t="n">
         <v>12.0</v>
       </c>
-      <c r="L9" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M9" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="N9" t="s">
-        <v>122</v>
-      </c>
-      <c r="O9" t="n">
-        <v>114.0</v>
-      </c>
-      <c r="P9" t="n">
-        <v>80.0</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>27464.0</v>
-      </c>
-      <c r="R9" t="n">
-        <v>41.0</v>
-      </c>
       <c r="S9" t="n">
-        <v>78380.0</v>
+        <v>50432.0</v>
       </c>
       <c r="T9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="U9" t="n" s="2">
-        <v>43302.0</v>
+        <v>43390.0</v>
       </c>
       <c r="V9" t="n">
-        <v>107.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="10">
@@ -1085,61 +1082,61 @@
         <v>11.0</v>
       </c>
       <c r="D10" t="n">
-        <v>4231.0</v>
+        <v>3401.0</v>
       </c>
       <c r="E10" t="n">
-        <v>4489.0</v>
+        <v>3656.0</v>
       </c>
       <c r="F10" t="n">
-        <v>2955.0</v>
+        <v>1096.0</v>
       </c>
       <c r="G10" t="n">
-        <v>2657.0</v>
+        <v>1149.0</v>
       </c>
       <c r="H10" t="n">
-        <v>7007.0</v>
+        <v>4621.0</v>
       </c>
       <c r="I10" t="n">
-        <v>681.0</v>
+        <v>1231.0</v>
       </c>
       <c r="J10" t="n">
-        <v>4151.0</v>
+        <v>858.0</v>
       </c>
       <c r="K10" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="L10" t="n">
-        <v>52.0</v>
+        <v>25.0</v>
       </c>
       <c r="M10" t="n">
-        <v>166.0</v>
+        <v>18.0</v>
       </c>
       <c r="N10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O10" t="n">
-        <v>0.0</v>
+        <v>28.0</v>
       </c>
       <c r="P10" t="n">
-        <v>40.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q10" t="n">
-        <v>2125.0</v>
+        <v>28849.0</v>
       </c>
       <c r="R10" t="n">
-        <v>38.0</v>
+        <v>7.0</v>
       </c>
       <c r="S10" t="n">
-        <v>53720.0</v>
+        <v>11970.0</v>
       </c>
       <c r="T10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U10" t="n" s="2">
-        <v>43364.0</v>
+        <v>43123.0</v>
       </c>
       <c r="V10" t="n">
-        <v>45.0</v>
+        <v>286.0</v>
       </c>
     </row>
     <row r="11">
@@ -1153,28 +1150,28 @@
         <v>11.0</v>
       </c>
       <c r="D11" t="n">
-        <v>4223.0</v>
+        <v>4274.0</v>
       </c>
       <c r="E11" t="n">
-        <v>4497.0</v>
+        <v>4501.0</v>
       </c>
       <c r="F11" t="n">
-        <v>1894.0</v>
+        <v>2323.0</v>
       </c>
       <c r="G11" t="n">
-        <v>1797.0</v>
+        <v>2157.0</v>
       </c>
       <c r="H11" t="n">
-        <v>7523.0</v>
+        <v>10508.0</v>
       </c>
       <c r="I11" t="n">
-        <v>1110.0</v>
+        <v>2347.0</v>
       </c>
       <c r="J11" t="n">
-        <v>1384.0</v>
+        <v>1906.0</v>
       </c>
       <c r="K11" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="L11" t="n">
         <v>0.0</v>
@@ -1183,31 +1180,31 @@
         <v>0.0</v>
       </c>
       <c r="N11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O11" t="n">
-        <v>8.0</v>
+        <v>10.0</v>
       </c>
       <c r="P11" t="n">
-        <v>30.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q11" t="n">
-        <v>24903.0</v>
+        <v>3142.0</v>
       </c>
       <c r="R11" t="n">
-        <v>55.0</v>
+        <v>54.0</v>
       </c>
       <c r="S11" t="n">
-        <v>67035.0</v>
+        <v>75150.0</v>
       </c>
       <c r="T11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="U11" t="n" s="2">
-        <v>43058.0</v>
+        <v>43123.0</v>
       </c>
       <c r="V11" t="n">
-        <v>351.0</v>
+        <v>286.0</v>
       </c>
     </row>
     <row r="12">
@@ -1218,64 +1215,64 @@
         <v>81</v>
       </c>
       <c r="C12" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="D12" t="n">
-        <v>4203.0</v>
+        <v>4353.0</v>
       </c>
       <c r="E12" t="n">
-        <v>4389.0</v>
+        <v>4731.0</v>
       </c>
       <c r="F12" t="n">
-        <v>1344.0</v>
+        <v>2237.0</v>
       </c>
       <c r="G12" t="n">
-        <v>1193.0</v>
+        <v>1752.0</v>
       </c>
       <c r="H12" t="n">
-        <v>5460.0</v>
+        <v>9364.0</v>
       </c>
       <c r="I12" t="n">
-        <v>753.0</v>
+        <v>1358.0</v>
       </c>
       <c r="J12" t="n">
-        <v>1199.0</v>
+        <v>4199.0</v>
       </c>
       <c r="K12" t="n">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="L12" t="n">
         <v>0.0</v>
       </c>
       <c r="M12" t="n">
-        <v>11.0</v>
+        <v>7.0</v>
       </c>
       <c r="N12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="O12" t="n">
-        <v>18.0</v>
+        <v>180.0</v>
       </c>
       <c r="P12" t="n">
-        <v>32.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q12" t="n">
-        <v>37227.0</v>
+        <v>88577.0</v>
       </c>
       <c r="R12" t="n">
-        <v>59.0</v>
+        <v>72.0</v>
       </c>
       <c r="S12" t="n">
-        <v>70800.0</v>
+        <v>70640.0</v>
       </c>
       <c r="T12" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="U12" t="n" s="2">
-        <v>43218.0</v>
+        <v>43397.0</v>
       </c>
       <c r="V12" t="n">
-        <v>191.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="13">
@@ -1286,64 +1283,64 @@
         <v>82</v>
       </c>
       <c r="C13" t="n">
-        <v>12.0</v>
+        <v>11.0</v>
       </c>
       <c r="D13" t="n">
-        <v>4181.0</v>
+        <v>3957.0</v>
       </c>
       <c r="E13" t="n">
-        <v>4619.0</v>
+        <v>4163.0</v>
       </c>
       <c r="F13" t="n">
-        <v>6346.0</v>
+        <v>3147.0</v>
       </c>
       <c r="G13" t="n">
-        <v>6138.0</v>
+        <v>3322.0</v>
       </c>
       <c r="H13" t="n">
-        <v>14012.0</v>
+        <v>8557.0</v>
       </c>
       <c r="I13" t="n">
-        <v>2651.0</v>
+        <v>1337.0</v>
       </c>
       <c r="J13" t="n">
-        <v>6501.0</v>
+        <v>1906.0</v>
       </c>
       <c r="K13" t="n">
         <v>10.0</v>
       </c>
       <c r="L13" t="n">
-        <v>60.0</v>
+        <v>0.0</v>
       </c>
       <c r="M13" t="n">
-        <v>93.0</v>
+        <v>0.0</v>
       </c>
       <c r="N13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O13" t="n">
         <v>0.0</v>
       </c>
       <c r="P13" t="n">
-        <v>40.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q13" t="n">
-        <v>46903.0</v>
+        <v>14205.0</v>
       </c>
       <c r="R13" t="n">
-        <v>27.0</v>
+        <v>17.0</v>
       </c>
       <c r="S13" t="n">
-        <v>40920.0</v>
+        <v>27880.0</v>
       </c>
       <c r="T13" t="s">
         <v>126</v>
       </c>
       <c r="U13" t="n" s="2">
-        <v>43314.0</v>
+        <v>43218.0</v>
       </c>
       <c r="V13" t="n">
-        <v>95.0</v>
+        <v>191.0</v>
       </c>
     </row>
     <row r="14">
@@ -1354,64 +1351,64 @@
         <v>83</v>
       </c>
       <c r="C14" t="n">
-        <v>12.0</v>
+        <v>11.0</v>
       </c>
       <c r="D14" t="n">
-        <v>4168.0</v>
+        <v>4203.0</v>
       </c>
       <c r="E14" t="n">
-        <v>4363.0</v>
+        <v>4389.0</v>
       </c>
       <c r="F14" t="n">
-        <v>3290.0</v>
+        <v>1344.0</v>
       </c>
       <c r="G14" t="n">
-        <v>3478.0</v>
+        <v>1193.0</v>
       </c>
       <c r="H14" t="n">
-        <v>12132.0</v>
+        <v>5463.0</v>
       </c>
       <c r="I14" t="n">
-        <v>1677.0</v>
+        <v>753.0</v>
       </c>
       <c r="J14" t="n">
-        <v>2757.0</v>
+        <v>1199.0</v>
       </c>
       <c r="K14" t="n">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="L14" t="n">
         <v>0.0</v>
       </c>
       <c r="M14" t="n">
-        <v>0.0</v>
+        <v>11.0</v>
       </c>
       <c r="N14" t="s">
         <v>122</v>
       </c>
       <c r="O14" t="n">
-        <v>104.0</v>
+        <v>56.0</v>
       </c>
       <c r="P14" t="n">
-        <v>10.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q14" t="n">
-        <v>41404.0</v>
+        <v>37265.0</v>
       </c>
       <c r="R14" t="n">
-        <v>63.0</v>
+        <v>59.0</v>
       </c>
       <c r="S14" t="n">
-        <v>69203.0</v>
+        <v>70800.0</v>
       </c>
       <c r="T14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="U14" t="n" s="2">
-        <v>43214.0</v>
+        <v>43218.0</v>
       </c>
       <c r="V14" t="n">
-        <v>195.0</v>
+        <v>191.0</v>
       </c>
     </row>
     <row r="15">
@@ -1422,58 +1419,58 @@
         <v>84</v>
       </c>
       <c r="C15" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="D15" t="n">
-        <v>4168.0</v>
+        <v>4192.0</v>
       </c>
       <c r="E15" t="n">
-        <v>4496.0</v>
+        <v>4521.0</v>
       </c>
       <c r="F15" t="n">
-        <v>2318.0</v>
+        <v>4590.0</v>
       </c>
       <c r="G15" t="n">
-        <v>2248.0</v>
+        <v>5004.0</v>
       </c>
       <c r="H15" t="n">
-        <v>5101.0</v>
+        <v>10636.0</v>
       </c>
       <c r="I15" t="n">
-        <v>892.0</v>
+        <v>2056.0</v>
       </c>
       <c r="J15" t="n">
-        <v>1622.0</v>
+        <v>1842.0</v>
       </c>
       <c r="K15" t="n">
         <v>10.0</v>
       </c>
       <c r="L15" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="M15" t="n">
-        <v>3.0</v>
+        <v>15.0</v>
       </c>
       <c r="N15" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="O15" t="n">
-        <v>0.0</v>
+        <v>114.0</v>
       </c>
       <c r="P15" t="n">
-        <v>0.0</v>
+        <v>70.0</v>
       </c>
       <c r="Q15" t="n">
-        <v>24651.0</v>
+        <v>52305.0</v>
       </c>
       <c r="R15" t="n">
-        <v>12.0</v>
+        <v>29.0</v>
       </c>
       <c r="S15" t="n">
-        <v>50432.0</v>
+        <v>76930.0</v>
       </c>
       <c r="T15" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="U15" t="n" s="2">
         <v>43390.0</v>
@@ -1490,64 +1487,64 @@
         <v>85</v>
       </c>
       <c r="C16" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>4099.0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>4416.0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>2265.0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>2067.0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>6676.0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>1068.0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>3630.0</v>
+      </c>
+      <c r="K16" t="n">
         <v>12.0</v>
       </c>
-      <c r="D16" t="n">
-        <v>4158.0</v>
-      </c>
-      <c r="E16" t="n">
-        <v>4512.0</v>
-      </c>
-      <c r="F16" t="n">
-        <v>2967.0</v>
-      </c>
-      <c r="G16" t="n">
-        <v>2856.0</v>
-      </c>
-      <c r="H16" t="n">
-        <v>6748.0</v>
-      </c>
-      <c r="I16" t="n">
-        <v>1235.0</v>
-      </c>
-      <c r="J16" t="n">
-        <v>2092.0</v>
-      </c>
-      <c r="K16" t="n">
+      <c r="L16" t="n">
+        <v>1200.0</v>
+      </c>
+      <c r="M16" t="n">
         <v>11.0</v>
       </c>
-      <c r="L16" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="M16" t="n">
-        <v>51.0</v>
-      </c>
       <c r="N16" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="O16" t="n">
-        <v>24.0</v>
+        <v>0.0</v>
       </c>
       <c r="P16" t="n">
         <v>40.0</v>
       </c>
       <c r="Q16" t="n">
-        <v>45106.0</v>
+        <v>20365.0</v>
       </c>
       <c r="R16" t="n">
-        <v>33.0</v>
+        <v>42.0</v>
       </c>
       <c r="S16" t="n">
-        <v>47235.0</v>
+        <v>46501.0</v>
       </c>
       <c r="T16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="U16" t="n" s="2">
-        <v>43312.0</v>
+        <v>43275.0</v>
       </c>
       <c r="V16" t="n">
-        <v>97.0</v>
+        <v>134.0</v>
       </c>
     </row>
     <row r="17">
@@ -1561,61 +1558,61 @@
         <v>11.0</v>
       </c>
       <c r="D17" t="n">
-        <v>4128.0</v>
+        <v>3956.0</v>
       </c>
       <c r="E17" t="n">
-        <v>4318.0</v>
+        <v>4076.0</v>
       </c>
       <c r="F17" t="n">
-        <v>3778.0</v>
+        <v>1530.0</v>
       </c>
       <c r="G17" t="n">
-        <v>4089.0</v>
+        <v>1456.0</v>
       </c>
       <c r="H17" t="n">
-        <v>8585.0</v>
+        <v>3616.0</v>
       </c>
       <c r="I17" t="n">
-        <v>2016.0</v>
+        <v>999.0</v>
       </c>
       <c r="J17" t="n">
-        <v>1331.0</v>
+        <v>2611.0</v>
       </c>
       <c r="K17" t="n">
         <v>10.0</v>
       </c>
       <c r="L17" t="n">
-        <v>4.0</v>
+        <v>33.0</v>
       </c>
       <c r="M17" t="n">
-        <v>0.0</v>
+        <v>34.0</v>
       </c>
       <c r="N17" t="s">
         <v>120</v>
       </c>
       <c r="O17" t="n">
-        <v>38.0</v>
+        <v>30.0</v>
       </c>
       <c r="P17" t="n">
-        <v>30.0</v>
+        <v>50.0</v>
       </c>
       <c r="Q17" t="n">
-        <v>21107.0</v>
+        <v>30326.0</v>
       </c>
       <c r="R17" t="n">
-        <v>19.0</v>
+        <v>12.0</v>
       </c>
       <c r="S17" t="n">
-        <v>68372.0</v>
+        <v>23538.0</v>
       </c>
       <c r="T17" t="s">
         <v>126</v>
       </c>
       <c r="U17" t="n" s="2">
-        <v>43390.0</v>
+        <v>43220.0</v>
       </c>
       <c r="V17" t="n">
-        <v>19.0</v>
+        <v>189.0</v>
       </c>
     </row>
     <row r="18">
@@ -1629,61 +1626,61 @@
         <v>11.0</v>
       </c>
       <c r="D18" t="n">
-        <v>4123.0</v>
+        <v>4241.0</v>
       </c>
       <c r="E18" t="n">
-        <v>4379.0</v>
+        <v>4577.0</v>
       </c>
       <c r="F18" t="n">
-        <v>1120.0</v>
+        <v>2737.0</v>
       </c>
       <c r="G18" t="n">
-        <v>974.0</v>
+        <v>2505.0</v>
       </c>
       <c r="H18" t="n">
-        <v>4306.0</v>
+        <v>6512.0</v>
       </c>
       <c r="I18" t="n">
-        <v>449.0</v>
+        <v>703.0</v>
       </c>
       <c r="J18" t="n">
-        <v>2215.0</v>
+        <v>3595.0</v>
       </c>
       <c r="K18" t="n">
-        <v>8.0</v>
+        <v>10.0</v>
       </c>
       <c r="L18" t="n">
-        <v>81.0</v>
+        <v>0.0</v>
       </c>
       <c r="M18" t="n">
-        <v>202.0</v>
+        <v>0.0</v>
       </c>
       <c r="N18" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="O18" t="n">
-        <v>26.0</v>
+        <v>20.0</v>
       </c>
       <c r="P18" t="n">
         <v>40.0</v>
       </c>
       <c r="Q18" t="n">
-        <v>24789.0</v>
+        <v>21664.0</v>
       </c>
       <c r="R18" t="n">
-        <v>37.0</v>
+        <v>46.0</v>
       </c>
       <c r="S18" t="n">
-        <v>71706.0</v>
+        <v>73665.0</v>
       </c>
       <c r="T18" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="U18" t="n" s="2">
-        <v>43284.0</v>
+        <v>43058.0</v>
       </c>
       <c r="V18" t="n">
-        <v>125.0</v>
+        <v>351.0</v>
       </c>
     </row>
     <row r="19">
@@ -1697,61 +1694,61 @@
         <v>12.0</v>
       </c>
       <c r="D19" t="n">
-        <v>4118.0</v>
+        <v>4164.0</v>
       </c>
       <c r="E19" t="n">
-        <v>4280.0</v>
+        <v>4512.0</v>
       </c>
       <c r="F19" t="n">
-        <v>4392.0</v>
+        <v>2969.0</v>
       </c>
       <c r="G19" t="n">
-        <v>4355.0</v>
+        <v>2858.0</v>
       </c>
       <c r="H19" t="n">
-        <v>18362.0</v>
+        <v>6752.0</v>
       </c>
       <c r="I19" t="n">
-        <v>2921.0</v>
+        <v>1235.0</v>
       </c>
       <c r="J19" t="n">
-        <v>2740.0</v>
+        <v>2092.0</v>
       </c>
       <c r="K19" t="n">
         <v>11.0</v>
       </c>
       <c r="L19" t="n">
-        <v>2641.0</v>
+        <v>8.0</v>
       </c>
       <c r="M19" t="n">
-        <v>15601.0</v>
+        <v>51.0</v>
       </c>
       <c r="N19" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="O19" t="n">
-        <v>0.0</v>
+        <v>62.0</v>
       </c>
       <c r="P19" t="n">
-        <v>40.0</v>
+        <v>70.0</v>
       </c>
       <c r="Q19" t="n">
-        <v>6260.0</v>
+        <v>45144.0</v>
       </c>
       <c r="R19" t="n">
-        <v>77.0</v>
+        <v>33.0</v>
       </c>
       <c r="S19" t="n">
-        <v>76625.0</v>
+        <v>47235.0</v>
       </c>
       <c r="T19" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="U19" t="n" s="2">
-        <v>42614.0</v>
+        <v>43312.0</v>
       </c>
       <c r="V19" t="n">
-        <v>795.0</v>
+        <v>97.0</v>
       </c>
     </row>
     <row r="20">
@@ -1762,64 +1759,64 @@
         <v>89</v>
       </c>
       <c r="C20" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="D20" t="n">
-        <v>4113.0</v>
+        <v>4331.0</v>
       </c>
       <c r="E20" t="n">
-        <v>4323.0</v>
+        <v>4767.0</v>
       </c>
       <c r="F20" t="n">
-        <v>2368.0</v>
+        <v>6660.0</v>
       </c>
       <c r="G20" t="n">
-        <v>2293.0</v>
+        <v>6616.0</v>
       </c>
       <c r="H20" t="n">
-        <v>5946.0</v>
+        <v>23470.0</v>
       </c>
       <c r="I20" t="n">
-        <v>1172.0</v>
+        <v>2753.0</v>
       </c>
       <c r="J20" t="n">
-        <v>2792.0</v>
+        <v>2570.0</v>
       </c>
       <c r="K20" t="n">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="L20" t="n">
-        <v>0.0</v>
+        <v>433.0</v>
       </c>
       <c r="M20" t="n">
-        <v>0.0</v>
+        <v>2512.0</v>
       </c>
       <c r="N20" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="O20" t="n">
-        <v>110.0</v>
+        <v>72.0</v>
       </c>
       <c r="P20" t="n">
         <v>80.0</v>
       </c>
       <c r="Q20" t="n">
-        <v>21091.0</v>
+        <v>67001.0</v>
       </c>
       <c r="R20" t="n">
-        <v>15.0</v>
+        <v>85.0</v>
       </c>
       <c r="S20" t="n">
-        <v>28132.0</v>
+        <v>79935.0</v>
       </c>
       <c r="T20" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="U20" t="n" s="2">
-        <v>43370.0</v>
+        <v>42705.0</v>
       </c>
       <c r="V20" t="n">
-        <v>39.0</v>
+        <v>704.0</v>
       </c>
     </row>
     <row r="21">
@@ -1833,61 +1830,61 @@
         <v>11.0</v>
       </c>
       <c r="D21" t="n">
-        <v>4096.0</v>
+        <v>2907.0</v>
       </c>
       <c r="E21" t="n">
-        <v>4416.0</v>
+        <v>3176.0</v>
       </c>
       <c r="F21" t="n">
-        <v>2264.0</v>
+        <v>3245.0</v>
       </c>
       <c r="G21" t="n">
-        <v>2066.0</v>
+        <v>4540.0</v>
       </c>
       <c r="H21" t="n">
-        <v>6674.0</v>
+        <v>9090.0</v>
       </c>
       <c r="I21" t="n">
-        <v>1067.0</v>
+        <v>2928.0</v>
       </c>
       <c r="J21" t="n">
-        <v>3630.0</v>
+        <v>444.0</v>
       </c>
       <c r="K21" t="n">
-        <v>12.0</v>
+        <v>10.0</v>
       </c>
       <c r="L21" t="n">
-        <v>1200.0</v>
+        <v>0.0</v>
       </c>
       <c r="M21" t="n">
-        <v>11.0</v>
+        <v>0.0</v>
       </c>
       <c r="N21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O21" t="n">
         <v>0.0</v>
       </c>
       <c r="P21" t="n">
-        <v>40.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q21" t="n">
-        <v>20365.0</v>
+        <v>37407.0</v>
       </c>
       <c r="R21" t="n">
-        <v>42.0</v>
+        <v>26.0</v>
       </c>
       <c r="S21" t="n">
-        <v>46501.0</v>
+        <v>42987.0</v>
       </c>
       <c r="T21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="U21" t="n" s="2">
-        <v>43275.0</v>
+        <v>43151.0</v>
       </c>
       <c r="V21" t="n">
-        <v>134.0</v>
+        <v>258.0</v>
       </c>
     </row>
     <row r="22">
@@ -1901,61 +1898,61 @@
         <v>11.0</v>
       </c>
       <c r="D22" t="n">
-        <v>4061.0</v>
+        <v>4046.0</v>
       </c>
       <c r="E22" t="n">
-        <v>4325.0</v>
+        <v>4253.0</v>
       </c>
       <c r="F22" t="n">
-        <v>6344.0</v>
+        <v>1330.0</v>
       </c>
       <c r="G22" t="n">
-        <v>6598.0</v>
+        <v>1392.0</v>
       </c>
       <c r="H22" t="n">
-        <v>18174.0</v>
+        <v>4561.0</v>
       </c>
       <c r="I22" t="n">
-        <v>3755.0</v>
+        <v>871.0</v>
       </c>
       <c r="J22" t="n">
-        <v>4372.0</v>
+        <v>507.0</v>
       </c>
       <c r="K22" t="n">
         <v>10.0</v>
       </c>
       <c r="L22" t="n">
-        <v>47.0</v>
+        <v>0.0</v>
       </c>
       <c r="M22" t="n">
-        <v>459.0</v>
+        <v>0.0</v>
       </c>
       <c r="N22" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="O22" t="n">
-        <v>24.0</v>
+        <v>0.0</v>
       </c>
       <c r="P22" t="n">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q22" t="n">
-        <v>20651.0</v>
+        <v>21493.0</v>
       </c>
       <c r="R22" t="n">
-        <v>56.0</v>
+        <v>25.0</v>
       </c>
       <c r="S22" t="n">
-        <v>72677.0</v>
+        <v>45901.0</v>
       </c>
       <c r="T22" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="U22" t="n" s="2">
-        <v>43184.0</v>
+        <v>43254.0</v>
       </c>
       <c r="V22" t="n">
-        <v>225.0</v>
+        <v>155.0</v>
       </c>
     </row>
     <row r="23">
@@ -1966,64 +1963,64 @@
         <v>92</v>
       </c>
       <c r="C23" t="n">
-        <v>12.0</v>
+        <v>11.0</v>
       </c>
       <c r="D23" t="n">
-        <v>4061.0</v>
+        <v>4148.0</v>
       </c>
       <c r="E23" t="n">
-        <v>4061.0</v>
+        <v>4345.0</v>
       </c>
       <c r="F23" t="n">
-        <v>3012.0</v>
+        <v>1884.0</v>
       </c>
       <c r="G23" t="n">
-        <v>3028.0</v>
+        <v>1793.0</v>
       </c>
       <c r="H23" t="n">
-        <v>15411.0</v>
+        <v>7970.0</v>
       </c>
       <c r="I23" t="n">
-        <v>3265.0</v>
+        <v>2049.0</v>
       </c>
       <c r="J23" t="n">
-        <v>1889.0</v>
+        <v>1562.0</v>
       </c>
       <c r="K23" t="n">
         <v>11.0</v>
       </c>
       <c r="L23" t="n">
-        <v>4.0</v>
+        <v>10.0</v>
       </c>
       <c r="M23" t="n">
-        <v>26.0</v>
+        <v>11.0</v>
       </c>
       <c r="N23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O23" t="n">
-        <v>110.0</v>
+        <v>58.0</v>
       </c>
       <c r="P23" t="n">
         <v>40.0</v>
       </c>
       <c r="Q23" t="n">
-        <v>32670.0</v>
+        <v>55674.0</v>
       </c>
       <c r="R23" t="n">
-        <v>35.0</v>
+        <v>28.0</v>
       </c>
       <c r="S23" t="n">
-        <v>64695.0</v>
+        <v>64580.0</v>
       </c>
       <c r="T23" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="U23" t="n" s="2">
-        <v>43230.0</v>
+        <v>43380.0</v>
       </c>
       <c r="V23" t="n">
-        <v>179.0</v>
+        <v>29.0</v>
       </c>
     </row>
     <row r="24">
@@ -2034,64 +2031,64 @@
         <v>93</v>
       </c>
       <c r="C24" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>4118.0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>4280.0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>4392.0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>4355.0</v>
+      </c>
+      <c r="H24" t="n">
+        <v>18365.0</v>
+      </c>
+      <c r="I24" t="n">
+        <v>2923.0</v>
+      </c>
+      <c r="J24" t="n">
+        <v>2740.0</v>
+      </c>
+      <c r="K24" t="n">
         <v>11.0</v>
       </c>
-      <c r="D24" t="n">
-        <v>4055.0</v>
-      </c>
-      <c r="E24" t="n">
-        <v>4258.0</v>
-      </c>
-      <c r="F24" t="n">
-        <v>1345.0</v>
-      </c>
-      <c r="G24" t="n">
-        <v>1117.0</v>
-      </c>
-      <c r="H24" t="n">
-        <v>6482.0</v>
-      </c>
-      <c r="I24" t="n">
-        <v>1427.0</v>
-      </c>
-      <c r="J24" t="n">
-        <v>1859.0</v>
-      </c>
-      <c r="K24" t="n">
-        <v>10.0</v>
-      </c>
       <c r="L24" t="n">
-        <v>14.0</v>
+        <v>2641.0</v>
       </c>
       <c r="M24" t="n">
-        <v>21.0</v>
+        <v>15623.0</v>
       </c>
       <c r="N24" t="s">
         <v>122</v>
       </c>
       <c r="O24" t="n">
-        <v>50.0</v>
+        <v>8.0</v>
       </c>
       <c r="P24" t="n">
-        <v>40.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q24" t="n">
-        <v>12124.0</v>
+        <v>6268.0</v>
       </c>
       <c r="R24" t="n">
-        <v>55.0</v>
+        <v>77.0</v>
       </c>
       <c r="S24" t="n">
-        <v>71462.0</v>
+        <v>76625.0</v>
       </c>
       <c r="T24" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="U24" t="n" s="2">
-        <v>43058.0</v>
+        <v>42614.0</v>
       </c>
       <c r="V24" t="n">
-        <v>351.0</v>
+        <v>795.0</v>
       </c>
     </row>
     <row r="25">
@@ -2102,64 +2099,64 @@
         <v>94</v>
       </c>
       <c r="C25" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="D25" t="n">
+        <v>3855.0</v>
+      </c>
+      <c r="E25" t="n">
+        <v>4008.0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>1362.0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>1382.0</v>
+      </c>
+      <c r="H25" t="n">
+        <v>3946.0</v>
+      </c>
+      <c r="I25" t="n">
+        <v>644.0</v>
+      </c>
+      <c r="J25" t="n">
+        <v>793.0</v>
+      </c>
+      <c r="K25" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N25" t="s">
+        <v>121</v>
+      </c>
+      <c r="O25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P25" t="n">
+        <v>80.0</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>9620.0</v>
+      </c>
+      <c r="R25" t="n">
         <v>11.0</v>
       </c>
-      <c r="D25" t="n">
-        <v>4046.0</v>
-      </c>
-      <c r="E25" t="n">
-        <v>4253.0</v>
-      </c>
-      <c r="F25" t="n">
-        <v>1330.0</v>
-      </c>
-      <c r="G25" t="n">
-        <v>1392.0</v>
-      </c>
-      <c r="H25" t="n">
-        <v>4561.0</v>
-      </c>
-      <c r="I25" t="n">
-        <v>871.0</v>
-      </c>
-      <c r="J25" t="n">
-        <v>507.0</v>
-      </c>
-      <c r="K25" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="L25" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M25" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N25" t="s">
-        <v>120</v>
-      </c>
-      <c r="O25" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P25" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q25" t="n">
-        <v>21493.0</v>
-      </c>
-      <c r="R25" t="n">
-        <v>25.0</v>
-      </c>
       <c r="S25" t="n">
-        <v>45901.0</v>
+        <v>22867.0</v>
       </c>
       <c r="T25" t="s">
         <v>126</v>
       </c>
       <c r="U25" t="n" s="2">
-        <v>43254.0</v>
+        <v>43400.0</v>
       </c>
       <c r="V25" t="n">
-        <v>155.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="26">
@@ -2173,61 +2170,61 @@
         <v>12.0</v>
       </c>
       <c r="D26" t="n">
-        <v>4419.0</v>
+        <v>4202.0</v>
       </c>
       <c r="E26" t="n">
-        <v>4473.0</v>
+        <v>4363.0</v>
       </c>
       <c r="F26" t="n">
-        <v>2626.0</v>
+        <v>3293.0</v>
       </c>
       <c r="G26" t="n">
-        <v>2571.0</v>
+        <v>3480.0</v>
       </c>
       <c r="H26" t="n">
-        <v>7174.0</v>
+        <v>12142.0</v>
       </c>
       <c r="I26" t="n">
-        <v>1373.0</v>
+        <v>1679.0</v>
       </c>
       <c r="J26" t="n">
-        <v>3497.0</v>
+        <v>2757.0</v>
       </c>
       <c r="K26" t="n">
         <v>10.0</v>
       </c>
       <c r="L26" t="n">
-        <v>106.0</v>
+        <v>0.0</v>
       </c>
       <c r="M26" t="n">
-        <v>144.0</v>
+        <v>0.0</v>
       </c>
       <c r="N26" t="s">
         <v>120</v>
       </c>
       <c r="O26" t="n">
-        <v>0.0</v>
+        <v>150.0</v>
       </c>
       <c r="P26" t="n">
-        <v>0.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q26" t="n">
-        <v>48638.0</v>
+        <v>41450.0</v>
       </c>
       <c r="R26" t="n">
-        <v>29.0</v>
+        <v>63.0</v>
       </c>
       <c r="S26" t="n">
-        <v>37485.0</v>
+        <v>69203.0</v>
       </c>
       <c r="T26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U26" t="n" s="2">
-        <v>43390.0</v>
+        <v>43214.0</v>
       </c>
       <c r="V26" t="n">
-        <v>19.0</v>
+        <v>195.0</v>
       </c>
     </row>
     <row r="27">
@@ -2238,64 +2235,64 @@
         <v>96</v>
       </c>
       <c r="C27" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="D27" t="n">
+        <v>4335.0</v>
+      </c>
+      <c r="E27" t="n">
+        <v>4653.0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>3688.0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>3406.0</v>
+      </c>
+      <c r="H27" t="n">
+        <v>11319.0</v>
+      </c>
+      <c r="I27" t="n">
+        <v>1547.0</v>
+      </c>
+      <c r="J27" t="n">
+        <v>3040.0</v>
+      </c>
+      <c r="K27" t="n">
         <v>11.0</v>
       </c>
-      <c r="D27" t="n">
-        <v>4422.0</v>
-      </c>
-      <c r="E27" t="n">
-        <v>4577.0</v>
-      </c>
-      <c r="F27" t="n">
-        <v>2736.0</v>
-      </c>
-      <c r="G27" t="n">
-        <v>2505.0</v>
-      </c>
-      <c r="H27" t="n">
-        <v>6510.0</v>
-      </c>
-      <c r="I27" t="n">
-        <v>703.0</v>
-      </c>
-      <c r="J27" t="n">
-        <v>3595.0</v>
-      </c>
-      <c r="K27" t="n">
-        <v>10.0</v>
-      </c>
       <c r="L27" t="n">
-        <v>0.0</v>
+        <v>100.0</v>
       </c>
       <c r="M27" t="n">
-        <v>0.0</v>
+        <v>195.0</v>
       </c>
       <c r="N27" t="s">
         <v>122</v>
       </c>
       <c r="O27" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="P27" t="n">
-        <v>0.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q27" t="n">
-        <v>21644.0</v>
+        <v>32533.0</v>
       </c>
       <c r="R27" t="n">
-        <v>46.0</v>
+        <v>59.0</v>
       </c>
       <c r="S27" t="n">
-        <v>73665.0</v>
+        <v>72275.0</v>
       </c>
       <c r="T27" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="U27" t="n" s="2">
-        <v>43058.0</v>
+        <v>42614.0</v>
       </c>
       <c r="V27" t="n">
-        <v>351.0</v>
+        <v>795.0</v>
       </c>
     </row>
     <row r="28">
@@ -2306,64 +2303,64 @@
         <v>97</v>
       </c>
       <c r="C28" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="D28" t="n">
-        <v>4367.0</v>
+        <v>4026.0</v>
       </c>
       <c r="E28" t="n">
-        <v>4405.0</v>
+        <v>4420.0</v>
       </c>
       <c r="F28" t="n">
-        <v>1092.0</v>
+        <v>3108.0</v>
       </c>
       <c r="G28" t="n">
-        <v>991.0</v>
+        <v>3083.0</v>
       </c>
       <c r="H28" t="n">
-        <v>3121.0</v>
+        <v>7813.0</v>
       </c>
       <c r="I28" t="n">
-        <v>651.0</v>
+        <v>877.0</v>
       </c>
       <c r="J28" t="n">
-        <v>1700.0</v>
+        <v>2715.0</v>
       </c>
       <c r="K28" t="n">
-        <v>7.0</v>
+        <v>10.0</v>
       </c>
       <c r="L28" t="n">
         <v>0.0</v>
       </c>
       <c r="M28" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="N28" t="s">
         <v>120</v>
       </c>
       <c r="O28" t="n">
-        <v>20.0</v>
+        <v>0.0</v>
       </c>
       <c r="P28" t="n">
-        <v>40.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q28" t="n">
-        <v>19710.0</v>
+        <v>12646.0</v>
       </c>
       <c r="R28" t="n">
-        <v>15.0</v>
+        <v>65.0</v>
       </c>
       <c r="S28" t="n">
-        <v>48040.0</v>
+        <v>69961.0</v>
       </c>
       <c r="T28" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U28" t="n" s="2">
-        <v>43352.0</v>
+        <v>43254.0</v>
       </c>
       <c r="V28" t="n">
-        <v>57.0</v>
+        <v>155.0</v>
       </c>
     </row>
     <row r="29">
@@ -2377,61 +2374,61 @@
         <v>11.0</v>
       </c>
       <c r="D29" t="n">
-        <v>4345.0</v>
+        <v>4055.0</v>
       </c>
       <c r="E29" t="n">
-        <v>4345.0</v>
+        <v>4258.0</v>
       </c>
       <c r="F29" t="n">
-        <v>1883.0</v>
+        <v>1345.0</v>
       </c>
       <c r="G29" t="n">
-        <v>1791.0</v>
+        <v>1117.0</v>
       </c>
       <c r="H29" t="n">
-        <v>7966.0</v>
+        <v>6482.0</v>
       </c>
       <c r="I29" t="n">
-        <v>2047.0</v>
+        <v>1427.0</v>
       </c>
       <c r="J29" t="n">
-        <v>1562.0</v>
+        <v>1859.0</v>
       </c>
       <c r="K29" t="n">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="L29" t="n">
-        <v>10.0</v>
+        <v>14.0</v>
       </c>
       <c r="M29" t="n">
-        <v>11.0</v>
+        <v>21.0</v>
       </c>
       <c r="N29" t="s">
         <v>120</v>
       </c>
       <c r="O29" t="n">
-        <v>0.0</v>
+        <v>98.0</v>
       </c>
       <c r="P29" t="n">
-        <v>0.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q29" t="n">
-        <v>55616.0</v>
+        <v>12172.0</v>
       </c>
       <c r="R29" t="n">
-        <v>28.0</v>
+        <v>55.0</v>
       </c>
       <c r="S29" t="n">
-        <v>64580.0</v>
+        <v>71462.0</v>
       </c>
       <c r="T29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U29" t="n" s="2">
-        <v>43380.0</v>
+        <v>43058.0</v>
       </c>
       <c r="V29" t="n">
-        <v>29.0</v>
+        <v>351.0</v>
       </c>
     </row>
     <row r="30">
@@ -2442,64 +2439,64 @@
         <v>99</v>
       </c>
       <c r="C30" t="n">
-        <v>12.0</v>
+        <v>10.0</v>
       </c>
       <c r="D30" t="n">
-        <v>4328.0</v>
+        <v>3982.0</v>
       </c>
       <c r="E30" t="n">
-        <v>4521.0</v>
+        <v>4006.0</v>
       </c>
       <c r="F30" t="n">
-        <v>4588.0</v>
+        <v>667.0</v>
       </c>
       <c r="G30" t="n">
-        <v>5003.0</v>
+        <v>535.0</v>
       </c>
       <c r="H30" t="n">
-        <v>10633.0</v>
+        <v>3342.0</v>
       </c>
       <c r="I30" t="n">
-        <v>2056.0</v>
+        <v>735.0</v>
       </c>
       <c r="J30" t="n">
-        <v>1842.0</v>
+        <v>838.0</v>
       </c>
       <c r="K30" t="n">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="L30" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="M30" t="n">
-        <v>15.0</v>
+        <v>0.0</v>
       </c>
       <c r="N30" t="s">
         <v>120</v>
       </c>
       <c r="O30" t="n">
-        <v>38.0</v>
+        <v>0.0</v>
       </c>
       <c r="P30" t="n">
-        <v>40.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q30" t="n">
-        <v>52229.0</v>
+        <v>4623.0</v>
       </c>
       <c r="R30" t="n">
-        <v>29.0</v>
+        <v>50.0</v>
       </c>
       <c r="S30" t="n">
-        <v>76930.0</v>
+        <v>63691.0</v>
       </c>
       <c r="T30" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="U30" t="n" s="2">
-        <v>43390.0</v>
+        <v>43138.0</v>
       </c>
       <c r="V30" t="n">
-        <v>19.0</v>
+        <v>271.0</v>
       </c>
     </row>
     <row r="31">
@@ -2513,25 +2510,25 @@
         <v>12.0</v>
       </c>
       <c r="D31" t="n">
-        <v>4252.0</v>
+        <v>4014.0</v>
       </c>
       <c r="E31" t="n">
-        <v>4272.0</v>
+        <v>4140.0</v>
       </c>
       <c r="F31" t="n">
-        <v>2723.0</v>
+        <v>2128.0</v>
       </c>
       <c r="G31" t="n">
-        <v>2652.0</v>
+        <v>2179.0</v>
       </c>
       <c r="H31" t="n">
-        <v>7744.0</v>
+        <v>6889.0</v>
       </c>
       <c r="I31" t="n">
-        <v>2255.0</v>
+        <v>1551.0</v>
       </c>
       <c r="J31" t="n">
-        <v>2311.0</v>
+        <v>1474.0</v>
       </c>
       <c r="K31" t="n">
         <v>10.0</v>
@@ -2540,34 +2537,34 @@
         <v>0.0</v>
       </c>
       <c r="M31" t="n">
-        <v>0.0</v>
+        <v>41.0</v>
       </c>
       <c r="N31" t="s">
         <v>120</v>
       </c>
       <c r="O31" t="n">
-        <v>34.0</v>
+        <v>48.0</v>
       </c>
       <c r="P31" t="n">
-        <v>0.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q31" t="n">
-        <v>31323.0</v>
+        <v>42027.0</v>
       </c>
       <c r="R31" t="n">
-        <v>21.0</v>
+        <v>35.0</v>
       </c>
       <c r="S31" t="n">
-        <v>21975.0</v>
+        <v>67193.0</v>
       </c>
       <c r="T31" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="U31" t="n" s="2">
-        <v>43382.0</v>
+        <v>42920.0</v>
       </c>
       <c r="V31" t="n">
-        <v>27.0</v>
+        <v>489.0</v>
       </c>
     </row>
     <row r="32">
@@ -2578,64 +2575,64 @@
         <v>101</v>
       </c>
       <c r="C32" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="D32" t="n">
-        <v>4148.0</v>
+        <v>4218.0</v>
       </c>
       <c r="E32" t="n">
-        <v>4254.0</v>
+        <v>4798.0</v>
       </c>
       <c r="F32" t="n">
-        <v>2570.0</v>
+        <v>5098.0</v>
       </c>
       <c r="G32" t="n">
-        <v>2613.0</v>
+        <v>5216.0</v>
       </c>
       <c r="H32" t="n">
-        <v>6173.0</v>
+        <v>12236.0</v>
       </c>
       <c r="I32" t="n">
-        <v>1063.0</v>
+        <v>2230.0</v>
       </c>
       <c r="J32" t="n">
-        <v>1649.0</v>
+        <v>1728.0</v>
       </c>
       <c r="K32" t="n">
-        <v>12.0</v>
+        <v>10.0</v>
       </c>
       <c r="L32" t="n">
-        <v>0.0</v>
+        <v>31.0</v>
       </c>
       <c r="M32" t="n">
-        <v>9.0</v>
+        <v>43.0</v>
       </c>
       <c r="N32" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="O32" t="n">
-        <v>0.0</v>
+        <v>116.0</v>
       </c>
       <c r="P32" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>58853.0</v>
+      </c>
+      <c r="R32" t="n">
         <v>30.0</v>
       </c>
-      <c r="Q32" t="n">
-        <v>8910.0</v>
-      </c>
-      <c r="R32" t="n">
-        <v>41.0</v>
-      </c>
       <c r="S32" t="n">
-        <v>57166.0</v>
+        <v>74870.0</v>
       </c>
       <c r="T32" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="U32" t="n" s="2">
-        <v>43082.0</v>
+        <v>43058.0</v>
       </c>
       <c r="V32" t="n">
-        <v>327.0</v>
+        <v>351.0</v>
       </c>
     </row>
     <row r="33">
@@ -2646,28 +2643,28 @@
         <v>102</v>
       </c>
       <c r="C33" t="n">
-        <v>12.0</v>
+        <v>9.0</v>
       </c>
       <c r="D33" t="n">
-        <v>4127.0</v>
+        <v>3010.0</v>
       </c>
       <c r="E33" t="n">
-        <v>4140.0</v>
+        <v>3010.0</v>
       </c>
       <c r="F33" t="n">
-        <v>2126.0</v>
+        <v>377.0</v>
       </c>
       <c r="G33" t="n">
-        <v>2175.0</v>
+        <v>219.0</v>
       </c>
       <c r="H33" t="n">
-        <v>6883.0</v>
+        <v>1545.0</v>
       </c>
       <c r="I33" t="n">
-        <v>1550.0</v>
+        <v>264.0</v>
       </c>
       <c r="J33" t="n">
-        <v>1474.0</v>
+        <v>147.0</v>
       </c>
       <c r="K33" t="n">
         <v>10.0</v>
@@ -2676,34 +2673,34 @@
         <v>0.0</v>
       </c>
       <c r="M33" t="n">
-        <v>41.0</v>
+        <v>0.0</v>
       </c>
       <c r="N33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O33" t="n">
-        <v>20.0</v>
+        <v>0.0</v>
       </c>
       <c r="P33" t="n">
-        <v>40.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q33" t="n">
-        <v>41999.0</v>
+        <v>4091.0</v>
       </c>
       <c r="R33" t="n">
-        <v>35.0</v>
+        <v>0.0</v>
       </c>
       <c r="S33" t="n">
-        <v>67193.0</v>
+        <v>0.0</v>
       </c>
       <c r="T33" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="U33" t="n" s="2">
-        <v>42920.0</v>
+        <v>43409.0</v>
       </c>
       <c r="V33" t="n">
-        <v>489.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="34">
@@ -2714,31 +2711,31 @@
         <v>103</v>
       </c>
       <c r="C34" t="n">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="D34" t="n">
-        <v>4026.0</v>
+        <v>3962.0</v>
       </c>
       <c r="E34" t="n">
-        <v>4420.0</v>
+        <v>3962.0</v>
       </c>
       <c r="F34" t="n">
-        <v>3108.0</v>
+        <v>944.0</v>
       </c>
       <c r="G34" t="n">
-        <v>3083.0</v>
+        <v>968.0</v>
       </c>
       <c r="H34" t="n">
-        <v>7813.0</v>
+        <v>4180.0</v>
       </c>
       <c r="I34" t="n">
-        <v>877.0</v>
+        <v>988.0</v>
       </c>
       <c r="J34" t="n">
-        <v>2715.0</v>
+        <v>278.0</v>
       </c>
       <c r="K34" t="n">
-        <v>10.0</v>
+        <v>6.0</v>
       </c>
       <c r="L34" t="n">
         <v>0.0</v>
@@ -2747,31 +2744,31 @@
         <v>0.0</v>
       </c>
       <c r="N34" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O34" t="n">
-        <v>0.0</v>
+        <v>18.0</v>
       </c>
       <c r="P34" t="n">
-        <v>0.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q34" t="n">
-        <v>12646.0</v>
+        <v>8328.0</v>
       </c>
       <c r="R34" t="n">
-        <v>65.0</v>
+        <v>25.0</v>
       </c>
       <c r="S34" t="n">
-        <v>69961.0</v>
+        <v>58973.0</v>
       </c>
       <c r="T34" t="s">
         <v>126</v>
       </c>
       <c r="U34" t="n" s="2">
-        <v>43254.0</v>
+        <v>43312.0</v>
       </c>
       <c r="V34" t="n">
-        <v>155.0</v>
+        <v>97.0</v>
       </c>
     </row>
     <row r="35">
@@ -2785,61 +2782,61 @@
         <v>10.0</v>
       </c>
       <c r="D35" t="n">
-        <v>4023.0</v>
+        <v>3676.0</v>
       </c>
       <c r="E35" t="n">
-        <v>4077.0</v>
+        <v>4007.0</v>
       </c>
       <c r="F35" t="n">
-        <v>1648.0</v>
+        <v>545.0</v>
       </c>
       <c r="G35" t="n">
-        <v>1431.0</v>
+        <v>481.0</v>
       </c>
       <c r="H35" t="n">
-        <v>4285.0</v>
+        <v>3311.0</v>
       </c>
       <c r="I35" t="n">
-        <v>827.0</v>
+        <v>688.0</v>
       </c>
       <c r="J35" t="n">
-        <v>2400.0</v>
+        <v>278.0</v>
       </c>
       <c r="K35" t="n">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="L35" t="n">
         <v>0.0</v>
       </c>
       <c r="M35" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="N35" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="O35" t="n">
-        <v>0.0</v>
+        <v>66.0</v>
       </c>
       <c r="P35" t="n">
-        <v>0.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q35" t="n">
-        <v>17819.0</v>
+        <v>16637.0</v>
       </c>
       <c r="R35" t="n">
-        <v>14.0</v>
+        <v>23.0</v>
       </c>
       <c r="S35" t="n">
-        <v>26960.0</v>
+        <v>58710.0</v>
       </c>
       <c r="T35" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U35" t="n" s="2">
-        <v>43372.0</v>
+        <v>43274.0</v>
       </c>
       <c r="V35" t="n">
-        <v>37.0</v>
+        <v>135.0</v>
       </c>
     </row>
     <row r="36">
@@ -2850,31 +2847,31 @@
         <v>105</v>
       </c>
       <c r="C36" t="n">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="D36" t="n">
-        <v>3957.0</v>
+        <v>3959.0</v>
       </c>
       <c r="E36" t="n">
-        <v>4163.0</v>
+        <v>4078.0</v>
       </c>
       <c r="F36" t="n">
-        <v>3147.0</v>
+        <v>3373.0</v>
       </c>
       <c r="G36" t="n">
-        <v>3322.0</v>
+        <v>3933.0</v>
       </c>
       <c r="H36" t="n">
-        <v>8557.0</v>
+        <v>9366.0</v>
       </c>
       <c r="I36" t="n">
-        <v>1337.0</v>
+        <v>1723.0</v>
       </c>
       <c r="J36" t="n">
-        <v>1906.0</v>
+        <v>224.0</v>
       </c>
       <c r="K36" t="n">
-        <v>10.0</v>
+        <v>4.0</v>
       </c>
       <c r="L36" t="n">
         <v>0.0</v>
@@ -2889,25 +2886,25 @@
         <v>0.0</v>
       </c>
       <c r="P36" t="n">
-        <v>0.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q36" t="n">
-        <v>14205.0</v>
+        <v>14193.0</v>
       </c>
       <c r="R36" t="n">
-        <v>17.0</v>
+        <v>34.0</v>
       </c>
       <c r="S36" t="n">
-        <v>27880.0</v>
+        <v>65653.0</v>
       </c>
       <c r="T36" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="U36" t="n" s="2">
-        <v>43218.0</v>
+        <v>43280.0</v>
       </c>
       <c r="V36" t="n">
-        <v>191.0</v>
+        <v>129.0</v>
       </c>
     </row>
     <row r="37">
@@ -2918,64 +2915,64 @@
         <v>106</v>
       </c>
       <c r="C37" t="n">
-        <v>11.0</v>
+        <v>8.0</v>
       </c>
       <c r="D37" t="n">
-        <v>3956.0</v>
+        <v>3425.0</v>
       </c>
       <c r="E37" t="n">
-        <v>4076.0</v>
+        <v>3497.0</v>
       </c>
       <c r="F37" t="n">
-        <v>1530.0</v>
+        <v>286.0</v>
       </c>
       <c r="G37" t="n">
-        <v>1456.0</v>
+        <v>158.0</v>
       </c>
       <c r="H37" t="n">
-        <v>3616.0</v>
+        <v>560.0</v>
       </c>
       <c r="I37" t="n">
-        <v>999.0</v>
+        <v>103.0</v>
       </c>
       <c r="J37" t="n">
-        <v>2611.0</v>
+        <v>373.0</v>
       </c>
       <c r="K37" t="n">
-        <v>10.0</v>
+        <v>6.0</v>
       </c>
       <c r="L37" t="n">
-        <v>33.0</v>
+        <v>0.0</v>
       </c>
       <c r="M37" t="n">
-        <v>34.0</v>
+        <v>0.0</v>
       </c>
       <c r="N37" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O37" t="n">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
       <c r="P37" t="n">
-        <v>10.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q37" t="n">
-        <v>30296.0</v>
+        <v>2397.0</v>
       </c>
       <c r="R37" t="n">
-        <v>12.0</v>
+        <v>1.0</v>
       </c>
       <c r="S37" t="n">
-        <v>23538.0</v>
+        <v>7471.0</v>
       </c>
       <c r="T37" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="U37" t="n" s="2">
-        <v>43220.0</v>
+        <v>43360.0</v>
       </c>
       <c r="V37" t="n">
-        <v>189.0</v>
+        <v>49.0</v>
       </c>
     </row>
     <row r="38">
@@ -2986,64 +2983,64 @@
         <v>107</v>
       </c>
       <c r="C38" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="D38" t="n">
-        <v>3956.0</v>
+        <v>4123.0</v>
       </c>
       <c r="E38" t="n">
-        <v>4142.0</v>
+        <v>4379.0</v>
       </c>
       <c r="F38" t="n">
-        <v>1221.0</v>
+        <v>1120.0</v>
       </c>
       <c r="G38" t="n">
-        <v>1252.0</v>
+        <v>974.0</v>
       </c>
       <c r="H38" t="n">
-        <v>3143.0</v>
+        <v>4306.0</v>
       </c>
       <c r="I38" t="n">
-        <v>496.0</v>
+        <v>449.0</v>
       </c>
       <c r="J38" t="n">
-        <v>310.0</v>
+        <v>2215.0</v>
       </c>
       <c r="K38" t="n">
-        <v>10.0</v>
+        <v>8.0</v>
       </c>
       <c r="L38" t="n">
-        <v>0.0</v>
+        <v>81.0</v>
       </c>
       <c r="M38" t="n">
-        <v>0.0</v>
+        <v>202.0</v>
       </c>
       <c r="N38" t="s">
         <v>120</v>
       </c>
       <c r="O38" t="n">
-        <v>64.0</v>
+        <v>44.0</v>
       </c>
       <c r="P38" t="n">
-        <v>32.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q38" t="n">
-        <v>15322.0</v>
+        <v>24807.0</v>
       </c>
       <c r="R38" t="n">
-        <v>28.0</v>
+        <v>37.0</v>
       </c>
       <c r="S38" t="n">
-        <v>38427.0</v>
+        <v>71706.0</v>
       </c>
       <c r="T38" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="U38" t="n" s="2">
-        <v>43356.0</v>
+        <v>43284.0</v>
       </c>
       <c r="V38" t="n">
-        <v>53.0</v>
+        <v>125.0</v>
       </c>
     </row>
     <row r="39">
@@ -3057,61 +3054,61 @@
         <v>10.0</v>
       </c>
       <c r="D39" t="n">
-        <v>3952.0</v>
+        <v>4367.0</v>
       </c>
       <c r="E39" t="n">
-        <v>4006.0</v>
+        <v>4405.0</v>
       </c>
       <c r="F39" t="n">
-        <v>666.0</v>
+        <v>1092.0</v>
       </c>
       <c r="G39" t="n">
-        <v>535.0</v>
+        <v>991.0</v>
       </c>
       <c r="H39" t="n">
-        <v>3339.0</v>
+        <v>3121.0</v>
       </c>
       <c r="I39" t="n">
-        <v>735.0</v>
+        <v>651.0</v>
       </c>
       <c r="J39" t="n">
-        <v>838.0</v>
+        <v>1700.0</v>
       </c>
       <c r="K39" t="n">
-        <v>9.0</v>
+        <v>7.0</v>
       </c>
       <c r="L39" t="n">
         <v>0.0</v>
       </c>
       <c r="M39" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="N39" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O39" t="n">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
       <c r="P39" t="n">
-        <v>0.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q39" t="n">
-        <v>4623.0</v>
+        <v>19710.0</v>
       </c>
       <c r="R39" t="n">
-        <v>50.0</v>
+        <v>15.0</v>
       </c>
       <c r="S39" t="n">
-        <v>63691.0</v>
+        <v>48040.0</v>
       </c>
       <c r="T39" t="s">
         <v>127</v>
       </c>
       <c r="U39" t="n" s="2">
-        <v>43138.0</v>
+        <v>43352.0</v>
       </c>
       <c r="V39" t="n">
-        <v>271.0</v>
+        <v>57.0</v>
       </c>
     </row>
     <row r="40">
@@ -3122,31 +3119,31 @@
         <v>109</v>
       </c>
       <c r="C40" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="D40" t="n">
-        <v>3924.0</v>
+        <v>4306.0</v>
       </c>
       <c r="E40" t="n">
-        <v>3950.0</v>
+        <v>4553.0</v>
       </c>
       <c r="F40" t="n">
-        <v>941.0</v>
+        <v>4635.0</v>
       </c>
       <c r="G40" t="n">
-        <v>966.0</v>
+        <v>4693.0</v>
       </c>
       <c r="H40" t="n">
-        <v>4172.0</v>
+        <v>26531.0</v>
       </c>
       <c r="I40" t="n">
-        <v>986.0</v>
+        <v>3613.0</v>
       </c>
       <c r="J40" t="n">
-        <v>278.0</v>
+        <v>2006.0</v>
       </c>
       <c r="K40" t="n">
-        <v>6.0</v>
+        <v>11.0</v>
       </c>
       <c r="L40" t="n">
         <v>0.0</v>
@@ -3161,25 +3158,25 @@
         <v>0.0</v>
       </c>
       <c r="P40" t="n">
-        <v>0.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q40" t="n">
-        <v>8310.0</v>
+        <v>7112.0</v>
       </c>
       <c r="R40" t="n">
-        <v>25.0</v>
+        <v>57.0</v>
       </c>
       <c r="S40" t="n">
-        <v>58973.0</v>
+        <v>69835.0</v>
       </c>
       <c r="T40" t="s">
         <v>127</v>
       </c>
       <c r="U40" t="n" s="2">
-        <v>43312.0</v>
+        <v>43252.0</v>
       </c>
       <c r="V40" t="n">
-        <v>97.0</v>
+        <v>157.0</v>
       </c>
     </row>
     <row r="41">
@@ -3190,31 +3187,31 @@
         <v>110</v>
       </c>
       <c r="C41" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="D41" t="n">
-        <v>3901.0</v>
+        <v>4060.0</v>
       </c>
       <c r="E41" t="n">
-        <v>3901.0</v>
+        <v>4323.0</v>
       </c>
       <c r="F41" t="n">
-        <v>853.0</v>
+        <v>2368.0</v>
       </c>
       <c r="G41" t="n">
-        <v>729.0</v>
+        <v>2295.0</v>
       </c>
       <c r="H41" t="n">
-        <v>3868.0</v>
+        <v>5948.0</v>
       </c>
       <c r="I41" t="n">
-        <v>892.0</v>
+        <v>1172.0</v>
       </c>
       <c r="J41" t="n">
-        <v>535.0</v>
+        <v>2792.0</v>
       </c>
       <c r="K41" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="L41" t="n">
         <v>0.0</v>
@@ -3223,31 +3220,31 @@
         <v>0.0</v>
       </c>
       <c r="N41" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="O41" t="n">
-        <v>0.0</v>
+        <v>156.0</v>
       </c>
       <c r="P41" t="n">
-        <v>0.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q41" t="n">
-        <v>24388.0</v>
+        <v>21137.0</v>
       </c>
       <c r="R41" t="n">
         <v>15.0</v>
       </c>
       <c r="S41" t="n">
-        <v>13894.0</v>
+        <v>28132.0</v>
       </c>
       <c r="T41" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="U41" t="n" s="2">
-        <v>43254.0</v>
+        <v>43370.0</v>
       </c>
       <c r="V41" t="n">
-        <v>155.0</v>
+        <v>39.0</v>
       </c>
     </row>
     <row r="42">
@@ -3258,31 +3255,31 @@
         <v>111</v>
       </c>
       <c r="C42" t="n">
-        <v>10.0</v>
+        <v>12.0</v>
       </c>
       <c r="D42" t="n">
-        <v>3884.0</v>
+        <v>4126.0</v>
       </c>
       <c r="E42" t="n">
-        <v>4078.0</v>
+        <v>4272.0</v>
       </c>
       <c r="F42" t="n">
-        <v>3367.0</v>
+        <v>2723.0</v>
       </c>
       <c r="G42" t="n">
-        <v>3929.0</v>
+        <v>2652.0</v>
       </c>
       <c r="H42" t="n">
-        <v>9352.0</v>
+        <v>7745.0</v>
       </c>
       <c r="I42" t="n">
-        <v>1721.0</v>
+        <v>2256.0</v>
       </c>
       <c r="J42" t="n">
-        <v>224.0</v>
+        <v>2311.0</v>
       </c>
       <c r="K42" t="n">
-        <v>4.0</v>
+        <v>10.0</v>
       </c>
       <c r="L42" t="n">
         <v>0.0</v>
@@ -3291,31 +3288,31 @@
         <v>0.0</v>
       </c>
       <c r="N42" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O42" t="n">
-        <v>0.0</v>
+        <v>60.0</v>
       </c>
       <c r="P42" t="n">
-        <v>0.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q42" t="n">
-        <v>14193.0</v>
+        <v>31349.0</v>
       </c>
       <c r="R42" t="n">
-        <v>34.0</v>
+        <v>21.0</v>
       </c>
       <c r="S42" t="n">
-        <v>65653.0</v>
+        <v>21975.0</v>
       </c>
       <c r="T42" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="U42" t="n" s="2">
-        <v>43280.0</v>
+        <v>43382.0</v>
       </c>
       <c r="V42" t="n">
-        <v>129.0</v>
+        <v>27.0</v>
       </c>
     </row>
     <row r="43">
@@ -3326,64 +3323,64 @@
         <v>112</v>
       </c>
       <c r="C43" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="D43" t="n">
-        <v>3855.0</v>
+        <v>4128.0</v>
       </c>
       <c r="E43" t="n">
-        <v>4008.0</v>
+        <v>4318.0</v>
       </c>
       <c r="F43" t="n">
-        <v>1362.0</v>
+        <v>3778.0</v>
       </c>
       <c r="G43" t="n">
-        <v>1382.0</v>
+        <v>4089.0</v>
       </c>
       <c r="H43" t="n">
-        <v>3946.0</v>
+        <v>8585.0</v>
       </c>
       <c r="I43" t="n">
-        <v>644.0</v>
+        <v>2016.0</v>
       </c>
       <c r="J43" t="n">
-        <v>793.0</v>
+        <v>1331.0</v>
       </c>
       <c r="K43" t="n">
         <v>10.0</v>
       </c>
       <c r="L43" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="M43" t="n">
         <v>0.0</v>
       </c>
       <c r="N43" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="O43" t="n">
-        <v>0.0</v>
+        <v>38.0</v>
       </c>
       <c r="P43" t="n">
-        <v>60.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q43" t="n">
-        <v>9620.0</v>
+        <v>21107.0</v>
       </c>
       <c r="R43" t="n">
-        <v>11.0</v>
+        <v>19.0</v>
       </c>
       <c r="S43" t="n">
-        <v>22867.0</v>
+        <v>68372.0</v>
       </c>
       <c r="T43" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="U43" t="n" s="2">
-        <v>43400.0</v>
+        <v>43390.0</v>
       </c>
       <c r="V43" t="n">
-        <v>9.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="44">
@@ -3394,64 +3391,64 @@
         <v>113</v>
       </c>
       <c r="C44" t="n">
-        <v>10.0</v>
+        <v>12.0</v>
       </c>
       <c r="D44" t="n">
-        <v>3712.0</v>
+        <v>4182.0</v>
       </c>
       <c r="E44" t="n">
-        <v>3764.0</v>
+        <v>4473.0</v>
       </c>
       <c r="F44" t="n">
-        <v>693.0</v>
+        <v>2626.0</v>
       </c>
       <c r="G44" t="n">
-        <v>640.0</v>
+        <v>2572.0</v>
       </c>
       <c r="H44" t="n">
-        <v>1953.0</v>
+        <v>7175.0</v>
       </c>
       <c r="I44" t="n">
-        <v>381.0</v>
+        <v>1373.0</v>
       </c>
       <c r="J44" t="n">
-        <v>1428.0</v>
+        <v>3497.0</v>
       </c>
       <c r="K44" t="n">
         <v>10.0</v>
       </c>
       <c r="L44" t="n">
-        <v>0.0</v>
+        <v>106.0</v>
       </c>
       <c r="M44" t="n">
-        <v>4.0</v>
+        <v>144.0</v>
       </c>
       <c r="N44" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="O44" t="n">
-        <v>30.0</v>
+        <v>84.0</v>
       </c>
       <c r="P44" t="n">
         <v>40.0</v>
       </c>
       <c r="Q44" t="n">
-        <v>16366.0</v>
+        <v>48722.0</v>
       </c>
       <c r="R44" t="n">
-        <v>4.0</v>
+        <v>29.0</v>
       </c>
       <c r="S44" t="n">
-        <v>8680.0</v>
+        <v>37485.0</v>
       </c>
       <c r="T44" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="U44" t="n" s="2">
-        <v>43397.0</v>
+        <v>43390.0</v>
       </c>
       <c r="V44" t="n">
-        <v>12.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="45">
@@ -3462,31 +3459,31 @@
         <v>114</v>
       </c>
       <c r="C45" t="n">
-        <v>10.0</v>
+        <v>7.0</v>
       </c>
       <c r="D45" t="n">
-        <v>3647.0</v>
+        <v>2264.0</v>
       </c>
       <c r="E45" t="n">
-        <v>4007.0</v>
+        <v>2297.0</v>
       </c>
       <c r="F45" t="n">
-        <v>544.0</v>
+        <v>155.0</v>
       </c>
       <c r="G45" t="n">
-        <v>481.0</v>
+        <v>80.0</v>
       </c>
       <c r="H45" t="n">
-        <v>3309.0</v>
+        <v>275.0</v>
       </c>
       <c r="I45" t="n">
-        <v>688.0</v>
+        <v>72.0</v>
       </c>
       <c r="J45" t="n">
-        <v>278.0</v>
+        <v>0.0</v>
       </c>
       <c r="K45" t="n">
-        <v>9.0</v>
+        <v>0.0</v>
       </c>
       <c r="L45" t="n">
         <v>0.0</v>
@@ -3495,31 +3492,31 @@
         <v>0.0</v>
       </c>
       <c r="N45" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="O45" t="n">
-        <v>18.0</v>
+        <v>0.0</v>
       </c>
       <c r="P45" t="n">
-        <v>40.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q45" t="n">
-        <v>16589.0</v>
+        <v>929.0</v>
       </c>
       <c r="R45" t="n">
-        <v>23.0</v>
+        <v>0.0</v>
       </c>
       <c r="S45" t="n">
-        <v>58710.0</v>
+        <v>0.0</v>
       </c>
       <c r="T45" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="U45" t="n" s="2">
-        <v>43274.0</v>
+        <v>43376.0</v>
       </c>
       <c r="V45" t="n">
-        <v>135.0</v>
+        <v>33.0</v>
       </c>
     </row>
     <row r="46">
@@ -3530,64 +3527,64 @@
         <v>115</v>
       </c>
       <c r="C46" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="D46" t="n">
-        <v>3401.0</v>
+        <v>4379.0</v>
       </c>
       <c r="E46" t="n">
-        <v>3656.0</v>
+        <v>4919.0</v>
       </c>
       <c r="F46" t="n">
-        <v>1096.0</v>
+        <v>10796.0</v>
       </c>
       <c r="G46" t="n">
-        <v>1149.0</v>
+        <v>11507.0</v>
       </c>
       <c r="H46" t="n">
-        <v>4621.0</v>
+        <v>25745.0</v>
       </c>
       <c r="I46" t="n">
-        <v>1231.0</v>
+        <v>8871.0</v>
       </c>
       <c r="J46" t="n">
-        <v>858.0</v>
+        <v>2205.0</v>
       </c>
       <c r="K46" t="n">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="L46" t="n">
-        <v>25.0</v>
+        <v>0.0</v>
       </c>
       <c r="M46" t="n">
-        <v>18.0</v>
+        <v>4.0</v>
       </c>
       <c r="N46" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="O46" t="n">
-        <v>28.0</v>
+        <v>182.0</v>
       </c>
       <c r="P46" t="n">
-        <v>0.0</v>
+        <v>60.0</v>
       </c>
       <c r="Q46" t="n">
-        <v>28849.0</v>
+        <v>73886.0</v>
       </c>
       <c r="R46" t="n">
-        <v>7.0</v>
+        <v>20.0</v>
       </c>
       <c r="S46" t="n">
-        <v>11970.0</v>
+        <v>77870.0</v>
       </c>
       <c r="T46" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="U46" t="n" s="2">
-        <v>43123.0</v>
+        <v>43390.0</v>
       </c>
       <c r="V46" t="n">
-        <v>286.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="47">
@@ -3598,64 +3595,64 @@
         <v>116</v>
       </c>
       <c r="C47" t="n">
-        <v>8.0</v>
+        <v>12.0</v>
       </c>
       <c r="D47" t="n">
-        <v>3391.0</v>
+        <v>4061.0</v>
       </c>
       <c r="E47" t="n">
-        <v>3497.0</v>
+        <v>4061.0</v>
       </c>
       <c r="F47" t="n">
-        <v>284.0</v>
+        <v>3012.0</v>
       </c>
       <c r="G47" t="n">
-        <v>157.0</v>
+        <v>3028.0</v>
       </c>
       <c r="H47" t="n">
-        <v>555.0</v>
+        <v>15413.0</v>
       </c>
       <c r="I47" t="n">
-        <v>103.0</v>
+        <v>3265.0</v>
       </c>
       <c r="J47" t="n">
-        <v>373.0</v>
+        <v>1889.0</v>
       </c>
       <c r="K47" t="n">
-        <v>6.0</v>
+        <v>11.0</v>
       </c>
       <c r="L47" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="M47" t="n">
-        <v>0.0</v>
+        <v>26.0</v>
       </c>
       <c r="N47" t="s">
         <v>120</v>
       </c>
       <c r="O47" t="n">
-        <v>0.0</v>
+        <v>156.0</v>
       </c>
       <c r="P47" t="n">
-        <v>0.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q47" t="n">
-        <v>2377.0</v>
+        <v>32716.0</v>
       </c>
       <c r="R47" t="n">
-        <v>1.0</v>
+        <v>35.0</v>
       </c>
       <c r="S47" t="n">
-        <v>7471.0</v>
+        <v>64695.0</v>
       </c>
       <c r="T47" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="U47" t="n" s="2">
-        <v>43360.0</v>
+        <v>43230.0</v>
       </c>
       <c r="V47" t="n">
-        <v>49.0</v>
+        <v>179.0</v>
       </c>
     </row>
     <row r="48">
@@ -3666,64 +3663,64 @@
         <v>117</v>
       </c>
       <c r="C48" t="n">
-        <v>9.0</v>
+        <v>11.0</v>
       </c>
       <c r="D48" t="n">
-        <v>3010.0</v>
+        <v>4218.0</v>
       </c>
       <c r="E48" t="n">
-        <v>3010.0</v>
+        <v>4325.0</v>
       </c>
       <c r="F48" t="n">
-        <v>377.0</v>
+        <v>6352.0</v>
       </c>
       <c r="G48" t="n">
-        <v>219.0</v>
+        <v>6601.0</v>
       </c>
       <c r="H48" t="n">
-        <v>1545.0</v>
+        <v>18186.0</v>
       </c>
       <c r="I48" t="n">
-        <v>264.0</v>
+        <v>3759.0</v>
       </c>
       <c r="J48" t="n">
-        <v>147.0</v>
+        <v>4372.0</v>
       </c>
       <c r="K48" t="n">
         <v>10.0</v>
       </c>
       <c r="L48" t="n">
-        <v>0.0</v>
+        <v>47.0</v>
       </c>
       <c r="M48" t="n">
-        <v>0.0</v>
+        <v>459.0</v>
       </c>
       <c r="N48" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="O48" t="n">
-        <v>0.0</v>
+        <v>24.0</v>
       </c>
       <c r="P48" t="n">
-        <v>0.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q48" t="n">
-        <v>4091.0</v>
+        <v>20651.0</v>
       </c>
       <c r="R48" t="n">
-        <v>0.0</v>
+        <v>56.0</v>
       </c>
       <c r="S48" t="n">
-        <v>0.0</v>
+        <v>72677.0</v>
       </c>
       <c r="T48" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="U48" t="n" s="2">
-        <v>43409.0</v>
+        <v>43184.0</v>
       </c>
       <c r="V48" t="n">
-        <v>0.0</v>
+        <v>225.0</v>
       </c>
     </row>
     <row r="49">
@@ -3734,37 +3731,37 @@
         <v>118</v>
       </c>
       <c r="C49" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="D49" t="n">
-        <v>2907.0</v>
+        <v>4181.0</v>
       </c>
       <c r="E49" t="n">
-        <v>3176.0</v>
+        <v>4619.0</v>
       </c>
       <c r="F49" t="n">
-        <v>3245.0</v>
+        <v>6346.0</v>
       </c>
       <c r="G49" t="n">
-        <v>4540.0</v>
+        <v>6138.0</v>
       </c>
       <c r="H49" t="n">
-        <v>9090.0</v>
+        <v>14012.0</v>
       </c>
       <c r="I49" t="n">
-        <v>2928.0</v>
+        <v>2651.0</v>
       </c>
       <c r="J49" t="n">
-        <v>444.0</v>
+        <v>6501.0</v>
       </c>
       <c r="K49" t="n">
         <v>10.0</v>
       </c>
       <c r="L49" t="n">
-        <v>0.0</v>
+        <v>60.0</v>
       </c>
       <c r="M49" t="n">
-        <v>0.0</v>
+        <v>93.0</v>
       </c>
       <c r="N49" t="s">
         <v>120</v>
@@ -3773,25 +3770,25 @@
         <v>0.0</v>
       </c>
       <c r="P49" t="n">
-        <v>0.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q49" t="n">
-        <v>37407.0</v>
+        <v>46903.0</v>
       </c>
       <c r="R49" t="n">
-        <v>26.0</v>
+        <v>27.0</v>
       </c>
       <c r="S49" t="n">
-        <v>42987.0</v>
+        <v>40920.0</v>
       </c>
       <c r="T49" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="U49" t="n" s="2">
-        <v>43151.0</v>
+        <v>43314.0</v>
       </c>
       <c r="V49" t="n">
-        <v>258.0</v>
+        <v>95.0</v>
       </c>
     </row>
     <row r="50">
@@ -3802,64 +3799,64 @@
         <v>119</v>
       </c>
       <c r="C50" t="n">
-        <v>7.0</v>
+        <v>10.0</v>
       </c>
       <c r="D50" t="n">
-        <v>2264.0</v>
+        <v>3901.0</v>
       </c>
       <c r="E50" t="n">
-        <v>2297.0</v>
+        <v>3901.0</v>
       </c>
       <c r="F50" t="n">
+        <v>853.0</v>
+      </c>
+      <c r="G50" t="n">
+        <v>729.0</v>
+      </c>
+      <c r="H50" t="n">
+        <v>3868.0</v>
+      </c>
+      <c r="I50" t="n">
+        <v>892.0</v>
+      </c>
+      <c r="J50" t="n">
+        <v>535.0</v>
+      </c>
+      <c r="K50" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="L50" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M50" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N50" t="s">
+        <v>121</v>
+      </c>
+      <c r="O50" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P50" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q50" t="n">
+        <v>24388.0</v>
+      </c>
+      <c r="R50" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="S50" t="n">
+        <v>13894.0</v>
+      </c>
+      <c r="T50" t="s">
+        <v>126</v>
+      </c>
+      <c r="U50" t="n" s="2">
+        <v>43254.0</v>
+      </c>
+      <c r="V50" t="n">
         <v>155.0</v>
-      </c>
-      <c r="G50" t="n">
-        <v>80.0</v>
-      </c>
-      <c r="H50" t="n">
-        <v>275.0</v>
-      </c>
-      <c r="I50" t="n">
-        <v>72.0</v>
-      </c>
-      <c r="J50" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K50" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L50" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M50" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N50" t="s">
-        <v>120</v>
-      </c>
-      <c r="O50" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P50" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q50" t="n">
-        <v>929.0</v>
-      </c>
-      <c r="R50" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="S50" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="T50" t="s">
-        <v>131</v>
-      </c>
-      <c r="U50" t="n" s="2">
-        <v>43376.0</v>
-      </c>
-      <c r="V50" t="n">
-        <v>33.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Restructuring of HTML generation. Sort doesn't work.
</commit_message>
<xml_diff>
--- a/docs/data/memberstats.xlsx
+++ b/docs/data/memberstats.xlsx
@@ -544,22 +544,22 @@
         <v>11.0</v>
       </c>
       <c r="D2" t="n">
-        <v>4333.0</v>
+        <v>4396.0</v>
       </c>
       <c r="E2" t="n">
         <v>4653.0</v>
       </c>
       <c r="F2" t="n">
-        <v>2230.0</v>
+        <v>2234.0</v>
       </c>
       <c r="G2" t="n">
-        <v>2075.0</v>
+        <v>2077.0</v>
       </c>
       <c r="H2" t="n">
-        <v>6981.0</v>
+        <v>6993.0</v>
       </c>
       <c r="I2" t="n">
-        <v>1146.0</v>
+        <v>1147.0</v>
       </c>
       <c r="J2" t="n">
         <v>2664.0</v>
@@ -577,19 +577,19 @@
         <v>122</v>
       </c>
       <c r="O2" t="n">
-        <v>302.0</v>
+        <v>466.0</v>
       </c>
       <c r="P2" t="n">
-        <v>200.0</v>
+        <v>280.0</v>
       </c>
       <c r="Q2" t="n">
-        <v>27652.0</v>
+        <v>27816.0</v>
       </c>
       <c r="R2" t="n">
-        <v>42.0</v>
+        <v>43.0</v>
       </c>
       <c r="S2" t="n">
-        <v>79500.0</v>
+        <v>80620.0</v>
       </c>
       <c r="T2" t="s">
         <v>126</v>
@@ -598,7 +598,7 @@
         <v>43302.0</v>
       </c>
       <c r="V2" t="n">
-        <v>109.0</v>
+        <v>110.0</v>
       </c>
     </row>
     <row r="3">
@@ -624,7 +624,7 @@
         <v>1431.0</v>
       </c>
       <c r="H3" t="n">
-        <v>4290.0</v>
+        <v>4293.0</v>
       </c>
       <c r="I3" t="n">
         <v>828.0</v>
@@ -645,19 +645,19 @@
         <v>123</v>
       </c>
       <c r="O3" t="n">
-        <v>155.0</v>
+        <v>239.0</v>
       </c>
       <c r="P3" t="n">
-        <v>80.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q3" t="n">
-        <v>17974.0</v>
+        <v>18058.0</v>
       </c>
       <c r="R3" t="n">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
       <c r="S3" t="n">
-        <v>28360.0</v>
+        <v>29760.0</v>
       </c>
       <c r="T3" t="s">
         <v>127</v>
@@ -666,7 +666,7 @@
         <v>43372.0</v>
       </c>
       <c r="V3" t="n">
-        <v>39.0</v>
+        <v>40.0</v>
       </c>
     </row>
     <row r="4">
@@ -680,19 +680,19 @@
         <v>11.0</v>
       </c>
       <c r="D4" t="n">
-        <v>4081.0</v>
+        <v>4084.0</v>
       </c>
       <c r="E4" t="n">
         <v>4254.0</v>
       </c>
       <c r="F4" t="n">
-        <v>2572.0</v>
+        <v>2573.0</v>
       </c>
       <c r="G4" t="n">
-        <v>2615.0</v>
+        <v>2616.0</v>
       </c>
       <c r="H4" t="n">
-        <v>6180.0</v>
+        <v>6184.0</v>
       </c>
       <c r="I4" t="n">
         <v>1064.0</v>
@@ -716,16 +716,16 @@
         <v>26.0</v>
       </c>
       <c r="P4" t="n">
-        <v>240.0</v>
+        <v>320.0</v>
       </c>
       <c r="Q4" t="n">
         <v>8936.0</v>
       </c>
       <c r="R4" t="n">
-        <v>42.0</v>
+        <v>43.0</v>
       </c>
       <c r="S4" t="n">
-        <v>58846.0</v>
+        <v>59126.0</v>
       </c>
       <c r="T4" t="s">
         <v>127</v>
@@ -734,7 +734,7 @@
         <v>43082.0</v>
       </c>
       <c r="V4" t="n">
-        <v>329.0</v>
+        <v>330.0</v>
       </c>
     </row>
     <row r="5">
@@ -757,16 +757,16 @@
         <v>700.0</v>
       </c>
       <c r="G5" t="n">
-        <v>649.0</v>
+        <v>652.0</v>
       </c>
       <c r="H5" t="n">
-        <v>1975.0</v>
+        <v>1980.0</v>
       </c>
       <c r="I5" t="n">
         <v>384.0</v>
       </c>
       <c r="J5" t="n">
-        <v>1428.0</v>
+        <v>1430.0</v>
       </c>
       <c r="K5" t="n">
         <v>10.0</v>
@@ -781,13 +781,13 @@
         <v>123</v>
       </c>
       <c r="O5" t="n">
-        <v>339.0</v>
+        <v>10.0</v>
       </c>
       <c r="P5" t="n">
-        <v>160.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q5" t="n">
-        <v>16675.0</v>
+        <v>16795.0</v>
       </c>
       <c r="R5" t="n">
         <v>4.0</v>
@@ -802,7 +802,7 @@
         <v>43397.0</v>
       </c>
       <c r="V5" t="n">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="6">
@@ -849,13 +849,13 @@
         <v>123</v>
       </c>
       <c r="O6" t="n">
-        <v>384.0</v>
+        <v>474.0</v>
       </c>
       <c r="P6" t="n">
-        <v>233.0</v>
+        <v>320.0</v>
       </c>
       <c r="Q6" t="n">
-        <v>15642.0</v>
+        <v>15732.0</v>
       </c>
       <c r="R6" t="n">
         <v>28.0</v>
@@ -870,7 +870,7 @@
         <v>43356.0</v>
       </c>
       <c r="V6" t="n">
-        <v>55.0</v>
+        <v>56.0</v>
       </c>
     </row>
     <row r="7">
@@ -926,7 +926,7 @@
         <v>2125.0</v>
       </c>
       <c r="R7" t="n">
-        <v>39.0</v>
+        <v>40.0</v>
       </c>
       <c r="S7" t="n">
         <v>55120.0</v>
@@ -938,7 +938,7 @@
         <v>43364.0</v>
       </c>
       <c r="V7" t="n">
-        <v>47.0</v>
+        <v>48.0</v>
       </c>
     </row>
     <row r="8">
@@ -952,22 +952,22 @@
         <v>11.0</v>
       </c>
       <c r="D8" t="n">
-        <v>4258.0</v>
+        <v>4291.0</v>
       </c>
       <c r="E8" t="n">
         <v>4497.0</v>
       </c>
       <c r="F8" t="n">
-        <v>1897.0</v>
+        <v>1902.0</v>
       </c>
       <c r="G8" t="n">
-        <v>1799.0</v>
+        <v>1803.0</v>
       </c>
       <c r="H8" t="n">
-        <v>7548.0</v>
+        <v>7560.0</v>
       </c>
       <c r="I8" t="n">
-        <v>1111.0</v>
+        <v>1112.0</v>
       </c>
       <c r="J8" t="n">
         <v>1384.0</v>
@@ -985,19 +985,19 @@
         <v>124</v>
       </c>
       <c r="O8" t="n">
-        <v>102.0</v>
+        <v>110.0</v>
       </c>
       <c r="P8" t="n">
-        <v>200.0</v>
+        <v>280.0</v>
       </c>
       <c r="Q8" t="n">
-        <v>24997.0</v>
+        <v>25005.0</v>
       </c>
       <c r="R8" t="n">
         <v>56.0</v>
       </c>
       <c r="S8" t="n">
-        <v>67035.0</v>
+        <v>68155.0</v>
       </c>
       <c r="T8" t="s">
         <v>127</v>
@@ -1006,7 +1006,7 @@
         <v>43058.0</v>
       </c>
       <c r="V8" t="n">
-        <v>353.0</v>
+        <v>354.0</v>
       </c>
     </row>
     <row r="9">
@@ -1020,19 +1020,19 @@
         <v>11.0</v>
       </c>
       <c r="D9" t="n">
-        <v>4179.0</v>
+        <v>4131.0</v>
       </c>
       <c r="E9" t="n">
         <v>4496.0</v>
       </c>
       <c r="F9" t="n">
-        <v>2321.0</v>
+        <v>2324.0</v>
       </c>
       <c r="G9" t="n">
-        <v>2251.0</v>
+        <v>2256.0</v>
       </c>
       <c r="H9" t="n">
-        <v>5107.0</v>
+        <v>5116.0</v>
       </c>
       <c r="I9" t="n">
         <v>893.0</v>
@@ -1053,19 +1053,19 @@
         <v>123</v>
       </c>
       <c r="O9" t="n">
-        <v>128.0</v>
+        <v>180.0</v>
       </c>
       <c r="P9" t="n">
-        <v>80.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q9" t="n">
-        <v>24779.0</v>
+        <v>24831.0</v>
       </c>
       <c r="R9" t="n">
         <v>13.0</v>
       </c>
       <c r="S9" t="n">
-        <v>50432.0</v>
+        <v>50712.0</v>
       </c>
       <c r="T9" t="s">
         <v>127</v>
@@ -1074,7 +1074,7 @@
         <v>43390.0</v>
       </c>
       <c r="V9" t="n">
-        <v>21.0</v>
+        <v>22.0</v>
       </c>
     </row>
     <row r="10">
@@ -1142,7 +1142,7 @@
         <v>43123.0</v>
       </c>
       <c r="V10" t="n">
-        <v>288.0</v>
+        <v>289.0</v>
       </c>
     </row>
     <row r="11">
@@ -1156,22 +1156,22 @@
         <v>11.0</v>
       </c>
       <c r="D11" t="n">
-        <v>4252.0</v>
+        <v>4317.0</v>
       </c>
       <c r="E11" t="n">
         <v>4501.0</v>
       </c>
       <c r="F11" t="n">
-        <v>2346.0</v>
+        <v>2363.0</v>
       </c>
       <c r="G11" t="n">
-        <v>2183.0</v>
+        <v>2199.0</v>
       </c>
       <c r="H11" t="n">
-        <v>10560.0</v>
+        <v>10596.0</v>
       </c>
       <c r="I11" t="n">
-        <v>2352.0</v>
+        <v>2355.0</v>
       </c>
       <c r="J11" t="n">
         <v>1906.0</v>
@@ -1192,25 +1192,25 @@
         <v>30.0</v>
       </c>
       <c r="P11" t="n">
-        <v>320.0</v>
+        <v>400.0</v>
       </c>
       <c r="Q11" t="n">
         <v>3162.0</v>
       </c>
       <c r="R11" t="n">
-        <v>55.0</v>
+        <v>56.0</v>
       </c>
       <c r="S11" t="n">
-        <v>76550.0</v>
+        <v>77390.0</v>
       </c>
       <c r="T11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="U11" t="n" s="2">
         <v>43123.0</v>
       </c>
       <c r="V11" t="n">
-        <v>288.0</v>
+        <v>289.0</v>
       </c>
     </row>
     <row r="12">
@@ -1236,10 +1236,10 @@
         <v>1752.0</v>
       </c>
       <c r="H12" t="n">
-        <v>9393.0</v>
+        <v>9397.0</v>
       </c>
       <c r="I12" t="n">
-        <v>1360.0</v>
+        <v>1361.0</v>
       </c>
       <c r="J12" t="n">
         <v>4199.0</v>
@@ -1257,16 +1257,16 @@
         <v>123</v>
       </c>
       <c r="O12" t="n">
-        <v>498.0</v>
+        <v>594.0</v>
       </c>
       <c r="P12" t="n">
-        <v>280.0</v>
+        <v>360.0</v>
       </c>
       <c r="Q12" t="n">
-        <v>88895.0</v>
+        <v>88991.0</v>
       </c>
       <c r="R12" t="n">
-        <v>73.0</v>
+        <v>74.0</v>
       </c>
       <c r="S12" t="n">
         <v>72320.0</v>
@@ -1278,7 +1278,7 @@
         <v>43397.0</v>
       </c>
       <c r="V12" t="n">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="13">
@@ -1292,22 +1292,22 @@
         <v>11.0</v>
       </c>
       <c r="D13" t="n">
-        <v>3960.0</v>
+        <v>3920.0</v>
       </c>
       <c r="E13" t="n">
         <v>4163.0</v>
       </c>
       <c r="F13" t="n">
-        <v>3148.0</v>
+        <v>3152.0</v>
       </c>
       <c r="G13" t="n">
-        <v>3323.0</v>
+        <v>3329.0</v>
       </c>
       <c r="H13" t="n">
-        <v>8566.0</v>
+        <v>8579.0</v>
       </c>
       <c r="I13" t="n">
-        <v>1339.0</v>
+        <v>1340.0</v>
       </c>
       <c r="J13" t="n">
         <v>1906.0</v>
@@ -1334,10 +1334,10 @@
         <v>14241.0</v>
       </c>
       <c r="R13" t="n">
-        <v>17.0</v>
+        <v>18.0</v>
       </c>
       <c r="S13" t="n">
-        <v>28929.0</v>
+        <v>29191.0</v>
       </c>
       <c r="T13" t="s">
         <v>129</v>
@@ -1346,7 +1346,7 @@
         <v>43218.0</v>
       </c>
       <c r="V13" t="n">
-        <v>193.0</v>
+        <v>194.0</v>
       </c>
     </row>
     <row r="14">
@@ -1372,7 +1372,7 @@
         <v>1199.0</v>
       </c>
       <c r="H14" t="n">
-        <v>5485.0</v>
+        <v>5488.0</v>
       </c>
       <c r="I14" t="n">
         <v>757.0</v>
@@ -1393,19 +1393,19 @@
         <v>124</v>
       </c>
       <c r="O14" t="n">
-        <v>328.0</v>
+        <v>370.0</v>
       </c>
       <c r="P14" t="n">
-        <v>280.0</v>
+        <v>360.0</v>
       </c>
       <c r="Q14" t="n">
-        <v>37537.0</v>
+        <v>37579.0</v>
       </c>
       <c r="R14" t="n">
-        <v>60.0</v>
+        <v>61.0</v>
       </c>
       <c r="S14" t="n">
-        <v>72200.0</v>
+        <v>73320.0</v>
       </c>
       <c r="T14" t="s">
         <v>127</v>
@@ -1414,7 +1414,7 @@
         <v>43218.0</v>
       </c>
       <c r="V14" t="n">
-        <v>193.0</v>
+        <v>194.0</v>
       </c>
     </row>
     <row r="15">
@@ -1428,22 +1428,22 @@
         <v>12.0</v>
       </c>
       <c r="D15" t="n">
-        <v>4248.0</v>
+        <v>4230.0</v>
       </c>
       <c r="E15" t="n">
         <v>4521.0</v>
       </c>
       <c r="F15" t="n">
-        <v>4603.0</v>
+        <v>4607.0</v>
       </c>
       <c r="G15" t="n">
-        <v>5016.0</v>
+        <v>5021.0</v>
       </c>
       <c r="H15" t="n">
-        <v>10670.0</v>
+        <v>10685.0</v>
       </c>
       <c r="I15" t="n">
-        <v>2062.0</v>
+        <v>2064.0</v>
       </c>
       <c r="J15" t="n">
         <v>1842.0</v>
@@ -1461,19 +1461,19 @@
         <v>123</v>
       </c>
       <c r="O15" t="n">
-        <v>364.0</v>
+        <v>474.0</v>
       </c>
       <c r="P15" t="n">
-        <v>240.0</v>
+        <v>320.0</v>
       </c>
       <c r="Q15" t="n">
-        <v>52555.0</v>
+        <v>52665.0</v>
       </c>
       <c r="R15" t="n">
         <v>30.0</v>
       </c>
       <c r="S15" t="n">
-        <v>78050.0</v>
+        <v>78890.0</v>
       </c>
       <c r="T15" t="s">
         <v>127</v>
@@ -1482,7 +1482,7 @@
         <v>43390.0</v>
       </c>
       <c r="V15" t="n">
-        <v>21.0</v>
+        <v>22.0</v>
       </c>
     </row>
     <row r="16">
@@ -1550,7 +1550,7 @@
         <v>43410.0</v>
       </c>
       <c r="V16" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="17">
@@ -1564,22 +1564,22 @@
         <v>11.0</v>
       </c>
       <c r="D17" t="n">
-        <v>4107.0</v>
+        <v>4094.0</v>
       </c>
       <c r="E17" t="n">
         <v>4416.0</v>
       </c>
       <c r="F17" t="n">
-        <v>2268.0</v>
+        <v>2272.0</v>
       </c>
       <c r="G17" t="n">
-        <v>2070.0</v>
+        <v>2075.0</v>
       </c>
       <c r="H17" t="n">
-        <v>6690.0</v>
+        <v>6699.0</v>
       </c>
       <c r="I17" t="n">
-        <v>1075.0</v>
+        <v>1079.0</v>
       </c>
       <c r="J17" t="n">
         <v>3630.0</v>
@@ -1600,7 +1600,7 @@
         <v>50.0</v>
       </c>
       <c r="P17" t="n">
-        <v>200.0</v>
+        <v>230.0</v>
       </c>
       <c r="Q17" t="n">
         <v>20415.0</v>
@@ -1618,7 +1618,7 @@
         <v>43275.0</v>
       </c>
       <c r="V17" t="n">
-        <v>136.0</v>
+        <v>137.0</v>
       </c>
     </row>
     <row r="18">
@@ -1665,16 +1665,16 @@
         <v>122</v>
       </c>
       <c r="O18" t="n">
-        <v>171.0</v>
+        <v>303.0</v>
       </c>
       <c r="P18" t="n">
-        <v>210.0</v>
+        <v>270.0</v>
       </c>
       <c r="Q18" t="n">
-        <v>30467.0</v>
+        <v>30599.0</v>
       </c>
       <c r="R18" t="n">
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
       <c r="S18" t="n">
         <v>25113.0</v>
@@ -1686,7 +1686,7 @@
         <v>43220.0</v>
       </c>
       <c r="V18" t="n">
-        <v>191.0</v>
+        <v>192.0</v>
       </c>
     </row>
     <row r="19">
@@ -1700,22 +1700,22 @@
         <v>11.0</v>
       </c>
       <c r="D19" t="n">
-        <v>4230.0</v>
+        <v>4263.0</v>
       </c>
       <c r="E19" t="n">
         <v>4577.0</v>
       </c>
       <c r="F19" t="n">
-        <v>2744.0</v>
+        <v>2747.0</v>
       </c>
       <c r="G19" t="n">
-        <v>2513.0</v>
+        <v>2515.0</v>
       </c>
       <c r="H19" t="n">
-        <v>6530.0</v>
+        <v>6538.0</v>
       </c>
       <c r="I19" t="n">
-        <v>703.0</v>
+        <v>707.0</v>
       </c>
       <c r="J19" t="n">
         <v>3595.0</v>
@@ -1733,19 +1733,19 @@
         <v>122</v>
       </c>
       <c r="O19" t="n">
-        <v>66.0</v>
+        <v>92.0</v>
       </c>
       <c r="P19" t="n">
-        <v>200.0</v>
+        <v>280.0</v>
       </c>
       <c r="Q19" t="n">
-        <v>21710.0</v>
+        <v>21736.0</v>
       </c>
       <c r="R19" t="n">
         <v>47.0</v>
       </c>
       <c r="S19" t="n">
-        <v>75065.0</v>
+        <v>76465.0</v>
       </c>
       <c r="T19" t="s">
         <v>127</v>
@@ -1754,7 +1754,7 @@
         <v>43058.0</v>
       </c>
       <c r="V19" t="n">
-        <v>353.0</v>
+        <v>354.0</v>
       </c>
     </row>
     <row r="20">
@@ -1801,13 +1801,13 @@
         <v>122</v>
       </c>
       <c r="O20" t="n">
-        <v>207.0</v>
+        <v>242.0</v>
       </c>
       <c r="P20" t="n">
-        <v>160.0</v>
+        <v>210.0</v>
       </c>
       <c r="Q20" t="n">
-        <v>45289.0</v>
+        <v>45324.0</v>
       </c>
       <c r="R20" t="n">
         <v>34.0</v>
@@ -1822,7 +1822,7 @@
         <v>43312.0</v>
       </c>
       <c r="V20" t="n">
-        <v>99.0</v>
+        <v>100.0</v>
       </c>
     </row>
     <row r="21">
@@ -1836,22 +1836,22 @@
         <v>12.0</v>
       </c>
       <c r="D21" t="n">
-        <v>4408.0</v>
+        <v>4429.0</v>
       </c>
       <c r="E21" t="n">
         <v>4767.0</v>
       </c>
       <c r="F21" t="n">
-        <v>6685.0</v>
+        <v>6695.0</v>
       </c>
       <c r="G21" t="n">
-        <v>6640.0</v>
+        <v>6650.0</v>
       </c>
       <c r="H21" t="n">
-        <v>23554.0</v>
+        <v>23594.0</v>
       </c>
       <c r="I21" t="n">
-        <v>2760.0</v>
+        <v>2764.0</v>
       </c>
       <c r="J21" t="n">
         <v>2570.0</v>
@@ -1869,19 +1869,19 @@
         <v>125</v>
       </c>
       <c r="O21" t="n">
-        <v>276.0</v>
+        <v>338.0</v>
       </c>
       <c r="P21" t="n">
-        <v>310.0</v>
+        <v>390.0</v>
       </c>
       <c r="Q21" t="n">
-        <v>67205.0</v>
+        <v>67267.0</v>
       </c>
       <c r="R21" t="n">
-        <v>86.0</v>
+        <v>87.0</v>
       </c>
       <c r="S21" t="n">
-        <v>81055.0</v>
+        <v>81895.0</v>
       </c>
       <c r="T21" t="s">
         <v>126</v>
@@ -1890,7 +1890,7 @@
         <v>42705.0</v>
       </c>
       <c r="V21" t="n">
-        <v>706.0</v>
+        <v>707.0</v>
       </c>
     </row>
     <row r="22">
@@ -1937,13 +1937,13 @@
         <v>123</v>
       </c>
       <c r="O22" t="n">
-        <v>118.0</v>
+        <v>214.0</v>
       </c>
       <c r="P22" t="n">
-        <v>60.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q22" t="n">
-        <v>37525.0</v>
+        <v>37621.0</v>
       </c>
       <c r="R22" t="n">
         <v>26.0</v>
@@ -1958,7 +1958,7 @@
         <v>43151.0</v>
       </c>
       <c r="V22" t="n">
-        <v>260.0</v>
+        <v>261.0</v>
       </c>
     </row>
     <row r="23">
@@ -1984,7 +1984,7 @@
         <v>1395.0</v>
       </c>
       <c r="H23" t="n">
-        <v>4566.0</v>
+        <v>4567.0</v>
       </c>
       <c r="I23" t="n">
         <v>872.0</v>
@@ -2017,7 +2017,7 @@
         <v>25.0</v>
       </c>
       <c r="S23" t="n">
-        <v>45901.0</v>
+        <v>46181.0</v>
       </c>
       <c r="T23" t="s">
         <v>127</v>
@@ -2026,7 +2026,7 @@
         <v>43254.0</v>
       </c>
       <c r="V23" t="n">
-        <v>157.0</v>
+        <v>158.0</v>
       </c>
     </row>
     <row r="24">
@@ -2040,19 +2040,19 @@
         <v>11.0</v>
       </c>
       <c r="D24" t="n">
-        <v>4148.0</v>
+        <v>4152.0</v>
       </c>
       <c r="E24" t="n">
         <v>4345.0</v>
       </c>
       <c r="F24" t="n">
-        <v>1884.0</v>
+        <v>1885.0</v>
       </c>
       <c r="G24" t="n">
-        <v>1793.0</v>
+        <v>1794.0</v>
       </c>
       <c r="H24" t="n">
-        <v>7970.0</v>
+        <v>7972.0</v>
       </c>
       <c r="I24" t="n">
         <v>2049.0</v>
@@ -2073,13 +2073,13 @@
         <v>123</v>
       </c>
       <c r="O24" t="n">
-        <v>58.0</v>
+        <v>68.0</v>
       </c>
       <c r="P24" t="n">
-        <v>40.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q24" t="n">
-        <v>55674.0</v>
+        <v>55684.0</v>
       </c>
       <c r="R24" t="n">
         <v>29.0</v>
@@ -2094,7 +2094,7 @@
         <v>43380.0</v>
       </c>
       <c r="V24" t="n">
-        <v>31.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="25">
@@ -2120,10 +2120,10 @@
         <v>4355.0</v>
       </c>
       <c r="H25" t="n">
-        <v>18398.0</v>
+        <v>18412.0</v>
       </c>
       <c r="I25" t="n">
-        <v>2927.0</v>
+        <v>2928.0</v>
       </c>
       <c r="J25" t="n">
         <v>2740.0</v>
@@ -2135,7 +2135,7 @@
         <v>2641.0</v>
       </c>
       <c r="M25" t="n">
-        <v>15729.0</v>
+        <v>15763.0</v>
       </c>
       <c r="N25" t="s">
         <v>124</v>
@@ -2144,16 +2144,16 @@
         <v>52.0</v>
       </c>
       <c r="P25" t="n">
-        <v>320.0</v>
+        <v>390.0</v>
       </c>
       <c r="Q25" t="n">
         <v>6312.0</v>
       </c>
       <c r="R25" t="n">
-        <v>78.0</v>
+        <v>79.0</v>
       </c>
       <c r="S25" t="n">
-        <v>77465.0</v>
+        <v>78585.0</v>
       </c>
       <c r="T25" t="s">
         <v>127</v>
@@ -2162,7 +2162,7 @@
         <v>42614.0</v>
       </c>
       <c r="V25" t="n">
-        <v>797.0</v>
+        <v>798.0</v>
       </c>
     </row>
     <row r="26">
@@ -2218,7 +2218,7 @@
         <v>9620.0</v>
       </c>
       <c r="R26" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="S26" t="n">
         <v>23129.0</v>
@@ -2230,7 +2230,7 @@
         <v>43400.0</v>
       </c>
       <c r="V26" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="27">
@@ -2256,10 +2256,10 @@
         <v>3486.0</v>
       </c>
       <c r="H27" t="n">
-        <v>12175.0</v>
+        <v>12183.0</v>
       </c>
       <c r="I27" t="n">
-        <v>1687.0</v>
+        <v>1689.0</v>
       </c>
       <c r="J27" t="n">
         <v>2757.0</v>
@@ -2277,19 +2277,19 @@
         <v>122</v>
       </c>
       <c r="O27" t="n">
-        <v>573.0</v>
+        <v>599.0</v>
       </c>
       <c r="P27" t="n">
-        <v>200.0</v>
+        <v>240.0</v>
       </c>
       <c r="Q27" t="n">
-        <v>41873.0</v>
+        <v>41899.0</v>
       </c>
       <c r="R27" t="n">
-        <v>64.0</v>
+        <v>65.0</v>
       </c>
       <c r="S27" t="n">
-        <v>70603.0</v>
+        <v>71723.0</v>
       </c>
       <c r="T27" t="s">
         <v>127</v>
@@ -2298,7 +2298,7 @@
         <v>43214.0</v>
       </c>
       <c r="V27" t="n">
-        <v>197.0</v>
+        <v>198.0</v>
       </c>
     </row>
     <row r="28">
@@ -2324,7 +2324,7 @@
         <v>3408.0</v>
       </c>
       <c r="H28" t="n">
-        <v>11339.0</v>
+        <v>11342.0</v>
       </c>
       <c r="I28" t="n">
         <v>1547.0</v>
@@ -2357,7 +2357,7 @@
         <v>60.0</v>
       </c>
       <c r="S28" t="n">
-        <v>73115.0</v>
+        <v>74515.0</v>
       </c>
       <c r="T28" t="s">
         <v>126</v>
@@ -2366,7 +2366,7 @@
         <v>42614.0</v>
       </c>
       <c r="V28" t="n">
-        <v>797.0</v>
+        <v>798.0</v>
       </c>
     </row>
     <row r="29">
@@ -2434,7 +2434,7 @@
         <v>43254.0</v>
       </c>
       <c r="V29" t="n">
-        <v>157.0</v>
+        <v>158.0</v>
       </c>
     </row>
     <row r="30">
@@ -2460,10 +2460,10 @@
         <v>1117.0</v>
       </c>
       <c r="H30" t="n">
-        <v>6503.0</v>
+        <v>6515.0</v>
       </c>
       <c r="I30" t="n">
-        <v>1431.0</v>
+        <v>1433.0</v>
       </c>
       <c r="J30" t="n">
         <v>1859.0</v>
@@ -2481,19 +2481,19 @@
         <v>122</v>
       </c>
       <c r="O30" t="n">
-        <v>266.0</v>
+        <v>350.0</v>
       </c>
       <c r="P30" t="n">
-        <v>240.0</v>
+        <v>320.0</v>
       </c>
       <c r="Q30" t="n">
-        <v>12340.0</v>
+        <v>12424.0</v>
       </c>
       <c r="R30" t="n">
         <v>55.0</v>
       </c>
       <c r="S30" t="n">
-        <v>73142.0</v>
+        <v>74542.0</v>
       </c>
       <c r="T30" t="s">
         <v>127</v>
@@ -2502,7 +2502,7 @@
         <v>43058.0</v>
       </c>
       <c r="V30" t="n">
-        <v>353.0</v>
+        <v>354.0</v>
       </c>
     </row>
     <row r="31">
@@ -2558,7 +2558,7 @@
         <v>4623.0</v>
       </c>
       <c r="R31" t="n">
-        <v>51.0</v>
+        <v>52.0</v>
       </c>
       <c r="S31" t="n">
         <v>64740.0</v>
@@ -2570,7 +2570,7 @@
         <v>43138.0</v>
       </c>
       <c r="V31" t="n">
-        <v>273.0</v>
+        <v>274.0</v>
       </c>
     </row>
     <row r="32">
@@ -2617,16 +2617,16 @@
         <v>122</v>
       </c>
       <c r="O32" t="n">
-        <v>130.0</v>
+        <v>214.0</v>
       </c>
       <c r="P32" t="n">
         <v>200.0</v>
       </c>
       <c r="Q32" t="n">
-        <v>42109.0</v>
+        <v>42193.0</v>
       </c>
       <c r="R32" t="n">
-        <v>35.0</v>
+        <v>36.0</v>
       </c>
       <c r="S32" t="n">
         <v>68593.0</v>
@@ -2638,7 +2638,7 @@
         <v>42920.0</v>
       </c>
       <c r="V32" t="n">
-        <v>491.0</v>
+        <v>492.0</v>
       </c>
     </row>
     <row r="33">
@@ -2652,19 +2652,19 @@
         <v>12.0</v>
       </c>
       <c r="D33" t="n">
-        <v>4408.0</v>
+        <v>4357.0</v>
       </c>
       <c r="E33" t="n">
         <v>4798.0</v>
       </c>
       <c r="F33" t="n">
-        <v>5114.0</v>
+        <v>5116.0</v>
       </c>
       <c r="G33" t="n">
-        <v>5226.0</v>
+        <v>5230.0</v>
       </c>
       <c r="H33" t="n">
-        <v>12266.0</v>
+        <v>12272.0</v>
       </c>
       <c r="I33" t="n">
         <v>2235.0</v>
@@ -2685,13 +2685,13 @@
         <v>122</v>
       </c>
       <c r="O33" t="n">
-        <v>136.0</v>
+        <v>194.0</v>
       </c>
       <c r="P33" t="n">
         <v>40.0</v>
       </c>
       <c r="Q33" t="n">
-        <v>58873.0</v>
+        <v>58931.0</v>
       </c>
       <c r="R33" t="n">
         <v>30.0</v>
@@ -2706,7 +2706,7 @@
         <v>43058.0</v>
       </c>
       <c r="V33" t="n">
-        <v>353.0</v>
+        <v>354.0</v>
       </c>
     </row>
     <row r="34">
@@ -2774,7 +2774,7 @@
         <v>43409.0</v>
       </c>
       <c r="V34" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="35">
@@ -2842,7 +2842,7 @@
         <v>43312.0</v>
       </c>
       <c r="V35" t="n">
-        <v>99.0</v>
+        <v>100.0</v>
       </c>
     </row>
     <row r="36">
@@ -2868,10 +2868,10 @@
         <v>481.0</v>
       </c>
       <c r="H36" t="n">
-        <v>3327.0</v>
+        <v>3330.0</v>
       </c>
       <c r="I36" t="n">
-        <v>688.0</v>
+        <v>689.0</v>
       </c>
       <c r="J36" t="n">
         <v>278.0</v>
@@ -2889,16 +2889,16 @@
         <v>123</v>
       </c>
       <c r="O36" t="n">
-        <v>262.0</v>
+        <v>288.0</v>
       </c>
       <c r="P36" t="n">
-        <v>200.0</v>
+        <v>280.0</v>
       </c>
       <c r="Q36" t="n">
-        <v>16833.0</v>
+        <v>16859.0</v>
       </c>
       <c r="R36" t="n">
-        <v>24.0</v>
+        <v>25.0</v>
       </c>
       <c r="S36" t="n">
         <v>58955.0</v>
@@ -2910,7 +2910,7 @@
         <v>43274.0</v>
       </c>
       <c r="V36" t="n">
-        <v>137.0</v>
+        <v>138.0</v>
       </c>
     </row>
     <row r="37">
@@ -2924,22 +2924,22 @@
         <v>10.0</v>
       </c>
       <c r="D37" t="n">
-        <v>3922.0</v>
+        <v>3945.0</v>
       </c>
       <c r="E37" t="n">
         <v>4078.0</v>
       </c>
       <c r="F37" t="n">
-        <v>3406.0</v>
+        <v>3413.0</v>
       </c>
       <c r="G37" t="n">
-        <v>3971.0</v>
+        <v>3978.0</v>
       </c>
       <c r="H37" t="n">
-        <v>9444.0</v>
+        <v>9467.0</v>
       </c>
       <c r="I37" t="n">
-        <v>1733.0</v>
+        <v>1739.0</v>
       </c>
       <c r="J37" t="n">
         <v>224.0</v>
@@ -2969,7 +2969,7 @@
         <v>34.0</v>
       </c>
       <c r="S37" t="n">
-        <v>67228.0</v>
+        <v>68068.0</v>
       </c>
       <c r="T37" t="s">
         <v>129</v>
@@ -2978,7 +2978,7 @@
         <v>43280.0</v>
       </c>
       <c r="V37" t="n">
-        <v>131.0</v>
+        <v>132.0</v>
       </c>
     </row>
     <row r="38">
@@ -2992,7 +2992,7 @@
         <v>8.0</v>
       </c>
       <c r="D38" t="n">
-        <v>3606.0</v>
+        <v>3554.0</v>
       </c>
       <c r="E38" t="n">
         <v>3630.0</v>
@@ -3001,10 +3001,10 @@
         <v>297.0</v>
       </c>
       <c r="G38" t="n">
-        <v>165.0</v>
+        <v>167.0</v>
       </c>
       <c r="H38" t="n">
-        <v>582.0</v>
+        <v>584.0</v>
       </c>
       <c r="I38" t="n">
         <v>106.0</v>
@@ -3025,13 +3025,13 @@
         <v>123</v>
       </c>
       <c r="O38" t="n">
-        <v>68.0</v>
+        <v>116.0</v>
       </c>
       <c r="P38" t="n">
-        <v>200.0</v>
+        <v>280.0</v>
       </c>
       <c r="Q38" t="n">
-        <v>2445.0</v>
+        <v>2493.0</v>
       </c>
       <c r="R38" t="n">
         <v>1.0</v>
@@ -3046,7 +3046,7 @@
         <v>43360.0</v>
       </c>
       <c r="V38" t="n">
-        <v>51.0</v>
+        <v>52.0</v>
       </c>
     </row>
     <row r="39">
@@ -3072,10 +3072,10 @@
         <v>974.0</v>
       </c>
       <c r="H39" t="n">
-        <v>4342.0</v>
+        <v>4359.0</v>
       </c>
       <c r="I39" t="n">
-        <v>452.0</v>
+        <v>454.0</v>
       </c>
       <c r="J39" t="n">
         <v>2215.0</v>
@@ -3093,19 +3093,19 @@
         <v>122</v>
       </c>
       <c r="O39" t="n">
-        <v>282.0</v>
+        <v>406.0</v>
       </c>
       <c r="P39" t="n">
-        <v>320.0</v>
+        <v>400.0</v>
       </c>
       <c r="Q39" t="n">
-        <v>25045.0</v>
+        <v>25169.0</v>
       </c>
       <c r="R39" t="n">
-        <v>37.0</v>
+        <v>38.0</v>
       </c>
       <c r="S39" t="n">
-        <v>73386.0</v>
+        <v>74506.0</v>
       </c>
       <c r="T39" t="s">
         <v>127</v>
@@ -3114,7 +3114,7 @@
         <v>43284.0</v>
       </c>
       <c r="V39" t="n">
-        <v>127.0</v>
+        <v>128.0</v>
       </c>
     </row>
     <row r="40">
@@ -3128,7 +3128,7 @@
         <v>10.0</v>
       </c>
       <c r="D40" t="n">
-        <v>4184.0</v>
+        <v>4157.0</v>
       </c>
       <c r="E40" t="n">
         <v>4405.0</v>
@@ -3137,13 +3137,13 @@
         <v>1092.0</v>
       </c>
       <c r="G40" t="n">
-        <v>991.0</v>
+        <v>992.0</v>
       </c>
       <c r="H40" t="n">
-        <v>3124.0</v>
+        <v>3127.0</v>
       </c>
       <c r="I40" t="n">
-        <v>651.0</v>
+        <v>652.0</v>
       </c>
       <c r="J40" t="n">
         <v>1700.0</v>
@@ -3161,19 +3161,19 @@
         <v>123</v>
       </c>
       <c r="O40" t="n">
-        <v>122.0</v>
+        <v>186.0</v>
       </c>
       <c r="P40" t="n">
-        <v>160.0</v>
+        <v>240.0</v>
       </c>
       <c r="Q40" t="n">
-        <v>19812.0</v>
+        <v>19876.0</v>
       </c>
       <c r="R40" t="n">
         <v>15.0</v>
       </c>
       <c r="S40" t="n">
-        <v>49440.0</v>
+        <v>50560.0</v>
       </c>
       <c r="T40" t="s">
         <v>127</v>
@@ -3182,7 +3182,7 @@
         <v>43352.0</v>
       </c>
       <c r="V40" t="n">
-        <v>59.0</v>
+        <v>60.0</v>
       </c>
     </row>
     <row r="41">
@@ -3208,10 +3208,10 @@
         <v>4693.0</v>
       </c>
       <c r="H41" t="n">
-        <v>26628.0</v>
+        <v>26657.0</v>
       </c>
       <c r="I41" t="n">
-        <v>3631.0</v>
+        <v>3634.0</v>
       </c>
       <c r="J41" t="n">
         <v>2006.0</v>
@@ -3232,16 +3232,16 @@
         <v>0.0</v>
       </c>
       <c r="P41" t="n">
-        <v>240.0</v>
+        <v>320.0</v>
       </c>
       <c r="Q41" t="n">
         <v>7112.0</v>
       </c>
       <c r="R41" t="n">
-        <v>57.0</v>
+        <v>58.0</v>
       </c>
       <c r="S41" t="n">
-        <v>71235.0</v>
+        <v>72635.0</v>
       </c>
       <c r="T41" t="s">
         <v>126</v>
@@ -3250,7 +3250,7 @@
         <v>43252.0</v>
       </c>
       <c r="V41" t="n">
-        <v>159.0</v>
+        <v>160.0</v>
       </c>
     </row>
     <row r="42">
@@ -3297,16 +3297,16 @@
         <v>123</v>
       </c>
       <c r="O42" t="n">
-        <v>338.0</v>
+        <v>346.0</v>
       </c>
       <c r="P42" t="n">
-        <v>240.0</v>
+        <v>320.0</v>
       </c>
       <c r="Q42" t="n">
-        <v>21319.0</v>
+        <v>21327.0</v>
       </c>
       <c r="R42" t="n">
-        <v>16.0</v>
+        <v>17.0</v>
       </c>
       <c r="S42" t="n">
         <v>29252.0</v>
@@ -3318,7 +3318,7 @@
         <v>43370.0</v>
       </c>
       <c r="V42" t="n">
-        <v>41.0</v>
+        <v>42.0</v>
       </c>
     </row>
     <row r="43">
@@ -3332,22 +3332,22 @@
         <v>12.0</v>
       </c>
       <c r="D43" t="n">
-        <v>4186.0</v>
+        <v>4216.0</v>
       </c>
       <c r="E43" t="n">
         <v>4272.0</v>
       </c>
       <c r="F43" t="n">
-        <v>2727.0</v>
+        <v>2728.0</v>
       </c>
       <c r="G43" t="n">
         <v>2654.0</v>
       </c>
       <c r="H43" t="n">
-        <v>7763.0</v>
+        <v>7766.0</v>
       </c>
       <c r="I43" t="n">
-        <v>2261.0</v>
+        <v>2263.0</v>
       </c>
       <c r="J43" t="n">
         <v>2311.0</v>
@@ -3377,7 +3377,7 @@
         <v>22.0</v>
       </c>
       <c r="S43" t="n">
-        <v>23095.0</v>
+        <v>23935.0</v>
       </c>
       <c r="T43" t="s">
         <v>127</v>
@@ -3386,7 +3386,7 @@
         <v>43382.0</v>
       </c>
       <c r="V43" t="n">
-        <v>29.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="44">
@@ -3400,22 +3400,22 @@
         <v>11.0</v>
       </c>
       <c r="D44" t="n">
-        <v>4192.0</v>
+        <v>4314.0</v>
       </c>
       <c r="E44" t="n">
         <v>4318.0</v>
       </c>
       <c r="F44" t="n">
-        <v>3783.0</v>
+        <v>3789.0</v>
       </c>
       <c r="G44" t="n">
-        <v>4093.0</v>
+        <v>4095.0</v>
       </c>
       <c r="H44" t="n">
-        <v>8597.0</v>
+        <v>8606.0</v>
       </c>
       <c r="I44" t="n">
-        <v>2021.0</v>
+        <v>2024.0</v>
       </c>
       <c r="J44" t="n">
         <v>1339.0</v>
@@ -3433,13 +3433,13 @@
         <v>123</v>
       </c>
       <c r="O44" t="n">
-        <v>120.0</v>
+        <v>200.0</v>
       </c>
       <c r="P44" t="n">
-        <v>160.0</v>
+        <v>200.0</v>
       </c>
       <c r="Q44" t="n">
-        <v>21189.0</v>
+        <v>21269.0</v>
       </c>
       <c r="R44" t="n">
         <v>19.0</v>
@@ -3448,13 +3448,13 @@
         <v>70052.0</v>
       </c>
       <c r="T44" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="U44" t="n" s="2">
         <v>43390.0</v>
       </c>
       <c r="V44" t="n">
-        <v>21.0</v>
+        <v>22.0</v>
       </c>
     </row>
     <row r="45">
@@ -3468,7 +3468,7 @@
         <v>12.0</v>
       </c>
       <c r="D45" t="n">
-        <v>4214.0</v>
+        <v>4134.0</v>
       </c>
       <c r="E45" t="n">
         <v>4473.0</v>
@@ -3477,10 +3477,10 @@
         <v>2628.0</v>
       </c>
       <c r="G45" t="n">
-        <v>2573.0</v>
+        <v>2576.0</v>
       </c>
       <c r="H45" t="n">
-        <v>7180.0</v>
+        <v>7183.0</v>
       </c>
       <c r="I45" t="n">
         <v>1376.0</v>
@@ -3501,16 +3501,16 @@
         <v>123</v>
       </c>
       <c r="O45" t="n">
-        <v>164.0</v>
+        <v>288.0</v>
       </c>
       <c r="P45" t="n">
-        <v>120.0</v>
+        <v>160.0</v>
       </c>
       <c r="Q45" t="n">
-        <v>48802.0</v>
+        <v>48926.0</v>
       </c>
       <c r="R45" t="n">
-        <v>29.0</v>
+        <v>30.0</v>
       </c>
       <c r="S45" t="n">
         <v>38045.0</v>
@@ -3522,7 +3522,7 @@
         <v>43390.0</v>
       </c>
       <c r="V45" t="n">
-        <v>21.0</v>
+        <v>22.0</v>
       </c>
     </row>
     <row r="46">
@@ -3536,7 +3536,7 @@
         <v>7.0</v>
       </c>
       <c r="D46" t="n">
-        <v>2343.0</v>
+        <v>2320.0</v>
       </c>
       <c r="E46" t="n">
         <v>2364.0</v>
@@ -3545,10 +3545,10 @@
         <v>159.0</v>
       </c>
       <c r="G46" t="n">
-        <v>82.0</v>
+        <v>83.0</v>
       </c>
       <c r="H46" t="n">
-        <v>282.0</v>
+        <v>286.0</v>
       </c>
       <c r="I46" t="n">
         <v>72.0</v>
@@ -3569,13 +3569,13 @@
         <v>123</v>
       </c>
       <c r="O46" t="n">
-        <v>93.0</v>
+        <v>139.0</v>
       </c>
       <c r="P46" t="n">
-        <v>60.0</v>
+        <v>90.0</v>
       </c>
       <c r="Q46" t="n">
-        <v>1022.0</v>
+        <v>1068.0</v>
       </c>
       <c r="R46" t="n">
         <v>0.0</v>
@@ -3590,7 +3590,7 @@
         <v>43376.0</v>
       </c>
       <c r="V46" t="n">
-        <v>35.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="47">
@@ -3604,22 +3604,22 @@
         <v>12.0</v>
       </c>
       <c r="D47" t="n">
-        <v>4201.0</v>
+        <v>4487.0</v>
       </c>
       <c r="E47" t="n">
         <v>4919.0</v>
       </c>
       <c r="F47" t="n">
-        <v>10832.0</v>
+        <v>10873.0</v>
       </c>
       <c r="G47" t="n">
-        <v>11552.0</v>
+        <v>11586.0</v>
       </c>
       <c r="H47" t="n">
-        <v>25848.0</v>
+        <v>25932.0</v>
       </c>
       <c r="I47" t="n">
-        <v>8900.0</v>
+        <v>8938.0</v>
       </c>
       <c r="J47" t="n">
         <v>2205.0</v>
@@ -3637,28 +3637,28 @@
         <v>123</v>
       </c>
       <c r="O47" t="n">
-        <v>630.0</v>
+        <v>842.0</v>
       </c>
       <c r="P47" t="n">
-        <v>250.0</v>
+        <v>290.0</v>
       </c>
       <c r="Q47" t="n">
-        <v>74334.0</v>
+        <v>74546.0</v>
       </c>
       <c r="R47" t="n">
-        <v>21.0</v>
+        <v>22.0</v>
       </c>
       <c r="S47" t="n">
-        <v>78990.0</v>
+        <v>80670.0</v>
       </c>
       <c r="T47" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="U47" t="n" s="2">
         <v>43390.0</v>
       </c>
       <c r="V47" t="n">
-        <v>21.0</v>
+        <v>22.0</v>
       </c>
     </row>
     <row r="48">
@@ -3684,10 +3684,10 @@
         <v>3028.0</v>
       </c>
       <c r="H48" t="n">
-        <v>15462.0</v>
+        <v>15477.0</v>
       </c>
       <c r="I48" t="n">
-        <v>3269.0</v>
+        <v>3271.0</v>
       </c>
       <c r="J48" t="n">
         <v>1889.0</v>
@@ -3705,19 +3705,19 @@
         <v>122</v>
       </c>
       <c r="O48" t="n">
-        <v>363.0</v>
+        <v>389.0</v>
       </c>
       <c r="P48" t="n">
-        <v>200.0</v>
+        <v>280.0</v>
       </c>
       <c r="Q48" t="n">
-        <v>32923.0</v>
+        <v>32949.0</v>
       </c>
       <c r="R48" t="n">
         <v>36.0</v>
       </c>
       <c r="S48" t="n">
-        <v>66095.0</v>
+        <v>67215.0</v>
       </c>
       <c r="T48" t="s">
         <v>127</v>
@@ -3726,7 +3726,7 @@
         <v>43230.0</v>
       </c>
       <c r="V48" t="n">
-        <v>181.0</v>
+        <v>182.0</v>
       </c>
     </row>
     <row r="49">
@@ -3740,7 +3740,7 @@
         <v>11.0</v>
       </c>
       <c r="D49" t="n">
-        <v>4165.0</v>
+        <v>4138.0</v>
       </c>
       <c r="E49" t="n">
         <v>4325.0</v>
@@ -3749,13 +3749,13 @@
         <v>6353.0</v>
       </c>
       <c r="G49" t="n">
-        <v>6604.0</v>
+        <v>6605.0</v>
       </c>
       <c r="H49" t="n">
-        <v>18199.0</v>
+        <v>18206.0</v>
       </c>
       <c r="I49" t="n">
-        <v>3762.0</v>
+        <v>3764.0</v>
       </c>
       <c r="J49" t="n">
         <v>4372.0</v>
@@ -3776,13 +3776,13 @@
         <v>36.0</v>
       </c>
       <c r="P49" t="n">
-        <v>120.0</v>
+        <v>160.0</v>
       </c>
       <c r="Q49" t="n">
         <v>20663.0</v>
       </c>
       <c r="R49" t="n">
-        <v>56.0</v>
+        <v>57.0</v>
       </c>
       <c r="S49" t="n">
         <v>74077.0</v>
@@ -3794,7 +3794,7 @@
         <v>43184.0</v>
       </c>
       <c r="V49" t="n">
-        <v>227.0</v>
+        <v>228.0</v>
       </c>
     </row>
     <row r="50">
@@ -3850,7 +3850,7 @@
         <v>46933.0</v>
       </c>
       <c r="R50" t="n">
-        <v>27.0</v>
+        <v>28.0</v>
       </c>
       <c r="S50" t="n">
         <v>41200.0</v>
@@ -3862,7 +3862,7 @@
         <v>43314.0</v>
       </c>
       <c r="V50" t="n">
-        <v>97.0</v>
+        <v>98.0</v>
       </c>
     </row>
     <row r="51">
@@ -3930,7 +3930,7 @@
         <v>43254.0</v>
       </c>
       <c r="V51" t="n">
-        <v>157.0</v>
+        <v>158.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed table sort + last update
</commit_message>
<xml_diff>
--- a/docs/data/memberstats.xlsx
+++ b/docs/data/memberstats.xlsx
@@ -395,13 +395,13 @@
     <t>League 2</t>
   </si>
   <si>
+    <t>Arena 12</t>
+  </si>
+  <si>
     <t>League 1</t>
   </si>
   <si>
     <t>Arena 11</t>
-  </si>
-  <si>
-    <t>Arena 12</t>
   </si>
   <si>
     <t>Arena 9</t>
@@ -544,22 +544,22 @@
         <v>11.0</v>
       </c>
       <c r="D2" t="n">
-        <v>4396.0</v>
+        <v>4353.0</v>
       </c>
       <c r="E2" t="n">
         <v>4653.0</v>
       </c>
       <c r="F2" t="n">
-        <v>2234.0</v>
+        <v>2241.0</v>
       </c>
       <c r="G2" t="n">
-        <v>2077.0</v>
+        <v>2084.0</v>
       </c>
       <c r="H2" t="n">
-        <v>6993.0</v>
+        <v>7011.0</v>
       </c>
       <c r="I2" t="n">
-        <v>1147.0</v>
+        <v>1148.0</v>
       </c>
       <c r="J2" t="n">
         <v>2664.0</v>
@@ -577,13 +577,13 @@
         <v>122</v>
       </c>
       <c r="O2" t="n">
-        <v>466.0</v>
+        <v>624.0</v>
       </c>
       <c r="P2" t="n">
-        <v>280.0</v>
+        <v>360.0</v>
       </c>
       <c r="Q2" t="n">
-        <v>27816.0</v>
+        <v>27974.0</v>
       </c>
       <c r="R2" t="n">
         <v>43.0</v>
@@ -598,7 +598,7 @@
         <v>43302.0</v>
       </c>
       <c r="V2" t="n">
-        <v>110.0</v>
+        <v>111.0</v>
       </c>
     </row>
     <row r="3">
@@ -612,22 +612,22 @@
         <v>10.0</v>
       </c>
       <c r="D3" t="n">
-        <v>4012.0</v>
+        <v>3903.0</v>
       </c>
       <c r="E3" t="n">
         <v>4077.0</v>
       </c>
       <c r="F3" t="n">
-        <v>1648.0</v>
+        <v>1654.0</v>
       </c>
       <c r="G3" t="n">
-        <v>1431.0</v>
+        <v>1435.0</v>
       </c>
       <c r="H3" t="n">
-        <v>4293.0</v>
+        <v>4302.0</v>
       </c>
       <c r="I3" t="n">
-        <v>828.0</v>
+        <v>830.0</v>
       </c>
       <c r="J3" t="n">
         <v>2400.0</v>
@@ -648,7 +648,7 @@
         <v>239.0</v>
       </c>
       <c r="P3" t="n">
-        <v>120.0</v>
+        <v>160.0</v>
       </c>
       <c r="Q3" t="n">
         <v>18058.0</v>
@@ -666,7 +666,7 @@
         <v>43372.0</v>
       </c>
       <c r="V3" t="n">
-        <v>40.0</v>
+        <v>41.0</v>
       </c>
     </row>
     <row r="4">
@@ -692,7 +692,7 @@
         <v>2616.0</v>
       </c>
       <c r="H4" t="n">
-        <v>6184.0</v>
+        <v>6187.0</v>
       </c>
       <c r="I4" t="n">
         <v>1064.0</v>
@@ -716,7 +716,7 @@
         <v>26.0</v>
       </c>
       <c r="P4" t="n">
-        <v>320.0</v>
+        <v>400.0</v>
       </c>
       <c r="Q4" t="n">
         <v>8936.0</v>
@@ -725,16 +725,16 @@
         <v>43.0</v>
       </c>
       <c r="S4" t="n">
-        <v>59126.0</v>
+        <v>59966.0</v>
       </c>
       <c r="T4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="U4" t="n" s="2">
         <v>43082.0</v>
       </c>
       <c r="V4" t="n">
-        <v>330.0</v>
+        <v>331.0</v>
       </c>
     </row>
     <row r="5">
@@ -748,25 +748,25 @@
         <v>10.0</v>
       </c>
       <c r="D5" t="n">
-        <v>3690.0</v>
+        <v>3732.0</v>
       </c>
       <c r="E5" t="n">
-        <v>3764.0</v>
+        <v>3785.0</v>
       </c>
       <c r="F5" t="n">
-        <v>700.0</v>
+        <v>707.0</v>
       </c>
       <c r="G5" t="n">
-        <v>652.0</v>
+        <v>658.0</v>
       </c>
       <c r="H5" t="n">
-        <v>1980.0</v>
+        <v>1997.0</v>
       </c>
       <c r="I5" t="n">
-        <v>384.0</v>
+        <v>386.0</v>
       </c>
       <c r="J5" t="n">
-        <v>1430.0</v>
+        <v>1432.0</v>
       </c>
       <c r="K5" t="n">
         <v>10.0</v>
@@ -781,13 +781,13 @@
         <v>123</v>
       </c>
       <c r="O5" t="n">
-        <v>10.0</v>
+        <v>130.0</v>
       </c>
       <c r="P5" t="n">
-        <v>0.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q5" t="n">
-        <v>16795.0</v>
+        <v>16925.0</v>
       </c>
       <c r="R5" t="n">
         <v>4.0</v>
@@ -796,13 +796,13 @@
         <v>9415.0</v>
       </c>
       <c r="T5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="U5" t="n" s="2">
         <v>43397.0</v>
       </c>
       <c r="V5" t="n">
-        <v>15.0</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="6">
@@ -816,19 +816,19 @@
         <v>10.0</v>
       </c>
       <c r="D6" t="n">
-        <v>3995.0</v>
+        <v>3925.0</v>
       </c>
       <c r="E6" t="n">
         <v>4142.0</v>
       </c>
       <c r="F6" t="n">
-        <v>1226.0</v>
+        <v>1228.0</v>
       </c>
       <c r="G6" t="n">
-        <v>1256.0</v>
+        <v>1261.0</v>
       </c>
       <c r="H6" t="n">
-        <v>3174.0</v>
+        <v>3188.0</v>
       </c>
       <c r="I6" t="n">
         <v>499.0</v>
@@ -849,13 +849,13 @@
         <v>123</v>
       </c>
       <c r="O6" t="n">
-        <v>474.0</v>
+        <v>647.0</v>
       </c>
       <c r="P6" t="n">
-        <v>320.0</v>
+        <v>464.0</v>
       </c>
       <c r="Q6" t="n">
-        <v>15732.0</v>
+        <v>15905.0</v>
       </c>
       <c r="R6" t="n">
         <v>28.0</v>
@@ -864,13 +864,13 @@
         <v>38951.0</v>
       </c>
       <c r="T6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="U6" t="n" s="2">
         <v>43356.0</v>
       </c>
       <c r="V6" t="n">
-        <v>56.0</v>
+        <v>57.0</v>
       </c>
     </row>
     <row r="7">
@@ -884,25 +884,25 @@
         <v>11.0</v>
       </c>
       <c r="D7" t="n">
-        <v>4231.0</v>
+        <v>4205.0</v>
       </c>
       <c r="E7" t="n">
         <v>4489.0</v>
       </c>
       <c r="F7" t="n">
-        <v>2956.0</v>
+        <v>2979.0</v>
       </c>
       <c r="G7" t="n">
-        <v>2658.0</v>
+        <v>2663.0</v>
       </c>
       <c r="H7" t="n">
-        <v>7013.0</v>
+        <v>7035.0</v>
       </c>
       <c r="I7" t="n">
-        <v>683.0</v>
+        <v>687.0</v>
       </c>
       <c r="J7" t="n">
-        <v>4151.0</v>
+        <v>4159.0</v>
       </c>
       <c r="K7" t="n">
         <v>10.0</v>
@@ -920,7 +920,7 @@
         <v>0.0</v>
       </c>
       <c r="P7" t="n">
-        <v>160.0</v>
+        <v>240.0</v>
       </c>
       <c r="Q7" t="n">
         <v>2125.0</v>
@@ -929,16 +929,16 @@
         <v>40.0</v>
       </c>
       <c r="S7" t="n">
-        <v>55120.0</v>
+        <v>55960.0</v>
       </c>
       <c r="T7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="U7" t="n" s="2">
         <v>43364.0</v>
       </c>
       <c r="V7" t="n">
-        <v>48.0</v>
+        <v>49.0</v>
       </c>
     </row>
     <row r="8">
@@ -952,22 +952,22 @@
         <v>11.0</v>
       </c>
       <c r="D8" t="n">
-        <v>4291.0</v>
+        <v>4293.0</v>
       </c>
       <c r="E8" t="n">
         <v>4497.0</v>
       </c>
       <c r="F8" t="n">
-        <v>1902.0</v>
+        <v>1903.0</v>
       </c>
       <c r="G8" t="n">
-        <v>1803.0</v>
+        <v>1804.0</v>
       </c>
       <c r="H8" t="n">
-        <v>7560.0</v>
+        <v>7567.0</v>
       </c>
       <c r="I8" t="n">
-        <v>1112.0</v>
+        <v>1114.0</v>
       </c>
       <c r="J8" t="n">
         <v>1384.0</v>
@@ -985,13 +985,13 @@
         <v>124</v>
       </c>
       <c r="O8" t="n">
-        <v>110.0</v>
+        <v>144.0</v>
       </c>
       <c r="P8" t="n">
-        <v>280.0</v>
+        <v>360.0</v>
       </c>
       <c r="Q8" t="n">
-        <v>25005.0</v>
+        <v>25039.0</v>
       </c>
       <c r="R8" t="n">
         <v>56.0</v>
@@ -1000,13 +1000,13 @@
         <v>68155.0</v>
       </c>
       <c r="T8" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="U8" t="n" s="2">
         <v>43058.0</v>
       </c>
       <c r="V8" t="n">
-        <v>354.0</v>
+        <v>355.0</v>
       </c>
     </row>
     <row r="9">
@@ -1020,7 +1020,7 @@
         <v>11.0</v>
       </c>
       <c r="D9" t="n">
-        <v>4131.0</v>
+        <v>4104.0</v>
       </c>
       <c r="E9" t="n">
         <v>4496.0</v>
@@ -1029,10 +1029,10 @@
         <v>2324.0</v>
       </c>
       <c r="G9" t="n">
-        <v>2256.0</v>
+        <v>2257.0</v>
       </c>
       <c r="H9" t="n">
-        <v>5116.0</v>
+        <v>5119.0</v>
       </c>
       <c r="I9" t="n">
         <v>893.0</v>
@@ -1053,28 +1053,28 @@
         <v>123</v>
       </c>
       <c r="O9" t="n">
-        <v>180.0</v>
+        <v>198.0</v>
       </c>
       <c r="P9" t="n">
         <v>120.0</v>
       </c>
       <c r="Q9" t="n">
-        <v>24831.0</v>
+        <v>24849.0</v>
       </c>
       <c r="R9" t="n">
         <v>13.0</v>
       </c>
       <c r="S9" t="n">
-        <v>50712.0</v>
+        <v>51272.0</v>
       </c>
       <c r="T9" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="U9" t="n" s="2">
         <v>43390.0</v>
       </c>
       <c r="V9" t="n">
-        <v>22.0</v>
+        <v>23.0</v>
       </c>
     </row>
     <row r="10">
@@ -1136,13 +1136,13 @@
         <v>11970.0</v>
       </c>
       <c r="T10" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="U10" t="n" s="2">
         <v>43123.0</v>
       </c>
       <c r="V10" t="n">
-        <v>289.0</v>
+        <v>290.0</v>
       </c>
     </row>
     <row r="11">
@@ -1156,22 +1156,22 @@
         <v>11.0</v>
       </c>
       <c r="D11" t="n">
-        <v>4317.0</v>
+        <v>4295.0</v>
       </c>
       <c r="E11" t="n">
         <v>4501.0</v>
       </c>
       <c r="F11" t="n">
-        <v>2363.0</v>
+        <v>2397.0</v>
       </c>
       <c r="G11" t="n">
-        <v>2199.0</v>
+        <v>2220.0</v>
       </c>
       <c r="H11" t="n">
-        <v>10596.0</v>
+        <v>10645.0</v>
       </c>
       <c r="I11" t="n">
-        <v>2355.0</v>
+        <v>2364.0</v>
       </c>
       <c r="J11" t="n">
         <v>1906.0</v>
@@ -1189,13 +1189,13 @@
         <v>124</v>
       </c>
       <c r="O11" t="n">
-        <v>30.0</v>
+        <v>66.0</v>
       </c>
       <c r="P11" t="n">
-        <v>400.0</v>
+        <v>520.0</v>
       </c>
       <c r="Q11" t="n">
-        <v>3162.0</v>
+        <v>3198.0</v>
       </c>
       <c r="R11" t="n">
         <v>56.0</v>
@@ -1204,13 +1204,13 @@
         <v>77390.0</v>
       </c>
       <c r="T11" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="U11" t="n" s="2">
         <v>43123.0</v>
       </c>
       <c r="V11" t="n">
-        <v>289.0</v>
+        <v>290.0</v>
       </c>
     </row>
     <row r="12">
@@ -1236,10 +1236,10 @@
         <v>1752.0</v>
       </c>
       <c r="H12" t="n">
-        <v>9397.0</v>
+        <v>9412.0</v>
       </c>
       <c r="I12" t="n">
-        <v>1361.0</v>
+        <v>1362.0</v>
       </c>
       <c r="J12" t="n">
         <v>4199.0</v>
@@ -1257,19 +1257,19 @@
         <v>123</v>
       </c>
       <c r="O12" t="n">
-        <v>594.0</v>
+        <v>783.0</v>
       </c>
       <c r="P12" t="n">
-        <v>360.0</v>
+        <v>520.0</v>
       </c>
       <c r="Q12" t="n">
-        <v>88991.0</v>
+        <v>89180.0</v>
       </c>
       <c r="R12" t="n">
         <v>74.0</v>
       </c>
       <c r="S12" t="n">
-        <v>72320.0</v>
+        <v>72880.0</v>
       </c>
       <c r="T12" t="s">
         <v>126</v>
@@ -1278,7 +1278,7 @@
         <v>43397.0</v>
       </c>
       <c r="V12" t="n">
-        <v>15.0</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="13">
@@ -1292,19 +1292,19 @@
         <v>11.0</v>
       </c>
       <c r="D13" t="n">
-        <v>3920.0</v>
+        <v>3871.0</v>
       </c>
       <c r="E13" t="n">
         <v>4163.0</v>
       </c>
       <c r="F13" t="n">
-        <v>3152.0</v>
+        <v>3153.0</v>
       </c>
       <c r="G13" t="n">
-        <v>3329.0</v>
+        <v>3332.0</v>
       </c>
       <c r="H13" t="n">
-        <v>8579.0</v>
+        <v>8583.0</v>
       </c>
       <c r="I13" t="n">
         <v>1340.0</v>
@@ -1340,13 +1340,13 @@
         <v>29191.0</v>
       </c>
       <c r="T13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="U13" t="n" s="2">
         <v>43218.0</v>
       </c>
       <c r="V13" t="n">
-        <v>194.0</v>
+        <v>195.0</v>
       </c>
     </row>
     <row r="14">
@@ -1360,22 +1360,22 @@
         <v>11.0</v>
       </c>
       <c r="D14" t="n">
-        <v>4276.0</v>
+        <v>4306.0</v>
       </c>
       <c r="E14" t="n">
         <v>4389.0</v>
       </c>
       <c r="F14" t="n">
-        <v>1352.0</v>
+        <v>1356.0</v>
       </c>
       <c r="G14" t="n">
         <v>1199.0</v>
       </c>
       <c r="H14" t="n">
-        <v>5488.0</v>
+        <v>5503.0</v>
       </c>
       <c r="I14" t="n">
-        <v>757.0</v>
+        <v>758.0</v>
       </c>
       <c r="J14" t="n">
         <v>1199.0</v>
@@ -1393,13 +1393,13 @@
         <v>124</v>
       </c>
       <c r="O14" t="n">
-        <v>370.0</v>
+        <v>521.0</v>
       </c>
       <c r="P14" t="n">
-        <v>360.0</v>
+        <v>480.0</v>
       </c>
       <c r="Q14" t="n">
-        <v>37579.0</v>
+        <v>37730.0</v>
       </c>
       <c r="R14" t="n">
         <v>61.0</v>
@@ -1408,13 +1408,13 @@
         <v>73320.0</v>
       </c>
       <c r="T14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="U14" t="n" s="2">
         <v>43218.0</v>
       </c>
       <c r="V14" t="n">
-        <v>194.0</v>
+        <v>195.0</v>
       </c>
     </row>
     <row r="15">
@@ -1428,22 +1428,22 @@
         <v>12.0</v>
       </c>
       <c r="D15" t="n">
-        <v>4230.0</v>
+        <v>4240.0</v>
       </c>
       <c r="E15" t="n">
         <v>4521.0</v>
       </c>
       <c r="F15" t="n">
-        <v>4607.0</v>
+        <v>4614.0</v>
       </c>
       <c r="G15" t="n">
-        <v>5021.0</v>
+        <v>5028.0</v>
       </c>
       <c r="H15" t="n">
-        <v>10685.0</v>
+        <v>10700.0</v>
       </c>
       <c r="I15" t="n">
-        <v>2064.0</v>
+        <v>2066.0</v>
       </c>
       <c r="J15" t="n">
         <v>1842.0</v>
@@ -1461,13 +1461,13 @@
         <v>123</v>
       </c>
       <c r="O15" t="n">
-        <v>474.0</v>
+        <v>678.0</v>
       </c>
       <c r="P15" t="n">
-        <v>320.0</v>
+        <v>400.0</v>
       </c>
       <c r="Q15" t="n">
-        <v>52665.0</v>
+        <v>52869.0</v>
       </c>
       <c r="R15" t="n">
         <v>30.0</v>
@@ -1476,13 +1476,13 @@
         <v>78890.0</v>
       </c>
       <c r="T15" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="U15" t="n" s="2">
         <v>43390.0</v>
       </c>
       <c r="V15" t="n">
-        <v>22.0</v>
+        <v>23.0</v>
       </c>
     </row>
     <row r="16">
@@ -1508,7 +1508,7 @@
         <v>1705.0</v>
       </c>
       <c r="H16" t="n">
-        <v>6596.0</v>
+        <v>6597.0</v>
       </c>
       <c r="I16" t="n">
         <v>1405.0</v>
@@ -1529,13 +1529,13 @@
         <v>123</v>
       </c>
       <c r="O16" t="n">
-        <v>36.0</v>
+        <v>70.0</v>
       </c>
       <c r="P16" t="n">
-        <v>80.0</v>
+        <v>160.0</v>
       </c>
       <c r="Q16" t="n">
-        <v>43983.0</v>
+        <v>44017.0</v>
       </c>
       <c r="R16" t="n">
         <v>32.0</v>
@@ -1544,13 +1544,13 @@
         <v>53689.0</v>
       </c>
       <c r="T16" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="U16" t="n" s="2">
         <v>43410.0</v>
       </c>
       <c r="V16" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="17">
@@ -1564,7 +1564,7 @@
         <v>11.0</v>
       </c>
       <c r="D17" t="n">
-        <v>4094.0</v>
+        <v>4067.0</v>
       </c>
       <c r="E17" t="n">
         <v>4416.0</v>
@@ -1573,10 +1573,10 @@
         <v>2272.0</v>
       </c>
       <c r="G17" t="n">
-        <v>2075.0</v>
+        <v>2076.0</v>
       </c>
       <c r="H17" t="n">
-        <v>6699.0</v>
+        <v>6703.0</v>
       </c>
       <c r="I17" t="n">
         <v>1079.0</v>
@@ -1597,28 +1597,28 @@
         <v>122</v>
       </c>
       <c r="O17" t="n">
-        <v>50.0</v>
+        <v>60.0</v>
       </c>
       <c r="P17" t="n">
-        <v>230.0</v>
+        <v>280.0</v>
       </c>
       <c r="Q17" t="n">
-        <v>20415.0</v>
+        <v>20425.0</v>
       </c>
       <c r="R17" t="n">
         <v>43.0</v>
       </c>
       <c r="S17" t="n">
-        <v>46501.0</v>
+        <v>47621.0</v>
       </c>
       <c r="T17" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="U17" t="n" s="2">
         <v>43275.0</v>
       </c>
       <c r="V17" t="n">
-        <v>137.0</v>
+        <v>138.0</v>
       </c>
     </row>
     <row r="18">
@@ -1638,13 +1638,13 @@
         <v>4076.0</v>
       </c>
       <c r="F18" t="n">
-        <v>1532.0</v>
+        <v>1534.0</v>
       </c>
       <c r="G18" t="n">
-        <v>1458.0</v>
+        <v>1460.0</v>
       </c>
       <c r="H18" t="n">
-        <v>3628.0</v>
+        <v>3635.0</v>
       </c>
       <c r="I18" t="n">
         <v>1002.0</v>
@@ -1665,28 +1665,28 @@
         <v>122</v>
       </c>
       <c r="O18" t="n">
-        <v>303.0</v>
+        <v>397.0</v>
       </c>
       <c r="P18" t="n">
-        <v>270.0</v>
+        <v>370.0</v>
       </c>
       <c r="Q18" t="n">
-        <v>30599.0</v>
+        <v>30693.0</v>
       </c>
       <c r="R18" t="n">
         <v>13.0</v>
       </c>
       <c r="S18" t="n">
-        <v>25113.0</v>
+        <v>25899.0</v>
       </c>
       <c r="T18" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="U18" t="n" s="2">
         <v>43220.0</v>
       </c>
       <c r="V18" t="n">
-        <v>192.0</v>
+        <v>193.0</v>
       </c>
     </row>
     <row r="19">
@@ -1700,22 +1700,22 @@
         <v>11.0</v>
       </c>
       <c r="D19" t="n">
-        <v>4263.0</v>
+        <v>4133.0</v>
       </c>
       <c r="E19" t="n">
         <v>4577.0</v>
       </c>
       <c r="F19" t="n">
-        <v>2747.0</v>
+        <v>2761.0</v>
       </c>
       <c r="G19" t="n">
-        <v>2515.0</v>
+        <v>2525.0</v>
       </c>
       <c r="H19" t="n">
-        <v>6538.0</v>
+        <v>6559.0</v>
       </c>
       <c r="I19" t="n">
-        <v>707.0</v>
+        <v>708.0</v>
       </c>
       <c r="J19" t="n">
         <v>3595.0</v>
@@ -1733,13 +1733,13 @@
         <v>122</v>
       </c>
       <c r="O19" t="n">
-        <v>92.0</v>
+        <v>141.0</v>
       </c>
       <c r="P19" t="n">
-        <v>280.0</v>
+        <v>360.0</v>
       </c>
       <c r="Q19" t="n">
-        <v>21736.0</v>
+        <v>21785.0</v>
       </c>
       <c r="R19" t="n">
         <v>47.0</v>
@@ -1748,13 +1748,13 @@
         <v>76465.0</v>
       </c>
       <c r="T19" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="U19" t="n" s="2">
         <v>43058.0</v>
       </c>
       <c r="V19" t="n">
-        <v>354.0</v>
+        <v>355.0</v>
       </c>
     </row>
     <row r="20">
@@ -1768,19 +1768,19 @@
         <v>12.0</v>
       </c>
       <c r="D20" t="n">
-        <v>4140.0</v>
+        <v>4214.0</v>
       </c>
       <c r="E20" t="n">
         <v>4512.0</v>
       </c>
       <c r="F20" t="n">
-        <v>2970.0</v>
+        <v>2978.0</v>
       </c>
       <c r="G20" t="n">
-        <v>2860.0</v>
+        <v>2865.0</v>
       </c>
       <c r="H20" t="n">
-        <v>6765.0</v>
+        <v>6778.0</v>
       </c>
       <c r="I20" t="n">
         <v>1236.0</v>
@@ -1801,13 +1801,13 @@
         <v>122</v>
       </c>
       <c r="O20" t="n">
-        <v>242.0</v>
+        <v>306.0</v>
       </c>
       <c r="P20" t="n">
-        <v>210.0</v>
+        <v>320.0</v>
       </c>
       <c r="Q20" t="n">
-        <v>45324.0</v>
+        <v>45388.0</v>
       </c>
       <c r="R20" t="n">
         <v>34.0</v>
@@ -1816,13 +1816,13 @@
         <v>48075.0</v>
       </c>
       <c r="T20" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="U20" t="n" s="2">
         <v>43312.0</v>
       </c>
       <c r="V20" t="n">
-        <v>100.0</v>
+        <v>101.0</v>
       </c>
     </row>
     <row r="21">
@@ -1836,22 +1836,22 @@
         <v>12.0</v>
       </c>
       <c r="D21" t="n">
-        <v>4429.0</v>
+        <v>4461.0</v>
       </c>
       <c r="E21" t="n">
         <v>4767.0</v>
       </c>
       <c r="F21" t="n">
-        <v>6695.0</v>
+        <v>6699.0</v>
       </c>
       <c r="G21" t="n">
-        <v>6650.0</v>
+        <v>6652.0</v>
       </c>
       <c r="H21" t="n">
-        <v>23594.0</v>
+        <v>23622.0</v>
       </c>
       <c r="I21" t="n">
-        <v>2764.0</v>
+        <v>2766.0</v>
       </c>
       <c r="J21" t="n">
         <v>2570.0</v>
@@ -1863,19 +1863,19 @@
         <v>433.0</v>
       </c>
       <c r="M21" t="n">
-        <v>2524.0</v>
+        <v>2527.0</v>
       </c>
       <c r="N21" t="s">
         <v>125</v>
       </c>
       <c r="O21" t="n">
-        <v>338.0</v>
+        <v>424.0</v>
       </c>
       <c r="P21" t="n">
-        <v>390.0</v>
+        <v>540.0</v>
       </c>
       <c r="Q21" t="n">
-        <v>67267.0</v>
+        <v>67353.0</v>
       </c>
       <c r="R21" t="n">
         <v>87.0</v>
@@ -1890,7 +1890,7 @@
         <v>42705.0</v>
       </c>
       <c r="V21" t="n">
-        <v>707.0</v>
+        <v>708.0</v>
       </c>
     </row>
     <row r="22">
@@ -1904,19 +1904,19 @@
         <v>11.0</v>
       </c>
       <c r="D22" t="n">
-        <v>2914.0</v>
+        <v>2893.0</v>
       </c>
       <c r="E22" t="n">
         <v>3176.0</v>
       </c>
       <c r="F22" t="n">
-        <v>3246.0</v>
+        <v>3248.0</v>
       </c>
       <c r="G22" t="n">
-        <v>4541.0</v>
+        <v>4542.0</v>
       </c>
       <c r="H22" t="n">
-        <v>9092.0</v>
+        <v>9094.0</v>
       </c>
       <c r="I22" t="n">
         <v>2929.0</v>
@@ -1937,13 +1937,13 @@
         <v>123</v>
       </c>
       <c r="O22" t="n">
-        <v>214.0</v>
+        <v>320.0</v>
       </c>
       <c r="P22" t="n">
-        <v>120.0</v>
+        <v>150.0</v>
       </c>
       <c r="Q22" t="n">
-        <v>37621.0</v>
+        <v>37727.0</v>
       </c>
       <c r="R22" t="n">
         <v>26.0</v>
@@ -1958,7 +1958,7 @@
         <v>43151.0</v>
       </c>
       <c r="V22" t="n">
-        <v>261.0</v>
+        <v>262.0</v>
       </c>
     </row>
     <row r="23">
@@ -1972,7 +1972,7 @@
         <v>11.0</v>
       </c>
       <c r="D23" t="n">
-        <v>4025.0</v>
+        <v>3971.0</v>
       </c>
       <c r="E23" t="n">
         <v>4253.0</v>
@@ -1981,13 +1981,13 @@
         <v>1332.0</v>
       </c>
       <c r="G23" t="n">
-        <v>1395.0</v>
+        <v>1397.0</v>
       </c>
       <c r="H23" t="n">
-        <v>4567.0</v>
+        <v>4571.0</v>
       </c>
       <c r="I23" t="n">
-        <v>872.0</v>
+        <v>873.0</v>
       </c>
       <c r="J23" t="n">
         <v>507.0</v>
@@ -2005,19 +2005,19 @@
         <v>123</v>
       </c>
       <c r="O23" t="n">
-        <v>0.0</v>
+        <v>52.0</v>
       </c>
       <c r="P23" t="n">
         <v>0.0</v>
       </c>
       <c r="Q23" t="n">
-        <v>21493.0</v>
+        <v>21545.0</v>
       </c>
       <c r="R23" t="n">
         <v>25.0</v>
       </c>
       <c r="S23" t="n">
-        <v>46181.0</v>
+        <v>47003.0</v>
       </c>
       <c r="T23" t="s">
         <v>127</v>
@@ -2026,7 +2026,7 @@
         <v>43254.0</v>
       </c>
       <c r="V23" t="n">
-        <v>158.0</v>
+        <v>159.0</v>
       </c>
     </row>
     <row r="24">
@@ -2088,13 +2088,13 @@
         <v>64580.0</v>
       </c>
       <c r="T24" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="U24" t="n" s="2">
         <v>43380.0</v>
       </c>
       <c r="V24" t="n">
-        <v>32.0</v>
+        <v>33.0</v>
       </c>
     </row>
     <row r="25">
@@ -2108,22 +2108,22 @@
         <v>12.0</v>
       </c>
       <c r="D25" t="n">
-        <v>4118.0</v>
+        <v>4177.0</v>
       </c>
       <c r="E25" t="n">
         <v>4280.0</v>
       </c>
       <c r="F25" t="n">
-        <v>4392.0</v>
+        <v>4415.0</v>
       </c>
       <c r="G25" t="n">
-        <v>4355.0</v>
+        <v>4359.0</v>
       </c>
       <c r="H25" t="n">
-        <v>18412.0</v>
+        <v>18438.0</v>
       </c>
       <c r="I25" t="n">
-        <v>2928.0</v>
+        <v>2934.0</v>
       </c>
       <c r="J25" t="n">
         <v>2740.0</v>
@@ -2135,7 +2135,7 @@
         <v>2641.0</v>
       </c>
       <c r="M25" t="n">
-        <v>15763.0</v>
+        <v>15809.0</v>
       </c>
       <c r="N25" t="s">
         <v>124</v>
@@ -2144,7 +2144,7 @@
         <v>52.0</v>
       </c>
       <c r="P25" t="n">
-        <v>390.0</v>
+        <v>510.0</v>
       </c>
       <c r="Q25" t="n">
         <v>6312.0</v>
@@ -2156,13 +2156,13 @@
         <v>78585.0</v>
       </c>
       <c r="T25" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="U25" t="n" s="2">
         <v>42614.0</v>
       </c>
       <c r="V25" t="n">
-        <v>798.0</v>
+        <v>799.0</v>
       </c>
     </row>
     <row r="26">
@@ -2176,22 +2176,22 @@
         <v>10.0</v>
       </c>
       <c r="D26" t="n">
-        <v>3855.0</v>
+        <v>3834.0</v>
       </c>
       <c r="E26" t="n">
         <v>4008.0</v>
       </c>
       <c r="F26" t="n">
-        <v>1362.0</v>
+        <v>1363.0</v>
       </c>
       <c r="G26" t="n">
-        <v>1382.0</v>
+        <v>1384.0</v>
       </c>
       <c r="H26" t="n">
-        <v>3949.0</v>
+        <v>3956.0</v>
       </c>
       <c r="I26" t="n">
-        <v>644.0</v>
+        <v>646.0</v>
       </c>
       <c r="J26" t="n">
         <v>793.0</v>
@@ -2221,16 +2221,16 @@
         <v>12.0</v>
       </c>
       <c r="S26" t="n">
-        <v>23129.0</v>
+        <v>24178.0</v>
       </c>
       <c r="T26" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="U26" t="n" s="2">
         <v>43400.0</v>
       </c>
       <c r="V26" t="n">
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="27">
@@ -2244,7 +2244,7 @@
         <v>12.0</v>
       </c>
       <c r="D27" t="n">
-        <v>4127.0</v>
+        <v>4100.0</v>
       </c>
       <c r="E27" t="n">
         <v>4363.0</v>
@@ -2253,13 +2253,13 @@
         <v>3296.0</v>
       </c>
       <c r="G27" t="n">
-        <v>3486.0</v>
+        <v>3487.0</v>
       </c>
       <c r="H27" t="n">
-        <v>12183.0</v>
+        <v>12193.0</v>
       </c>
       <c r="I27" t="n">
-        <v>1689.0</v>
+        <v>1692.0</v>
       </c>
       <c r="J27" t="n">
         <v>2757.0</v>
@@ -2277,13 +2277,13 @@
         <v>122</v>
       </c>
       <c r="O27" t="n">
-        <v>599.0</v>
+        <v>680.0</v>
       </c>
       <c r="P27" t="n">
-        <v>240.0</v>
+        <v>320.0</v>
       </c>
       <c r="Q27" t="n">
-        <v>41899.0</v>
+        <v>41980.0</v>
       </c>
       <c r="R27" t="n">
         <v>65.0</v>
@@ -2292,13 +2292,13 @@
         <v>71723.0</v>
       </c>
       <c r="T27" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="U27" t="n" s="2">
         <v>43214.0</v>
       </c>
       <c r="V27" t="n">
-        <v>198.0</v>
+        <v>199.0</v>
       </c>
     </row>
     <row r="28">
@@ -2312,7 +2312,7 @@
         <v>12.0</v>
       </c>
       <c r="D28" t="n">
-        <v>4427.0</v>
+        <v>4371.0</v>
       </c>
       <c r="E28" t="n">
         <v>4653.0</v>
@@ -2321,10 +2321,10 @@
         <v>3693.0</v>
       </c>
       <c r="G28" t="n">
-        <v>3408.0</v>
+        <v>3410.0</v>
       </c>
       <c r="H28" t="n">
-        <v>11342.0</v>
+        <v>11344.0</v>
       </c>
       <c r="I28" t="n">
         <v>1547.0</v>
@@ -2366,7 +2366,7 @@
         <v>42614.0</v>
       </c>
       <c r="V28" t="n">
-        <v>798.0</v>
+        <v>799.0</v>
       </c>
     </row>
     <row r="29">
@@ -2428,13 +2428,13 @@
         <v>69961.0</v>
       </c>
       <c r="T29" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="U29" t="n" s="2">
         <v>43254.0</v>
       </c>
       <c r="V29" t="n">
-        <v>158.0</v>
+        <v>159.0</v>
       </c>
     </row>
     <row r="30">
@@ -2460,10 +2460,10 @@
         <v>1117.0</v>
       </c>
       <c r="H30" t="n">
-        <v>6515.0</v>
+        <v>6541.0</v>
       </c>
       <c r="I30" t="n">
-        <v>1433.0</v>
+        <v>1443.0</v>
       </c>
       <c r="J30" t="n">
         <v>1859.0</v>
@@ -2481,13 +2481,13 @@
         <v>122</v>
       </c>
       <c r="O30" t="n">
-        <v>350.0</v>
+        <v>560.0</v>
       </c>
       <c r="P30" t="n">
-        <v>320.0</v>
+        <v>480.0</v>
       </c>
       <c r="Q30" t="n">
-        <v>12424.0</v>
+        <v>12634.0</v>
       </c>
       <c r="R30" t="n">
         <v>55.0</v>
@@ -2496,13 +2496,13 @@
         <v>74542.0</v>
       </c>
       <c r="T30" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="U30" t="n" s="2">
         <v>43058.0</v>
       </c>
       <c r="V30" t="n">
-        <v>354.0</v>
+        <v>355.0</v>
       </c>
     </row>
     <row r="31">
@@ -2528,10 +2528,10 @@
         <v>535.0</v>
       </c>
       <c r="H31" t="n">
-        <v>3350.0</v>
+        <v>3355.0</v>
       </c>
       <c r="I31" t="n">
-        <v>736.0</v>
+        <v>737.0</v>
       </c>
       <c r="J31" t="n">
         <v>838.0</v>
@@ -2561,16 +2561,16 @@
         <v>52.0</v>
       </c>
       <c r="S31" t="n">
-        <v>64740.0</v>
+        <v>65789.0</v>
       </c>
       <c r="T31" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="U31" t="n" s="2">
         <v>43138.0</v>
       </c>
       <c r="V31" t="n">
-        <v>274.0</v>
+        <v>275.0</v>
       </c>
     </row>
     <row r="32">
@@ -2584,22 +2584,22 @@
         <v>12.0</v>
       </c>
       <c r="D32" t="n">
-        <v>4049.0</v>
+        <v>4082.0</v>
       </c>
       <c r="E32" t="n">
         <v>4140.0</v>
       </c>
       <c r="F32" t="n">
-        <v>2131.0</v>
+        <v>2141.0</v>
       </c>
       <c r="G32" t="n">
-        <v>2181.0</v>
+        <v>2185.0</v>
       </c>
       <c r="H32" t="n">
-        <v>6908.0</v>
+        <v>6931.0</v>
       </c>
       <c r="I32" t="n">
-        <v>1559.0</v>
+        <v>1561.0</v>
       </c>
       <c r="J32" t="n">
         <v>1474.0</v>
@@ -2617,28 +2617,28 @@
         <v>122</v>
       </c>
       <c r="O32" t="n">
-        <v>214.0</v>
+        <v>336.0</v>
       </c>
       <c r="P32" t="n">
-        <v>200.0</v>
+        <v>280.0</v>
       </c>
       <c r="Q32" t="n">
-        <v>42193.0</v>
+        <v>42315.0</v>
       </c>
       <c r="R32" t="n">
         <v>36.0</v>
       </c>
       <c r="S32" t="n">
-        <v>68593.0</v>
+        <v>70273.0</v>
       </c>
       <c r="T32" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="U32" t="n" s="2">
         <v>42920.0</v>
       </c>
       <c r="V32" t="n">
-        <v>492.0</v>
+        <v>493.0</v>
       </c>
     </row>
     <row r="33">
@@ -2652,19 +2652,19 @@
         <v>12.0</v>
       </c>
       <c r="D33" t="n">
-        <v>4357.0</v>
+        <v>4394.0</v>
       </c>
       <c r="E33" t="n">
         <v>4798.0</v>
       </c>
       <c r="F33" t="n">
-        <v>5116.0</v>
+        <v>5122.0</v>
       </c>
       <c r="G33" t="n">
-        <v>5230.0</v>
+        <v>5235.0</v>
       </c>
       <c r="H33" t="n">
-        <v>12272.0</v>
+        <v>12282.0</v>
       </c>
       <c r="I33" t="n">
         <v>2235.0</v>
@@ -2685,13 +2685,13 @@
         <v>122</v>
       </c>
       <c r="O33" t="n">
-        <v>194.0</v>
+        <v>268.0</v>
       </c>
       <c r="P33" t="n">
         <v>40.0</v>
       </c>
       <c r="Q33" t="n">
-        <v>58931.0</v>
+        <v>59005.0</v>
       </c>
       <c r="R33" t="n">
         <v>30.0</v>
@@ -2706,7 +2706,7 @@
         <v>43058.0</v>
       </c>
       <c r="V33" t="n">
-        <v>354.0</v>
+        <v>355.0</v>
       </c>
     </row>
     <row r="34">
@@ -2729,13 +2729,13 @@
         <v>378.0</v>
       </c>
       <c r="G34" t="n">
-        <v>219.0</v>
+        <v>220.0</v>
       </c>
       <c r="H34" t="n">
-        <v>1556.0</v>
+        <v>1566.0</v>
       </c>
       <c r="I34" t="n">
-        <v>267.0</v>
+        <v>268.0</v>
       </c>
       <c r="J34" t="n">
         <v>147.0</v>
@@ -2753,13 +2753,13 @@
         <v>123</v>
       </c>
       <c r="O34" t="n">
+        <v>358.0</v>
+      </c>
+      <c r="P34" t="n">
         <v>200.0</v>
       </c>
-      <c r="P34" t="n">
-        <v>120.0</v>
-      </c>
       <c r="Q34" t="n">
-        <v>4291.0</v>
+        <v>4449.0</v>
       </c>
       <c r="R34" t="n">
         <v>0.0</v>
@@ -2774,7 +2774,7 @@
         <v>43409.0</v>
       </c>
       <c r="V34" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="35">
@@ -2788,22 +2788,22 @@
         <v>10.0</v>
       </c>
       <c r="D35" t="n">
-        <v>3962.0</v>
+        <v>3991.0</v>
       </c>
       <c r="E35" t="n">
-        <v>3962.0</v>
+        <v>3991.0</v>
       </c>
       <c r="F35" t="n">
-        <v>944.0</v>
+        <v>945.0</v>
       </c>
       <c r="G35" t="n">
         <v>968.0</v>
       </c>
       <c r="H35" t="n">
-        <v>4183.0</v>
+        <v>4188.0</v>
       </c>
       <c r="I35" t="n">
-        <v>988.0</v>
+        <v>989.0</v>
       </c>
       <c r="J35" t="n">
         <v>278.0</v>
@@ -2833,16 +2833,16 @@
         <v>26.0</v>
       </c>
       <c r="S35" t="n">
-        <v>60285.0</v>
+        <v>61334.0</v>
       </c>
       <c r="T35" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="U35" t="n" s="2">
         <v>43312.0</v>
       </c>
       <c r="V35" t="n">
-        <v>100.0</v>
+        <v>101.0</v>
       </c>
     </row>
     <row r="36">
@@ -2856,22 +2856,22 @@
         <v>10.0</v>
       </c>
       <c r="D36" t="n">
-        <v>3734.0</v>
+        <v>3742.0</v>
       </c>
       <c r="E36" t="n">
         <v>4007.0</v>
       </c>
       <c r="F36" t="n">
-        <v>547.0</v>
+        <v>555.0</v>
       </c>
       <c r="G36" t="n">
-        <v>481.0</v>
+        <v>491.0</v>
       </c>
       <c r="H36" t="n">
-        <v>3330.0</v>
+        <v>3353.0</v>
       </c>
       <c r="I36" t="n">
-        <v>689.0</v>
+        <v>691.0</v>
       </c>
       <c r="J36" t="n">
         <v>278.0</v>
@@ -2889,28 +2889,28 @@
         <v>123</v>
       </c>
       <c r="O36" t="n">
-        <v>288.0</v>
+        <v>354.0</v>
       </c>
       <c r="P36" t="n">
-        <v>280.0</v>
+        <v>400.0</v>
       </c>
       <c r="Q36" t="n">
-        <v>16859.0</v>
+        <v>16925.0</v>
       </c>
       <c r="R36" t="n">
         <v>25.0</v>
       </c>
       <c r="S36" t="n">
-        <v>58955.0</v>
+        <v>59445.0</v>
       </c>
       <c r="T36" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="U36" t="n" s="2">
         <v>43274.0</v>
       </c>
       <c r="V36" t="n">
-        <v>138.0</v>
+        <v>139.0</v>
       </c>
     </row>
     <row r="37">
@@ -2924,22 +2924,22 @@
         <v>10.0</v>
       </c>
       <c r="D37" t="n">
-        <v>3945.0</v>
+        <v>3872.0</v>
       </c>
       <c r="E37" t="n">
         <v>4078.0</v>
       </c>
       <c r="F37" t="n">
-        <v>3413.0</v>
+        <v>3443.0</v>
       </c>
       <c r="G37" t="n">
-        <v>3978.0</v>
+        <v>4004.0</v>
       </c>
       <c r="H37" t="n">
-        <v>9467.0</v>
+        <v>9519.0</v>
       </c>
       <c r="I37" t="n">
-        <v>1739.0</v>
+        <v>1747.0</v>
       </c>
       <c r="J37" t="n">
         <v>224.0</v>
@@ -2957,13 +2957,13 @@
         <v>122</v>
       </c>
       <c r="O37" t="n">
-        <v>0.0</v>
+        <v>114.0</v>
       </c>
       <c r="P37" t="n">
-        <v>40.0</v>
+        <v>160.0</v>
       </c>
       <c r="Q37" t="n">
-        <v>14193.0</v>
+        <v>14307.0</v>
       </c>
       <c r="R37" t="n">
         <v>34.0</v>
@@ -2972,13 +2972,13 @@
         <v>68068.0</v>
       </c>
       <c r="T37" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="U37" t="n" s="2">
         <v>43280.0</v>
       </c>
       <c r="V37" t="n">
-        <v>132.0</v>
+        <v>133.0</v>
       </c>
     </row>
     <row r="38">
@@ -2992,22 +2992,22 @@
         <v>8.0</v>
       </c>
       <c r="D38" t="n">
-        <v>3554.0</v>
+        <v>3494.0</v>
       </c>
       <c r="E38" t="n">
         <v>3630.0</v>
       </c>
       <c r="F38" t="n">
-        <v>297.0</v>
+        <v>303.0</v>
       </c>
       <c r="G38" t="n">
-        <v>167.0</v>
+        <v>176.0</v>
       </c>
       <c r="H38" t="n">
-        <v>584.0</v>
+        <v>603.0</v>
       </c>
       <c r="I38" t="n">
-        <v>106.0</v>
+        <v>109.0</v>
       </c>
       <c r="J38" t="n">
         <v>423.0</v>
@@ -3025,28 +3025,28 @@
         <v>123</v>
       </c>
       <c r="O38" t="n">
-        <v>116.0</v>
+        <v>146.0</v>
       </c>
       <c r="P38" t="n">
-        <v>280.0</v>
+        <v>360.0</v>
       </c>
       <c r="Q38" t="n">
-        <v>2493.0</v>
+        <v>2523.0</v>
       </c>
       <c r="R38" t="n">
         <v>1.0</v>
       </c>
       <c r="S38" t="n">
-        <v>7716.0</v>
+        <v>8941.0</v>
       </c>
       <c r="T38" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="U38" t="n" s="2">
         <v>43360.0</v>
       </c>
       <c r="V38" t="n">
-        <v>52.0</v>
+        <v>53.0</v>
       </c>
     </row>
     <row r="39">
@@ -3066,16 +3066,16 @@
         <v>4379.0</v>
       </c>
       <c r="F39" t="n">
-        <v>1120.0</v>
+        <v>1121.0</v>
       </c>
       <c r="G39" t="n">
         <v>974.0</v>
       </c>
       <c r="H39" t="n">
-        <v>4359.0</v>
+        <v>4382.0</v>
       </c>
       <c r="I39" t="n">
-        <v>454.0</v>
+        <v>456.0</v>
       </c>
       <c r="J39" t="n">
         <v>2215.0</v>
@@ -3093,13 +3093,13 @@
         <v>122</v>
       </c>
       <c r="O39" t="n">
-        <v>406.0</v>
+        <v>561.0</v>
       </c>
       <c r="P39" t="n">
-        <v>400.0</v>
+        <v>560.0</v>
       </c>
       <c r="Q39" t="n">
-        <v>25169.0</v>
+        <v>25324.0</v>
       </c>
       <c r="R39" t="n">
         <v>38.0</v>
@@ -3108,13 +3108,13 @@
         <v>74506.0</v>
       </c>
       <c r="T39" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="U39" t="n" s="2">
         <v>43284.0</v>
       </c>
       <c r="V39" t="n">
-        <v>128.0</v>
+        <v>129.0</v>
       </c>
     </row>
     <row r="40">
@@ -3128,22 +3128,22 @@
         <v>10.0</v>
       </c>
       <c r="D40" t="n">
-        <v>4157.0</v>
+        <v>4137.0</v>
       </c>
       <c r="E40" t="n">
         <v>4405.0</v>
       </c>
       <c r="F40" t="n">
-        <v>1092.0</v>
+        <v>1095.0</v>
       </c>
       <c r="G40" t="n">
-        <v>992.0</v>
+        <v>996.0</v>
       </c>
       <c r="H40" t="n">
-        <v>3127.0</v>
+        <v>3135.0</v>
       </c>
       <c r="I40" t="n">
-        <v>652.0</v>
+        <v>654.0</v>
       </c>
       <c r="J40" t="n">
         <v>1700.0</v>
@@ -3161,13 +3161,13 @@
         <v>123</v>
       </c>
       <c r="O40" t="n">
-        <v>186.0</v>
+        <v>204.0</v>
       </c>
       <c r="P40" t="n">
-        <v>240.0</v>
+        <v>280.0</v>
       </c>
       <c r="Q40" t="n">
-        <v>19876.0</v>
+        <v>19894.0</v>
       </c>
       <c r="R40" t="n">
         <v>15.0</v>
@@ -3176,13 +3176,13 @@
         <v>50560.0</v>
       </c>
       <c r="T40" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="U40" t="n" s="2">
         <v>43352.0</v>
       </c>
       <c r="V40" t="n">
-        <v>60.0</v>
+        <v>61.0</v>
       </c>
     </row>
     <row r="41">
@@ -3208,10 +3208,10 @@
         <v>4693.0</v>
       </c>
       <c r="H41" t="n">
-        <v>26657.0</v>
+        <v>26696.0</v>
       </c>
       <c r="I41" t="n">
-        <v>3634.0</v>
+        <v>3642.0</v>
       </c>
       <c r="J41" t="n">
         <v>2006.0</v>
@@ -3232,7 +3232,7 @@
         <v>0.0</v>
       </c>
       <c r="P41" t="n">
-        <v>320.0</v>
+        <v>400.0</v>
       </c>
       <c r="Q41" t="n">
         <v>7112.0</v>
@@ -3250,7 +3250,7 @@
         <v>43252.0</v>
       </c>
       <c r="V41" t="n">
-        <v>160.0</v>
+        <v>161.0</v>
       </c>
     </row>
     <row r="42">
@@ -3264,22 +3264,22 @@
         <v>11.0</v>
       </c>
       <c r="D42" t="n">
-        <v>4033.0</v>
+        <v>4100.0</v>
       </c>
       <c r="E42" t="n">
         <v>4323.0</v>
       </c>
       <c r="F42" t="n">
-        <v>2368.0</v>
+        <v>2373.0</v>
       </c>
       <c r="G42" t="n">
-        <v>2296.0</v>
+        <v>2299.0</v>
       </c>
       <c r="H42" t="n">
-        <v>5972.0</v>
+        <v>5983.0</v>
       </c>
       <c r="I42" t="n">
-        <v>1174.0</v>
+        <v>1177.0</v>
       </c>
       <c r="J42" t="n">
         <v>2792.0</v>
@@ -3297,28 +3297,28 @@
         <v>123</v>
       </c>
       <c r="O42" t="n">
-        <v>346.0</v>
+        <v>408.0</v>
       </c>
       <c r="P42" t="n">
-        <v>320.0</v>
+        <v>400.0</v>
       </c>
       <c r="Q42" t="n">
-        <v>21327.0</v>
+        <v>21389.0</v>
       </c>
       <c r="R42" t="n">
         <v>17.0</v>
       </c>
       <c r="S42" t="n">
-        <v>29252.0</v>
+        <v>30372.0</v>
       </c>
       <c r="T42" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="U42" t="n" s="2">
         <v>43370.0</v>
       </c>
       <c r="V42" t="n">
-        <v>42.0</v>
+        <v>43.0</v>
       </c>
     </row>
     <row r="43">
@@ -3332,22 +3332,22 @@
         <v>12.0</v>
       </c>
       <c r="D43" t="n">
-        <v>4216.0</v>
+        <v>4246.0</v>
       </c>
       <c r="E43" t="n">
         <v>4272.0</v>
       </c>
       <c r="F43" t="n">
-        <v>2728.0</v>
+        <v>2733.0</v>
       </c>
       <c r="G43" t="n">
-        <v>2654.0</v>
+        <v>2655.0</v>
       </c>
       <c r="H43" t="n">
-        <v>7766.0</v>
+        <v>7776.0</v>
       </c>
       <c r="I43" t="n">
-        <v>2263.0</v>
+        <v>2264.0</v>
       </c>
       <c r="J43" t="n">
         <v>2311.0</v>
@@ -3365,13 +3365,13 @@
         <v>123</v>
       </c>
       <c r="O43" t="n">
-        <v>178.0</v>
+        <v>304.0</v>
       </c>
       <c r="P43" t="n">
-        <v>160.0</v>
+        <v>280.0</v>
       </c>
       <c r="Q43" t="n">
-        <v>31467.0</v>
+        <v>31593.0</v>
       </c>
       <c r="R43" t="n">
         <v>22.0</v>
@@ -3380,13 +3380,13 @@
         <v>23935.0</v>
       </c>
       <c r="T43" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="U43" t="n" s="2">
         <v>43382.0</v>
       </c>
       <c r="V43" t="n">
-        <v>30.0</v>
+        <v>31.0</v>
       </c>
     </row>
     <row r="44">
@@ -3400,22 +3400,22 @@
         <v>11.0</v>
       </c>
       <c r="D44" t="n">
-        <v>4314.0</v>
+        <v>4267.0</v>
       </c>
       <c r="E44" t="n">
-        <v>4318.0</v>
+        <v>4374.0</v>
       </c>
       <c r="F44" t="n">
-        <v>3789.0</v>
+        <v>3791.0</v>
       </c>
       <c r="G44" t="n">
-        <v>4095.0</v>
+        <v>4099.0</v>
       </c>
       <c r="H44" t="n">
-        <v>8606.0</v>
+        <v>8615.0</v>
       </c>
       <c r="I44" t="n">
-        <v>2024.0</v>
+        <v>2025.0</v>
       </c>
       <c r="J44" t="n">
         <v>1339.0</v>
@@ -3433,28 +3433,28 @@
         <v>123</v>
       </c>
       <c r="O44" t="n">
-        <v>200.0</v>
+        <v>324.0</v>
       </c>
       <c r="P44" t="n">
-        <v>200.0</v>
+        <v>320.0</v>
       </c>
       <c r="Q44" t="n">
-        <v>21269.0</v>
+        <v>21393.0</v>
       </c>
       <c r="R44" t="n">
         <v>19.0</v>
       </c>
       <c r="S44" t="n">
-        <v>70052.0</v>
+        <v>71172.0</v>
       </c>
       <c r="T44" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="U44" t="n" s="2">
         <v>43390.0</v>
       </c>
       <c r="V44" t="n">
-        <v>22.0</v>
+        <v>23.0</v>
       </c>
     </row>
     <row r="45">
@@ -3480,7 +3480,7 @@
         <v>2576.0</v>
       </c>
       <c r="H45" t="n">
-        <v>7183.0</v>
+        <v>7185.0</v>
       </c>
       <c r="I45" t="n">
         <v>1376.0</v>
@@ -3501,28 +3501,28 @@
         <v>123</v>
       </c>
       <c r="O45" t="n">
-        <v>288.0</v>
+        <v>336.0</v>
       </c>
       <c r="P45" t="n">
         <v>160.0</v>
       </c>
       <c r="Q45" t="n">
-        <v>48926.0</v>
+        <v>48974.0</v>
       </c>
       <c r="R45" t="n">
         <v>30.0</v>
       </c>
       <c r="S45" t="n">
-        <v>38045.0</v>
+        <v>38605.0</v>
       </c>
       <c r="T45" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="U45" t="n" s="2">
         <v>43390.0</v>
       </c>
       <c r="V45" t="n">
-        <v>22.0</v>
+        <v>23.0</v>
       </c>
     </row>
     <row r="46">
@@ -3536,22 +3536,22 @@
         <v>7.0</v>
       </c>
       <c r="D46" t="n">
-        <v>2320.0</v>
+        <v>2304.0</v>
       </c>
       <c r="E46" t="n">
         <v>2364.0</v>
       </c>
       <c r="F46" t="n">
-        <v>159.0</v>
+        <v>180.0</v>
       </c>
       <c r="G46" t="n">
-        <v>83.0</v>
+        <v>85.0</v>
       </c>
       <c r="H46" t="n">
-        <v>286.0</v>
+        <v>308.0</v>
       </c>
       <c r="I46" t="n">
-        <v>72.0</v>
+        <v>77.0</v>
       </c>
       <c r="J46" t="n">
         <v>0.0</v>
@@ -3569,13 +3569,13 @@
         <v>123</v>
       </c>
       <c r="O46" t="n">
-        <v>139.0</v>
+        <v>179.0</v>
       </c>
       <c r="P46" t="n">
-        <v>90.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q46" t="n">
-        <v>1068.0</v>
+        <v>1108.0</v>
       </c>
       <c r="R46" t="n">
         <v>0.0</v>
@@ -3590,7 +3590,7 @@
         <v>43376.0</v>
       </c>
       <c r="V46" t="n">
-        <v>36.0</v>
+        <v>37.0</v>
       </c>
     </row>
     <row r="47">
@@ -3604,22 +3604,22 @@
         <v>12.0</v>
       </c>
       <c r="D47" t="n">
-        <v>4487.0</v>
+        <v>4401.0</v>
       </c>
       <c r="E47" t="n">
         <v>4919.0</v>
       </c>
       <c r="F47" t="n">
-        <v>10873.0</v>
+        <v>10892.0</v>
       </c>
       <c r="G47" t="n">
-        <v>11586.0</v>
+        <v>11609.0</v>
       </c>
       <c r="H47" t="n">
-        <v>25932.0</v>
+        <v>25974.0</v>
       </c>
       <c r="I47" t="n">
-        <v>8938.0</v>
+        <v>8953.0</v>
       </c>
       <c r="J47" t="n">
         <v>2205.0</v>
@@ -3637,13 +3637,13 @@
         <v>123</v>
       </c>
       <c r="O47" t="n">
-        <v>842.0</v>
+        <v>1156.0</v>
       </c>
       <c r="P47" t="n">
-        <v>290.0</v>
+        <v>370.0</v>
       </c>
       <c r="Q47" t="n">
-        <v>74546.0</v>
+        <v>74860.0</v>
       </c>
       <c r="R47" t="n">
         <v>22.0</v>
@@ -3658,7 +3658,7 @@
         <v>43390.0</v>
       </c>
       <c r="V47" t="n">
-        <v>22.0</v>
+        <v>23.0</v>
       </c>
     </row>
     <row r="48">
@@ -3684,10 +3684,10 @@
         <v>3028.0</v>
       </c>
       <c r="H48" t="n">
-        <v>15477.0</v>
+        <v>15489.0</v>
       </c>
       <c r="I48" t="n">
-        <v>3271.0</v>
+        <v>3272.0</v>
       </c>
       <c r="J48" t="n">
         <v>1889.0</v>
@@ -3705,13 +3705,13 @@
         <v>122</v>
       </c>
       <c r="O48" t="n">
-        <v>389.0</v>
+        <v>425.0</v>
       </c>
       <c r="P48" t="n">
-        <v>280.0</v>
+        <v>360.0</v>
       </c>
       <c r="Q48" t="n">
-        <v>32949.0</v>
+        <v>32985.0</v>
       </c>
       <c r="R48" t="n">
         <v>36.0</v>
@@ -3720,13 +3720,13 @@
         <v>67215.0</v>
       </c>
       <c r="T48" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="U48" t="n" s="2">
         <v>43230.0</v>
       </c>
       <c r="V48" t="n">
-        <v>182.0</v>
+        <v>183.0</v>
       </c>
     </row>
     <row r="49">
@@ -3740,22 +3740,22 @@
         <v>11.0</v>
       </c>
       <c r="D49" t="n">
-        <v>4138.0</v>
+        <v>4083.0</v>
       </c>
       <c r="E49" t="n">
         <v>4325.0</v>
       </c>
       <c r="F49" t="n">
-        <v>6353.0</v>
+        <v>6358.0</v>
       </c>
       <c r="G49" t="n">
-        <v>6605.0</v>
+        <v>6608.0</v>
       </c>
       <c r="H49" t="n">
-        <v>18206.0</v>
+        <v>18218.0</v>
       </c>
       <c r="I49" t="n">
-        <v>3764.0</v>
+        <v>3765.0</v>
       </c>
       <c r="J49" t="n">
         <v>4372.0</v>
@@ -3773,28 +3773,28 @@
         <v>124</v>
       </c>
       <c r="O49" t="n">
-        <v>36.0</v>
+        <v>54.0</v>
       </c>
       <c r="P49" t="n">
-        <v>160.0</v>
+        <v>240.0</v>
       </c>
       <c r="Q49" t="n">
-        <v>20663.0</v>
+        <v>20681.0</v>
       </c>
       <c r="R49" t="n">
         <v>57.0</v>
       </c>
       <c r="S49" t="n">
-        <v>74077.0</v>
+        <v>75197.0</v>
       </c>
       <c r="T49" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="U49" t="n" s="2">
         <v>43184.0</v>
       </c>
       <c r="V49" t="n">
-        <v>228.0</v>
+        <v>229.0</v>
       </c>
     </row>
     <row r="50">
@@ -3841,13 +3841,13 @@
         <v>122</v>
       </c>
       <c r="O50" t="n">
-        <v>30.0</v>
+        <v>70.0</v>
       </c>
       <c r="P50" t="n">
-        <v>80.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q50" t="n">
-        <v>46933.0</v>
+        <v>46973.0</v>
       </c>
       <c r="R50" t="n">
         <v>28.0</v>
@@ -3856,13 +3856,13 @@
         <v>41200.0</v>
       </c>
       <c r="T50" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="U50" t="n" s="2">
         <v>43314.0</v>
       </c>
       <c r="V50" t="n">
-        <v>98.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="51">
@@ -3924,13 +3924,13 @@
         <v>13894.0</v>
       </c>
       <c r="T51" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="U51" t="n" s="2">
         <v>43254.0</v>
       </c>
       <c r="V51" t="n">
-        <v>158.0</v>
+        <v>159.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bugfixes and data update
</commit_message>
<xml_diff>
--- a/docs/data/memberstats.xlsx
+++ b/docs/data/memberstats.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="134">
   <si>
     <t>tag</t>
   </si>
@@ -405,6 +405,9 @@
   </si>
   <si>
     <t>Arena 9</t>
+  </si>
+  <si>
+    <t>League 3</t>
   </si>
   <si>
     <t>Arena 10</t>
@@ -556,10 +559,10 @@
         <v>2084.0</v>
       </c>
       <c r="H2" t="n">
-        <v>7011.0</v>
+        <v>7015.0</v>
       </c>
       <c r="I2" t="n">
-        <v>1148.0</v>
+        <v>1149.0</v>
       </c>
       <c r="J2" t="n">
         <v>2664.0</v>
@@ -577,19 +580,19 @@
         <v>122</v>
       </c>
       <c r="O2" t="n">
-        <v>624.0</v>
+        <v>658.0</v>
       </c>
       <c r="P2" t="n">
-        <v>360.0</v>
+        <v>400.0</v>
       </c>
       <c r="Q2" t="n">
-        <v>27974.0</v>
+        <v>28008.0</v>
       </c>
       <c r="R2" t="n">
-        <v>43.0</v>
+        <v>44.0</v>
       </c>
       <c r="S2" t="n">
-        <v>80620.0</v>
+        <v>81460.0</v>
       </c>
       <c r="T2" t="s">
         <v>126</v>
@@ -598,7 +601,7 @@
         <v>43302.0</v>
       </c>
       <c r="V2" t="n">
-        <v>111.0</v>
+        <v>112.0</v>
       </c>
     </row>
     <row r="3">
@@ -666,7 +669,7 @@
         <v>43372.0</v>
       </c>
       <c r="V3" t="n">
-        <v>41.0</v>
+        <v>42.0</v>
       </c>
     </row>
     <row r="4">
@@ -680,22 +683,22 @@
         <v>11.0</v>
       </c>
       <c r="D4" t="n">
-        <v>4084.0</v>
+        <v>4175.0</v>
       </c>
       <c r="E4" t="n">
         <v>4254.0</v>
       </c>
       <c r="F4" t="n">
-        <v>2573.0</v>
+        <v>2586.0</v>
       </c>
       <c r="G4" t="n">
-        <v>2616.0</v>
+        <v>2619.0</v>
       </c>
       <c r="H4" t="n">
-        <v>6187.0</v>
+        <v>6201.0</v>
       </c>
       <c r="I4" t="n">
-        <v>1064.0</v>
+        <v>1067.0</v>
       </c>
       <c r="J4" t="n">
         <v>1649.0</v>
@@ -713,19 +716,19 @@
         <v>122</v>
       </c>
       <c r="O4" t="n">
-        <v>26.0</v>
+        <v>76.0</v>
       </c>
       <c r="P4" t="n">
-        <v>400.0</v>
+        <v>480.0</v>
       </c>
       <c r="Q4" t="n">
-        <v>8936.0</v>
+        <v>8986.0</v>
       </c>
       <c r="R4" t="n">
-        <v>43.0</v>
+        <v>44.0</v>
       </c>
       <c r="S4" t="n">
-        <v>59966.0</v>
+        <v>61366.0</v>
       </c>
       <c r="T4" t="s">
         <v>128</v>
@@ -734,7 +737,7 @@
         <v>43082.0</v>
       </c>
       <c r="V4" t="n">
-        <v>331.0</v>
+        <v>332.0</v>
       </c>
     </row>
     <row r="5">
@@ -784,7 +787,7 @@
         <v>130.0</v>
       </c>
       <c r="P5" t="n">
-        <v>80.0</v>
+        <v>144.0</v>
       </c>
       <c r="Q5" t="n">
         <v>16925.0</v>
@@ -802,7 +805,7 @@
         <v>43397.0</v>
       </c>
       <c r="V5" t="n">
-        <v>16.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="6">
@@ -816,19 +819,19 @@
         <v>10.0</v>
       </c>
       <c r="D6" t="n">
-        <v>3925.0</v>
+        <v>3933.0</v>
       </c>
       <c r="E6" t="n">
         <v>4142.0</v>
       </c>
       <c r="F6" t="n">
-        <v>1228.0</v>
+        <v>1230.0</v>
       </c>
       <c r="G6" t="n">
-        <v>1261.0</v>
+        <v>1263.0</v>
       </c>
       <c r="H6" t="n">
-        <v>3188.0</v>
+        <v>3192.0</v>
       </c>
       <c r="I6" t="n">
         <v>499.0</v>
@@ -849,13 +852,13 @@
         <v>123</v>
       </c>
       <c r="O6" t="n">
-        <v>647.0</v>
+        <v>713.0</v>
       </c>
       <c r="P6" t="n">
-        <v>464.0</v>
+        <v>520.0</v>
       </c>
       <c r="Q6" t="n">
-        <v>15905.0</v>
+        <v>15971.0</v>
       </c>
       <c r="R6" t="n">
         <v>28.0</v>
@@ -870,7 +873,7 @@
         <v>43356.0</v>
       </c>
       <c r="V6" t="n">
-        <v>57.0</v>
+        <v>58.0</v>
       </c>
     </row>
     <row r="7">
@@ -884,7 +887,7 @@
         <v>11.0</v>
       </c>
       <c r="D7" t="n">
-        <v>4205.0</v>
+        <v>4180.0</v>
       </c>
       <c r="E7" t="n">
         <v>4489.0</v>
@@ -893,13 +896,13 @@
         <v>2979.0</v>
       </c>
       <c r="G7" t="n">
-        <v>2663.0</v>
+        <v>2664.0</v>
       </c>
       <c r="H7" t="n">
-        <v>7035.0</v>
+        <v>7039.0</v>
       </c>
       <c r="I7" t="n">
-        <v>687.0</v>
+        <v>688.0</v>
       </c>
       <c r="J7" t="n">
         <v>4159.0</v>
@@ -920,7 +923,7 @@
         <v>0.0</v>
       </c>
       <c r="P7" t="n">
-        <v>240.0</v>
+        <v>280.0</v>
       </c>
       <c r="Q7" t="n">
         <v>2125.0</v>
@@ -929,7 +932,7 @@
         <v>40.0</v>
       </c>
       <c r="S7" t="n">
-        <v>55960.0</v>
+        <v>57080.0</v>
       </c>
       <c r="T7" t="s">
         <v>128</v>
@@ -938,7 +941,7 @@
         <v>43364.0</v>
       </c>
       <c r="V7" t="n">
-        <v>49.0</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="8">
@@ -958,16 +961,16 @@
         <v>4497.0</v>
       </c>
       <c r="F8" t="n">
-        <v>1903.0</v>
+        <v>1910.0</v>
       </c>
       <c r="G8" t="n">
-        <v>1804.0</v>
+        <v>1806.0</v>
       </c>
       <c r="H8" t="n">
-        <v>7567.0</v>
+        <v>7586.0</v>
       </c>
       <c r="I8" t="n">
-        <v>1114.0</v>
+        <v>1115.0</v>
       </c>
       <c r="J8" t="n">
         <v>1384.0</v>
@@ -985,19 +988,19 @@
         <v>124</v>
       </c>
       <c r="O8" t="n">
-        <v>144.0</v>
+        <v>205.0</v>
       </c>
       <c r="P8" t="n">
-        <v>360.0</v>
+        <v>440.0</v>
       </c>
       <c r="Q8" t="n">
-        <v>25039.0</v>
+        <v>25100.0</v>
       </c>
       <c r="R8" t="n">
         <v>56.0</v>
       </c>
       <c r="S8" t="n">
-        <v>68155.0</v>
+        <v>69275.0</v>
       </c>
       <c r="T8" t="s">
         <v>128</v>
@@ -1006,7 +1009,7 @@
         <v>43058.0</v>
       </c>
       <c r="V8" t="n">
-        <v>355.0</v>
+        <v>356.0</v>
       </c>
     </row>
     <row r="9">
@@ -1020,22 +1023,22 @@
         <v>11.0</v>
       </c>
       <c r="D9" t="n">
-        <v>4104.0</v>
+        <v>4135.0</v>
       </c>
       <c r="E9" t="n">
         <v>4496.0</v>
       </c>
       <c r="F9" t="n">
-        <v>2324.0</v>
+        <v>2332.0</v>
       </c>
       <c r="G9" t="n">
-        <v>2257.0</v>
+        <v>2258.0</v>
       </c>
       <c r="H9" t="n">
-        <v>5119.0</v>
+        <v>5127.0</v>
       </c>
       <c r="I9" t="n">
-        <v>893.0</v>
+        <v>894.0</v>
       </c>
       <c r="J9" t="n">
         <v>1622.0</v>
@@ -1053,19 +1056,19 @@
         <v>123</v>
       </c>
       <c r="O9" t="n">
-        <v>198.0</v>
+        <v>242.0</v>
       </c>
       <c r="P9" t="n">
-        <v>120.0</v>
+        <v>160.0</v>
       </c>
       <c r="Q9" t="n">
-        <v>24849.0</v>
+        <v>24893.0</v>
       </c>
       <c r="R9" t="n">
         <v>13.0</v>
       </c>
       <c r="S9" t="n">
-        <v>51272.0</v>
+        <v>51832.0</v>
       </c>
       <c r="T9" t="s">
         <v>128</v>
@@ -1074,7 +1077,7 @@
         <v>43390.0</v>
       </c>
       <c r="V9" t="n">
-        <v>23.0</v>
+        <v>24.0</v>
       </c>
     </row>
     <row r="10">
@@ -1142,7 +1145,7 @@
         <v>43123.0</v>
       </c>
       <c r="V10" t="n">
-        <v>290.0</v>
+        <v>291.0</v>
       </c>
     </row>
     <row r="11">
@@ -1156,7 +1159,7 @@
         <v>11.0</v>
       </c>
       <c r="D11" t="n">
-        <v>4295.0</v>
+        <v>4267.0</v>
       </c>
       <c r="E11" t="n">
         <v>4501.0</v>
@@ -1165,13 +1168,13 @@
         <v>2397.0</v>
       </c>
       <c r="G11" t="n">
-        <v>2220.0</v>
+        <v>2221.0</v>
       </c>
       <c r="H11" t="n">
-        <v>10645.0</v>
+        <v>10650.0</v>
       </c>
       <c r="I11" t="n">
-        <v>2364.0</v>
+        <v>2365.0</v>
       </c>
       <c r="J11" t="n">
         <v>1906.0</v>
@@ -1189,19 +1192,19 @@
         <v>124</v>
       </c>
       <c r="O11" t="n">
-        <v>66.0</v>
+        <v>76.0</v>
       </c>
       <c r="P11" t="n">
-        <v>520.0</v>
+        <v>560.0</v>
       </c>
       <c r="Q11" t="n">
-        <v>3198.0</v>
+        <v>3208.0</v>
       </c>
       <c r="R11" t="n">
-        <v>56.0</v>
+        <v>57.0</v>
       </c>
       <c r="S11" t="n">
-        <v>77390.0</v>
+        <v>78510.0</v>
       </c>
       <c r="T11" t="s">
         <v>128</v>
@@ -1210,7 +1213,7 @@
         <v>43123.0</v>
       </c>
       <c r="V11" t="n">
-        <v>290.0</v>
+        <v>291.0</v>
       </c>
     </row>
     <row r="12">
@@ -1230,16 +1233,16 @@
         <v>4731.0</v>
       </c>
       <c r="F12" t="n">
-        <v>2237.0</v>
+        <v>2240.0</v>
       </c>
       <c r="G12" t="n">
         <v>1752.0</v>
       </c>
       <c r="H12" t="n">
-        <v>9412.0</v>
+        <v>9421.0</v>
       </c>
       <c r="I12" t="n">
-        <v>1362.0</v>
+        <v>1363.0</v>
       </c>
       <c r="J12" t="n">
         <v>4199.0</v>
@@ -1257,16 +1260,16 @@
         <v>123</v>
       </c>
       <c r="O12" t="n">
-        <v>783.0</v>
+        <v>988.0</v>
       </c>
       <c r="P12" t="n">
-        <v>520.0</v>
+        <v>590.0</v>
       </c>
       <c r="Q12" t="n">
-        <v>89180.0</v>
+        <v>89385.0</v>
       </c>
       <c r="R12" t="n">
-        <v>74.0</v>
+        <v>75.0</v>
       </c>
       <c r="S12" t="n">
         <v>72880.0</v>
@@ -1278,7 +1281,7 @@
         <v>43397.0</v>
       </c>
       <c r="V12" t="n">
-        <v>16.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="13">
@@ -1292,22 +1295,22 @@
         <v>11.0</v>
       </c>
       <c r="D13" t="n">
-        <v>3871.0</v>
+        <v>3887.0</v>
       </c>
       <c r="E13" t="n">
         <v>4163.0</v>
       </c>
       <c r="F13" t="n">
-        <v>3153.0</v>
+        <v>3158.0</v>
       </c>
       <c r="G13" t="n">
-        <v>3332.0</v>
+        <v>3338.0</v>
       </c>
       <c r="H13" t="n">
-        <v>8583.0</v>
+        <v>8595.0</v>
       </c>
       <c r="I13" t="n">
-        <v>1340.0</v>
+        <v>1342.0</v>
       </c>
       <c r="J13" t="n">
         <v>1906.0</v>
@@ -1334,7 +1337,7 @@
         <v>14241.0</v>
       </c>
       <c r="R13" t="n">
-        <v>18.0</v>
+        <v>19.0</v>
       </c>
       <c r="S13" t="n">
         <v>29191.0</v>
@@ -1346,7 +1349,7 @@
         <v>43218.0</v>
       </c>
       <c r="V13" t="n">
-        <v>195.0</v>
+        <v>196.0</v>
       </c>
     </row>
     <row r="14">
@@ -1372,7 +1375,7 @@
         <v>1199.0</v>
       </c>
       <c r="H14" t="n">
-        <v>5503.0</v>
+        <v>5506.0</v>
       </c>
       <c r="I14" t="n">
         <v>758.0</v>
@@ -1393,16 +1396,16 @@
         <v>124</v>
       </c>
       <c r="O14" t="n">
-        <v>521.0</v>
+        <v>537.0</v>
       </c>
       <c r="P14" t="n">
-        <v>480.0</v>
+        <v>520.0</v>
       </c>
       <c r="Q14" t="n">
-        <v>37730.0</v>
+        <v>37746.0</v>
       </c>
       <c r="R14" t="n">
-        <v>61.0</v>
+        <v>62.0</v>
       </c>
       <c r="S14" t="n">
         <v>73320.0</v>
@@ -1414,7 +1417,7 @@
         <v>43218.0</v>
       </c>
       <c r="V14" t="n">
-        <v>195.0</v>
+        <v>196.0</v>
       </c>
     </row>
     <row r="15">
@@ -1428,22 +1431,22 @@
         <v>12.0</v>
       </c>
       <c r="D15" t="n">
-        <v>4240.0</v>
+        <v>4296.0</v>
       </c>
       <c r="E15" t="n">
         <v>4521.0</v>
       </c>
       <c r="F15" t="n">
-        <v>4614.0</v>
+        <v>4646.0</v>
       </c>
       <c r="G15" t="n">
-        <v>5028.0</v>
+        <v>5040.0</v>
       </c>
       <c r="H15" t="n">
-        <v>10700.0</v>
+        <v>10739.0</v>
       </c>
       <c r="I15" t="n">
-        <v>2066.0</v>
+        <v>2073.0</v>
       </c>
       <c r="J15" t="n">
         <v>1842.0</v>
@@ -1461,19 +1464,19 @@
         <v>123</v>
       </c>
       <c r="O15" t="n">
-        <v>678.0</v>
+        <v>938.0</v>
       </c>
       <c r="P15" t="n">
-        <v>400.0</v>
+        <v>480.0</v>
       </c>
       <c r="Q15" t="n">
-        <v>52869.0</v>
+        <v>53129.0</v>
       </c>
       <c r="R15" t="n">
-        <v>30.0</v>
+        <v>31.0</v>
       </c>
       <c r="S15" t="n">
-        <v>78890.0</v>
+        <v>80010.0</v>
       </c>
       <c r="T15" t="s">
         <v>128</v>
@@ -1482,7 +1485,7 @@
         <v>43390.0</v>
       </c>
       <c r="V15" t="n">
-        <v>23.0</v>
+        <v>24.0</v>
       </c>
     </row>
     <row r="16">
@@ -1550,7 +1553,7 @@
         <v>43410.0</v>
       </c>
       <c r="V16" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="17">
@@ -1573,10 +1576,10 @@
         <v>2272.0</v>
       </c>
       <c r="G17" t="n">
-        <v>2076.0</v>
+        <v>2077.0</v>
       </c>
       <c r="H17" t="n">
-        <v>6703.0</v>
+        <v>6704.0</v>
       </c>
       <c r="I17" t="n">
         <v>1079.0</v>
@@ -1600,7 +1603,7 @@
         <v>60.0</v>
       </c>
       <c r="P17" t="n">
-        <v>280.0</v>
+        <v>360.0</v>
       </c>
       <c r="Q17" t="n">
         <v>20425.0</v>
@@ -1618,7 +1621,7 @@
         <v>43275.0</v>
       </c>
       <c r="V17" t="n">
-        <v>138.0</v>
+        <v>139.0</v>
       </c>
     </row>
     <row r="18">
@@ -1644,10 +1647,10 @@
         <v>1460.0</v>
       </c>
       <c r="H18" t="n">
-        <v>3635.0</v>
+        <v>3638.0</v>
       </c>
       <c r="I18" t="n">
-        <v>1002.0</v>
+        <v>1003.0</v>
       </c>
       <c r="J18" t="n">
         <v>2611.0</v>
@@ -1665,19 +1668,19 @@
         <v>122</v>
       </c>
       <c r="O18" t="n">
-        <v>397.0</v>
+        <v>417.0</v>
       </c>
       <c r="P18" t="n">
-        <v>370.0</v>
+        <v>410.0</v>
       </c>
       <c r="Q18" t="n">
-        <v>30693.0</v>
+        <v>30713.0</v>
       </c>
       <c r="R18" t="n">
-        <v>13.0</v>
+        <v>14.0</v>
       </c>
       <c r="S18" t="n">
-        <v>25899.0</v>
+        <v>26948.0</v>
       </c>
       <c r="T18" t="s">
         <v>127</v>
@@ -1686,7 +1689,7 @@
         <v>43220.0</v>
       </c>
       <c r="V18" t="n">
-        <v>193.0</v>
+        <v>194.0</v>
       </c>
     </row>
     <row r="19">
@@ -1700,22 +1703,22 @@
         <v>11.0</v>
       </c>
       <c r="D19" t="n">
-        <v>4133.0</v>
+        <v>4170.0</v>
       </c>
       <c r="E19" t="n">
         <v>4577.0</v>
       </c>
       <c r="F19" t="n">
-        <v>2761.0</v>
+        <v>2773.0</v>
       </c>
       <c r="G19" t="n">
-        <v>2525.0</v>
+        <v>2527.0</v>
       </c>
       <c r="H19" t="n">
-        <v>6559.0</v>
+        <v>6570.0</v>
       </c>
       <c r="I19" t="n">
-        <v>708.0</v>
+        <v>711.0</v>
       </c>
       <c r="J19" t="n">
         <v>3595.0</v>
@@ -1733,19 +1736,19 @@
         <v>122</v>
       </c>
       <c r="O19" t="n">
-        <v>141.0</v>
+        <v>149.0</v>
       </c>
       <c r="P19" t="n">
-        <v>360.0</v>
+        <v>410.0</v>
       </c>
       <c r="Q19" t="n">
-        <v>21785.0</v>
+        <v>21793.0</v>
       </c>
       <c r="R19" t="n">
         <v>47.0</v>
       </c>
       <c r="S19" t="n">
-        <v>76465.0</v>
+        <v>77025.0</v>
       </c>
       <c r="T19" t="s">
         <v>128</v>
@@ -1754,7 +1757,7 @@
         <v>43058.0</v>
       </c>
       <c r="V19" t="n">
-        <v>355.0</v>
+        <v>356.0</v>
       </c>
     </row>
     <row r="20">
@@ -1768,19 +1771,19 @@
         <v>12.0</v>
       </c>
       <c r="D20" t="n">
-        <v>4214.0</v>
+        <v>4244.0</v>
       </c>
       <c r="E20" t="n">
         <v>4512.0</v>
       </c>
       <c r="F20" t="n">
-        <v>2978.0</v>
+        <v>2979.0</v>
       </c>
       <c r="G20" t="n">
         <v>2865.0</v>
       </c>
       <c r="H20" t="n">
-        <v>6778.0</v>
+        <v>6779.0</v>
       </c>
       <c r="I20" t="n">
         <v>1236.0</v>
@@ -1801,13 +1804,13 @@
         <v>122</v>
       </c>
       <c r="O20" t="n">
-        <v>306.0</v>
+        <v>362.0</v>
       </c>
       <c r="P20" t="n">
-        <v>320.0</v>
+        <v>360.0</v>
       </c>
       <c r="Q20" t="n">
-        <v>45388.0</v>
+        <v>45444.0</v>
       </c>
       <c r="R20" t="n">
         <v>34.0</v>
@@ -1822,7 +1825,7 @@
         <v>43312.0</v>
       </c>
       <c r="V20" t="n">
-        <v>101.0</v>
+        <v>102.0</v>
       </c>
     </row>
     <row r="21">
@@ -1836,22 +1839,22 @@
         <v>12.0</v>
       </c>
       <c r="D21" t="n">
-        <v>4461.0</v>
+        <v>4450.0</v>
       </c>
       <c r="E21" t="n">
         <v>4767.0</v>
       </c>
       <c r="F21" t="n">
-        <v>6699.0</v>
+        <v>6712.0</v>
       </c>
       <c r="G21" t="n">
-        <v>6652.0</v>
+        <v>6660.0</v>
       </c>
       <c r="H21" t="n">
-        <v>23622.0</v>
+        <v>23651.0</v>
       </c>
       <c r="I21" t="n">
-        <v>2766.0</v>
+        <v>2770.0</v>
       </c>
       <c r="J21" t="n">
         <v>2570.0</v>
@@ -1863,22 +1866,22 @@
         <v>433.0</v>
       </c>
       <c r="M21" t="n">
-        <v>2527.0</v>
+        <v>2531.0</v>
       </c>
       <c r="N21" t="s">
         <v>125</v>
       </c>
       <c r="O21" t="n">
-        <v>424.0</v>
+        <v>500.0</v>
       </c>
       <c r="P21" t="n">
-        <v>540.0</v>
+        <v>630.0</v>
       </c>
       <c r="Q21" t="n">
-        <v>67353.0</v>
+        <v>67429.0</v>
       </c>
       <c r="R21" t="n">
-        <v>87.0</v>
+        <v>88.0</v>
       </c>
       <c r="S21" t="n">
         <v>81895.0</v>
@@ -1890,7 +1893,7 @@
         <v>42705.0</v>
       </c>
       <c r="V21" t="n">
-        <v>708.0</v>
+        <v>709.0</v>
       </c>
     </row>
     <row r="22">
@@ -1904,19 +1907,19 @@
         <v>11.0</v>
       </c>
       <c r="D22" t="n">
-        <v>2893.0</v>
+        <v>2871.0</v>
       </c>
       <c r="E22" t="n">
         <v>3176.0</v>
       </c>
       <c r="F22" t="n">
-        <v>3248.0</v>
+        <v>3254.0</v>
       </c>
       <c r="G22" t="n">
-        <v>4542.0</v>
+        <v>4544.0</v>
       </c>
       <c r="H22" t="n">
-        <v>9094.0</v>
+        <v>9100.0</v>
       </c>
       <c r="I22" t="n">
         <v>2929.0</v>
@@ -1937,13 +1940,13 @@
         <v>123</v>
       </c>
       <c r="O22" t="n">
-        <v>320.0</v>
+        <v>402.0</v>
       </c>
       <c r="P22" t="n">
-        <v>150.0</v>
+        <v>188.0</v>
       </c>
       <c r="Q22" t="n">
-        <v>37727.0</v>
+        <v>37809.0</v>
       </c>
       <c r="R22" t="n">
         <v>26.0</v>
@@ -1958,7 +1961,7 @@
         <v>43151.0</v>
       </c>
       <c r="V22" t="n">
-        <v>262.0</v>
+        <v>263.0</v>
       </c>
     </row>
     <row r="23">
@@ -1972,22 +1975,22 @@
         <v>11.0</v>
       </c>
       <c r="D23" t="n">
-        <v>3971.0</v>
+        <v>4092.0</v>
       </c>
       <c r="E23" t="n">
         <v>4253.0</v>
       </c>
       <c r="F23" t="n">
-        <v>1332.0</v>
+        <v>1337.0</v>
       </c>
       <c r="G23" t="n">
-        <v>1397.0</v>
+        <v>1398.0</v>
       </c>
       <c r="H23" t="n">
-        <v>4571.0</v>
+        <v>4578.0</v>
       </c>
       <c r="I23" t="n">
-        <v>873.0</v>
+        <v>875.0</v>
       </c>
       <c r="J23" t="n">
         <v>507.0</v>
@@ -2005,28 +2008,28 @@
         <v>123</v>
       </c>
       <c r="O23" t="n">
-        <v>52.0</v>
+        <v>160.0</v>
       </c>
       <c r="P23" t="n">
-        <v>0.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q23" t="n">
-        <v>21545.0</v>
+        <v>21653.0</v>
       </c>
       <c r="R23" t="n">
-        <v>25.0</v>
+        <v>26.0</v>
       </c>
       <c r="S23" t="n">
         <v>47003.0</v>
       </c>
       <c r="T23" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="U23" t="n" s="2">
         <v>43254.0</v>
       </c>
       <c r="V23" t="n">
-        <v>159.0</v>
+        <v>160.0</v>
       </c>
     </row>
     <row r="24">
@@ -2094,7 +2097,7 @@
         <v>43380.0</v>
       </c>
       <c r="V24" t="n">
-        <v>33.0</v>
+        <v>34.0</v>
       </c>
     </row>
     <row r="25">
@@ -2108,22 +2111,22 @@
         <v>12.0</v>
       </c>
       <c r="D25" t="n">
-        <v>4177.0</v>
+        <v>4179.0</v>
       </c>
       <c r="E25" t="n">
         <v>4280.0</v>
       </c>
       <c r="F25" t="n">
-        <v>4415.0</v>
+        <v>4416.0</v>
       </c>
       <c r="G25" t="n">
-        <v>4359.0</v>
+        <v>4360.0</v>
       </c>
       <c r="H25" t="n">
-        <v>18438.0</v>
+        <v>18451.0</v>
       </c>
       <c r="I25" t="n">
-        <v>2934.0</v>
+        <v>2935.0</v>
       </c>
       <c r="J25" t="n">
         <v>2740.0</v>
@@ -2135,25 +2138,25 @@
         <v>2641.0</v>
       </c>
       <c r="M25" t="n">
-        <v>15809.0</v>
+        <v>15828.0</v>
       </c>
       <c r="N25" t="s">
         <v>124</v>
       </c>
       <c r="O25" t="n">
-        <v>52.0</v>
+        <v>78.0</v>
       </c>
       <c r="P25" t="n">
-        <v>510.0</v>
+        <v>630.0</v>
       </c>
       <c r="Q25" t="n">
-        <v>6312.0</v>
+        <v>6338.0</v>
       </c>
       <c r="R25" t="n">
         <v>79.0</v>
       </c>
       <c r="S25" t="n">
-        <v>78585.0</v>
+        <v>79705.0</v>
       </c>
       <c r="T25" t="s">
         <v>128</v>
@@ -2162,7 +2165,7 @@
         <v>42614.0</v>
       </c>
       <c r="V25" t="n">
-        <v>799.0</v>
+        <v>800.0</v>
       </c>
     </row>
     <row r="26">
@@ -2176,7 +2179,7 @@
         <v>10.0</v>
       </c>
       <c r="D26" t="n">
-        <v>3834.0</v>
+        <v>3808.0</v>
       </c>
       <c r="E26" t="n">
         <v>4008.0</v>
@@ -2185,10 +2188,10 @@
         <v>1363.0</v>
       </c>
       <c r="G26" t="n">
-        <v>1384.0</v>
+        <v>1385.0</v>
       </c>
       <c r="H26" t="n">
-        <v>3956.0</v>
+        <v>3959.0</v>
       </c>
       <c r="I26" t="n">
         <v>646.0</v>
@@ -2218,10 +2221,10 @@
         <v>9620.0</v>
       </c>
       <c r="R26" t="n">
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
       <c r="S26" t="n">
-        <v>24178.0</v>
+        <v>25228.0</v>
       </c>
       <c r="T26" t="s">
         <v>127</v>
@@ -2230,7 +2233,7 @@
         <v>43400.0</v>
       </c>
       <c r="V26" t="n">
-        <v>13.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="27">
@@ -2244,22 +2247,22 @@
         <v>12.0</v>
       </c>
       <c r="D27" t="n">
-        <v>4100.0</v>
+        <v>4074.0</v>
       </c>
       <c r="E27" t="n">
         <v>4363.0</v>
       </c>
       <c r="F27" t="n">
-        <v>3296.0</v>
+        <v>3308.0</v>
       </c>
       <c r="G27" t="n">
-        <v>3487.0</v>
+        <v>3490.0</v>
       </c>
       <c r="H27" t="n">
-        <v>12193.0</v>
+        <v>12219.0</v>
       </c>
       <c r="I27" t="n">
-        <v>1692.0</v>
+        <v>1694.0</v>
       </c>
       <c r="J27" t="n">
         <v>2757.0</v>
@@ -2277,19 +2280,19 @@
         <v>122</v>
       </c>
       <c r="O27" t="n">
-        <v>680.0</v>
+        <v>878.0</v>
       </c>
       <c r="P27" t="n">
-        <v>320.0</v>
+        <v>400.0</v>
       </c>
       <c r="Q27" t="n">
-        <v>41980.0</v>
+        <v>42178.0</v>
       </c>
       <c r="R27" t="n">
-        <v>65.0</v>
+        <v>66.0</v>
       </c>
       <c r="S27" t="n">
-        <v>71723.0</v>
+        <v>73403.0</v>
       </c>
       <c r="T27" t="s">
         <v>128</v>
@@ -2298,7 +2301,7 @@
         <v>43214.0</v>
       </c>
       <c r="V27" t="n">
-        <v>199.0</v>
+        <v>200.0</v>
       </c>
     </row>
     <row r="28">
@@ -2312,7 +2315,7 @@
         <v>12.0</v>
       </c>
       <c r="D28" t="n">
-        <v>4371.0</v>
+        <v>4344.0</v>
       </c>
       <c r="E28" t="n">
         <v>4653.0</v>
@@ -2321,10 +2324,10 @@
         <v>3693.0</v>
       </c>
       <c r="G28" t="n">
-        <v>3410.0</v>
+        <v>3411.0</v>
       </c>
       <c r="H28" t="n">
-        <v>11344.0</v>
+        <v>11346.0</v>
       </c>
       <c r="I28" t="n">
         <v>1547.0</v>
@@ -2345,16 +2348,16 @@
         <v>124</v>
       </c>
       <c r="O28" t="n">
-        <v>48.0</v>
+        <v>66.0</v>
       </c>
       <c r="P28" t="n">
         <v>160.0</v>
       </c>
       <c r="Q28" t="n">
-        <v>32571.0</v>
+        <v>32589.0</v>
       </c>
       <c r="R28" t="n">
-        <v>60.0</v>
+        <v>61.0</v>
       </c>
       <c r="S28" t="n">
         <v>74515.0</v>
@@ -2366,7 +2369,7 @@
         <v>42614.0</v>
       </c>
       <c r="V28" t="n">
-        <v>799.0</v>
+        <v>800.0</v>
       </c>
     </row>
     <row r="29">
@@ -2434,7 +2437,7 @@
         <v>43254.0</v>
       </c>
       <c r="V29" t="n">
-        <v>159.0</v>
+        <v>160.0</v>
       </c>
     </row>
     <row r="30">
@@ -2460,10 +2463,10 @@
         <v>1117.0</v>
       </c>
       <c r="H30" t="n">
-        <v>6541.0</v>
+        <v>6548.0</v>
       </c>
       <c r="I30" t="n">
-        <v>1443.0</v>
+        <v>1444.0</v>
       </c>
       <c r="J30" t="n">
         <v>1859.0</v>
@@ -2481,19 +2484,19 @@
         <v>122</v>
       </c>
       <c r="O30" t="n">
+        <v>608.0</v>
+      </c>
+      <c r="P30" t="n">
         <v>560.0</v>
       </c>
-      <c r="P30" t="n">
-        <v>480.0</v>
-      </c>
       <c r="Q30" t="n">
-        <v>12634.0</v>
+        <v>12682.0</v>
       </c>
       <c r="R30" t="n">
-        <v>55.0</v>
+        <v>56.0</v>
       </c>
       <c r="S30" t="n">
-        <v>74542.0</v>
+        <v>75662.0</v>
       </c>
       <c r="T30" t="s">
         <v>128</v>
@@ -2502,7 +2505,7 @@
         <v>43058.0</v>
       </c>
       <c r="V30" t="n">
-        <v>355.0</v>
+        <v>356.0</v>
       </c>
     </row>
     <row r="31">
@@ -2528,10 +2531,10 @@
         <v>535.0</v>
       </c>
       <c r="H31" t="n">
-        <v>3355.0</v>
+        <v>3358.0</v>
       </c>
       <c r="I31" t="n">
-        <v>737.0</v>
+        <v>738.0</v>
       </c>
       <c r="J31" t="n">
         <v>838.0</v>
@@ -2561,7 +2564,7 @@
         <v>52.0</v>
       </c>
       <c r="S31" t="n">
-        <v>65789.0</v>
+        <v>67101.0</v>
       </c>
       <c r="T31" t="s">
         <v>127</v>
@@ -2570,7 +2573,7 @@
         <v>43138.0</v>
       </c>
       <c r="V31" t="n">
-        <v>275.0</v>
+        <v>276.0</v>
       </c>
     </row>
     <row r="32">
@@ -2596,10 +2599,10 @@
         <v>2185.0</v>
       </c>
       <c r="H32" t="n">
-        <v>6931.0</v>
+        <v>6935.0</v>
       </c>
       <c r="I32" t="n">
-        <v>1561.0</v>
+        <v>1562.0</v>
       </c>
       <c r="J32" t="n">
         <v>1474.0</v>
@@ -2617,19 +2620,19 @@
         <v>122</v>
       </c>
       <c r="O32" t="n">
-        <v>336.0</v>
+        <v>424.0</v>
       </c>
       <c r="P32" t="n">
-        <v>280.0</v>
+        <v>360.0</v>
       </c>
       <c r="Q32" t="n">
-        <v>42315.0</v>
+        <v>42403.0</v>
       </c>
       <c r="R32" t="n">
-        <v>36.0</v>
+        <v>37.0</v>
       </c>
       <c r="S32" t="n">
-        <v>70273.0</v>
+        <v>70553.0</v>
       </c>
       <c r="T32" t="s">
         <v>128</v>
@@ -2638,7 +2641,7 @@
         <v>42920.0</v>
       </c>
       <c r="V32" t="n">
-        <v>493.0</v>
+        <v>494.0</v>
       </c>
     </row>
     <row r="33">
@@ -2652,22 +2655,22 @@
         <v>12.0</v>
       </c>
       <c r="D33" t="n">
-        <v>4394.0</v>
+        <v>4601.0</v>
       </c>
       <c r="E33" t="n">
         <v>4798.0</v>
       </c>
       <c r="F33" t="n">
-        <v>5122.0</v>
+        <v>5131.0</v>
       </c>
       <c r="G33" t="n">
-        <v>5235.0</v>
+        <v>5237.0</v>
       </c>
       <c r="H33" t="n">
-        <v>12282.0</v>
+        <v>12299.0</v>
       </c>
       <c r="I33" t="n">
-        <v>2235.0</v>
+        <v>2243.0</v>
       </c>
       <c r="J33" t="n">
         <v>1728.0</v>
@@ -2685,13 +2688,13 @@
         <v>122</v>
       </c>
       <c r="O33" t="n">
-        <v>268.0</v>
+        <v>278.0</v>
       </c>
       <c r="P33" t="n">
         <v>40.0</v>
       </c>
       <c r="Q33" t="n">
-        <v>59005.0</v>
+        <v>59015.0</v>
       </c>
       <c r="R33" t="n">
         <v>30.0</v>
@@ -2700,13 +2703,13 @@
         <v>76270.0</v>
       </c>
       <c r="T33" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="U33" t="n" s="2">
         <v>43058.0</v>
       </c>
       <c r="V33" t="n">
-        <v>355.0</v>
+        <v>356.0</v>
       </c>
     </row>
     <row r="34">
@@ -2726,13 +2729,13 @@
         <v>3039.0</v>
       </c>
       <c r="F34" t="n">
-        <v>378.0</v>
+        <v>379.0</v>
       </c>
       <c r="G34" t="n">
         <v>220.0</v>
       </c>
       <c r="H34" t="n">
-        <v>1566.0</v>
+        <v>1567.0</v>
       </c>
       <c r="I34" t="n">
         <v>268.0</v>
@@ -2753,13 +2756,13 @@
         <v>123</v>
       </c>
       <c r="O34" t="n">
-        <v>358.0</v>
+        <v>388.0</v>
       </c>
       <c r="P34" t="n">
-        <v>200.0</v>
+        <v>240.0</v>
       </c>
       <c r="Q34" t="n">
-        <v>4449.0</v>
+        <v>4479.0</v>
       </c>
       <c r="R34" t="n">
         <v>0.0</v>
@@ -2768,13 +2771,13 @@
         <v>1137.0</v>
       </c>
       <c r="T34" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="U34" t="n" s="2">
         <v>43409.0</v>
       </c>
       <c r="V34" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="35">
@@ -2794,16 +2797,16 @@
         <v>3991.0</v>
       </c>
       <c r="F35" t="n">
-        <v>945.0</v>
+        <v>951.0</v>
       </c>
       <c r="G35" t="n">
         <v>968.0</v>
       </c>
       <c r="H35" t="n">
-        <v>4188.0</v>
+        <v>4193.0</v>
       </c>
       <c r="I35" t="n">
-        <v>989.0</v>
+        <v>991.0</v>
       </c>
       <c r="J35" t="n">
         <v>278.0</v>
@@ -2821,16 +2824,16 @@
         <v>123</v>
       </c>
       <c r="O35" t="n">
-        <v>18.0</v>
+        <v>38.0</v>
       </c>
       <c r="P35" t="n">
-        <v>80.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q35" t="n">
-        <v>8328.0</v>
+        <v>8348.0</v>
       </c>
       <c r="R35" t="n">
-        <v>26.0</v>
+        <v>27.0</v>
       </c>
       <c r="S35" t="n">
         <v>61334.0</v>
@@ -2842,7 +2845,7 @@
         <v>43312.0</v>
       </c>
       <c r="V35" t="n">
-        <v>101.0</v>
+        <v>102.0</v>
       </c>
     </row>
     <row r="36">
@@ -2889,13 +2892,13 @@
         <v>123</v>
       </c>
       <c r="O36" t="n">
-        <v>354.0</v>
+        <v>362.0</v>
       </c>
       <c r="P36" t="n">
-        <v>400.0</v>
+        <v>440.0</v>
       </c>
       <c r="Q36" t="n">
-        <v>16925.0</v>
+        <v>16933.0</v>
       </c>
       <c r="R36" t="n">
         <v>25.0</v>
@@ -2910,7 +2913,7 @@
         <v>43274.0</v>
       </c>
       <c r="V36" t="n">
-        <v>139.0</v>
+        <v>140.0</v>
       </c>
     </row>
     <row r="37">
@@ -2924,22 +2927,22 @@
         <v>10.0</v>
       </c>
       <c r="D37" t="n">
-        <v>3872.0</v>
+        <v>4052.0</v>
       </c>
       <c r="E37" t="n">
         <v>4078.0</v>
       </c>
       <c r="F37" t="n">
-        <v>3443.0</v>
+        <v>3457.0</v>
       </c>
       <c r="G37" t="n">
-        <v>4004.0</v>
+        <v>4006.0</v>
       </c>
       <c r="H37" t="n">
-        <v>9519.0</v>
+        <v>9535.0</v>
       </c>
       <c r="I37" t="n">
-        <v>1747.0</v>
+        <v>1754.0</v>
       </c>
       <c r="J37" t="n">
         <v>224.0</v>
@@ -2957,28 +2960,28 @@
         <v>122</v>
       </c>
       <c r="O37" t="n">
-        <v>114.0</v>
+        <v>144.0</v>
       </c>
       <c r="P37" t="n">
-        <v>160.0</v>
+        <v>200.0</v>
       </c>
       <c r="Q37" t="n">
-        <v>14307.0</v>
+        <v>14337.0</v>
       </c>
       <c r="R37" t="n">
         <v>34.0</v>
       </c>
       <c r="S37" t="n">
-        <v>68068.0</v>
+        <v>69188.0</v>
       </c>
       <c r="T37" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="U37" t="n" s="2">
         <v>43280.0</v>
       </c>
       <c r="V37" t="n">
-        <v>133.0</v>
+        <v>134.0</v>
       </c>
     </row>
     <row r="38">
@@ -2998,13 +3001,13 @@
         <v>3630.0</v>
       </c>
       <c r="F38" t="n">
-        <v>303.0</v>
+        <v>307.0</v>
       </c>
       <c r="G38" t="n">
         <v>176.0</v>
       </c>
       <c r="H38" t="n">
-        <v>603.0</v>
+        <v>609.0</v>
       </c>
       <c r="I38" t="n">
         <v>109.0</v>
@@ -3025,19 +3028,19 @@
         <v>123</v>
       </c>
       <c r="O38" t="n">
-        <v>146.0</v>
+        <v>174.0</v>
       </c>
       <c r="P38" t="n">
-        <v>360.0</v>
+        <v>408.0</v>
       </c>
       <c r="Q38" t="n">
-        <v>2523.0</v>
+        <v>2551.0</v>
       </c>
       <c r="R38" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="S38" t="n">
-        <v>8941.0</v>
+        <v>10411.0</v>
       </c>
       <c r="T38" t="s">
         <v>129</v>
@@ -3046,7 +3049,7 @@
         <v>43360.0</v>
       </c>
       <c r="V38" t="n">
-        <v>53.0</v>
+        <v>54.0</v>
       </c>
     </row>
     <row r="39">
@@ -3060,22 +3063,22 @@
         <v>11.0</v>
       </c>
       <c r="D39" t="n">
-        <v>4123.0</v>
+        <v>4052.0</v>
       </c>
       <c r="E39" t="n">
         <v>4379.0</v>
       </c>
       <c r="F39" t="n">
-        <v>1121.0</v>
+        <v>1130.0</v>
       </c>
       <c r="G39" t="n">
-        <v>974.0</v>
+        <v>981.0</v>
       </c>
       <c r="H39" t="n">
-        <v>4382.0</v>
+        <v>4403.0</v>
       </c>
       <c r="I39" t="n">
-        <v>456.0</v>
+        <v>459.0</v>
       </c>
       <c r="J39" t="n">
         <v>2215.0</v>
@@ -3093,16 +3096,16 @@
         <v>122</v>
       </c>
       <c r="O39" t="n">
-        <v>561.0</v>
+        <v>589.0</v>
       </c>
       <c r="P39" t="n">
-        <v>560.0</v>
+        <v>620.0</v>
       </c>
       <c r="Q39" t="n">
-        <v>25324.0</v>
+        <v>25352.0</v>
       </c>
       <c r="R39" t="n">
-        <v>38.0</v>
+        <v>39.0</v>
       </c>
       <c r="S39" t="n">
         <v>74506.0</v>
@@ -3114,7 +3117,7 @@
         <v>43284.0</v>
       </c>
       <c r="V39" t="n">
-        <v>129.0</v>
+        <v>130.0</v>
       </c>
     </row>
     <row r="40">
@@ -3170,7 +3173,7 @@
         <v>19894.0</v>
       </c>
       <c r="R40" t="n">
-        <v>15.0</v>
+        <v>16.0</v>
       </c>
       <c r="S40" t="n">
         <v>50560.0</v>
@@ -3182,7 +3185,7 @@
         <v>43352.0</v>
       </c>
       <c r="V40" t="n">
-        <v>61.0</v>
+        <v>62.0</v>
       </c>
     </row>
     <row r="41">
@@ -3208,10 +3211,10 @@
         <v>4693.0</v>
       </c>
       <c r="H41" t="n">
-        <v>26696.0</v>
+        <v>26726.0</v>
       </c>
       <c r="I41" t="n">
-        <v>3642.0</v>
+        <v>3648.0</v>
       </c>
       <c r="J41" t="n">
         <v>2006.0</v>
@@ -3232,16 +3235,16 @@
         <v>0.0</v>
       </c>
       <c r="P41" t="n">
-        <v>400.0</v>
+        <v>440.0</v>
       </c>
       <c r="Q41" t="n">
         <v>7112.0</v>
       </c>
       <c r="R41" t="n">
-        <v>58.0</v>
+        <v>59.0</v>
       </c>
       <c r="S41" t="n">
-        <v>72635.0</v>
+        <v>73755.0</v>
       </c>
       <c r="T41" t="s">
         <v>126</v>
@@ -3250,7 +3253,7 @@
         <v>43252.0</v>
       </c>
       <c r="V41" t="n">
-        <v>161.0</v>
+        <v>162.0</v>
       </c>
     </row>
     <row r="42">
@@ -3264,7 +3267,7 @@
         <v>11.0</v>
       </c>
       <c r="D42" t="n">
-        <v>4100.0</v>
+        <v>4075.0</v>
       </c>
       <c r="E42" t="n">
         <v>4323.0</v>
@@ -3273,10 +3276,10 @@
         <v>2373.0</v>
       </c>
       <c r="G42" t="n">
-        <v>2299.0</v>
+        <v>2300.0</v>
       </c>
       <c r="H42" t="n">
-        <v>5983.0</v>
+        <v>5984.0</v>
       </c>
       <c r="I42" t="n">
         <v>1177.0</v>
@@ -3297,16 +3300,16 @@
         <v>123</v>
       </c>
       <c r="O42" t="n">
-        <v>408.0</v>
+        <v>421.0</v>
       </c>
       <c r="P42" t="n">
-        <v>400.0</v>
+        <v>440.0</v>
       </c>
       <c r="Q42" t="n">
-        <v>21389.0</v>
+        <v>21402.0</v>
       </c>
       <c r="R42" t="n">
-        <v>17.0</v>
+        <v>18.0</v>
       </c>
       <c r="S42" t="n">
         <v>30372.0</v>
@@ -3318,7 +3321,7 @@
         <v>43370.0</v>
       </c>
       <c r="V42" t="n">
-        <v>43.0</v>
+        <v>44.0</v>
       </c>
     </row>
     <row r="43">
@@ -3374,10 +3377,10 @@
         <v>31593.0</v>
       </c>
       <c r="R43" t="n">
-        <v>22.0</v>
+        <v>23.0</v>
       </c>
       <c r="S43" t="n">
-        <v>23935.0</v>
+        <v>24495.0</v>
       </c>
       <c r="T43" t="s">
         <v>128</v>
@@ -3386,7 +3389,7 @@
         <v>43382.0</v>
       </c>
       <c r="V43" t="n">
-        <v>31.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="44">
@@ -3400,22 +3403,22 @@
         <v>11.0</v>
       </c>
       <c r="D44" t="n">
-        <v>4267.0</v>
+        <v>4270.0</v>
       </c>
       <c r="E44" t="n">
         <v>4374.0</v>
       </c>
       <c r="F44" t="n">
-        <v>3791.0</v>
+        <v>3794.0</v>
       </c>
       <c r="G44" t="n">
-        <v>4099.0</v>
+        <v>4102.0</v>
       </c>
       <c r="H44" t="n">
-        <v>8615.0</v>
+        <v>8621.0</v>
       </c>
       <c r="I44" t="n">
-        <v>2025.0</v>
+        <v>2026.0</v>
       </c>
       <c r="J44" t="n">
         <v>1339.0</v>
@@ -3433,13 +3436,13 @@
         <v>123</v>
       </c>
       <c r="O44" t="n">
-        <v>324.0</v>
+        <v>448.0</v>
       </c>
       <c r="P44" t="n">
-        <v>320.0</v>
+        <v>400.0</v>
       </c>
       <c r="Q44" t="n">
-        <v>21393.0</v>
+        <v>21517.0</v>
       </c>
       <c r="R44" t="n">
         <v>19.0</v>
@@ -3454,7 +3457,7 @@
         <v>43390.0</v>
       </c>
       <c r="V44" t="n">
-        <v>23.0</v>
+        <v>24.0</v>
       </c>
     </row>
     <row r="45">
@@ -3480,10 +3483,10 @@
         <v>2576.0</v>
       </c>
       <c r="H45" t="n">
-        <v>7185.0</v>
+        <v>7190.0</v>
       </c>
       <c r="I45" t="n">
-        <v>1376.0</v>
+        <v>1377.0</v>
       </c>
       <c r="J45" t="n">
         <v>3497.0</v>
@@ -3501,19 +3504,19 @@
         <v>123</v>
       </c>
       <c r="O45" t="n">
-        <v>336.0</v>
+        <v>424.0</v>
       </c>
       <c r="P45" t="n">
-        <v>160.0</v>
+        <v>200.0</v>
       </c>
       <c r="Q45" t="n">
-        <v>48974.0</v>
+        <v>49062.0</v>
       </c>
       <c r="R45" t="n">
-        <v>30.0</v>
+        <v>31.0</v>
       </c>
       <c r="S45" t="n">
-        <v>38605.0</v>
+        <v>40005.0</v>
       </c>
       <c r="T45" t="s">
         <v>128</v>
@@ -3522,7 +3525,7 @@
         <v>43390.0</v>
       </c>
       <c r="V45" t="n">
-        <v>23.0</v>
+        <v>24.0</v>
       </c>
     </row>
     <row r="46">
@@ -3536,19 +3539,19 @@
         <v>7.0</v>
       </c>
       <c r="D46" t="n">
-        <v>2304.0</v>
+        <v>2318.0</v>
       </c>
       <c r="E46" t="n">
         <v>2364.0</v>
       </c>
       <c r="F46" t="n">
-        <v>180.0</v>
+        <v>182.0</v>
       </c>
       <c r="G46" t="n">
-        <v>85.0</v>
+        <v>87.0</v>
       </c>
       <c r="H46" t="n">
-        <v>308.0</v>
+        <v>312.0</v>
       </c>
       <c r="I46" t="n">
         <v>77.0</v>
@@ -3584,13 +3587,13 @@
         <v>0.0</v>
       </c>
       <c r="T46" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="U46" t="n" s="2">
         <v>43376.0</v>
       </c>
       <c r="V46" t="n">
-        <v>37.0</v>
+        <v>38.0</v>
       </c>
     </row>
     <row r="47">
@@ -3604,22 +3607,22 @@
         <v>12.0</v>
       </c>
       <c r="D47" t="n">
-        <v>4401.0</v>
+        <v>4196.0</v>
       </c>
       <c r="E47" t="n">
         <v>4919.0</v>
       </c>
       <c r="F47" t="n">
-        <v>10892.0</v>
+        <v>10920.0</v>
       </c>
       <c r="G47" t="n">
-        <v>11609.0</v>
+        <v>11625.0</v>
       </c>
       <c r="H47" t="n">
-        <v>25974.0</v>
+        <v>26011.0</v>
       </c>
       <c r="I47" t="n">
-        <v>8953.0</v>
+        <v>8962.0</v>
       </c>
       <c r="J47" t="n">
         <v>2205.0</v>
@@ -3637,28 +3640,28 @@
         <v>123</v>
       </c>
       <c r="O47" t="n">
-        <v>1156.0</v>
+        <v>1316.0</v>
       </c>
       <c r="P47" t="n">
-        <v>370.0</v>
+        <v>450.0</v>
       </c>
       <c r="Q47" t="n">
-        <v>74860.0</v>
+        <v>75020.0</v>
       </c>
       <c r="R47" t="n">
         <v>22.0</v>
       </c>
       <c r="S47" t="n">
-        <v>80670.0</v>
+        <v>81790.0</v>
       </c>
       <c r="T47" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="U47" t="n" s="2">
         <v>43390.0</v>
       </c>
       <c r="V47" t="n">
-        <v>23.0</v>
+        <v>24.0</v>
       </c>
     </row>
     <row r="48">
@@ -3678,16 +3681,16 @@
         <v>4117.0</v>
       </c>
       <c r="F48" t="n">
-        <v>3014.0</v>
+        <v>3016.0</v>
       </c>
       <c r="G48" t="n">
         <v>3028.0</v>
       </c>
       <c r="H48" t="n">
-        <v>15489.0</v>
+        <v>15497.0</v>
       </c>
       <c r="I48" t="n">
-        <v>3272.0</v>
+        <v>3273.0</v>
       </c>
       <c r="J48" t="n">
         <v>1889.0</v>
@@ -3705,16 +3708,16 @@
         <v>122</v>
       </c>
       <c r="O48" t="n">
-        <v>425.0</v>
+        <v>483.0</v>
       </c>
       <c r="P48" t="n">
-        <v>360.0</v>
+        <v>440.0</v>
       </c>
       <c r="Q48" t="n">
-        <v>32985.0</v>
+        <v>33043.0</v>
       </c>
       <c r="R48" t="n">
-        <v>36.0</v>
+        <v>37.0</v>
       </c>
       <c r="S48" t="n">
         <v>67215.0</v>
@@ -3726,7 +3729,7 @@
         <v>43230.0</v>
       </c>
       <c r="V48" t="n">
-        <v>183.0</v>
+        <v>184.0</v>
       </c>
     </row>
     <row r="49">
@@ -3746,16 +3749,16 @@
         <v>4325.0</v>
       </c>
       <c r="F49" t="n">
-        <v>6358.0</v>
+        <v>6373.0</v>
       </c>
       <c r="G49" t="n">
-        <v>6608.0</v>
+        <v>6609.0</v>
       </c>
       <c r="H49" t="n">
-        <v>18218.0</v>
+        <v>18230.0</v>
       </c>
       <c r="I49" t="n">
-        <v>3765.0</v>
+        <v>3767.0</v>
       </c>
       <c r="J49" t="n">
         <v>4372.0</v>
@@ -3773,19 +3776,19 @@
         <v>124</v>
       </c>
       <c r="O49" t="n">
-        <v>54.0</v>
+        <v>59.0</v>
       </c>
       <c r="P49" t="n">
-        <v>240.0</v>
+        <v>280.0</v>
       </c>
       <c r="Q49" t="n">
-        <v>20681.0</v>
+        <v>20686.0</v>
       </c>
       <c r="R49" t="n">
-        <v>57.0</v>
+        <v>58.0</v>
       </c>
       <c r="S49" t="n">
-        <v>75197.0</v>
+        <v>76317.0</v>
       </c>
       <c r="T49" t="s">
         <v>128</v>
@@ -3794,7 +3797,7 @@
         <v>43184.0</v>
       </c>
       <c r="V49" t="n">
-        <v>229.0</v>
+        <v>230.0</v>
       </c>
     </row>
     <row r="50">
@@ -3808,19 +3811,19 @@
         <v>12.0</v>
       </c>
       <c r="D50" t="n">
-        <v>4181.0</v>
+        <v>4210.0</v>
       </c>
       <c r="E50" t="n">
         <v>4619.0</v>
       </c>
       <c r="F50" t="n">
-        <v>6346.0</v>
+        <v>6347.0</v>
       </c>
       <c r="G50" t="n">
         <v>6138.0</v>
       </c>
       <c r="H50" t="n">
-        <v>14014.0</v>
+        <v>14015.0</v>
       </c>
       <c r="I50" t="n">
         <v>2651.0</v>
@@ -3862,7 +3865,7 @@
         <v>43314.0</v>
       </c>
       <c r="V50" t="n">
-        <v>99.0</v>
+        <v>100.0</v>
       </c>
     </row>
     <row r="51">
@@ -3930,7 +3933,7 @@
         <v>43254.0</v>
       </c>
       <c r="V51" t="n">
-        <v>159.0</v>
+        <v>160.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Scrollbars and visual improvements
</commit_message>
<xml_diff>
--- a/docs/data/memberstats.xlsx
+++ b/docs/data/memberstats.xlsx
@@ -374,7 +374,7 @@
     <t>Inferno</t>
   </si>
   <si>
-    <t>topdosl33ts</t>
+    <t>CarvaPower.</t>
   </si>
   <si>
     <t>Bruno Lopez</t>
@@ -407,13 +407,13 @@
     <t>Arena 9</t>
   </si>
   <si>
+    <t>Arena 10</t>
+  </si>
+  <si>
+    <t>Arena 8</t>
+  </si>
+  <si>
     <t>League 3</t>
-  </si>
-  <si>
-    <t>Arena 10</t>
-  </si>
-  <si>
-    <t>Arena 8</t>
   </si>
 </sst>
 </file>
@@ -547,22 +547,22 @@
         <v>11.0</v>
       </c>
       <c r="D2" t="n">
-        <v>4353.0</v>
+        <v>4504.0</v>
       </c>
       <c r="E2" t="n">
         <v>4653.0</v>
       </c>
       <c r="F2" t="n">
-        <v>2241.0</v>
+        <v>2268.0</v>
       </c>
       <c r="G2" t="n">
-        <v>2084.0</v>
+        <v>2091.0</v>
       </c>
       <c r="H2" t="n">
-        <v>7015.0</v>
+        <v>7049.0</v>
       </c>
       <c r="I2" t="n">
-        <v>1149.0</v>
+        <v>1156.0</v>
       </c>
       <c r="J2" t="n">
         <v>2664.0</v>
@@ -580,19 +580,19 @@
         <v>122</v>
       </c>
       <c r="O2" t="n">
-        <v>658.0</v>
+        <v>90.0</v>
       </c>
       <c r="P2" t="n">
-        <v>400.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q2" t="n">
-        <v>28008.0</v>
+        <v>28316.0</v>
       </c>
       <c r="R2" t="n">
         <v>44.0</v>
       </c>
       <c r="S2" t="n">
-        <v>81460.0</v>
+        <v>83420.0</v>
       </c>
       <c r="T2" t="s">
         <v>126</v>
@@ -601,7 +601,7 @@
         <v>43302.0</v>
       </c>
       <c r="V2" t="n">
-        <v>112.0</v>
+        <v>114.0</v>
       </c>
     </row>
     <row r="3">
@@ -627,7 +627,7 @@
         <v>1435.0</v>
       </c>
       <c r="H3" t="n">
-        <v>4302.0</v>
+        <v>4305.0</v>
       </c>
       <c r="I3" t="n">
         <v>830.0</v>
@@ -648,19 +648,19 @@
         <v>123</v>
       </c>
       <c r="O3" t="n">
-        <v>239.0</v>
+        <v>88.0</v>
       </c>
       <c r="P3" t="n">
-        <v>160.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q3" t="n">
-        <v>18058.0</v>
+        <v>18146.0</v>
       </c>
       <c r="R3" t="n">
         <v>15.0</v>
       </c>
       <c r="S3" t="n">
-        <v>29760.0</v>
+        <v>30809.0</v>
       </c>
       <c r="T3" t="s">
         <v>127</v>
@@ -669,7 +669,7 @@
         <v>43372.0</v>
       </c>
       <c r="V3" t="n">
-        <v>42.0</v>
+        <v>44.0</v>
       </c>
     </row>
     <row r="4">
@@ -683,22 +683,22 @@
         <v>11.0</v>
       </c>
       <c r="D4" t="n">
-        <v>4175.0</v>
+        <v>4084.0</v>
       </c>
       <c r="E4" t="n">
-        <v>4254.0</v>
+        <v>4292.0</v>
       </c>
       <c r="F4" t="n">
-        <v>2586.0</v>
+        <v>2606.0</v>
       </c>
       <c r="G4" t="n">
-        <v>2619.0</v>
+        <v>2634.0</v>
       </c>
       <c r="H4" t="n">
-        <v>6201.0</v>
+        <v>6233.0</v>
       </c>
       <c r="I4" t="n">
-        <v>1067.0</v>
+        <v>1069.0</v>
       </c>
       <c r="J4" t="n">
         <v>1649.0</v>
@@ -716,16 +716,16 @@
         <v>122</v>
       </c>
       <c r="O4" t="n">
-        <v>76.0</v>
+        <v>10.0</v>
       </c>
       <c r="P4" t="n">
-        <v>480.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q4" t="n">
-        <v>8986.0</v>
+        <v>9028.0</v>
       </c>
       <c r="R4" t="n">
-        <v>44.0</v>
+        <v>45.0</v>
       </c>
       <c r="S4" t="n">
         <v>61366.0</v>
@@ -737,7 +737,7 @@
         <v>43082.0</v>
       </c>
       <c r="V4" t="n">
-        <v>332.0</v>
+        <v>334.0</v>
       </c>
     </row>
     <row r="5">
@@ -763,10 +763,10 @@
         <v>658.0</v>
       </c>
       <c r="H5" t="n">
-        <v>1997.0</v>
+        <v>2000.0</v>
       </c>
       <c r="I5" t="n">
-        <v>386.0</v>
+        <v>387.0</v>
       </c>
       <c r="J5" t="n">
         <v>1432.0</v>
@@ -784,19 +784,19 @@
         <v>123</v>
       </c>
       <c r="O5" t="n">
-        <v>130.0</v>
+        <v>21.0</v>
       </c>
       <c r="P5" t="n">
-        <v>144.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q5" t="n">
-        <v>16925.0</v>
+        <v>16956.0</v>
       </c>
       <c r="R5" t="n">
         <v>4.0</v>
       </c>
       <c r="S5" t="n">
-        <v>9415.0</v>
+        <v>10640.0</v>
       </c>
       <c r="T5" t="s">
         <v>129</v>
@@ -805,7 +805,7 @@
         <v>43397.0</v>
       </c>
       <c r="V5" t="n">
-        <v>17.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="6">
@@ -819,22 +819,22 @@
         <v>10.0</v>
       </c>
       <c r="D6" t="n">
-        <v>3933.0</v>
+        <v>4021.0</v>
       </c>
       <c r="E6" t="n">
         <v>4142.0</v>
       </c>
       <c r="F6" t="n">
-        <v>1230.0</v>
+        <v>1238.0</v>
       </c>
       <c r="G6" t="n">
-        <v>1263.0</v>
+        <v>1269.0</v>
       </c>
       <c r="H6" t="n">
-        <v>3192.0</v>
+        <v>3211.0</v>
       </c>
       <c r="I6" t="n">
-        <v>499.0</v>
+        <v>502.0</v>
       </c>
       <c r="J6" t="n">
         <v>310.0</v>
@@ -852,28 +852,28 @@
         <v>123</v>
       </c>
       <c r="O6" t="n">
-        <v>713.0</v>
+        <v>69.0</v>
       </c>
       <c r="P6" t="n">
-        <v>520.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q6" t="n">
-        <v>15971.0</v>
+        <v>16206.0</v>
       </c>
       <c r="R6" t="n">
         <v>28.0</v>
       </c>
       <c r="S6" t="n">
-        <v>38951.0</v>
+        <v>41120.0</v>
       </c>
       <c r="T6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="U6" t="n" s="2">
         <v>43356.0</v>
       </c>
       <c r="V6" t="n">
-        <v>58.0</v>
+        <v>60.0</v>
       </c>
     </row>
     <row r="7">
@@ -923,7 +923,7 @@
         <v>0.0</v>
       </c>
       <c r="P7" t="n">
-        <v>280.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q7" t="n">
         <v>2125.0</v>
@@ -941,7 +941,7 @@
         <v>43364.0</v>
       </c>
       <c r="V7" t="n">
-        <v>50.0</v>
+        <v>52.0</v>
       </c>
     </row>
     <row r="8">
@@ -955,22 +955,22 @@
         <v>11.0</v>
       </c>
       <c r="D8" t="n">
-        <v>4293.0</v>
+        <v>4325.0</v>
       </c>
       <c r="E8" t="n">
         <v>4497.0</v>
       </c>
       <c r="F8" t="n">
-        <v>1910.0</v>
+        <v>1916.0</v>
       </c>
       <c r="G8" t="n">
-        <v>1806.0</v>
+        <v>1808.0</v>
       </c>
       <c r="H8" t="n">
-        <v>7586.0</v>
+        <v>7612.0</v>
       </c>
       <c r="I8" t="n">
-        <v>1115.0</v>
+        <v>1119.0</v>
       </c>
       <c r="J8" t="n">
         <v>1384.0</v>
@@ -988,28 +988,28 @@
         <v>124</v>
       </c>
       <c r="O8" t="n">
-        <v>205.0</v>
+        <v>48.0</v>
       </c>
       <c r="P8" t="n">
-        <v>440.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q8" t="n">
-        <v>25100.0</v>
+        <v>25224.0</v>
       </c>
       <c r="R8" t="n">
-        <v>56.0</v>
+        <v>57.0</v>
       </c>
       <c r="S8" t="n">
-        <v>69275.0</v>
+        <v>70395.0</v>
       </c>
       <c r="T8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="U8" t="n" s="2">
         <v>43058.0</v>
       </c>
       <c r="V8" t="n">
-        <v>356.0</v>
+        <v>358.0</v>
       </c>
     </row>
     <row r="9">
@@ -1023,22 +1023,22 @@
         <v>11.0</v>
       </c>
       <c r="D9" t="n">
-        <v>4135.0</v>
+        <v>4145.0</v>
       </c>
       <c r="E9" t="n">
         <v>4496.0</v>
       </c>
       <c r="F9" t="n">
-        <v>2332.0</v>
+        <v>2335.0</v>
       </c>
       <c r="G9" t="n">
-        <v>2258.0</v>
+        <v>2261.0</v>
       </c>
       <c r="H9" t="n">
-        <v>5127.0</v>
+        <v>5138.0</v>
       </c>
       <c r="I9" t="n">
-        <v>894.0</v>
+        <v>895.0</v>
       </c>
       <c r="J9" t="n">
         <v>1622.0</v>
@@ -1056,19 +1056,19 @@
         <v>123</v>
       </c>
       <c r="O9" t="n">
-        <v>242.0</v>
+        <v>95.0</v>
       </c>
       <c r="P9" t="n">
-        <v>160.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q9" t="n">
-        <v>24893.0</v>
+        <v>25060.0</v>
       </c>
       <c r="R9" t="n">
-        <v>13.0</v>
+        <v>14.0</v>
       </c>
       <c r="S9" t="n">
-        <v>51832.0</v>
+        <v>53792.0</v>
       </c>
       <c r="T9" t="s">
         <v>128</v>
@@ -1077,7 +1077,7 @@
         <v>43390.0</v>
       </c>
       <c r="V9" t="n">
-        <v>24.0</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="10">
@@ -1103,10 +1103,10 @@
         <v>1149.0</v>
       </c>
       <c r="H10" t="n">
-        <v>4621.0</v>
+        <v>4623.0</v>
       </c>
       <c r="I10" t="n">
-        <v>1231.0</v>
+        <v>1232.0</v>
       </c>
       <c r="J10" t="n">
         <v>858.0</v>
@@ -1124,13 +1124,13 @@
         <v>123</v>
       </c>
       <c r="O10" t="n">
-        <v>52.0</v>
+        <v>0.0</v>
       </c>
       <c r="P10" t="n">
-        <v>40.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q10" t="n">
-        <v>28873.0</v>
+        <v>28889.0</v>
       </c>
       <c r="R10" t="n">
         <v>7.0</v>
@@ -1145,7 +1145,7 @@
         <v>43123.0</v>
       </c>
       <c r="V10" t="n">
-        <v>291.0</v>
+        <v>293.0</v>
       </c>
     </row>
     <row r="11">
@@ -1159,22 +1159,22 @@
         <v>11.0</v>
       </c>
       <c r="D11" t="n">
-        <v>4267.0</v>
+        <v>4260.0</v>
       </c>
       <c r="E11" t="n">
         <v>4501.0</v>
       </c>
       <c r="F11" t="n">
-        <v>2397.0</v>
+        <v>2410.0</v>
       </c>
       <c r="G11" t="n">
-        <v>2221.0</v>
+        <v>2235.0</v>
       </c>
       <c r="H11" t="n">
-        <v>10650.0</v>
+        <v>10682.0</v>
       </c>
       <c r="I11" t="n">
-        <v>2365.0</v>
+        <v>2372.0</v>
       </c>
       <c r="J11" t="n">
         <v>1906.0</v>
@@ -1192,19 +1192,19 @@
         <v>124</v>
       </c>
       <c r="O11" t="n">
-        <v>76.0</v>
+        <v>10.0</v>
       </c>
       <c r="P11" t="n">
-        <v>560.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q11" t="n">
-        <v>3208.0</v>
+        <v>3268.0</v>
       </c>
       <c r="R11" t="n">
         <v>57.0</v>
       </c>
       <c r="S11" t="n">
-        <v>78510.0</v>
+        <v>80190.0</v>
       </c>
       <c r="T11" t="s">
         <v>128</v>
@@ -1213,7 +1213,7 @@
         <v>43123.0</v>
       </c>
       <c r="V11" t="n">
-        <v>291.0</v>
+        <v>293.0</v>
       </c>
     </row>
     <row r="12">
@@ -1233,16 +1233,16 @@
         <v>4731.0</v>
       </c>
       <c r="F12" t="n">
-        <v>2240.0</v>
+        <v>2258.0</v>
       </c>
       <c r="G12" t="n">
-        <v>1752.0</v>
+        <v>1753.0</v>
       </c>
       <c r="H12" t="n">
-        <v>9421.0</v>
+        <v>9471.0</v>
       </c>
       <c r="I12" t="n">
-        <v>1363.0</v>
+        <v>1367.0</v>
       </c>
       <c r="J12" t="n">
         <v>4199.0</v>
@@ -1260,19 +1260,19 @@
         <v>123</v>
       </c>
       <c r="O12" t="n">
-        <v>988.0</v>
+        <v>194.0</v>
       </c>
       <c r="P12" t="n">
-        <v>590.0</v>
+        <v>90.0</v>
       </c>
       <c r="Q12" t="n">
-        <v>89385.0</v>
+        <v>89983.0</v>
       </c>
       <c r="R12" t="n">
-        <v>75.0</v>
+        <v>76.0</v>
       </c>
       <c r="S12" t="n">
-        <v>72880.0</v>
+        <v>74280.0</v>
       </c>
       <c r="T12" t="s">
         <v>126</v>
@@ -1281,7 +1281,7 @@
         <v>43397.0</v>
       </c>
       <c r="V12" t="n">
-        <v>17.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="13">
@@ -1328,7 +1328,7 @@
         <v>123</v>
       </c>
       <c r="O13" t="n">
-        <v>36.0</v>
+        <v>0.0</v>
       </c>
       <c r="P13" t="n">
         <v>0.0</v>
@@ -1349,7 +1349,7 @@
         <v>43218.0</v>
       </c>
       <c r="V13" t="n">
-        <v>196.0</v>
+        <v>198.0</v>
       </c>
     </row>
     <row r="14">
@@ -1363,22 +1363,22 @@
         <v>11.0</v>
       </c>
       <c r="D14" t="n">
-        <v>4306.0</v>
+        <v>4204.0</v>
       </c>
       <c r="E14" t="n">
         <v>4389.0</v>
       </c>
       <c r="F14" t="n">
-        <v>1356.0</v>
+        <v>1368.0</v>
       </c>
       <c r="G14" t="n">
-        <v>1199.0</v>
+        <v>1212.0</v>
       </c>
       <c r="H14" t="n">
-        <v>5506.0</v>
+        <v>5535.0</v>
       </c>
       <c r="I14" t="n">
-        <v>758.0</v>
+        <v>762.0</v>
       </c>
       <c r="J14" t="n">
         <v>1199.0</v>
@@ -1396,28 +1396,28 @@
         <v>124</v>
       </c>
       <c r="O14" t="n">
-        <v>537.0</v>
+        <v>32.0</v>
       </c>
       <c r="P14" t="n">
-        <v>520.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q14" t="n">
-        <v>37746.0</v>
+        <v>38008.0</v>
       </c>
       <c r="R14" t="n">
         <v>62.0</v>
       </c>
       <c r="S14" t="n">
-        <v>73320.0</v>
+        <v>75000.0</v>
       </c>
       <c r="T14" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="U14" t="n" s="2">
         <v>43218.0</v>
       </c>
       <c r="V14" t="n">
-        <v>196.0</v>
+        <v>198.0</v>
       </c>
     </row>
     <row r="15">
@@ -1431,19 +1431,19 @@
         <v>12.0</v>
       </c>
       <c r="D15" t="n">
-        <v>4296.0</v>
+        <v>4244.0</v>
       </c>
       <c r="E15" t="n">
         <v>4521.0</v>
       </c>
       <c r="F15" t="n">
-        <v>4646.0</v>
+        <v>4647.0</v>
       </c>
       <c r="G15" t="n">
-        <v>5040.0</v>
+        <v>5043.0</v>
       </c>
       <c r="H15" t="n">
-        <v>10739.0</v>
+        <v>10744.0</v>
       </c>
       <c r="I15" t="n">
         <v>2073.0</v>
@@ -1464,13 +1464,13 @@
         <v>123</v>
       </c>
       <c r="O15" t="n">
-        <v>938.0</v>
+        <v>36.0</v>
       </c>
       <c r="P15" t="n">
-        <v>480.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q15" t="n">
-        <v>53129.0</v>
+        <v>53413.0</v>
       </c>
       <c r="R15" t="n">
         <v>31.0</v>
@@ -1485,7 +1485,7 @@
         <v>43390.0</v>
       </c>
       <c r="V15" t="n">
-        <v>24.0</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="16">
@@ -1508,10 +1508,10 @@
         <v>1778.0</v>
       </c>
       <c r="G16" t="n">
-        <v>1705.0</v>
+        <v>1706.0</v>
       </c>
       <c r="H16" t="n">
-        <v>6597.0</v>
+        <v>6598.0</v>
       </c>
       <c r="I16" t="n">
         <v>1405.0</v>
@@ -1532,10 +1532,10 @@
         <v>123</v>
       </c>
       <c r="O16" t="n">
-        <v>70.0</v>
+        <v>0.0</v>
       </c>
       <c r="P16" t="n">
-        <v>160.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q16" t="n">
         <v>44017.0</v>
@@ -1553,7 +1553,7 @@
         <v>43410.0</v>
       </c>
       <c r="V16" t="n">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="17">
@@ -1567,22 +1567,22 @@
         <v>11.0</v>
       </c>
       <c r="D17" t="n">
-        <v>4067.0</v>
+        <v>4249.0</v>
       </c>
       <c r="E17" t="n">
         <v>4416.0</v>
       </c>
       <c r="F17" t="n">
-        <v>2272.0</v>
+        <v>2279.0</v>
       </c>
       <c r="G17" t="n">
-        <v>2077.0</v>
+        <v>2079.0</v>
       </c>
       <c r="H17" t="n">
-        <v>6704.0</v>
+        <v>6713.0</v>
       </c>
       <c r="I17" t="n">
-        <v>1079.0</v>
+        <v>1082.0</v>
       </c>
       <c r="J17" t="n">
         <v>3630.0</v>
@@ -1600,13 +1600,13 @@
         <v>122</v>
       </c>
       <c r="O17" t="n">
-        <v>60.0</v>
+        <v>16.0</v>
       </c>
       <c r="P17" t="n">
-        <v>360.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q17" t="n">
-        <v>20425.0</v>
+        <v>20567.0</v>
       </c>
       <c r="R17" t="n">
         <v>43.0</v>
@@ -1621,7 +1621,7 @@
         <v>43275.0</v>
       </c>
       <c r="V17" t="n">
-        <v>139.0</v>
+        <v>141.0</v>
       </c>
     </row>
     <row r="18">
@@ -1668,13 +1668,13 @@
         <v>122</v>
       </c>
       <c r="O18" t="n">
-        <v>417.0</v>
+        <v>0.0</v>
       </c>
       <c r="P18" t="n">
-        <v>410.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q18" t="n">
-        <v>30713.0</v>
+        <v>30761.0</v>
       </c>
       <c r="R18" t="n">
         <v>14.0</v>
@@ -1689,7 +1689,7 @@
         <v>43220.0</v>
       </c>
       <c r="V18" t="n">
-        <v>194.0</v>
+        <v>196.0</v>
       </c>
     </row>
     <row r="19">
@@ -1703,22 +1703,22 @@
         <v>11.0</v>
       </c>
       <c r="D19" t="n">
-        <v>4170.0</v>
+        <v>4141.0</v>
       </c>
       <c r="E19" t="n">
         <v>4577.0</v>
       </c>
       <c r="F19" t="n">
-        <v>2773.0</v>
+        <v>2783.0</v>
       </c>
       <c r="G19" t="n">
-        <v>2527.0</v>
+        <v>2539.0</v>
       </c>
       <c r="H19" t="n">
-        <v>6570.0</v>
+        <v>6597.0</v>
       </c>
       <c r="I19" t="n">
-        <v>711.0</v>
+        <v>716.0</v>
       </c>
       <c r="J19" t="n">
         <v>3595.0</v>
@@ -1736,19 +1736,19 @@
         <v>122</v>
       </c>
       <c r="O19" t="n">
-        <v>149.0</v>
+        <v>20.0</v>
       </c>
       <c r="P19" t="n">
-        <v>410.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q19" t="n">
-        <v>21793.0</v>
+        <v>21823.0</v>
       </c>
       <c r="R19" t="n">
-        <v>47.0</v>
+        <v>48.0</v>
       </c>
       <c r="S19" t="n">
-        <v>77025.0</v>
+        <v>78985.0</v>
       </c>
       <c r="T19" t="s">
         <v>128</v>
@@ -1757,7 +1757,7 @@
         <v>43058.0</v>
       </c>
       <c r="V19" t="n">
-        <v>356.0</v>
+        <v>358.0</v>
       </c>
     </row>
     <row r="20">
@@ -1771,22 +1771,22 @@
         <v>12.0</v>
       </c>
       <c r="D20" t="n">
-        <v>4244.0</v>
+        <v>4335.0</v>
       </c>
       <c r="E20" t="n">
         <v>4512.0</v>
       </c>
       <c r="F20" t="n">
-        <v>2979.0</v>
+        <v>2989.0</v>
       </c>
       <c r="G20" t="n">
-        <v>2865.0</v>
+        <v>2868.0</v>
       </c>
       <c r="H20" t="n">
-        <v>6779.0</v>
+        <v>6791.0</v>
       </c>
       <c r="I20" t="n">
-        <v>1236.0</v>
+        <v>1239.0</v>
       </c>
       <c r="J20" t="n">
         <v>2092.0</v>
@@ -1804,28 +1804,28 @@
         <v>122</v>
       </c>
       <c r="O20" t="n">
-        <v>362.0</v>
+        <v>74.0</v>
       </c>
       <c r="P20" t="n">
-        <v>360.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q20" t="n">
-        <v>45444.0</v>
+        <v>45578.0</v>
       </c>
       <c r="R20" t="n">
         <v>34.0</v>
       </c>
       <c r="S20" t="n">
-        <v>48075.0</v>
+        <v>48635.0</v>
       </c>
       <c r="T20" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="U20" t="n" s="2">
         <v>43312.0</v>
       </c>
       <c r="V20" t="n">
-        <v>102.0</v>
+        <v>104.0</v>
       </c>
     </row>
     <row r="21">
@@ -1839,22 +1839,22 @@
         <v>12.0</v>
       </c>
       <c r="D21" t="n">
-        <v>4450.0</v>
+        <v>4539.0</v>
       </c>
       <c r="E21" t="n">
         <v>4767.0</v>
       </c>
       <c r="F21" t="n">
-        <v>6712.0</v>
+        <v>6727.0</v>
       </c>
       <c r="G21" t="n">
-        <v>6660.0</v>
+        <v>6663.0</v>
       </c>
       <c r="H21" t="n">
-        <v>23651.0</v>
+        <v>23732.0</v>
       </c>
       <c r="I21" t="n">
-        <v>2770.0</v>
+        <v>2778.0</v>
       </c>
       <c r="J21" t="n">
         <v>2570.0</v>
@@ -1866,25 +1866,25 @@
         <v>433.0</v>
       </c>
       <c r="M21" t="n">
-        <v>2531.0</v>
+        <v>2562.0</v>
       </c>
       <c r="N21" t="s">
         <v>125</v>
       </c>
       <c r="O21" t="n">
-        <v>500.0</v>
+        <v>50.0</v>
       </c>
       <c r="P21" t="n">
-        <v>630.0</v>
+        <v>60.0</v>
       </c>
       <c r="Q21" t="n">
-        <v>67429.0</v>
+        <v>67681.0</v>
       </c>
       <c r="R21" t="n">
-        <v>88.0</v>
+        <v>89.0</v>
       </c>
       <c r="S21" t="n">
-        <v>81895.0</v>
+        <v>83015.0</v>
       </c>
       <c r="T21" t="s">
         <v>126</v>
@@ -1893,7 +1893,7 @@
         <v>42705.0</v>
       </c>
       <c r="V21" t="n">
-        <v>709.0</v>
+        <v>711.0</v>
       </c>
     </row>
     <row r="22">
@@ -1907,22 +1907,22 @@
         <v>11.0</v>
       </c>
       <c r="D22" t="n">
-        <v>2871.0</v>
+        <v>2828.0</v>
       </c>
       <c r="E22" t="n">
         <v>3176.0</v>
       </c>
       <c r="F22" t="n">
-        <v>3254.0</v>
+        <v>3268.0</v>
       </c>
       <c r="G22" t="n">
-        <v>4544.0</v>
+        <v>4551.0</v>
       </c>
       <c r="H22" t="n">
-        <v>9100.0</v>
+        <v>9120.0</v>
       </c>
       <c r="I22" t="n">
-        <v>2929.0</v>
+        <v>2931.0</v>
       </c>
       <c r="J22" t="n">
         <v>444.0</v>
@@ -1940,19 +1940,19 @@
         <v>123</v>
       </c>
       <c r="O22" t="n">
-        <v>402.0</v>
+        <v>0.0</v>
       </c>
       <c r="P22" t="n">
-        <v>188.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q22" t="n">
-        <v>37809.0</v>
+        <v>37927.0</v>
       </c>
       <c r="R22" t="n">
-        <v>26.0</v>
+        <v>27.0</v>
       </c>
       <c r="S22" t="n">
-        <v>42987.0</v>
+        <v>43197.0</v>
       </c>
       <c r="T22" t="s">
         <v>130</v>
@@ -1961,7 +1961,7 @@
         <v>43151.0</v>
       </c>
       <c r="V22" t="n">
-        <v>263.0</v>
+        <v>265.0</v>
       </c>
     </row>
     <row r="23">
@@ -1975,22 +1975,22 @@
         <v>11.0</v>
       </c>
       <c r="D23" t="n">
-        <v>4092.0</v>
+        <v>4047.0</v>
       </c>
       <c r="E23" t="n">
         <v>4253.0</v>
       </c>
       <c r="F23" t="n">
-        <v>1337.0</v>
+        <v>1342.0</v>
       </c>
       <c r="G23" t="n">
-        <v>1398.0</v>
+        <v>1403.0</v>
       </c>
       <c r="H23" t="n">
-        <v>4578.0</v>
+        <v>4593.0</v>
       </c>
       <c r="I23" t="n">
-        <v>875.0</v>
+        <v>878.0</v>
       </c>
       <c r="J23" t="n">
         <v>507.0</v>
@@ -2008,19 +2008,19 @@
         <v>123</v>
       </c>
       <c r="O23" t="n">
-        <v>160.0</v>
+        <v>44.0</v>
       </c>
       <c r="P23" t="n">
-        <v>80.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q23" t="n">
-        <v>21653.0</v>
+        <v>21777.0</v>
       </c>
       <c r="R23" t="n">
         <v>26.0</v>
       </c>
       <c r="S23" t="n">
-        <v>47003.0</v>
+        <v>49243.0</v>
       </c>
       <c r="T23" t="s">
         <v>128</v>
@@ -2029,7 +2029,7 @@
         <v>43254.0</v>
       </c>
       <c r="V23" t="n">
-        <v>160.0</v>
+        <v>162.0</v>
       </c>
     </row>
     <row r="24">
@@ -2049,13 +2049,13 @@
         <v>4345.0</v>
       </c>
       <c r="F24" t="n">
-        <v>1885.0</v>
+        <v>1886.0</v>
       </c>
       <c r="G24" t="n">
-        <v>1794.0</v>
+        <v>1797.0</v>
       </c>
       <c r="H24" t="n">
-        <v>7972.0</v>
+        <v>7976.0</v>
       </c>
       <c r="I24" t="n">
         <v>2049.0</v>
@@ -2076,13 +2076,13 @@
         <v>123</v>
       </c>
       <c r="O24" t="n">
-        <v>68.0</v>
+        <v>0.0</v>
       </c>
       <c r="P24" t="n">
-        <v>80.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q24" t="n">
-        <v>55684.0</v>
+        <v>55742.0</v>
       </c>
       <c r="R24" t="n">
         <v>29.0</v>
@@ -2097,7 +2097,7 @@
         <v>43380.0</v>
       </c>
       <c r="V24" t="n">
-        <v>34.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="25">
@@ -2111,22 +2111,22 @@
         <v>12.0</v>
       </c>
       <c r="D25" t="n">
-        <v>4179.0</v>
+        <v>4208.0</v>
       </c>
       <c r="E25" t="n">
         <v>4280.0</v>
       </c>
       <c r="F25" t="n">
-        <v>4416.0</v>
+        <v>4417.0</v>
       </c>
       <c r="G25" t="n">
         <v>4360.0</v>
       </c>
       <c r="H25" t="n">
-        <v>18451.0</v>
+        <v>18496.0</v>
       </c>
       <c r="I25" t="n">
-        <v>2935.0</v>
+        <v>2938.0</v>
       </c>
       <c r="J25" t="n">
         <v>2740.0</v>
@@ -2138,25 +2138,25 @@
         <v>2641.0</v>
       </c>
       <c r="M25" t="n">
-        <v>15828.0</v>
+        <v>15912.0</v>
       </c>
       <c r="N25" t="s">
         <v>124</v>
       </c>
       <c r="O25" t="n">
-        <v>78.0</v>
+        <v>0.0</v>
       </c>
       <c r="P25" t="n">
-        <v>630.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q25" t="n">
-        <v>6338.0</v>
+        <v>6378.0</v>
       </c>
       <c r="R25" t="n">
         <v>79.0</v>
       </c>
       <c r="S25" t="n">
-        <v>79705.0</v>
+        <v>81105.0</v>
       </c>
       <c r="T25" t="s">
         <v>128</v>
@@ -2165,7 +2165,7 @@
         <v>42614.0</v>
       </c>
       <c r="V25" t="n">
-        <v>800.0</v>
+        <v>802.0</v>
       </c>
     </row>
     <row r="26">
@@ -2215,7 +2215,7 @@
         <v>0.0</v>
       </c>
       <c r="P26" t="n">
-        <v>80.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q26" t="n">
         <v>9620.0</v>
@@ -2233,7 +2233,7 @@
         <v>43400.0</v>
       </c>
       <c r="V26" t="n">
-        <v>14.0</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="27">
@@ -2247,22 +2247,22 @@
         <v>12.0</v>
       </c>
       <c r="D27" t="n">
-        <v>4074.0</v>
+        <v>4124.0</v>
       </c>
       <c r="E27" t="n">
         <v>4363.0</v>
       </c>
       <c r="F27" t="n">
-        <v>3308.0</v>
+        <v>3323.0</v>
       </c>
       <c r="G27" t="n">
-        <v>3490.0</v>
+        <v>3496.0</v>
       </c>
       <c r="H27" t="n">
-        <v>12219.0</v>
+        <v>12246.0</v>
       </c>
       <c r="I27" t="n">
-        <v>1694.0</v>
+        <v>1699.0</v>
       </c>
       <c r="J27" t="n">
         <v>2757.0</v>
@@ -2280,19 +2280,19 @@
         <v>122</v>
       </c>
       <c r="O27" t="n">
-        <v>878.0</v>
+        <v>48.0</v>
       </c>
       <c r="P27" t="n">
-        <v>400.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q27" t="n">
-        <v>42178.0</v>
+        <v>42469.0</v>
       </c>
       <c r="R27" t="n">
-        <v>66.0</v>
+        <v>67.0</v>
       </c>
       <c r="S27" t="n">
-        <v>73403.0</v>
+        <v>74803.0</v>
       </c>
       <c r="T27" t="s">
         <v>128</v>
@@ -2301,7 +2301,7 @@
         <v>43214.0</v>
       </c>
       <c r="V27" t="n">
-        <v>200.0</v>
+        <v>202.0</v>
       </c>
     </row>
     <row r="28">
@@ -2315,22 +2315,22 @@
         <v>12.0</v>
       </c>
       <c r="D28" t="n">
-        <v>4344.0</v>
+        <v>4446.0</v>
       </c>
       <c r="E28" t="n">
         <v>4653.0</v>
       </c>
       <c r="F28" t="n">
-        <v>3693.0</v>
+        <v>3702.0</v>
       </c>
       <c r="G28" t="n">
-        <v>3411.0</v>
+        <v>3417.0</v>
       </c>
       <c r="H28" t="n">
-        <v>11346.0</v>
+        <v>11366.0</v>
       </c>
       <c r="I28" t="n">
-        <v>1547.0</v>
+        <v>1549.0</v>
       </c>
       <c r="J28" t="n">
         <v>3040.0</v>
@@ -2348,19 +2348,19 @@
         <v>124</v>
       </c>
       <c r="O28" t="n">
-        <v>66.0</v>
+        <v>18.0</v>
       </c>
       <c r="P28" t="n">
-        <v>160.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q28" t="n">
-        <v>32589.0</v>
+        <v>32627.0</v>
       </c>
       <c r="R28" t="n">
-        <v>61.0</v>
+        <v>62.0</v>
       </c>
       <c r="S28" t="n">
-        <v>74515.0</v>
+        <v>75915.0</v>
       </c>
       <c r="T28" t="s">
         <v>126</v>
@@ -2369,7 +2369,7 @@
         <v>42614.0</v>
       </c>
       <c r="V28" t="n">
-        <v>800.0</v>
+        <v>802.0</v>
       </c>
     </row>
     <row r="29">
@@ -2437,7 +2437,7 @@
         <v>43254.0</v>
       </c>
       <c r="V29" t="n">
-        <v>160.0</v>
+        <v>162.0</v>
       </c>
     </row>
     <row r="30">
@@ -2457,16 +2457,16 @@
         <v>4258.0</v>
       </c>
       <c r="F30" t="n">
-        <v>1345.0</v>
+        <v>1357.0</v>
       </c>
       <c r="G30" t="n">
-        <v>1117.0</v>
+        <v>1122.0</v>
       </c>
       <c r="H30" t="n">
-        <v>6548.0</v>
+        <v>6589.0</v>
       </c>
       <c r="I30" t="n">
-        <v>1444.0</v>
+        <v>1449.0</v>
       </c>
       <c r="J30" t="n">
         <v>1859.0</v>
@@ -2484,19 +2484,19 @@
         <v>122</v>
       </c>
       <c r="O30" t="n">
-        <v>608.0</v>
+        <v>10.0</v>
       </c>
       <c r="P30" t="n">
-        <v>560.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q30" t="n">
-        <v>12682.0</v>
+        <v>12760.0</v>
       </c>
       <c r="R30" t="n">
         <v>56.0</v>
       </c>
       <c r="S30" t="n">
-        <v>75662.0</v>
+        <v>76502.0</v>
       </c>
       <c r="T30" t="s">
         <v>128</v>
@@ -2505,7 +2505,7 @@
         <v>43058.0</v>
       </c>
       <c r="V30" t="n">
-        <v>356.0</v>
+        <v>358.0</v>
       </c>
     </row>
     <row r="31">
@@ -2519,22 +2519,22 @@
         <v>10.0</v>
       </c>
       <c r="D31" t="n">
-        <v>3982.0</v>
+        <v>3955.0</v>
       </c>
       <c r="E31" t="n">
         <v>4006.0</v>
       </c>
       <c r="F31" t="n">
-        <v>667.0</v>
+        <v>668.0</v>
       </c>
       <c r="G31" t="n">
-        <v>535.0</v>
+        <v>537.0</v>
       </c>
       <c r="H31" t="n">
-        <v>3358.0</v>
+        <v>3372.0</v>
       </c>
       <c r="I31" t="n">
-        <v>738.0</v>
+        <v>743.0</v>
       </c>
       <c r="J31" t="n">
         <v>838.0</v>
@@ -2555,7 +2555,7 @@
         <v>0.0</v>
       </c>
       <c r="P31" t="n">
-        <v>120.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q31" t="n">
         <v>4623.0</v>
@@ -2564,7 +2564,7 @@
         <v>52.0</v>
       </c>
       <c r="S31" t="n">
-        <v>67101.0</v>
+        <v>68676.0</v>
       </c>
       <c r="T31" t="s">
         <v>127</v>
@@ -2573,7 +2573,7 @@
         <v>43138.0</v>
       </c>
       <c r="V31" t="n">
-        <v>276.0</v>
+        <v>278.0</v>
       </c>
     </row>
     <row r="32">
@@ -2587,22 +2587,22 @@
         <v>12.0</v>
       </c>
       <c r="D32" t="n">
-        <v>4082.0</v>
+        <v>4066.0</v>
       </c>
       <c r="E32" t="n">
         <v>4140.0</v>
       </c>
       <c r="F32" t="n">
-        <v>2141.0</v>
+        <v>2151.0</v>
       </c>
       <c r="G32" t="n">
-        <v>2185.0</v>
+        <v>2193.0</v>
       </c>
       <c r="H32" t="n">
-        <v>6935.0</v>
+        <v>6963.0</v>
       </c>
       <c r="I32" t="n">
-        <v>1562.0</v>
+        <v>1566.0</v>
       </c>
       <c r="J32" t="n">
         <v>1474.0</v>
@@ -2620,19 +2620,19 @@
         <v>122</v>
       </c>
       <c r="O32" t="n">
-        <v>424.0</v>
+        <v>132.0</v>
       </c>
       <c r="P32" t="n">
-        <v>360.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q32" t="n">
-        <v>42403.0</v>
+        <v>42715.0</v>
       </c>
       <c r="R32" t="n">
         <v>37.0</v>
       </c>
       <c r="S32" t="n">
-        <v>70553.0</v>
+        <v>72233.0</v>
       </c>
       <c r="T32" t="s">
         <v>128</v>
@@ -2641,7 +2641,7 @@
         <v>42920.0</v>
       </c>
       <c r="V32" t="n">
-        <v>494.0</v>
+        <v>496.0</v>
       </c>
     </row>
     <row r="33">
@@ -2655,22 +2655,22 @@
         <v>12.0</v>
       </c>
       <c r="D33" t="n">
-        <v>4601.0</v>
+        <v>4553.0</v>
       </c>
       <c r="E33" t="n">
         <v>4798.0</v>
       </c>
       <c r="F33" t="n">
-        <v>5131.0</v>
+        <v>5146.0</v>
       </c>
       <c r="G33" t="n">
-        <v>5237.0</v>
+        <v>5247.0</v>
       </c>
       <c r="H33" t="n">
-        <v>12299.0</v>
+        <v>12325.0</v>
       </c>
       <c r="I33" t="n">
-        <v>2243.0</v>
+        <v>2246.0</v>
       </c>
       <c r="J33" t="n">
         <v>1728.0</v>
@@ -2688,28 +2688,28 @@
         <v>122</v>
       </c>
       <c r="O33" t="n">
-        <v>278.0</v>
+        <v>64.0</v>
       </c>
       <c r="P33" t="n">
-        <v>40.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q33" t="n">
-        <v>59015.0</v>
+        <v>59087.0</v>
       </c>
       <c r="R33" t="n">
         <v>30.0</v>
       </c>
       <c r="S33" t="n">
-        <v>76270.0</v>
+        <v>78230.0</v>
       </c>
       <c r="T33" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="U33" t="n" s="2">
         <v>43058.0</v>
       </c>
       <c r="V33" t="n">
-        <v>356.0</v>
+        <v>358.0</v>
       </c>
     </row>
     <row r="34">
@@ -2732,10 +2732,10 @@
         <v>379.0</v>
       </c>
       <c r="G34" t="n">
-        <v>220.0</v>
+        <v>221.0</v>
       </c>
       <c r="H34" t="n">
-        <v>1567.0</v>
+        <v>1570.0</v>
       </c>
       <c r="I34" t="n">
         <v>268.0</v>
@@ -2756,28 +2756,28 @@
         <v>123</v>
       </c>
       <c r="O34" t="n">
-        <v>388.0</v>
+        <v>0.0</v>
       </c>
       <c r="P34" t="n">
-        <v>240.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q34" t="n">
-        <v>4479.0</v>
+        <v>4521.0</v>
       </c>
       <c r="R34" t="n">
         <v>0.0</v>
       </c>
       <c r="S34" t="n">
-        <v>1137.0</v>
+        <v>1591.0</v>
       </c>
       <c r="T34" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U34" t="n" s="2">
         <v>43409.0</v>
       </c>
       <c r="V34" t="n">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="35">
@@ -2791,19 +2791,19 @@
         <v>10.0</v>
       </c>
       <c r="D35" t="n">
-        <v>3991.0</v>
+        <v>4021.0</v>
       </c>
       <c r="E35" t="n">
-        <v>3991.0</v>
+        <v>4021.0</v>
       </c>
       <c r="F35" t="n">
-        <v>951.0</v>
+        <v>954.0</v>
       </c>
       <c r="G35" t="n">
         <v>968.0</v>
       </c>
       <c r="H35" t="n">
-        <v>4193.0</v>
+        <v>4204.0</v>
       </c>
       <c r="I35" t="n">
         <v>991.0</v>
@@ -2824,28 +2824,28 @@
         <v>123</v>
       </c>
       <c r="O35" t="n">
-        <v>38.0</v>
+        <v>0.0</v>
       </c>
       <c r="P35" t="n">
-        <v>120.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q35" t="n">
-        <v>8348.0</v>
+        <v>8401.0</v>
       </c>
       <c r="R35" t="n">
-        <v>27.0</v>
+        <v>28.0</v>
       </c>
       <c r="S35" t="n">
-        <v>61334.0</v>
+        <v>62383.0</v>
       </c>
       <c r="T35" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="U35" t="n" s="2">
         <v>43312.0</v>
       </c>
       <c r="V35" t="n">
-        <v>102.0</v>
+        <v>104.0</v>
       </c>
     </row>
     <row r="36">
@@ -2859,22 +2859,22 @@
         <v>10.0</v>
       </c>
       <c r="D36" t="n">
-        <v>3742.0</v>
+        <v>3800.0</v>
       </c>
       <c r="E36" t="n">
         <v>4007.0</v>
       </c>
       <c r="F36" t="n">
-        <v>555.0</v>
+        <v>558.0</v>
       </c>
       <c r="G36" t="n">
-        <v>491.0</v>
+        <v>495.0</v>
       </c>
       <c r="H36" t="n">
-        <v>3353.0</v>
+        <v>3366.0</v>
       </c>
       <c r="I36" t="n">
-        <v>691.0</v>
+        <v>696.0</v>
       </c>
       <c r="J36" t="n">
         <v>278.0</v>
@@ -2892,28 +2892,28 @@
         <v>123</v>
       </c>
       <c r="O36" t="n">
-        <v>362.0</v>
+        <v>26.0</v>
       </c>
       <c r="P36" t="n">
-        <v>440.0</v>
+        <v>32.0</v>
       </c>
       <c r="Q36" t="n">
-        <v>16933.0</v>
+        <v>16999.0</v>
       </c>
       <c r="R36" t="n">
-        <v>25.0</v>
+        <v>26.0</v>
       </c>
       <c r="S36" t="n">
-        <v>59445.0</v>
+        <v>60915.0</v>
       </c>
       <c r="T36" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="U36" t="n" s="2">
         <v>43274.0</v>
       </c>
       <c r="V36" t="n">
-        <v>140.0</v>
+        <v>142.0</v>
       </c>
     </row>
     <row r="37">
@@ -2927,22 +2927,22 @@
         <v>10.0</v>
       </c>
       <c r="D37" t="n">
-        <v>4052.0</v>
+        <v>3840.0</v>
       </c>
       <c r="E37" t="n">
         <v>4078.0</v>
       </c>
       <c r="F37" t="n">
-        <v>3457.0</v>
+        <v>3486.0</v>
       </c>
       <c r="G37" t="n">
-        <v>4006.0</v>
+        <v>4046.0</v>
       </c>
       <c r="H37" t="n">
-        <v>9535.0</v>
+        <v>9610.0</v>
       </c>
       <c r="I37" t="n">
-        <v>1754.0</v>
+        <v>1761.0</v>
       </c>
       <c r="J37" t="n">
         <v>224.0</v>
@@ -2960,28 +2960,28 @@
         <v>122</v>
       </c>
       <c r="O37" t="n">
-        <v>144.0</v>
+        <v>92.0</v>
       </c>
       <c r="P37" t="n">
-        <v>200.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q37" t="n">
-        <v>14337.0</v>
+        <v>14565.0</v>
       </c>
       <c r="R37" t="n">
-        <v>34.0</v>
+        <v>35.0</v>
       </c>
       <c r="S37" t="n">
-        <v>69188.0</v>
+        <v>70237.0</v>
       </c>
       <c r="T37" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="U37" t="n" s="2">
         <v>43280.0</v>
       </c>
       <c r="V37" t="n">
-        <v>134.0</v>
+        <v>136.0</v>
       </c>
     </row>
     <row r="38">
@@ -2995,7 +2995,7 @@
         <v>8.0</v>
       </c>
       <c r="D38" t="n">
-        <v>3494.0</v>
+        <v>3470.0</v>
       </c>
       <c r="E38" t="n">
         <v>3630.0</v>
@@ -3004,10 +3004,10 @@
         <v>307.0</v>
       </c>
       <c r="G38" t="n">
-        <v>176.0</v>
+        <v>177.0</v>
       </c>
       <c r="H38" t="n">
-        <v>609.0</v>
+        <v>611.0</v>
       </c>
       <c r="I38" t="n">
         <v>109.0</v>
@@ -3028,13 +3028,13 @@
         <v>123</v>
       </c>
       <c r="O38" t="n">
-        <v>174.0</v>
+        <v>0.0</v>
       </c>
       <c r="P38" t="n">
-        <v>408.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q38" t="n">
-        <v>2551.0</v>
+        <v>2629.0</v>
       </c>
       <c r="R38" t="n">
         <v>2.0</v>
@@ -3049,7 +3049,7 @@
         <v>43360.0</v>
       </c>
       <c r="V38" t="n">
-        <v>54.0</v>
+        <v>56.0</v>
       </c>
     </row>
     <row r="39">
@@ -3063,22 +3063,22 @@
         <v>11.0</v>
       </c>
       <c r="D39" t="n">
-        <v>4052.0</v>
+        <v>4087.0</v>
       </c>
       <c r="E39" t="n">
         <v>4379.0</v>
       </c>
       <c r="F39" t="n">
-        <v>1130.0</v>
+        <v>1143.0</v>
       </c>
       <c r="G39" t="n">
-        <v>981.0</v>
+        <v>987.0</v>
       </c>
       <c r="H39" t="n">
-        <v>4403.0</v>
+        <v>4442.0</v>
       </c>
       <c r="I39" t="n">
-        <v>459.0</v>
+        <v>464.0</v>
       </c>
       <c r="J39" t="n">
         <v>2215.0</v>
@@ -3096,19 +3096,19 @@
         <v>122</v>
       </c>
       <c r="O39" t="n">
-        <v>589.0</v>
+        <v>116.0</v>
       </c>
       <c r="P39" t="n">
-        <v>620.0</v>
+        <v>110.0</v>
       </c>
       <c r="Q39" t="n">
-        <v>25352.0</v>
+        <v>25694.0</v>
       </c>
       <c r="R39" t="n">
         <v>39.0</v>
       </c>
       <c r="S39" t="n">
-        <v>74506.0</v>
+        <v>76466.0</v>
       </c>
       <c r="T39" t="s">
         <v>128</v>
@@ -3117,7 +3117,7 @@
         <v>43284.0</v>
       </c>
       <c r="V39" t="n">
-        <v>130.0</v>
+        <v>132.0</v>
       </c>
     </row>
     <row r="40">
@@ -3131,7 +3131,7 @@
         <v>10.0</v>
       </c>
       <c r="D40" t="n">
-        <v>4137.0</v>
+        <v>4111.0</v>
       </c>
       <c r="E40" t="n">
         <v>4405.0</v>
@@ -3140,13 +3140,13 @@
         <v>1095.0</v>
       </c>
       <c r="G40" t="n">
-        <v>996.0</v>
+        <v>997.0</v>
       </c>
       <c r="H40" t="n">
-        <v>3135.0</v>
+        <v>3140.0</v>
       </c>
       <c r="I40" t="n">
-        <v>654.0</v>
+        <v>657.0</v>
       </c>
       <c r="J40" t="n">
         <v>1700.0</v>
@@ -3164,19 +3164,19 @@
         <v>123</v>
       </c>
       <c r="O40" t="n">
-        <v>204.0</v>
+        <v>105.0</v>
       </c>
       <c r="P40" t="n">
-        <v>280.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q40" t="n">
-        <v>19894.0</v>
+        <v>20067.0</v>
       </c>
       <c r="R40" t="n">
         <v>16.0</v>
       </c>
       <c r="S40" t="n">
-        <v>50560.0</v>
+        <v>52520.0</v>
       </c>
       <c r="T40" t="s">
         <v>128</v>
@@ -3185,7 +3185,7 @@
         <v>43352.0</v>
       </c>
       <c r="V40" t="n">
-        <v>62.0</v>
+        <v>64.0</v>
       </c>
     </row>
     <row r="41">
@@ -3205,16 +3205,16 @@
         <v>4553.0</v>
       </c>
       <c r="F41" t="n">
-        <v>4635.0</v>
+        <v>4639.0</v>
       </c>
       <c r="G41" t="n">
-        <v>4693.0</v>
+        <v>4695.0</v>
       </c>
       <c r="H41" t="n">
-        <v>26726.0</v>
+        <v>26774.0</v>
       </c>
       <c r="I41" t="n">
-        <v>3648.0</v>
+        <v>3653.0</v>
       </c>
       <c r="J41" t="n">
         <v>2006.0</v>
@@ -3235,16 +3235,16 @@
         <v>0.0</v>
       </c>
       <c r="P41" t="n">
-        <v>440.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q41" t="n">
-        <v>7112.0</v>
+        <v>7122.0</v>
       </c>
       <c r="R41" t="n">
-        <v>59.0</v>
+        <v>60.0</v>
       </c>
       <c r="S41" t="n">
-        <v>73755.0</v>
+        <v>74595.0</v>
       </c>
       <c r="T41" t="s">
         <v>126</v>
@@ -3253,7 +3253,7 @@
         <v>43252.0</v>
       </c>
       <c r="V41" t="n">
-        <v>162.0</v>
+        <v>164.0</v>
       </c>
     </row>
     <row r="42">
@@ -3267,22 +3267,22 @@
         <v>11.0</v>
       </c>
       <c r="D42" t="n">
-        <v>4075.0</v>
+        <v>4001.0</v>
       </c>
       <c r="E42" t="n">
         <v>4323.0</v>
       </c>
       <c r="F42" t="n">
-        <v>2373.0</v>
+        <v>2394.0</v>
       </c>
       <c r="G42" t="n">
-        <v>2300.0</v>
+        <v>2316.0</v>
       </c>
       <c r="H42" t="n">
-        <v>5984.0</v>
+        <v>6022.0</v>
       </c>
       <c r="I42" t="n">
-        <v>1177.0</v>
+        <v>1180.0</v>
       </c>
       <c r="J42" t="n">
         <v>2792.0</v>
@@ -3300,19 +3300,19 @@
         <v>123</v>
       </c>
       <c r="O42" t="n">
-        <v>421.0</v>
+        <v>38.0</v>
       </c>
       <c r="P42" t="n">
-        <v>440.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q42" t="n">
-        <v>21402.0</v>
+        <v>21598.0</v>
       </c>
       <c r="R42" t="n">
-        <v>18.0</v>
+        <v>19.0</v>
       </c>
       <c r="S42" t="n">
-        <v>30372.0</v>
+        <v>32332.0</v>
       </c>
       <c r="T42" t="s">
         <v>128</v>
@@ -3321,7 +3321,7 @@
         <v>43370.0</v>
       </c>
       <c r="V42" t="n">
-        <v>44.0</v>
+        <v>46.0</v>
       </c>
     </row>
     <row r="43">
@@ -3341,16 +3341,16 @@
         <v>4272.0</v>
       </c>
       <c r="F43" t="n">
-        <v>2733.0</v>
+        <v>2749.0</v>
       </c>
       <c r="G43" t="n">
-        <v>2655.0</v>
+        <v>2660.0</v>
       </c>
       <c r="H43" t="n">
-        <v>7776.0</v>
+        <v>7799.0</v>
       </c>
       <c r="I43" t="n">
-        <v>2264.0</v>
+        <v>2271.0</v>
       </c>
       <c r="J43" t="n">
         <v>2311.0</v>
@@ -3368,19 +3368,19 @@
         <v>123</v>
       </c>
       <c r="O43" t="n">
-        <v>304.0</v>
+        <v>72.0</v>
       </c>
       <c r="P43" t="n">
-        <v>280.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q43" t="n">
-        <v>31593.0</v>
+        <v>31729.0</v>
       </c>
       <c r="R43" t="n">
-        <v>23.0</v>
+        <v>24.0</v>
       </c>
       <c r="S43" t="n">
-        <v>24495.0</v>
+        <v>26735.0</v>
       </c>
       <c r="T43" t="s">
         <v>128</v>
@@ -3389,7 +3389,7 @@
         <v>43382.0</v>
       </c>
       <c r="V43" t="n">
-        <v>32.0</v>
+        <v>34.0</v>
       </c>
     </row>
     <row r="44">
@@ -3403,22 +3403,22 @@
         <v>11.0</v>
       </c>
       <c r="D44" t="n">
-        <v>4270.0</v>
+        <v>4376.0</v>
       </c>
       <c r="E44" t="n">
-        <v>4374.0</v>
+        <v>4400.0</v>
       </c>
       <c r="F44" t="n">
-        <v>3794.0</v>
+        <v>3816.0</v>
       </c>
       <c r="G44" t="n">
-        <v>4102.0</v>
+        <v>4116.0</v>
       </c>
       <c r="H44" t="n">
-        <v>8621.0</v>
+        <v>8661.0</v>
       </c>
       <c r="I44" t="n">
-        <v>2026.0</v>
+        <v>2033.0</v>
       </c>
       <c r="J44" t="n">
         <v>1339.0</v>
@@ -3436,28 +3436,28 @@
         <v>123</v>
       </c>
       <c r="O44" t="n">
-        <v>448.0</v>
+        <v>10.0</v>
       </c>
       <c r="P44" t="n">
-        <v>400.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q44" t="n">
-        <v>21517.0</v>
+        <v>21859.0</v>
       </c>
       <c r="R44" t="n">
         <v>19.0</v>
       </c>
       <c r="S44" t="n">
-        <v>71172.0</v>
+        <v>73412.0</v>
       </c>
       <c r="T44" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="U44" t="n" s="2">
         <v>43390.0</v>
       </c>
       <c r="V44" t="n">
-        <v>24.0</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="45">
@@ -3471,7 +3471,7 @@
         <v>12.0</v>
       </c>
       <c r="D45" t="n">
-        <v>4134.0</v>
+        <v>4108.0</v>
       </c>
       <c r="E45" t="n">
         <v>4473.0</v>
@@ -3480,10 +3480,10 @@
         <v>2628.0</v>
       </c>
       <c r="G45" t="n">
-        <v>2576.0</v>
+        <v>2577.0</v>
       </c>
       <c r="H45" t="n">
-        <v>7190.0</v>
+        <v>7194.0</v>
       </c>
       <c r="I45" t="n">
         <v>1377.0</v>
@@ -3504,19 +3504,19 @@
         <v>123</v>
       </c>
       <c r="O45" t="n">
-        <v>424.0</v>
+        <v>56.0</v>
       </c>
       <c r="P45" t="n">
-        <v>200.0</v>
+        <v>30.0</v>
       </c>
       <c r="Q45" t="n">
-        <v>49062.0</v>
+        <v>49158.0</v>
       </c>
       <c r="R45" t="n">
-        <v>31.0</v>
+        <v>32.0</v>
       </c>
       <c r="S45" t="n">
-        <v>40005.0</v>
+        <v>40845.0</v>
       </c>
       <c r="T45" t="s">
         <v>128</v>
@@ -3525,7 +3525,7 @@
         <v>43390.0</v>
       </c>
       <c r="V45" t="n">
-        <v>24.0</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="46">
@@ -3536,25 +3536,25 @@
         <v>116</v>
       </c>
       <c r="C46" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="D46" t="n">
-        <v>2318.0</v>
+        <v>2387.0</v>
       </c>
       <c r="E46" t="n">
-        <v>2364.0</v>
+        <v>2387.0</v>
       </c>
       <c r="F46" t="n">
-        <v>182.0</v>
+        <v>185.0</v>
       </c>
       <c r="G46" t="n">
-        <v>87.0</v>
+        <v>88.0</v>
       </c>
       <c r="H46" t="n">
-        <v>312.0</v>
+        <v>325.0</v>
       </c>
       <c r="I46" t="n">
-        <v>77.0</v>
+        <v>79.0</v>
       </c>
       <c r="J46" t="n">
         <v>0.0</v>
@@ -3572,28 +3572,28 @@
         <v>123</v>
       </c>
       <c r="O46" t="n">
-        <v>179.0</v>
+        <v>6.0</v>
       </c>
       <c r="P46" t="n">
-        <v>120.0</v>
+        <v>30.0</v>
       </c>
       <c r="Q46" t="n">
-        <v>1108.0</v>
+        <v>1134.0</v>
       </c>
       <c r="R46" t="n">
         <v>0.0</v>
       </c>
       <c r="S46" t="n">
-        <v>0.0</v>
+        <v>2117.0</v>
       </c>
       <c r="T46" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="U46" t="n" s="2">
         <v>43376.0</v>
       </c>
       <c r="V46" t="n">
-        <v>38.0</v>
+        <v>40.0</v>
       </c>
     </row>
     <row r="47">
@@ -3607,22 +3607,22 @@
         <v>12.0</v>
       </c>
       <c r="D47" t="n">
-        <v>4196.0</v>
+        <v>4685.0</v>
       </c>
       <c r="E47" t="n">
         <v>4919.0</v>
       </c>
       <c r="F47" t="n">
-        <v>10920.0</v>
+        <v>10951.0</v>
       </c>
       <c r="G47" t="n">
-        <v>11625.0</v>
+        <v>11640.0</v>
       </c>
       <c r="H47" t="n">
-        <v>26011.0</v>
+        <v>26060.0</v>
       </c>
       <c r="I47" t="n">
-        <v>8962.0</v>
+        <v>8989.0</v>
       </c>
       <c r="J47" t="n">
         <v>2205.0</v>
@@ -3640,28 +3640,28 @@
         <v>123</v>
       </c>
       <c r="O47" t="n">
-        <v>1316.0</v>
+        <v>86.0</v>
       </c>
       <c r="P47" t="n">
-        <v>450.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q47" t="n">
-        <v>75020.0</v>
+        <v>75484.0</v>
       </c>
       <c r="R47" t="n">
-        <v>22.0</v>
+        <v>23.0</v>
       </c>
       <c r="S47" t="n">
-        <v>81790.0</v>
+        <v>82910.0</v>
       </c>
       <c r="T47" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="U47" t="n" s="2">
         <v>43390.0</v>
       </c>
       <c r="V47" t="n">
-        <v>24.0</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="48">
@@ -3681,16 +3681,16 @@
         <v>4117.0</v>
       </c>
       <c r="F48" t="n">
-        <v>3016.0</v>
+        <v>3034.0</v>
       </c>
       <c r="G48" t="n">
-        <v>3028.0</v>
+        <v>3037.0</v>
       </c>
       <c r="H48" t="n">
-        <v>15497.0</v>
+        <v>15553.0</v>
       </c>
       <c r="I48" t="n">
-        <v>3273.0</v>
+        <v>3281.0</v>
       </c>
       <c r="J48" t="n">
         <v>1889.0</v>
@@ -3708,19 +3708,19 @@
         <v>122</v>
       </c>
       <c r="O48" t="n">
-        <v>483.0</v>
+        <v>44.0</v>
       </c>
       <c r="P48" t="n">
-        <v>440.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q48" t="n">
-        <v>33043.0</v>
+        <v>33165.0</v>
       </c>
       <c r="R48" t="n">
-        <v>37.0</v>
+        <v>38.0</v>
       </c>
       <c r="S48" t="n">
-        <v>67215.0</v>
+        <v>69735.0</v>
       </c>
       <c r="T48" t="s">
         <v>128</v>
@@ -3729,7 +3729,7 @@
         <v>43230.0</v>
       </c>
       <c r="V48" t="n">
-        <v>184.0</v>
+        <v>186.0</v>
       </c>
     </row>
     <row r="49">
@@ -3743,22 +3743,22 @@
         <v>11.0</v>
       </c>
       <c r="D49" t="n">
-        <v>4083.0</v>
+        <v>4174.0</v>
       </c>
       <c r="E49" t="n">
         <v>4325.0</v>
       </c>
       <c r="F49" t="n">
-        <v>6373.0</v>
+        <v>6376.0</v>
       </c>
       <c r="G49" t="n">
         <v>6609.0</v>
       </c>
       <c r="H49" t="n">
-        <v>18230.0</v>
+        <v>18239.0</v>
       </c>
       <c r="I49" t="n">
-        <v>3767.0</v>
+        <v>3769.0</v>
       </c>
       <c r="J49" t="n">
         <v>4372.0</v>
@@ -3776,19 +3776,19 @@
         <v>124</v>
       </c>
       <c r="O49" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="P49" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q49" t="n">
+        <v>20714.0</v>
+      </c>
+      <c r="R49" t="n">
         <v>59.0</v>
       </c>
-      <c r="P49" t="n">
-        <v>280.0</v>
-      </c>
-      <c r="Q49" t="n">
-        <v>20686.0</v>
-      </c>
-      <c r="R49" t="n">
-        <v>58.0</v>
-      </c>
       <c r="S49" t="n">
-        <v>76317.0</v>
+        <v>77717.0</v>
       </c>
       <c r="T49" t="s">
         <v>128</v>
@@ -3797,7 +3797,7 @@
         <v>43184.0</v>
       </c>
       <c r="V49" t="n">
-        <v>230.0</v>
+        <v>232.0</v>
       </c>
     </row>
     <row r="50">
@@ -3811,22 +3811,22 @@
         <v>12.0</v>
       </c>
       <c r="D50" t="n">
-        <v>4210.0</v>
+        <v>4173.0</v>
       </c>
       <c r="E50" t="n">
         <v>4619.0</v>
       </c>
       <c r="F50" t="n">
-        <v>6347.0</v>
+        <v>6372.0</v>
       </c>
       <c r="G50" t="n">
-        <v>6138.0</v>
+        <v>6150.0</v>
       </c>
       <c r="H50" t="n">
-        <v>14015.0</v>
+        <v>14044.0</v>
       </c>
       <c r="I50" t="n">
-        <v>2651.0</v>
+        <v>2660.0</v>
       </c>
       <c r="J50" t="n">
         <v>6501.0</v>
@@ -3844,19 +3844,19 @@
         <v>122</v>
       </c>
       <c r="O50" t="n">
-        <v>70.0</v>
+        <v>0.0</v>
       </c>
       <c r="P50" t="n">
-        <v>120.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q50" t="n">
-        <v>46973.0</v>
+        <v>46993.0</v>
       </c>
       <c r="R50" t="n">
-        <v>28.0</v>
+        <v>29.0</v>
       </c>
       <c r="S50" t="n">
-        <v>41200.0</v>
+        <v>42600.0</v>
       </c>
       <c r="T50" t="s">
         <v>128</v>
@@ -3865,7 +3865,7 @@
         <v>43314.0</v>
       </c>
       <c r="V50" t="n">
-        <v>100.0</v>
+        <v>102.0</v>
       </c>
     </row>
     <row r="51">
@@ -3891,7 +3891,7 @@
         <v>729.0</v>
       </c>
       <c r="H51" t="n">
-        <v>3868.0</v>
+        <v>3869.0</v>
       </c>
       <c r="I51" t="n">
         <v>892.0</v>
@@ -3912,13 +3912,13 @@
         <v>123</v>
       </c>
       <c r="O51" t="n">
-        <v>28.0</v>
+        <v>10.0</v>
       </c>
       <c r="P51" t="n">
-        <v>0.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q51" t="n">
-        <v>24416.0</v>
+        <v>24472.0</v>
       </c>
       <c r="R51" t="n">
         <v>15.0</v>
@@ -3933,7 +3933,7 @@
         <v>43254.0</v>
       </c>
       <c r="V51" t="n">
-        <v>160.0</v>
+        <v>162.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Before removing factors from name and tag
</commit_message>
<xml_diff>
--- a/docs/data/memberstats.xlsx
+++ b/docs/data/memberstats.xlsx
@@ -547,19 +547,19 @@
         <v>11.0</v>
       </c>
       <c r="D2" t="n">
-        <v>4504.0</v>
+        <v>4452.0</v>
       </c>
       <c r="E2" t="n">
         <v>4653.0</v>
       </c>
       <c r="F2" t="n">
-        <v>2268.0</v>
+        <v>2269.0</v>
       </c>
       <c r="G2" t="n">
-        <v>2091.0</v>
+        <v>2094.0</v>
       </c>
       <c r="H2" t="n">
-        <v>7049.0</v>
+        <v>7056.0</v>
       </c>
       <c r="I2" t="n">
         <v>1156.0</v>
@@ -580,13 +580,13 @@
         <v>122</v>
       </c>
       <c r="O2" t="n">
-        <v>90.0</v>
+        <v>209.0</v>
       </c>
       <c r="P2" t="n">
-        <v>40.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q2" t="n">
-        <v>28316.0</v>
+        <v>28435.0</v>
       </c>
       <c r="R2" t="n">
         <v>44.0</v>
@@ -601,7 +601,7 @@
         <v>43302.0</v>
       </c>
       <c r="V2" t="n">
-        <v>114.0</v>
+        <v>115.0</v>
       </c>
     </row>
     <row r="3">
@@ -627,7 +627,7 @@
         <v>1435.0</v>
       </c>
       <c r="H3" t="n">
-        <v>4305.0</v>
+        <v>4306.0</v>
       </c>
       <c r="I3" t="n">
         <v>830.0</v>
@@ -648,13 +648,13 @@
         <v>123</v>
       </c>
       <c r="O3" t="n">
-        <v>88.0</v>
+        <v>194.0</v>
       </c>
       <c r="P3" t="n">
-        <v>40.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q3" t="n">
-        <v>18146.0</v>
+        <v>18252.0</v>
       </c>
       <c r="R3" t="n">
         <v>15.0</v>
@@ -669,7 +669,7 @@
         <v>43372.0</v>
       </c>
       <c r="V3" t="n">
-        <v>44.0</v>
+        <v>45.0</v>
       </c>
     </row>
     <row r="4">
@@ -683,22 +683,22 @@
         <v>11.0</v>
       </c>
       <c r="D4" t="n">
-        <v>4084.0</v>
+        <v>4099.0</v>
       </c>
       <c r="E4" t="n">
         <v>4292.0</v>
       </c>
       <c r="F4" t="n">
-        <v>2606.0</v>
+        <v>2611.0</v>
       </c>
       <c r="G4" t="n">
-        <v>2634.0</v>
+        <v>2639.0</v>
       </c>
       <c r="H4" t="n">
-        <v>6233.0</v>
+        <v>6247.0</v>
       </c>
       <c r="I4" t="n">
-        <v>1069.0</v>
+        <v>1071.0</v>
       </c>
       <c r="J4" t="n">
         <v>1649.0</v>
@@ -719,7 +719,7 @@
         <v>10.0</v>
       </c>
       <c r="P4" t="n">
-        <v>40.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q4" t="n">
         <v>9028.0</v>
@@ -728,7 +728,7 @@
         <v>45.0</v>
       </c>
       <c r="S4" t="n">
-        <v>61366.0</v>
+        <v>62766.0</v>
       </c>
       <c r="T4" t="s">
         <v>128</v>
@@ -737,7 +737,7 @@
         <v>43082.0</v>
       </c>
       <c r="V4" t="n">
-        <v>334.0</v>
+        <v>335.0</v>
       </c>
     </row>
     <row r="5">
@@ -787,7 +787,7 @@
         <v>21.0</v>
       </c>
       <c r="P5" t="n">
-        <v>40.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q5" t="n">
         <v>16956.0</v>
@@ -805,7 +805,7 @@
         <v>43397.0</v>
       </c>
       <c r="V5" t="n">
-        <v>19.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="6">
@@ -819,19 +819,19 @@
         <v>10.0</v>
       </c>
       <c r="D6" t="n">
-        <v>4021.0</v>
+        <v>4040.0</v>
       </c>
       <c r="E6" t="n">
         <v>4142.0</v>
       </c>
       <c r="F6" t="n">
-        <v>1238.0</v>
+        <v>1244.0</v>
       </c>
       <c r="G6" t="n">
-        <v>1269.0</v>
+        <v>1275.0</v>
       </c>
       <c r="H6" t="n">
-        <v>3211.0</v>
+        <v>3225.0</v>
       </c>
       <c r="I6" t="n">
         <v>502.0</v>
@@ -852,13 +852,13 @@
         <v>123</v>
       </c>
       <c r="O6" t="n">
-        <v>69.0</v>
+        <v>203.0</v>
       </c>
       <c r="P6" t="n">
-        <v>40.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q6" t="n">
-        <v>16206.0</v>
+        <v>16340.0</v>
       </c>
       <c r="R6" t="n">
         <v>28.0</v>
@@ -873,7 +873,7 @@
         <v>43356.0</v>
       </c>
       <c r="V6" t="n">
-        <v>60.0</v>
+        <v>61.0</v>
       </c>
     </row>
     <row r="7">
@@ -899,7 +899,7 @@
         <v>2664.0</v>
       </c>
       <c r="H7" t="n">
-        <v>7039.0</v>
+        <v>7040.0</v>
       </c>
       <c r="I7" t="n">
         <v>688.0</v>
@@ -923,7 +923,7 @@
         <v>0.0</v>
       </c>
       <c r="P7" t="n">
-        <v>0.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q7" t="n">
         <v>2125.0</v>
@@ -932,7 +932,7 @@
         <v>40.0</v>
       </c>
       <c r="S7" t="n">
-        <v>57080.0</v>
+        <v>57360.0</v>
       </c>
       <c r="T7" t="s">
         <v>128</v>
@@ -941,7 +941,7 @@
         <v>43364.0</v>
       </c>
       <c r="V7" t="n">
-        <v>52.0</v>
+        <v>53.0</v>
       </c>
     </row>
     <row r="8">
@@ -967,10 +967,10 @@
         <v>1808.0</v>
       </c>
       <c r="H8" t="n">
-        <v>7612.0</v>
+        <v>7622.0</v>
       </c>
       <c r="I8" t="n">
-        <v>1119.0</v>
+        <v>1121.0</v>
       </c>
       <c r="J8" t="n">
         <v>1384.0</v>
@@ -988,19 +988,19 @@
         <v>124</v>
       </c>
       <c r="O8" t="n">
-        <v>48.0</v>
+        <v>74.0</v>
       </c>
       <c r="P8" t="n">
-        <v>40.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q8" t="n">
-        <v>25224.0</v>
+        <v>25250.0</v>
       </c>
       <c r="R8" t="n">
         <v>57.0</v>
       </c>
       <c r="S8" t="n">
-        <v>70395.0</v>
+        <v>70675.0</v>
       </c>
       <c r="T8" t="s">
         <v>126</v>
@@ -1009,7 +1009,7 @@
         <v>43058.0</v>
       </c>
       <c r="V8" t="n">
-        <v>358.0</v>
+        <v>359.0</v>
       </c>
     </row>
     <row r="9">
@@ -1023,7 +1023,7 @@
         <v>11.0</v>
       </c>
       <c r="D9" t="n">
-        <v>4145.0</v>
+        <v>4116.0</v>
       </c>
       <c r="E9" t="n">
         <v>4496.0</v>
@@ -1032,10 +1032,10 @@
         <v>2335.0</v>
       </c>
       <c r="G9" t="n">
-        <v>2261.0</v>
+        <v>2262.0</v>
       </c>
       <c r="H9" t="n">
-        <v>5138.0</v>
+        <v>5140.0</v>
       </c>
       <c r="I9" t="n">
         <v>895.0</v>
@@ -1059,7 +1059,7 @@
         <v>95.0</v>
       </c>
       <c r="P9" t="n">
-        <v>40.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q9" t="n">
         <v>25060.0</v>
@@ -1077,7 +1077,7 @@
         <v>43390.0</v>
       </c>
       <c r="V9" t="n">
-        <v>26.0</v>
+        <v>27.0</v>
       </c>
     </row>
     <row r="10">
@@ -1145,7 +1145,7 @@
         <v>43123.0</v>
       </c>
       <c r="V10" t="n">
-        <v>293.0</v>
+        <v>294.0</v>
       </c>
     </row>
     <row r="11">
@@ -1159,22 +1159,22 @@
         <v>11.0</v>
       </c>
       <c r="D11" t="n">
-        <v>4260.0</v>
+        <v>4458.0</v>
       </c>
       <c r="E11" t="n">
         <v>4501.0</v>
       </c>
       <c r="F11" t="n">
-        <v>2410.0</v>
+        <v>2429.0</v>
       </c>
       <c r="G11" t="n">
-        <v>2235.0</v>
+        <v>2248.0</v>
       </c>
       <c r="H11" t="n">
-        <v>10682.0</v>
+        <v>10716.0</v>
       </c>
       <c r="I11" t="n">
-        <v>2372.0</v>
+        <v>2380.0</v>
       </c>
       <c r="J11" t="n">
         <v>1906.0</v>
@@ -1192,13 +1192,13 @@
         <v>124</v>
       </c>
       <c r="O11" t="n">
-        <v>10.0</v>
+        <v>30.0</v>
       </c>
       <c r="P11" t="n">
-        <v>80.0</v>
+        <v>160.0</v>
       </c>
       <c r="Q11" t="n">
-        <v>3268.0</v>
+        <v>3288.0</v>
       </c>
       <c r="R11" t="n">
         <v>57.0</v>
@@ -1207,13 +1207,13 @@
         <v>80190.0</v>
       </c>
       <c r="T11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="U11" t="n" s="2">
         <v>43123.0</v>
       </c>
       <c r="V11" t="n">
-        <v>293.0</v>
+        <v>294.0</v>
       </c>
     </row>
     <row r="12">
@@ -1239,10 +1239,10 @@
         <v>1753.0</v>
       </c>
       <c r="H12" t="n">
-        <v>9471.0</v>
+        <v>9488.0</v>
       </c>
       <c r="I12" t="n">
-        <v>1367.0</v>
+        <v>1369.0</v>
       </c>
       <c r="J12" t="n">
         <v>4199.0</v>
@@ -1260,19 +1260,19 @@
         <v>123</v>
       </c>
       <c r="O12" t="n">
-        <v>194.0</v>
+        <v>356.0</v>
       </c>
       <c r="P12" t="n">
-        <v>90.0</v>
+        <v>190.0</v>
       </c>
       <c r="Q12" t="n">
-        <v>89983.0</v>
+        <v>90145.0</v>
       </c>
       <c r="R12" t="n">
         <v>76.0</v>
       </c>
       <c r="S12" t="n">
-        <v>74280.0</v>
+        <v>75680.0</v>
       </c>
       <c r="T12" t="s">
         <v>126</v>
@@ -1281,7 +1281,7 @@
         <v>43397.0</v>
       </c>
       <c r="V12" t="n">
-        <v>19.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="13">
@@ -1295,19 +1295,19 @@
         <v>11.0</v>
       </c>
       <c r="D13" t="n">
-        <v>3887.0</v>
+        <v>3891.0</v>
       </c>
       <c r="E13" t="n">
         <v>4163.0</v>
       </c>
       <c r="F13" t="n">
-        <v>3158.0</v>
+        <v>3159.0</v>
       </c>
       <c r="G13" t="n">
-        <v>3338.0</v>
+        <v>3339.0</v>
       </c>
       <c r="H13" t="n">
-        <v>8595.0</v>
+        <v>8601.0</v>
       </c>
       <c r="I13" t="n">
         <v>1342.0</v>
@@ -1340,7 +1340,7 @@
         <v>19.0</v>
       </c>
       <c r="S13" t="n">
-        <v>29191.0</v>
+        <v>30240.0</v>
       </c>
       <c r="T13" t="s">
         <v>127</v>
@@ -1349,7 +1349,7 @@
         <v>43218.0</v>
       </c>
       <c r="V13" t="n">
-        <v>198.0</v>
+        <v>199.0</v>
       </c>
     </row>
     <row r="14">
@@ -1363,22 +1363,22 @@
         <v>11.0</v>
       </c>
       <c r="D14" t="n">
-        <v>4204.0</v>
+        <v>4205.0</v>
       </c>
       <c r="E14" t="n">
         <v>4389.0</v>
       </c>
       <c r="F14" t="n">
-        <v>1368.0</v>
+        <v>1369.0</v>
       </c>
       <c r="G14" t="n">
-        <v>1212.0</v>
+        <v>1213.0</v>
       </c>
       <c r="H14" t="n">
-        <v>5535.0</v>
+        <v>5542.0</v>
       </c>
       <c r="I14" t="n">
-        <v>762.0</v>
+        <v>765.0</v>
       </c>
       <c r="J14" t="n">
         <v>1199.0</v>
@@ -1396,13 +1396,13 @@
         <v>124</v>
       </c>
       <c r="O14" t="n">
-        <v>32.0</v>
+        <v>132.0</v>
       </c>
       <c r="P14" t="n">
-        <v>80.0</v>
+        <v>200.0</v>
       </c>
       <c r="Q14" t="n">
-        <v>38008.0</v>
+        <v>38108.0</v>
       </c>
       <c r="R14" t="n">
         <v>62.0</v>
@@ -1417,7 +1417,7 @@
         <v>43218.0</v>
       </c>
       <c r="V14" t="n">
-        <v>198.0</v>
+        <v>199.0</v>
       </c>
     </row>
     <row r="15">
@@ -1431,22 +1431,22 @@
         <v>12.0</v>
       </c>
       <c r="D15" t="n">
-        <v>4244.0</v>
+        <v>4257.0</v>
       </c>
       <c r="E15" t="n">
         <v>4521.0</v>
       </c>
       <c r="F15" t="n">
-        <v>4647.0</v>
+        <v>4652.0</v>
       </c>
       <c r="G15" t="n">
-        <v>5043.0</v>
+        <v>5048.0</v>
       </c>
       <c r="H15" t="n">
-        <v>10744.0</v>
+        <v>10757.0</v>
       </c>
       <c r="I15" t="n">
-        <v>2073.0</v>
+        <v>2079.0</v>
       </c>
       <c r="J15" t="n">
         <v>1842.0</v>
@@ -1458,25 +1458,25 @@
         <v>4.0</v>
       </c>
       <c r="M15" t="n">
-        <v>15.0</v>
+        <v>22.0</v>
       </c>
       <c r="N15" t="s">
         <v>123</v>
       </c>
       <c r="O15" t="n">
-        <v>36.0</v>
+        <v>308.0</v>
       </c>
       <c r="P15" t="n">
-        <v>40.0</v>
+        <v>160.0</v>
       </c>
       <c r="Q15" t="n">
-        <v>53413.0</v>
+        <v>53685.0</v>
       </c>
       <c r="R15" t="n">
         <v>31.0</v>
       </c>
       <c r="S15" t="n">
-        <v>80010.0</v>
+        <v>81410.0</v>
       </c>
       <c r="T15" t="s">
         <v>128</v>
@@ -1485,7 +1485,7 @@
         <v>43390.0</v>
       </c>
       <c r="V15" t="n">
-        <v>26.0</v>
+        <v>27.0</v>
       </c>
     </row>
     <row r="16">
@@ -1553,7 +1553,7 @@
         <v>43410.0</v>
       </c>
       <c r="V16" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="17">
@@ -1567,19 +1567,19 @@
         <v>11.0</v>
       </c>
       <c r="D17" t="n">
-        <v>4249.0</v>
+        <v>4199.0</v>
       </c>
       <c r="E17" t="n">
         <v>4416.0</v>
       </c>
       <c r="F17" t="n">
-        <v>2279.0</v>
+        <v>2280.0</v>
       </c>
       <c r="G17" t="n">
-        <v>2079.0</v>
+        <v>2082.0</v>
       </c>
       <c r="H17" t="n">
-        <v>6713.0</v>
+        <v>6717.0</v>
       </c>
       <c r="I17" t="n">
         <v>1082.0</v>
@@ -1600,13 +1600,13 @@
         <v>122</v>
       </c>
       <c r="O17" t="n">
-        <v>16.0</v>
+        <v>60.0</v>
       </c>
       <c r="P17" t="n">
-        <v>40.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q17" t="n">
-        <v>20567.0</v>
+        <v>20611.0</v>
       </c>
       <c r="R17" t="n">
         <v>43.0</v>
@@ -1621,7 +1621,7 @@
         <v>43275.0</v>
       </c>
       <c r="V17" t="n">
-        <v>141.0</v>
+        <v>142.0</v>
       </c>
     </row>
     <row r="18">
@@ -1668,13 +1668,13 @@
         <v>122</v>
       </c>
       <c r="O18" t="n">
-        <v>0.0</v>
+        <v>60.0</v>
       </c>
       <c r="P18" t="n">
-        <v>0.0</v>
+        <v>60.0</v>
       </c>
       <c r="Q18" t="n">
-        <v>30761.0</v>
+        <v>30821.0</v>
       </c>
       <c r="R18" t="n">
         <v>14.0</v>
@@ -1689,7 +1689,7 @@
         <v>43220.0</v>
       </c>
       <c r="V18" t="n">
-        <v>196.0</v>
+        <v>197.0</v>
       </c>
     </row>
     <row r="19">
@@ -1703,22 +1703,22 @@
         <v>11.0</v>
       </c>
       <c r="D19" t="n">
-        <v>4141.0</v>
+        <v>4337.0</v>
       </c>
       <c r="E19" t="n">
         <v>4577.0</v>
       </c>
       <c r="F19" t="n">
-        <v>2783.0</v>
+        <v>2792.0</v>
       </c>
       <c r="G19" t="n">
-        <v>2539.0</v>
+        <v>2542.0</v>
       </c>
       <c r="H19" t="n">
-        <v>6597.0</v>
+        <v>6610.0</v>
       </c>
       <c r="I19" t="n">
-        <v>716.0</v>
+        <v>717.0</v>
       </c>
       <c r="J19" t="n">
         <v>3595.0</v>
@@ -1736,13 +1736,13 @@
         <v>122</v>
       </c>
       <c r="O19" t="n">
-        <v>20.0</v>
+        <v>38.0</v>
       </c>
       <c r="P19" t="n">
-        <v>40.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q19" t="n">
-        <v>21823.0</v>
+        <v>21841.0</v>
       </c>
       <c r="R19" t="n">
         <v>48.0</v>
@@ -1751,13 +1751,13 @@
         <v>78985.0</v>
       </c>
       <c r="T19" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="U19" t="n" s="2">
         <v>43058.0</v>
       </c>
       <c r="V19" t="n">
-        <v>358.0</v>
+        <v>359.0</v>
       </c>
     </row>
     <row r="20">
@@ -1771,22 +1771,22 @@
         <v>12.0</v>
       </c>
       <c r="D20" t="n">
-        <v>4335.0</v>
+        <v>4260.0</v>
       </c>
       <c r="E20" t="n">
         <v>4512.0</v>
       </c>
       <c r="F20" t="n">
-        <v>2989.0</v>
+        <v>2992.0</v>
       </c>
       <c r="G20" t="n">
-        <v>2868.0</v>
+        <v>2874.0</v>
       </c>
       <c r="H20" t="n">
-        <v>6791.0</v>
+        <v>6804.0</v>
       </c>
       <c r="I20" t="n">
-        <v>1239.0</v>
+        <v>1243.0</v>
       </c>
       <c r="J20" t="n">
         <v>2092.0</v>
@@ -1804,28 +1804,28 @@
         <v>122</v>
       </c>
       <c r="O20" t="n">
-        <v>74.0</v>
+        <v>270.0</v>
       </c>
       <c r="P20" t="n">
-        <v>80.0</v>
+        <v>160.0</v>
       </c>
       <c r="Q20" t="n">
-        <v>45578.0</v>
+        <v>45774.0</v>
       </c>
       <c r="R20" t="n">
         <v>34.0</v>
       </c>
       <c r="S20" t="n">
-        <v>48635.0</v>
+        <v>49475.0</v>
       </c>
       <c r="T20" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="U20" t="n" s="2">
         <v>43312.0</v>
       </c>
       <c r="V20" t="n">
-        <v>104.0</v>
+        <v>105.0</v>
       </c>
     </row>
     <row r="21">
@@ -1839,22 +1839,22 @@
         <v>12.0</v>
       </c>
       <c r="D21" t="n">
-        <v>4539.0</v>
+        <v>4567.0</v>
       </c>
       <c r="E21" t="n">
         <v>4767.0</v>
       </c>
       <c r="F21" t="n">
-        <v>6727.0</v>
+        <v>6728.0</v>
       </c>
       <c r="G21" t="n">
         <v>6663.0</v>
       </c>
       <c r="H21" t="n">
-        <v>23732.0</v>
+        <v>23750.0</v>
       </c>
       <c r="I21" t="n">
-        <v>2778.0</v>
+        <v>2783.0</v>
       </c>
       <c r="J21" t="n">
         <v>2570.0</v>
@@ -1866,25 +1866,25 @@
         <v>433.0</v>
       </c>
       <c r="M21" t="n">
-        <v>2562.0</v>
+        <v>2569.0</v>
       </c>
       <c r="N21" t="s">
         <v>125</v>
       </c>
       <c r="O21" t="n">
-        <v>50.0</v>
+        <v>196.0</v>
       </c>
       <c r="P21" t="n">
-        <v>60.0</v>
+        <v>140.0</v>
       </c>
       <c r="Q21" t="n">
-        <v>67681.0</v>
+        <v>67827.0</v>
       </c>
       <c r="R21" t="n">
         <v>89.0</v>
       </c>
       <c r="S21" t="n">
-        <v>83015.0</v>
+        <v>84415.0</v>
       </c>
       <c r="T21" t="s">
         <v>126</v>
@@ -1893,7 +1893,7 @@
         <v>42705.0</v>
       </c>
       <c r="V21" t="n">
-        <v>711.0</v>
+        <v>712.0</v>
       </c>
     </row>
     <row r="22">
@@ -1919,10 +1919,10 @@
         <v>4551.0</v>
       </c>
       <c r="H22" t="n">
-        <v>9120.0</v>
+        <v>9123.0</v>
       </c>
       <c r="I22" t="n">
-        <v>2931.0</v>
+        <v>2933.0</v>
       </c>
       <c r="J22" t="n">
         <v>444.0</v>
@@ -1952,7 +1952,7 @@
         <v>27.0</v>
       </c>
       <c r="S22" t="n">
-        <v>43197.0</v>
+        <v>44247.0</v>
       </c>
       <c r="T22" t="s">
         <v>130</v>
@@ -1961,7 +1961,7 @@
         <v>43151.0</v>
       </c>
       <c r="V22" t="n">
-        <v>265.0</v>
+        <v>266.0</v>
       </c>
     </row>
     <row r="23">
@@ -1975,19 +1975,19 @@
         <v>11.0</v>
       </c>
       <c r="D23" t="n">
-        <v>4047.0</v>
+        <v>4077.0</v>
       </c>
       <c r="E23" t="n">
         <v>4253.0</v>
       </c>
       <c r="F23" t="n">
-        <v>1342.0</v>
+        <v>1343.0</v>
       </c>
       <c r="G23" t="n">
         <v>1403.0</v>
       </c>
       <c r="H23" t="n">
-        <v>4593.0</v>
+        <v>4594.0</v>
       </c>
       <c r="I23" t="n">
         <v>878.0</v>
@@ -2029,7 +2029,7 @@
         <v>43254.0</v>
       </c>
       <c r="V23" t="n">
-        <v>162.0</v>
+        <v>163.0</v>
       </c>
     </row>
     <row r="24">
@@ -2097,7 +2097,7 @@
         <v>43380.0</v>
       </c>
       <c r="V24" t="n">
-        <v>36.0</v>
+        <v>37.0</v>
       </c>
     </row>
     <row r="25">
@@ -2123,10 +2123,10 @@
         <v>4360.0</v>
       </c>
       <c r="H25" t="n">
-        <v>18496.0</v>
+        <v>18507.0</v>
       </c>
       <c r="I25" t="n">
-        <v>2938.0</v>
+        <v>2940.0</v>
       </c>
       <c r="J25" t="n">
         <v>2740.0</v>
@@ -2138,19 +2138,19 @@
         <v>2641.0</v>
       </c>
       <c r="M25" t="n">
-        <v>15912.0</v>
+        <v>15946.0</v>
       </c>
       <c r="N25" t="s">
         <v>124</v>
       </c>
       <c r="O25" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="P25" t="n">
-        <v>80.0</v>
+        <v>160.0</v>
       </c>
       <c r="Q25" t="n">
-        <v>6378.0</v>
+        <v>6382.0</v>
       </c>
       <c r="R25" t="n">
         <v>79.0</v>
@@ -2165,7 +2165,7 @@
         <v>42614.0</v>
       </c>
       <c r="V25" t="n">
-        <v>802.0</v>
+        <v>803.0</v>
       </c>
     </row>
     <row r="26">
@@ -2233,7 +2233,7 @@
         <v>43400.0</v>
       </c>
       <c r="V26" t="n">
-        <v>16.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="27">
@@ -2247,19 +2247,19 @@
         <v>12.0</v>
       </c>
       <c r="D27" t="n">
-        <v>4124.0</v>
+        <v>4184.0</v>
       </c>
       <c r="E27" t="n">
         <v>4363.0</v>
       </c>
       <c r="F27" t="n">
-        <v>3323.0</v>
+        <v>3325.0</v>
       </c>
       <c r="G27" t="n">
         <v>3496.0</v>
       </c>
       <c r="H27" t="n">
-        <v>12246.0</v>
+        <v>12250.0</v>
       </c>
       <c r="I27" t="n">
         <v>1699.0</v>
@@ -2280,13 +2280,13 @@
         <v>122</v>
       </c>
       <c r="O27" t="n">
-        <v>48.0</v>
+        <v>104.0</v>
       </c>
       <c r="P27" t="n">
-        <v>40.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q27" t="n">
-        <v>42469.0</v>
+        <v>42525.0</v>
       </c>
       <c r="R27" t="n">
         <v>67.0</v>
@@ -2301,7 +2301,7 @@
         <v>43214.0</v>
       </c>
       <c r="V27" t="n">
-        <v>202.0</v>
+        <v>203.0</v>
       </c>
     </row>
     <row r="28">
@@ -2315,22 +2315,22 @@
         <v>12.0</v>
       </c>
       <c r="D28" t="n">
-        <v>4446.0</v>
+        <v>4427.0</v>
       </c>
       <c r="E28" t="n">
         <v>4653.0</v>
       </c>
       <c r="F28" t="n">
-        <v>3702.0</v>
+        <v>3704.0</v>
       </c>
       <c r="G28" t="n">
-        <v>3417.0</v>
+        <v>3420.0</v>
       </c>
       <c r="H28" t="n">
-        <v>11366.0</v>
+        <v>11372.0</v>
       </c>
       <c r="I28" t="n">
-        <v>1549.0</v>
+        <v>1550.0</v>
       </c>
       <c r="J28" t="n">
         <v>3040.0</v>
@@ -2348,13 +2348,13 @@
         <v>124</v>
       </c>
       <c r="O28" t="n">
-        <v>18.0</v>
+        <v>28.0</v>
       </c>
       <c r="P28" t="n">
         <v>0.0</v>
       </c>
       <c r="Q28" t="n">
-        <v>32627.0</v>
+        <v>32637.0</v>
       </c>
       <c r="R28" t="n">
         <v>62.0</v>
@@ -2369,7 +2369,7 @@
         <v>42614.0</v>
       </c>
       <c r="V28" t="n">
-        <v>802.0</v>
+        <v>803.0</v>
       </c>
     </row>
     <row r="29">
@@ -2437,7 +2437,7 @@
         <v>43254.0</v>
       </c>
       <c r="V29" t="n">
-        <v>162.0</v>
+        <v>163.0</v>
       </c>
     </row>
     <row r="30">
@@ -2463,10 +2463,10 @@
         <v>1122.0</v>
       </c>
       <c r="H30" t="n">
-        <v>6589.0</v>
+        <v>6597.0</v>
       </c>
       <c r="I30" t="n">
-        <v>1449.0</v>
+        <v>1450.0</v>
       </c>
       <c r="J30" t="n">
         <v>1859.0</v>
@@ -2484,13 +2484,13 @@
         <v>122</v>
       </c>
       <c r="O30" t="n">
-        <v>10.0</v>
+        <v>128.0</v>
       </c>
       <c r="P30" t="n">
-        <v>40.0</v>
+        <v>160.0</v>
       </c>
       <c r="Q30" t="n">
-        <v>12760.0</v>
+        <v>12878.0</v>
       </c>
       <c r="R30" t="n">
         <v>56.0</v>
@@ -2505,7 +2505,7 @@
         <v>43058.0</v>
       </c>
       <c r="V30" t="n">
-        <v>358.0</v>
+        <v>359.0</v>
       </c>
     </row>
     <row r="31">
@@ -2519,7 +2519,7 @@
         <v>10.0</v>
       </c>
       <c r="D31" t="n">
-        <v>3955.0</v>
+        <v>3928.0</v>
       </c>
       <c r="E31" t="n">
         <v>4006.0</v>
@@ -2528,13 +2528,13 @@
         <v>668.0</v>
       </c>
       <c r="G31" t="n">
-        <v>537.0</v>
+        <v>538.0</v>
       </c>
       <c r="H31" t="n">
-        <v>3372.0</v>
+        <v>3379.0</v>
       </c>
       <c r="I31" t="n">
-        <v>743.0</v>
+        <v>744.0</v>
       </c>
       <c r="J31" t="n">
         <v>838.0</v>
@@ -2555,7 +2555,7 @@
         <v>0.0</v>
       </c>
       <c r="P31" t="n">
-        <v>40.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q31" t="n">
         <v>4623.0</v>
@@ -2573,7 +2573,7 @@
         <v>43138.0</v>
       </c>
       <c r="V31" t="n">
-        <v>278.0</v>
+        <v>279.0</v>
       </c>
     </row>
     <row r="32">
@@ -2587,22 +2587,22 @@
         <v>12.0</v>
       </c>
       <c r="D32" t="n">
-        <v>4066.0</v>
+        <v>4074.0</v>
       </c>
       <c r="E32" t="n">
         <v>4140.0</v>
       </c>
       <c r="F32" t="n">
-        <v>2151.0</v>
+        <v>2153.0</v>
       </c>
       <c r="G32" t="n">
-        <v>2193.0</v>
+        <v>2195.0</v>
       </c>
       <c r="H32" t="n">
-        <v>6963.0</v>
+        <v>6970.0</v>
       </c>
       <c r="I32" t="n">
-        <v>1566.0</v>
+        <v>1568.0</v>
       </c>
       <c r="J32" t="n">
         <v>1474.0</v>
@@ -2620,13 +2620,13 @@
         <v>122</v>
       </c>
       <c r="O32" t="n">
-        <v>132.0</v>
+        <v>242.0</v>
       </c>
       <c r="P32" t="n">
-        <v>40.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q32" t="n">
-        <v>42715.0</v>
+        <v>42825.0</v>
       </c>
       <c r="R32" t="n">
         <v>37.0</v>
@@ -2641,7 +2641,7 @@
         <v>42920.0</v>
       </c>
       <c r="V32" t="n">
-        <v>496.0</v>
+        <v>497.0</v>
       </c>
     </row>
     <row r="33">
@@ -2655,22 +2655,22 @@
         <v>12.0</v>
       </c>
       <c r="D33" t="n">
-        <v>4553.0</v>
+        <v>4471.0</v>
       </c>
       <c r="E33" t="n">
         <v>4798.0</v>
       </c>
       <c r="F33" t="n">
-        <v>5146.0</v>
+        <v>5152.0</v>
       </c>
       <c r="G33" t="n">
-        <v>5247.0</v>
+        <v>5256.0</v>
       </c>
       <c r="H33" t="n">
-        <v>12325.0</v>
+        <v>12341.0</v>
       </c>
       <c r="I33" t="n">
-        <v>2246.0</v>
+        <v>2247.0</v>
       </c>
       <c r="J33" t="n">
         <v>1728.0</v>
@@ -2688,13 +2688,13 @@
         <v>122</v>
       </c>
       <c r="O33" t="n">
-        <v>64.0</v>
+        <v>90.0</v>
       </c>
       <c r="P33" t="n">
-        <v>0.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q33" t="n">
-        <v>59087.0</v>
+        <v>59113.0</v>
       </c>
       <c r="R33" t="n">
         <v>30.0</v>
@@ -2709,7 +2709,7 @@
         <v>43058.0</v>
       </c>
       <c r="V33" t="n">
-        <v>358.0</v>
+        <v>359.0</v>
       </c>
     </row>
     <row r="34">
@@ -2735,7 +2735,7 @@
         <v>221.0</v>
       </c>
       <c r="H34" t="n">
-        <v>1570.0</v>
+        <v>1574.0</v>
       </c>
       <c r="I34" t="n">
         <v>268.0</v>
@@ -2756,13 +2756,13 @@
         <v>123</v>
       </c>
       <c r="O34" t="n">
-        <v>0.0</v>
+        <v>111.0</v>
       </c>
       <c r="P34" t="n">
-        <v>0.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q34" t="n">
-        <v>4521.0</v>
+        <v>4632.0</v>
       </c>
       <c r="R34" t="n">
         <v>0.0</v>
@@ -2777,7 +2777,7 @@
         <v>43409.0</v>
       </c>
       <c r="V34" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="35">
@@ -2791,22 +2791,22 @@
         <v>10.0</v>
       </c>
       <c r="D35" t="n">
-        <v>4021.0</v>
+        <v>3994.0</v>
       </c>
       <c r="E35" t="n">
         <v>4021.0</v>
       </c>
       <c r="F35" t="n">
-        <v>954.0</v>
+        <v>955.0</v>
       </c>
       <c r="G35" t="n">
-        <v>968.0</v>
+        <v>970.0</v>
       </c>
       <c r="H35" t="n">
-        <v>4204.0</v>
+        <v>4216.0</v>
       </c>
       <c r="I35" t="n">
-        <v>991.0</v>
+        <v>993.0</v>
       </c>
       <c r="J35" t="n">
         <v>278.0</v>
@@ -2824,28 +2824,28 @@
         <v>123</v>
       </c>
       <c r="O35" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="P35" t="n">
-        <v>0.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q35" t="n">
-        <v>8401.0</v>
+        <v>8411.0</v>
       </c>
       <c r="R35" t="n">
         <v>28.0</v>
       </c>
       <c r="S35" t="n">
-        <v>62383.0</v>
+        <v>63503.0</v>
       </c>
       <c r="T35" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="U35" t="n" s="2">
         <v>43312.0</v>
       </c>
       <c r="V35" t="n">
-        <v>104.0</v>
+        <v>105.0</v>
       </c>
     </row>
     <row r="36">
@@ -2871,10 +2871,10 @@
         <v>495.0</v>
       </c>
       <c r="H36" t="n">
-        <v>3366.0</v>
+        <v>3375.0</v>
       </c>
       <c r="I36" t="n">
-        <v>696.0</v>
+        <v>698.0</v>
       </c>
       <c r="J36" t="n">
         <v>278.0</v>
@@ -2892,19 +2892,19 @@
         <v>123</v>
       </c>
       <c r="O36" t="n">
-        <v>26.0</v>
+        <v>168.0</v>
       </c>
       <c r="P36" t="n">
-        <v>32.0</v>
+        <v>152.0</v>
       </c>
       <c r="Q36" t="n">
-        <v>16999.0</v>
+        <v>17141.0</v>
       </c>
       <c r="R36" t="n">
         <v>26.0</v>
       </c>
       <c r="S36" t="n">
-        <v>60915.0</v>
+        <v>61964.0</v>
       </c>
       <c r="T36" t="s">
         <v>127</v>
@@ -2913,7 +2913,7 @@
         <v>43274.0</v>
       </c>
       <c r="V36" t="n">
-        <v>142.0</v>
+        <v>143.0</v>
       </c>
     </row>
     <row r="37">
@@ -2927,22 +2927,22 @@
         <v>10.0</v>
       </c>
       <c r="D37" t="n">
-        <v>3840.0</v>
+        <v>3890.0</v>
       </c>
       <c r="E37" t="n">
         <v>4078.0</v>
       </c>
       <c r="F37" t="n">
-        <v>3486.0</v>
+        <v>3493.0</v>
       </c>
       <c r="G37" t="n">
-        <v>4046.0</v>
+        <v>4052.0</v>
       </c>
       <c r="H37" t="n">
-        <v>9610.0</v>
+        <v>9625.0</v>
       </c>
       <c r="I37" t="n">
-        <v>1761.0</v>
+        <v>1762.0</v>
       </c>
       <c r="J37" t="n">
         <v>224.0</v>
@@ -2960,13 +2960,13 @@
         <v>122</v>
       </c>
       <c r="O37" t="n">
-        <v>92.0</v>
+        <v>112.0</v>
       </c>
       <c r="P37" t="n">
-        <v>40.0</v>
+        <v>100.0</v>
       </c>
       <c r="Q37" t="n">
-        <v>14565.0</v>
+        <v>14585.0</v>
       </c>
       <c r="R37" t="n">
         <v>35.0</v>
@@ -2981,7 +2981,7 @@
         <v>43280.0</v>
       </c>
       <c r="V37" t="n">
-        <v>136.0</v>
+        <v>137.0</v>
       </c>
     </row>
     <row r="38">
@@ -3028,13 +3028,13 @@
         <v>123</v>
       </c>
       <c r="O38" t="n">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
       <c r="P38" t="n">
-        <v>40.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q38" t="n">
-        <v>2629.0</v>
+        <v>2649.0</v>
       </c>
       <c r="R38" t="n">
         <v>2.0</v>
@@ -3049,7 +3049,7 @@
         <v>43360.0</v>
       </c>
       <c r="V38" t="n">
-        <v>56.0</v>
+        <v>57.0</v>
       </c>
     </row>
     <row r="39">
@@ -3075,10 +3075,10 @@
         <v>987.0</v>
       </c>
       <c r="H39" t="n">
-        <v>4442.0</v>
+        <v>4451.0</v>
       </c>
       <c r="I39" t="n">
-        <v>464.0</v>
+        <v>467.0</v>
       </c>
       <c r="J39" t="n">
         <v>2215.0</v>
@@ -3096,13 +3096,13 @@
         <v>122</v>
       </c>
       <c r="O39" t="n">
-        <v>116.0</v>
+        <v>200.0</v>
       </c>
       <c r="P39" t="n">
-        <v>110.0</v>
+        <v>210.0</v>
       </c>
       <c r="Q39" t="n">
-        <v>25694.0</v>
+        <v>25778.0</v>
       </c>
       <c r="R39" t="n">
         <v>39.0</v>
@@ -3117,7 +3117,7 @@
         <v>43284.0</v>
       </c>
       <c r="V39" t="n">
-        <v>132.0</v>
+        <v>133.0</v>
       </c>
     </row>
     <row r="40">
@@ -3164,13 +3164,13 @@
         <v>123</v>
       </c>
       <c r="O40" t="n">
-        <v>105.0</v>
+        <v>123.0</v>
       </c>
       <c r="P40" t="n">
-        <v>80.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q40" t="n">
-        <v>20067.0</v>
+        <v>20085.0</v>
       </c>
       <c r="R40" t="n">
         <v>16.0</v>
@@ -3185,7 +3185,7 @@
         <v>43352.0</v>
       </c>
       <c r="V40" t="n">
-        <v>64.0</v>
+        <v>65.0</v>
       </c>
     </row>
     <row r="41">
@@ -3211,7 +3211,7 @@
         <v>4695.0</v>
       </c>
       <c r="H41" t="n">
-        <v>26774.0</v>
+        <v>26782.0</v>
       </c>
       <c r="I41" t="n">
         <v>3653.0</v>
@@ -3253,7 +3253,7 @@
         <v>43252.0</v>
       </c>
       <c r="V41" t="n">
-        <v>164.0</v>
+        <v>165.0</v>
       </c>
     </row>
     <row r="42">
@@ -3267,22 +3267,22 @@
         <v>11.0</v>
       </c>
       <c r="D42" t="n">
-        <v>4001.0</v>
+        <v>4043.0</v>
       </c>
       <c r="E42" t="n">
         <v>4323.0</v>
       </c>
       <c r="F42" t="n">
-        <v>2394.0</v>
+        <v>2399.0</v>
       </c>
       <c r="G42" t="n">
-        <v>2316.0</v>
+        <v>2320.0</v>
       </c>
       <c r="H42" t="n">
-        <v>6022.0</v>
+        <v>6033.0</v>
       </c>
       <c r="I42" t="n">
-        <v>1180.0</v>
+        <v>1182.0</v>
       </c>
       <c r="J42" t="n">
         <v>2792.0</v>
@@ -3300,13 +3300,13 @@
         <v>123</v>
       </c>
       <c r="O42" t="n">
-        <v>38.0</v>
+        <v>96.0</v>
       </c>
       <c r="P42" t="n">
-        <v>80.0</v>
+        <v>160.0</v>
       </c>
       <c r="Q42" t="n">
-        <v>21598.0</v>
+        <v>21656.0</v>
       </c>
       <c r="R42" t="n">
         <v>19.0</v>
@@ -3321,7 +3321,7 @@
         <v>43370.0</v>
       </c>
       <c r="V42" t="n">
-        <v>46.0</v>
+        <v>47.0</v>
       </c>
     </row>
     <row r="43">
@@ -3335,19 +3335,19 @@
         <v>12.0</v>
       </c>
       <c r="D43" t="n">
-        <v>4246.0</v>
+        <v>4275.0</v>
       </c>
       <c r="E43" t="n">
-        <v>4272.0</v>
+        <v>4275.0</v>
       </c>
       <c r="F43" t="n">
-        <v>2749.0</v>
+        <v>2750.0</v>
       </c>
       <c r="G43" t="n">
         <v>2660.0</v>
       </c>
       <c r="H43" t="n">
-        <v>7799.0</v>
+        <v>7801.0</v>
       </c>
       <c r="I43" t="n">
         <v>2271.0</v>
@@ -3368,13 +3368,13 @@
         <v>123</v>
       </c>
       <c r="O43" t="n">
-        <v>72.0</v>
+        <v>82.0</v>
       </c>
       <c r="P43" t="n">
-        <v>40.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q43" t="n">
-        <v>31729.0</v>
+        <v>31739.0</v>
       </c>
       <c r="R43" t="n">
         <v>24.0</v>
@@ -3389,7 +3389,7 @@
         <v>43382.0</v>
       </c>
       <c r="V43" t="n">
-        <v>34.0</v>
+        <v>35.0</v>
       </c>
     </row>
     <row r="44">
@@ -3403,7 +3403,7 @@
         <v>11.0</v>
       </c>
       <c r="D44" t="n">
-        <v>4376.0</v>
+        <v>4293.0</v>
       </c>
       <c r="E44" t="n">
         <v>4400.0</v>
@@ -3412,13 +3412,13 @@
         <v>3816.0</v>
       </c>
       <c r="G44" t="n">
-        <v>4116.0</v>
+        <v>4119.0</v>
       </c>
       <c r="H44" t="n">
-        <v>8661.0</v>
+        <v>8665.0</v>
       </c>
       <c r="I44" t="n">
-        <v>2033.0</v>
+        <v>2034.0</v>
       </c>
       <c r="J44" t="n">
         <v>1339.0</v>
@@ -3436,13 +3436,13 @@
         <v>123</v>
       </c>
       <c r="O44" t="n">
-        <v>10.0</v>
+        <v>68.0</v>
       </c>
       <c r="P44" t="n">
-        <v>40.0</v>
+        <v>100.0</v>
       </c>
       <c r="Q44" t="n">
-        <v>21859.0</v>
+        <v>21917.0</v>
       </c>
       <c r="R44" t="n">
         <v>19.0</v>
@@ -3451,13 +3451,13 @@
         <v>73412.0</v>
       </c>
       <c r="T44" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="U44" t="n" s="2">
         <v>43390.0</v>
       </c>
       <c r="V44" t="n">
-        <v>26.0</v>
+        <v>27.0</v>
       </c>
     </row>
     <row r="45">
@@ -3483,7 +3483,7 @@
         <v>2577.0</v>
       </c>
       <c r="H45" t="n">
-        <v>7194.0</v>
+        <v>7195.0</v>
       </c>
       <c r="I45" t="n">
         <v>1377.0</v>
@@ -3504,19 +3504,19 @@
         <v>123</v>
       </c>
       <c r="O45" t="n">
-        <v>56.0</v>
+        <v>82.0</v>
       </c>
       <c r="P45" t="n">
-        <v>30.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q45" t="n">
-        <v>49158.0</v>
+        <v>49184.0</v>
       </c>
       <c r="R45" t="n">
         <v>32.0</v>
       </c>
       <c r="S45" t="n">
-        <v>40845.0</v>
+        <v>41125.0</v>
       </c>
       <c r="T45" t="s">
         <v>128</v>
@@ -3525,7 +3525,7 @@
         <v>43390.0</v>
       </c>
       <c r="V45" t="n">
-        <v>26.0</v>
+        <v>27.0</v>
       </c>
     </row>
     <row r="46">
@@ -3539,22 +3539,22 @@
         <v>8.0</v>
       </c>
       <c r="D46" t="n">
-        <v>2387.0</v>
+        <v>2377.0</v>
       </c>
       <c r="E46" t="n">
-        <v>2387.0</v>
+        <v>2422.0</v>
       </c>
       <c r="F46" t="n">
-        <v>185.0</v>
+        <v>187.0</v>
       </c>
       <c r="G46" t="n">
-        <v>88.0</v>
+        <v>91.0</v>
       </c>
       <c r="H46" t="n">
-        <v>325.0</v>
+        <v>331.0</v>
       </c>
       <c r="I46" t="n">
-        <v>79.0</v>
+        <v>80.0</v>
       </c>
       <c r="J46" t="n">
         <v>0.0</v>
@@ -3572,13 +3572,13 @@
         <v>123</v>
       </c>
       <c r="O46" t="n">
-        <v>6.0</v>
+        <v>86.0</v>
       </c>
       <c r="P46" t="n">
-        <v>30.0</v>
+        <v>90.0</v>
       </c>
       <c r="Q46" t="n">
-        <v>1134.0</v>
+        <v>1214.0</v>
       </c>
       <c r="R46" t="n">
         <v>0.0</v>
@@ -3593,7 +3593,7 @@
         <v>43376.0</v>
       </c>
       <c r="V46" t="n">
-        <v>40.0</v>
+        <v>41.0</v>
       </c>
     </row>
     <row r="47">
@@ -3607,22 +3607,22 @@
         <v>12.0</v>
       </c>
       <c r="D47" t="n">
-        <v>4685.0</v>
+        <v>4622.0</v>
       </c>
       <c r="E47" t="n">
         <v>4919.0</v>
       </c>
       <c r="F47" t="n">
-        <v>10951.0</v>
+        <v>10974.0</v>
       </c>
       <c r="G47" t="n">
-        <v>11640.0</v>
+        <v>11666.0</v>
       </c>
       <c r="H47" t="n">
-        <v>26060.0</v>
+        <v>26110.0</v>
       </c>
       <c r="I47" t="n">
-        <v>8989.0</v>
+        <v>9008.0</v>
       </c>
       <c r="J47" t="n">
         <v>2205.0</v>
@@ -3634,25 +3634,25 @@
         <v>0.0</v>
       </c>
       <c r="M47" t="n">
-        <v>4.0</v>
+        <v>8.0</v>
       </c>
       <c r="N47" t="s">
         <v>123</v>
       </c>
       <c r="O47" t="n">
-        <v>86.0</v>
+        <v>291.0</v>
       </c>
       <c r="P47" t="n">
-        <v>80.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q47" t="n">
-        <v>75484.0</v>
+        <v>75689.0</v>
       </c>
       <c r="R47" t="n">
         <v>23.0</v>
       </c>
       <c r="S47" t="n">
-        <v>82910.0</v>
+        <v>83190.0</v>
       </c>
       <c r="T47" t="s">
         <v>133</v>
@@ -3661,7 +3661,7 @@
         <v>43390.0</v>
       </c>
       <c r="V47" t="n">
-        <v>26.0</v>
+        <v>27.0</v>
       </c>
     </row>
     <row r="48">
@@ -3687,7 +3687,7 @@
         <v>3037.0</v>
       </c>
       <c r="H48" t="n">
-        <v>15553.0</v>
+        <v>15573.0</v>
       </c>
       <c r="I48" t="n">
         <v>3281.0</v>
@@ -3708,13 +3708,13 @@
         <v>122</v>
       </c>
       <c r="O48" t="n">
-        <v>44.0</v>
+        <v>98.0</v>
       </c>
       <c r="P48" t="n">
-        <v>40.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q48" t="n">
-        <v>33165.0</v>
+        <v>33219.0</v>
       </c>
       <c r="R48" t="n">
         <v>38.0</v>
@@ -3729,7 +3729,7 @@
         <v>43230.0</v>
       </c>
       <c r="V48" t="n">
-        <v>186.0</v>
+        <v>187.0</v>
       </c>
     </row>
     <row r="49">
@@ -3743,22 +3743,22 @@
         <v>11.0</v>
       </c>
       <c r="D49" t="n">
-        <v>4174.0</v>
+        <v>4207.0</v>
       </c>
       <c r="E49" t="n">
         <v>4325.0</v>
       </c>
       <c r="F49" t="n">
-        <v>6376.0</v>
+        <v>6382.0</v>
       </c>
       <c r="G49" t="n">
-        <v>6609.0</v>
+        <v>6612.0</v>
       </c>
       <c r="H49" t="n">
-        <v>18239.0</v>
+        <v>18253.0</v>
       </c>
       <c r="I49" t="n">
-        <v>3769.0</v>
+        <v>3772.0</v>
       </c>
       <c r="J49" t="n">
         <v>4372.0</v>
@@ -3776,13 +3776,13 @@
         <v>124</v>
       </c>
       <c r="O49" t="n">
-        <v>2.0</v>
+        <v>29.0</v>
       </c>
       <c r="P49" t="n">
-        <v>0.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q49" t="n">
-        <v>20714.0</v>
+        <v>20741.0</v>
       </c>
       <c r="R49" t="n">
         <v>59.0</v>
@@ -3797,7 +3797,7 @@
         <v>43184.0</v>
       </c>
       <c r="V49" t="n">
-        <v>232.0</v>
+        <v>233.0</v>
       </c>
     </row>
     <row r="50">
@@ -3811,19 +3811,19 @@
         <v>12.0</v>
       </c>
       <c r="D50" t="n">
-        <v>4173.0</v>
+        <v>4203.0</v>
       </c>
       <c r="E50" t="n">
         <v>4619.0</v>
       </c>
       <c r="F50" t="n">
-        <v>6372.0</v>
+        <v>6373.0</v>
       </c>
       <c r="G50" t="n">
         <v>6150.0</v>
       </c>
       <c r="H50" t="n">
-        <v>14044.0</v>
+        <v>14046.0</v>
       </c>
       <c r="I50" t="n">
         <v>2660.0</v>
@@ -3856,7 +3856,7 @@
         <v>29.0</v>
       </c>
       <c r="S50" t="n">
-        <v>42600.0</v>
+        <v>43160.0</v>
       </c>
       <c r="T50" t="s">
         <v>128</v>
@@ -3865,7 +3865,7 @@
         <v>43314.0</v>
       </c>
       <c r="V50" t="n">
-        <v>102.0</v>
+        <v>103.0</v>
       </c>
     </row>
     <row r="51">
@@ -3933,7 +3933,7 @@
         <v>43254.0</v>
       </c>
       <c r="V51" t="n">
-        <v>162.0</v>
+        <v>163.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug corrected: duplicate names in war map
</commit_message>
<xml_diff>
--- a/docs/data/memberstats.xlsx
+++ b/docs/data/memberstats.xlsx
@@ -404,10 +404,10 @@
     <t>Arena 11</t>
   </si>
   <si>
+    <t>Arena 9</t>
+  </si>
+  <si>
     <t>League 3</t>
-  </si>
-  <si>
-    <t>Arena 9</t>
   </si>
   <si>
     <t>Arena 10</t>
@@ -544,19 +544,19 @@
         <v>11.0</v>
       </c>
       <c r="D2" t="n">
-        <v>4401.0</v>
+        <v>4379.0</v>
       </c>
       <c r="E2" t="n">
         <v>4653.0</v>
       </c>
       <c r="F2" t="n">
-        <v>2274.0</v>
+        <v>2275.0</v>
       </c>
       <c r="G2" t="n">
-        <v>2101.0</v>
+        <v>2103.0</v>
       </c>
       <c r="H2" t="n">
-        <v>7071.0</v>
+        <v>7078.0</v>
       </c>
       <c r="I2" t="n">
         <v>1156.0</v>
@@ -577,19 +577,19 @@
         <v>122</v>
       </c>
       <c r="O2" t="n">
-        <v>447.0</v>
+        <v>537.0</v>
       </c>
       <c r="P2" t="n">
-        <v>280.0</v>
+        <v>360.0</v>
       </c>
       <c r="Q2" t="n">
-        <v>28673.0</v>
+        <v>28763.0</v>
       </c>
       <c r="R2" t="n">
         <v>45.0</v>
       </c>
       <c r="S2" t="n">
-        <v>85100.0</v>
+        <v>85940.0</v>
       </c>
       <c r="T2" t="s">
         <v>126</v>
@@ -598,7 +598,7 @@
         <v>43302.0</v>
       </c>
       <c r="V2" t="n">
-        <v>117.0</v>
+        <v>118.0</v>
       </c>
     </row>
     <row r="3">
@@ -666,7 +666,7 @@
         <v>43372.0</v>
       </c>
       <c r="V3" t="n">
-        <v>47.0</v>
+        <v>48.0</v>
       </c>
     </row>
     <row r="4">
@@ -680,22 +680,22 @@
         <v>11.0</v>
       </c>
       <c r="D4" t="n">
-        <v>4132.0</v>
+        <v>4134.0</v>
       </c>
       <c r="E4" t="n">
         <v>4292.0</v>
       </c>
       <c r="F4" t="n">
-        <v>2622.0</v>
+        <v>2623.0</v>
       </c>
       <c r="G4" t="n">
-        <v>2650.0</v>
+        <v>2651.0</v>
       </c>
       <c r="H4" t="n">
-        <v>6272.0</v>
+        <v>6274.0</v>
       </c>
       <c r="I4" t="n">
-        <v>1072.0</v>
+        <v>1073.0</v>
       </c>
       <c r="J4" t="n">
         <v>1649.0</v>
@@ -713,13 +713,13 @@
         <v>122</v>
       </c>
       <c r="O4" t="n">
-        <v>80.0</v>
+        <v>88.0</v>
       </c>
       <c r="P4" t="n">
-        <v>360.0</v>
+        <v>440.0</v>
       </c>
       <c r="Q4" t="n">
-        <v>9098.0</v>
+        <v>9106.0</v>
       </c>
       <c r="R4" t="n">
         <v>46.0</v>
@@ -734,7 +734,7 @@
         <v>43082.0</v>
       </c>
       <c r="V4" t="n">
-        <v>337.0</v>
+        <v>338.0</v>
       </c>
     </row>
     <row r="5">
@@ -784,13 +784,13 @@
         <v>62.0</v>
       </c>
       <c r="P5" t="n">
-        <v>218.0</v>
+        <v>272.0</v>
       </c>
       <c r="Q5" t="n">
         <v>16997.0</v>
       </c>
       <c r="R5" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="S5" t="n">
         <v>10885.0</v>
@@ -802,7 +802,7 @@
         <v>43397.0</v>
       </c>
       <c r="V5" t="n">
-        <v>22.0</v>
+        <v>23.0</v>
       </c>
     </row>
     <row r="6">
@@ -816,19 +816,19 @@
         <v>10.0</v>
       </c>
       <c r="D6" t="n">
-        <v>4027.0</v>
+        <v>4099.0</v>
       </c>
       <c r="E6" t="n">
         <v>4142.0</v>
       </c>
       <c r="F6" t="n">
-        <v>1249.0</v>
+        <v>1255.0</v>
       </c>
       <c r="G6" t="n">
-        <v>1281.0</v>
+        <v>1285.0</v>
       </c>
       <c r="H6" t="n">
-        <v>3239.0</v>
+        <v>3252.0</v>
       </c>
       <c r="I6" t="n">
         <v>502.0</v>
@@ -849,19 +849,19 @@
         <v>123</v>
       </c>
       <c r="O6" t="n">
-        <v>400.0</v>
+        <v>516.0</v>
       </c>
       <c r="P6" t="n">
-        <v>400.0</v>
+        <v>520.0</v>
       </c>
       <c r="Q6" t="n">
-        <v>16537.0</v>
+        <v>16653.0</v>
       </c>
       <c r="R6" t="n">
         <v>29.0</v>
       </c>
       <c r="S6" t="n">
-        <v>41906.0</v>
+        <v>43026.0</v>
       </c>
       <c r="T6" t="s">
         <v>128</v>
@@ -870,7 +870,7 @@
         <v>43356.0</v>
       </c>
       <c r="V6" t="n">
-        <v>63.0</v>
+        <v>64.0</v>
       </c>
     </row>
     <row r="7">
@@ -890,19 +890,19 @@
         <v>4489.0</v>
       </c>
       <c r="F7" t="n">
-        <v>2979.0</v>
+        <v>2982.0</v>
       </c>
       <c r="G7" t="n">
-        <v>2664.0</v>
+        <v>2667.0</v>
       </c>
       <c r="H7" t="n">
-        <v>7044.0</v>
+        <v>7051.0</v>
       </c>
       <c r="I7" t="n">
-        <v>689.0</v>
+        <v>690.0</v>
       </c>
       <c r="J7" t="n">
-        <v>4159.0</v>
+        <v>4167.0</v>
       </c>
       <c r="K7" t="n">
         <v>10.0</v>
@@ -911,7 +911,7 @@
         <v>52.0</v>
       </c>
       <c r="M7" t="n">
-        <v>166.0</v>
+        <v>167.0</v>
       </c>
       <c r="N7" t="s">
         <v>122</v>
@@ -920,13 +920,13 @@
         <v>0.0</v>
       </c>
       <c r="P7" t="n">
-        <v>120.0</v>
+        <v>160.0</v>
       </c>
       <c r="Q7" t="n">
         <v>2125.0</v>
       </c>
       <c r="R7" t="n">
-        <v>41.0</v>
+        <v>42.0</v>
       </c>
       <c r="S7" t="n">
         <v>58760.0</v>
@@ -938,7 +938,7 @@
         <v>43364.0</v>
       </c>
       <c r="V7" t="n">
-        <v>55.0</v>
+        <v>56.0</v>
       </c>
     </row>
     <row r="8">
@@ -952,19 +952,19 @@
         <v>11.0</v>
       </c>
       <c r="D8" t="n">
-        <v>4332.0</v>
+        <v>4362.0</v>
       </c>
       <c r="E8" t="n">
         <v>4497.0</v>
       </c>
       <c r="F8" t="n">
-        <v>1920.0</v>
+        <v>1921.0</v>
       </c>
       <c r="G8" t="n">
         <v>1812.0</v>
       </c>
       <c r="H8" t="n">
-        <v>7642.0</v>
+        <v>7644.0</v>
       </c>
       <c r="I8" t="n">
         <v>1121.0</v>
@@ -988,7 +988,7 @@
         <v>142.0</v>
       </c>
       <c r="P8" t="n">
-        <v>240.0</v>
+        <v>280.0</v>
       </c>
       <c r="Q8" t="n">
         <v>25318.0</v>
@@ -997,7 +997,7 @@
         <v>57.0</v>
       </c>
       <c r="S8" t="n">
-        <v>71515.0</v>
+        <v>71795.0</v>
       </c>
       <c r="T8" t="s">
         <v>126</v>
@@ -1006,7 +1006,7 @@
         <v>43058.0</v>
       </c>
       <c r="V8" t="n">
-        <v>361.0</v>
+        <v>362.0</v>
       </c>
     </row>
     <row r="9">
@@ -1074,7 +1074,7 @@
         <v>43123.0</v>
       </c>
       <c r="V9" t="n">
-        <v>296.0</v>
+        <v>297.0</v>
       </c>
     </row>
     <row r="10">
@@ -1088,25 +1088,25 @@
         <v>11.0</v>
       </c>
       <c r="D10" t="n">
-        <v>4319.0</v>
+        <v>4334.0</v>
       </c>
       <c r="E10" t="n">
         <v>4509.0</v>
       </c>
       <c r="F10" t="n">
-        <v>2456.0</v>
+        <v>2468.0</v>
       </c>
       <c r="G10" t="n">
-        <v>2282.0</v>
+        <v>2296.0</v>
       </c>
       <c r="H10" t="n">
-        <v>10791.0</v>
+        <v>10830.0</v>
       </c>
       <c r="I10" t="n">
-        <v>2389.0</v>
+        <v>2392.0</v>
       </c>
       <c r="J10" t="n">
-        <v>1906.0</v>
+        <v>1922.0</v>
       </c>
       <c r="K10" t="n">
         <v>11.0</v>
@@ -1124,7 +1124,7 @@
         <v>58.0</v>
       </c>
       <c r="P10" t="n">
-        <v>440.0</v>
+        <v>520.0</v>
       </c>
       <c r="Q10" t="n">
         <v>3316.0</v>
@@ -1133,7 +1133,7 @@
         <v>58.0</v>
       </c>
       <c r="S10" t="n">
-        <v>81590.0</v>
+        <v>82710.0</v>
       </c>
       <c r="T10" t="s">
         <v>126</v>
@@ -1142,7 +1142,7 @@
         <v>43123.0</v>
       </c>
       <c r="V10" t="n">
-        <v>296.0</v>
+        <v>297.0</v>
       </c>
     </row>
     <row r="11">
@@ -1168,10 +1168,10 @@
         <v>1753.0</v>
       </c>
       <c r="H11" t="n">
-        <v>9509.0</v>
+        <v>9520.0</v>
       </c>
       <c r="I11" t="n">
-        <v>1370.0</v>
+        <v>1371.0</v>
       </c>
       <c r="J11" t="n">
         <v>4199.0</v>
@@ -1189,19 +1189,19 @@
         <v>123</v>
       </c>
       <c r="O11" t="n">
-        <v>820.0</v>
+        <v>960.0</v>
       </c>
       <c r="P11" t="n">
-        <v>430.0</v>
+        <v>520.0</v>
       </c>
       <c r="Q11" t="n">
-        <v>90609.0</v>
+        <v>90749.0</v>
       </c>
       <c r="R11" t="n">
-        <v>76.0</v>
+        <v>77.0</v>
       </c>
       <c r="S11" t="n">
-        <v>77080.0</v>
+        <v>78480.0</v>
       </c>
       <c r="T11" t="s">
         <v>126</v>
@@ -1210,7 +1210,7 @@
         <v>43397.0</v>
       </c>
       <c r="V11" t="n">
-        <v>22.0</v>
+        <v>23.0</v>
       </c>
     </row>
     <row r="12">
@@ -1230,13 +1230,13 @@
         <v>4389.0</v>
       </c>
       <c r="F12" t="n">
-        <v>1375.0</v>
+        <v>1376.0</v>
       </c>
       <c r="G12" t="n">
-        <v>1218.0</v>
+        <v>1219.0</v>
       </c>
       <c r="H12" t="n">
-        <v>5567.0</v>
+        <v>5575.0</v>
       </c>
       <c r="I12" t="n">
         <v>770.0</v>
@@ -1257,19 +1257,19 @@
         <v>124</v>
       </c>
       <c r="O12" t="n">
-        <v>314.0</v>
+        <v>403.0</v>
       </c>
       <c r="P12" t="n">
-        <v>360.0</v>
+        <v>440.0</v>
       </c>
       <c r="Q12" t="n">
-        <v>38290.0</v>
+        <v>38379.0</v>
       </c>
       <c r="R12" t="n">
-        <v>63.0</v>
+        <v>64.0</v>
       </c>
       <c r="S12" t="n">
-        <v>75840.0</v>
+        <v>76960.0</v>
       </c>
       <c r="T12" t="s">
         <v>128</v>
@@ -1278,7 +1278,7 @@
         <v>43218.0</v>
       </c>
       <c r="V12" t="n">
-        <v>201.0</v>
+        <v>202.0</v>
       </c>
     </row>
     <row r="13">
@@ -1292,22 +1292,22 @@
         <v>12.0</v>
       </c>
       <c r="D13" t="n">
-        <v>4343.0</v>
+        <v>4331.0</v>
       </c>
       <c r="E13" t="n">
         <v>4521.0</v>
       </c>
       <c r="F13" t="n">
-        <v>4668.0</v>
+        <v>4674.0</v>
       </c>
       <c r="G13" t="n">
-        <v>5062.0</v>
+        <v>5069.0</v>
       </c>
       <c r="H13" t="n">
-        <v>10791.0</v>
+        <v>10807.0</v>
       </c>
       <c r="I13" t="n">
-        <v>2087.0</v>
+        <v>2090.0</v>
       </c>
       <c r="J13" t="n">
         <v>1842.0</v>
@@ -1325,19 +1325,19 @@
         <v>123</v>
       </c>
       <c r="O13" t="n">
-        <v>588.0</v>
+        <v>830.0</v>
       </c>
       <c r="P13" t="n">
-        <v>280.0</v>
+        <v>360.0</v>
       </c>
       <c r="Q13" t="n">
-        <v>53965.0</v>
+        <v>54207.0</v>
       </c>
       <c r="R13" t="n">
         <v>31.0</v>
       </c>
       <c r="S13" t="n">
-        <v>82530.0</v>
+        <v>83650.0</v>
       </c>
       <c r="T13" t="s">
         <v>126</v>
@@ -1346,7 +1346,7 @@
         <v>43390.0</v>
       </c>
       <c r="V13" t="n">
-        <v>29.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="14">
@@ -1372,7 +1372,7 @@
         <v>1706.0</v>
       </c>
       <c r="H14" t="n">
-        <v>6602.0</v>
+        <v>6603.0</v>
       </c>
       <c r="I14" t="n">
         <v>1405.0</v>
@@ -1402,10 +1402,10 @@
         <v>44038.0</v>
       </c>
       <c r="R14" t="n">
-        <v>32.0</v>
+        <v>33.0</v>
       </c>
       <c r="S14" t="n">
-        <v>54809.0</v>
+        <v>55089.0</v>
       </c>
       <c r="T14" t="s">
         <v>128</v>
@@ -1414,7 +1414,7 @@
         <v>43410.0</v>
       </c>
       <c r="V14" t="n">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="15">
@@ -1428,22 +1428,22 @@
         <v>11.0</v>
       </c>
       <c r="D15" t="n">
-        <v>4289.0</v>
+        <v>4262.0</v>
       </c>
       <c r="E15" t="n">
         <v>4416.0</v>
       </c>
       <c r="F15" t="n">
-        <v>2284.0</v>
+        <v>2287.0</v>
       </c>
       <c r="G15" t="n">
-        <v>2083.0</v>
+        <v>2086.0</v>
       </c>
       <c r="H15" t="n">
-        <v>6722.0</v>
+        <v>6733.0</v>
       </c>
       <c r="I15" t="n">
-        <v>1084.0</v>
+        <v>1085.0</v>
       </c>
       <c r="J15" t="n">
         <v>3630.0</v>
@@ -1461,13 +1461,13 @@
         <v>122</v>
       </c>
       <c r="O15" t="n">
-        <v>60.0</v>
+        <v>70.0</v>
       </c>
       <c r="P15" t="n">
-        <v>160.0</v>
+        <v>240.0</v>
       </c>
       <c r="Q15" t="n">
-        <v>20611.0</v>
+        <v>20621.0</v>
       </c>
       <c r="R15" t="n">
         <v>43.0</v>
@@ -1482,7 +1482,7 @@
         <v>43275.0</v>
       </c>
       <c r="V15" t="n">
-        <v>144.0</v>
+        <v>145.0</v>
       </c>
     </row>
     <row r="16">
@@ -1508,10 +1508,10 @@
         <v>1460.0</v>
       </c>
       <c r="H16" t="n">
-        <v>3642.0</v>
+        <v>3645.0</v>
       </c>
       <c r="I16" t="n">
-        <v>1004.0</v>
+        <v>1005.0</v>
       </c>
       <c r="J16" t="n">
         <v>2611.0</v>
@@ -1529,19 +1529,19 @@
         <v>122</v>
       </c>
       <c r="O16" t="n">
-        <v>198.0</v>
+        <v>246.0</v>
       </c>
       <c r="P16" t="n">
-        <v>240.0</v>
+        <v>320.0</v>
       </c>
       <c r="Q16" t="n">
-        <v>30959.0</v>
+        <v>31007.0</v>
       </c>
       <c r="R16" t="n">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
       <c r="S16" t="n">
-        <v>27997.0</v>
+        <v>29309.0</v>
       </c>
       <c r="T16" t="s">
         <v>127</v>
@@ -1550,7 +1550,7 @@
         <v>43220.0</v>
       </c>
       <c r="V16" t="n">
-        <v>199.0</v>
+        <v>200.0</v>
       </c>
     </row>
     <row r="17">
@@ -1600,7 +1600,7 @@
         <v>48.0</v>
       </c>
       <c r="P17" t="n">
-        <v>64.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q17" t="n">
         <v>27465.0</v>
@@ -1618,7 +1618,7 @@
         <v>43419.0</v>
       </c>
       <c r="V17" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="18">
@@ -1632,25 +1632,25 @@
         <v>11.0</v>
       </c>
       <c r="D18" t="n">
-        <v>4308.0</v>
+        <v>4346.0</v>
       </c>
       <c r="E18" t="n">
         <v>4577.0</v>
       </c>
       <c r="F18" t="n">
-        <v>2802.0</v>
+        <v>2807.0</v>
       </c>
       <c r="G18" t="n">
-        <v>2554.0</v>
+        <v>2561.0</v>
       </c>
       <c r="H18" t="n">
-        <v>6636.0</v>
+        <v>6654.0</v>
       </c>
       <c r="I18" t="n">
-        <v>721.0</v>
+        <v>722.0</v>
       </c>
       <c r="J18" t="n">
-        <v>3595.0</v>
+        <v>3598.0</v>
       </c>
       <c r="K18" t="n">
         <v>10.0</v>
@@ -1665,19 +1665,19 @@
         <v>122</v>
       </c>
       <c r="O18" t="n">
-        <v>64.0</v>
+        <v>76.0</v>
       </c>
       <c r="P18" t="n">
-        <v>240.0</v>
+        <v>320.0</v>
       </c>
       <c r="Q18" t="n">
-        <v>21867.0</v>
+        <v>21879.0</v>
       </c>
       <c r="R18" t="n">
-        <v>49.0</v>
+        <v>50.0</v>
       </c>
       <c r="S18" t="n">
-        <v>80105.0</v>
+        <v>80945.0</v>
       </c>
       <c r="T18" t="s">
         <v>126</v>
@@ -1686,7 +1686,7 @@
         <v>43058.0</v>
       </c>
       <c r="V18" t="n">
-        <v>361.0</v>
+        <v>362.0</v>
       </c>
     </row>
     <row r="19">
@@ -1700,25 +1700,25 @@
         <v>12.0</v>
       </c>
       <c r="D19" t="n">
-        <v>4288.0</v>
+        <v>4233.0</v>
       </c>
       <c r="E19" t="n">
         <v>4512.0</v>
       </c>
       <c r="F19" t="n">
-        <v>3004.0</v>
+        <v>3007.0</v>
       </c>
       <c r="G19" t="n">
-        <v>2886.0</v>
+        <v>2891.0</v>
       </c>
       <c r="H19" t="n">
-        <v>6831.0</v>
+        <v>6847.0</v>
       </c>
       <c r="I19" t="n">
-        <v>1246.0</v>
+        <v>1248.0</v>
       </c>
       <c r="J19" t="n">
-        <v>2092.0</v>
+        <v>2104.0</v>
       </c>
       <c r="K19" t="n">
         <v>11.0</v>
@@ -1733,19 +1733,19 @@
         <v>122</v>
       </c>
       <c r="O19" t="n">
-        <v>582.0</v>
+        <v>676.0</v>
       </c>
       <c r="P19" t="n">
-        <v>400.0</v>
+        <v>440.0</v>
       </c>
       <c r="Q19" t="n">
-        <v>46086.0</v>
+        <v>46180.0</v>
       </c>
       <c r="R19" t="n">
         <v>35.0</v>
       </c>
       <c r="S19" t="n">
-        <v>50875.0</v>
+        <v>51995.0</v>
       </c>
       <c r="T19" t="s">
         <v>128</v>
@@ -1754,7 +1754,7 @@
         <v>43312.0</v>
       </c>
       <c r="V19" t="n">
-        <v>107.0</v>
+        <v>108.0</v>
       </c>
     </row>
     <row r="20">
@@ -1768,22 +1768,22 @@
         <v>12.0</v>
       </c>
       <c r="D20" t="n">
-        <v>4600.0</v>
+        <v>4596.0</v>
       </c>
       <c r="E20" t="n">
         <v>4767.0</v>
       </c>
       <c r="F20" t="n">
-        <v>6740.0</v>
+        <v>6743.0</v>
       </c>
       <c r="G20" t="n">
-        <v>6674.0</v>
+        <v>6677.0</v>
       </c>
       <c r="H20" t="n">
-        <v>23808.0</v>
+        <v>23822.0</v>
       </c>
       <c r="I20" t="n">
-        <v>2788.0</v>
+        <v>2790.0</v>
       </c>
       <c r="J20" t="n">
         <v>2570.0</v>
@@ -1795,34 +1795,34 @@
         <v>433.0</v>
       </c>
       <c r="M20" t="n">
-        <v>2570.0</v>
+        <v>2585.0</v>
       </c>
       <c r="N20" t="s">
         <v>125</v>
       </c>
       <c r="O20" t="n">
-        <v>550.0</v>
+        <v>690.0</v>
       </c>
       <c r="P20" t="n">
-        <v>410.0</v>
+        <v>530.0</v>
       </c>
       <c r="Q20" t="n">
-        <v>68181.0</v>
+        <v>68321.0</v>
       </c>
       <c r="R20" t="n">
-        <v>90.0</v>
+        <v>91.0</v>
       </c>
       <c r="S20" t="n">
         <v>85815.0</v>
       </c>
       <c r="T20" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="U20" t="n" s="2">
         <v>42705.0</v>
       </c>
       <c r="V20" t="n">
-        <v>714.0</v>
+        <v>715.0</v>
       </c>
     </row>
     <row r="21">
@@ -1842,16 +1842,16 @@
         <v>3176.0</v>
       </c>
       <c r="F21" t="n">
-        <v>3272.0</v>
+        <v>3273.0</v>
       </c>
       <c r="G21" t="n">
-        <v>4551.0</v>
+        <v>4553.0</v>
       </c>
       <c r="H21" t="n">
-        <v>9130.0</v>
+        <v>9139.0</v>
       </c>
       <c r="I21" t="n">
-        <v>2937.0</v>
+        <v>2938.0</v>
       </c>
       <c r="J21" t="n">
         <v>444.0</v>
@@ -1881,16 +1881,16 @@
         <v>27.0</v>
       </c>
       <c r="S21" t="n">
-        <v>44877.0</v>
+        <v>45507.0</v>
       </c>
       <c r="T21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="U21" t="n" s="2">
         <v>43151.0</v>
       </c>
       <c r="V21" t="n">
-        <v>268.0</v>
+        <v>269.0</v>
       </c>
     </row>
     <row r="22">
@@ -1904,22 +1904,22 @@
         <v>11.0</v>
       </c>
       <c r="D22" t="n">
-        <v>3922.0</v>
+        <v>3899.0</v>
       </c>
       <c r="E22" t="n">
         <v>4253.0</v>
       </c>
       <c r="F22" t="n">
-        <v>1345.0</v>
+        <v>1346.0</v>
       </c>
       <c r="G22" t="n">
-        <v>1411.0</v>
+        <v>1413.0</v>
       </c>
       <c r="H22" t="n">
-        <v>4609.0</v>
+        <v>4616.0</v>
       </c>
       <c r="I22" t="n">
-        <v>880.0</v>
+        <v>881.0</v>
       </c>
       <c r="J22" t="n">
         <v>507.0</v>
@@ -1937,19 +1937,19 @@
         <v>123</v>
       </c>
       <c r="O22" t="n">
-        <v>98.0</v>
+        <v>182.0</v>
       </c>
       <c r="P22" t="n">
-        <v>80.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q22" t="n">
-        <v>21831.0</v>
+        <v>21915.0</v>
       </c>
       <c r="R22" t="n">
-        <v>26.0</v>
+        <v>27.0</v>
       </c>
       <c r="S22" t="n">
-        <v>50608.0</v>
+        <v>51395.0</v>
       </c>
       <c r="T22" t="s">
         <v>127</v>
@@ -1958,7 +1958,7 @@
         <v>43254.0</v>
       </c>
       <c r="V22" t="n">
-        <v>165.0</v>
+        <v>166.0</v>
       </c>
     </row>
     <row r="23">
@@ -2026,7 +2026,7 @@
         <v>43380.0</v>
       </c>
       <c r="V23" t="n">
-        <v>39.0</v>
+        <v>40.0</v>
       </c>
     </row>
     <row r="24">
@@ -2049,16 +2049,16 @@
         <v>4424.0</v>
       </c>
       <c r="G24" t="n">
-        <v>4364.0</v>
+        <v>4367.0</v>
       </c>
       <c r="H24" t="n">
-        <v>18553.0</v>
+        <v>18579.0</v>
       </c>
       <c r="I24" t="n">
-        <v>2943.0</v>
+        <v>2947.0</v>
       </c>
       <c r="J24" t="n">
-        <v>2740.0</v>
+        <v>2743.0</v>
       </c>
       <c r="K24" t="n">
         <v>11.0</v>
@@ -2067,25 +2067,25 @@
         <v>2641.0</v>
       </c>
       <c r="M24" t="n">
-        <v>16002.0</v>
+        <v>16031.0</v>
       </c>
       <c r="N24" t="s">
         <v>124</v>
       </c>
       <c r="O24" t="n">
-        <v>5.0</v>
+        <v>15.0</v>
       </c>
       <c r="P24" t="n">
-        <v>400.0</v>
+        <v>520.0</v>
       </c>
       <c r="Q24" t="n">
-        <v>6383.0</v>
+        <v>6393.0</v>
       </c>
       <c r="R24" t="n">
         <v>79.0</v>
       </c>
       <c r="S24" t="n">
-        <v>81945.0</v>
+        <v>83065.0</v>
       </c>
       <c r="T24" t="s">
         <v>126</v>
@@ -2094,7 +2094,7 @@
         <v>42614.0</v>
       </c>
       <c r="V24" t="n">
-        <v>805.0</v>
+        <v>806.0</v>
       </c>
     </row>
     <row r="25">
@@ -2108,22 +2108,22 @@
         <v>10.0</v>
       </c>
       <c r="D25" t="n">
-        <v>3808.0</v>
+        <v>3869.0</v>
       </c>
       <c r="E25" t="n">
         <v>4008.0</v>
       </c>
       <c r="F25" t="n">
-        <v>1363.0</v>
+        <v>1366.0</v>
       </c>
       <c r="G25" t="n">
-        <v>1385.0</v>
+        <v>1386.0</v>
       </c>
       <c r="H25" t="n">
-        <v>3961.0</v>
+        <v>3966.0</v>
       </c>
       <c r="I25" t="n">
-        <v>646.0</v>
+        <v>648.0</v>
       </c>
       <c r="J25" t="n">
         <v>793.0</v>
@@ -2153,7 +2153,7 @@
         <v>13.0</v>
       </c>
       <c r="S25" t="n">
-        <v>26015.0</v>
+        <v>26277.0</v>
       </c>
       <c r="T25" t="s">
         <v>127</v>
@@ -2162,7 +2162,7 @@
         <v>43400.0</v>
       </c>
       <c r="V25" t="n">
-        <v>19.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="26">
@@ -2176,22 +2176,22 @@
         <v>12.0</v>
       </c>
       <c r="D26" t="n">
-        <v>4118.0</v>
+        <v>4187.0</v>
       </c>
       <c r="E26" t="n">
         <v>4363.0</v>
       </c>
       <c r="F26" t="n">
-        <v>3329.0</v>
+        <v>3337.0</v>
       </c>
       <c r="G26" t="n">
-        <v>3503.0</v>
+        <v>3507.0</v>
       </c>
       <c r="H26" t="n">
-        <v>12300.0</v>
+        <v>12326.0</v>
       </c>
       <c r="I26" t="n">
-        <v>1709.0</v>
+        <v>1714.0</v>
       </c>
       <c r="J26" t="n">
         <v>2757.0</v>
@@ -2209,19 +2209,19 @@
         <v>122</v>
       </c>
       <c r="O26" t="n">
-        <v>366.0</v>
+        <v>508.0</v>
       </c>
       <c r="P26" t="n">
-        <v>280.0</v>
+        <v>400.0</v>
       </c>
       <c r="Q26" t="n">
-        <v>42787.0</v>
+        <v>42929.0</v>
       </c>
       <c r="R26" t="n">
         <v>68.0</v>
       </c>
       <c r="S26" t="n">
-        <v>75643.0</v>
+        <v>76483.0</v>
       </c>
       <c r="T26" t="s">
         <v>128</v>
@@ -2230,7 +2230,7 @@
         <v>43214.0</v>
       </c>
       <c r="V26" t="n">
-        <v>205.0</v>
+        <v>206.0</v>
       </c>
     </row>
     <row r="27">
@@ -2244,22 +2244,22 @@
         <v>12.0</v>
       </c>
       <c r="D27" t="n">
-        <v>4334.0</v>
+        <v>4314.0</v>
       </c>
       <c r="E27" t="n">
         <v>4653.0</v>
       </c>
       <c r="F27" t="n">
-        <v>3711.0</v>
+        <v>3713.0</v>
       </c>
       <c r="G27" t="n">
-        <v>3431.0</v>
+        <v>3434.0</v>
       </c>
       <c r="H27" t="n">
-        <v>11393.0</v>
+        <v>11398.0</v>
       </c>
       <c r="I27" t="n">
-        <v>1551.0</v>
+        <v>1552.0</v>
       </c>
       <c r="J27" t="n">
         <v>3040.0</v>
@@ -2298,7 +2298,7 @@
         <v>42614.0</v>
       </c>
       <c r="V27" t="n">
-        <v>805.0</v>
+        <v>806.0</v>
       </c>
     </row>
     <row r="28">
@@ -2366,7 +2366,7 @@
         <v>43254.0</v>
       </c>
       <c r="V28" t="n">
-        <v>165.0</v>
+        <v>166.0</v>
       </c>
     </row>
     <row r="29">
@@ -2392,10 +2392,10 @@
         <v>1122.0</v>
       </c>
       <c r="H29" t="n">
-        <v>6629.0</v>
+        <v>6644.0</v>
       </c>
       <c r="I29" t="n">
-        <v>1453.0</v>
+        <v>1456.0</v>
       </c>
       <c r="J29" t="n">
         <v>1859.0</v>
@@ -2413,19 +2413,19 @@
         <v>122</v>
       </c>
       <c r="O29" t="n">
-        <v>450.0</v>
+        <v>576.0</v>
       </c>
       <c r="P29" t="n">
-        <v>400.0</v>
+        <v>480.0</v>
       </c>
       <c r="Q29" t="n">
-        <v>13200.0</v>
+        <v>13326.0</v>
       </c>
       <c r="R29" t="n">
-        <v>57.0</v>
+        <v>58.0</v>
       </c>
       <c r="S29" t="n">
-        <v>77622.0</v>
+        <v>78462.0</v>
       </c>
       <c r="T29" t="s">
         <v>128</v>
@@ -2434,7 +2434,7 @@
         <v>43058.0</v>
       </c>
       <c r="V29" t="n">
-        <v>361.0</v>
+        <v>362.0</v>
       </c>
     </row>
     <row r="30">
@@ -2493,7 +2493,7 @@
         <v>53.0</v>
       </c>
       <c r="S30" t="n">
-        <v>69988.0</v>
+        <v>71300.0</v>
       </c>
       <c r="T30" t="s">
         <v>127</v>
@@ -2502,7 +2502,7 @@
         <v>43138.0</v>
       </c>
       <c r="V30" t="n">
-        <v>281.0</v>
+        <v>282.0</v>
       </c>
     </row>
     <row r="31">
@@ -2516,7 +2516,7 @@
         <v>12.0</v>
       </c>
       <c r="D31" t="n">
-        <v>4164.0</v>
+        <v>4137.0</v>
       </c>
       <c r="E31" t="n">
         <v>4190.0</v>
@@ -2525,13 +2525,13 @@
         <v>2157.0</v>
       </c>
       <c r="G31" t="n">
-        <v>2196.0</v>
+        <v>2197.0</v>
       </c>
       <c r="H31" t="n">
-        <v>6982.0</v>
+        <v>6989.0</v>
       </c>
       <c r="I31" t="n">
-        <v>1572.0</v>
+        <v>1573.0</v>
       </c>
       <c r="J31" t="n">
         <v>1474.0</v>
@@ -2549,19 +2549,19 @@
         <v>122</v>
       </c>
       <c r="O31" t="n">
-        <v>407.0</v>
+        <v>497.0</v>
       </c>
       <c r="P31" t="n">
-        <v>240.0</v>
+        <v>320.0</v>
       </c>
       <c r="Q31" t="n">
-        <v>42990.0</v>
+        <v>43080.0</v>
       </c>
       <c r="R31" t="n">
         <v>37.0</v>
       </c>
       <c r="S31" t="n">
-        <v>73633.0</v>
+        <v>74753.0</v>
       </c>
       <c r="T31" t="s">
         <v>128</v>
@@ -2570,7 +2570,7 @@
         <v>42920.0</v>
       </c>
       <c r="V31" t="n">
-        <v>499.0</v>
+        <v>500.0</v>
       </c>
     </row>
     <row r="32">
@@ -2584,22 +2584,22 @@
         <v>12.0</v>
       </c>
       <c r="D32" t="n">
-        <v>4611.0</v>
+        <v>4613.0</v>
       </c>
       <c r="E32" t="n">
         <v>4798.0</v>
       </c>
       <c r="F32" t="n">
-        <v>5175.0</v>
+        <v>5179.0</v>
       </c>
       <c r="G32" t="n">
-        <v>5275.0</v>
+        <v>5280.0</v>
       </c>
       <c r="H32" t="n">
-        <v>12388.0</v>
+        <v>12398.0</v>
       </c>
       <c r="I32" t="n">
-        <v>2256.0</v>
+        <v>2257.0</v>
       </c>
       <c r="J32" t="n">
         <v>1728.0</v>
@@ -2632,13 +2632,13 @@
         <v>79630.0</v>
       </c>
       <c r="T32" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="U32" t="n" s="2">
         <v>43058.0</v>
       </c>
       <c r="V32" t="n">
-        <v>361.0</v>
+        <v>362.0</v>
       </c>
     </row>
     <row r="33">
@@ -2664,7 +2664,7 @@
         <v>221.0</v>
       </c>
       <c r="H33" t="n">
-        <v>1580.0</v>
+        <v>1587.0</v>
       </c>
       <c r="I33" t="n">
         <v>270.0</v>
@@ -2685,19 +2685,19 @@
         <v>123</v>
       </c>
       <c r="O33" t="n">
-        <v>184.0</v>
+        <v>248.0</v>
       </c>
       <c r="P33" t="n">
-        <v>120.0</v>
+        <v>200.0</v>
       </c>
       <c r="Q33" t="n">
-        <v>4705.0</v>
+        <v>4769.0</v>
       </c>
       <c r="R33" t="n">
         <v>0.0</v>
       </c>
       <c r="S33" t="n">
-        <v>1591.0</v>
+        <v>2045.0</v>
       </c>
       <c r="T33" t="s">
         <v>132</v>
@@ -2706,7 +2706,7 @@
         <v>43409.0</v>
       </c>
       <c r="V33" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="34">
@@ -2726,19 +2726,19 @@
         <v>4021.0</v>
       </c>
       <c r="F34" t="n">
-        <v>956.0</v>
+        <v>959.0</v>
       </c>
       <c r="G34" t="n">
-        <v>972.0</v>
+        <v>975.0</v>
       </c>
       <c r="H34" t="n">
-        <v>4226.0</v>
+        <v>4241.0</v>
       </c>
       <c r="I34" t="n">
-        <v>994.0</v>
+        <v>997.0</v>
       </c>
       <c r="J34" t="n">
-        <v>278.0</v>
+        <v>290.0</v>
       </c>
       <c r="K34" t="n">
         <v>6.0</v>
@@ -2753,19 +2753,19 @@
         <v>123</v>
       </c>
       <c r="O34" t="n">
-        <v>42.0</v>
+        <v>78.0</v>
       </c>
       <c r="P34" t="n">
         <v>120.0</v>
       </c>
       <c r="Q34" t="n">
-        <v>8443.0</v>
+        <v>8479.0</v>
       </c>
       <c r="R34" t="n">
-        <v>28.0</v>
+        <v>29.0</v>
       </c>
       <c r="S34" t="n">
-        <v>64552.0</v>
+        <v>65601.0</v>
       </c>
       <c r="T34" t="s">
         <v>127</v>
@@ -2774,7 +2774,7 @@
         <v>43312.0</v>
       </c>
       <c r="V34" t="n">
-        <v>107.0</v>
+        <v>108.0</v>
       </c>
     </row>
     <row r="35">
@@ -2788,22 +2788,22 @@
         <v>10.0</v>
       </c>
       <c r="D35" t="n">
-        <v>3859.0</v>
+        <v>3846.0</v>
       </c>
       <c r="E35" t="n">
         <v>4007.0</v>
       </c>
       <c r="F35" t="n">
-        <v>560.0</v>
+        <v>563.0</v>
       </c>
       <c r="G35" t="n">
-        <v>495.0</v>
+        <v>499.0</v>
       </c>
       <c r="H35" t="n">
-        <v>3395.0</v>
+        <v>3414.0</v>
       </c>
       <c r="I35" t="n">
-        <v>705.0</v>
+        <v>708.0</v>
       </c>
       <c r="J35" t="n">
         <v>278.0</v>
@@ -2821,19 +2821,19 @@
         <v>123</v>
       </c>
       <c r="O35" t="n">
-        <v>264.0</v>
+        <v>380.0</v>
       </c>
       <c r="P35" t="n">
-        <v>272.0</v>
+        <v>392.0</v>
       </c>
       <c r="Q35" t="n">
-        <v>17237.0</v>
+        <v>17353.0</v>
       </c>
       <c r="R35" t="n">
         <v>26.0</v>
       </c>
       <c r="S35" t="n">
-        <v>63276.0</v>
+        <v>64325.0</v>
       </c>
       <c r="T35" t="s">
         <v>127</v>
@@ -2842,7 +2842,7 @@
         <v>43274.0</v>
       </c>
       <c r="V35" t="n">
-        <v>145.0</v>
+        <v>146.0</v>
       </c>
     </row>
     <row r="36">
@@ -2856,19 +2856,19 @@
         <v>10.0</v>
       </c>
       <c r="D36" t="n">
-        <v>4086.0</v>
+        <v>3957.0</v>
       </c>
       <c r="E36" t="n">
         <v>4135.0</v>
       </c>
       <c r="F36" t="n">
-        <v>3513.0</v>
+        <v>3521.0</v>
       </c>
       <c r="G36" t="n">
-        <v>4067.0</v>
+        <v>4081.0</v>
       </c>
       <c r="H36" t="n">
-        <v>9674.0</v>
+        <v>9700.0</v>
       </c>
       <c r="I36" t="n">
         <v>1773.0</v>
@@ -2889,28 +2889,28 @@
         <v>122</v>
       </c>
       <c r="O36" t="n">
-        <v>178.0</v>
+        <v>229.0</v>
       </c>
       <c r="P36" t="n">
-        <v>180.0</v>
+        <v>270.0</v>
       </c>
       <c r="Q36" t="n">
-        <v>14651.0</v>
+        <v>14702.0</v>
       </c>
       <c r="R36" t="n">
         <v>35.0</v>
       </c>
       <c r="S36" t="n">
-        <v>71637.0</v>
+        <v>73037.0</v>
       </c>
       <c r="T36" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="U36" t="n" s="2">
         <v>43280.0</v>
       </c>
       <c r="V36" t="n">
-        <v>139.0</v>
+        <v>140.0</v>
       </c>
     </row>
     <row r="37">
@@ -2957,13 +2957,13 @@
         <v>123</v>
       </c>
       <c r="O37" t="n">
-        <v>120.0</v>
+        <v>138.0</v>
       </c>
       <c r="P37" t="n">
-        <v>240.0</v>
+        <v>280.0</v>
       </c>
       <c r="Q37" t="n">
-        <v>2749.0</v>
+        <v>2767.0</v>
       </c>
       <c r="R37" t="n">
         <v>2.0</v>
@@ -2978,7 +2978,7 @@
         <v>43360.0</v>
       </c>
       <c r="V37" t="n">
-        <v>59.0</v>
+        <v>60.0</v>
       </c>
     </row>
     <row r="38">
@@ -3004,10 +3004,10 @@
         <v>991.0</v>
       </c>
       <c r="H38" t="n">
-        <v>4487.0</v>
+        <v>4500.0</v>
       </c>
       <c r="I38" t="n">
-        <v>471.0</v>
+        <v>472.0</v>
       </c>
       <c r="J38" t="n">
         <v>2215.0</v>
@@ -3025,19 +3025,19 @@
         <v>122</v>
       </c>
       <c r="O38" t="n">
-        <v>472.0</v>
+        <v>534.0</v>
       </c>
       <c r="P38" t="n">
-        <v>460.0</v>
+        <v>580.0</v>
       </c>
       <c r="Q38" t="n">
-        <v>26050.0</v>
+        <v>26112.0</v>
       </c>
       <c r="R38" t="n">
-        <v>40.0</v>
+        <v>41.0</v>
       </c>
       <c r="S38" t="n">
-        <v>77866.0</v>
+        <v>78706.0</v>
       </c>
       <c r="T38" t="s">
         <v>128</v>
@@ -3046,7 +3046,7 @@
         <v>43284.0</v>
       </c>
       <c r="V38" t="n">
-        <v>135.0</v>
+        <v>136.0</v>
       </c>
     </row>
     <row r="39">
@@ -3060,22 +3060,22 @@
         <v>10.0</v>
       </c>
       <c r="D39" t="n">
-        <v>4060.0</v>
+        <v>4061.0</v>
       </c>
       <c r="E39" t="n">
         <v>4405.0</v>
       </c>
       <c r="F39" t="n">
-        <v>1095.0</v>
+        <v>1096.0</v>
       </c>
       <c r="G39" t="n">
-        <v>999.0</v>
+        <v>1000.0</v>
       </c>
       <c r="H39" t="n">
-        <v>3146.0</v>
+        <v>3149.0</v>
       </c>
       <c r="I39" t="n">
-        <v>657.0</v>
+        <v>658.0</v>
       </c>
       <c r="J39" t="n">
         <v>1700.0</v>
@@ -3093,19 +3093,19 @@
         <v>123</v>
       </c>
       <c r="O39" t="n">
-        <v>223.0</v>
+        <v>303.0</v>
       </c>
       <c r="P39" t="n">
-        <v>280.0</v>
+        <v>320.0</v>
       </c>
       <c r="Q39" t="n">
-        <v>20185.0</v>
+        <v>20265.0</v>
       </c>
       <c r="R39" t="n">
-        <v>16.0</v>
+        <v>17.0</v>
       </c>
       <c r="S39" t="n">
-        <v>53360.0</v>
+        <v>54200.0</v>
       </c>
       <c r="T39" t="s">
         <v>128</v>
@@ -3114,7 +3114,7 @@
         <v>43352.0</v>
       </c>
       <c r="V39" t="n">
-        <v>67.0</v>
+        <v>68.0</v>
       </c>
     </row>
     <row r="40">
@@ -3134,16 +3134,16 @@
         <v>4553.0</v>
       </c>
       <c r="F40" t="n">
-        <v>4639.0</v>
+        <v>4640.0</v>
       </c>
       <c r="G40" t="n">
         <v>4695.0</v>
       </c>
       <c r="H40" t="n">
-        <v>26808.0</v>
+        <v>26820.0</v>
       </c>
       <c r="I40" t="n">
-        <v>3655.0</v>
+        <v>3656.0</v>
       </c>
       <c r="J40" t="n">
         <v>2006.0</v>
@@ -3164,16 +3164,16 @@
         <v>0.0</v>
       </c>
       <c r="P40" t="n">
-        <v>120.0</v>
+        <v>160.0</v>
       </c>
       <c r="Q40" t="n">
         <v>7122.0</v>
       </c>
       <c r="R40" t="n">
-        <v>61.0</v>
+        <v>62.0</v>
       </c>
       <c r="S40" t="n">
-        <v>74875.0</v>
+        <v>76275.0</v>
       </c>
       <c r="T40" t="s">
         <v>126</v>
@@ -3182,7 +3182,7 @@
         <v>43252.0</v>
       </c>
       <c r="V40" t="n">
-        <v>167.0</v>
+        <v>168.0</v>
       </c>
     </row>
     <row r="41">
@@ -3196,25 +3196,25 @@
         <v>11.0</v>
       </c>
       <c r="D41" t="n">
-        <v>4034.0</v>
+        <v>4105.0</v>
       </c>
       <c r="E41" t="n">
         <v>4323.0</v>
       </c>
       <c r="F41" t="n">
-        <v>2406.0</v>
+        <v>2414.0</v>
       </c>
       <c r="G41" t="n">
-        <v>2328.0</v>
+        <v>2334.0</v>
       </c>
       <c r="H41" t="n">
-        <v>6056.0</v>
+        <v>6077.0</v>
       </c>
       <c r="I41" t="n">
-        <v>1186.0</v>
+        <v>1189.0</v>
       </c>
       <c r="J41" t="n">
-        <v>2792.0</v>
+        <v>2804.0</v>
       </c>
       <c r="K41" t="n">
         <v>11.0</v>
@@ -3229,19 +3229,19 @@
         <v>123</v>
       </c>
       <c r="O41" t="n">
-        <v>298.0</v>
+        <v>406.0</v>
       </c>
       <c r="P41" t="n">
-        <v>360.0</v>
+        <v>400.0</v>
       </c>
       <c r="Q41" t="n">
-        <v>21858.0</v>
+        <v>21966.0</v>
       </c>
       <c r="R41" t="n">
         <v>19.0</v>
       </c>
       <c r="S41" t="n">
-        <v>33732.0</v>
+        <v>34852.0</v>
       </c>
       <c r="T41" t="s">
         <v>128</v>
@@ -3250,7 +3250,7 @@
         <v>43370.0</v>
       </c>
       <c r="V41" t="n">
-        <v>49.0</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="42">
@@ -3270,16 +3270,16 @@
         <v>3965.0</v>
       </c>
       <c r="F42" t="n">
-        <v>1263.0</v>
+        <v>1266.0</v>
       </c>
       <c r="G42" t="n">
-        <v>1103.0</v>
+        <v>1104.0</v>
       </c>
       <c r="H42" t="n">
-        <v>4288.0</v>
+        <v>4301.0</v>
       </c>
       <c r="I42" t="n">
-        <v>737.0</v>
+        <v>739.0</v>
       </c>
       <c r="J42" t="n">
         <v>1905.0</v>
@@ -3297,19 +3297,19 @@
         <v>123</v>
       </c>
       <c r="O42" t="n">
-        <v>146.0</v>
+        <v>270.0</v>
       </c>
       <c r="P42" t="n">
-        <v>80.0</v>
+        <v>160.0</v>
       </c>
       <c r="Q42" t="n">
-        <v>28011.0</v>
+        <v>28135.0</v>
       </c>
       <c r="R42" t="n">
         <v>22.0</v>
       </c>
       <c r="S42" t="n">
-        <v>19010.0</v>
+        <v>20322.0</v>
       </c>
       <c r="T42" t="s">
         <v>127</v>
@@ -3318,7 +3318,7 @@
         <v>43419.0</v>
       </c>
       <c r="V42" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="43">
@@ -3332,22 +3332,22 @@
         <v>12.0</v>
       </c>
       <c r="D43" t="n">
-        <v>4275.0</v>
+        <v>4309.0</v>
       </c>
       <c r="E43" t="n">
-        <v>4275.0</v>
+        <v>4309.0</v>
       </c>
       <c r="F43" t="n">
-        <v>2750.0</v>
+        <v>2752.0</v>
       </c>
       <c r="G43" t="n">
-        <v>2660.0</v>
+        <v>2661.0</v>
       </c>
       <c r="H43" t="n">
-        <v>7806.0</v>
+        <v>7813.0</v>
       </c>
       <c r="I43" t="n">
-        <v>2273.0</v>
+        <v>2276.0</v>
       </c>
       <c r="J43" t="n">
         <v>2311.0</v>
@@ -3365,28 +3365,28 @@
         <v>123</v>
       </c>
       <c r="O43" t="n">
-        <v>92.0</v>
+        <v>138.0</v>
       </c>
       <c r="P43" t="n">
-        <v>120.0</v>
+        <v>152.0</v>
       </c>
       <c r="Q43" t="n">
-        <v>31749.0</v>
+        <v>31795.0</v>
       </c>
       <c r="R43" t="n">
         <v>24.0</v>
       </c>
       <c r="S43" t="n">
-        <v>28135.0</v>
+        <v>29535.0</v>
       </c>
       <c r="T43" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="U43" t="n" s="2">
         <v>43382.0</v>
       </c>
       <c r="V43" t="n">
-        <v>37.0</v>
+        <v>38.0</v>
       </c>
     </row>
     <row r="44">
@@ -3400,22 +3400,22 @@
         <v>11.0</v>
       </c>
       <c r="D44" t="n">
-        <v>4335.0</v>
+        <v>4285.0</v>
       </c>
       <c r="E44" t="n">
         <v>4400.0</v>
       </c>
       <c r="F44" t="n">
-        <v>3823.0</v>
+        <v>3829.0</v>
       </c>
       <c r="G44" t="n">
-        <v>4125.0</v>
+        <v>4132.0</v>
       </c>
       <c r="H44" t="n">
-        <v>8681.0</v>
+        <v>8694.0</v>
       </c>
       <c r="I44" t="n">
-        <v>2038.0</v>
+        <v>2040.0</v>
       </c>
       <c r="J44" t="n">
         <v>1339.0</v>
@@ -3433,13 +3433,13 @@
         <v>123</v>
       </c>
       <c r="O44" t="n">
-        <v>307.0</v>
+        <v>403.0</v>
       </c>
       <c r="P44" t="n">
-        <v>280.0</v>
+        <v>320.0</v>
       </c>
       <c r="Q44" t="n">
-        <v>22127.0</v>
+        <v>22252.0</v>
       </c>
       <c r="R44" t="n">
         <v>20.0</v>
@@ -3448,13 +3448,13 @@
         <v>74532.0</v>
       </c>
       <c r="T44" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="U44" t="n" s="2">
         <v>43390.0</v>
       </c>
       <c r="V44" t="n">
-        <v>29.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="45">
@@ -3468,7 +3468,7 @@
         <v>12.0</v>
       </c>
       <c r="D45" t="n">
-        <v>4171.0</v>
+        <v>4118.0</v>
       </c>
       <c r="E45" t="n">
         <v>4473.0</v>
@@ -3477,13 +3477,13 @@
         <v>2634.0</v>
       </c>
       <c r="G45" t="n">
-        <v>2581.0</v>
+        <v>2583.0</v>
       </c>
       <c r="H45" t="n">
-        <v>7214.0</v>
+        <v>7219.0</v>
       </c>
       <c r="I45" t="n">
-        <v>1382.0</v>
+        <v>1383.0</v>
       </c>
       <c r="J45" t="n">
         <v>3505.0</v>
@@ -3501,19 +3501,19 @@
         <v>123</v>
       </c>
       <c r="O45" t="n">
-        <v>507.0</v>
+        <v>599.0</v>
       </c>
       <c r="P45" t="n">
-        <v>240.0</v>
+        <v>320.0</v>
       </c>
       <c r="Q45" t="n">
-        <v>49609.0</v>
+        <v>49701.0</v>
       </c>
       <c r="R45" t="n">
         <v>33.0</v>
       </c>
       <c r="S45" t="n">
-        <v>42245.0</v>
+        <v>43365.0</v>
       </c>
       <c r="T45" t="s">
         <v>128</v>
@@ -3522,7 +3522,7 @@
         <v>43390.0</v>
       </c>
       <c r="V45" t="n">
-        <v>29.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="46">
@@ -3536,28 +3536,28 @@
         <v>8.0</v>
       </c>
       <c r="D46" t="n">
-        <v>2716.0</v>
+        <v>2818.0</v>
       </c>
       <c r="E46" t="n">
-        <v>2716.0</v>
+        <v>2841.0</v>
       </c>
       <c r="F46" t="n">
-        <v>201.0</v>
+        <v>217.0</v>
       </c>
       <c r="G46" t="n">
-        <v>94.0</v>
+        <v>103.0</v>
       </c>
       <c r="H46" t="n">
-        <v>354.0</v>
+        <v>393.0</v>
       </c>
       <c r="I46" t="n">
-        <v>92.0</v>
+        <v>100.0</v>
       </c>
       <c r="J46" t="n">
-        <v>0.0</v>
+        <v>58.0</v>
       </c>
       <c r="K46" t="n">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="L46" t="n">
         <v>0.0</v>
@@ -3569,28 +3569,28 @@
         <v>123</v>
       </c>
       <c r="O46" t="n">
-        <v>140.0</v>
+        <v>202.0</v>
       </c>
       <c r="P46" t="n">
-        <v>180.0</v>
+        <v>210.0</v>
       </c>
       <c r="Q46" t="n">
-        <v>1268.0</v>
+        <v>1330.0</v>
       </c>
       <c r="R46" t="n">
         <v>1.0</v>
       </c>
       <c r="S46" t="n">
-        <v>3079.0</v>
+        <v>4339.0</v>
       </c>
       <c r="T46" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="U46" t="n" s="2">
         <v>43376.0</v>
       </c>
       <c r="V46" t="n">
-        <v>43.0</v>
+        <v>44.0</v>
       </c>
     </row>
     <row r="47">
@@ -3604,25 +3604,25 @@
         <v>12.0</v>
       </c>
       <c r="D47" t="n">
-        <v>4152.0</v>
+        <v>4406.0</v>
       </c>
       <c r="E47" t="n">
         <v>4919.0</v>
       </c>
       <c r="F47" t="n">
-        <v>11004.0</v>
+        <v>11024.0</v>
       </c>
       <c r="G47" t="n">
-        <v>11714.0</v>
+        <v>11730.0</v>
       </c>
       <c r="H47" t="n">
-        <v>26195.0</v>
+        <v>26243.0</v>
       </c>
       <c r="I47" t="n">
-        <v>9033.0</v>
+        <v>9051.0</v>
       </c>
       <c r="J47" t="n">
-        <v>2205.0</v>
+        <v>2212.0</v>
       </c>
       <c r="K47" t="n">
         <v>10.0</v>
@@ -3637,28 +3637,28 @@
         <v>123</v>
       </c>
       <c r="O47" t="n">
-        <v>755.0</v>
+        <v>849.0</v>
       </c>
       <c r="P47" t="n">
-        <v>340.0</v>
+        <v>350.0</v>
       </c>
       <c r="Q47" t="n">
-        <v>76153.0</v>
+        <v>76247.0</v>
       </c>
       <c r="R47" t="n">
         <v>24.0</v>
       </c>
       <c r="S47" t="n">
-        <v>84590.0</v>
+        <v>85430.0</v>
       </c>
       <c r="T47" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="U47" t="n" s="2">
         <v>43390.0</v>
       </c>
       <c r="V47" t="n">
-        <v>29.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="48">
@@ -3684,10 +3684,10 @@
         <v>3042.0</v>
       </c>
       <c r="H48" t="n">
-        <v>15608.0</v>
+        <v>15621.0</v>
       </c>
       <c r="I48" t="n">
-        <v>3283.0</v>
+        <v>3285.0</v>
       </c>
       <c r="J48" t="n">
         <v>1889.0</v>
@@ -3705,19 +3705,19 @@
         <v>122</v>
       </c>
       <c r="O48" t="n">
-        <v>248.0</v>
+        <v>266.0</v>
       </c>
       <c r="P48" t="n">
-        <v>360.0</v>
+        <v>400.0</v>
       </c>
       <c r="Q48" t="n">
-        <v>33369.0</v>
+        <v>33387.0</v>
       </c>
       <c r="R48" t="n">
-        <v>38.0</v>
+        <v>39.0</v>
       </c>
       <c r="S48" t="n">
-        <v>71135.0</v>
+        <v>72535.0</v>
       </c>
       <c r="T48" t="s">
         <v>128</v>
@@ -3726,7 +3726,7 @@
         <v>43230.0</v>
       </c>
       <c r="V48" t="n">
-        <v>189.0</v>
+        <v>190.0</v>
       </c>
     </row>
     <row r="49">
@@ -3749,16 +3749,16 @@
         <v>6388.0</v>
       </c>
       <c r="G49" t="n">
-        <v>6617.0</v>
+        <v>6620.0</v>
       </c>
       <c r="H49" t="n">
-        <v>18272.0</v>
+        <v>18281.0</v>
       </c>
       <c r="I49" t="n">
-        <v>3777.0</v>
+        <v>3778.0</v>
       </c>
       <c r="J49" t="n">
-        <v>4380.0</v>
+        <v>4383.0</v>
       </c>
       <c r="K49" t="n">
         <v>10.0</v>
@@ -3773,19 +3773,19 @@
         <v>124</v>
       </c>
       <c r="O49" t="n">
-        <v>113.0</v>
+        <v>127.0</v>
       </c>
       <c r="P49" t="n">
-        <v>200.0</v>
+        <v>240.0</v>
       </c>
       <c r="Q49" t="n">
-        <v>20825.0</v>
+        <v>20839.0</v>
       </c>
       <c r="R49" t="n">
-        <v>60.0</v>
+        <v>61.0</v>
       </c>
       <c r="S49" t="n">
-        <v>79117.0</v>
+        <v>80517.0</v>
       </c>
       <c r="T49" t="s">
         <v>126</v>
@@ -3794,7 +3794,7 @@
         <v>43184.0</v>
       </c>
       <c r="V49" t="n">
-        <v>235.0</v>
+        <v>236.0</v>
       </c>
     </row>
     <row r="50">
@@ -3862,7 +3862,7 @@
         <v>43314.0</v>
       </c>
       <c r="V50" t="n">
-        <v>105.0</v>
+        <v>106.0</v>
       </c>
     </row>
     <row r="51">
@@ -3930,7 +3930,7 @@
         <v>43254.0</v>
       </c>
       <c r="V51" t="n">
-        <v>165.0</v>
+        <v>166.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Core refactoring + last month presence stat
</commit_message>
<xml_diff>
--- a/docs/data/memberstats.xlsx
+++ b/docs/data/memberstats.xlsx
@@ -541,22 +541,22 @@
         <v>11.0</v>
       </c>
       <c r="D2" t="n">
-        <v>4355.0</v>
+        <v>4500.0</v>
       </c>
       <c r="E2" t="n">
         <v>4653.0</v>
       </c>
       <c r="F2" t="n">
-        <v>2279.0</v>
+        <v>2284.0</v>
       </c>
       <c r="G2" t="n">
         <v>2109.0</v>
       </c>
       <c r="H2" t="n">
-        <v>7102.0</v>
+        <v>7108.0</v>
       </c>
       <c r="I2" t="n">
-        <v>1158.0</v>
+        <v>1159.0</v>
       </c>
       <c r="J2" t="n">
         <v>2672.0</v>
@@ -574,13 +574,13 @@
         <v>122</v>
       </c>
       <c r="O2" t="n">
-        <v>32.0</v>
+        <v>160.0</v>
       </c>
       <c r="P2" t="n">
-        <v>40.0</v>
+        <v>190.0</v>
       </c>
       <c r="Q2" t="n">
-        <v>28905.0</v>
+        <v>29033.0</v>
       </c>
       <c r="R2" t="n">
         <v>46.0</v>
@@ -595,7 +595,7 @@
         <v>43302.0</v>
       </c>
       <c r="V2" t="n">
-        <v>122.0</v>
+        <v>123.0</v>
       </c>
     </row>
     <row r="3">
@@ -663,7 +663,7 @@
         <v>43372.0</v>
       </c>
       <c r="V3" t="n">
-        <v>52.0</v>
+        <v>53.0</v>
       </c>
     </row>
     <row r="4">
@@ -677,7 +677,7 @@
         <v>11.0</v>
       </c>
       <c r="D4" t="n">
-        <v>4093.0</v>
+        <v>4039.0</v>
       </c>
       <c r="E4" t="n">
         <v>4292.0</v>
@@ -686,10 +686,10 @@
         <v>2653.0</v>
       </c>
       <c r="G4" t="n">
-        <v>2687.0</v>
+        <v>2689.0</v>
       </c>
       <c r="H4" t="n">
-        <v>6352.0</v>
+        <v>6358.0</v>
       </c>
       <c r="I4" t="n">
         <v>1077.0</v>
@@ -713,7 +713,7 @@
         <v>8.0</v>
       </c>
       <c r="P4" t="n">
-        <v>40.0</v>
+        <v>136.0</v>
       </c>
       <c r="Q4" t="n">
         <v>9148.0</v>
@@ -722,7 +722,7 @@
         <v>48.0</v>
       </c>
       <c r="S4" t="n">
-        <v>66406.0</v>
+        <v>67526.0</v>
       </c>
       <c r="T4" t="s">
         <v>128</v>
@@ -731,7 +731,7 @@
         <v>43082.0</v>
       </c>
       <c r="V4" t="n">
-        <v>342.0</v>
+        <v>343.0</v>
       </c>
     </row>
     <row r="5">
@@ -757,7 +757,7 @@
         <v>659.0</v>
       </c>
       <c r="H5" t="n">
-        <v>2003.0</v>
+        <v>2004.0</v>
       </c>
       <c r="I5" t="n">
         <v>387.0</v>
@@ -781,7 +781,7 @@
         <v>0.0</v>
       </c>
       <c r="P5" t="n">
-        <v>0.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q5" t="n">
         <v>16997.0</v>
@@ -790,7 +790,7 @@
         <v>5.0</v>
       </c>
       <c r="S5" t="n">
-        <v>10885.0</v>
+        <v>11130.0</v>
       </c>
       <c r="T5" t="s">
         <v>129</v>
@@ -799,7 +799,7 @@
         <v>43397.0</v>
       </c>
       <c r="V5" t="n">
-        <v>27.0</v>
+        <v>28.0</v>
       </c>
     </row>
     <row r="6">
@@ -813,22 +813,22 @@
         <v>10.0</v>
       </c>
       <c r="D6" t="n">
-        <v>4028.0</v>
+        <v>4086.0</v>
       </c>
       <c r="E6" t="n">
         <v>4142.0</v>
       </c>
       <c r="F6" t="n">
-        <v>1257.0</v>
+        <v>1259.0</v>
       </c>
       <c r="G6" t="n">
         <v>1290.0</v>
       </c>
       <c r="H6" t="n">
-        <v>3277.0</v>
+        <v>3281.0</v>
       </c>
       <c r="I6" t="n">
-        <v>503.0</v>
+        <v>504.0</v>
       </c>
       <c r="J6" t="n">
         <v>310.0</v>
@@ -846,13 +846,13 @@
         <v>123</v>
       </c>
       <c r="O6" t="n">
-        <v>90.0</v>
+        <v>184.0</v>
       </c>
       <c r="P6" t="n">
-        <v>200.0</v>
+        <v>280.0</v>
       </c>
       <c r="Q6" t="n">
-        <v>16987.0</v>
+        <v>17081.0</v>
       </c>
       <c r="R6" t="n">
         <v>30.0</v>
@@ -867,7 +867,7 @@
         <v>43356.0</v>
       </c>
       <c r="V6" t="n">
-        <v>68.0</v>
+        <v>69.0</v>
       </c>
     </row>
     <row r="7">
@@ -935,7 +935,7 @@
         <v>43364.0</v>
       </c>
       <c r="V7" t="n">
-        <v>60.0</v>
+        <v>61.0</v>
       </c>
     </row>
     <row r="8">
@@ -949,22 +949,22 @@
         <v>11.0</v>
       </c>
       <c r="D8" t="n">
-        <v>4410.0</v>
+        <v>4449.0</v>
       </c>
       <c r="E8" t="n">
-        <v>4497.0</v>
+        <v>4532.0</v>
       </c>
       <c r="F8" t="n">
-        <v>1935.0</v>
+        <v>1942.0</v>
       </c>
       <c r="G8" t="n">
-        <v>1825.0</v>
+        <v>1831.0</v>
       </c>
       <c r="H8" t="n">
-        <v>7690.0</v>
+        <v>7717.0</v>
       </c>
       <c r="I8" t="n">
-        <v>1123.0</v>
+        <v>1124.0</v>
       </c>
       <c r="J8" t="n">
         <v>1396.0</v>
@@ -982,19 +982,19 @@
         <v>124</v>
       </c>
       <c r="O8" t="n">
-        <v>94.0</v>
+        <v>218.0</v>
       </c>
       <c r="P8" t="n">
-        <v>80.0</v>
+        <v>180.0</v>
       </c>
       <c r="Q8" t="n">
-        <v>25478.0</v>
+        <v>25602.0</v>
       </c>
       <c r="R8" t="n">
         <v>58.0</v>
       </c>
       <c r="S8" t="n">
-        <v>73195.0</v>
+        <v>74035.0</v>
       </c>
       <c r="T8" t="s">
         <v>126</v>
@@ -1003,7 +1003,7 @@
         <v>43058.0</v>
       </c>
       <c r="V8" t="n">
-        <v>366.0</v>
+        <v>367.0</v>
       </c>
     </row>
     <row r="9">
@@ -1071,7 +1071,7 @@
         <v>43123.0</v>
       </c>
       <c r="V9" t="n">
-        <v>301.0</v>
+        <v>302.0</v>
       </c>
     </row>
     <row r="10">
@@ -1085,22 +1085,22 @@
         <v>11.0</v>
       </c>
       <c r="D10" t="n">
-        <v>4487.0</v>
+        <v>4611.0</v>
       </c>
       <c r="E10" t="n">
-        <v>4545.0</v>
+        <v>4611.0</v>
       </c>
       <c r="F10" t="n">
-        <v>2489.0</v>
+        <v>2495.0</v>
       </c>
       <c r="G10" t="n">
-        <v>2313.0</v>
+        <v>2315.0</v>
       </c>
       <c r="H10" t="n">
-        <v>10919.0</v>
+        <v>10944.0</v>
       </c>
       <c r="I10" t="n">
-        <v>2415.0</v>
+        <v>2418.0</v>
       </c>
       <c r="J10" t="n">
         <v>1922.0</v>
@@ -1118,13 +1118,13 @@
         <v>124</v>
       </c>
       <c r="O10" t="n">
-        <v>20.0</v>
+        <v>50.0</v>
       </c>
       <c r="P10" t="n">
-        <v>120.0</v>
+        <v>240.0</v>
       </c>
       <c r="Q10" t="n">
-        <v>3376.0</v>
+        <v>3406.0</v>
       </c>
       <c r="R10" t="n">
         <v>59.0</v>
@@ -1133,13 +1133,13 @@
         <v>84670.0</v>
       </c>
       <c r="T10" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="U10" t="n" s="2">
         <v>43123.0</v>
       </c>
       <c r="V10" t="n">
-        <v>301.0</v>
+        <v>302.0</v>
       </c>
     </row>
     <row r="11">
@@ -1153,22 +1153,22 @@
         <v>12.0</v>
       </c>
       <c r="D11" t="n">
-        <v>4382.0</v>
+        <v>4419.0</v>
       </c>
       <c r="E11" t="n">
         <v>4731.0</v>
       </c>
       <c r="F11" t="n">
-        <v>2263.0</v>
+        <v>2267.0</v>
       </c>
       <c r="G11" t="n">
-        <v>1756.0</v>
+        <v>1759.0</v>
       </c>
       <c r="H11" t="n">
-        <v>9572.0</v>
+        <v>9593.0</v>
       </c>
       <c r="I11" t="n">
-        <v>1375.0</v>
+        <v>1376.0</v>
       </c>
       <c r="J11" t="n">
         <v>4216.0</v>
@@ -1186,19 +1186,19 @@
         <v>123</v>
       </c>
       <c r="O11" t="n">
-        <v>303.0</v>
+        <v>613.0</v>
       </c>
       <c r="P11" t="n">
-        <v>120.0</v>
+        <v>220.0</v>
       </c>
       <c r="Q11" t="n">
-        <v>91600.0</v>
+        <v>91910.0</v>
       </c>
       <c r="R11" t="n">
         <v>77.0</v>
       </c>
       <c r="S11" t="n">
-        <v>79880.0</v>
+        <v>80720.0</v>
       </c>
       <c r="T11" t="s">
         <v>126</v>
@@ -1207,7 +1207,7 @@
         <v>43397.0</v>
       </c>
       <c r="V11" t="n">
-        <v>27.0</v>
+        <v>28.0</v>
       </c>
     </row>
     <row r="12">
@@ -1221,22 +1221,22 @@
         <v>11.0</v>
       </c>
       <c r="D12" t="n">
-        <v>4225.0</v>
+        <v>4315.0</v>
       </c>
       <c r="E12" t="n">
         <v>4389.0</v>
       </c>
       <c r="F12" t="n">
-        <v>1389.0</v>
+        <v>1392.0</v>
       </c>
       <c r="G12" t="n">
         <v>1231.0</v>
       </c>
       <c r="H12" t="n">
-        <v>5647.0</v>
+        <v>5670.0</v>
       </c>
       <c r="I12" t="n">
-        <v>778.0</v>
+        <v>779.0</v>
       </c>
       <c r="J12" t="n">
         <v>1235.0</v>
@@ -1254,13 +1254,13 @@
         <v>124</v>
       </c>
       <c r="O12" t="n">
-        <v>186.0</v>
+        <v>343.0</v>
       </c>
       <c r="P12" t="n">
-        <v>120.0</v>
+        <v>200.0</v>
       </c>
       <c r="Q12" t="n">
-        <v>38834.0</v>
+        <v>38991.0</v>
       </c>
       <c r="R12" t="n">
         <v>65.0</v>
@@ -1269,13 +1269,13 @@
         <v>79200.0</v>
       </c>
       <c r="T12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="U12" t="n" s="2">
         <v>43218.0</v>
       </c>
       <c r="V12" t="n">
-        <v>206.0</v>
+        <v>207.0</v>
       </c>
     </row>
     <row r="13">
@@ -1289,22 +1289,22 @@
         <v>12.0</v>
       </c>
       <c r="D13" t="n">
-        <v>4404.0</v>
+        <v>4244.0</v>
       </c>
       <c r="E13" t="n">
         <v>4521.0</v>
       </c>
       <c r="F13" t="n">
-        <v>4694.0</v>
+        <v>4697.0</v>
       </c>
       <c r="G13" t="n">
-        <v>5094.0</v>
+        <v>5103.0</v>
       </c>
       <c r="H13" t="n">
-        <v>10870.0</v>
+        <v>10883.0</v>
       </c>
       <c r="I13" t="n">
-        <v>2095.0</v>
+        <v>2097.0</v>
       </c>
       <c r="J13" t="n">
         <v>1860.0</v>
@@ -1322,13 +1322,13 @@
         <v>123</v>
       </c>
       <c r="O13" t="n">
-        <v>297.0</v>
+        <v>634.0</v>
       </c>
       <c r="P13" t="n">
-        <v>160.0</v>
+        <v>320.0</v>
       </c>
       <c r="Q13" t="n">
-        <v>54932.0</v>
+        <v>55269.0</v>
       </c>
       <c r="R13" t="n">
         <v>31.0</v>
@@ -1337,13 +1337,13 @@
         <v>86170.0</v>
       </c>
       <c r="T13" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="U13" t="n" s="2">
         <v>43390.0</v>
       </c>
       <c r="V13" t="n">
-        <v>34.0</v>
+        <v>35.0</v>
       </c>
     </row>
     <row r="14">
@@ -1369,7 +1369,7 @@
         <v>1708.0</v>
       </c>
       <c r="H14" t="n">
-        <v>6618.0</v>
+        <v>6619.0</v>
       </c>
       <c r="I14" t="n">
         <v>1410.0</v>
@@ -1390,13 +1390,13 @@
         <v>123</v>
       </c>
       <c r="O14" t="n">
-        <v>64.0</v>
+        <v>86.0</v>
       </c>
       <c r="P14" t="n">
-        <v>80.0</v>
+        <v>160.0</v>
       </c>
       <c r="Q14" t="n">
-        <v>44186.0</v>
+        <v>44208.0</v>
       </c>
       <c r="R14" t="n">
         <v>35.0</v>
@@ -1411,7 +1411,7 @@
         <v>43410.0</v>
       </c>
       <c r="V14" t="n">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="15">
@@ -1425,22 +1425,22 @@
         <v>11.0</v>
       </c>
       <c r="D15" t="n">
-        <v>4184.0</v>
+        <v>4286.0</v>
       </c>
       <c r="E15" t="n">
         <v>4416.0</v>
       </c>
       <c r="F15" t="n">
-        <v>2292.0</v>
+        <v>2304.0</v>
       </c>
       <c r="G15" t="n">
-        <v>2093.0</v>
+        <v>2102.0</v>
       </c>
       <c r="H15" t="n">
-        <v>6752.0</v>
+        <v>6773.0</v>
       </c>
       <c r="I15" t="n">
-        <v>1086.0</v>
+        <v>1088.0</v>
       </c>
       <c r="J15" t="n">
         <v>3654.0</v>
@@ -1461,7 +1461,7 @@
         <v>0.0</v>
       </c>
       <c r="P15" t="n">
-        <v>80.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q15" t="n">
         <v>20621.0</v>
@@ -1479,7 +1479,7 @@
         <v>43275.0</v>
       </c>
       <c r="V15" t="n">
-        <v>149.0</v>
+        <v>150.0</v>
       </c>
     </row>
     <row r="16">
@@ -1505,10 +1505,10 @@
         <v>1463.0</v>
       </c>
       <c r="H16" t="n">
-        <v>3663.0</v>
+        <v>3674.0</v>
       </c>
       <c r="I16" t="n">
-        <v>1007.0</v>
+        <v>1010.0</v>
       </c>
       <c r="J16" t="n">
         <v>2616.0</v>
@@ -1526,13 +1526,13 @@
         <v>122</v>
       </c>
       <c r="O16" t="n">
-        <v>241.0</v>
+        <v>285.0</v>
       </c>
       <c r="P16" t="n">
-        <v>120.0</v>
+        <v>200.0</v>
       </c>
       <c r="Q16" t="n">
-        <v>31438.0</v>
+        <v>31482.0</v>
       </c>
       <c r="R16" t="n">
         <v>17.0</v>
@@ -1547,7 +1547,7 @@
         <v>43220.0</v>
       </c>
       <c r="V16" t="n">
-        <v>204.0</v>
+        <v>205.0</v>
       </c>
     </row>
     <row r="17">
@@ -1594,13 +1594,13 @@
         <v>123</v>
       </c>
       <c r="O17" t="n">
-        <v>26.0</v>
+        <v>42.0</v>
       </c>
       <c r="P17" t="n">
-        <v>40.0</v>
+        <v>115.0</v>
       </c>
       <c r="Q17" t="n">
-        <v>27691.0</v>
+        <v>27707.0</v>
       </c>
       <c r="R17" t="n">
         <v>3.0</v>
@@ -1615,7 +1615,7 @@
         <v>43419.0</v>
       </c>
       <c r="V17" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="18">
@@ -1629,22 +1629,22 @@
         <v>11.0</v>
       </c>
       <c r="D18" t="n">
-        <v>4356.0</v>
+        <v>4344.0</v>
       </c>
       <c r="E18" t="n">
         <v>4577.0</v>
       </c>
       <c r="F18" t="n">
-        <v>2827.0</v>
+        <v>2834.0</v>
       </c>
       <c r="G18" t="n">
-        <v>2581.0</v>
+        <v>2589.0</v>
       </c>
       <c r="H18" t="n">
-        <v>6708.0</v>
+        <v>6724.0</v>
       </c>
       <c r="I18" t="n">
-        <v>724.0</v>
+        <v>727.0</v>
       </c>
       <c r="J18" t="n">
         <v>3615.0</v>
@@ -1662,13 +1662,13 @@
         <v>122</v>
       </c>
       <c r="O18" t="n">
-        <v>63.0</v>
+        <v>71.0</v>
       </c>
       <c r="P18" t="n">
-        <v>120.0</v>
+        <v>200.0</v>
       </c>
       <c r="Q18" t="n">
-        <v>22016.0</v>
+        <v>22024.0</v>
       </c>
       <c r="R18" t="n">
         <v>51.0</v>
@@ -1683,7 +1683,7 @@
         <v>43058.0</v>
       </c>
       <c r="V18" t="n">
-        <v>366.0</v>
+        <v>367.0</v>
       </c>
     </row>
     <row r="19">
@@ -1697,22 +1697,22 @@
         <v>12.0</v>
       </c>
       <c r="D19" t="n">
-        <v>4454.0</v>
+        <v>4375.0</v>
       </c>
       <c r="E19" t="n">
         <v>4512.0</v>
       </c>
       <c r="F19" t="n">
-        <v>3024.0</v>
+        <v>3026.0</v>
       </c>
       <c r="G19" t="n">
-        <v>2906.0</v>
+        <v>2911.0</v>
       </c>
       <c r="H19" t="n">
-        <v>6899.0</v>
+        <v>6908.0</v>
       </c>
       <c r="I19" t="n">
-        <v>1255.0</v>
+        <v>1256.0</v>
       </c>
       <c r="J19" t="n">
         <v>2122.0</v>
@@ -1730,19 +1730,19 @@
         <v>122</v>
       </c>
       <c r="O19" t="n">
-        <v>128.0</v>
+        <v>269.0</v>
       </c>
       <c r="P19" t="n">
-        <v>160.0</v>
+        <v>240.0</v>
       </c>
       <c r="Q19" t="n">
-        <v>46504.0</v>
+        <v>46645.0</v>
       </c>
       <c r="R19" t="n">
         <v>36.0</v>
       </c>
       <c r="S19" t="n">
-        <v>53675.0</v>
+        <v>54235.0</v>
       </c>
       <c r="T19" t="s">
         <v>126</v>
@@ -1751,7 +1751,7 @@
         <v>43312.0</v>
       </c>
       <c r="V19" t="n">
-        <v>112.0</v>
+        <v>113.0</v>
       </c>
     </row>
     <row r="20">
@@ -1777,7 +1777,7 @@
         <v>1692.0</v>
       </c>
       <c r="H20" t="n">
-        <v>4304.0</v>
+        <v>4305.0</v>
       </c>
       <c r="I20" t="n">
         <v>621.0</v>
@@ -1798,13 +1798,13 @@
         <v>123</v>
       </c>
       <c r="O20" t="n">
-        <v>116.0</v>
+        <v>235.0</v>
       </c>
       <c r="P20" t="n">
-        <v>40.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q20" t="n">
-        <v>12129.0</v>
+        <v>12248.0</v>
       </c>
       <c r="R20" t="n">
         <v>18.0</v>
@@ -1819,7 +1819,7 @@
         <v>43421.0</v>
       </c>
       <c r="V20" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="21">
@@ -1833,22 +1833,22 @@
         <v>12.0</v>
       </c>
       <c r="D21" t="n">
-        <v>4629.0</v>
+        <v>4659.0</v>
       </c>
       <c r="E21" t="n">
         <v>4767.0</v>
       </c>
       <c r="F21" t="n">
-        <v>6761.0</v>
+        <v>6764.0</v>
       </c>
       <c r="G21" t="n">
-        <v>6689.0</v>
+        <v>6691.0</v>
       </c>
       <c r="H21" t="n">
-        <v>23963.0</v>
+        <v>23991.0</v>
       </c>
       <c r="I21" t="n">
-        <v>2799.0</v>
+        <v>2804.0</v>
       </c>
       <c r="J21" t="n">
         <v>2628.0</v>
@@ -1860,25 +1860,25 @@
         <v>433.0</v>
       </c>
       <c r="M21" t="n">
-        <v>2598.0</v>
+        <v>2608.0</v>
       </c>
       <c r="N21" t="s">
         <v>125</v>
       </c>
       <c r="O21" t="n">
-        <v>179.0</v>
+        <v>329.0</v>
       </c>
       <c r="P21" t="n">
-        <v>170.0</v>
+        <v>320.0</v>
       </c>
       <c r="Q21" t="n">
-        <v>68794.0</v>
+        <v>68944.0</v>
       </c>
       <c r="R21" t="n">
         <v>93.0</v>
       </c>
       <c r="S21" t="n">
-        <v>88615.0</v>
+        <v>89735.0</v>
       </c>
       <c r="T21" t="s">
         <v>130</v>
@@ -1887,7 +1887,7 @@
         <v>42705.0</v>
       </c>
       <c r="V21" t="n">
-        <v>719.0</v>
+        <v>720.0</v>
       </c>
     </row>
     <row r="22">
@@ -1901,7 +1901,7 @@
         <v>11.0</v>
       </c>
       <c r="D22" t="n">
-        <v>2959.0</v>
+        <v>2935.0</v>
       </c>
       <c r="E22" t="n">
         <v>3176.0</v>
@@ -1910,10 +1910,10 @@
         <v>3275.0</v>
       </c>
       <c r="G22" t="n">
-        <v>4557.0</v>
+        <v>4558.0</v>
       </c>
       <c r="H22" t="n">
-        <v>9147.0</v>
+        <v>9148.0</v>
       </c>
       <c r="I22" t="n">
         <v>2940.0</v>
@@ -1934,13 +1934,13 @@
         <v>123</v>
       </c>
       <c r="O22" t="n">
-        <v>30.0</v>
+        <v>36.0</v>
       </c>
       <c r="P22" t="n">
-        <v>30.0</v>
+        <v>60.0</v>
       </c>
       <c r="Q22" t="n">
-        <v>38155.0</v>
+        <v>38161.0</v>
       </c>
       <c r="R22" t="n">
         <v>27.0</v>
@@ -1955,7 +1955,7 @@
         <v>43151.0</v>
       </c>
       <c r="V22" t="n">
-        <v>273.0</v>
+        <v>274.0</v>
       </c>
     </row>
     <row r="23">
@@ -2002,13 +2002,13 @@
         <v>123</v>
       </c>
       <c r="O23" t="n">
-        <v>56.0</v>
+        <v>66.0</v>
       </c>
       <c r="P23" t="n">
-        <v>40.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q23" t="n">
-        <v>22115.0</v>
+        <v>22125.0</v>
       </c>
       <c r="R23" t="n">
         <v>28.0</v>
@@ -2023,7 +2023,7 @@
         <v>43254.0</v>
       </c>
       <c r="V23" t="n">
-        <v>170.0</v>
+        <v>171.0</v>
       </c>
     </row>
     <row r="24">
@@ -2037,19 +2037,19 @@
         <v>11.0</v>
       </c>
       <c r="D24" t="n">
-        <v>4275.0</v>
+        <v>4305.0</v>
       </c>
       <c r="E24" t="n">
         <v>4345.0</v>
       </c>
       <c r="F24" t="n">
-        <v>1892.0</v>
+        <v>1893.0</v>
       </c>
       <c r="G24" t="n">
         <v>1799.0</v>
       </c>
       <c r="H24" t="n">
-        <v>7984.0</v>
+        <v>7985.0</v>
       </c>
       <c r="I24" t="n">
         <v>2052.0</v>
@@ -2070,13 +2070,13 @@
         <v>123</v>
       </c>
       <c r="O24" t="n">
-        <v>36.0</v>
+        <v>54.0</v>
       </c>
       <c r="P24" t="n">
-        <v>40.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q24" t="n">
-        <v>55808.0</v>
+        <v>55826.0</v>
       </c>
       <c r="R24" t="n">
         <v>29.0</v>
@@ -2085,13 +2085,13 @@
         <v>64580.0</v>
       </c>
       <c r="T24" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="U24" t="n" s="2">
         <v>43380.0</v>
       </c>
       <c r="V24" t="n">
-        <v>44.0</v>
+        <v>45.0</v>
       </c>
     </row>
     <row r="25">
@@ -2117,10 +2117,10 @@
         <v>4367.0</v>
       </c>
       <c r="H25" t="n">
-        <v>18642.0</v>
+        <v>18655.0</v>
       </c>
       <c r="I25" t="n">
-        <v>2957.0</v>
+        <v>2961.0</v>
       </c>
       <c r="J25" t="n">
         <v>2743.0</v>
@@ -2132,19 +2132,19 @@
         <v>2641.0</v>
       </c>
       <c r="M25" t="n">
-        <v>16115.0</v>
+        <v>16145.0</v>
       </c>
       <c r="N25" t="s">
         <v>124</v>
       </c>
       <c r="O25" t="n">
-        <v>18.0</v>
+        <v>32.0</v>
       </c>
       <c r="P25" t="n">
-        <v>160.0</v>
+        <v>320.0</v>
       </c>
       <c r="Q25" t="n">
-        <v>6455.0</v>
+        <v>6469.0</v>
       </c>
       <c r="R25" t="n">
         <v>80.0</v>
@@ -2159,7 +2159,7 @@
         <v>42614.0</v>
       </c>
       <c r="V25" t="n">
-        <v>810.0</v>
+        <v>811.0</v>
       </c>
     </row>
     <row r="26">
@@ -2185,7 +2185,7 @@
         <v>1388.0</v>
       </c>
       <c r="H26" t="n">
-        <v>3971.0</v>
+        <v>3973.0</v>
       </c>
       <c r="I26" t="n">
         <v>648.0</v>
@@ -2227,7 +2227,7 @@
         <v>43400.0</v>
       </c>
       <c r="V26" t="n">
-        <v>24.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="27">
@@ -2253,10 +2253,10 @@
         <v>3517.0</v>
       </c>
       <c r="H27" t="n">
-        <v>12401.0</v>
+        <v>12407.0</v>
       </c>
       <c r="I27" t="n">
-        <v>1722.0</v>
+        <v>1723.0</v>
       </c>
       <c r="J27" t="n">
         <v>2774.0</v>
@@ -2274,13 +2274,13 @@
         <v>122</v>
       </c>
       <c r="O27" t="n">
-        <v>214.0</v>
+        <v>324.0</v>
       </c>
       <c r="P27" t="n">
-        <v>120.0</v>
+        <v>200.0</v>
       </c>
       <c r="Q27" t="n">
-        <v>43523.0</v>
+        <v>43633.0</v>
       </c>
       <c r="R27" t="n">
         <v>69.0</v>
@@ -2295,7 +2295,7 @@
         <v>43214.0</v>
       </c>
       <c r="V27" t="n">
-        <v>210.0</v>
+        <v>211.0</v>
       </c>
     </row>
     <row r="28">
@@ -2321,7 +2321,7 @@
         <v>3449.0</v>
       </c>
       <c r="H28" t="n">
-        <v>11451.0</v>
+        <v>11457.0</v>
       </c>
       <c r="I28" t="n">
         <v>1560.0</v>
@@ -2342,13 +2342,13 @@
         <v>124</v>
       </c>
       <c r="O28" t="n">
-        <v>55.0</v>
+        <v>75.0</v>
       </c>
       <c r="P28" t="n">
-        <v>40.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q28" t="n">
-        <v>32839.0</v>
+        <v>32859.0</v>
       </c>
       <c r="R28" t="n">
         <v>65.0</v>
@@ -2363,7 +2363,7 @@
         <v>42614.0</v>
       </c>
       <c r="V28" t="n">
-        <v>810.0</v>
+        <v>811.0</v>
       </c>
     </row>
     <row r="29">
@@ -2431,7 +2431,7 @@
         <v>43423.0</v>
       </c>
       <c r="V29" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="30">
@@ -2499,7 +2499,7 @@
         <v>43254.0</v>
       </c>
       <c r="V30" t="n">
-        <v>170.0</v>
+        <v>171.0</v>
       </c>
     </row>
     <row r="31">
@@ -2513,22 +2513,22 @@
         <v>11.0</v>
       </c>
       <c r="D31" t="n">
-        <v>4055.0</v>
+        <v>4202.0</v>
       </c>
       <c r="E31" t="n">
         <v>4258.0</v>
       </c>
       <c r="F31" t="n">
-        <v>1358.0</v>
+        <v>1370.0</v>
       </c>
       <c r="G31" t="n">
-        <v>1125.0</v>
+        <v>1133.0</v>
       </c>
       <c r="H31" t="n">
-        <v>6692.0</v>
+        <v>6725.0</v>
       </c>
       <c r="I31" t="n">
-        <v>1468.0</v>
+        <v>1473.0</v>
       </c>
       <c r="J31" t="n">
         <v>1864.0</v>
@@ -2546,19 +2546,19 @@
         <v>122</v>
       </c>
       <c r="O31" t="n">
-        <v>176.0</v>
+        <v>346.0</v>
       </c>
       <c r="P31" t="n">
-        <v>160.0</v>
+        <v>290.0</v>
       </c>
       <c r="Q31" t="n">
-        <v>13658.0</v>
+        <v>13828.0</v>
       </c>
       <c r="R31" t="n">
         <v>60.0</v>
       </c>
       <c r="S31" t="n">
-        <v>79862.0</v>
+        <v>80982.0</v>
       </c>
       <c r="T31" t="s">
         <v>128</v>
@@ -2567,7 +2567,7 @@
         <v>43058.0</v>
       </c>
       <c r="V31" t="n">
-        <v>366.0</v>
+        <v>367.0</v>
       </c>
     </row>
     <row r="32">
@@ -2581,22 +2581,22 @@
         <v>10.0</v>
       </c>
       <c r="D32" t="n">
-        <v>3941.0</v>
+        <v>4150.0</v>
       </c>
       <c r="E32" t="n">
-        <v>4006.0</v>
+        <v>4177.0</v>
       </c>
       <c r="F32" t="n">
-        <v>673.0</v>
+        <v>692.0</v>
       </c>
       <c r="G32" t="n">
-        <v>543.0</v>
+        <v>557.0</v>
       </c>
       <c r="H32" t="n">
-        <v>3422.0</v>
+        <v>3457.0</v>
       </c>
       <c r="I32" t="n">
-        <v>753.0</v>
+        <v>757.0</v>
       </c>
       <c r="J32" t="n">
         <v>838.0</v>
@@ -2614,13 +2614,13 @@
         <v>122</v>
       </c>
       <c r="O32" t="n">
-        <v>40.0</v>
+        <v>54.0</v>
       </c>
       <c r="P32" t="n">
-        <v>120.0</v>
+        <v>190.0</v>
       </c>
       <c r="Q32" t="n">
-        <v>4731.0</v>
+        <v>4745.0</v>
       </c>
       <c r="R32" t="n">
         <v>53.0</v>
@@ -2629,13 +2629,13 @@
         <v>74187.0</v>
       </c>
       <c r="T32" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="U32" t="n" s="2">
         <v>43138.0</v>
       </c>
       <c r="V32" t="n">
-        <v>286.0</v>
+        <v>287.0</v>
       </c>
     </row>
     <row r="33">
@@ -2649,19 +2649,19 @@
         <v>12.0</v>
       </c>
       <c r="D33" t="n">
-        <v>4081.0</v>
+        <v>4030.0</v>
       </c>
       <c r="E33" t="n">
         <v>4190.0</v>
       </c>
       <c r="F33" t="n">
-        <v>2164.0</v>
+        <v>2165.0</v>
       </c>
       <c r="G33" t="n">
-        <v>2209.0</v>
+        <v>2212.0</v>
       </c>
       <c r="H33" t="n">
-        <v>7022.0</v>
+        <v>7028.0</v>
       </c>
       <c r="I33" t="n">
         <v>1583.0</v>
@@ -2682,19 +2682,19 @@
         <v>122</v>
       </c>
       <c r="O33" t="n">
-        <v>109.0</v>
+        <v>173.0</v>
       </c>
       <c r="P33" t="n">
-        <v>120.0</v>
+        <v>200.0</v>
       </c>
       <c r="Q33" t="n">
-        <v>43410.0</v>
+        <v>43474.0</v>
       </c>
       <c r="R33" t="n">
         <v>38.0</v>
       </c>
       <c r="S33" t="n">
-        <v>75873.0</v>
+        <v>76433.0</v>
       </c>
       <c r="T33" t="s">
         <v>128</v>
@@ -2703,7 +2703,7 @@
         <v>42920.0</v>
       </c>
       <c r="V33" t="n">
-        <v>504.0</v>
+        <v>505.0</v>
       </c>
     </row>
     <row r="34">
@@ -2717,22 +2717,22 @@
         <v>12.0</v>
       </c>
       <c r="D34" t="n">
-        <v>4624.0</v>
+        <v>4581.0</v>
       </c>
       <c r="E34" t="n">
         <v>4798.0</v>
       </c>
       <c r="F34" t="n">
-        <v>5203.0</v>
+        <v>5210.0</v>
       </c>
       <c r="G34" t="n">
-        <v>5301.0</v>
+        <v>5310.0</v>
       </c>
       <c r="H34" t="n">
-        <v>12455.0</v>
+        <v>12471.0</v>
       </c>
       <c r="I34" t="n">
-        <v>2266.0</v>
+        <v>2268.0</v>
       </c>
       <c r="J34" t="n">
         <v>1752.0</v>
@@ -2750,13 +2750,13 @@
         <v>122</v>
       </c>
       <c r="O34" t="n">
-        <v>0.0</v>
+        <v>16.0</v>
       </c>
       <c r="P34" t="n">
-        <v>0.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q34" t="n">
-        <v>59317.0</v>
+        <v>59333.0</v>
       </c>
       <c r="R34" t="n">
         <v>30.0</v>
@@ -2765,13 +2765,13 @@
         <v>81030.0</v>
       </c>
       <c r="T34" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="U34" t="n" s="2">
         <v>43058.0</v>
       </c>
       <c r="V34" t="n">
-        <v>366.0</v>
+        <v>367.0</v>
       </c>
     </row>
     <row r="35">
@@ -2785,7 +2785,7 @@
         <v>10.0</v>
       </c>
       <c r="D35" t="n">
-        <v>3922.0</v>
+        <v>3895.0</v>
       </c>
       <c r="E35" t="n">
         <v>4021.0</v>
@@ -2794,13 +2794,13 @@
         <v>960.0</v>
       </c>
       <c r="G35" t="n">
-        <v>978.0</v>
+        <v>979.0</v>
       </c>
       <c r="H35" t="n">
-        <v>4258.0</v>
+        <v>4264.0</v>
       </c>
       <c r="I35" t="n">
-        <v>1000.0</v>
+        <v>1001.0</v>
       </c>
       <c r="J35" t="n">
         <v>290.0</v>
@@ -2818,13 +2818,13 @@
         <v>123</v>
       </c>
       <c r="O35" t="n">
-        <v>10.0</v>
+        <v>20.0</v>
       </c>
       <c r="P35" t="n">
-        <v>80.0</v>
+        <v>90.0</v>
       </c>
       <c r="Q35" t="n">
-        <v>8499.0</v>
+        <v>8509.0</v>
       </c>
       <c r="R35" t="n">
         <v>30.0</v>
@@ -2839,7 +2839,7 @@
         <v>43312.0</v>
       </c>
       <c r="V35" t="n">
-        <v>112.0</v>
+        <v>113.0</v>
       </c>
     </row>
     <row r="36">
@@ -2853,22 +2853,22 @@
         <v>10.0</v>
       </c>
       <c r="D36" t="n">
-        <v>3866.0</v>
+        <v>3774.0</v>
       </c>
       <c r="E36" t="n">
         <v>4007.0</v>
       </c>
       <c r="F36" t="n">
-        <v>571.0</v>
+        <v>574.0</v>
       </c>
       <c r="G36" t="n">
-        <v>508.0</v>
+        <v>515.0</v>
       </c>
       <c r="H36" t="n">
-        <v>3455.0</v>
+        <v>3481.0</v>
       </c>
       <c r="I36" t="n">
-        <v>719.0</v>
+        <v>720.0</v>
       </c>
       <c r="J36" t="n">
         <v>286.0</v>
@@ -2886,28 +2886,28 @@
         <v>123</v>
       </c>
       <c r="O36" t="n">
-        <v>44.0</v>
+        <v>105.0</v>
       </c>
       <c r="P36" t="n">
-        <v>160.0</v>
+        <v>280.0</v>
       </c>
       <c r="Q36" t="n">
-        <v>17507.0</v>
+        <v>17568.0</v>
       </c>
       <c r="R36" t="n">
         <v>26.0</v>
       </c>
       <c r="S36" t="n">
-        <v>65900.0</v>
+        <v>66686.0</v>
       </c>
       <c r="T36" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="U36" t="n" s="2">
         <v>43274.0</v>
       </c>
       <c r="V36" t="n">
-        <v>150.0</v>
+        <v>151.0</v>
       </c>
     </row>
     <row r="37">
@@ -2921,22 +2921,22 @@
         <v>10.0</v>
       </c>
       <c r="D37" t="n">
-        <v>3897.0</v>
+        <v>3971.0</v>
       </c>
       <c r="E37" t="n">
         <v>4135.0</v>
       </c>
       <c r="F37" t="n">
-        <v>3555.0</v>
+        <v>3564.0</v>
       </c>
       <c r="G37" t="n">
-        <v>4124.0</v>
+        <v>4131.0</v>
       </c>
       <c r="H37" t="n">
-        <v>9799.0</v>
+        <v>9819.0</v>
       </c>
       <c r="I37" t="n">
-        <v>1788.0</v>
+        <v>1791.0</v>
       </c>
       <c r="J37" t="n">
         <v>227.0</v>
@@ -2954,19 +2954,19 @@
         <v>122</v>
       </c>
       <c r="O37" t="n">
-        <v>85.0</v>
+        <v>118.0</v>
       </c>
       <c r="P37" t="n">
-        <v>120.0</v>
+        <v>200.0</v>
       </c>
       <c r="Q37" t="n">
-        <v>14910.0</v>
+        <v>14943.0</v>
       </c>
       <c r="R37" t="n">
         <v>37.0</v>
       </c>
       <c r="S37" t="n">
-        <v>74068.0</v>
+        <v>75118.0</v>
       </c>
       <c r="T37" t="s">
         <v>127</v>
@@ -2975,7 +2975,7 @@
         <v>43280.0</v>
       </c>
       <c r="V37" t="n">
-        <v>144.0</v>
+        <v>145.0</v>
       </c>
     </row>
     <row r="38">
@@ -3001,10 +3001,10 @@
         <v>188.0</v>
       </c>
       <c r="H38" t="n">
-        <v>643.0</v>
+        <v>653.0</v>
       </c>
       <c r="I38" t="n">
-        <v>116.0</v>
+        <v>119.0</v>
       </c>
       <c r="J38" t="n">
         <v>516.0</v>
@@ -3022,13 +3022,13 @@
         <v>123</v>
       </c>
       <c r="O38" t="n">
-        <v>104.0</v>
+        <v>134.0</v>
       </c>
       <c r="P38" t="n">
-        <v>120.0</v>
+        <v>200.0</v>
       </c>
       <c r="Q38" t="n">
-        <v>2917.0</v>
+        <v>2947.0</v>
       </c>
       <c r="R38" t="n">
         <v>2.0</v>
@@ -3043,7 +3043,7 @@
         <v>43360.0</v>
       </c>
       <c r="V38" t="n">
-        <v>64.0</v>
+        <v>65.0</v>
       </c>
     </row>
     <row r="39">
@@ -3111,7 +3111,7 @@
         <v>43284.0</v>
       </c>
       <c r="V39" t="n">
-        <v>140.0</v>
+        <v>141.0</v>
       </c>
     </row>
     <row r="40">
@@ -3125,22 +3125,22 @@
         <v>10.0</v>
       </c>
       <c r="D40" t="n">
-        <v>4066.0</v>
+        <v>4152.0</v>
       </c>
       <c r="E40" t="n">
         <v>4405.0</v>
       </c>
       <c r="F40" t="n">
-        <v>1097.0</v>
+        <v>1100.0</v>
       </c>
       <c r="G40" t="n">
         <v>1001.0</v>
       </c>
       <c r="H40" t="n">
-        <v>3156.0</v>
+        <v>3160.0</v>
       </c>
       <c r="I40" t="n">
-        <v>660.0</v>
+        <v>663.0</v>
       </c>
       <c r="J40" t="n">
         <v>1700.0</v>
@@ -3158,13 +3158,13 @@
         <v>123</v>
       </c>
       <c r="O40" t="n">
-        <v>46.0</v>
+        <v>130.0</v>
       </c>
       <c r="P40" t="n">
-        <v>120.0</v>
+        <v>200.0</v>
       </c>
       <c r="Q40" t="n">
-        <v>20412.0</v>
+        <v>20496.0</v>
       </c>
       <c r="R40" t="n">
         <v>18.0</v>
@@ -3179,7 +3179,7 @@
         <v>43352.0</v>
       </c>
       <c r="V40" t="n">
-        <v>72.0</v>
+        <v>73.0</v>
       </c>
     </row>
     <row r="41">
@@ -3205,10 +3205,10 @@
         <v>4736.0</v>
       </c>
       <c r="H41" t="n">
-        <v>27044.0</v>
+        <v>27058.0</v>
       </c>
       <c r="I41" t="n">
-        <v>3683.0</v>
+        <v>3686.0</v>
       </c>
       <c r="J41" t="n">
         <v>2014.0</v>
@@ -3226,13 +3226,13 @@
         <v>122</v>
       </c>
       <c r="O41" t="n">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="P41" t="n">
-        <v>80.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q41" t="n">
-        <v>7122.0</v>
+        <v>7130.0</v>
       </c>
       <c r="R41" t="n">
         <v>62.0</v>
@@ -3247,7 +3247,7 @@
         <v>43252.0</v>
       </c>
       <c r="V41" t="n">
-        <v>172.0</v>
+        <v>173.0</v>
       </c>
     </row>
     <row r="42">
@@ -3261,7 +3261,7 @@
         <v>11.0</v>
       </c>
       <c r="D42" t="n">
-        <v>4146.0</v>
+        <v>4119.0</v>
       </c>
       <c r="E42" t="n">
         <v>4323.0</v>
@@ -3270,13 +3270,13 @@
         <v>2434.0</v>
       </c>
       <c r="G42" t="n">
-        <v>2359.0</v>
+        <v>2360.0</v>
       </c>
       <c r="H42" t="n">
-        <v>6139.0</v>
+        <v>6142.0</v>
       </c>
       <c r="I42" t="n">
-        <v>1192.0</v>
+        <v>1193.0</v>
       </c>
       <c r="J42" t="n">
         <v>2822.0</v>
@@ -3294,19 +3294,19 @@
         <v>123</v>
       </c>
       <c r="O42" t="n">
-        <v>106.0</v>
+        <v>157.0</v>
       </c>
       <c r="P42" t="n">
-        <v>80.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q42" t="n">
-        <v>22368.0</v>
+        <v>22419.0</v>
       </c>
       <c r="R42" t="n">
         <v>20.0</v>
       </c>
       <c r="S42" t="n">
-        <v>35972.0</v>
+        <v>37372.0</v>
       </c>
       <c r="T42" t="s">
         <v>128</v>
@@ -3315,7 +3315,7 @@
         <v>43370.0</v>
       </c>
       <c r="V42" t="n">
-        <v>54.0</v>
+        <v>55.0</v>
       </c>
     </row>
     <row r="43">
@@ -3329,22 +3329,22 @@
         <v>11.0</v>
       </c>
       <c r="D43" t="n">
-        <v>3964.0</v>
+        <v>3948.0</v>
       </c>
       <c r="E43" t="n">
-        <v>3965.0</v>
+        <v>3993.0</v>
       </c>
       <c r="F43" t="n">
-        <v>1275.0</v>
+        <v>1287.0</v>
       </c>
       <c r="G43" t="n">
-        <v>1112.0</v>
+        <v>1126.0</v>
       </c>
       <c r="H43" t="n">
-        <v>4340.0</v>
+        <v>4372.0</v>
       </c>
       <c r="I43" t="n">
-        <v>743.0</v>
+        <v>746.0</v>
       </c>
       <c r="J43" t="n">
         <v>1917.0</v>
@@ -3362,19 +3362,19 @@
         <v>123</v>
       </c>
       <c r="O43" t="n">
-        <v>254.0</v>
+        <v>518.0</v>
       </c>
       <c r="P43" t="n">
-        <v>120.0</v>
+        <v>280.0</v>
       </c>
       <c r="Q43" t="n">
-        <v>28717.0</v>
+        <v>28981.0</v>
       </c>
       <c r="R43" t="n">
         <v>24.0</v>
       </c>
       <c r="S43" t="n">
-        <v>21634.0</v>
+        <v>22420.0</v>
       </c>
       <c r="T43" t="s">
         <v>127</v>
@@ -3383,7 +3383,7 @@
         <v>43419.0</v>
       </c>
       <c r="V43" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="44">
@@ -3451,7 +3451,7 @@
         <v>43382.0</v>
       </c>
       <c r="V44" t="n">
-        <v>42.0</v>
+        <v>43.0</v>
       </c>
     </row>
     <row r="45">
@@ -3465,22 +3465,22 @@
         <v>11.0</v>
       </c>
       <c r="D45" t="n">
-        <v>4248.0</v>
+        <v>4335.0</v>
       </c>
       <c r="E45" t="n">
         <v>4400.0</v>
       </c>
       <c r="F45" t="n">
-        <v>3846.0</v>
+        <v>3849.0</v>
       </c>
       <c r="G45" t="n">
         <v>4153.0</v>
       </c>
       <c r="H45" t="n">
-        <v>8755.0</v>
+        <v>8760.0</v>
       </c>
       <c r="I45" t="n">
-        <v>2049.0</v>
+        <v>2050.0</v>
       </c>
       <c r="J45" t="n">
         <v>1381.0</v>
@@ -3498,28 +3498,28 @@
         <v>123</v>
       </c>
       <c r="O45" t="n">
-        <v>30.0</v>
+        <v>132.0</v>
       </c>
       <c r="P45" t="n">
-        <v>40.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q45" t="n">
-        <v>22693.0</v>
+        <v>22795.0</v>
       </c>
       <c r="R45" t="n">
         <v>20.0</v>
       </c>
       <c r="S45" t="n">
-        <v>76772.0</v>
+        <v>77612.0</v>
       </c>
       <c r="T45" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="U45" t="n" s="2">
         <v>43390.0</v>
       </c>
       <c r="V45" t="n">
-        <v>34.0</v>
+        <v>35.0</v>
       </c>
     </row>
     <row r="46">
@@ -3533,22 +3533,22 @@
         <v>12.0</v>
       </c>
       <c r="D46" t="n">
-        <v>4149.0</v>
+        <v>4180.0</v>
       </c>
       <c r="E46" t="n">
         <v>4473.0</v>
       </c>
       <c r="F46" t="n">
-        <v>2638.0</v>
+        <v>2641.0</v>
       </c>
       <c r="G46" t="n">
-        <v>2585.0</v>
+        <v>2587.0</v>
       </c>
       <c r="H46" t="n">
-        <v>7234.0</v>
+        <v>7242.0</v>
       </c>
       <c r="I46" t="n">
-        <v>1385.0</v>
+        <v>1388.0</v>
       </c>
       <c r="J46" t="n">
         <v>3505.0</v>
@@ -3566,13 +3566,13 @@
         <v>123</v>
       </c>
       <c r="O46" t="n">
-        <v>26.0</v>
+        <v>228.0</v>
       </c>
       <c r="P46" t="n">
-        <v>80.0</v>
+        <v>200.0</v>
       </c>
       <c r="Q46" t="n">
-        <v>49927.0</v>
+        <v>50129.0</v>
       </c>
       <c r="R46" t="n">
         <v>36.0</v>
@@ -3587,7 +3587,7 @@
         <v>43390.0</v>
       </c>
       <c r="V46" t="n">
-        <v>34.0</v>
+        <v>35.0</v>
       </c>
     </row>
     <row r="47">
@@ -3655,7 +3655,7 @@
         <v>43376.0</v>
       </c>
       <c r="V47" t="n">
-        <v>48.0</v>
+        <v>49.0</v>
       </c>
     </row>
     <row r="48">
@@ -3669,22 +3669,22 @@
         <v>12.0</v>
       </c>
       <c r="D48" t="n">
-        <v>4809.0</v>
+        <v>4771.0</v>
       </c>
       <c r="E48" t="n">
         <v>4919.0</v>
       </c>
       <c r="F48" t="n">
-        <v>11084.0</v>
+        <v>11115.0</v>
       </c>
       <c r="G48" t="n">
-        <v>11784.0</v>
+        <v>11817.0</v>
       </c>
       <c r="H48" t="n">
-        <v>26403.0</v>
+        <v>26471.0</v>
       </c>
       <c r="I48" t="n">
-        <v>9114.0</v>
+        <v>9137.0</v>
       </c>
       <c r="J48" t="n">
         <v>2228.0</v>
@@ -3702,13 +3702,13 @@
         <v>123</v>
       </c>
       <c r="O48" t="n">
-        <v>380.0</v>
+        <v>646.0</v>
       </c>
       <c r="P48" t="n">
-        <v>160.0</v>
+        <v>280.0</v>
       </c>
       <c r="Q48" t="n">
-        <v>77065.0</v>
+        <v>77351.0</v>
       </c>
       <c r="R48" t="n">
         <v>26.0</v>
@@ -3723,7 +3723,7 @@
         <v>43390.0</v>
       </c>
       <c r="V48" t="n">
-        <v>34.0</v>
+        <v>35.0</v>
       </c>
     </row>
     <row r="49">
@@ -3749,10 +3749,10 @@
         <v>3042.0</v>
       </c>
       <c r="H49" t="n">
-        <v>15673.0</v>
+        <v>15694.0</v>
       </c>
       <c r="I49" t="n">
-        <v>3296.0</v>
+        <v>3298.0</v>
       </c>
       <c r="J49" t="n">
         <v>1889.0</v>
@@ -3770,13 +3770,13 @@
         <v>122</v>
       </c>
       <c r="O49" t="n">
-        <v>159.0</v>
+        <v>233.0</v>
       </c>
       <c r="P49" t="n">
-        <v>120.0</v>
+        <v>200.0</v>
       </c>
       <c r="Q49" t="n">
-        <v>33686.0</v>
+        <v>33760.0</v>
       </c>
       <c r="R49" t="n">
         <v>40.0</v>
@@ -3791,7 +3791,7 @@
         <v>43230.0</v>
       </c>
       <c r="V49" t="n">
-        <v>194.0</v>
+        <v>195.0</v>
       </c>
     </row>
     <row r="50">
@@ -3805,19 +3805,19 @@
         <v>11.0</v>
       </c>
       <c r="D50" t="n">
-        <v>4343.0</v>
+        <v>4320.0</v>
       </c>
       <c r="E50" t="n">
         <v>4396.0</v>
       </c>
       <c r="F50" t="n">
-        <v>6396.0</v>
+        <v>6400.0</v>
       </c>
       <c r="G50" t="n">
-        <v>6628.0</v>
+        <v>6633.0</v>
       </c>
       <c r="H50" t="n">
-        <v>18338.0</v>
+        <v>18352.0</v>
       </c>
       <c r="I50" t="n">
         <v>3782.0</v>
@@ -3832,19 +3832,19 @@
         <v>47.0</v>
       </c>
       <c r="M50" t="n">
-        <v>467.0</v>
+        <v>475.0</v>
       </c>
       <c r="N50" t="s">
         <v>124</v>
       </c>
       <c r="O50" t="n">
-        <v>61.0</v>
+        <v>105.0</v>
       </c>
       <c r="P50" t="n">
-        <v>120.0</v>
+        <v>200.0</v>
       </c>
       <c r="Q50" t="n">
-        <v>20944.0</v>
+        <v>20988.0</v>
       </c>
       <c r="R50" t="n">
         <v>62.0</v>
@@ -3859,7 +3859,7 @@
         <v>43184.0</v>
       </c>
       <c r="V50" t="n">
-        <v>240.0</v>
+        <v>241.0</v>
       </c>
     </row>
     <row r="51">
@@ -3885,10 +3885,10 @@
         <v>6155.0</v>
       </c>
       <c r="H51" t="n">
-        <v>14065.0</v>
+        <v>14068.0</v>
       </c>
       <c r="I51" t="n">
-        <v>2664.0</v>
+        <v>2665.0</v>
       </c>
       <c r="J51" t="n">
         <v>6586.0</v>
@@ -3918,7 +3918,7 @@
         <v>30.0</v>
       </c>
       <c r="S51" t="n">
-        <v>44280.0</v>
+        <v>45400.0</v>
       </c>
       <c r="T51" t="s">
         <v>126</v>
@@ -3927,7 +3927,7 @@
         <v>43314.0</v>
       </c>
       <c r="V51" t="n">
-        <v>110.0</v>
+        <v>111.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Icon and background --> black
</commit_message>
<xml_diff>
--- a/docs/data/memberstats.xlsx
+++ b/docs/data/memberstats.xlsx
@@ -550,13 +550,13 @@
         <v>4653.0</v>
       </c>
       <c r="F2" t="n">
-        <v>2287.0</v>
+        <v>2293.0</v>
       </c>
       <c r="G2" t="n">
-        <v>2110.0</v>
+        <v>2111.0</v>
       </c>
       <c r="H2" t="n">
-        <v>7115.0</v>
+        <v>7120.0</v>
       </c>
       <c r="I2" t="n">
         <v>1160.0</v>
@@ -577,13 +577,13 @@
         <v>122</v>
       </c>
       <c r="O2" t="n">
-        <v>250.0</v>
+        <v>251.0</v>
       </c>
       <c r="P2" t="n">
         <v>360.0</v>
       </c>
       <c r="Q2" t="n">
-        <v>29123.0</v>
+        <v>29124.0</v>
       </c>
       <c r="R2" t="n">
         <v>46.0</v>
@@ -816,22 +816,22 @@
         <v>10.0</v>
       </c>
       <c r="D6" t="n">
-        <v>4086.0</v>
+        <v>4093.0</v>
       </c>
       <c r="E6" t="n">
         <v>4142.0</v>
       </c>
       <c r="F6" t="n">
-        <v>1259.0</v>
+        <v>1266.0</v>
       </c>
       <c r="G6" t="n">
-        <v>1290.0</v>
+        <v>1292.0</v>
       </c>
       <c r="H6" t="n">
-        <v>3287.0</v>
+        <v>3293.0</v>
       </c>
       <c r="I6" t="n">
-        <v>506.0</v>
+        <v>507.0</v>
       </c>
       <c r="J6" t="n">
         <v>310.0</v>
@@ -849,13 +849,13 @@
         <v>123</v>
       </c>
       <c r="O6" t="n">
-        <v>278.0</v>
+        <v>306.0</v>
       </c>
       <c r="P6" t="n">
-        <v>440.0</v>
+        <v>472.0</v>
       </c>
       <c r="Q6" t="n">
-        <v>17175.0</v>
+        <v>17203.0</v>
       </c>
       <c r="R6" t="n">
         <v>30.0</v>
@@ -890,13 +890,13 @@
         <v>4489.0</v>
       </c>
       <c r="F7" t="n">
-        <v>2990.0</v>
+        <v>2991.0</v>
       </c>
       <c r="G7" t="n">
-        <v>2671.0</v>
+        <v>2673.0</v>
       </c>
       <c r="H7" t="n">
-        <v>7079.0</v>
+        <v>7083.0</v>
       </c>
       <c r="I7" t="n">
         <v>691.0</v>
@@ -920,7 +920,7 @@
         <v>0.0</v>
       </c>
       <c r="P7" t="n">
-        <v>80.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q7" t="n">
         <v>2125.0</v>
@@ -952,22 +952,22 @@
         <v>11.0</v>
       </c>
       <c r="D8" t="n">
-        <v>4537.0</v>
+        <v>4482.0</v>
       </c>
       <c r="E8" t="n">
         <v>4537.0</v>
       </c>
       <c r="F8" t="n">
-        <v>1945.0</v>
+        <v>1949.0</v>
       </c>
       <c r="G8" t="n">
-        <v>1831.0</v>
+        <v>1833.0</v>
       </c>
       <c r="H8" t="n">
-        <v>7725.0</v>
+        <v>7737.0</v>
       </c>
       <c r="I8" t="n">
-        <v>1124.0</v>
+        <v>1126.0</v>
       </c>
       <c r="J8" t="n">
         <v>1396.0</v>
@@ -985,13 +985,13 @@
         <v>124</v>
       </c>
       <c r="O8" t="n">
-        <v>268.0</v>
+        <v>304.0</v>
       </c>
       <c r="P8" t="n">
-        <v>270.0</v>
+        <v>280.0</v>
       </c>
       <c r="Q8" t="n">
-        <v>25652.0</v>
+        <v>25688.0</v>
       </c>
       <c r="R8" t="n">
         <v>58.0</v>
@@ -1020,25 +1020,25 @@
         <v>11.0</v>
       </c>
       <c r="D9" t="n">
-        <v>4517.0</v>
+        <v>4468.0</v>
       </c>
       <c r="E9" t="n">
         <v>4634.0</v>
       </c>
       <c r="F9" t="n">
-        <v>2514.0</v>
+        <v>2523.0</v>
       </c>
       <c r="G9" t="n">
-        <v>2334.0</v>
+        <v>2345.0</v>
       </c>
       <c r="H9" t="n">
-        <v>10998.0</v>
+        <v>11022.0</v>
       </c>
       <c r="I9" t="n">
-        <v>2426.0</v>
+        <v>2428.0</v>
       </c>
       <c r="J9" t="n">
-        <v>1922.0</v>
+        <v>1925.0</v>
       </c>
       <c r="K9" t="n">
         <v>11.0</v>
@@ -1053,13 +1053,13 @@
         <v>124</v>
       </c>
       <c r="O9" t="n">
-        <v>57.0</v>
+        <v>67.0</v>
       </c>
       <c r="P9" t="n">
-        <v>440.0</v>
+        <v>480.0</v>
       </c>
       <c r="Q9" t="n">
-        <v>3413.0</v>
+        <v>3423.0</v>
       </c>
       <c r="R9" t="n">
         <v>59.0</v>
@@ -1088,19 +1088,19 @@
         <v>12.0</v>
       </c>
       <c r="D10" t="n">
-        <v>4478.0</v>
+        <v>4537.0</v>
       </c>
       <c r="E10" t="n">
         <v>4731.0</v>
       </c>
       <c r="F10" t="n">
-        <v>2270.0</v>
+        <v>2274.0</v>
       </c>
       <c r="G10" t="n">
-        <v>1761.0</v>
+        <v>1763.0</v>
       </c>
       <c r="H10" t="n">
-        <v>9607.0</v>
+        <v>9613.0</v>
       </c>
       <c r="I10" t="n">
         <v>1378.0</v>
@@ -1121,13 +1121,13 @@
         <v>123</v>
       </c>
       <c r="O10" t="n">
-        <v>824.0</v>
+        <v>924.0</v>
       </c>
       <c r="P10" t="n">
         <v>400.0</v>
       </c>
       <c r="Q10" t="n">
-        <v>92121.0</v>
+        <v>92221.0</v>
       </c>
       <c r="R10" t="n">
         <v>78.0</v>
@@ -1162,19 +1162,19 @@
         <v>4389.0</v>
       </c>
       <c r="F11" t="n">
-        <v>1398.0</v>
+        <v>1402.0</v>
       </c>
       <c r="G11" t="n">
-        <v>1232.0</v>
+        <v>1235.0</v>
       </c>
       <c r="H11" t="n">
-        <v>5698.0</v>
+        <v>5710.0</v>
       </c>
       <c r="I11" t="n">
-        <v>784.0</v>
+        <v>789.0</v>
       </c>
       <c r="J11" t="n">
-        <v>1235.0</v>
+        <v>1238.0</v>
       </c>
       <c r="K11" t="n">
         <v>9.0</v>
@@ -1189,13 +1189,13 @@
         <v>124</v>
       </c>
       <c r="O11" t="n">
-        <v>599.0</v>
+        <v>677.0</v>
       </c>
       <c r="P11" t="n">
-        <v>390.0</v>
+        <v>400.0</v>
       </c>
       <c r="Q11" t="n">
-        <v>39247.0</v>
+        <v>39325.0</v>
       </c>
       <c r="R11" t="n">
         <v>66.0</v>
@@ -1251,7 +1251,7 @@
         <v>4.0</v>
       </c>
       <c r="M12" t="n">
-        <v>22.0</v>
+        <v>26.0</v>
       </c>
       <c r="N12" t="s">
         <v>123</v>
@@ -1260,7 +1260,7 @@
         <v>1018.0</v>
       </c>
       <c r="P12" t="n">
-        <v>480.0</v>
+        <v>520.0</v>
       </c>
       <c r="Q12" t="n">
         <v>55653.0</v>
@@ -1360,22 +1360,22 @@
         <v>11.0</v>
       </c>
       <c r="D14" t="n">
-        <v>4238.0</v>
+        <v>4239.0</v>
       </c>
       <c r="E14" t="n">
         <v>4416.0</v>
       </c>
       <c r="F14" t="n">
-        <v>2315.0</v>
+        <v>2317.0</v>
       </c>
       <c r="G14" t="n">
-        <v>2107.0</v>
+        <v>2109.0</v>
       </c>
       <c r="H14" t="n">
-        <v>6789.0</v>
+        <v>6793.0</v>
       </c>
       <c r="I14" t="n">
-        <v>1090.0</v>
+        <v>1091.0</v>
       </c>
       <c r="J14" t="n">
         <v>3662.0</v>
@@ -1396,7 +1396,7 @@
         <v>0.0</v>
       </c>
       <c r="P14" t="n">
-        <v>280.0</v>
+        <v>310.0</v>
       </c>
       <c r="Q14" t="n">
         <v>20621.0</v>
@@ -1440,7 +1440,7 @@
         <v>1463.0</v>
       </c>
       <c r="H15" t="n">
-        <v>3676.0</v>
+        <v>3677.0</v>
       </c>
       <c r="I15" t="n">
         <v>1010.0</v>
@@ -1461,13 +1461,13 @@
         <v>122</v>
       </c>
       <c r="O15" t="n">
-        <v>305.0</v>
+        <v>345.0</v>
       </c>
       <c r="P15" t="n">
-        <v>320.0</v>
+        <v>360.0</v>
       </c>
       <c r="Q15" t="n">
-        <v>31502.0</v>
+        <v>31542.0</v>
       </c>
       <c r="R15" t="n">
         <v>18.0</v>
@@ -1570,13 +1570,13 @@
         <v>4577.0</v>
       </c>
       <c r="F17" t="n">
-        <v>2841.0</v>
+        <v>2843.0</v>
       </c>
       <c r="G17" t="n">
-        <v>2595.0</v>
+        <v>2596.0</v>
       </c>
       <c r="H17" t="n">
-        <v>6741.0</v>
+        <v>6744.0</v>
       </c>
       <c r="I17" t="n">
         <v>728.0</v>
@@ -1801,13 +1801,13 @@
         <v>125</v>
       </c>
       <c r="O20" t="n">
-        <v>581.0</v>
+        <v>635.0</v>
       </c>
       <c r="P20" t="n">
-        <v>520.0</v>
+        <v>560.0</v>
       </c>
       <c r="Q20" t="n">
-        <v>69196.0</v>
+        <v>69250.0</v>
       </c>
       <c r="R20" t="n">
         <v>93.0</v>
@@ -1904,7 +1904,7 @@
         <v>11.0</v>
       </c>
       <c r="D22" t="n">
-        <v>4000.0</v>
+        <v>3975.0</v>
       </c>
       <c r="E22" t="n">
         <v>4253.0</v>
@@ -1913,10 +1913,10 @@
         <v>1356.0</v>
       </c>
       <c r="G22" t="n">
-        <v>1420.0</v>
+        <v>1421.0</v>
       </c>
       <c r="H22" t="n">
-        <v>4639.0</v>
+        <v>4642.0</v>
       </c>
       <c r="I22" t="n">
         <v>886.0</v>
@@ -1952,7 +1952,7 @@
         <v>53231.0</v>
       </c>
       <c r="T22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="U22" t="n" s="2">
         <v>43254.0</v>
@@ -2052,7 +2052,7 @@
         <v>4371.0</v>
       </c>
       <c r="H24" t="n">
-        <v>18705.0</v>
+        <v>18708.0</v>
       </c>
       <c r="I24" t="n">
         <v>2967.0</v>
@@ -2067,7 +2067,7 @@
         <v>2641.0</v>
       </c>
       <c r="M24" t="n">
-        <v>16159.0</v>
+        <v>16173.0</v>
       </c>
       <c r="N24" t="s">
         <v>124</v>
@@ -2076,7 +2076,7 @@
         <v>57.0</v>
       </c>
       <c r="P24" t="n">
-        <v>480.0</v>
+        <v>520.0</v>
       </c>
       <c r="Q24" t="n">
         <v>6494.0</v>
@@ -2108,19 +2108,19 @@
         <v>10.0</v>
       </c>
       <c r="D25" t="n">
-        <v>3905.0</v>
+        <v>3908.0</v>
       </c>
       <c r="E25" t="n">
         <v>4008.0</v>
       </c>
       <c r="F25" t="n">
-        <v>1375.0</v>
+        <v>1382.0</v>
       </c>
       <c r="G25" t="n">
-        <v>1393.0</v>
+        <v>1398.0</v>
       </c>
       <c r="H25" t="n">
-        <v>3988.0</v>
+        <v>4000.0</v>
       </c>
       <c r="I25" t="n">
         <v>648.0</v>
@@ -2144,7 +2144,7 @@
         <v>10.0</v>
       </c>
       <c r="P25" t="n">
-        <v>60.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q25" t="n">
         <v>9630.0</v>
@@ -2185,16 +2185,16 @@
         <v>3357.0</v>
       </c>
       <c r="G26" t="n">
-        <v>3518.0</v>
+        <v>3521.0</v>
       </c>
       <c r="H26" t="n">
-        <v>12438.0</v>
+        <v>12441.0</v>
       </c>
       <c r="I26" t="n">
         <v>1730.0</v>
       </c>
       <c r="J26" t="n">
-        <v>2774.0</v>
+        <v>2776.0</v>
       </c>
       <c r="K26" t="n">
         <v>10.0</v>
@@ -2212,7 +2212,7 @@
         <v>530.0</v>
       </c>
       <c r="P26" t="n">
-        <v>340.0</v>
+        <v>360.0</v>
       </c>
       <c r="Q26" t="n">
         <v>43839.0</v>
@@ -2250,13 +2250,13 @@
         <v>4653.0</v>
       </c>
       <c r="F27" t="n">
-        <v>3743.0</v>
+        <v>3746.0</v>
       </c>
       <c r="G27" t="n">
         <v>3451.0</v>
       </c>
       <c r="H27" t="n">
-        <v>11471.0</v>
+        <v>11473.0</v>
       </c>
       <c r="I27" t="n">
         <v>1561.0</v>
@@ -2280,7 +2280,7 @@
         <v>121.0</v>
       </c>
       <c r="P27" t="n">
-        <v>80.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q27" t="n">
         <v>32905.0</v>
@@ -2318,16 +2318,16 @@
         <v>4107.0</v>
       </c>
       <c r="F28" t="n">
-        <v>858.0</v>
+        <v>865.0</v>
       </c>
       <c r="G28" t="n">
-        <v>708.0</v>
+        <v>709.0</v>
       </c>
       <c r="H28" t="n">
-        <v>2596.0</v>
+        <v>2600.0</v>
       </c>
       <c r="I28" t="n">
-        <v>349.0</v>
+        <v>351.0</v>
       </c>
       <c r="J28" t="n">
         <v>1289.0</v>
@@ -2345,10 +2345,10 @@
         <v>123</v>
       </c>
       <c r="O28" t="n">
-        <v>124.0</v>
+        <v>142.0</v>
       </c>
       <c r="P28" t="n">
-        <v>80.0</v>
+        <v>96.0</v>
       </c>
       <c r="Q28" t="n">
         <v>11303.0</v>
@@ -2460,10 +2460,10 @@
         <v>1135.0</v>
       </c>
       <c r="H30" t="n">
-        <v>6747.0</v>
+        <v>6751.0</v>
       </c>
       <c r="I30" t="n">
-        <v>1475.0</v>
+        <v>1476.0</v>
       </c>
       <c r="J30" t="n">
         <v>1864.0</v>
@@ -2481,13 +2481,13 @@
         <v>122</v>
       </c>
       <c r="O30" t="n">
-        <v>496.0</v>
+        <v>532.0</v>
       </c>
       <c r="P30" t="n">
-        <v>440.0</v>
+        <v>480.0</v>
       </c>
       <c r="Q30" t="n">
-        <v>13978.0</v>
+        <v>14014.0</v>
       </c>
       <c r="R30" t="n">
         <v>61.0</v>
@@ -2516,19 +2516,19 @@
         <v>10.0</v>
       </c>
       <c r="D31" t="n">
-        <v>4109.0</v>
+        <v>4135.0</v>
       </c>
       <c r="E31" t="n">
         <v>4206.0</v>
       </c>
       <c r="F31" t="n">
-        <v>696.0</v>
+        <v>697.0</v>
       </c>
       <c r="G31" t="n">
         <v>563.0</v>
       </c>
       <c r="H31" t="n">
-        <v>3470.0</v>
+        <v>3472.0</v>
       </c>
       <c r="I31" t="n">
         <v>757.0</v>
@@ -2552,7 +2552,7 @@
         <v>54.0</v>
       </c>
       <c r="P31" t="n">
-        <v>240.0</v>
+        <v>280.0</v>
       </c>
       <c r="Q31" t="n">
         <v>4745.0</v>
@@ -2590,16 +2590,16 @@
         <v>4190.0</v>
       </c>
       <c r="F32" t="n">
-        <v>2168.0</v>
+        <v>2171.0</v>
       </c>
       <c r="G32" t="n">
         <v>2216.0</v>
       </c>
       <c r="H32" t="n">
-        <v>7044.0</v>
+        <v>7046.0</v>
       </c>
       <c r="I32" t="n">
-        <v>1586.0</v>
+        <v>1587.0</v>
       </c>
       <c r="J32" t="n">
         <v>1479.0</v>
@@ -2658,19 +2658,19 @@
         <v>4798.0</v>
       </c>
       <c r="F33" t="n">
-        <v>5223.0</v>
+        <v>5230.0</v>
       </c>
       <c r="G33" t="n">
-        <v>5317.0</v>
+        <v>5323.0</v>
       </c>
       <c r="H33" t="n">
-        <v>12490.0</v>
+        <v>12504.0</v>
       </c>
       <c r="I33" t="n">
-        <v>2272.0</v>
+        <v>2274.0</v>
       </c>
       <c r="J33" t="n">
-        <v>1752.0</v>
+        <v>1764.0</v>
       </c>
       <c r="K33" t="n">
         <v>10.0</v>
@@ -2685,13 +2685,13 @@
         <v>122</v>
       </c>
       <c r="O33" t="n">
-        <v>42.0</v>
+        <v>72.0</v>
       </c>
       <c r="P33" t="n">
         <v>80.0</v>
       </c>
       <c r="Q33" t="n">
-        <v>59359.0</v>
+        <v>59389.0</v>
       </c>
       <c r="R33" t="n">
         <v>30.0</v>
@@ -2726,16 +2726,16 @@
         <v>4021.0</v>
       </c>
       <c r="F34" t="n">
-        <v>961.0</v>
+        <v>964.0</v>
       </c>
       <c r="G34" t="n">
         <v>981.0</v>
       </c>
       <c r="H34" t="n">
-        <v>4274.0</v>
+        <v>4276.0</v>
       </c>
       <c r="I34" t="n">
-        <v>1003.0</v>
+        <v>1005.0</v>
       </c>
       <c r="J34" t="n">
         <v>290.0</v>
@@ -2756,7 +2756,7 @@
         <v>30.0</v>
       </c>
       <c r="P34" t="n">
-        <v>160.0</v>
+        <v>190.0</v>
       </c>
       <c r="Q34" t="n">
         <v>8519.0</v>
@@ -2794,13 +2794,13 @@
         <v>4007.0</v>
       </c>
       <c r="F35" t="n">
-        <v>593.0</v>
+        <v>594.0</v>
       </c>
       <c r="G35" t="n">
-        <v>518.0</v>
+        <v>520.0</v>
       </c>
       <c r="H35" t="n">
-        <v>3514.0</v>
+        <v>3518.0</v>
       </c>
       <c r="I35" t="n">
         <v>724.0</v>
@@ -2821,13 +2821,13 @@
         <v>123</v>
       </c>
       <c r="O35" t="n">
-        <v>289.0</v>
+        <v>317.0</v>
       </c>
       <c r="P35" t="n">
-        <v>440.0</v>
+        <v>480.0</v>
       </c>
       <c r="Q35" t="n">
-        <v>17752.0</v>
+        <v>17780.0</v>
       </c>
       <c r="R35" t="n">
         <v>26.0</v>
@@ -2856,19 +2856,19 @@
         <v>10.0</v>
       </c>
       <c r="D36" t="n">
-        <v>4004.0</v>
+        <v>3961.0</v>
       </c>
       <c r="E36" t="n">
         <v>4135.0</v>
       </c>
       <c r="F36" t="n">
-        <v>3576.0</v>
+        <v>3579.0</v>
       </c>
       <c r="G36" t="n">
-        <v>4143.0</v>
+        <v>4147.0</v>
       </c>
       <c r="H36" t="n">
-        <v>9848.0</v>
+        <v>9857.0</v>
       </c>
       <c r="I36" t="n">
         <v>1795.0</v>
@@ -2889,13 +2889,13 @@
         <v>122</v>
       </c>
       <c r="O36" t="n">
-        <v>271.0</v>
+        <v>319.0</v>
       </c>
       <c r="P36" t="n">
-        <v>320.0</v>
+        <v>360.0</v>
       </c>
       <c r="Q36" t="n">
-        <v>15096.0</v>
+        <v>15144.0</v>
       </c>
       <c r="R36" t="n">
         <v>37.0</v>
@@ -2904,7 +2904,7 @@
         <v>76448.0</v>
       </c>
       <c r="T36" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="U36" t="n" s="2">
         <v>43280.0</v>
@@ -2930,19 +2930,19 @@
         <v>3630.0</v>
       </c>
       <c r="F37" t="n">
-        <v>317.0</v>
+        <v>338.0</v>
       </c>
       <c r="G37" t="n">
-        <v>189.0</v>
+        <v>194.0</v>
       </c>
       <c r="H37" t="n">
-        <v>659.0</v>
+        <v>679.0</v>
       </c>
       <c r="I37" t="n">
-        <v>120.0</v>
+        <v>128.0</v>
       </c>
       <c r="J37" t="n">
-        <v>516.0</v>
+        <v>666.0</v>
       </c>
       <c r="K37" t="n">
         <v>6.0</v>
@@ -2957,13 +2957,13 @@
         <v>123</v>
       </c>
       <c r="O37" t="n">
-        <v>190.0</v>
+        <v>264.0</v>
       </c>
       <c r="P37" t="n">
-        <v>280.0</v>
+        <v>320.0</v>
       </c>
       <c r="Q37" t="n">
-        <v>3003.0</v>
+        <v>3077.0</v>
       </c>
       <c r="R37" t="n">
         <v>2.0</v>
@@ -3060,19 +3060,19 @@
         <v>10.0</v>
       </c>
       <c r="D39" t="n">
-        <v>3964.0</v>
+        <v>3943.0</v>
       </c>
       <c r="E39" t="n">
         <v>4072.0</v>
       </c>
       <c r="F39" t="n">
-        <v>655.0</v>
+        <v>658.0</v>
       </c>
       <c r="G39" t="n">
-        <v>372.0</v>
+        <v>376.0</v>
       </c>
       <c r="H39" t="n">
-        <v>1750.0</v>
+        <v>1757.0</v>
       </c>
       <c r="I39" t="n">
         <v>286.0</v>
@@ -3093,13 +3093,13 @@
         <v>123</v>
       </c>
       <c r="O39" t="n">
-        <v>68.0</v>
+        <v>96.0</v>
       </c>
       <c r="P39" t="n">
-        <v>112.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q39" t="n">
-        <v>8081.0</v>
+        <v>8109.0</v>
       </c>
       <c r="R39" t="n">
         <v>20.0</v>
@@ -3128,22 +3128,22 @@
         <v>10.0</v>
       </c>
       <c r="D40" t="n">
-        <v>4210.0</v>
+        <v>4329.0</v>
       </c>
       <c r="E40" t="n">
         <v>4405.0</v>
       </c>
       <c r="F40" t="n">
-        <v>1102.0</v>
+        <v>1106.0</v>
       </c>
       <c r="G40" t="n">
         <v>1001.0</v>
       </c>
       <c r="H40" t="n">
-        <v>3162.0</v>
+        <v>3166.0</v>
       </c>
       <c r="I40" t="n">
-        <v>664.0</v>
+        <v>665.0</v>
       </c>
       <c r="J40" t="n">
         <v>1700.0</v>
@@ -3161,13 +3161,13 @@
         <v>123</v>
       </c>
       <c r="O40" t="n">
-        <v>198.0</v>
+        <v>206.0</v>
       </c>
       <c r="P40" t="n">
-        <v>280.0</v>
+        <v>320.0</v>
       </c>
       <c r="Q40" t="n">
-        <v>20564.0</v>
+        <v>20572.0</v>
       </c>
       <c r="R40" t="n">
         <v>19.0</v>
@@ -3176,7 +3176,7 @@
         <v>57000.0</v>
       </c>
       <c r="T40" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="U40" t="n" s="2">
         <v>43352.0</v>
@@ -3208,10 +3208,10 @@
         <v>4741.0</v>
       </c>
       <c r="H41" t="n">
-        <v>27102.0</v>
+        <v>27112.0</v>
       </c>
       <c r="I41" t="n">
-        <v>3692.0</v>
+        <v>3693.0</v>
       </c>
       <c r="J41" t="n">
         <v>2014.0</v>
@@ -3232,7 +3232,7 @@
         <v>8.0</v>
       </c>
       <c r="P41" t="n">
-        <v>200.0</v>
+        <v>240.0</v>
       </c>
       <c r="Q41" t="n">
         <v>7130.0</v>
@@ -3264,22 +3264,22 @@
         <v>11.0</v>
       </c>
       <c r="D42" t="n">
-        <v>4187.0</v>
+        <v>4168.0</v>
       </c>
       <c r="E42" t="n">
         <v>4323.0</v>
       </c>
       <c r="F42" t="n">
-        <v>2439.0</v>
+        <v>2441.0</v>
       </c>
       <c r="G42" t="n">
-        <v>2363.0</v>
+        <v>2366.0</v>
       </c>
       <c r="H42" t="n">
-        <v>6155.0</v>
+        <v>6160.0</v>
       </c>
       <c r="I42" t="n">
-        <v>1196.0</v>
+        <v>1197.0</v>
       </c>
       <c r="J42" t="n">
         <v>2822.0</v>
@@ -3297,13 +3297,13 @@
         <v>123</v>
       </c>
       <c r="O42" t="n">
-        <v>262.0</v>
+        <v>316.0</v>
       </c>
       <c r="P42" t="n">
-        <v>240.0</v>
+        <v>280.0</v>
       </c>
       <c r="Q42" t="n">
-        <v>22524.0</v>
+        <v>22578.0</v>
       </c>
       <c r="R42" t="n">
         <v>20.0</v>
@@ -3332,19 +3332,19 @@
         <v>11.0</v>
       </c>
       <c r="D43" t="n">
-        <v>3907.0</v>
+        <v>3879.0</v>
       </c>
       <c r="E43" t="n">
         <v>4038.0</v>
       </c>
       <c r="F43" t="n">
-        <v>1300.0</v>
+        <v>1301.0</v>
       </c>
       <c r="G43" t="n">
-        <v>1132.0</v>
+        <v>1133.0</v>
       </c>
       <c r="H43" t="n">
-        <v>4390.0</v>
+        <v>4392.0</v>
       </c>
       <c r="I43" t="n">
         <v>749.0</v>
@@ -3365,13 +3365,13 @@
         <v>123</v>
       </c>
       <c r="O43" t="n">
-        <v>758.0</v>
+        <v>778.0</v>
       </c>
       <c r="P43" t="n">
-        <v>440.0</v>
+        <v>480.0</v>
       </c>
       <c r="Q43" t="n">
-        <v>29221.0</v>
+        <v>29241.0</v>
       </c>
       <c r="R43" t="n">
         <v>25.0</v>
@@ -3412,7 +3412,7 @@
         <v>2667.0</v>
       </c>
       <c r="H44" t="n">
-        <v>7846.0</v>
+        <v>7847.0</v>
       </c>
       <c r="I44" t="n">
         <v>2282.0</v>
@@ -3433,13 +3433,13 @@
         <v>123</v>
       </c>
       <c r="O44" t="n">
-        <v>140.0</v>
+        <v>166.0</v>
       </c>
       <c r="P44" t="n">
         <v>120.0</v>
       </c>
       <c r="Q44" t="n">
-        <v>31988.0</v>
+        <v>32014.0</v>
       </c>
       <c r="R44" t="n">
         <v>25.0</v>
@@ -3501,13 +3501,13 @@
         <v>123</v>
       </c>
       <c r="O45" t="n">
-        <v>286.0</v>
+        <v>297.0</v>
       </c>
       <c r="P45" t="n">
-        <v>200.0</v>
+        <v>230.0</v>
       </c>
       <c r="Q45" t="n">
-        <v>22949.0</v>
+        <v>22960.0</v>
       </c>
       <c r="R45" t="n">
         <v>20.0</v>
@@ -3678,13 +3678,13 @@
         <v>4919.0</v>
       </c>
       <c r="F48" t="n">
-        <v>11153.0</v>
+        <v>11154.0</v>
       </c>
       <c r="G48" t="n">
-        <v>11851.0</v>
+        <v>11855.0</v>
       </c>
       <c r="H48" t="n">
-        <v>26565.0</v>
+        <v>26570.0</v>
       </c>
       <c r="I48" t="n">
         <v>9171.0</v>
@@ -3705,13 +3705,13 @@
         <v>123</v>
       </c>
       <c r="O48" t="n">
-        <v>1031.0</v>
+        <v>1153.0</v>
       </c>
       <c r="P48" t="n">
-        <v>480.0</v>
+        <v>520.0</v>
       </c>
       <c r="Q48" t="n">
-        <v>77736.0</v>
+        <v>77858.0</v>
       </c>
       <c r="R48" t="n">
         <v>26.0</v>
@@ -3752,7 +3752,7 @@
         <v>3043.0</v>
       </c>
       <c r="H49" t="n">
-        <v>15729.0</v>
+        <v>15731.0</v>
       </c>
       <c r="I49" t="n">
         <v>3302.0</v>
@@ -3773,13 +3773,13 @@
         <v>122</v>
       </c>
       <c r="O49" t="n">
-        <v>387.0</v>
+        <v>413.0</v>
       </c>
       <c r="P49" t="n">
         <v>360.0</v>
       </c>
       <c r="Q49" t="n">
-        <v>33914.0</v>
+        <v>33940.0</v>
       </c>
       <c r="R49" t="n">
         <v>41.0</v>

</xml_diff>

<commit_message>
Bugfix in members with no wars + Data update
</commit_message>
<xml_diff>
--- a/docs/data/memberstats.xlsx
+++ b/docs/data/memberstats.xlsx
@@ -553,10 +553,10 @@
         <v>2115.0</v>
       </c>
       <c r="H2" t="n">
-        <v>7143.0</v>
+        <v>7151.0</v>
       </c>
       <c r="I2" t="n">
-        <v>1163.0</v>
+        <v>1165.0</v>
       </c>
       <c r="J2" t="n">
         <v>2684.0</v>
@@ -574,19 +574,19 @@
         <v>122</v>
       </c>
       <c r="O2" t="n">
-        <v>58.0</v>
+        <v>96.0</v>
       </c>
       <c r="P2" t="n">
-        <v>40.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q2" t="n">
-        <v>29224.0</v>
+        <v>29262.0</v>
       </c>
       <c r="R2" t="n">
-        <v>47.0</v>
+        <v>49.0</v>
       </c>
       <c r="S2" t="n">
-        <v>93500.0</v>
+        <v>94620.0</v>
       </c>
       <c r="T2" t="s">
         <v>126</v>
@@ -595,7 +595,7 @@
         <v>43302.0</v>
       </c>
       <c r="V2" t="n">
-        <v>128.0</v>
+        <v>130.0</v>
       </c>
     </row>
     <row r="3">
@@ -663,7 +663,7 @@
         <v>43372.0</v>
       </c>
       <c r="V3" t="n">
-        <v>58.0</v>
+        <v>60.0</v>
       </c>
     </row>
     <row r="4">
@@ -677,22 +677,22 @@
         <v>11.0</v>
       </c>
       <c r="D4" t="n">
-        <v>4133.0</v>
+        <v>4147.0</v>
       </c>
       <c r="E4" t="n">
         <v>4292.0</v>
       </c>
       <c r="F4" t="n">
-        <v>2690.0</v>
+        <v>2698.0</v>
       </c>
       <c r="G4" t="n">
-        <v>2717.0</v>
+        <v>2724.0</v>
       </c>
       <c r="H4" t="n">
-        <v>6429.0</v>
+        <v>6446.0</v>
       </c>
       <c r="I4" t="n">
-        <v>1086.0</v>
+        <v>1090.0</v>
       </c>
       <c r="J4" t="n">
         <v>1671.0</v>
@@ -710,19 +710,19 @@
         <v>122</v>
       </c>
       <c r="O4" t="n">
-        <v>20.0</v>
+        <v>62.0</v>
       </c>
       <c r="P4" t="n">
-        <v>40.0</v>
+        <v>240.0</v>
       </c>
       <c r="Q4" t="n">
-        <v>9288.0</v>
+        <v>9330.0</v>
       </c>
       <c r="R4" t="n">
-        <v>51.0</v>
+        <v>52.0</v>
       </c>
       <c r="S4" t="n">
-        <v>69766.0</v>
+        <v>70046.0</v>
       </c>
       <c r="T4" t="s">
         <v>128</v>
@@ -731,7 +731,7 @@
         <v>43082.0</v>
       </c>
       <c r="V4" t="n">
-        <v>348.0</v>
+        <v>350.0</v>
       </c>
     </row>
     <row r="5">
@@ -781,7 +781,7 @@
         <v>0.0</v>
       </c>
       <c r="P5" t="n">
-        <v>16.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q5" t="n">
         <v>16997.0</v>
@@ -799,7 +799,7 @@
         <v>43397.0</v>
       </c>
       <c r="V5" t="n">
-        <v>33.0</v>
+        <v>35.0</v>
       </c>
     </row>
     <row r="6">
@@ -813,22 +813,22 @@
         <v>10.0</v>
       </c>
       <c r="D6" t="n">
-        <v>4069.0</v>
+        <v>4023.0</v>
       </c>
       <c r="E6" t="n">
         <v>4176.0</v>
       </c>
       <c r="F6" t="n">
-        <v>1278.0</v>
+        <v>1280.0</v>
       </c>
       <c r="G6" t="n">
-        <v>1305.0</v>
+        <v>1309.0</v>
       </c>
       <c r="H6" t="n">
-        <v>3316.0</v>
+        <v>3327.0</v>
       </c>
       <c r="I6" t="n">
-        <v>509.0</v>
+        <v>511.0</v>
       </c>
       <c r="J6" t="n">
         <v>313.0</v>
@@ -846,19 +846,19 @@
         <v>123</v>
       </c>
       <c r="O6" t="n">
-        <v>0.0</v>
+        <v>126.0</v>
       </c>
       <c r="P6" t="n">
-        <v>0.0</v>
+        <v>160.0</v>
       </c>
       <c r="Q6" t="n">
-        <v>17369.0</v>
+        <v>17495.0</v>
       </c>
       <c r="R6" t="n">
         <v>30.0</v>
       </c>
       <c r="S6" t="n">
-        <v>45826.0</v>
+        <v>47506.0</v>
       </c>
       <c r="T6" t="s">
         <v>128</v>
@@ -867,7 +867,7 @@
         <v>43356.0</v>
       </c>
       <c r="V6" t="n">
-        <v>74.0</v>
+        <v>76.0</v>
       </c>
     </row>
     <row r="7">
@@ -881,25 +881,25 @@
         <v>11.0</v>
       </c>
       <c r="D7" t="n">
-        <v>4313.0</v>
+        <v>4326.0</v>
       </c>
       <c r="E7" t="n">
         <v>4489.0</v>
       </c>
       <c r="F7" t="n">
-        <v>3017.0</v>
+        <v>3032.0</v>
       </c>
       <c r="G7" t="n">
-        <v>2684.0</v>
+        <v>2695.0</v>
       </c>
       <c r="H7" t="n">
-        <v>7121.0</v>
+        <v>7151.0</v>
       </c>
       <c r="I7" t="n">
-        <v>695.0</v>
+        <v>697.0</v>
       </c>
       <c r="J7" t="n">
-        <v>4259.0</v>
+        <v>4297.0</v>
       </c>
       <c r="K7" t="n">
         <v>10.0</v>
@@ -917,16 +917,16 @@
         <v>0.0</v>
       </c>
       <c r="P7" t="n">
-        <v>0.0</v>
+        <v>160.0</v>
       </c>
       <c r="Q7" t="n">
         <v>2125.0</v>
       </c>
       <c r="R7" t="n">
-        <v>46.0</v>
+        <v>47.0</v>
       </c>
       <c r="S7" t="n">
-        <v>62120.0</v>
+        <v>63240.0</v>
       </c>
       <c r="T7" t="s">
         <v>126</v>
@@ -935,7 +935,7 @@
         <v>43364.0</v>
       </c>
       <c r="V7" t="n">
-        <v>66.0</v>
+        <v>68.0</v>
       </c>
     </row>
     <row r="8">
@@ -949,22 +949,22 @@
         <v>11.0</v>
       </c>
       <c r="D8" t="n">
-        <v>4535.0</v>
+        <v>4353.0</v>
       </c>
       <c r="E8" t="n">
         <v>4568.0</v>
       </c>
       <c r="F8" t="n">
-        <v>1960.0</v>
+        <v>1964.0</v>
       </c>
       <c r="G8" t="n">
-        <v>1840.0</v>
+        <v>1851.0</v>
       </c>
       <c r="H8" t="n">
-        <v>7774.0</v>
+        <v>7797.0</v>
       </c>
       <c r="I8" t="n">
-        <v>1132.0</v>
+        <v>1135.0</v>
       </c>
       <c r="J8" t="n">
         <v>1401.0</v>
@@ -982,19 +982,19 @@
         <v>124</v>
       </c>
       <c r="O8" t="n">
-        <v>30.0</v>
+        <v>161.0</v>
       </c>
       <c r="P8" t="n">
-        <v>80.0</v>
+        <v>200.0</v>
       </c>
       <c r="Q8" t="n">
-        <v>25807.0</v>
+        <v>25938.0</v>
       </c>
       <c r="R8" t="n">
-        <v>59.0</v>
+        <v>60.0</v>
       </c>
       <c r="S8" t="n">
-        <v>76555.0</v>
+        <v>77395.0</v>
       </c>
       <c r="T8" t="s">
         <v>126</v>
@@ -1003,7 +1003,7 @@
         <v>43058.0</v>
       </c>
       <c r="V8" t="n">
-        <v>372.0</v>
+        <v>374.0</v>
       </c>
     </row>
     <row r="9">
@@ -1017,25 +1017,25 @@
         <v>11.0</v>
       </c>
       <c r="D9" t="n">
-        <v>4451.0</v>
+        <v>4492.0</v>
       </c>
       <c r="E9" t="n">
         <v>4634.0</v>
       </c>
       <c r="F9" t="n">
-        <v>2555.0</v>
+        <v>2566.0</v>
       </c>
       <c r="G9" t="n">
-        <v>2379.0</v>
+        <v>2390.0</v>
       </c>
       <c r="H9" t="n">
-        <v>11117.0</v>
+        <v>11149.0</v>
       </c>
       <c r="I9" t="n">
-        <v>2448.0</v>
+        <v>2454.0</v>
       </c>
       <c r="J9" t="n">
-        <v>1968.0</v>
+        <v>1981.0</v>
       </c>
       <c r="K9" t="n">
         <v>11.0</v>
@@ -1050,19 +1050,19 @@
         <v>124</v>
       </c>
       <c r="O9" t="n">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
       <c r="P9" t="n">
-        <v>40.0</v>
+        <v>200.0</v>
       </c>
       <c r="Q9" t="n">
-        <v>3423.0</v>
+        <v>3443.0</v>
       </c>
       <c r="R9" t="n">
         <v>61.0</v>
       </c>
       <c r="S9" t="n">
-        <v>88030.0</v>
+        <v>88590.0</v>
       </c>
       <c r="T9" t="s">
         <v>126</v>
@@ -1071,7 +1071,7 @@
         <v>43123.0</v>
       </c>
       <c r="V9" t="n">
-        <v>307.0</v>
+        <v>309.0</v>
       </c>
     </row>
     <row r="10">
@@ -1085,19 +1085,19 @@
         <v>12.0</v>
       </c>
       <c r="D10" t="n">
-        <v>4512.0</v>
+        <v>4608.0</v>
       </c>
       <c r="E10" t="n">
         <v>4731.0</v>
       </c>
       <c r="F10" t="n">
-        <v>2296.0</v>
+        <v>2303.0</v>
       </c>
       <c r="G10" t="n">
-        <v>1776.0</v>
+        <v>1780.0</v>
       </c>
       <c r="H10" t="n">
-        <v>9660.0</v>
+        <v>9673.0</v>
       </c>
       <c r="I10" t="n">
         <v>1382.0</v>
@@ -1118,28 +1118,28 @@
         <v>123</v>
       </c>
       <c r="O10" t="n">
-        <v>36.0</v>
+        <v>279.0</v>
       </c>
       <c r="P10" t="n">
-        <v>40.0</v>
+        <v>280.0</v>
       </c>
       <c r="Q10" t="n">
-        <v>92681.0</v>
+        <v>92924.0</v>
       </c>
       <c r="R10" t="n">
-        <v>81.0</v>
+        <v>82.0</v>
       </c>
       <c r="S10" t="n">
         <v>85200.0</v>
       </c>
       <c r="T10" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="U10" t="n" s="2">
         <v>43397.0</v>
       </c>
       <c r="V10" t="n">
-        <v>33.0</v>
+        <v>35.0</v>
       </c>
     </row>
     <row r="11">
@@ -1153,22 +1153,22 @@
         <v>11.0</v>
       </c>
       <c r="D11" t="n">
-        <v>4322.0</v>
+        <v>4274.0</v>
       </c>
       <c r="E11" t="n">
         <v>4389.0</v>
       </c>
       <c r="F11" t="n">
-        <v>1414.0</v>
+        <v>1422.0</v>
       </c>
       <c r="G11" t="n">
-        <v>1247.0</v>
+        <v>1259.0</v>
       </c>
       <c r="H11" t="n">
-        <v>5756.0</v>
+        <v>5780.0</v>
       </c>
       <c r="I11" t="n">
-        <v>795.0</v>
+        <v>796.0</v>
       </c>
       <c r="J11" t="n">
         <v>1298.0</v>
@@ -1186,28 +1186,28 @@
         <v>124</v>
       </c>
       <c r="O11" t="n">
-        <v>70.0</v>
+        <v>216.0</v>
       </c>
       <c r="P11" t="n">
-        <v>40.0</v>
+        <v>190.0</v>
       </c>
       <c r="Q11" t="n">
-        <v>39651.0</v>
+        <v>39797.0</v>
       </c>
       <c r="R11" t="n">
-        <v>68.0</v>
+        <v>69.0</v>
       </c>
       <c r="S11" t="n">
-        <v>83400.0</v>
+        <v>84240.0</v>
       </c>
       <c r="T11" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="U11" t="n" s="2">
         <v>43218.0</v>
       </c>
       <c r="V11" t="n">
-        <v>212.0</v>
+        <v>214.0</v>
       </c>
     </row>
     <row r="12">
@@ -1221,22 +1221,22 @@
         <v>12.0</v>
       </c>
       <c r="D12" t="n">
-        <v>4425.0</v>
+        <v>4382.0</v>
       </c>
       <c r="E12" t="n">
         <v>4553.0</v>
       </c>
       <c r="F12" t="n">
-        <v>4739.0</v>
+        <v>4747.0</v>
       </c>
       <c r="G12" t="n">
-        <v>5137.0</v>
+        <v>5147.0</v>
       </c>
       <c r="H12" t="n">
-        <v>10970.0</v>
+        <v>10996.0</v>
       </c>
       <c r="I12" t="n">
-        <v>2108.0</v>
+        <v>2112.0</v>
       </c>
       <c r="J12" t="n">
         <v>1862.0</v>
@@ -1254,19 +1254,19 @@
         <v>123</v>
       </c>
       <c r="O12" t="n">
-        <v>84.0</v>
+        <v>508.0</v>
       </c>
       <c r="P12" t="n">
-        <v>40.0</v>
+        <v>240.0</v>
       </c>
       <c r="Q12" t="n">
-        <v>56225.0</v>
+        <v>56649.0</v>
       </c>
       <c r="R12" t="n">
-        <v>33.0</v>
+        <v>34.0</v>
       </c>
       <c r="S12" t="n">
-        <v>89810.0</v>
+        <v>90930.0</v>
       </c>
       <c r="T12" t="s">
         <v>126</v>
@@ -1275,7 +1275,7 @@
         <v>43390.0</v>
       </c>
       <c r="V12" t="n">
-        <v>40.0</v>
+        <v>42.0</v>
       </c>
     </row>
     <row r="13">
@@ -1301,7 +1301,7 @@
         <v>1708.0</v>
       </c>
       <c r="H13" t="n">
-        <v>6626.0</v>
+        <v>6627.0</v>
       </c>
       <c r="I13" t="n">
         <v>1411.0</v>
@@ -1322,13 +1322,13 @@
         <v>123</v>
       </c>
       <c r="O13" t="n">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
       <c r="P13" t="n">
-        <v>16.0</v>
+        <v>56.0</v>
       </c>
       <c r="Q13" t="n">
-        <v>44282.0</v>
+        <v>44302.0</v>
       </c>
       <c r="R13" t="n">
         <v>35.0</v>
@@ -1343,7 +1343,7 @@
         <v>43410.0</v>
       </c>
       <c r="V13" t="n">
-        <v>20.0</v>
+        <v>22.0</v>
       </c>
     </row>
     <row r="14">
@@ -1357,22 +1357,22 @@
         <v>11.0</v>
       </c>
       <c r="D14" t="n">
-        <v>4268.0</v>
+        <v>4290.0</v>
       </c>
       <c r="E14" t="n">
         <v>4416.0</v>
       </c>
       <c r="F14" t="n">
-        <v>2338.0</v>
+        <v>2352.0</v>
       </c>
       <c r="G14" t="n">
-        <v>2120.0</v>
+        <v>2131.0</v>
       </c>
       <c r="H14" t="n">
-        <v>6833.0</v>
+        <v>6861.0</v>
       </c>
       <c r="I14" t="n">
-        <v>1096.0</v>
+        <v>1098.0</v>
       </c>
       <c r="J14" t="n">
         <v>3769.0</v>
@@ -1393,7 +1393,7 @@
         <v>0.0</v>
       </c>
       <c r="P14" t="n">
-        <v>0.0</v>
+        <v>160.0</v>
       </c>
       <c r="Q14" t="n">
         <v>20631.0</v>
@@ -1402,7 +1402,7 @@
         <v>44.0</v>
       </c>
       <c r="S14" t="n">
-        <v>50701.0</v>
+        <v>50981.0</v>
       </c>
       <c r="T14" t="s">
         <v>128</v>
@@ -1411,7 +1411,7 @@
         <v>43275.0</v>
       </c>
       <c r="V14" t="n">
-        <v>155.0</v>
+        <v>157.0</v>
       </c>
     </row>
     <row r="15">
@@ -1437,10 +1437,10 @@
         <v>1463.0</v>
       </c>
       <c r="H15" t="n">
-        <v>3681.0</v>
+        <v>3687.0</v>
       </c>
       <c r="I15" t="n">
-        <v>1010.0</v>
+        <v>1012.0</v>
       </c>
       <c r="J15" t="n">
         <v>2616.0</v>
@@ -1458,19 +1458,19 @@
         <v>122</v>
       </c>
       <c r="O15" t="n">
-        <v>0.0</v>
+        <v>68.0</v>
       </c>
       <c r="P15" t="n">
-        <v>0.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q15" t="n">
-        <v>31630.0</v>
+        <v>31698.0</v>
       </c>
       <c r="R15" t="n">
         <v>20.0</v>
       </c>
       <c r="S15" t="n">
-        <v>33242.0</v>
+        <v>35603.0</v>
       </c>
       <c r="T15" t="s">
         <v>127</v>
@@ -1479,7 +1479,7 @@
         <v>43220.0</v>
       </c>
       <c r="V15" t="n">
-        <v>210.0</v>
+        <v>212.0</v>
       </c>
     </row>
     <row r="16">
@@ -1547,7 +1547,7 @@
         <v>43419.0</v>
       </c>
       <c r="V16" t="n">
-        <v>11.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="17">
@@ -1561,19 +1561,19 @@
         <v>11.0</v>
       </c>
       <c r="D17" t="n">
-        <v>4331.0</v>
+        <v>4422.0</v>
       </c>
       <c r="E17" t="n">
         <v>4577.0</v>
       </c>
       <c r="F17" t="n">
-        <v>2861.0</v>
+        <v>2868.0</v>
       </c>
       <c r="G17" t="n">
-        <v>2606.0</v>
+        <v>2611.0</v>
       </c>
       <c r="H17" t="n">
-        <v>6777.0</v>
+        <v>6793.0</v>
       </c>
       <c r="I17" t="n">
         <v>733.0</v>
@@ -1594,19 +1594,19 @@
         <v>122</v>
       </c>
       <c r="O17" t="n">
-        <v>10.0</v>
+        <v>50.0</v>
       </c>
       <c r="P17" t="n">
-        <v>60.0</v>
+        <v>180.0</v>
       </c>
       <c r="Q17" t="n">
-        <v>22149.0</v>
+        <v>22189.0</v>
       </c>
       <c r="R17" t="n">
-        <v>54.0</v>
+        <v>55.0</v>
       </c>
       <c r="S17" t="n">
-        <v>86265.0</v>
+        <v>87665.0</v>
       </c>
       <c r="T17" t="s">
         <v>126</v>
@@ -1615,7 +1615,7 @@
         <v>43058.0</v>
       </c>
       <c r="V17" t="n">
-        <v>372.0</v>
+        <v>374.0</v>
       </c>
     </row>
     <row r="18">
@@ -1629,19 +1629,19 @@
         <v>12.0</v>
       </c>
       <c r="D18" t="n">
-        <v>4327.0</v>
+        <v>4364.0</v>
       </c>
       <c r="E18" t="n">
         <v>4512.0</v>
       </c>
       <c r="F18" t="n">
-        <v>3042.0</v>
+        <v>3046.0</v>
       </c>
       <c r="G18" t="n">
-        <v>2923.0</v>
+        <v>2926.0</v>
       </c>
       <c r="H18" t="n">
-        <v>6940.0</v>
+        <v>6953.0</v>
       </c>
       <c r="I18" t="n">
         <v>1262.0</v>
@@ -1662,19 +1662,19 @@
         <v>122</v>
       </c>
       <c r="O18" t="n">
-        <v>8.0</v>
+        <v>130.0</v>
       </c>
       <c r="P18" t="n">
-        <v>60.0</v>
+        <v>180.0</v>
       </c>
       <c r="Q18" t="n">
-        <v>46826.0</v>
+        <v>46948.0</v>
       </c>
       <c r="R18" t="n">
         <v>37.0</v>
       </c>
       <c r="S18" t="n">
-        <v>57595.0</v>
+        <v>59835.0</v>
       </c>
       <c r="T18" t="s">
         <v>126</v>
@@ -1683,7 +1683,7 @@
         <v>43312.0</v>
       </c>
       <c r="V18" t="n">
-        <v>118.0</v>
+        <v>120.0</v>
       </c>
     </row>
     <row r="19">
@@ -1697,25 +1697,25 @@
         <v>11.0</v>
       </c>
       <c r="D19" t="n">
-        <v>3940.0</v>
+        <v>3882.0</v>
       </c>
       <c r="E19" t="n">
         <v>4059.0</v>
       </c>
       <c r="F19" t="n">
-        <v>1683.0</v>
+        <v>1692.0</v>
       </c>
       <c r="G19" t="n">
-        <v>1741.0</v>
+        <v>1752.0</v>
       </c>
       <c r="H19" t="n">
-        <v>4436.0</v>
+        <v>4462.0</v>
       </c>
       <c r="I19" t="n">
-        <v>655.0</v>
+        <v>657.0</v>
       </c>
       <c r="J19" t="n">
-        <v>3481.0</v>
+        <v>3491.0</v>
       </c>
       <c r="K19" t="n">
         <v>8.0</v>
@@ -1724,25 +1724,25 @@
         <v>34.0</v>
       </c>
       <c r="M19" t="n">
-        <v>186.0</v>
+        <v>199.0</v>
       </c>
       <c r="N19" t="s">
         <v>123</v>
       </c>
       <c r="O19" t="n">
-        <v>0.0</v>
+        <v>134.0</v>
       </c>
       <c r="P19" t="n">
-        <v>0.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q19" t="n">
-        <v>12782.0</v>
+        <v>12916.0</v>
       </c>
       <c r="R19" t="n">
         <v>19.0</v>
       </c>
       <c r="S19" t="n">
-        <v>22074.0</v>
+        <v>23123.0</v>
       </c>
       <c r="T19" t="s">
         <v>127</v>
@@ -1751,7 +1751,7 @@
         <v>43421.0</v>
       </c>
       <c r="V19" t="n">
-        <v>9.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="20">
@@ -1765,22 +1765,22 @@
         <v>12.0</v>
       </c>
       <c r="D20" t="n">
-        <v>4702.0</v>
+        <v>4737.0</v>
       </c>
       <c r="E20" t="n">
         <v>4767.0</v>
       </c>
       <c r="F20" t="n">
-        <v>6786.0</v>
+        <v>6789.0</v>
       </c>
       <c r="G20" t="n">
-        <v>6699.0</v>
+        <v>6701.0</v>
       </c>
       <c r="H20" t="n">
-        <v>24130.0</v>
+        <v>24161.0</v>
       </c>
       <c r="I20" t="n">
-        <v>2812.0</v>
+        <v>2816.0</v>
       </c>
       <c r="J20" t="n">
         <v>2696.0</v>
@@ -1792,25 +1792,25 @@
         <v>433.0</v>
       </c>
       <c r="M20" t="n">
-        <v>2699.0</v>
+        <v>2731.0</v>
       </c>
       <c r="N20" t="s">
         <v>125</v>
       </c>
       <c r="O20" t="n">
-        <v>98.0</v>
+        <v>428.0</v>
       </c>
       <c r="P20" t="n">
-        <v>40.0</v>
+        <v>280.0</v>
       </c>
       <c r="Q20" t="n">
-        <v>69806.0</v>
+        <v>70136.0</v>
       </c>
       <c r="R20" t="n">
-        <v>94.0</v>
+        <v>95.0</v>
       </c>
       <c r="S20" t="n">
-        <v>93095.0</v>
+        <v>93655.0</v>
       </c>
       <c r="T20" t="s">
         <v>130</v>
@@ -1819,7 +1819,7 @@
         <v>42705.0</v>
       </c>
       <c r="V20" t="n">
-        <v>725.0</v>
+        <v>727.0</v>
       </c>
     </row>
     <row r="21">
@@ -1887,7 +1887,7 @@
         <v>43151.0</v>
       </c>
       <c r="V21" t="n">
-        <v>279.0</v>
+        <v>281.0</v>
       </c>
     </row>
     <row r="22">
@@ -1901,22 +1901,22 @@
         <v>11.0</v>
       </c>
       <c r="D22" t="n">
-        <v>4046.0</v>
+        <v>4051.0</v>
       </c>
       <c r="E22" t="n">
         <v>4253.0</v>
       </c>
       <c r="F22" t="n">
-        <v>1362.0</v>
+        <v>1364.0</v>
       </c>
       <c r="G22" t="n">
-        <v>1425.0</v>
+        <v>1427.0</v>
       </c>
       <c r="H22" t="n">
-        <v>4656.0</v>
+        <v>4660.0</v>
       </c>
       <c r="I22" t="n">
-        <v>889.0</v>
+        <v>890.0</v>
       </c>
       <c r="J22" t="n">
         <v>507.0</v>
@@ -1934,13 +1934,13 @@
         <v>123</v>
       </c>
       <c r="O22" t="n">
-        <v>30.0</v>
+        <v>121.0</v>
       </c>
       <c r="P22" t="n">
-        <v>40.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q22" t="n">
-        <v>22205.0</v>
+        <v>22296.0</v>
       </c>
       <c r="R22" t="n">
         <v>29.0</v>
@@ -1955,7 +1955,7 @@
         <v>43254.0</v>
       </c>
       <c r="V22" t="n">
-        <v>176.0</v>
+        <v>178.0</v>
       </c>
     </row>
     <row r="23">
@@ -2023,7 +2023,7 @@
         <v>43380.0</v>
       </c>
       <c r="V23" t="n">
-        <v>50.0</v>
+        <v>52.0</v>
       </c>
     </row>
     <row r="24">
@@ -2046,16 +2046,16 @@
         <v>4437.0</v>
       </c>
       <c r="G24" t="n">
-        <v>4371.0</v>
+        <v>4374.0</v>
       </c>
       <c r="H24" t="n">
-        <v>18759.0</v>
+        <v>18799.0</v>
       </c>
       <c r="I24" t="n">
-        <v>2974.0</v>
+        <v>2978.0</v>
       </c>
       <c r="J24" t="n">
-        <v>2751.0</v>
+        <v>2753.0</v>
       </c>
       <c r="K24" t="n">
         <v>11.0</v>
@@ -2064,25 +2064,25 @@
         <v>2641.0</v>
       </c>
       <c r="M24" t="n">
-        <v>16234.0</v>
+        <v>16278.0</v>
       </c>
       <c r="N24" t="s">
         <v>124</v>
       </c>
       <c r="O24" t="n">
-        <v>10.0</v>
+        <v>40.0</v>
       </c>
       <c r="P24" t="n">
-        <v>40.0</v>
+        <v>240.0</v>
       </c>
       <c r="Q24" t="n">
-        <v>6564.0</v>
+        <v>6594.0</v>
       </c>
       <c r="R24" t="n">
-        <v>82.0</v>
+        <v>83.0</v>
       </c>
       <c r="S24" t="n">
-        <v>89225.0</v>
+        <v>90345.0</v>
       </c>
       <c r="T24" t="s">
         <v>126</v>
@@ -2091,7 +2091,7 @@
         <v>42614.0</v>
       </c>
       <c r="V24" t="n">
-        <v>816.0</v>
+        <v>818.0</v>
       </c>
     </row>
     <row r="25">
@@ -2105,25 +2105,25 @@
         <v>10.0</v>
       </c>
       <c r="D25" t="n">
-        <v>3895.0</v>
+        <v>3846.0</v>
       </c>
       <c r="E25" t="n">
         <v>4008.0</v>
       </c>
       <c r="F25" t="n">
-        <v>1388.0</v>
+        <v>1401.0</v>
       </c>
       <c r="G25" t="n">
-        <v>1406.0</v>
+        <v>1424.0</v>
       </c>
       <c r="H25" t="n">
-        <v>4017.0</v>
+        <v>4057.0</v>
       </c>
       <c r="I25" t="n">
-        <v>650.0</v>
+        <v>656.0</v>
       </c>
       <c r="J25" t="n">
-        <v>807.0</v>
+        <v>818.0</v>
       </c>
       <c r="K25" t="n">
         <v>10.0</v>
@@ -2138,19 +2138,19 @@
         <v>123</v>
       </c>
       <c r="O25" t="n">
-        <v>112.0</v>
+        <v>176.0</v>
       </c>
       <c r="P25" t="n">
-        <v>20.0</v>
+        <v>160.0</v>
       </c>
       <c r="Q25" t="n">
-        <v>9742.0</v>
+        <v>9806.0</v>
       </c>
       <c r="R25" t="n">
         <v>14.0</v>
       </c>
       <c r="S25" t="n">
-        <v>29426.0</v>
+        <v>30738.0</v>
       </c>
       <c r="T25" t="s">
         <v>127</v>
@@ -2159,7 +2159,7 @@
         <v>43400.0</v>
       </c>
       <c r="V25" t="n">
-        <v>30.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="26">
@@ -2173,22 +2173,22 @@
         <v>12.0</v>
       </c>
       <c r="D26" t="n">
-        <v>4275.0</v>
+        <v>4366.0</v>
       </c>
       <c r="E26" t="n">
-        <v>4363.0</v>
+        <v>4366.0</v>
       </c>
       <c r="F26" t="n">
-        <v>3368.0</v>
+        <v>3374.0</v>
       </c>
       <c r="G26" t="n">
-        <v>3542.0</v>
+        <v>3545.0</v>
       </c>
       <c r="H26" t="n">
-        <v>12500.0</v>
+        <v>12528.0</v>
       </c>
       <c r="I26" t="n">
-        <v>1739.0</v>
+        <v>1740.0</v>
       </c>
       <c r="J26" t="n">
         <v>2811.0</v>
@@ -2206,28 +2206,28 @@
         <v>122</v>
       </c>
       <c r="O26" t="n">
-        <v>94.0</v>
+        <v>410.0</v>
       </c>
       <c r="P26" t="n">
-        <v>80.0</v>
+        <v>210.0</v>
       </c>
       <c r="Q26" t="n">
-        <v>44363.0</v>
+        <v>44679.0</v>
       </c>
       <c r="R26" t="n">
         <v>71.0</v>
       </c>
       <c r="S26" t="n">
-        <v>81243.0</v>
+        <v>83483.0</v>
       </c>
       <c r="T26" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="U26" t="n" s="2">
         <v>43214.0</v>
       </c>
       <c r="V26" t="n">
-        <v>216.0</v>
+        <v>218.0</v>
       </c>
     </row>
     <row r="27">
@@ -2241,25 +2241,25 @@
         <v>12.0</v>
       </c>
       <c r="D27" t="n">
-        <v>4671.0</v>
+        <v>4553.0</v>
       </c>
       <c r="E27" t="n">
         <v>4699.0</v>
       </c>
       <c r="F27" t="n">
-        <v>3777.0</v>
+        <v>3803.0</v>
       </c>
       <c r="G27" t="n">
-        <v>3482.0</v>
+        <v>3515.0</v>
       </c>
       <c r="H27" t="n">
-        <v>11576.0</v>
+        <v>11640.0</v>
       </c>
       <c r="I27" t="n">
-        <v>1572.0</v>
+        <v>1578.0</v>
       </c>
       <c r="J27" t="n">
-        <v>3116.0</v>
+        <v>3119.0</v>
       </c>
       <c r="K27" t="n">
         <v>11.0</v>
@@ -2274,28 +2274,28 @@
         <v>124</v>
       </c>
       <c r="O27" t="n">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
       <c r="P27" t="n">
-        <v>0.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q27" t="n">
-        <v>32993.0</v>
+        <v>33023.0</v>
       </c>
       <c r="R27" t="n">
-        <v>66.0</v>
+        <v>67.0</v>
       </c>
       <c r="S27" t="n">
-        <v>84875.0</v>
+        <v>85995.0</v>
       </c>
       <c r="T27" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="U27" t="n" s="2">
         <v>42614.0</v>
       </c>
       <c r="V27" t="n">
-        <v>816.0</v>
+        <v>818.0</v>
       </c>
     </row>
     <row r="28">
@@ -2309,7 +2309,7 @@
         <v>10.0</v>
       </c>
       <c r="D28" t="n">
-        <v>3902.0</v>
+        <v>3828.0</v>
       </c>
       <c r="E28" t="n">
         <v>4107.0</v>
@@ -2318,13 +2318,13 @@
         <v>893.0</v>
       </c>
       <c r="G28" t="n">
-        <v>736.0</v>
+        <v>739.0</v>
       </c>
       <c r="H28" t="n">
-        <v>2666.0</v>
+        <v>2681.0</v>
       </c>
       <c r="I28" t="n">
-        <v>360.0</v>
+        <v>364.0</v>
       </c>
       <c r="J28" t="n">
         <v>1411.0</v>
@@ -2342,19 +2342,19 @@
         <v>123</v>
       </c>
       <c r="O28" t="n">
-        <v>56.0</v>
+        <v>220.0</v>
       </c>
       <c r="P28" t="n">
-        <v>40.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q28" t="n">
-        <v>11909.0</v>
+        <v>12073.0</v>
       </c>
       <c r="R28" t="n">
         <v>15.0</v>
       </c>
       <c r="S28" t="n">
-        <v>40561.0</v>
+        <v>42136.0</v>
       </c>
       <c r="T28" t="s">
         <v>127</v>
@@ -2363,7 +2363,7 @@
         <v>43423.0</v>
       </c>
       <c r="V28" t="n">
-        <v>7.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="29">
@@ -2377,19 +2377,19 @@
         <v>11.0</v>
       </c>
       <c r="D29" t="n">
-        <v>4043.0</v>
+        <v>4096.0</v>
       </c>
       <c r="E29" t="n">
         <v>4420.0</v>
       </c>
       <c r="F29" t="n">
-        <v>3109.0</v>
+        <v>3118.0</v>
       </c>
       <c r="G29" t="n">
-        <v>3083.0</v>
+        <v>3091.0</v>
       </c>
       <c r="H29" t="n">
-        <v>7816.0</v>
+        <v>7834.0</v>
       </c>
       <c r="I29" t="n">
         <v>877.0</v>
@@ -2410,19 +2410,19 @@
         <v>122</v>
       </c>
       <c r="O29" t="n">
-        <v>30.0</v>
+        <v>48.0</v>
       </c>
       <c r="P29" t="n">
         <v>40.0</v>
       </c>
       <c r="Q29" t="n">
-        <v>12676.0</v>
+        <v>12694.0</v>
       </c>
       <c r="R29" t="n">
         <v>65.0</v>
       </c>
       <c r="S29" t="n">
-        <v>71081.0</v>
+        <v>71641.0</v>
       </c>
       <c r="T29" t="s">
         <v>128</v>
@@ -2431,7 +2431,7 @@
         <v>43254.0</v>
       </c>
       <c r="V29" t="n">
-        <v>176.0</v>
+        <v>178.0</v>
       </c>
     </row>
     <row r="30">
@@ -2445,22 +2445,22 @@
         <v>11.0</v>
       </c>
       <c r="D30" t="n">
-        <v>4178.0</v>
+        <v>4143.0</v>
       </c>
       <c r="E30" t="n">
         <v>4258.0</v>
       </c>
       <c r="F30" t="n">
-        <v>1384.0</v>
+        <v>1390.0</v>
       </c>
       <c r="G30" t="n">
-        <v>1146.0</v>
+        <v>1154.0</v>
       </c>
       <c r="H30" t="n">
-        <v>6804.0</v>
+        <v>6839.0</v>
       </c>
       <c r="I30" t="n">
-        <v>1484.0</v>
+        <v>1488.0</v>
       </c>
       <c r="J30" t="n">
         <v>1878.0</v>
@@ -2478,19 +2478,19 @@
         <v>122</v>
       </c>
       <c r="O30" t="n">
-        <v>50.0</v>
+        <v>190.0</v>
       </c>
       <c r="P30" t="n">
-        <v>40.0</v>
+        <v>200.0</v>
       </c>
       <c r="Q30" t="n">
-        <v>14190.0</v>
+        <v>14330.0</v>
       </c>
       <c r="R30" t="n">
-        <v>62.0</v>
+        <v>63.0</v>
       </c>
       <c r="S30" t="n">
-        <v>84902.0</v>
+        <v>86302.0</v>
       </c>
       <c r="T30" t="s">
         <v>128</v>
@@ -2499,7 +2499,7 @@
         <v>43058.0</v>
       </c>
       <c r="V30" t="n">
-        <v>372.0</v>
+        <v>374.0</v>
       </c>
     </row>
     <row r="31">
@@ -2513,22 +2513,22 @@
         <v>10.0</v>
       </c>
       <c r="D31" t="n">
-        <v>4177.0</v>
+        <v>4054.0</v>
       </c>
       <c r="E31" t="n">
         <v>4227.0</v>
       </c>
       <c r="F31" t="n">
-        <v>705.0</v>
+        <v>717.0</v>
       </c>
       <c r="G31" t="n">
-        <v>570.0</v>
+        <v>588.0</v>
       </c>
       <c r="H31" t="n">
-        <v>3494.0</v>
+        <v>3527.0</v>
       </c>
       <c r="I31" t="n">
-        <v>759.0</v>
+        <v>764.0</v>
       </c>
       <c r="J31" t="n">
         <v>838.0</v>
@@ -2549,7 +2549,7 @@
         <v>0.0</v>
       </c>
       <c r="P31" t="n">
-        <v>10.0</v>
+        <v>90.0</v>
       </c>
       <c r="Q31" t="n">
         <v>4765.0</v>
@@ -2558,7 +2558,7 @@
         <v>54.0</v>
       </c>
       <c r="S31" t="n">
-        <v>77827.0</v>
+        <v>79227.0</v>
       </c>
       <c r="T31" t="s">
         <v>128</v>
@@ -2567,7 +2567,7 @@
         <v>43138.0</v>
       </c>
       <c r="V31" t="n">
-        <v>292.0</v>
+        <v>294.0</v>
       </c>
     </row>
     <row r="32">
@@ -2581,22 +2581,22 @@
         <v>12.0</v>
       </c>
       <c r="D32" t="n">
-        <v>4111.0</v>
+        <v>4120.0</v>
       </c>
       <c r="E32" t="n">
         <v>4190.0</v>
       </c>
       <c r="F32" t="n">
-        <v>2183.0</v>
+        <v>2186.0</v>
       </c>
       <c r="G32" t="n">
-        <v>2223.0</v>
+        <v>2226.0</v>
       </c>
       <c r="H32" t="n">
-        <v>7076.0</v>
+        <v>7093.0</v>
       </c>
       <c r="I32" t="n">
-        <v>1593.0</v>
+        <v>1596.0</v>
       </c>
       <c r="J32" t="n">
         <v>1482.0</v>
@@ -2614,19 +2614,19 @@
         <v>122</v>
       </c>
       <c r="O32" t="n">
-        <v>28.0</v>
+        <v>194.0</v>
       </c>
       <c r="P32" t="n">
-        <v>40.0</v>
+        <v>200.0</v>
       </c>
       <c r="Q32" t="n">
-        <v>43807.0</v>
+        <v>43973.0</v>
       </c>
       <c r="R32" t="n">
-        <v>40.0</v>
+        <v>41.0</v>
       </c>
       <c r="S32" t="n">
-        <v>79233.0</v>
+        <v>81193.0</v>
       </c>
       <c r="T32" t="s">
         <v>128</v>
@@ -2635,7 +2635,7 @@
         <v>42920.0</v>
       </c>
       <c r="V32" t="n">
-        <v>510.0</v>
+        <v>512.0</v>
       </c>
     </row>
     <row r="33">
@@ -2649,22 +2649,22 @@
         <v>12.0</v>
       </c>
       <c r="D33" t="n">
-        <v>4537.0</v>
+        <v>4626.0</v>
       </c>
       <c r="E33" t="n">
         <v>4798.0</v>
       </c>
       <c r="F33" t="n">
-        <v>5248.0</v>
+        <v>5272.0</v>
       </c>
       <c r="G33" t="n">
-        <v>5339.0</v>
+        <v>5361.0</v>
       </c>
       <c r="H33" t="n">
-        <v>12548.0</v>
+        <v>12598.0</v>
       </c>
       <c r="I33" t="n">
-        <v>2286.0</v>
+        <v>2297.0</v>
       </c>
       <c r="J33" t="n">
         <v>1829.0</v>
@@ -2682,28 +2682,28 @@
         <v>122</v>
       </c>
       <c r="O33" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="P33" t="n">
-        <v>0.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q33" t="n">
-        <v>59417.0</v>
+        <v>59427.0</v>
       </c>
       <c r="R33" t="n">
-        <v>31.0</v>
+        <v>32.0</v>
       </c>
       <c r="S33" t="n">
         <v>84110.0</v>
       </c>
       <c r="T33" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="U33" t="n" s="2">
         <v>43058.0</v>
       </c>
       <c r="V33" t="n">
-        <v>372.0</v>
+        <v>374.0</v>
       </c>
     </row>
     <row r="34">
@@ -2729,7 +2729,7 @@
         <v>985.0</v>
       </c>
       <c r="H34" t="n">
-        <v>4308.0</v>
+        <v>4311.0</v>
       </c>
       <c r="I34" t="n">
         <v>1011.0</v>
@@ -2750,19 +2750,19 @@
         <v>123</v>
       </c>
       <c r="O34" t="n">
-        <v>16.0</v>
+        <v>36.0</v>
       </c>
       <c r="P34" t="n">
-        <v>0.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q34" t="n">
-        <v>8573.0</v>
+        <v>8593.0</v>
       </c>
       <c r="R34" t="n">
         <v>32.0</v>
       </c>
       <c r="S34" t="n">
-        <v>70410.0</v>
+        <v>71196.0</v>
       </c>
       <c r="T34" t="s">
         <v>127</v>
@@ -2771,7 +2771,7 @@
         <v>43312.0</v>
       </c>
       <c r="V34" t="n">
-        <v>118.0</v>
+        <v>120.0</v>
       </c>
     </row>
     <row r="35">
@@ -2782,25 +2782,25 @@
         <v>105</v>
       </c>
       <c r="C35" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="D35" t="n">
-        <v>3931.0</v>
+        <v>4007.0</v>
       </c>
       <c r="E35" t="n">
         <v>4007.0</v>
       </c>
       <c r="F35" t="n">
-        <v>594.0</v>
+        <v>601.0</v>
       </c>
       <c r="G35" t="n">
-        <v>521.0</v>
+        <v>526.0</v>
       </c>
       <c r="H35" t="n">
-        <v>3550.0</v>
+        <v>3577.0</v>
       </c>
       <c r="I35" t="n">
-        <v>731.0</v>
+        <v>737.0</v>
       </c>
       <c r="J35" t="n">
         <v>289.0</v>
@@ -2818,28 +2818,28 @@
         <v>123</v>
       </c>
       <c r="O35" t="n">
-        <v>0.0</v>
+        <v>134.0</v>
       </c>
       <c r="P35" t="n">
-        <v>80.0</v>
+        <v>160.0</v>
       </c>
       <c r="Q35" t="n">
-        <v>17922.0</v>
+        <v>18056.0</v>
       </c>
       <c r="R35" t="n">
         <v>26.0</v>
       </c>
       <c r="S35" t="n">
-        <v>69310.0</v>
+        <v>72022.0</v>
       </c>
       <c r="T35" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="U35" t="n" s="2">
         <v>43274.0</v>
       </c>
       <c r="V35" t="n">
-        <v>156.0</v>
+        <v>158.0</v>
       </c>
     </row>
     <row r="36">
@@ -2853,22 +2853,22 @@
         <v>10.0</v>
       </c>
       <c r="D36" t="n">
-        <v>3996.0</v>
+        <v>3936.0</v>
       </c>
       <c r="E36" t="n">
         <v>4135.0</v>
       </c>
       <c r="F36" t="n">
-        <v>3617.0</v>
+        <v>3630.0</v>
       </c>
       <c r="G36" t="n">
-        <v>4181.0</v>
+        <v>4198.0</v>
       </c>
       <c r="H36" t="n">
-        <v>9934.0</v>
+        <v>9994.0</v>
       </c>
       <c r="I36" t="n">
-        <v>1809.0</v>
+        <v>1815.0</v>
       </c>
       <c r="J36" t="n">
         <v>239.0</v>
@@ -2886,19 +2886,19 @@
         <v>122</v>
       </c>
       <c r="O36" t="n">
-        <v>18.0</v>
+        <v>164.0</v>
       </c>
       <c r="P36" t="n">
-        <v>0.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q36" t="n">
-        <v>15324.0</v>
+        <v>15470.0</v>
       </c>
       <c r="R36" t="n">
         <v>37.0</v>
       </c>
       <c r="S36" t="n">
-        <v>78283.0</v>
+        <v>79893.0</v>
       </c>
       <c r="T36" t="s">
         <v>127</v>
@@ -2907,7 +2907,7 @@
         <v>43280.0</v>
       </c>
       <c r="V36" t="n">
-        <v>150.0</v>
+        <v>152.0</v>
       </c>
     </row>
     <row r="37">
@@ -2921,19 +2921,19 @@
         <v>9.0</v>
       </c>
       <c r="D37" t="n">
-        <v>3382.0</v>
+        <v>3442.0</v>
       </c>
       <c r="E37" t="n">
         <v>3630.0</v>
       </c>
       <c r="F37" t="n">
-        <v>340.0</v>
+        <v>342.0</v>
       </c>
       <c r="G37" t="n">
         <v>200.0</v>
       </c>
       <c r="H37" t="n">
-        <v>693.0</v>
+        <v>695.0</v>
       </c>
       <c r="I37" t="n">
         <v>133.0</v>
@@ -2954,13 +2954,13 @@
         <v>123</v>
       </c>
       <c r="O37" t="n">
-        <v>0.0</v>
+        <v>128.0</v>
       </c>
       <c r="P37" t="n">
-        <v>16.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q37" t="n">
-        <v>3223.0</v>
+        <v>3351.0</v>
       </c>
       <c r="R37" t="n">
         <v>2.0</v>
@@ -2975,7 +2975,7 @@
         <v>43360.0</v>
       </c>
       <c r="V37" t="n">
-        <v>70.0</v>
+        <v>72.0</v>
       </c>
     </row>
     <row r="38">
@@ -2998,13 +2998,13 @@
         <v>813.0</v>
       </c>
       <c r="G38" t="n">
-        <v>739.0</v>
+        <v>741.0</v>
       </c>
       <c r="H38" t="n">
-        <v>4260.0</v>
+        <v>4272.0</v>
       </c>
       <c r="I38" t="n">
-        <v>806.0</v>
+        <v>809.0</v>
       </c>
       <c r="J38" t="n">
         <v>411.0</v>
@@ -3022,19 +3022,19 @@
         <v>123</v>
       </c>
       <c r="O38" t="n">
-        <v>47.0</v>
+        <v>325.0</v>
       </c>
       <c r="P38" t="n">
-        <v>40.0</v>
+        <v>150.0</v>
       </c>
       <c r="Q38" t="n">
-        <v>12085.0</v>
+        <v>12363.0</v>
       </c>
       <c r="R38" t="n">
         <v>12.0</v>
       </c>
       <c r="S38" t="n">
-        <v>44167.0</v>
+        <v>45567.0</v>
       </c>
       <c r="T38" t="s">
         <v>128</v>
@@ -3043,7 +3043,7 @@
         <v>43430.0</v>
       </c>
       <c r="V38" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="39">
@@ -3111,7 +3111,7 @@
         <v>43284.0</v>
       </c>
       <c r="V39" t="n">
-        <v>146.0</v>
+        <v>148.0</v>
       </c>
     </row>
     <row r="40">
@@ -3125,25 +3125,25 @@
         <v>10.0</v>
       </c>
       <c r="D40" t="n">
-        <v>3899.0</v>
+        <v>3922.0</v>
       </c>
       <c r="E40" t="n">
         <v>4072.0</v>
       </c>
       <c r="F40" t="n">
-        <v>682.0</v>
+        <v>694.0</v>
       </c>
       <c r="G40" t="n">
-        <v>397.0</v>
+        <v>406.0</v>
       </c>
       <c r="H40" t="n">
-        <v>1815.0</v>
+        <v>1840.0</v>
       </c>
       <c r="I40" t="n">
-        <v>292.0</v>
+        <v>293.0</v>
       </c>
       <c r="J40" t="n">
-        <v>1227.0</v>
+        <v>1250.0</v>
       </c>
       <c r="K40" t="n">
         <v>14.0</v>
@@ -3158,19 +3158,19 @@
         <v>123</v>
       </c>
       <c r="O40" t="n">
-        <v>110.0</v>
+        <v>326.0</v>
       </c>
       <c r="P40" t="n">
-        <v>40.0</v>
+        <v>200.0</v>
       </c>
       <c r="Q40" t="n">
-        <v>8454.0</v>
+        <v>8670.0</v>
       </c>
       <c r="R40" t="n">
-        <v>20.0</v>
+        <v>21.0</v>
       </c>
       <c r="S40" t="n">
-        <v>53996.0</v>
+        <v>54520.0</v>
       </c>
       <c r="T40" t="s">
         <v>127</v>
@@ -3179,7 +3179,7 @@
         <v>43426.0</v>
       </c>
       <c r="V40" t="n">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="41">
@@ -3193,22 +3193,22 @@
         <v>10.0</v>
       </c>
       <c r="D41" t="n">
-        <v>4363.0</v>
+        <v>4426.0</v>
       </c>
       <c r="E41" t="n">
-        <v>4405.0</v>
+        <v>4482.0</v>
       </c>
       <c r="F41" t="n">
-        <v>1119.0</v>
+        <v>1123.0</v>
       </c>
       <c r="G41" t="n">
-        <v>1006.0</v>
+        <v>1008.0</v>
       </c>
       <c r="H41" t="n">
-        <v>3185.0</v>
+        <v>3193.0</v>
       </c>
       <c r="I41" t="n">
-        <v>670.0</v>
+        <v>672.0</v>
       </c>
       <c r="J41" t="n">
         <v>1702.0</v>
@@ -3226,19 +3226,19 @@
         <v>123</v>
       </c>
       <c r="O41" t="n">
-        <v>28.0</v>
+        <v>183.0</v>
       </c>
       <c r="P41" t="n">
-        <v>48.0</v>
+        <v>208.0</v>
       </c>
       <c r="Q41" t="n">
-        <v>20696.0</v>
+        <v>20851.0</v>
       </c>
       <c r="R41" t="n">
-        <v>19.0</v>
+        <v>20.0</v>
       </c>
       <c r="S41" t="n">
-        <v>60080.0</v>
+        <v>61200.0</v>
       </c>
       <c r="T41" t="s">
         <v>126</v>
@@ -3247,7 +3247,7 @@
         <v>43352.0</v>
       </c>
       <c r="V41" t="n">
-        <v>78.0</v>
+        <v>80.0</v>
       </c>
     </row>
     <row r="42">
@@ -3261,25 +3261,25 @@
         <v>11.0</v>
       </c>
       <c r="D42" t="n">
-        <v>4399.0</v>
+        <v>4557.0</v>
       </c>
       <c r="E42" t="n">
-        <v>4553.0</v>
+        <v>4557.0</v>
       </c>
       <c r="F42" t="n">
-        <v>4710.0</v>
+        <v>4786.0</v>
       </c>
       <c r="G42" t="n">
-        <v>4764.0</v>
+        <v>4842.0</v>
       </c>
       <c r="H42" t="n">
-        <v>27247.0</v>
+        <v>27429.0</v>
       </c>
       <c r="I42" t="n">
-        <v>3707.0</v>
+        <v>3718.0</v>
       </c>
       <c r="J42" t="n">
-        <v>2045.0</v>
+        <v>2047.0</v>
       </c>
       <c r="K42" t="n">
         <v>11.0</v>
@@ -3297,16 +3297,16 @@
         <v>0.0</v>
       </c>
       <c r="P42" t="n">
-        <v>40.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q42" t="n">
         <v>7130.0</v>
       </c>
       <c r="R42" t="n">
-        <v>63.0</v>
+        <v>64.0</v>
       </c>
       <c r="S42" t="n">
-        <v>82715.0</v>
+        <v>84115.0</v>
       </c>
       <c r="T42" t="s">
         <v>126</v>
@@ -3315,7 +3315,7 @@
         <v>43252.0</v>
       </c>
       <c r="V42" t="n">
-        <v>178.0</v>
+        <v>180.0</v>
       </c>
     </row>
     <row r="43">
@@ -3329,19 +3329,19 @@
         <v>11.0</v>
       </c>
       <c r="D43" t="n">
-        <v>4223.0</v>
+        <v>4254.0</v>
       </c>
       <c r="E43" t="n">
         <v>4323.0</v>
       </c>
       <c r="F43" t="n">
-        <v>2454.0</v>
+        <v>2455.0</v>
       </c>
       <c r="G43" t="n">
-        <v>2378.0</v>
+        <v>2379.0</v>
       </c>
       <c r="H43" t="n">
-        <v>6192.0</v>
+        <v>6199.0</v>
       </c>
       <c r="I43" t="n">
         <v>1200.0</v>
@@ -3362,19 +3362,19 @@
         <v>123</v>
       </c>
       <c r="O43" t="n">
-        <v>32.0</v>
+        <v>126.0</v>
       </c>
       <c r="P43" t="n">
-        <v>80.0</v>
+        <v>240.0</v>
       </c>
       <c r="Q43" t="n">
-        <v>22932.0</v>
+        <v>23026.0</v>
       </c>
       <c r="R43" t="n">
         <v>21.0</v>
       </c>
       <c r="S43" t="n">
-        <v>41012.0</v>
+        <v>41852.0</v>
       </c>
       <c r="T43" t="s">
         <v>128</v>
@@ -3383,7 +3383,7 @@
         <v>43370.0</v>
       </c>
       <c r="V43" t="n">
-        <v>60.0</v>
+        <v>62.0</v>
       </c>
     </row>
     <row r="44">
@@ -3397,22 +3397,22 @@
         <v>11.0</v>
       </c>
       <c r="D44" t="n">
-        <v>3981.0</v>
+        <v>4009.0</v>
       </c>
       <c r="E44" t="n">
         <v>4038.0</v>
       </c>
       <c r="F44" t="n">
-        <v>1314.0</v>
+        <v>1319.0</v>
       </c>
       <c r="G44" t="n">
-        <v>1145.0</v>
+        <v>1146.0</v>
       </c>
       <c r="H44" t="n">
-        <v>4428.0</v>
+        <v>4447.0</v>
       </c>
       <c r="I44" t="n">
-        <v>755.0</v>
+        <v>757.0</v>
       </c>
       <c r="J44" t="n">
         <v>1955.0</v>
@@ -3430,13 +3430,13 @@
         <v>123</v>
       </c>
       <c r="O44" t="n">
-        <v>90.0</v>
+        <v>346.0</v>
       </c>
       <c r="P44" t="n">
-        <v>40.0</v>
+        <v>240.0</v>
       </c>
       <c r="Q44" t="n">
-        <v>29651.0</v>
+        <v>29907.0</v>
       </c>
       <c r="R44" t="n">
         <v>26.0</v>
@@ -3445,13 +3445,13 @@
         <v>25830.0</v>
       </c>
       <c r="T44" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="U44" t="n" s="2">
         <v>43419.0</v>
       </c>
       <c r="V44" t="n">
-        <v>11.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="45">
@@ -3477,10 +3477,10 @@
         <v>2676.0</v>
       </c>
       <c r="H45" t="n">
-        <v>7879.0</v>
+        <v>7893.0</v>
       </c>
       <c r="I45" t="n">
-        <v>2290.0</v>
+        <v>2295.0</v>
       </c>
       <c r="J45" t="n">
         <v>2329.0</v>
@@ -3498,19 +3498,19 @@
         <v>123</v>
       </c>
       <c r="O45" t="n">
-        <v>24.0</v>
+        <v>144.0</v>
       </c>
       <c r="P45" t="n">
-        <v>80.0</v>
+        <v>160.0</v>
       </c>
       <c r="Q45" t="n">
-        <v>32088.0</v>
+        <v>32208.0</v>
       </c>
       <c r="R45" t="n">
         <v>26.0</v>
       </c>
       <c r="S45" t="n">
-        <v>33175.0</v>
+        <v>33455.0</v>
       </c>
       <c r="T45" t="s">
         <v>126</v>
@@ -3519,7 +3519,7 @@
         <v>43382.0</v>
       </c>
       <c r="V45" t="n">
-        <v>48.0</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="46">
@@ -3533,25 +3533,25 @@
         <v>11.0</v>
       </c>
       <c r="D46" t="n">
-        <v>4368.0</v>
+        <v>4431.0</v>
       </c>
       <c r="E46" t="n">
-        <v>4400.0</v>
+        <v>4431.0</v>
       </c>
       <c r="F46" t="n">
-        <v>3871.0</v>
+        <v>3878.0</v>
       </c>
       <c r="G46" t="n">
-        <v>4168.0</v>
+        <v>4173.0</v>
       </c>
       <c r="H46" t="n">
-        <v>8802.0</v>
+        <v>8817.0</v>
       </c>
       <c r="I46" t="n">
-        <v>2059.0</v>
+        <v>2062.0</v>
       </c>
       <c r="J46" t="n">
-        <v>1398.0</v>
+        <v>1403.0</v>
       </c>
       <c r="K46" t="n">
         <v>10.0</v>
@@ -3566,19 +3566,19 @@
         <v>123</v>
       </c>
       <c r="O46" t="n">
-        <v>0.0</v>
+        <v>59.0</v>
       </c>
       <c r="P46" t="n">
-        <v>0.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q46" t="n">
-        <v>23229.0</v>
+        <v>23288.0</v>
       </c>
       <c r="R46" t="n">
         <v>20.0</v>
       </c>
       <c r="S46" t="n">
-        <v>80412.0</v>
+        <v>82092.0</v>
       </c>
       <c r="T46" t="s">
         <v>126</v>
@@ -3587,7 +3587,7 @@
         <v>43390.0</v>
       </c>
       <c r="V46" t="n">
-        <v>40.0</v>
+        <v>42.0</v>
       </c>
     </row>
     <row r="47">
@@ -3601,25 +3601,25 @@
         <v>12.0</v>
       </c>
       <c r="D47" t="n">
-        <v>4295.0</v>
+        <v>4422.0</v>
       </c>
       <c r="E47" t="n">
         <v>4473.0</v>
       </c>
       <c r="F47" t="n">
-        <v>2663.0</v>
+        <v>2678.0</v>
       </c>
       <c r="G47" t="n">
-        <v>2599.0</v>
+        <v>2607.0</v>
       </c>
       <c r="H47" t="n">
-        <v>7293.0</v>
+        <v>7326.0</v>
       </c>
       <c r="I47" t="n">
-        <v>1400.0</v>
+        <v>1411.0</v>
       </c>
       <c r="J47" t="n">
-        <v>3518.0</v>
+        <v>3530.0</v>
       </c>
       <c r="K47" t="n">
         <v>10.0</v>
@@ -3634,28 +3634,28 @@
         <v>123</v>
       </c>
       <c r="O47" t="n">
-        <v>160.0</v>
+        <v>527.0</v>
       </c>
       <c r="P47" t="n">
+        <v>240.0</v>
+      </c>
+      <c r="Q47" t="n">
+        <v>51286.0</v>
+      </c>
+      <c r="R47" t="n">
         <v>40.0</v>
       </c>
-      <c r="Q47" t="n">
-        <v>50919.0</v>
-      </c>
-      <c r="R47" t="n">
-        <v>39.0</v>
-      </c>
       <c r="S47" t="n">
-        <v>49525.0</v>
+        <v>51205.0</v>
       </c>
       <c r="T47" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="U47" t="n" s="2">
         <v>43390.0</v>
       </c>
       <c r="V47" t="n">
-        <v>40.0</v>
+        <v>42.0</v>
       </c>
     </row>
     <row r="48">
@@ -3669,22 +3669,22 @@
         <v>12.0</v>
       </c>
       <c r="D48" t="n">
-        <v>4850.0</v>
+        <v>4676.0</v>
       </c>
       <c r="E48" t="n">
-        <v>4972.0</v>
+        <v>4984.0</v>
       </c>
       <c r="F48" t="n">
-        <v>11196.0</v>
+        <v>11270.0</v>
       </c>
       <c r="G48" t="n">
-        <v>11903.0</v>
+        <v>11984.0</v>
       </c>
       <c r="H48" t="n">
-        <v>26686.0</v>
+        <v>26846.0</v>
       </c>
       <c r="I48" t="n">
-        <v>9210.0</v>
+        <v>9261.0</v>
       </c>
       <c r="J48" t="n">
         <v>2228.0</v>
@@ -3702,19 +3702,19 @@
         <v>123</v>
       </c>
       <c r="O48" t="n">
-        <v>44.0</v>
+        <v>444.0</v>
       </c>
       <c r="P48" t="n">
-        <v>40.0</v>
+        <v>200.0</v>
       </c>
       <c r="Q48" t="n">
-        <v>78460.0</v>
+        <v>78860.0</v>
       </c>
       <c r="R48" t="n">
         <v>26.0</v>
       </c>
       <c r="S48" t="n">
-        <v>92535.0</v>
+        <v>93375.0</v>
       </c>
       <c r="T48" t="s">
         <v>130</v>
@@ -3723,7 +3723,7 @@
         <v>43390.0</v>
       </c>
       <c r="V48" t="n">
-        <v>40.0</v>
+        <v>42.0</v>
       </c>
     </row>
     <row r="49">
@@ -3749,10 +3749,10 @@
         <v>3047.0</v>
       </c>
       <c r="H49" t="n">
-        <v>15780.0</v>
+        <v>15805.0</v>
       </c>
       <c r="I49" t="n">
-        <v>3309.0</v>
+        <v>3312.0</v>
       </c>
       <c r="J49" t="n">
         <v>1891.0</v>
@@ -3770,19 +3770,19 @@
         <v>122</v>
       </c>
       <c r="O49" t="n">
-        <v>78.0</v>
+        <v>136.0</v>
       </c>
       <c r="P49" t="n">
-        <v>40.0</v>
+        <v>200.0</v>
       </c>
       <c r="Q49" t="n">
-        <v>34170.0</v>
+        <v>34228.0</v>
       </c>
       <c r="R49" t="n">
         <v>41.0</v>
       </c>
       <c r="S49" t="n">
-        <v>78415.0</v>
+        <v>79535.0</v>
       </c>
       <c r="T49" t="s">
         <v>128</v>
@@ -3791,7 +3791,7 @@
         <v>43230.0</v>
       </c>
       <c r="V49" t="n">
-        <v>200.0</v>
+        <v>202.0</v>
       </c>
     </row>
     <row r="50">
@@ -3805,22 +3805,22 @@
         <v>11.0</v>
       </c>
       <c r="D50" t="n">
-        <v>4148.0</v>
+        <v>4320.0</v>
       </c>
       <c r="E50" t="n">
         <v>4396.0</v>
       </c>
       <c r="F50" t="n">
-        <v>6425.0</v>
+        <v>6442.0</v>
       </c>
       <c r="G50" t="n">
-        <v>6665.0</v>
+        <v>6677.0</v>
       </c>
       <c r="H50" t="n">
-        <v>18436.0</v>
+        <v>18471.0</v>
       </c>
       <c r="I50" t="n">
-        <v>3793.0</v>
+        <v>3796.0</v>
       </c>
       <c r="J50" t="n">
         <v>4417.0</v>
@@ -3832,19 +3832,19 @@
         <v>47.0</v>
       </c>
       <c r="M50" t="n">
-        <v>485.0</v>
+        <v>505.0</v>
       </c>
       <c r="N50" t="s">
         <v>124</v>
       </c>
       <c r="O50" t="n">
-        <v>15.0</v>
+        <v>129.0</v>
       </c>
       <c r="P50" t="n">
-        <v>40.0</v>
+        <v>160.0</v>
       </c>
       <c r="Q50" t="n">
-        <v>21279.0</v>
+        <v>21393.0</v>
       </c>
       <c r="R50" t="n">
         <v>65.0</v>
@@ -3853,13 +3853,13 @@
         <v>85557.0</v>
       </c>
       <c r="T50" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="U50" t="n" s="2">
         <v>43184.0</v>
       </c>
       <c r="V50" t="n">
-        <v>246.0</v>
+        <v>248.0</v>
       </c>
     </row>
     <row r="51">
@@ -3927,7 +3927,7 @@
         <v>43314.0</v>
       </c>
       <c r="V51" t="n">
-        <v>116.0</v>
+        <v>118.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small bug squashed + data update
</commit_message>
<xml_diff>
--- a/docs/data/memberstats.xlsx
+++ b/docs/data/memberstats.xlsx
@@ -122,9 +122,6 @@
     <t>#2PUJ8JLGJ</t>
   </si>
   <si>
-    <t>#2Q28CPQC2</t>
-  </si>
-  <si>
     <t>#2Q9PULLCQ</t>
   </si>
   <si>
@@ -212,6 +209,9 @@
     <t>#GYUPYYL</t>
   </si>
   <si>
+    <t>#L2CJVVY9</t>
+  </si>
+  <si>
     <t>#L8RYLJRC</t>
   </si>
   <si>
@@ -272,9 +272,6 @@
     <t>supercell</t>
   </si>
   <si>
-    <t>RubenVski</t>
-  </si>
-  <si>
     <t>Madnasty</t>
   </si>
   <si>
@@ -360,6 +357,9 @@
   </si>
   <si>
     <t>Savler</t>
+  </si>
+  <si>
+    <t>diogo</t>
   </si>
   <si>
     <t>hugo</t>
@@ -547,16 +547,16 @@
         <v>4653.0</v>
       </c>
       <c r="F2" t="n">
-        <v>2300.0</v>
+        <v>2302.0</v>
       </c>
       <c r="G2" t="n">
-        <v>2115.0</v>
+        <v>2117.0</v>
       </c>
       <c r="H2" t="n">
-        <v>7151.0</v>
+        <v>7155.0</v>
       </c>
       <c r="I2" t="n">
-        <v>1165.0</v>
+        <v>1166.0</v>
       </c>
       <c r="J2" t="n">
         <v>2684.0</v>
@@ -574,13 +574,13 @@
         <v>122</v>
       </c>
       <c r="O2" t="n">
-        <v>96.0</v>
+        <v>122.0</v>
       </c>
       <c r="P2" t="n">
-        <v>120.0</v>
+        <v>210.0</v>
       </c>
       <c r="Q2" t="n">
-        <v>29262.0</v>
+        <v>29288.0</v>
       </c>
       <c r="R2" t="n">
         <v>49.0</v>
@@ -595,7 +595,7 @@
         <v>43302.0</v>
       </c>
       <c r="V2" t="n">
-        <v>130.0</v>
+        <v>131.0</v>
       </c>
     </row>
     <row r="3">
@@ -663,7 +663,7 @@
         <v>43372.0</v>
       </c>
       <c r="V3" t="n">
-        <v>60.0</v>
+        <v>61.0</v>
       </c>
     </row>
     <row r="4">
@@ -677,22 +677,22 @@
         <v>11.0</v>
       </c>
       <c r="D4" t="n">
-        <v>4147.0</v>
+        <v>4206.0</v>
       </c>
       <c r="E4" t="n">
         <v>4292.0</v>
       </c>
       <c r="F4" t="n">
-        <v>2698.0</v>
+        <v>2700.0</v>
       </c>
       <c r="G4" t="n">
         <v>2724.0</v>
       </c>
       <c r="H4" t="n">
-        <v>6446.0</v>
+        <v>6451.0</v>
       </c>
       <c r="I4" t="n">
-        <v>1090.0</v>
+        <v>1094.0</v>
       </c>
       <c r="J4" t="n">
         <v>1671.0</v>
@@ -710,19 +710,19 @@
         <v>122</v>
       </c>
       <c r="O4" t="n">
-        <v>62.0</v>
+        <v>82.0</v>
       </c>
       <c r="P4" t="n">
-        <v>240.0</v>
+        <v>320.0</v>
       </c>
       <c r="Q4" t="n">
-        <v>9330.0</v>
+        <v>9350.0</v>
       </c>
       <c r="R4" t="n">
         <v>52.0</v>
       </c>
       <c r="S4" t="n">
-        <v>70046.0</v>
+        <v>71726.0</v>
       </c>
       <c r="T4" t="s">
         <v>128</v>
@@ -731,7 +731,7 @@
         <v>43082.0</v>
       </c>
       <c r="V4" t="n">
-        <v>350.0</v>
+        <v>351.0</v>
       </c>
     </row>
     <row r="5">
@@ -799,7 +799,7 @@
         <v>43397.0</v>
       </c>
       <c r="V5" t="n">
-        <v>35.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="6">
@@ -846,13 +846,13 @@
         <v>123</v>
       </c>
       <c r="O6" t="n">
-        <v>126.0</v>
+        <v>174.0</v>
       </c>
       <c r="P6" t="n">
-        <v>160.0</v>
+        <v>272.0</v>
       </c>
       <c r="Q6" t="n">
-        <v>17495.0</v>
+        <v>17543.0</v>
       </c>
       <c r="R6" t="n">
         <v>30.0</v>
@@ -867,7 +867,7 @@
         <v>43356.0</v>
       </c>
       <c r="V6" t="n">
-        <v>76.0</v>
+        <v>77.0</v>
       </c>
     </row>
     <row r="7">
@@ -893,7 +893,7 @@
         <v>2695.0</v>
       </c>
       <c r="H7" t="n">
-        <v>7151.0</v>
+        <v>7152.0</v>
       </c>
       <c r="I7" t="n">
         <v>697.0</v>
@@ -926,7 +926,7 @@
         <v>47.0</v>
       </c>
       <c r="S7" t="n">
-        <v>63240.0</v>
+        <v>63800.0</v>
       </c>
       <c r="T7" t="s">
         <v>126</v>
@@ -935,7 +935,7 @@
         <v>43364.0</v>
       </c>
       <c r="V7" t="n">
-        <v>68.0</v>
+        <v>69.0</v>
       </c>
     </row>
     <row r="8">
@@ -961,10 +961,10 @@
         <v>1851.0</v>
       </c>
       <c r="H8" t="n">
-        <v>7797.0</v>
+        <v>7801.0</v>
       </c>
       <c r="I8" t="n">
-        <v>1135.0</v>
+        <v>1136.0</v>
       </c>
       <c r="J8" t="n">
         <v>1401.0</v>
@@ -985,7 +985,7 @@
         <v>161.0</v>
       </c>
       <c r="P8" t="n">
-        <v>200.0</v>
+        <v>280.0</v>
       </c>
       <c r="Q8" t="n">
         <v>25938.0</v>
@@ -994,7 +994,7 @@
         <v>60.0</v>
       </c>
       <c r="S8" t="n">
-        <v>77395.0</v>
+        <v>78515.0</v>
       </c>
       <c r="T8" t="s">
         <v>126</v>
@@ -1003,7 +1003,7 @@
         <v>43058.0</v>
       </c>
       <c r="V8" t="n">
-        <v>374.0</v>
+        <v>375.0</v>
       </c>
     </row>
     <row r="9">
@@ -1017,19 +1017,19 @@
         <v>11.0</v>
       </c>
       <c r="D9" t="n">
-        <v>4492.0</v>
+        <v>4523.0</v>
       </c>
       <c r="E9" t="n">
         <v>4634.0</v>
       </c>
       <c r="F9" t="n">
-        <v>2566.0</v>
+        <v>2568.0</v>
       </c>
       <c r="G9" t="n">
-        <v>2390.0</v>
+        <v>2391.0</v>
       </c>
       <c r="H9" t="n">
-        <v>11149.0</v>
+        <v>11156.0</v>
       </c>
       <c r="I9" t="n">
         <v>2454.0</v>
@@ -1050,19 +1050,19 @@
         <v>124</v>
       </c>
       <c r="O9" t="n">
-        <v>20.0</v>
+        <v>30.0</v>
       </c>
       <c r="P9" t="n">
-        <v>200.0</v>
+        <v>280.0</v>
       </c>
       <c r="Q9" t="n">
-        <v>3443.0</v>
+        <v>3453.0</v>
       </c>
       <c r="R9" t="n">
         <v>61.0</v>
       </c>
       <c r="S9" t="n">
-        <v>88590.0</v>
+        <v>89430.0</v>
       </c>
       <c r="T9" t="s">
         <v>126</v>
@@ -1071,7 +1071,7 @@
         <v>43123.0</v>
       </c>
       <c r="V9" t="n">
-        <v>309.0</v>
+        <v>310.0</v>
       </c>
     </row>
     <row r="10">
@@ -1091,13 +1091,13 @@
         <v>4731.0</v>
       </c>
       <c r="F10" t="n">
-        <v>2303.0</v>
+        <v>2304.0</v>
       </c>
       <c r="G10" t="n">
         <v>1780.0</v>
       </c>
       <c r="H10" t="n">
-        <v>9673.0</v>
+        <v>9683.0</v>
       </c>
       <c r="I10" t="n">
         <v>1382.0</v>
@@ -1115,22 +1115,22 @@
         <v>7.0</v>
       </c>
       <c r="N10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O10" t="n">
-        <v>279.0</v>
+        <v>371.0</v>
       </c>
       <c r="P10" t="n">
-        <v>280.0</v>
+        <v>400.0</v>
       </c>
       <c r="Q10" t="n">
-        <v>92924.0</v>
+        <v>93016.0</v>
       </c>
       <c r="R10" t="n">
         <v>82.0</v>
       </c>
       <c r="S10" t="n">
-        <v>85200.0</v>
+        <v>86320.0</v>
       </c>
       <c r="T10" t="s">
         <v>130</v>
@@ -1139,7 +1139,7 @@
         <v>43397.0</v>
       </c>
       <c r="V10" t="n">
-        <v>35.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="11">
@@ -1153,25 +1153,25 @@
         <v>11.0</v>
       </c>
       <c r="D11" t="n">
-        <v>4274.0</v>
+        <v>4306.0</v>
       </c>
       <c r="E11" t="n">
         <v>4389.0</v>
       </c>
       <c r="F11" t="n">
-        <v>1422.0</v>
+        <v>1425.0</v>
       </c>
       <c r="G11" t="n">
-        <v>1259.0</v>
+        <v>1261.0</v>
       </c>
       <c r="H11" t="n">
-        <v>5780.0</v>
+        <v>5788.0</v>
       </c>
       <c r="I11" t="n">
-        <v>796.0</v>
+        <v>799.0</v>
       </c>
       <c r="J11" t="n">
-        <v>1298.0</v>
+        <v>1301.0</v>
       </c>
       <c r="K11" t="n">
         <v>9.0</v>
@@ -1186,13 +1186,13 @@
         <v>124</v>
       </c>
       <c r="O11" t="n">
-        <v>216.0</v>
+        <v>384.0</v>
       </c>
       <c r="P11" t="n">
-        <v>190.0</v>
+        <v>300.0</v>
       </c>
       <c r="Q11" t="n">
-        <v>39797.0</v>
+        <v>39965.0</v>
       </c>
       <c r="R11" t="n">
         <v>69.0</v>
@@ -1201,13 +1201,13 @@
         <v>84240.0</v>
       </c>
       <c r="T11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="U11" t="n" s="2">
         <v>43218.0</v>
       </c>
       <c r="V11" t="n">
-        <v>214.0</v>
+        <v>215.0</v>
       </c>
     </row>
     <row r="12">
@@ -1221,25 +1221,25 @@
         <v>12.0</v>
       </c>
       <c r="D12" t="n">
-        <v>4382.0</v>
+        <v>4338.0</v>
       </c>
       <c r="E12" t="n">
         <v>4553.0</v>
       </c>
       <c r="F12" t="n">
-        <v>4747.0</v>
+        <v>4756.0</v>
       </c>
       <c r="G12" t="n">
-        <v>5147.0</v>
+        <v>5159.0</v>
       </c>
       <c r="H12" t="n">
-        <v>10996.0</v>
+        <v>11018.0</v>
       </c>
       <c r="I12" t="n">
-        <v>2112.0</v>
+        <v>2116.0</v>
       </c>
       <c r="J12" t="n">
-        <v>1862.0</v>
+        <v>1867.0</v>
       </c>
       <c r="K12" t="n">
         <v>10.0</v>
@@ -1254,13 +1254,13 @@
         <v>123</v>
       </c>
       <c r="O12" t="n">
-        <v>508.0</v>
+        <v>730.0</v>
       </c>
       <c r="P12" t="n">
-        <v>240.0</v>
+        <v>360.0</v>
       </c>
       <c r="Q12" t="n">
-        <v>56649.0</v>
+        <v>56871.0</v>
       </c>
       <c r="R12" t="n">
         <v>34.0</v>
@@ -1275,7 +1275,7 @@
         <v>43390.0</v>
       </c>
       <c r="V12" t="n">
-        <v>42.0</v>
+        <v>43.0</v>
       </c>
     </row>
     <row r="13">
@@ -1343,7 +1343,7 @@
         <v>43410.0</v>
       </c>
       <c r="V13" t="n">
-        <v>22.0</v>
+        <v>23.0</v>
       </c>
     </row>
     <row r="14">
@@ -1357,25 +1357,25 @@
         <v>11.0</v>
       </c>
       <c r="D14" t="n">
-        <v>4290.0</v>
+        <v>4238.0</v>
       </c>
       <c r="E14" t="n">
         <v>4416.0</v>
       </c>
       <c r="F14" t="n">
-        <v>2352.0</v>
+        <v>2357.0</v>
       </c>
       <c r="G14" t="n">
-        <v>2131.0</v>
+        <v>2134.0</v>
       </c>
       <c r="H14" t="n">
-        <v>6861.0</v>
+        <v>6870.0</v>
       </c>
       <c r="I14" t="n">
-        <v>1098.0</v>
+        <v>1099.0</v>
       </c>
       <c r="J14" t="n">
-        <v>3769.0</v>
+        <v>3819.0</v>
       </c>
       <c r="K14" t="n">
         <v>12.0</v>
@@ -1393,7 +1393,7 @@
         <v>0.0</v>
       </c>
       <c r="P14" t="n">
-        <v>160.0</v>
+        <v>200.0</v>
       </c>
       <c r="Q14" t="n">
         <v>20631.0</v>
@@ -1411,7 +1411,7 @@
         <v>43275.0</v>
       </c>
       <c r="V14" t="n">
-        <v>157.0</v>
+        <v>158.0</v>
       </c>
     </row>
     <row r="15">
@@ -1431,16 +1431,16 @@
         <v>4076.0</v>
       </c>
       <c r="F15" t="n">
-        <v>1537.0</v>
+        <v>1540.0</v>
       </c>
       <c r="G15" t="n">
-        <v>1463.0</v>
+        <v>1465.0</v>
       </c>
       <c r="H15" t="n">
-        <v>3687.0</v>
+        <v>3692.0</v>
       </c>
       <c r="I15" t="n">
-        <v>1012.0</v>
+        <v>1013.0</v>
       </c>
       <c r="J15" t="n">
         <v>2616.0</v>
@@ -1458,13 +1458,13 @@
         <v>122</v>
       </c>
       <c r="O15" t="n">
-        <v>68.0</v>
+        <v>146.0</v>
       </c>
       <c r="P15" t="n">
-        <v>80.0</v>
+        <v>160.0</v>
       </c>
       <c r="Q15" t="n">
-        <v>31698.0</v>
+        <v>31776.0</v>
       </c>
       <c r="R15" t="n">
         <v>20.0</v>
@@ -1479,7 +1479,7 @@
         <v>43220.0</v>
       </c>
       <c r="V15" t="n">
-        <v>212.0</v>
+        <v>213.0</v>
       </c>
     </row>
     <row r="16">
@@ -1493,61 +1493,61 @@
         <v>11.0</v>
       </c>
       <c r="D16" t="n">
-        <v>4090.0</v>
+        <v>4396.0</v>
       </c>
       <c r="E16" t="n">
-        <v>4117.0</v>
+        <v>4577.0</v>
       </c>
       <c r="F16" t="n">
-        <v>780.0</v>
+        <v>2875.0</v>
       </c>
       <c r="G16" t="n">
-        <v>732.0</v>
+        <v>2622.0</v>
       </c>
       <c r="H16" t="n">
-        <v>3182.0</v>
+        <v>6811.0</v>
       </c>
       <c r="I16" t="n">
-        <v>790.0</v>
+        <v>736.0</v>
       </c>
       <c r="J16" t="n">
-        <v>1639.0</v>
+        <v>3669.0</v>
       </c>
       <c r="K16" t="n">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="L16" t="n">
-        <v>64.0</v>
+        <v>0.0</v>
       </c>
       <c r="M16" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="N16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O16" t="n">
-        <v>0.0</v>
+        <v>98.0</v>
       </c>
       <c r="P16" t="n">
-        <v>0.0</v>
+        <v>260.0</v>
       </c>
       <c r="Q16" t="n">
-        <v>27823.0</v>
+        <v>22237.0</v>
       </c>
       <c r="R16" t="n">
-        <v>4.0</v>
+        <v>55.0</v>
       </c>
       <c r="S16" t="n">
-        <v>6545.0</v>
+        <v>87665.0</v>
       </c>
       <c r="T16" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="U16" t="n" s="2">
-        <v>43419.0</v>
+        <v>43058.0</v>
       </c>
       <c r="V16" t="n">
-        <v>13.0</v>
+        <v>375.0</v>
       </c>
     </row>
     <row r="17">
@@ -1558,64 +1558,64 @@
         <v>87</v>
       </c>
       <c r="C17" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>4405.0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>4512.0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>3052.0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>2932.0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>6966.0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>1264.0</v>
+      </c>
+      <c r="J17" t="n">
+        <v>2127.0</v>
+      </c>
+      <c r="K17" t="n">
         <v>11.0</v>
       </c>
-      <c r="D17" t="n">
-        <v>4422.0</v>
-      </c>
-      <c r="E17" t="n">
-        <v>4577.0</v>
-      </c>
-      <c r="F17" t="n">
-        <v>2868.0</v>
-      </c>
-      <c r="G17" t="n">
-        <v>2611.0</v>
-      </c>
-      <c r="H17" t="n">
-        <v>6793.0</v>
-      </c>
-      <c r="I17" t="n">
-        <v>733.0</v>
-      </c>
-      <c r="J17" t="n">
-        <v>3652.0</v>
-      </c>
-      <c r="K17" t="n">
-        <v>10.0</v>
-      </c>
       <c r="L17" t="n">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="M17" t="n">
-        <v>0.0</v>
+        <v>51.0</v>
       </c>
       <c r="N17" t="s">
         <v>122</v>
       </c>
       <c r="O17" t="n">
-        <v>50.0</v>
+        <v>266.0</v>
       </c>
       <c r="P17" t="n">
-        <v>180.0</v>
+        <v>300.0</v>
       </c>
       <c r="Q17" t="n">
-        <v>22189.0</v>
+        <v>47084.0</v>
       </c>
       <c r="R17" t="n">
-        <v>55.0</v>
+        <v>37.0</v>
       </c>
       <c r="S17" t="n">
-        <v>87665.0</v>
+        <v>59835.0</v>
       </c>
       <c r="T17" t="s">
         <v>126</v>
       </c>
       <c r="U17" t="n" s="2">
-        <v>43058.0</v>
+        <v>43312.0</v>
       </c>
       <c r="V17" t="n">
-        <v>374.0</v>
+        <v>121.0</v>
       </c>
     </row>
     <row r="18">
@@ -1626,64 +1626,64 @@
         <v>88</v>
       </c>
       <c r="C18" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>3885.0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>4059.0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1697.0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1757.0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>4472.0</v>
+      </c>
+      <c r="I18" t="n">
+        <v>658.0</v>
+      </c>
+      <c r="J18" t="n">
+        <v>3496.0</v>
+      </c>
+      <c r="K18" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="L18" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="M18" t="n">
+        <v>199.0</v>
+      </c>
+      <c r="N18" t="s">
+        <v>123</v>
+      </c>
+      <c r="O18" t="n">
+        <v>154.0</v>
+      </c>
+      <c r="P18" t="n">
+        <v>120.0</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>12936.0</v>
+      </c>
+      <c r="R18" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="S18" t="n">
+        <v>23123.0</v>
+      </c>
+      <c r="T18" t="s">
+        <v>127</v>
+      </c>
+      <c r="U18" t="n" s="2">
+        <v>43421.0</v>
+      </c>
+      <c r="V18" t="n">
         <v>12.0</v>
-      </c>
-      <c r="D18" t="n">
-        <v>4364.0</v>
-      </c>
-      <c r="E18" t="n">
-        <v>4512.0</v>
-      </c>
-      <c r="F18" t="n">
-        <v>3046.0</v>
-      </c>
-      <c r="G18" t="n">
-        <v>2926.0</v>
-      </c>
-      <c r="H18" t="n">
-        <v>6953.0</v>
-      </c>
-      <c r="I18" t="n">
-        <v>1262.0</v>
-      </c>
-      <c r="J18" t="n">
-        <v>2127.0</v>
-      </c>
-      <c r="K18" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="L18" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="M18" t="n">
-        <v>51.0</v>
-      </c>
-      <c r="N18" t="s">
-        <v>122</v>
-      </c>
-      <c r="O18" t="n">
-        <v>130.0</v>
-      </c>
-      <c r="P18" t="n">
-        <v>180.0</v>
-      </c>
-      <c r="Q18" t="n">
-        <v>46948.0</v>
-      </c>
-      <c r="R18" t="n">
-        <v>37.0</v>
-      </c>
-      <c r="S18" t="n">
-        <v>59835.0</v>
-      </c>
-      <c r="T18" t="s">
-        <v>126</v>
-      </c>
-      <c r="U18" t="n" s="2">
-        <v>43312.0</v>
-      </c>
-      <c r="V18" t="n">
-        <v>120.0</v>
       </c>
     </row>
     <row r="19">
@@ -1694,64 +1694,64 @@
         <v>89</v>
       </c>
       <c r="C19" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="D19" t="n">
-        <v>3882.0</v>
+        <v>4737.0</v>
       </c>
       <c r="E19" t="n">
-        <v>4059.0</v>
+        <v>4767.0</v>
       </c>
       <c r="F19" t="n">
-        <v>1692.0</v>
+        <v>6789.0</v>
       </c>
       <c r="G19" t="n">
-        <v>1752.0</v>
+        <v>6701.0</v>
       </c>
       <c r="H19" t="n">
-        <v>4462.0</v>
+        <v>24164.0</v>
       </c>
       <c r="I19" t="n">
-        <v>657.0</v>
+        <v>2816.0</v>
       </c>
       <c r="J19" t="n">
-        <v>3491.0</v>
+        <v>2696.0</v>
       </c>
       <c r="K19" t="n">
-        <v>8.0</v>
+        <v>10.0</v>
       </c>
       <c r="L19" t="n">
-        <v>34.0</v>
+        <v>433.0</v>
       </c>
       <c r="M19" t="n">
-        <v>199.0</v>
+        <v>2743.0</v>
       </c>
       <c r="N19" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="O19" t="n">
-        <v>134.0</v>
+        <v>590.0</v>
       </c>
       <c r="P19" t="n">
-        <v>80.0</v>
+        <v>400.0</v>
       </c>
       <c r="Q19" t="n">
-        <v>12916.0</v>
+        <v>70298.0</v>
       </c>
       <c r="R19" t="n">
-        <v>19.0</v>
+        <v>95.0</v>
       </c>
       <c r="S19" t="n">
-        <v>23123.0</v>
+        <v>94215.0</v>
       </c>
       <c r="T19" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="U19" t="n" s="2">
-        <v>43421.0</v>
+        <v>42705.0</v>
       </c>
       <c r="V19" t="n">
-        <v>11.0</v>
+        <v>728.0</v>
       </c>
     </row>
     <row r="20">
@@ -1762,64 +1762,64 @@
         <v>90</v>
       </c>
       <c r="C20" t="n">
-        <v>12.0</v>
+        <v>11.0</v>
       </c>
       <c r="D20" t="n">
-        <v>4737.0</v>
+        <v>2865.0</v>
       </c>
       <c r="E20" t="n">
-        <v>4767.0</v>
+        <v>3176.0</v>
       </c>
       <c r="F20" t="n">
-        <v>6789.0</v>
+        <v>3284.0</v>
       </c>
       <c r="G20" t="n">
-        <v>6701.0</v>
+        <v>4565.0</v>
       </c>
       <c r="H20" t="n">
-        <v>24161.0</v>
+        <v>9165.0</v>
       </c>
       <c r="I20" t="n">
-        <v>2816.0</v>
+        <v>2942.0</v>
       </c>
       <c r="J20" t="n">
-        <v>2696.0</v>
+        <v>452.0</v>
       </c>
       <c r="K20" t="n">
         <v>10.0</v>
       </c>
       <c r="L20" t="n">
-        <v>433.0</v>
+        <v>0.0</v>
       </c>
       <c r="M20" t="n">
-        <v>2731.0</v>
+        <v>0.0</v>
       </c>
       <c r="N20" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="O20" t="n">
-        <v>428.0</v>
+        <v>0.0</v>
       </c>
       <c r="P20" t="n">
-        <v>280.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q20" t="n">
-        <v>70136.0</v>
+        <v>38319.0</v>
       </c>
       <c r="R20" t="n">
-        <v>95.0</v>
+        <v>28.0</v>
       </c>
       <c r="S20" t="n">
-        <v>93655.0</v>
+        <v>46137.0</v>
       </c>
       <c r="T20" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="U20" t="n" s="2">
-        <v>42705.0</v>
+        <v>43151.0</v>
       </c>
       <c r="V20" t="n">
-        <v>727.0</v>
+        <v>282.0</v>
       </c>
     </row>
     <row r="21">
@@ -1833,25 +1833,25 @@
         <v>11.0</v>
       </c>
       <c r="D21" t="n">
-        <v>2865.0</v>
+        <v>4000.0</v>
       </c>
       <c r="E21" t="n">
-        <v>3176.0</v>
+        <v>4253.0</v>
       </c>
       <c r="F21" t="n">
-        <v>3284.0</v>
+        <v>1364.0</v>
       </c>
       <c r="G21" t="n">
-        <v>4565.0</v>
+        <v>1429.0</v>
       </c>
       <c r="H21" t="n">
-        <v>9165.0</v>
+        <v>4665.0</v>
       </c>
       <c r="I21" t="n">
-        <v>2942.0</v>
+        <v>890.0</v>
       </c>
       <c r="J21" t="n">
-        <v>452.0</v>
+        <v>507.0</v>
       </c>
       <c r="K21" t="n">
         <v>10.0</v>
@@ -1866,28 +1866,28 @@
         <v>123</v>
       </c>
       <c r="O21" t="n">
-        <v>0.0</v>
+        <v>131.0</v>
       </c>
       <c r="P21" t="n">
-        <v>0.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q21" t="n">
-        <v>38319.0</v>
+        <v>22306.0</v>
       </c>
       <c r="R21" t="n">
-        <v>28.0</v>
+        <v>29.0</v>
       </c>
       <c r="S21" t="n">
-        <v>46137.0</v>
+        <v>55138.0</v>
       </c>
       <c r="T21" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="U21" t="n" s="2">
-        <v>43151.0</v>
+        <v>43254.0</v>
       </c>
       <c r="V21" t="n">
-        <v>281.0</v>
+        <v>179.0</v>
       </c>
     </row>
     <row r="22">
@@ -1901,61 +1901,61 @@
         <v>11.0</v>
       </c>
       <c r="D22" t="n">
-        <v>4051.0</v>
+        <v>4305.0</v>
       </c>
       <c r="E22" t="n">
-        <v>4253.0</v>
+        <v>4345.0</v>
       </c>
       <c r="F22" t="n">
-        <v>1364.0</v>
+        <v>1893.0</v>
       </c>
       <c r="G22" t="n">
-        <v>1427.0</v>
+        <v>1799.0</v>
       </c>
       <c r="H22" t="n">
-        <v>4660.0</v>
+        <v>7985.0</v>
       </c>
       <c r="I22" t="n">
-        <v>890.0</v>
+        <v>2052.0</v>
       </c>
       <c r="J22" t="n">
-        <v>507.0</v>
+        <v>1562.0</v>
       </c>
       <c r="K22" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="L22" t="n">
         <v>10.0</v>
       </c>
-      <c r="L22" t="n">
-        <v>0.0</v>
-      </c>
       <c r="M22" t="n">
-        <v>0.0</v>
+        <v>11.0</v>
       </c>
       <c r="N22" t="s">
         <v>123</v>
       </c>
       <c r="O22" t="n">
-        <v>121.0</v>
+        <v>0.0</v>
       </c>
       <c r="P22" t="n">
-        <v>80.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q22" t="n">
-        <v>22296.0</v>
+        <v>55844.0</v>
       </c>
       <c r="R22" t="n">
         <v>29.0</v>
       </c>
       <c r="S22" t="n">
-        <v>54298.0</v>
+        <v>64580.0</v>
       </c>
       <c r="T22" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="U22" t="n" s="2">
-        <v>43254.0</v>
+        <v>43380.0</v>
       </c>
       <c r="V22" t="n">
-        <v>178.0</v>
+        <v>53.0</v>
       </c>
     </row>
     <row r="23">
@@ -1966,64 +1966,64 @@
         <v>93</v>
       </c>
       <c r="C23" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="D23" t="n">
-        <v>4305.0</v>
+        <v>4307.0</v>
       </c>
       <c r="E23" t="n">
-        <v>4345.0</v>
+        <v>4307.0</v>
       </c>
       <c r="F23" t="n">
-        <v>1893.0</v>
+        <v>4437.0</v>
       </c>
       <c r="G23" t="n">
-        <v>1799.0</v>
+        <v>4374.0</v>
       </c>
       <c r="H23" t="n">
-        <v>7985.0</v>
+        <v>18808.0</v>
       </c>
       <c r="I23" t="n">
-        <v>2052.0</v>
+        <v>2980.0</v>
       </c>
       <c r="J23" t="n">
-        <v>1562.0</v>
+        <v>2753.0</v>
       </c>
       <c r="K23" t="n">
         <v>11.0</v>
       </c>
       <c r="L23" t="n">
-        <v>10.0</v>
+        <v>2641.0</v>
       </c>
       <c r="M23" t="n">
-        <v>11.0</v>
+        <v>16297.0</v>
       </c>
       <c r="N23" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="O23" t="n">
-        <v>0.0</v>
+        <v>48.0</v>
       </c>
       <c r="P23" t="n">
-        <v>0.0</v>
+        <v>360.0</v>
       </c>
       <c r="Q23" t="n">
-        <v>55844.0</v>
+        <v>6602.0</v>
       </c>
       <c r="R23" t="n">
-        <v>29.0</v>
+        <v>83.0</v>
       </c>
       <c r="S23" t="n">
-        <v>64580.0</v>
+        <v>90345.0</v>
       </c>
       <c r="T23" t="s">
         <v>126</v>
       </c>
       <c r="U23" t="n" s="2">
-        <v>43380.0</v>
+        <v>42614.0</v>
       </c>
       <c r="V23" t="n">
-        <v>52.0</v>
+        <v>819.0</v>
       </c>
     </row>
     <row r="24">
@@ -2034,64 +2034,64 @@
         <v>94</v>
       </c>
       <c r="C24" t="n">
-        <v>12.0</v>
+        <v>10.0</v>
       </c>
       <c r="D24" t="n">
-        <v>4307.0</v>
+        <v>3920.0</v>
       </c>
       <c r="E24" t="n">
-        <v>4307.0</v>
+        <v>4008.0</v>
       </c>
       <c r="F24" t="n">
-        <v>4437.0</v>
+        <v>1413.0</v>
       </c>
       <c r="G24" t="n">
-        <v>4374.0</v>
+        <v>1434.0</v>
       </c>
       <c r="H24" t="n">
-        <v>18799.0</v>
+        <v>4082.0</v>
       </c>
       <c r="I24" t="n">
-        <v>2978.0</v>
+        <v>658.0</v>
       </c>
       <c r="J24" t="n">
-        <v>2753.0</v>
+        <v>835.0</v>
       </c>
       <c r="K24" t="n">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="L24" t="n">
-        <v>2641.0</v>
+        <v>0.0</v>
       </c>
       <c r="M24" t="n">
-        <v>16278.0</v>
+        <v>0.0</v>
       </c>
       <c r="N24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="O24" t="n">
-        <v>40.0</v>
+        <v>186.0</v>
       </c>
       <c r="P24" t="n">
-        <v>240.0</v>
+        <v>200.0</v>
       </c>
       <c r="Q24" t="n">
-        <v>6594.0</v>
+        <v>9816.0</v>
       </c>
       <c r="R24" t="n">
-        <v>83.0</v>
+        <v>14.0</v>
       </c>
       <c r="S24" t="n">
-        <v>90345.0</v>
+        <v>30738.0</v>
       </c>
       <c r="T24" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="U24" t="n" s="2">
-        <v>42614.0</v>
+        <v>43400.0</v>
       </c>
       <c r="V24" t="n">
-        <v>818.0</v>
+        <v>33.0</v>
       </c>
     </row>
     <row r="25">
@@ -2102,28 +2102,28 @@
         <v>95</v>
       </c>
       <c r="C25" t="n">
-        <v>10.0</v>
+        <v>12.0</v>
       </c>
       <c r="D25" t="n">
-        <v>3846.0</v>
+        <v>4366.0</v>
       </c>
       <c r="E25" t="n">
-        <v>4008.0</v>
+        <v>4366.0</v>
       </c>
       <c r="F25" t="n">
-        <v>1401.0</v>
+        <v>3379.0</v>
       </c>
       <c r="G25" t="n">
-        <v>1424.0</v>
+        <v>3551.0</v>
       </c>
       <c r="H25" t="n">
-        <v>4057.0</v>
+        <v>12551.0</v>
       </c>
       <c r="I25" t="n">
-        <v>656.0</v>
+        <v>1746.0</v>
       </c>
       <c r="J25" t="n">
-        <v>818.0</v>
+        <v>2826.0</v>
       </c>
       <c r="K25" t="n">
         <v>10.0</v>
@@ -2135,31 +2135,31 @@
         <v>0.0</v>
       </c>
       <c r="N25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O25" t="n">
-        <v>176.0</v>
+        <v>554.0</v>
       </c>
       <c r="P25" t="n">
-        <v>160.0</v>
+        <v>280.0</v>
       </c>
       <c r="Q25" t="n">
-        <v>9806.0</v>
+        <v>44823.0</v>
       </c>
       <c r="R25" t="n">
-        <v>14.0</v>
+        <v>71.0</v>
       </c>
       <c r="S25" t="n">
-        <v>30738.0</v>
+        <v>83483.0</v>
       </c>
       <c r="T25" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="U25" t="n" s="2">
-        <v>43400.0</v>
+        <v>43214.0</v>
       </c>
       <c r="V25" t="n">
-        <v>32.0</v>
+        <v>219.0</v>
       </c>
     </row>
     <row r="26">
@@ -2173,61 +2173,61 @@
         <v>12.0</v>
       </c>
       <c r="D26" t="n">
-        <v>4366.0</v>
+        <v>4505.0</v>
       </c>
       <c r="E26" t="n">
-        <v>4366.0</v>
+        <v>4699.0</v>
       </c>
       <c r="F26" t="n">
-        <v>3374.0</v>
+        <v>3812.0</v>
       </c>
       <c r="G26" t="n">
-        <v>3545.0</v>
+        <v>3526.0</v>
       </c>
       <c r="H26" t="n">
-        <v>12528.0</v>
+        <v>11660.0</v>
       </c>
       <c r="I26" t="n">
-        <v>1740.0</v>
+        <v>1582.0</v>
       </c>
       <c r="J26" t="n">
-        <v>2811.0</v>
+        <v>3119.0</v>
       </c>
       <c r="K26" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="L26" t="n">
-        <v>0.0</v>
+        <v>100.0</v>
       </c>
       <c r="M26" t="n">
-        <v>0.0</v>
+        <v>195.0</v>
       </c>
       <c r="N26" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="O26" t="n">
-        <v>410.0</v>
+        <v>55.0</v>
       </c>
       <c r="P26" t="n">
-        <v>210.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q26" t="n">
-        <v>44679.0</v>
+        <v>33048.0</v>
       </c>
       <c r="R26" t="n">
-        <v>71.0</v>
+        <v>67.0</v>
       </c>
       <c r="S26" t="n">
-        <v>83483.0</v>
+        <v>85995.0</v>
       </c>
       <c r="T26" t="s">
         <v>126</v>
       </c>
       <c r="U26" t="n" s="2">
-        <v>43214.0</v>
+        <v>42614.0</v>
       </c>
       <c r="V26" t="n">
-        <v>218.0</v>
+        <v>819.0</v>
       </c>
     </row>
     <row r="27">
@@ -2238,64 +2238,64 @@
         <v>97</v>
       </c>
       <c r="C27" t="n">
-        <v>12.0</v>
+        <v>10.0</v>
       </c>
       <c r="D27" t="n">
-        <v>4553.0</v>
+        <v>3828.0</v>
       </c>
       <c r="E27" t="n">
-        <v>4699.0</v>
+        <v>4107.0</v>
       </c>
       <c r="F27" t="n">
-        <v>3803.0</v>
+        <v>895.0</v>
       </c>
       <c r="G27" t="n">
-        <v>3515.0</v>
+        <v>742.0</v>
       </c>
       <c r="H27" t="n">
-        <v>11640.0</v>
+        <v>2691.0</v>
       </c>
       <c r="I27" t="n">
-        <v>1578.0</v>
+        <v>366.0</v>
       </c>
       <c r="J27" t="n">
-        <v>3119.0</v>
+        <v>1416.0</v>
       </c>
       <c r="K27" t="n">
-        <v>11.0</v>
+        <v>9.0</v>
       </c>
       <c r="L27" t="n">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="M27" t="n">
-        <v>195.0</v>
+        <v>6.0</v>
       </c>
       <c r="N27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="O27" t="n">
-        <v>30.0</v>
+        <v>314.0</v>
       </c>
       <c r="P27" t="n">
-        <v>40.0</v>
+        <v>200.0</v>
       </c>
       <c r="Q27" t="n">
-        <v>33023.0</v>
+        <v>12167.0</v>
       </c>
       <c r="R27" t="n">
-        <v>67.0</v>
+        <v>15.0</v>
       </c>
       <c r="S27" t="n">
-        <v>85995.0</v>
+        <v>43185.0</v>
       </c>
       <c r="T27" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="U27" t="n" s="2">
-        <v>42614.0</v>
+        <v>43423.0</v>
       </c>
       <c r="V27" t="n">
-        <v>818.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="28">
@@ -2306,64 +2306,64 @@
         <v>98</v>
       </c>
       <c r="C28" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>4185.0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>4420.0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>3124.0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>3092.0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>7844.0</v>
+      </c>
+      <c r="I28" t="n">
+        <v>877.0</v>
+      </c>
+      <c r="J28" t="n">
+        <v>2715.0</v>
+      </c>
+      <c r="K28" t="n">
         <v>10.0</v>
       </c>
-      <c r="D28" t="n">
-        <v>3828.0</v>
-      </c>
-      <c r="E28" t="n">
-        <v>4107.0</v>
-      </c>
-      <c r="F28" t="n">
-        <v>893.0</v>
-      </c>
-      <c r="G28" t="n">
-        <v>739.0</v>
-      </c>
-      <c r="H28" t="n">
-        <v>2681.0</v>
-      </c>
-      <c r="I28" t="n">
-        <v>364.0</v>
-      </c>
-      <c r="J28" t="n">
-        <v>1411.0</v>
-      </c>
-      <c r="K28" t="n">
-        <v>9.0</v>
-      </c>
       <c r="L28" t="n">
         <v>0.0</v>
       </c>
       <c r="M28" t="n">
-        <v>6.0</v>
+        <v>0.0</v>
       </c>
       <c r="N28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O28" t="n">
-        <v>220.0</v>
+        <v>48.0</v>
       </c>
       <c r="P28" t="n">
-        <v>120.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q28" t="n">
-        <v>12073.0</v>
+        <v>12694.0</v>
       </c>
       <c r="R28" t="n">
-        <v>15.0</v>
+        <v>65.0</v>
       </c>
       <c r="S28" t="n">
-        <v>42136.0</v>
+        <v>73041.0</v>
       </c>
       <c r="T28" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="U28" t="n" s="2">
-        <v>43423.0</v>
+        <v>43254.0</v>
       </c>
       <c r="V28" t="n">
-        <v>9.0</v>
+        <v>179.0</v>
       </c>
     </row>
     <row r="29">
@@ -2377,61 +2377,61 @@
         <v>11.0</v>
       </c>
       <c r="D29" t="n">
-        <v>4096.0</v>
+        <v>4121.0</v>
       </c>
       <c r="E29" t="n">
-        <v>4420.0</v>
+        <v>4258.0</v>
       </c>
       <c r="F29" t="n">
-        <v>3118.0</v>
+        <v>1393.0</v>
       </c>
       <c r="G29" t="n">
-        <v>3091.0</v>
+        <v>1158.0</v>
       </c>
       <c r="H29" t="n">
-        <v>7834.0</v>
+        <v>6858.0</v>
       </c>
       <c r="I29" t="n">
-        <v>877.0</v>
+        <v>1489.0</v>
       </c>
       <c r="J29" t="n">
-        <v>2715.0</v>
+        <v>1878.0</v>
       </c>
       <c r="K29" t="n">
         <v>10.0</v>
       </c>
       <c r="L29" t="n">
-        <v>0.0</v>
+        <v>14.0</v>
       </c>
       <c r="M29" t="n">
-        <v>0.0</v>
+        <v>21.0</v>
       </c>
       <c r="N29" t="s">
         <v>122</v>
       </c>
       <c r="O29" t="n">
-        <v>48.0</v>
+        <v>250.0</v>
       </c>
       <c r="P29" t="n">
-        <v>40.0</v>
+        <v>320.0</v>
       </c>
       <c r="Q29" t="n">
-        <v>12694.0</v>
+        <v>14390.0</v>
       </c>
       <c r="R29" t="n">
-        <v>65.0</v>
+        <v>63.0</v>
       </c>
       <c r="S29" t="n">
-        <v>71641.0</v>
+        <v>86862.0</v>
       </c>
       <c r="T29" t="s">
         <v>128</v>
       </c>
       <c r="U29" t="n" s="2">
-        <v>43254.0</v>
+        <v>43058.0</v>
       </c>
       <c r="V29" t="n">
-        <v>178.0</v>
+        <v>375.0</v>
       </c>
     </row>
     <row r="30">
@@ -2442,64 +2442,64 @@
         <v>100</v>
       </c>
       <c r="C30" t="n">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="D30" t="n">
-        <v>4143.0</v>
+        <v>4010.0</v>
       </c>
       <c r="E30" t="n">
-        <v>4258.0</v>
+        <v>4227.0</v>
       </c>
       <c r="F30" t="n">
-        <v>1390.0</v>
+        <v>720.0</v>
       </c>
       <c r="G30" t="n">
-        <v>1154.0</v>
+        <v>593.0</v>
       </c>
       <c r="H30" t="n">
-        <v>6839.0</v>
+        <v>3537.0</v>
       </c>
       <c r="I30" t="n">
-        <v>1488.0</v>
+        <v>764.0</v>
       </c>
       <c r="J30" t="n">
-        <v>1878.0</v>
+        <v>838.0</v>
       </c>
       <c r="K30" t="n">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="L30" t="n">
-        <v>14.0</v>
+        <v>0.0</v>
       </c>
       <c r="M30" t="n">
-        <v>21.0</v>
+        <v>0.0</v>
       </c>
       <c r="N30" t="s">
         <v>122</v>
       </c>
       <c r="O30" t="n">
-        <v>190.0</v>
+        <v>0.0</v>
       </c>
       <c r="P30" t="n">
-        <v>200.0</v>
+        <v>170.0</v>
       </c>
       <c r="Q30" t="n">
-        <v>14330.0</v>
+        <v>4765.0</v>
       </c>
       <c r="R30" t="n">
-        <v>63.0</v>
+        <v>54.0</v>
       </c>
       <c r="S30" t="n">
-        <v>86302.0</v>
+        <v>79227.0</v>
       </c>
       <c r="T30" t="s">
         <v>128</v>
       </c>
       <c r="U30" t="n" s="2">
-        <v>43058.0</v>
+        <v>43138.0</v>
       </c>
       <c r="V30" t="n">
-        <v>374.0</v>
+        <v>295.0</v>
       </c>
     </row>
     <row r="31">
@@ -2510,64 +2510,64 @@
         <v>101</v>
       </c>
       <c r="C31" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="D31" t="n">
+        <v>4065.0</v>
+      </c>
+      <c r="E31" t="n">
+        <v>4190.0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>2187.0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>2229.0</v>
+      </c>
+      <c r="H31" t="n">
+        <v>7100.0</v>
+      </c>
+      <c r="I31" t="n">
+        <v>1597.0</v>
+      </c>
+      <c r="J31" t="n">
+        <v>1482.0</v>
+      </c>
+      <c r="K31" t="n">
         <v>10.0</v>
       </c>
-      <c r="D31" t="n">
-        <v>4054.0</v>
-      </c>
-      <c r="E31" t="n">
-        <v>4227.0</v>
-      </c>
-      <c r="F31" t="n">
-        <v>717.0</v>
-      </c>
-      <c r="G31" t="n">
-        <v>588.0</v>
-      </c>
-      <c r="H31" t="n">
-        <v>3527.0</v>
-      </c>
-      <c r="I31" t="n">
-        <v>764.0</v>
-      </c>
-      <c r="J31" t="n">
-        <v>838.0</v>
-      </c>
-      <c r="K31" t="n">
-        <v>9.0</v>
-      </c>
       <c r="L31" t="n">
         <v>0.0</v>
       </c>
       <c r="M31" t="n">
-        <v>0.0</v>
+        <v>41.0</v>
       </c>
       <c r="N31" t="s">
         <v>122</v>
       </c>
       <c r="O31" t="n">
-        <v>0.0</v>
+        <v>270.0</v>
       </c>
       <c r="P31" t="n">
-        <v>90.0</v>
+        <v>240.0</v>
       </c>
       <c r="Q31" t="n">
-        <v>4765.0</v>
+        <v>44049.0</v>
       </c>
       <c r="R31" t="n">
-        <v>54.0</v>
+        <v>41.0</v>
       </c>
       <c r="S31" t="n">
-        <v>79227.0</v>
+        <v>81753.0</v>
       </c>
       <c r="T31" t="s">
         <v>128</v>
       </c>
       <c r="U31" t="n" s="2">
-        <v>43138.0</v>
+        <v>42920.0</v>
       </c>
       <c r="V31" t="n">
-        <v>294.0</v>
+        <v>513.0</v>
       </c>
     </row>
     <row r="32">
@@ -2581,61 +2581,61 @@
         <v>12.0</v>
       </c>
       <c r="D32" t="n">
-        <v>4120.0</v>
+        <v>4567.0</v>
       </c>
       <c r="E32" t="n">
-        <v>4190.0</v>
+        <v>4798.0</v>
       </c>
       <c r="F32" t="n">
-        <v>2186.0</v>
+        <v>5277.0</v>
       </c>
       <c r="G32" t="n">
-        <v>2226.0</v>
+        <v>5370.0</v>
       </c>
       <c r="H32" t="n">
-        <v>7093.0</v>
+        <v>12616.0</v>
       </c>
       <c r="I32" t="n">
-        <v>1596.0</v>
+        <v>2300.0</v>
       </c>
       <c r="J32" t="n">
-        <v>1482.0</v>
+        <v>1842.0</v>
       </c>
       <c r="K32" t="n">
         <v>10.0</v>
       </c>
       <c r="L32" t="n">
-        <v>0.0</v>
+        <v>31.0</v>
       </c>
       <c r="M32" t="n">
-        <v>41.0</v>
+        <v>43.0</v>
       </c>
       <c r="N32" t="s">
         <v>122</v>
       </c>
       <c r="O32" t="n">
-        <v>194.0</v>
+        <v>48.0</v>
       </c>
       <c r="P32" t="n">
-        <v>200.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q32" t="n">
-        <v>43973.0</v>
+        <v>59465.0</v>
       </c>
       <c r="R32" t="n">
-        <v>41.0</v>
+        <v>32.0</v>
       </c>
       <c r="S32" t="n">
-        <v>81193.0</v>
+        <v>85230.0</v>
       </c>
       <c r="T32" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="U32" t="n" s="2">
-        <v>42920.0</v>
+        <v>43058.0</v>
       </c>
       <c r="V32" t="n">
-        <v>512.0</v>
+        <v>375.0</v>
       </c>
     </row>
     <row r="33">
@@ -2646,64 +2646,64 @@
         <v>103</v>
       </c>
       <c r="C33" t="n">
-        <v>12.0</v>
+        <v>10.0</v>
       </c>
       <c r="D33" t="n">
-        <v>4626.0</v>
+        <v>3992.0</v>
       </c>
       <c r="E33" t="n">
-        <v>4798.0</v>
+        <v>4021.0</v>
       </c>
       <c r="F33" t="n">
-        <v>5272.0</v>
+        <v>979.0</v>
       </c>
       <c r="G33" t="n">
-        <v>5361.0</v>
+        <v>985.0</v>
       </c>
       <c r="H33" t="n">
-        <v>12598.0</v>
+        <v>4313.0</v>
       </c>
       <c r="I33" t="n">
-        <v>2297.0</v>
+        <v>1011.0</v>
       </c>
       <c r="J33" t="n">
-        <v>1829.0</v>
+        <v>302.0</v>
       </c>
       <c r="K33" t="n">
-        <v>10.0</v>
+        <v>6.0</v>
       </c>
       <c r="L33" t="n">
-        <v>31.0</v>
+        <v>0.0</v>
       </c>
       <c r="M33" t="n">
-        <v>43.0</v>
+        <v>0.0</v>
       </c>
       <c r="N33" t="s">
         <v>122</v>
       </c>
       <c r="O33" t="n">
-        <v>10.0</v>
+        <v>36.0</v>
       </c>
       <c r="P33" t="n">
-        <v>40.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q33" t="n">
-        <v>59427.0</v>
+        <v>8593.0</v>
       </c>
       <c r="R33" t="n">
         <v>32.0</v>
       </c>
       <c r="S33" t="n">
-        <v>84110.0</v>
+        <v>72246.0</v>
       </c>
       <c r="T33" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="U33" t="n" s="2">
-        <v>43058.0</v>
+        <v>43312.0</v>
       </c>
       <c r="V33" t="n">
-        <v>374.0</v>
+        <v>121.0</v>
       </c>
     </row>
     <row r="34">
@@ -2714,31 +2714,31 @@
         <v>104</v>
       </c>
       <c r="C34" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="D34" t="n">
-        <v>3992.0</v>
+        <v>4007.0</v>
       </c>
       <c r="E34" t="n">
-        <v>4021.0</v>
+        <v>4007.0</v>
       </c>
       <c r="F34" t="n">
-        <v>979.0</v>
+        <v>602.0</v>
       </c>
       <c r="G34" t="n">
-        <v>985.0</v>
+        <v>529.0</v>
       </c>
       <c r="H34" t="n">
-        <v>4311.0</v>
+        <v>3583.0</v>
       </c>
       <c r="I34" t="n">
-        <v>1011.0</v>
+        <v>738.0</v>
       </c>
       <c r="J34" t="n">
-        <v>302.0</v>
+        <v>292.0</v>
       </c>
       <c r="K34" t="n">
-        <v>6.0</v>
+        <v>9.0</v>
       </c>
       <c r="L34" t="n">
         <v>0.0</v>
@@ -2750,28 +2750,28 @@
         <v>123</v>
       </c>
       <c r="O34" t="n">
-        <v>36.0</v>
+        <v>193.0</v>
       </c>
       <c r="P34" t="n">
-        <v>80.0</v>
+        <v>238.0</v>
       </c>
       <c r="Q34" t="n">
-        <v>8593.0</v>
+        <v>18115.0</v>
       </c>
       <c r="R34" t="n">
-        <v>32.0</v>
+        <v>26.0</v>
       </c>
       <c r="S34" t="n">
-        <v>71196.0</v>
+        <v>72022.0</v>
       </c>
       <c r="T34" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="U34" t="n" s="2">
-        <v>43312.0</v>
+        <v>43274.0</v>
       </c>
       <c r="V34" t="n">
-        <v>120.0</v>
+        <v>159.0</v>
       </c>
     </row>
     <row r="35">
@@ -2782,31 +2782,31 @@
         <v>105</v>
       </c>
       <c r="C35" t="n">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="D35" t="n">
-        <v>4007.0</v>
+        <v>3878.0</v>
       </c>
       <c r="E35" t="n">
-        <v>4007.0</v>
+        <v>4135.0</v>
       </c>
       <c r="F35" t="n">
-        <v>601.0</v>
+        <v>3637.0</v>
       </c>
       <c r="G35" t="n">
-        <v>526.0</v>
+        <v>4208.0</v>
       </c>
       <c r="H35" t="n">
-        <v>3577.0</v>
+        <v>10011.0</v>
       </c>
       <c r="I35" t="n">
-        <v>737.0</v>
+        <v>1816.0</v>
       </c>
       <c r="J35" t="n">
-        <v>289.0</v>
+        <v>239.0</v>
       </c>
       <c r="K35" t="n">
-        <v>9.0</v>
+        <v>4.0</v>
       </c>
       <c r="L35" t="n">
         <v>0.0</v>
@@ -2815,31 +2815,31 @@
         <v>0.0</v>
       </c>
       <c r="N35" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O35" t="n">
-        <v>134.0</v>
+        <v>251.0</v>
       </c>
       <c r="P35" t="n">
-        <v>160.0</v>
+        <v>150.0</v>
       </c>
       <c r="Q35" t="n">
-        <v>18056.0</v>
+        <v>15557.0</v>
       </c>
       <c r="R35" t="n">
-        <v>26.0</v>
+        <v>37.0</v>
       </c>
       <c r="S35" t="n">
-        <v>72022.0</v>
+        <v>79893.0</v>
       </c>
       <c r="T35" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="U35" t="n" s="2">
-        <v>43274.0</v>
+        <v>43280.0</v>
       </c>
       <c r="V35" t="n">
-        <v>158.0</v>
+        <v>153.0</v>
       </c>
     </row>
     <row r="36">
@@ -2850,31 +2850,31 @@
         <v>106</v>
       </c>
       <c r="C36" t="n">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="D36" t="n">
-        <v>3936.0</v>
+        <v>3445.0</v>
       </c>
       <c r="E36" t="n">
-        <v>4135.0</v>
+        <v>3630.0</v>
       </c>
       <c r="F36" t="n">
-        <v>3630.0</v>
+        <v>351.0</v>
       </c>
       <c r="G36" t="n">
-        <v>4198.0</v>
+        <v>204.0</v>
       </c>
       <c r="H36" t="n">
-        <v>9994.0</v>
+        <v>711.0</v>
       </c>
       <c r="I36" t="n">
-        <v>1815.0</v>
+        <v>136.0</v>
       </c>
       <c r="J36" t="n">
-        <v>239.0</v>
+        <v>704.0</v>
       </c>
       <c r="K36" t="n">
-        <v>4.0</v>
+        <v>8.0</v>
       </c>
       <c r="L36" t="n">
         <v>0.0</v>
@@ -2883,31 +2883,31 @@
         <v>0.0</v>
       </c>
       <c r="N36" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O36" t="n">
-        <v>164.0</v>
+        <v>224.0</v>
       </c>
       <c r="P36" t="n">
-        <v>120.0</v>
+        <v>200.0</v>
       </c>
       <c r="Q36" t="n">
-        <v>15470.0</v>
+        <v>3447.0</v>
       </c>
       <c r="R36" t="n">
-        <v>37.0</v>
+        <v>2.0</v>
       </c>
       <c r="S36" t="n">
-        <v>79893.0</v>
+        <v>17516.0</v>
       </c>
       <c r="T36" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="U36" t="n" s="2">
-        <v>43280.0</v>
+        <v>43360.0</v>
       </c>
       <c r="V36" t="n">
-        <v>152.0</v>
+        <v>73.0</v>
       </c>
     </row>
     <row r="37">
@@ -2918,64 +2918,64 @@
         <v>107</v>
       </c>
       <c r="C37" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="D37" t="n">
+        <v>4018.0</v>
+      </c>
+      <c r="E37" t="n">
+        <v>4047.0</v>
+      </c>
+      <c r="F37" t="n">
+        <v>834.0</v>
+      </c>
+      <c r="G37" t="n">
+        <v>757.0</v>
+      </c>
+      <c r="H37" t="n">
+        <v>4317.0</v>
+      </c>
+      <c r="I37" t="n">
+        <v>816.0</v>
+      </c>
+      <c r="J37" t="n">
+        <v>462.0</v>
+      </c>
+      <c r="K37" t="n">
         <v>9.0</v>
       </c>
-      <c r="D37" t="n">
-        <v>3442.0</v>
-      </c>
-      <c r="E37" t="n">
-        <v>3630.0</v>
-      </c>
-      <c r="F37" t="n">
-        <v>342.0</v>
-      </c>
-      <c r="G37" t="n">
-        <v>200.0</v>
-      </c>
-      <c r="H37" t="n">
-        <v>695.0</v>
-      </c>
-      <c r="I37" t="n">
-        <v>133.0</v>
-      </c>
-      <c r="J37" t="n">
-        <v>666.0</v>
-      </c>
-      <c r="K37" t="n">
-        <v>6.0</v>
-      </c>
       <c r="L37" t="n">
         <v>0.0</v>
       </c>
       <c r="M37" t="n">
-        <v>0.0</v>
+        <v>11.0</v>
       </c>
       <c r="N37" t="s">
         <v>123</v>
       </c>
       <c r="O37" t="n">
-        <v>128.0</v>
+        <v>555.0</v>
       </c>
       <c r="P37" t="n">
-        <v>120.0</v>
+        <v>200.0</v>
       </c>
       <c r="Q37" t="n">
-        <v>3351.0</v>
+        <v>12593.0</v>
       </c>
       <c r="R37" t="n">
-        <v>2.0</v>
+        <v>12.0</v>
       </c>
       <c r="S37" t="n">
-        <v>16291.0</v>
+        <v>45567.0</v>
       </c>
       <c r="T37" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="U37" t="n" s="2">
-        <v>43360.0</v>
+        <v>43430.0</v>
       </c>
       <c r="V37" t="n">
-        <v>72.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="38">
@@ -2986,64 +2986,64 @@
         <v>108</v>
       </c>
       <c r="C38" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="D38" t="n">
-        <v>4016.0</v>
+        <v>4083.0</v>
       </c>
       <c r="E38" t="n">
-        <v>4016.0</v>
+        <v>4379.0</v>
       </c>
       <c r="F38" t="n">
-        <v>813.0</v>
+        <v>1172.0</v>
       </c>
       <c r="G38" t="n">
-        <v>741.0</v>
+        <v>1015.0</v>
       </c>
       <c r="H38" t="n">
-        <v>4272.0</v>
+        <v>4594.0</v>
       </c>
       <c r="I38" t="n">
-        <v>809.0</v>
+        <v>484.0</v>
       </c>
       <c r="J38" t="n">
-        <v>411.0</v>
+        <v>2272.0</v>
       </c>
       <c r="K38" t="n">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="L38" t="n">
-        <v>0.0</v>
+        <v>81.0</v>
       </c>
       <c r="M38" t="n">
-        <v>11.0</v>
+        <v>202.0</v>
       </c>
       <c r="N38" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O38" t="n">
-        <v>325.0</v>
+        <v>0.0</v>
       </c>
       <c r="P38" t="n">
-        <v>150.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q38" t="n">
-        <v>12363.0</v>
+        <v>26532.0</v>
       </c>
       <c r="R38" t="n">
-        <v>12.0</v>
+        <v>41.0</v>
       </c>
       <c r="S38" t="n">
-        <v>45567.0</v>
+        <v>80386.0</v>
       </c>
       <c r="T38" t="s">
         <v>128</v>
       </c>
       <c r="U38" t="n" s="2">
-        <v>43430.0</v>
+        <v>43284.0</v>
       </c>
       <c r="V38" t="n">
-        <v>2.0</v>
+        <v>149.0</v>
       </c>
     </row>
     <row r="39">
@@ -3054,64 +3054,64 @@
         <v>109</v>
       </c>
       <c r="C39" t="n">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="D39" t="n">
-        <v>4083.0</v>
+        <v>3928.0</v>
       </c>
       <c r="E39" t="n">
-        <v>4379.0</v>
+        <v>4072.0</v>
       </c>
       <c r="F39" t="n">
-        <v>1172.0</v>
+        <v>710.0</v>
       </c>
       <c r="G39" t="n">
-        <v>1015.0</v>
+        <v>412.0</v>
       </c>
       <c r="H39" t="n">
-        <v>4594.0</v>
+        <v>1864.0</v>
       </c>
       <c r="I39" t="n">
-        <v>484.0</v>
+        <v>296.0</v>
       </c>
       <c r="J39" t="n">
-        <v>2272.0</v>
+        <v>1273.0</v>
       </c>
       <c r="K39" t="n">
-        <v>8.0</v>
+        <v>14.0</v>
       </c>
       <c r="L39" t="n">
-        <v>81.0</v>
+        <v>0.0</v>
       </c>
       <c r="M39" t="n">
-        <v>202.0</v>
+        <v>0.0</v>
       </c>
       <c r="N39" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O39" t="n">
-        <v>0.0</v>
+        <v>472.0</v>
       </c>
       <c r="P39" t="n">
-        <v>0.0</v>
+        <v>240.0</v>
       </c>
       <c r="Q39" t="n">
-        <v>26532.0</v>
+        <v>8816.0</v>
       </c>
       <c r="R39" t="n">
-        <v>41.0</v>
+        <v>21.0</v>
       </c>
       <c r="S39" t="n">
-        <v>80386.0</v>
+        <v>54782.0</v>
       </c>
       <c r="T39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="U39" t="n" s="2">
-        <v>43284.0</v>
+        <v>43426.0</v>
       </c>
       <c r="V39" t="n">
-        <v>148.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="40">
@@ -3125,61 +3125,61 @@
         <v>10.0</v>
       </c>
       <c r="D40" t="n">
-        <v>3922.0</v>
+        <v>4345.0</v>
       </c>
       <c r="E40" t="n">
-        <v>4072.0</v>
+        <v>4482.0</v>
       </c>
       <c r="F40" t="n">
-        <v>694.0</v>
+        <v>1123.0</v>
       </c>
       <c r="G40" t="n">
-        <v>406.0</v>
+        <v>1011.0</v>
       </c>
       <c r="H40" t="n">
-        <v>1840.0</v>
+        <v>3196.0</v>
       </c>
       <c r="I40" t="n">
-        <v>293.0</v>
+        <v>672.0</v>
       </c>
       <c r="J40" t="n">
-        <v>1250.0</v>
+        <v>1702.0</v>
       </c>
       <c r="K40" t="n">
-        <v>14.0</v>
+        <v>7.0</v>
       </c>
       <c r="L40" t="n">
         <v>0.0</v>
       </c>
       <c r="M40" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="N40" t="s">
         <v>123</v>
       </c>
       <c r="O40" t="n">
-        <v>326.0</v>
+        <v>263.0</v>
       </c>
       <c r="P40" t="n">
-        <v>200.0</v>
+        <v>288.0</v>
       </c>
       <c r="Q40" t="n">
-        <v>8670.0</v>
+        <v>20931.0</v>
       </c>
       <c r="R40" t="n">
-        <v>21.0</v>
+        <v>20.0</v>
       </c>
       <c r="S40" t="n">
-        <v>54520.0</v>
+        <v>61200.0</v>
       </c>
       <c r="T40" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="U40" t="n" s="2">
-        <v>43426.0</v>
+        <v>43352.0</v>
       </c>
       <c r="V40" t="n">
-        <v>6.0</v>
+        <v>81.0</v>
       </c>
     </row>
     <row r="41">
@@ -3190,64 +3190,64 @@
         <v>111</v>
       </c>
       <c r="C41" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="D41" t="n">
-        <v>4426.0</v>
+        <v>4572.0</v>
       </c>
       <c r="E41" t="n">
-        <v>4482.0</v>
+        <v>4572.0</v>
       </c>
       <c r="F41" t="n">
-        <v>1123.0</v>
+        <v>4807.0</v>
       </c>
       <c r="G41" t="n">
-        <v>1008.0</v>
+        <v>4864.0</v>
       </c>
       <c r="H41" t="n">
-        <v>3193.0</v>
+        <v>27490.0</v>
       </c>
       <c r="I41" t="n">
-        <v>672.0</v>
+        <v>3729.0</v>
       </c>
       <c r="J41" t="n">
-        <v>1702.0</v>
+        <v>2055.0</v>
       </c>
       <c r="K41" t="n">
-        <v>7.0</v>
+        <v>11.0</v>
       </c>
       <c r="L41" t="n">
         <v>0.0</v>
       </c>
       <c r="M41" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="N41" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O41" t="n">
-        <v>183.0</v>
+        <v>2.0</v>
       </c>
       <c r="P41" t="n">
-        <v>208.0</v>
+        <v>200.0</v>
       </c>
       <c r="Q41" t="n">
-        <v>20851.0</v>
+        <v>7132.0</v>
       </c>
       <c r="R41" t="n">
-        <v>20.0</v>
+        <v>64.0</v>
       </c>
       <c r="S41" t="n">
-        <v>61200.0</v>
+        <v>84115.0</v>
       </c>
       <c r="T41" t="s">
         <v>126</v>
       </c>
       <c r="U41" t="n" s="2">
-        <v>43352.0</v>
+        <v>43252.0</v>
       </c>
       <c r="V41" t="n">
-        <v>80.0</v>
+        <v>181.0</v>
       </c>
     </row>
     <row r="42">
@@ -3261,25 +3261,25 @@
         <v>11.0</v>
       </c>
       <c r="D42" t="n">
-        <v>4557.0</v>
+        <v>4262.0</v>
       </c>
       <c r="E42" t="n">
-        <v>4557.0</v>
+        <v>4323.0</v>
       </c>
       <c r="F42" t="n">
-        <v>4786.0</v>
+        <v>2460.0</v>
       </c>
       <c r="G42" t="n">
-        <v>4842.0</v>
+        <v>2385.0</v>
       </c>
       <c r="H42" t="n">
-        <v>27429.0</v>
+        <v>6210.0</v>
       </c>
       <c r="I42" t="n">
-        <v>3718.0</v>
+        <v>1202.0</v>
       </c>
       <c r="J42" t="n">
-        <v>2047.0</v>
+        <v>2822.0</v>
       </c>
       <c r="K42" t="n">
         <v>11.0</v>
@@ -3291,31 +3291,31 @@
         <v>0.0</v>
       </c>
       <c r="N42" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O42" t="n">
-        <v>0.0</v>
+        <v>237.0</v>
       </c>
       <c r="P42" t="n">
-        <v>120.0</v>
+        <v>320.0</v>
       </c>
       <c r="Q42" t="n">
-        <v>7130.0</v>
+        <v>23137.0</v>
       </c>
       <c r="R42" t="n">
-        <v>64.0</v>
+        <v>21.0</v>
       </c>
       <c r="S42" t="n">
-        <v>84115.0</v>
+        <v>41852.0</v>
       </c>
       <c r="T42" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="U42" t="n" s="2">
-        <v>43252.0</v>
+        <v>43370.0</v>
       </c>
       <c r="V42" t="n">
-        <v>180.0</v>
+        <v>63.0</v>
       </c>
     </row>
     <row r="43">
@@ -3329,61 +3329,61 @@
         <v>11.0</v>
       </c>
       <c r="D43" t="n">
-        <v>4254.0</v>
+        <v>4037.0</v>
       </c>
       <c r="E43" t="n">
-        <v>4323.0</v>
+        <v>4038.0</v>
       </c>
       <c r="F43" t="n">
-        <v>2455.0</v>
+        <v>1322.0</v>
       </c>
       <c r="G43" t="n">
-        <v>2379.0</v>
+        <v>1150.0</v>
       </c>
       <c r="H43" t="n">
-        <v>6199.0</v>
+        <v>4459.0</v>
       </c>
       <c r="I43" t="n">
-        <v>1200.0</v>
+        <v>758.0</v>
       </c>
       <c r="J43" t="n">
-        <v>2822.0</v>
+        <v>1972.0</v>
       </c>
       <c r="K43" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="L43" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="M43" t="n">
         <v>11.0</v>
-      </c>
-      <c r="L43" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M43" t="n">
-        <v>0.0</v>
       </c>
       <c r="N43" t="s">
         <v>123</v>
       </c>
       <c r="O43" t="n">
-        <v>126.0</v>
+        <v>396.0</v>
       </c>
       <c r="P43" t="n">
-        <v>240.0</v>
+        <v>360.0</v>
       </c>
       <c r="Q43" t="n">
-        <v>23026.0</v>
+        <v>29957.0</v>
       </c>
       <c r="R43" t="n">
-        <v>21.0</v>
+        <v>26.0</v>
       </c>
       <c r="S43" t="n">
-        <v>41852.0</v>
+        <v>27230.0</v>
       </c>
       <c r="T43" t="s">
         <v>128</v>
       </c>
       <c r="U43" t="n" s="2">
-        <v>43370.0</v>
+        <v>43419.0</v>
       </c>
       <c r="V43" t="n">
-        <v>62.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="44">
@@ -3394,64 +3394,64 @@
         <v>114</v>
       </c>
       <c r="C44" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="D44" t="n">
-        <v>4009.0</v>
+        <v>4309.0</v>
       </c>
       <c r="E44" t="n">
-        <v>4038.0</v>
+        <v>4309.0</v>
       </c>
       <c r="F44" t="n">
-        <v>1319.0</v>
+        <v>2769.0</v>
       </c>
       <c r="G44" t="n">
-        <v>1146.0</v>
+        <v>2678.0</v>
       </c>
       <c r="H44" t="n">
-        <v>4447.0</v>
+        <v>7902.0</v>
       </c>
       <c r="I44" t="n">
-        <v>757.0</v>
+        <v>2299.0</v>
       </c>
       <c r="J44" t="n">
-        <v>1955.0</v>
+        <v>2329.0</v>
       </c>
       <c r="K44" t="n">
         <v>10.0</v>
       </c>
       <c r="L44" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="M44" t="n">
-        <v>11.0</v>
+        <v>0.0</v>
       </c>
       <c r="N44" t="s">
         <v>123</v>
       </c>
       <c r="O44" t="n">
-        <v>346.0</v>
+        <v>154.0</v>
       </c>
       <c r="P44" t="n">
         <v>240.0</v>
       </c>
       <c r="Q44" t="n">
-        <v>29907.0</v>
+        <v>32218.0</v>
       </c>
       <c r="R44" t="n">
         <v>26.0</v>
       </c>
       <c r="S44" t="n">
-        <v>25830.0</v>
+        <v>34295.0</v>
       </c>
       <c r="T44" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="U44" t="n" s="2">
-        <v>43419.0</v>
+        <v>43382.0</v>
       </c>
       <c r="V44" t="n">
-        <v>13.0</v>
+        <v>51.0</v>
       </c>
     </row>
     <row r="45">
@@ -3462,64 +3462,64 @@
         <v>115</v>
       </c>
       <c r="C45" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="D45" t="n">
+        <v>4038.0</v>
+      </c>
+      <c r="E45" t="n">
+        <v>4053.0</v>
+      </c>
+      <c r="F45" t="n">
+        <v>2386.0</v>
+      </c>
+      <c r="G45" t="n">
+        <v>2251.0</v>
+      </c>
+      <c r="H45" t="n">
+        <v>6332.0</v>
+      </c>
+      <c r="I45" t="n">
+        <v>1179.0</v>
+      </c>
+      <c r="J45" t="n">
+        <v>4212.0</v>
+      </c>
+      <c r="K45" t="n">
         <v>12.0</v>
       </c>
-      <c r="D45" t="n">
-        <v>4309.0</v>
-      </c>
-      <c r="E45" t="n">
-        <v>4309.0</v>
-      </c>
-      <c r="F45" t="n">
-        <v>2767.0</v>
-      </c>
-      <c r="G45" t="n">
-        <v>2676.0</v>
-      </c>
-      <c r="H45" t="n">
-        <v>7893.0</v>
-      </c>
-      <c r="I45" t="n">
-        <v>2295.0</v>
-      </c>
-      <c r="J45" t="n">
-        <v>2329.0</v>
-      </c>
-      <c r="K45" t="n">
-        <v>10.0</v>
-      </c>
       <c r="L45" t="n">
-        <v>0.0</v>
+        <v>278.0</v>
       </c>
       <c r="M45" t="n">
-        <v>0.0</v>
+        <v>244.0</v>
       </c>
       <c r="N45" t="s">
         <v>123</v>
       </c>
       <c r="O45" t="n">
-        <v>144.0</v>
+        <v>135.0</v>
       </c>
       <c r="P45" t="n">
-        <v>160.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q45" t="n">
-        <v>32208.0</v>
+        <v>38495.0</v>
       </c>
       <c r="R45" t="n">
-        <v>26.0</v>
+        <v>0.0</v>
       </c>
       <c r="S45" t="n">
-        <v>33455.0</v>
+        <v>2220.0</v>
       </c>
       <c r="T45" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="U45" t="n" s="2">
-        <v>43382.0</v>
+        <v>43432.0</v>
       </c>
       <c r="V45" t="n">
-        <v>50.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="46">
@@ -3539,19 +3539,19 @@
         <v>4431.0</v>
       </c>
       <c r="F46" t="n">
-        <v>3878.0</v>
+        <v>3879.0</v>
       </c>
       <c r="G46" t="n">
-        <v>4173.0</v>
+        <v>4178.0</v>
       </c>
       <c r="H46" t="n">
-        <v>8817.0</v>
+        <v>8823.0</v>
       </c>
       <c r="I46" t="n">
         <v>2062.0</v>
       </c>
       <c r="J46" t="n">
-        <v>1403.0</v>
+        <v>1405.0</v>
       </c>
       <c r="K46" t="n">
         <v>10.0</v>
@@ -3566,13 +3566,13 @@
         <v>123</v>
       </c>
       <c r="O46" t="n">
-        <v>59.0</v>
+        <v>143.0</v>
       </c>
       <c r="P46" t="n">
-        <v>80.0</v>
+        <v>160.0</v>
       </c>
       <c r="Q46" t="n">
-        <v>23288.0</v>
+        <v>23372.0</v>
       </c>
       <c r="R46" t="n">
         <v>20.0</v>
@@ -3587,7 +3587,7 @@
         <v>43390.0</v>
       </c>
       <c r="V46" t="n">
-        <v>42.0</v>
+        <v>43.0</v>
       </c>
     </row>
     <row r="47">
@@ -3601,25 +3601,25 @@
         <v>12.0</v>
       </c>
       <c r="D47" t="n">
-        <v>4422.0</v>
+        <v>4399.0</v>
       </c>
       <c r="E47" t="n">
         <v>4473.0</v>
       </c>
       <c r="F47" t="n">
-        <v>2678.0</v>
+        <v>2686.0</v>
       </c>
       <c r="G47" t="n">
-        <v>2607.0</v>
+        <v>2615.0</v>
       </c>
       <c r="H47" t="n">
-        <v>7326.0</v>
+        <v>7343.0</v>
       </c>
       <c r="I47" t="n">
-        <v>1411.0</v>
+        <v>1415.0</v>
       </c>
       <c r="J47" t="n">
-        <v>3530.0</v>
+        <v>3559.0</v>
       </c>
       <c r="K47" t="n">
         <v>10.0</v>
@@ -3631,16 +3631,16 @@
         <v>149.0</v>
       </c>
       <c r="N47" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O47" t="n">
-        <v>527.0</v>
+        <v>708.0</v>
       </c>
       <c r="P47" t="n">
-        <v>240.0</v>
+        <v>360.0</v>
       </c>
       <c r="Q47" t="n">
-        <v>51286.0</v>
+        <v>51467.0</v>
       </c>
       <c r="R47" t="n">
         <v>40.0</v>
@@ -3655,7 +3655,7 @@
         <v>43390.0</v>
       </c>
       <c r="V47" t="n">
-        <v>42.0</v>
+        <v>43.0</v>
       </c>
     </row>
     <row r="48">
@@ -3669,22 +3669,22 @@
         <v>12.0</v>
       </c>
       <c r="D48" t="n">
-        <v>4676.0</v>
+        <v>4735.0</v>
       </c>
       <c r="E48" t="n">
         <v>4984.0</v>
       </c>
       <c r="F48" t="n">
-        <v>11270.0</v>
+        <v>11298.0</v>
       </c>
       <c r="G48" t="n">
-        <v>11984.0</v>
+        <v>12010.0</v>
       </c>
       <c r="H48" t="n">
-        <v>26846.0</v>
+        <v>26915.0</v>
       </c>
       <c r="I48" t="n">
-        <v>9261.0</v>
+        <v>9284.0</v>
       </c>
       <c r="J48" t="n">
         <v>2228.0</v>
@@ -3699,22 +3699,22 @@
         <v>8.0</v>
       </c>
       <c r="N48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O48" t="n">
-        <v>444.0</v>
+        <v>674.0</v>
       </c>
       <c r="P48" t="n">
-        <v>200.0</v>
+        <v>280.0</v>
       </c>
       <c r="Q48" t="n">
-        <v>78860.0</v>
+        <v>79090.0</v>
       </c>
       <c r="R48" t="n">
         <v>26.0</v>
       </c>
       <c r="S48" t="n">
-        <v>93375.0</v>
+        <v>94775.0</v>
       </c>
       <c r="T48" t="s">
         <v>130</v>
@@ -3723,7 +3723,7 @@
         <v>43390.0</v>
       </c>
       <c r="V48" t="n">
-        <v>42.0</v>
+        <v>43.0</v>
       </c>
     </row>
     <row r="49">
@@ -3749,10 +3749,10 @@
         <v>3047.0</v>
       </c>
       <c r="H49" t="n">
-        <v>15805.0</v>
+        <v>15813.0</v>
       </c>
       <c r="I49" t="n">
-        <v>3312.0</v>
+        <v>3314.0</v>
       </c>
       <c r="J49" t="n">
         <v>1891.0</v>
@@ -3770,13 +3770,13 @@
         <v>122</v>
       </c>
       <c r="O49" t="n">
-        <v>136.0</v>
+        <v>252.0</v>
       </c>
       <c r="P49" t="n">
-        <v>200.0</v>
+        <v>280.0</v>
       </c>
       <c r="Q49" t="n">
-        <v>34228.0</v>
+        <v>34344.0</v>
       </c>
       <c r="R49" t="n">
         <v>41.0</v>
@@ -3791,7 +3791,7 @@
         <v>43230.0</v>
       </c>
       <c r="V49" t="n">
-        <v>202.0</v>
+        <v>203.0</v>
       </c>
     </row>
     <row r="50">
@@ -3811,19 +3811,19 @@
         <v>4396.0</v>
       </c>
       <c r="F50" t="n">
-        <v>6442.0</v>
+        <v>6449.0</v>
       </c>
       <c r="G50" t="n">
-        <v>6677.0</v>
+        <v>6684.0</v>
       </c>
       <c r="H50" t="n">
-        <v>18471.0</v>
+        <v>18491.0</v>
       </c>
       <c r="I50" t="n">
-        <v>3796.0</v>
+        <v>3800.0</v>
       </c>
       <c r="J50" t="n">
-        <v>4417.0</v>
+        <v>4428.0</v>
       </c>
       <c r="K50" t="n">
         <v>10.0</v>
@@ -3838,19 +3838,19 @@
         <v>124</v>
       </c>
       <c r="O50" t="n">
-        <v>129.0</v>
+        <v>175.0</v>
       </c>
       <c r="P50" t="n">
-        <v>160.0</v>
+        <v>280.0</v>
       </c>
       <c r="Q50" t="n">
-        <v>21393.0</v>
+        <v>21439.0</v>
       </c>
       <c r="R50" t="n">
         <v>65.0</v>
       </c>
       <c r="S50" t="n">
-        <v>85557.0</v>
+        <v>86957.0</v>
       </c>
       <c r="T50" t="s">
         <v>126</v>
@@ -3859,7 +3859,7 @@
         <v>43184.0</v>
       </c>
       <c r="V50" t="n">
-        <v>248.0</v>
+        <v>249.0</v>
       </c>
     </row>
     <row r="51">
@@ -3885,13 +3885,13 @@
         <v>6157.0</v>
       </c>
       <c r="H51" t="n">
-        <v>14074.0</v>
+        <v>14075.0</v>
       </c>
       <c r="I51" t="n">
         <v>2666.0</v>
       </c>
       <c r="J51" t="n">
-        <v>6586.0</v>
+        <v>6588.0</v>
       </c>
       <c r="K51" t="n">
         <v>10.0</v>
@@ -3909,7 +3909,7 @@
         <v>0.0</v>
       </c>
       <c r="P51" t="n">
-        <v>0.0</v>
+        <v>40.0</v>
       </c>
       <c r="Q51" t="n">
         <v>47001.0</v>
@@ -3918,7 +3918,7 @@
         <v>30.0</v>
       </c>
       <c r="S51" t="n">
-        <v>45400.0</v>
+        <v>45960.0</v>
       </c>
       <c r="T51" t="s">
         <v>126</v>
@@ -3927,7 +3927,7 @@
         <v>43314.0</v>
       </c>
       <c r="V51" t="n">
-        <v>118.0</v>
+        <v>119.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data update + Remove battle misses from performance score
</commit_message>
<xml_diff>
--- a/docs/data/memberstats.xlsx
+++ b/docs/data/memberstats.xlsx
@@ -128,15 +128,15 @@
     <t>#2UVYQPG2J</t>
   </si>
   <si>
-    <t>#2V80YRPPV</t>
-  </si>
-  <si>
     <t>#2VQPQJGCU</t>
   </si>
   <si>
     <t>#2YGVGG2YU</t>
   </si>
   <si>
+    <t>#80YYLLL9J</t>
+  </si>
+  <si>
     <t>#828Q2QRQ</t>
   </si>
   <si>
@@ -164,6 +164,9 @@
     <t>#8VJC8LL9</t>
   </si>
   <si>
+    <t>#8VJYGGUPC</t>
+  </si>
+  <si>
     <t>#8YQ829JPL</t>
   </si>
   <si>
@@ -206,9 +209,6 @@
     <t>#GYUPYYL</t>
   </si>
   <si>
-    <t>#L8RYLJRC</t>
-  </si>
-  <si>
     <t>#LGURPQV8</t>
   </si>
   <si>
@@ -278,15 +278,15 @@
     <t>bascenso</t>
   </si>
   <si>
-    <t>Manu</t>
-  </si>
-  <si>
     <t>thunder</t>
   </si>
   <si>
     <t>Pp</t>
   </si>
   <si>
+    <t>Olakas</t>
+  </si>
+  <si>
     <t>King Bonixe</t>
   </si>
   <si>
@@ -314,6 +314,9 @@
     <t>huracan</t>
   </si>
   <si>
+    <t>Akof</t>
+  </si>
+  <si>
     <t>casanova</t>
   </si>
   <si>
@@ -395,13 +398,10 @@
     <t>Master I</t>
   </si>
   <si>
-    <t>Master II</t>
+    <t>Challenger II</t>
   </si>
   <si>
     <t>Legendary Arena</t>
-  </si>
-  <si>
-    <t>Challenger II</t>
   </si>
 </sst>
 </file>
@@ -535,22 +535,22 @@
         <v>12.0</v>
       </c>
       <c r="D2" t="n">
-        <v>4827.0</v>
+        <v>4684.0</v>
       </c>
       <c r="E2" t="n">
-        <v>4827.0</v>
+        <v>5108.0</v>
       </c>
       <c r="F2" t="n">
-        <v>2654.0</v>
+        <v>2677.0</v>
       </c>
       <c r="G2" t="n">
-        <v>2423.0</v>
+        <v>2438.0</v>
       </c>
       <c r="H2" t="n">
-        <v>8311.0</v>
+        <v>8366.0</v>
       </c>
       <c r="I2" t="n">
-        <v>1342.0</v>
+        <v>1350.0</v>
       </c>
       <c r="J2" t="n">
         <v>2987.0</v>
@@ -562,34 +562,34 @@
         <v>0.0</v>
       </c>
       <c r="M2" t="n">
-        <v>154.0</v>
+        <v>163.0</v>
       </c>
       <c r="N2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="O2" t="n">
-        <v>96.0</v>
+        <v>160.0</v>
       </c>
       <c r="P2" t="n">
-        <v>120.0</v>
+        <v>320.0</v>
       </c>
       <c r="Q2" t="n">
-        <v>38464.0</v>
+        <v>38774.0</v>
       </c>
       <c r="R2" t="n">
-        <v>83.0</v>
+        <v>86.0</v>
       </c>
       <c r="S2" t="n">
-        <v>187700.0</v>
+        <v>194849.0</v>
       </c>
       <c r="T2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="U2" t="n" s="2">
         <v>43302.0</v>
       </c>
       <c r="V2" t="n">
-        <v>284.0</v>
+        <v>295.0</v>
       </c>
     </row>
     <row r="3">
@@ -600,28 +600,28 @@
         <v>73</v>
       </c>
       <c r="C3" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="D3" t="n">
-        <v>4779.0</v>
+        <v>4690.0</v>
       </c>
       <c r="E3" t="n">
-        <v>4910.0</v>
+        <v>5027.0</v>
       </c>
       <c r="F3" t="n">
-        <v>3184.0</v>
+        <v>3241.0</v>
       </c>
       <c r="G3" t="n">
-        <v>3206.0</v>
+        <v>3278.0</v>
       </c>
       <c r="H3" t="n">
-        <v>7707.0</v>
+        <v>7860.0</v>
       </c>
       <c r="I3" t="n">
-        <v>1290.0</v>
+        <v>1310.0</v>
       </c>
       <c r="J3" t="n">
-        <v>1989.0</v>
+        <v>1994.0</v>
       </c>
       <c r="K3" t="n">
         <v>12.0</v>
@@ -630,34 +630,34 @@
         <v>0.0</v>
       </c>
       <c r="M3" t="n">
-        <v>110.0</v>
+        <v>119.0</v>
       </c>
       <c r="N3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O3" t="n">
-        <v>30.0</v>
+        <v>62.0</v>
       </c>
       <c r="P3" t="n">
-        <v>240.0</v>
+        <v>560.0</v>
       </c>
       <c r="Q3" t="n">
-        <v>12440.0</v>
+        <v>12582.0</v>
       </c>
       <c r="R3" t="n">
-        <v>88.0</v>
+        <v>91.0</v>
       </c>
       <c r="S3" t="n">
-        <v>154187.0</v>
+        <v>161281.0</v>
       </c>
       <c r="T3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="U3" t="n" s="2">
         <v>43082.0</v>
       </c>
       <c r="V3" t="n">
-        <v>504.0</v>
+        <v>515.0</v>
       </c>
     </row>
     <row r="4">
@@ -671,22 +671,22 @@
         <v>11.0</v>
       </c>
       <c r="D4" t="n">
-        <v>4651.0</v>
+        <v>4691.0</v>
       </c>
       <c r="E4" t="n">
-        <v>4651.0</v>
+        <v>4912.0</v>
       </c>
       <c r="F4" t="n">
-        <v>1523.0</v>
+        <v>1556.0</v>
       </c>
       <c r="G4" t="n">
-        <v>1577.0</v>
+        <v>1594.0</v>
       </c>
       <c r="H4" t="n">
-        <v>4360.0</v>
+        <v>4427.0</v>
       </c>
       <c r="I4" t="n">
-        <v>658.0</v>
+        <v>672.0</v>
       </c>
       <c r="J4" t="n">
         <v>387.0</v>
@@ -701,31 +701,31 @@
         <v>59.0</v>
       </c>
       <c r="N4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="O4" t="n">
-        <v>152.0</v>
+        <v>327.0</v>
       </c>
       <c r="P4" t="n">
-        <v>240.0</v>
+        <v>520.0</v>
       </c>
       <c r="Q4" t="n">
-        <v>26996.0</v>
+        <v>27699.0</v>
       </c>
       <c r="R4" t="n">
-        <v>44.0</v>
+        <v>46.0</v>
       </c>
       <c r="S4" t="n">
-        <v>118797.0</v>
+        <v>125917.0</v>
       </c>
       <c r="T4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="U4" t="n" s="2">
         <v>43356.0</v>
       </c>
       <c r="V4" t="n">
-        <v>230.0</v>
+        <v>241.0</v>
       </c>
     </row>
     <row r="5">
@@ -739,22 +739,22 @@
         <v>11.0</v>
       </c>
       <c r="D5" t="n">
-        <v>5057.0</v>
+        <v>4807.0</v>
       </c>
       <c r="E5" t="n">
         <v>5135.0</v>
       </c>
       <c r="F5" t="n">
-        <v>3461.0</v>
+        <v>3493.0</v>
       </c>
       <c r="G5" t="n">
-        <v>2988.0</v>
+        <v>3006.0</v>
       </c>
       <c r="H5" t="n">
-        <v>8136.0</v>
+        <v>8199.0</v>
       </c>
       <c r="I5" t="n">
-        <v>812.0</v>
+        <v>821.0</v>
       </c>
       <c r="J5" t="n">
         <v>4912.0</v>
@@ -766,25 +766,25 @@
         <v>52.0</v>
       </c>
       <c r="M5" t="n">
-        <v>367.0</v>
+        <v>409.0</v>
       </c>
       <c r="N5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="O5" t="n">
         <v>0.0</v>
       </c>
       <c r="P5" t="n">
-        <v>70.0</v>
+        <v>320.0</v>
       </c>
       <c r="Q5" t="n">
         <v>4066.0</v>
       </c>
       <c r="R5" t="n">
-        <v>84.0</v>
+        <v>86.0</v>
       </c>
       <c r="S5" t="n">
-        <v>151046.0</v>
+        <v>157492.0</v>
       </c>
       <c r="T5" t="s">
         <v>126</v>
@@ -793,7 +793,7 @@
         <v>43364.0</v>
       </c>
       <c r="V5" t="n">
-        <v>222.0</v>
+        <v>233.0</v>
       </c>
     </row>
     <row r="6">
@@ -807,22 +807,22 @@
         <v>12.0</v>
       </c>
       <c r="D6" t="n">
-        <v>5114.0</v>
+        <v>5080.0</v>
       </c>
       <c r="E6" t="n">
-        <v>5114.0</v>
+        <v>5147.0</v>
       </c>
       <c r="F6" t="n">
-        <v>2509.0</v>
+        <v>2546.0</v>
       </c>
       <c r="G6" t="n">
-        <v>2361.0</v>
+        <v>2386.0</v>
       </c>
       <c r="H6" t="n">
-        <v>9566.0</v>
+        <v>9643.0</v>
       </c>
       <c r="I6" t="n">
-        <v>1355.0</v>
+        <v>1363.0</v>
       </c>
       <c r="J6" t="n">
         <v>1634.0</v>
@@ -837,31 +837,31 @@
         <v>161.0</v>
       </c>
       <c r="N6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O6" t="n">
-        <v>40.0</v>
+        <v>321.0</v>
       </c>
       <c r="P6" t="n">
         <v>240.0</v>
       </c>
       <c r="Q6" t="n">
-        <v>35972.0</v>
+        <v>36331.0</v>
       </c>
       <c r="R6" t="n">
         <v>96.0</v>
       </c>
       <c r="S6" t="n">
-        <v>165482.0</v>
+        <v>169601.0</v>
       </c>
       <c r="T6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="U6" t="n" s="2">
         <v>43058.0</v>
       </c>
       <c r="V6" t="n">
-        <v>528.0</v>
+        <v>539.0</v>
       </c>
     </row>
     <row r="7">
@@ -875,22 +875,22 @@
         <v>12.0</v>
       </c>
       <c r="D7" t="n">
-        <v>5045.0</v>
+        <v>5020.0</v>
       </c>
       <c r="E7" t="n">
-        <v>5045.0</v>
+        <v>5088.0</v>
       </c>
       <c r="F7" t="n">
-        <v>2121.0</v>
+        <v>2174.0</v>
       </c>
       <c r="G7" t="n">
-        <v>1928.0</v>
+        <v>1978.0</v>
       </c>
       <c r="H7" t="n">
-        <v>11059.0</v>
+        <v>11209.0</v>
       </c>
       <c r="I7" t="n">
-        <v>2138.0</v>
+        <v>2156.0</v>
       </c>
       <c r="J7" t="n">
         <v>1815.0</v>
@@ -902,34 +902,34 @@
         <v>0.0</v>
       </c>
       <c r="M7" t="n">
-        <v>140.0</v>
+        <v>149.0</v>
       </c>
       <c r="N7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="O7" t="n">
-        <v>223.0</v>
+        <v>532.0</v>
       </c>
       <c r="P7" t="n">
-        <v>260.0</v>
+        <v>680.0</v>
       </c>
       <c r="Q7" t="n">
-        <v>61801.0</v>
+        <v>62701.0</v>
       </c>
       <c r="R7" t="n">
-        <v>53.0</v>
+        <v>56.0</v>
       </c>
       <c r="S7" t="n">
-        <v>129064.0</v>
+        <v>137889.0</v>
       </c>
       <c r="T7" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="U7" t="n" s="2">
         <v>43549.0</v>
       </c>
       <c r="V7" t="n">
-        <v>37.0</v>
+        <v>48.0</v>
       </c>
     </row>
     <row r="8">
@@ -943,22 +943,22 @@
         <v>12.0</v>
       </c>
       <c r="D8" t="n">
-        <v>5155.0</v>
+        <v>5206.0</v>
       </c>
       <c r="E8" t="n">
-        <v>5254.0</v>
+        <v>5525.0</v>
       </c>
       <c r="F8" t="n">
-        <v>3694.0</v>
+        <v>3803.0</v>
       </c>
       <c r="G8" t="n">
-        <v>3541.0</v>
+        <v>3652.0</v>
       </c>
       <c r="H8" t="n">
-        <v>14542.0</v>
+        <v>14802.0</v>
       </c>
       <c r="I8" t="n">
-        <v>3036.0</v>
+        <v>3063.0</v>
       </c>
       <c r="J8" t="n">
         <v>2334.0</v>
@@ -970,34 +970,34 @@
         <v>0.0</v>
       </c>
       <c r="M8" t="n">
-        <v>193.0</v>
+        <v>206.0</v>
       </c>
       <c r="N8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O8" t="n">
-        <v>378.0</v>
+        <v>1024.0</v>
       </c>
       <c r="P8" t="n">
-        <v>200.0</v>
+        <v>720.0</v>
       </c>
       <c r="Q8" t="n">
-        <v>7737.0</v>
+        <v>9412.0</v>
       </c>
       <c r="R8" t="n">
-        <v>99.0</v>
+        <v>103.0</v>
       </c>
       <c r="S8" t="n">
-        <v>193182.0</v>
+        <v>202881.0</v>
       </c>
       <c r="T8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="U8" t="n" s="2">
         <v>43123.0</v>
       </c>
       <c r="V8" t="n">
-        <v>463.0</v>
+        <v>474.0</v>
       </c>
     </row>
     <row r="9">
@@ -1011,22 +1011,22 @@
         <v>13.0</v>
       </c>
       <c r="D9" t="n">
-        <v>5259.0</v>
+        <v>5032.0</v>
       </c>
       <c r="E9" t="n">
-        <v>5281.0</v>
+        <v>5468.0</v>
       </c>
       <c r="F9" t="n">
-        <v>2628.0</v>
+        <v>2655.0</v>
       </c>
       <c r="G9" t="n">
-        <v>1967.0</v>
+        <v>1974.0</v>
       </c>
       <c r="H9" t="n">
-        <v>11701.0</v>
+        <v>11863.0</v>
       </c>
       <c r="I9" t="n">
-        <v>1535.0</v>
+        <v>1545.0</v>
       </c>
       <c r="J9" t="n">
         <v>4600.0</v>
@@ -1038,34 +1038,34 @@
         <v>0.0</v>
       </c>
       <c r="M9" t="n">
-        <v>166.0</v>
+        <v>178.0</v>
       </c>
       <c r="N9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O9" t="n">
-        <v>478.0</v>
+        <v>1394.0</v>
       </c>
       <c r="P9" t="n">
-        <v>280.0</v>
+        <v>720.0</v>
       </c>
       <c r="Q9" t="n">
-        <v>128952.0</v>
+        <v>131448.0</v>
       </c>
       <c r="R9" t="n">
-        <v>136.0</v>
+        <v>138.0</v>
       </c>
       <c r="S9" t="n">
-        <v>173726.0</v>
+        <v>180356.0</v>
       </c>
       <c r="T9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="U9" t="n" s="2">
         <v>43397.0</v>
       </c>
       <c r="V9" t="n">
-        <v>189.0</v>
+        <v>200.0</v>
       </c>
     </row>
     <row r="10">
@@ -1079,22 +1079,22 @@
         <v>12.0</v>
       </c>
       <c r="D10" t="n">
-        <v>5141.0</v>
+        <v>4893.0</v>
       </c>
       <c r="E10" t="n">
-        <v>5141.0</v>
+        <v>5285.0</v>
       </c>
       <c r="F10" t="n">
-        <v>7528.0</v>
+        <v>7572.0</v>
       </c>
       <c r="G10" t="n">
-        <v>7365.0</v>
+        <v>7410.0</v>
       </c>
       <c r="H10" t="n">
-        <v>19597.0</v>
+        <v>19706.0</v>
       </c>
       <c r="I10" t="n">
-        <v>4191.0</v>
+        <v>4201.0</v>
       </c>
       <c r="J10" t="n">
         <v>2312.0</v>
@@ -1109,22 +1109,22 @@
         <v>240.0</v>
       </c>
       <c r="N10" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="O10" t="n">
-        <v>10.0</v>
+        <v>106.0</v>
       </c>
       <c r="P10" t="n">
         <v>0.0</v>
       </c>
       <c r="Q10" t="n">
-        <v>82924.0</v>
+        <v>83070.0</v>
       </c>
       <c r="R10" t="n">
-        <v>86.0</v>
+        <v>89.0</v>
       </c>
       <c r="S10" t="n">
-        <v>243623.0</v>
+        <v>250905.0</v>
       </c>
       <c r="T10" t="s">
         <v>126</v>
@@ -1133,7 +1133,7 @@
         <v>43493.0</v>
       </c>
       <c r="V10" t="n">
-        <v>93.0</v>
+        <v>104.0</v>
       </c>
     </row>
     <row r="11">
@@ -1147,22 +1147,22 @@
         <v>12.0</v>
       </c>
       <c r="D11" t="n">
-        <v>5026.0</v>
+        <v>4854.0</v>
       </c>
       <c r="E11" t="n">
         <v>5026.0</v>
       </c>
       <c r="F11" t="n">
-        <v>1946.0</v>
+        <v>1967.0</v>
       </c>
       <c r="G11" t="n">
-        <v>1698.0</v>
+        <v>1715.0</v>
       </c>
       <c r="H11" t="n">
-        <v>8215.0</v>
+        <v>8313.0</v>
       </c>
       <c r="I11" t="n">
-        <v>1158.0</v>
+        <v>1187.0</v>
       </c>
       <c r="J11" t="n">
         <v>1721.0</v>
@@ -1174,25 +1174,25 @@
         <v>0.0</v>
       </c>
       <c r="M11" t="n">
-        <v>177.0</v>
+        <v>187.0</v>
       </c>
       <c r="N11" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O11" t="n">
-        <v>258.0</v>
+        <v>556.0</v>
       </c>
       <c r="P11" t="n">
-        <v>280.0</v>
+        <v>480.0</v>
       </c>
       <c r="Q11" t="n">
-        <v>61749.0</v>
+        <v>62671.0</v>
       </c>
       <c r="R11" t="n">
-        <v>108.0</v>
+        <v>111.0</v>
       </c>
       <c r="S11" t="n">
-        <v>171481.0</v>
+        <v>178767.0</v>
       </c>
       <c r="T11" t="s">
         <v>126</v>
@@ -1201,7 +1201,7 @@
         <v>43218.0</v>
       </c>
       <c r="V11" t="n">
-        <v>368.0</v>
+        <v>379.0</v>
       </c>
     </row>
     <row r="12">
@@ -1215,22 +1215,22 @@
         <v>13.0</v>
       </c>
       <c r="D12" t="n">
-        <v>5233.0</v>
+        <v>4981.0</v>
       </c>
       <c r="E12" t="n">
-        <v>5261.0</v>
+        <v>5357.0</v>
       </c>
       <c r="F12" t="n">
-        <v>5740.0</v>
+        <v>5864.0</v>
       </c>
       <c r="G12" t="n">
-        <v>6221.0</v>
+        <v>6378.0</v>
       </c>
       <c r="H12" t="n">
-        <v>13651.0</v>
+        <v>13970.0</v>
       </c>
       <c r="I12" t="n">
-        <v>2662.0</v>
+        <v>2714.0</v>
       </c>
       <c r="J12" t="n">
         <v>2359.0</v>
@@ -1242,25 +1242,25 @@
         <v>4.0</v>
       </c>
       <c r="M12" t="n">
-        <v>203.0</v>
+        <v>215.0</v>
       </c>
       <c r="N12" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O12" t="n">
-        <v>950.0</v>
+        <v>2228.0</v>
       </c>
       <c r="P12" t="n">
-        <v>280.0</v>
+        <v>760.0</v>
       </c>
       <c r="Q12" t="n">
-        <v>96101.0</v>
+        <v>99694.0</v>
       </c>
       <c r="R12" t="n">
-        <v>77.0</v>
+        <v>78.0</v>
       </c>
       <c r="S12" t="n">
-        <v>188499.0</v>
+        <v>197254.0</v>
       </c>
       <c r="T12" t="s">
         <v>126</v>
@@ -1269,7 +1269,7 @@
         <v>43390.0</v>
       </c>
       <c r="V12" t="n">
-        <v>196.0</v>
+        <v>207.0</v>
       </c>
     </row>
     <row r="13">
@@ -1283,22 +1283,22 @@
         <v>12.0</v>
       </c>
       <c r="D13" t="n">
-        <v>4986.0</v>
+        <v>4834.0</v>
       </c>
       <c r="E13" t="n">
-        <v>5029.0</v>
+        <v>5079.0</v>
       </c>
       <c r="F13" t="n">
-        <v>3313.0</v>
+        <v>3354.0</v>
       </c>
       <c r="G13" t="n">
-        <v>3013.0</v>
+        <v>3047.0</v>
       </c>
       <c r="H13" t="n">
-        <v>9074.0</v>
+        <v>9157.0</v>
       </c>
       <c r="I13" t="n">
-        <v>1268.0</v>
+        <v>1277.0</v>
       </c>
       <c r="J13" t="n">
         <v>4542.0</v>
@@ -1310,34 +1310,34 @@
         <v>1200.0</v>
       </c>
       <c r="M13" t="n">
-        <v>226.0</v>
+        <v>237.0</v>
       </c>
       <c r="N13" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="O13" t="n">
-        <v>40.0</v>
+        <v>108.0</v>
       </c>
       <c r="P13" t="n">
-        <v>200.0</v>
+        <v>520.0</v>
       </c>
       <c r="Q13" t="n">
-        <v>22410.0</v>
+        <v>22618.0</v>
       </c>
       <c r="R13" t="n">
-        <v>71.0</v>
+        <v>73.0</v>
       </c>
       <c r="S13" t="n">
-        <v>102541.0</v>
+        <v>105341.0</v>
       </c>
       <c r="T13" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="U13" t="n" s="2">
         <v>43275.0</v>
       </c>
       <c r="V13" t="n">
-        <v>311.0</v>
+        <v>322.0</v>
       </c>
     </row>
     <row r="14">
@@ -1351,22 +1351,22 @@
         <v>12.0</v>
       </c>
       <c r="D14" t="n">
-        <v>5121.0</v>
+        <v>4923.0</v>
       </c>
       <c r="E14" t="n">
-        <v>5170.0</v>
+        <v>5367.0</v>
       </c>
       <c r="F14" t="n">
-        <v>2370.0</v>
+        <v>2416.0</v>
       </c>
       <c r="G14" t="n">
-        <v>2347.0</v>
+        <v>2378.0</v>
       </c>
       <c r="H14" t="n">
-        <v>7962.0</v>
+        <v>8059.0</v>
       </c>
       <c r="I14" t="n">
-        <v>1561.0</v>
+        <v>1571.0</v>
       </c>
       <c r="J14" t="n">
         <v>969.0</v>
@@ -1378,25 +1378,25 @@
         <v>0.0</v>
       </c>
       <c r="M14" t="n">
-        <v>118.0</v>
+        <v>129.0</v>
       </c>
       <c r="N14" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="O14" t="n">
-        <v>504.0</v>
+        <v>754.0</v>
       </c>
       <c r="P14" t="n">
-        <v>280.0</v>
+        <v>557.0</v>
       </c>
       <c r="Q14" t="n">
-        <v>71228.0</v>
+        <v>72736.0</v>
       </c>
       <c r="R14" t="n">
         <v>57.0</v>
       </c>
       <c r="S14" t="n">
-        <v>176947.0</v>
+        <v>185720.0</v>
       </c>
       <c r="T14" t="s">
         <v>126</v>
@@ -1405,7 +1405,7 @@
         <v>43494.0</v>
       </c>
       <c r="V14" t="n">
-        <v>92.0</v>
+        <v>103.0</v>
       </c>
     </row>
     <row r="15">
@@ -1419,22 +1419,22 @@
         <v>12.0</v>
       </c>
       <c r="D15" t="n">
-        <v>5104.0</v>
+        <v>5005.0</v>
       </c>
       <c r="E15" t="n">
-        <v>5225.0</v>
+        <v>5240.0</v>
       </c>
       <c r="F15" t="n">
-        <v>3907.0</v>
+        <v>3998.0</v>
       </c>
       <c r="G15" t="n">
-        <v>3704.0</v>
+        <v>3796.0</v>
       </c>
       <c r="H15" t="n">
-        <v>9388.0</v>
+        <v>9593.0</v>
       </c>
       <c r="I15" t="n">
-        <v>1045.0</v>
+        <v>1062.0</v>
       </c>
       <c r="J15" t="n">
         <v>4096.0</v>
@@ -1446,34 +1446,34 @@
         <v>0.0</v>
       </c>
       <c r="M15" t="n">
-        <v>151.0</v>
+        <v>160.0</v>
       </c>
       <c r="N15" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O15" t="n">
-        <v>214.0</v>
+        <v>341.0</v>
       </c>
       <c r="P15" t="n">
-        <v>200.0</v>
+        <v>520.0</v>
       </c>
       <c r="Q15" t="n">
-        <v>30672.0</v>
+        <v>31303.0</v>
       </c>
       <c r="R15" t="n">
-        <v>93.0</v>
+        <v>95.0</v>
       </c>
       <c r="S15" t="n">
-        <v>188642.0</v>
+        <v>196672.0</v>
       </c>
       <c r="T15" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="U15" t="n" s="2">
         <v>43058.0</v>
       </c>
       <c r="V15" t="n">
-        <v>528.0</v>
+        <v>539.0</v>
       </c>
     </row>
     <row r="16">
@@ -1487,22 +1487,22 @@
         <v>12.0</v>
       </c>
       <c r="D16" t="n">
-        <v>5213.0</v>
+        <v>5041.0</v>
       </c>
       <c r="E16" t="n">
-        <v>5256.0</v>
+        <v>5327.0</v>
       </c>
       <c r="F16" t="n">
-        <v>3554.0</v>
+        <v>3597.0</v>
       </c>
       <c r="G16" t="n">
-        <v>3420.0</v>
+        <v>3454.0</v>
       </c>
       <c r="H16" t="n">
-        <v>8437.0</v>
+        <v>8527.0</v>
       </c>
       <c r="I16" t="n">
-        <v>1571.0</v>
+        <v>1591.0</v>
       </c>
       <c r="J16" t="n">
         <v>2307.0</v>
@@ -1514,34 +1514,34 @@
         <v>8.0</v>
       </c>
       <c r="M16" t="n">
-        <v>173.0</v>
+        <v>181.0</v>
       </c>
       <c r="N16" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="O16" t="n">
-        <v>196.0</v>
+        <v>274.0</v>
       </c>
       <c r="P16" t="n">
-        <v>200.0</v>
+        <v>400.0</v>
       </c>
       <c r="Q16" t="n">
-        <v>56932.0</v>
+        <v>57400.0</v>
       </c>
       <c r="R16" t="n">
-        <v>82.0</v>
+        <v>86.0</v>
       </c>
       <c r="S16" t="n">
-        <v>148899.0</v>
+        <v>155063.0</v>
       </c>
       <c r="T16" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="U16" t="n" s="2">
         <v>43312.0</v>
       </c>
       <c r="V16" t="n">
-        <v>274.0</v>
+        <v>285.0</v>
       </c>
     </row>
     <row r="17">
@@ -1555,22 +1555,22 @@
         <v>13.0</v>
       </c>
       <c r="D17" t="n">
-        <v>5492.0</v>
+        <v>5106.0</v>
       </c>
       <c r="E17" t="n">
-        <v>5492.0</v>
+        <v>5644.0</v>
       </c>
       <c r="F17" t="n">
-        <v>7435.0</v>
+        <v>7501.0</v>
       </c>
       <c r="G17" t="n">
-        <v>7228.0</v>
+        <v>7285.0</v>
       </c>
       <c r="H17" t="n">
-        <v>27417.0</v>
+        <v>27671.0</v>
       </c>
       <c r="I17" t="n">
-        <v>3335.0</v>
+        <v>3362.0</v>
       </c>
       <c r="J17" t="n">
         <v>2974.0</v>
@@ -1582,25 +1582,25 @@
         <v>433.0</v>
       </c>
       <c r="M17" t="n">
-        <v>5006.0</v>
+        <v>5060.0</v>
       </c>
       <c r="N17" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="O17" t="n">
-        <v>487.0</v>
+        <v>747.0</v>
       </c>
       <c r="P17" t="n">
-        <v>280.0</v>
+        <v>640.0</v>
       </c>
       <c r="Q17" t="n">
-        <v>97967.0</v>
+        <v>99444.0</v>
       </c>
       <c r="R17" t="n">
-        <v>152.0</v>
+        <v>158.0</v>
       </c>
       <c r="S17" t="n">
-        <v>194171.0</v>
+        <v>204000.0</v>
       </c>
       <c r="T17" t="s">
         <v>127</v>
@@ -1609,7 +1609,7 @@
         <v>42705.0</v>
       </c>
       <c r="V17" t="n">
-        <v>881.0</v>
+        <v>892.0</v>
       </c>
     </row>
     <row r="18">
@@ -1623,61 +1623,61 @@
         <v>12.0</v>
       </c>
       <c r="D18" t="n">
-        <v>4178.0</v>
+        <v>4773.0</v>
       </c>
       <c r="E18" t="n">
-        <v>4353.0</v>
+        <v>5012.0</v>
       </c>
       <c r="F18" t="n">
-        <v>4230.0</v>
+        <v>4689.0</v>
       </c>
       <c r="G18" t="n">
-        <v>5875.0</v>
+        <v>4551.0</v>
       </c>
       <c r="H18" t="n">
-        <v>11694.0</v>
+        <v>22044.0</v>
       </c>
       <c r="I18" t="n">
-        <v>3841.0</v>
+        <v>3678.0</v>
       </c>
       <c r="J18" t="n">
-        <v>543.0</v>
+        <v>2996.0</v>
       </c>
       <c r="K18" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="L18" t="n">
-        <v>0.0</v>
+        <v>2641.0</v>
       </c>
       <c r="M18" t="n">
-        <v>78.0</v>
+        <v>18627.0</v>
       </c>
       <c r="N18" t="s">
         <v>123</v>
       </c>
       <c r="O18" t="n">
-        <v>0.0</v>
+        <v>44.0</v>
       </c>
       <c r="P18" t="n">
-        <v>0.0</v>
+        <v>800.0</v>
       </c>
       <c r="Q18" t="n">
-        <v>48623.0</v>
+        <v>7610.0</v>
       </c>
       <c r="R18" t="n">
-        <v>44.0</v>
+        <v>142.0</v>
       </c>
       <c r="S18" t="n">
-        <v>105009.0</v>
+        <v>197636.0</v>
       </c>
       <c r="T18" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="U18" t="n" s="2">
-        <v>43151.0</v>
+        <v>42614.0</v>
       </c>
       <c r="V18" t="n">
-        <v>435.0</v>
+        <v>983.0</v>
       </c>
     </row>
     <row r="19">
@@ -1691,61 +1691,61 @@
         <v>12.0</v>
       </c>
       <c r="D19" t="n">
-        <v>4601.0</v>
+        <v>4932.0</v>
       </c>
       <c r="E19" t="n">
-        <v>4601.0</v>
+        <v>5142.0</v>
       </c>
       <c r="F19" t="n">
-        <v>4659.0</v>
+        <v>3886.0</v>
       </c>
       <c r="G19" t="n">
-        <v>4545.0</v>
+        <v>4437.0</v>
       </c>
       <c r="H19" t="n">
-        <v>21821.0</v>
+        <v>15185.0</v>
       </c>
       <c r="I19" t="n">
-        <v>3628.0</v>
+        <v>3459.0</v>
       </c>
       <c r="J19" t="n">
-        <v>2996.0</v>
+        <v>1719.0</v>
       </c>
       <c r="K19" t="n">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="L19" t="n">
-        <v>2641.0</v>
+        <v>0.0</v>
       </c>
       <c r="M19" t="n">
-        <v>18492.0</v>
+        <v>133.0</v>
       </c>
       <c r="N19" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="O19" t="n">
-        <v>0.0</v>
+        <v>944.0</v>
       </c>
       <c r="P19" t="n">
-        <v>280.0</v>
+        <v>600.0</v>
       </c>
       <c r="Q19" t="n">
-        <v>7556.0</v>
+        <v>43914.0</v>
       </c>
       <c r="R19" t="n">
-        <v>138.0</v>
+        <v>37.0</v>
       </c>
       <c r="S19" t="n">
-        <v>188945.0</v>
+        <v>103475.0</v>
       </c>
       <c r="T19" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="U19" t="n" s="2">
-        <v>42614.0</v>
+        <v>43536.0</v>
       </c>
       <c r="V19" t="n">
-        <v>972.0</v>
+        <v>61.0</v>
       </c>
     </row>
     <row r="20">
@@ -1756,64 +1756,64 @@
         <v>90</v>
       </c>
       <c r="C20" t="n">
-        <v>12.0</v>
+        <v>11.0</v>
       </c>
       <c r="D20" t="n">
-        <v>5018.0</v>
+        <v>4891.0</v>
       </c>
       <c r="E20" t="n">
-        <v>5018.0</v>
+        <v>5098.0</v>
       </c>
       <c r="F20" t="n">
-        <v>3768.0</v>
+        <v>2451.0</v>
       </c>
       <c r="G20" t="n">
-        <v>4283.0</v>
+        <v>2558.0</v>
       </c>
       <c r="H20" t="n">
-        <v>14820.0</v>
+        <v>6599.0</v>
       </c>
       <c r="I20" t="n">
-        <v>3417.0</v>
+        <v>1270.0</v>
       </c>
       <c r="J20" t="n">
-        <v>1719.0</v>
+        <v>952.0</v>
       </c>
       <c r="K20" t="n">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="L20" t="n">
-        <v>0.0</v>
+        <v>15.0</v>
       </c>
       <c r="M20" t="n">
-        <v>125.0</v>
+        <v>162.0</v>
       </c>
       <c r="N20" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="O20" t="n">
-        <v>228.0</v>
+        <v>272.0</v>
       </c>
       <c r="P20" t="n">
-        <v>200.0</v>
+        <v>240.0</v>
       </c>
       <c r="Q20" t="n">
-        <v>42495.0</v>
+        <v>22001.0</v>
       </c>
       <c r="R20" t="n">
-        <v>35.0</v>
+        <v>51.0</v>
       </c>
       <c r="S20" t="n">
-        <v>93806.0</v>
+        <v>106341.0</v>
       </c>
       <c r="T20" t="s">
         <v>126</v>
       </c>
       <c r="U20" t="n" s="2">
-        <v>43536.0</v>
+        <v>43593.0</v>
       </c>
       <c r="V20" t="n">
-        <v>50.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="21">
@@ -1827,22 +1827,22 @@
         <v>12.0</v>
       </c>
       <c r="D21" t="n">
-        <v>5017.0</v>
+        <v>5021.0</v>
       </c>
       <c r="E21" t="n">
-        <v>5017.0</v>
+        <v>5104.0</v>
       </c>
       <c r="F21" t="n">
-        <v>5100.0</v>
+        <v>5141.0</v>
       </c>
       <c r="G21" t="n">
-        <v>4809.0</v>
+        <v>4844.0</v>
       </c>
       <c r="H21" t="n">
-        <v>14994.0</v>
+        <v>15186.0</v>
       </c>
       <c r="I21" t="n">
-        <v>2005.0</v>
+        <v>2040.0</v>
       </c>
       <c r="J21" t="n">
         <v>3530.0</v>
@@ -1854,34 +1854,34 @@
         <v>100.0</v>
       </c>
       <c r="M21" t="n">
-        <v>449.0</v>
+        <v>502.0</v>
       </c>
       <c r="N21" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O21" t="n">
-        <v>156.0</v>
+        <v>164.0</v>
       </c>
       <c r="P21" t="n">
-        <v>200.0</v>
+        <v>150.0</v>
       </c>
       <c r="Q21" t="n">
-        <v>37209.0</v>
+        <v>37685.0</v>
       </c>
       <c r="R21" t="n">
-        <v>113.0</v>
+        <v>115.0</v>
       </c>
       <c r="S21" t="n">
-        <v>182139.0</v>
+        <v>191573.0</v>
       </c>
       <c r="T21" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="U21" t="n" s="2">
         <v>42614.0</v>
       </c>
       <c r="V21" t="n">
-        <v>972.0</v>
+        <v>983.0</v>
       </c>
     </row>
     <row r="22">
@@ -1895,25 +1895,25 @@
         <v>12.0</v>
       </c>
       <c r="D22" t="n">
-        <v>5005.0</v>
+        <v>4721.0</v>
       </c>
       <c r="E22" t="n">
-        <v>5005.0</v>
+        <v>5056.0</v>
       </c>
       <c r="F22" t="n">
-        <v>2072.0</v>
+        <v>2090.0</v>
       </c>
       <c r="G22" t="n">
-        <v>1870.0</v>
+        <v>1889.0</v>
       </c>
       <c r="H22" t="n">
-        <v>7037.0</v>
+        <v>7105.0</v>
       </c>
       <c r="I22" t="n">
-        <v>1365.0</v>
+        <v>1373.0</v>
       </c>
       <c r="J22" t="n">
-        <v>2475.0</v>
+        <v>2480.0</v>
       </c>
       <c r="K22" t="n">
         <v>11.0</v>
@@ -1922,25 +1922,25 @@
         <v>0.0</v>
       </c>
       <c r="M22" t="n">
-        <v>70.0</v>
+        <v>76.0</v>
       </c>
       <c r="N22" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="O22" t="n">
-        <v>337.0</v>
+        <v>296.0</v>
       </c>
       <c r="P22" t="n">
-        <v>160.0</v>
+        <v>480.0</v>
       </c>
       <c r="Q22" t="n">
-        <v>51886.0</v>
+        <v>52572.0</v>
       </c>
       <c r="R22" t="n">
-        <v>95.0</v>
+        <v>100.0</v>
       </c>
       <c r="S22" t="n">
-        <v>143728.0</v>
+        <v>152575.0</v>
       </c>
       <c r="T22" t="s">
         <v>126</v>
@@ -1949,7 +1949,7 @@
         <v>43284.0</v>
       </c>
       <c r="V22" t="n">
-        <v>302.0</v>
+        <v>313.0</v>
       </c>
     </row>
     <row r="23">
@@ -1963,22 +1963,22 @@
         <v>12.0</v>
       </c>
       <c r="D23" t="n">
-        <v>5005.0</v>
+        <v>4854.0</v>
       </c>
       <c r="E23" t="n">
         <v>5005.0</v>
       </c>
       <c r="F23" t="n">
-        <v>2587.0</v>
+        <v>2606.0</v>
       </c>
       <c r="G23" t="n">
-        <v>2392.0</v>
+        <v>2405.0</v>
       </c>
       <c r="H23" t="n">
-        <v>7627.0</v>
+        <v>7706.0</v>
       </c>
       <c r="I23" t="n">
-        <v>1049.0</v>
+        <v>1058.0</v>
       </c>
       <c r="J23" t="n">
         <v>2492.0</v>
@@ -1993,22 +1993,22 @@
         <v>67.0</v>
       </c>
       <c r="N23" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="O23" t="n">
-        <v>78.0</v>
+        <v>163.0</v>
       </c>
       <c r="P23" t="n">
-        <v>120.0</v>
+        <v>360.0</v>
       </c>
       <c r="Q23" t="n">
-        <v>29052.0</v>
+        <v>29344.0</v>
       </c>
       <c r="R23" t="n">
-        <v>84.0</v>
+        <v>88.0</v>
       </c>
       <c r="S23" t="n">
-        <v>131775.0</v>
+        <v>139993.0</v>
       </c>
       <c r="T23" t="s">
         <v>126</v>
@@ -2017,7 +2017,7 @@
         <v>43546.0</v>
       </c>
       <c r="V23" t="n">
-        <v>40.0</v>
+        <v>51.0</v>
       </c>
     </row>
     <row r="24">
@@ -2031,22 +2031,22 @@
         <v>12.0</v>
       </c>
       <c r="D24" t="n">
-        <v>4421.0</v>
+        <v>4730.0</v>
       </c>
       <c r="E24" t="n">
-        <v>4436.0</v>
+        <v>4787.0</v>
       </c>
       <c r="F24" t="n">
-        <v>1649.0</v>
+        <v>1685.0</v>
       </c>
       <c r="G24" t="n">
-        <v>1406.0</v>
+        <v>1421.0</v>
       </c>
       <c r="H24" t="n">
-        <v>8371.0</v>
+        <v>8437.0</v>
       </c>
       <c r="I24" t="n">
-        <v>1829.0</v>
+        <v>1842.0</v>
       </c>
       <c r="J24" t="n">
         <v>2322.0</v>
@@ -2058,34 +2058,34 @@
         <v>14.0</v>
       </c>
       <c r="M24" t="n">
-        <v>150.0</v>
+        <v>157.0</v>
       </c>
       <c r="N24" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="O24" t="n">
-        <v>18.0</v>
+        <v>107.0</v>
       </c>
       <c r="P24" t="n">
-        <v>160.0</v>
+        <v>440.0</v>
       </c>
       <c r="Q24" t="n">
-        <v>17675.0</v>
+        <v>17896.0</v>
       </c>
       <c r="R24" t="n">
-        <v>114.0</v>
+        <v>115.0</v>
       </c>
       <c r="S24" t="n">
-        <v>179290.0</v>
+        <v>185850.0</v>
       </c>
       <c r="T24" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="U24" t="n" s="2">
         <v>43058.0</v>
       </c>
       <c r="V24" t="n">
-        <v>528.0</v>
+        <v>539.0</v>
       </c>
     </row>
     <row r="25">
@@ -2099,22 +2099,22 @@
         <v>11.0</v>
       </c>
       <c r="D25" t="n">
-        <v>4844.0</v>
+        <v>4687.0</v>
       </c>
       <c r="E25" t="n">
-        <v>4882.0</v>
+        <v>5039.0</v>
       </c>
       <c r="F25" t="n">
-        <v>1200.0</v>
+        <v>1246.0</v>
       </c>
       <c r="G25" t="n">
-        <v>1025.0</v>
+        <v>1062.0</v>
       </c>
       <c r="H25" t="n">
-        <v>4930.0</v>
+        <v>5038.0</v>
       </c>
       <c r="I25" t="n">
-        <v>989.0</v>
+        <v>1007.0</v>
       </c>
       <c r="J25" t="n">
         <v>1067.0</v>
@@ -2126,34 +2126,34 @@
         <v>0.0</v>
       </c>
       <c r="M25" t="n">
-        <v>158.0</v>
+        <v>159.0</v>
       </c>
       <c r="N25" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="O25" t="n">
-        <v>60.0</v>
+        <v>0.0</v>
       </c>
       <c r="P25" t="n">
-        <v>0.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q25" t="n">
-        <v>6892.0</v>
+        <v>6910.0</v>
       </c>
       <c r="R25" t="n">
-        <v>98.0</v>
+        <v>102.0</v>
       </c>
       <c r="S25" t="n">
-        <v>172628.0</v>
+        <v>182508.0</v>
       </c>
       <c r="T25" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="U25" t="n" s="2">
         <v>43138.0</v>
       </c>
       <c r="V25" t="n">
-        <v>448.0</v>
+        <v>459.0</v>
       </c>
     </row>
     <row r="26">
@@ -2167,22 +2167,22 @@
         <v>12.0</v>
       </c>
       <c r="D26" t="n">
-        <v>5129.0</v>
+        <v>4953.0</v>
       </c>
       <c r="E26" t="n">
-        <v>5159.0</v>
+        <v>5260.0</v>
       </c>
       <c r="F26" t="n">
-        <v>6308.0</v>
+        <v>6411.0</v>
       </c>
       <c r="G26" t="n">
-        <v>7015.0</v>
+        <v>7137.0</v>
       </c>
       <c r="H26" t="n">
-        <v>18556.0</v>
+        <v>18883.0</v>
       </c>
       <c r="I26" t="n">
-        <v>1805.0</v>
+        <v>1830.0</v>
       </c>
       <c r="J26" t="n">
         <v>1168.0</v>
@@ -2194,25 +2194,25 @@
         <v>0.0</v>
       </c>
       <c r="M26" t="n">
-        <v>101.0</v>
+        <v>114.0</v>
       </c>
       <c r="N26" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="O26" t="n">
-        <v>219.0</v>
+        <v>962.0</v>
       </c>
       <c r="P26" t="n">
-        <v>200.0</v>
+        <v>640.0</v>
       </c>
       <c r="Q26" t="n">
-        <v>29936.0</v>
+        <v>31428.0</v>
       </c>
       <c r="R26" t="n">
-        <v>66.0</v>
+        <v>70.0</v>
       </c>
       <c r="S26" t="n">
-        <v>127666.0</v>
+        <v>135695.0</v>
       </c>
       <c r="T26" t="s">
         <v>126</v>
@@ -2221,7 +2221,7 @@
         <v>43542.0</v>
       </c>
       <c r="V26" t="n">
-        <v>44.0</v>
+        <v>55.0</v>
       </c>
     </row>
     <row r="27">
@@ -2235,22 +2235,22 @@
         <v>12.0</v>
       </c>
       <c r="D27" t="n">
-        <v>4674.0</v>
+        <v>4701.0</v>
       </c>
       <c r="E27" t="n">
-        <v>4792.0</v>
+        <v>4923.0</v>
       </c>
       <c r="F27" t="n">
-        <v>2546.0</v>
+        <v>2582.0</v>
       </c>
       <c r="G27" t="n">
-        <v>2653.0</v>
+        <v>2680.0</v>
       </c>
       <c r="H27" t="n">
-        <v>8419.0</v>
+        <v>8534.0</v>
       </c>
       <c r="I27" t="n">
-        <v>1914.0</v>
+        <v>1944.0</v>
       </c>
       <c r="J27" t="n">
         <v>1694.0</v>
@@ -2262,34 +2262,34 @@
         <v>0.0</v>
       </c>
       <c r="M27" t="n">
-        <v>103.0</v>
+        <v>109.0</v>
       </c>
       <c r="N27" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="O27" t="n">
-        <v>70.0</v>
+        <v>456.0</v>
       </c>
       <c r="P27" t="n">
-        <v>160.0</v>
+        <v>520.0</v>
       </c>
       <c r="Q27" t="n">
-        <v>53862.0</v>
+        <v>54542.0</v>
       </c>
       <c r="R27" t="n">
-        <v>79.0</v>
+        <v>80.0</v>
       </c>
       <c r="S27" t="n">
-        <v>165798.0</v>
+        <v>172518.0</v>
       </c>
       <c r="T27" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="U27" t="n" s="2">
         <v>42920.0</v>
       </c>
       <c r="V27" t="n">
-        <v>666.0</v>
+        <v>677.0</v>
       </c>
     </row>
     <row r="28">
@@ -2303,22 +2303,22 @@
         <v>12.0</v>
       </c>
       <c r="D28" t="n">
-        <v>5196.0</v>
+        <v>4998.0</v>
       </c>
       <c r="E28" t="n">
-        <v>5218.0</v>
+        <v>5306.0</v>
       </c>
       <c r="F28" t="n">
-        <v>6208.0</v>
+        <v>6275.0</v>
       </c>
       <c r="G28" t="n">
-        <v>6298.0</v>
+        <v>6368.0</v>
       </c>
       <c r="H28" t="n">
-        <v>14927.0</v>
+        <v>15085.0</v>
       </c>
       <c r="I28" t="n">
-        <v>2730.0</v>
+        <v>2756.0</v>
       </c>
       <c r="J28" t="n">
         <v>2506.0</v>
@@ -2330,25 +2330,25 @@
         <v>31.0</v>
       </c>
       <c r="M28" t="n">
-        <v>190.0</v>
+        <v>198.0</v>
       </c>
       <c r="N28" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="O28" t="n">
-        <v>84.0</v>
+        <v>38.0</v>
       </c>
       <c r="P28" t="n">
-        <v>40.0</v>
+        <v>240.0</v>
       </c>
       <c r="Q28" t="n">
-        <v>62694.0</v>
+        <v>62742.0</v>
       </c>
       <c r="R28" t="n">
-        <v>54.0</v>
+        <v>56.0</v>
       </c>
       <c r="S28" t="n">
-        <v>171373.0</v>
+        <v>180969.0</v>
       </c>
       <c r="T28" t="s">
         <v>126</v>
@@ -2357,7 +2357,7 @@
         <v>43058.0</v>
       </c>
       <c r="V28" t="n">
-        <v>528.0</v>
+        <v>539.0</v>
       </c>
     </row>
     <row r="29">
@@ -2371,22 +2371,22 @@
         <v>12.0</v>
       </c>
       <c r="D29" t="n">
-        <v>4918.0</v>
+        <v>4705.0</v>
       </c>
       <c r="E29" t="n">
-        <v>4986.0</v>
+        <v>5121.0</v>
       </c>
       <c r="F29" t="n">
-        <v>1800.0</v>
+        <v>1820.0</v>
       </c>
       <c r="G29" t="n">
-        <v>1691.0</v>
+        <v>1705.0</v>
       </c>
       <c r="H29" t="n">
-        <v>5783.0</v>
+        <v>5839.0</v>
       </c>
       <c r="I29" t="n">
-        <v>1045.0</v>
+        <v>1055.0</v>
       </c>
       <c r="J29" t="n">
         <v>2536.0</v>
@@ -2401,31 +2401,31 @@
         <v>97.0</v>
       </c>
       <c r="N29" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="O29" t="n">
-        <v>90.0</v>
+        <v>394.0</v>
       </c>
       <c r="P29" t="n">
-        <v>120.0</v>
+        <v>400.0</v>
       </c>
       <c r="Q29" t="n">
-        <v>53550.0</v>
+        <v>54149.0</v>
       </c>
       <c r="R29" t="n">
-        <v>78.0</v>
+        <v>80.0</v>
       </c>
       <c r="S29" t="n">
-        <v>231320.0</v>
+        <v>238322.0</v>
       </c>
       <c r="T29" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="U29" t="n" s="2">
         <v>43493.0</v>
       </c>
       <c r="V29" t="n">
-        <v>93.0</v>
+        <v>104.0</v>
       </c>
     </row>
     <row r="30">
@@ -2439,61 +2439,61 @@
         <v>11.0</v>
       </c>
       <c r="D30" t="n">
-        <v>4601.0</v>
+        <v>4725.0</v>
       </c>
       <c r="E30" t="n">
-        <v>4646.0</v>
+        <v>5015.0</v>
       </c>
       <c r="F30" t="n">
-        <v>1373.0</v>
+        <v>3563.0</v>
       </c>
       <c r="G30" t="n">
-        <v>1146.0</v>
+        <v>4138.0</v>
       </c>
       <c r="H30" t="n">
-        <v>5459.0</v>
+        <v>13216.0</v>
       </c>
       <c r="I30" t="n">
-        <v>1075.0</v>
+        <v>2765.0</v>
       </c>
       <c r="J30" t="n">
-        <v>2045.0</v>
+        <v>850.0</v>
       </c>
       <c r="K30" t="n">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="L30" t="n">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="M30" t="n">
-        <v>95.0</v>
+        <v>135.0</v>
       </c>
       <c r="N30" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="O30" t="n">
-        <v>8.0</v>
+        <v>199.0</v>
       </c>
       <c r="P30" t="n">
-        <v>160.0</v>
+        <v>400.0</v>
       </c>
       <c r="Q30" t="n">
-        <v>19055.0</v>
+        <v>15662.0</v>
       </c>
       <c r="R30" t="n">
-        <v>69.0</v>
+        <v>61.0</v>
       </c>
       <c r="S30" t="n">
-        <v>97501.0</v>
+        <v>139810.0</v>
       </c>
       <c r="T30" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="U30" t="n" s="2">
-        <v>43578.0</v>
+        <v>43584.0</v>
       </c>
       <c r="V30" t="n">
-        <v>8.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="31">
@@ -2507,61 +2507,61 @@
         <v>11.0</v>
       </c>
       <c r="D31" t="n">
-        <v>4401.0</v>
+        <v>4527.0</v>
       </c>
       <c r="E31" t="n">
-        <v>4401.0</v>
+        <v>4722.0</v>
       </c>
       <c r="F31" t="n">
-        <v>1095.0</v>
+        <v>1389.0</v>
       </c>
       <c r="G31" t="n">
-        <v>1175.0</v>
+        <v>1152.0</v>
       </c>
       <c r="H31" t="n">
-        <v>6095.0</v>
+        <v>5513.0</v>
       </c>
       <c r="I31" t="n">
-        <v>1009.0</v>
+        <v>1085.0</v>
       </c>
       <c r="J31" t="n">
-        <v>383.0</v>
+        <v>2045.0</v>
       </c>
       <c r="K31" t="n">
-        <v>4.0</v>
+        <v>10.0</v>
       </c>
       <c r="L31" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="M31" t="n">
-        <v>185.0</v>
+        <v>109.0</v>
       </c>
       <c r="N31" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="O31" t="n">
-        <v>110.0</v>
+        <v>173.0</v>
       </c>
       <c r="P31" t="n">
         <v>280.0</v>
       </c>
       <c r="Q31" t="n">
-        <v>23536.0</v>
+        <v>19348.0</v>
       </c>
       <c r="R31" t="n">
-        <v>45.0</v>
+        <v>70.0</v>
       </c>
       <c r="S31" t="n">
-        <v>149860.0</v>
+        <v>99341.0</v>
       </c>
       <c r="T31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="U31" t="n" s="2">
-        <v>43519.0</v>
+        <v>43577.0</v>
       </c>
       <c r="V31" t="n">
-        <v>67.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="32">
@@ -2572,64 +2572,64 @@
         <v>102</v>
       </c>
       <c r="C32" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="D32" t="n">
-        <v>4305.0</v>
+        <v>4569.0</v>
       </c>
       <c r="E32" t="n">
-        <v>4339.0</v>
+        <v>4723.0</v>
       </c>
       <c r="F32" t="n">
-        <v>1224.0</v>
+        <v>1124.0</v>
       </c>
       <c r="G32" t="n">
-        <v>1268.0</v>
+        <v>1193.0</v>
       </c>
       <c r="H32" t="n">
-        <v>5471.0</v>
+        <v>6222.0</v>
       </c>
       <c r="I32" t="n">
-        <v>1238.0</v>
+        <v>1042.0</v>
       </c>
       <c r="J32" t="n">
-        <v>496.0</v>
+        <v>383.0</v>
       </c>
       <c r="K32" t="n">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="L32" t="n">
         <v>0.0</v>
       </c>
       <c r="M32" t="n">
-        <v>97.0</v>
+        <v>187.0</v>
       </c>
       <c r="N32" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="O32" t="n">
-        <v>81.0</v>
+        <v>112.0</v>
       </c>
       <c r="P32" t="n">
-        <v>120.0</v>
+        <v>680.0</v>
       </c>
       <c r="Q32" t="n">
-        <v>11706.0</v>
+        <v>23936.0</v>
       </c>
       <c r="R32" t="n">
-        <v>67.0</v>
+        <v>46.0</v>
       </c>
       <c r="S32" t="n">
-        <v>161692.0</v>
+        <v>159140.0</v>
       </c>
       <c r="T32" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="U32" t="n" s="2">
-        <v>43312.0</v>
+        <v>43519.0</v>
       </c>
       <c r="V32" t="n">
-        <v>274.0</v>
+        <v>78.0</v>
       </c>
     </row>
     <row r="33">
@@ -2640,64 +2640,64 @@
         <v>103</v>
       </c>
       <c r="C33" t="n">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="D33" t="n">
-        <v>4973.0</v>
+        <v>4293.0</v>
       </c>
       <c r="E33" t="n">
-        <v>5029.0</v>
+        <v>4568.0</v>
       </c>
       <c r="F33" t="n">
-        <v>2634.0</v>
+        <v>1236.0</v>
       </c>
       <c r="G33" t="n">
-        <v>2728.0</v>
+        <v>1276.0</v>
       </c>
       <c r="H33" t="n">
-        <v>7187.0</v>
+        <v>5523.0</v>
       </c>
       <c r="I33" t="n">
-        <v>1046.0</v>
+        <v>1251.0</v>
       </c>
       <c r="J33" t="n">
-        <v>1329.0</v>
+        <v>496.0</v>
       </c>
       <c r="K33" t="n">
-        <v>8.0</v>
+        <v>6.0</v>
       </c>
       <c r="L33" t="n">
         <v>0.0</v>
       </c>
       <c r="M33" t="n">
-        <v>166.0</v>
+        <v>97.0</v>
       </c>
       <c r="N33" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O33" t="n">
-        <v>265.0</v>
+        <v>108.0</v>
       </c>
       <c r="P33" t="n">
-        <v>160.0</v>
+        <v>280.0</v>
       </c>
       <c r="Q33" t="n">
-        <v>15357.0</v>
+        <v>11952.0</v>
       </c>
       <c r="R33" t="n">
-        <v>70.0</v>
+        <v>69.0</v>
       </c>
       <c r="S33" t="n">
-        <v>123862.0</v>
+        <v>170412.0</v>
       </c>
       <c r="T33" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="U33" t="n" s="2">
-        <v>43527.0</v>
+        <v>43312.0</v>
       </c>
       <c r="V33" t="n">
-        <v>59.0</v>
+        <v>285.0</v>
       </c>
     </row>
     <row r="34">
@@ -2711,61 +2711,61 @@
         <v>11.0</v>
       </c>
       <c r="D34" t="n">
-        <v>4406.0</v>
+        <v>4765.0</v>
       </c>
       <c r="E34" t="n">
-        <v>4433.0</v>
+        <v>5109.0</v>
       </c>
       <c r="F34" t="n">
-        <v>1834.0</v>
+        <v>2678.0</v>
       </c>
       <c r="G34" t="n">
-        <v>1792.0</v>
+        <v>2764.0</v>
       </c>
       <c r="H34" t="n">
-        <v>4777.0</v>
+        <v>7314.0</v>
       </c>
       <c r="I34" t="n">
-        <v>961.0</v>
+        <v>1059.0</v>
       </c>
       <c r="J34" t="n">
-        <v>631.0</v>
+        <v>1329.0</v>
       </c>
       <c r="K34" t="n">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="L34" t="n">
         <v>0.0</v>
       </c>
       <c r="M34" t="n">
-        <v>114.0</v>
+        <v>182.0</v>
       </c>
       <c r="N34" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="O34" t="n">
-        <v>0.0</v>
+        <v>635.0</v>
       </c>
       <c r="P34" t="n">
-        <v>40.0</v>
+        <v>520.0</v>
       </c>
       <c r="Q34" t="n">
-        <v>24915.0</v>
+        <v>16325.0</v>
       </c>
       <c r="R34" t="n">
-        <v>72.0</v>
+        <v>73.0</v>
       </c>
       <c r="S34" t="n">
-        <v>214756.0</v>
+        <v>133371.0</v>
       </c>
       <c r="T34" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="U34" t="n" s="2">
-        <v>43493.0</v>
+        <v>43527.0</v>
       </c>
       <c r="V34" t="n">
-        <v>93.0</v>
+        <v>70.0</v>
       </c>
     </row>
     <row r="35">
@@ -2776,28 +2776,28 @@
         <v>105</v>
       </c>
       <c r="C35" t="n">
-        <v>12.0</v>
+        <v>11.0</v>
       </c>
       <c r="D35" t="n">
-        <v>4691.0</v>
+        <v>4213.0</v>
       </c>
       <c r="E35" t="n">
-        <v>4691.0</v>
+        <v>4433.0</v>
       </c>
       <c r="F35" t="n">
-        <v>1122.0</v>
+        <v>1835.0</v>
       </c>
       <c r="G35" t="n">
-        <v>960.0</v>
+        <v>1794.0</v>
       </c>
       <c r="H35" t="n">
-        <v>7930.0</v>
+        <v>4795.0</v>
       </c>
       <c r="I35" t="n">
-        <v>2072.0</v>
+        <v>963.0</v>
       </c>
       <c r="J35" t="n">
-        <v>1138.0</v>
+        <v>631.0</v>
       </c>
       <c r="K35" t="n">
         <v>9.0</v>
@@ -2806,34 +2806,34 @@
         <v>0.0</v>
       </c>
       <c r="M35" t="n">
-        <v>83.0</v>
+        <v>114.0</v>
       </c>
       <c r="N35" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O35" t="n">
-        <v>316.0</v>
+        <v>26.0</v>
       </c>
       <c r="P35" t="n">
-        <v>290.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q35" t="n">
-        <v>29262.0</v>
+        <v>24941.0</v>
       </c>
       <c r="R35" t="n">
-        <v>95.0</v>
+        <v>75.0</v>
       </c>
       <c r="S35" t="n">
-        <v>128729.0</v>
+        <v>219356.0</v>
       </c>
       <c r="T35" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="U35" t="n" s="2">
-        <v>43519.0</v>
+        <v>43493.0</v>
       </c>
       <c r="V35" t="n">
-        <v>67.0</v>
+        <v>104.0</v>
       </c>
     </row>
     <row r="36">
@@ -2844,64 +2844,64 @@
         <v>106</v>
       </c>
       <c r="C36" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="D36" t="n">
-        <v>4918.0</v>
+        <v>4694.0</v>
       </c>
       <c r="E36" t="n">
-        <v>4974.0</v>
+        <v>5022.0</v>
       </c>
       <c r="F36" t="n">
-        <v>4870.0</v>
+        <v>1152.0</v>
       </c>
       <c r="G36" t="n">
-        <v>5607.0</v>
+        <v>988.0</v>
       </c>
       <c r="H36" t="n">
-        <v>13405.0</v>
+        <v>8129.0</v>
       </c>
       <c r="I36" t="n">
-        <v>2420.0</v>
+        <v>2110.0</v>
       </c>
       <c r="J36" t="n">
-        <v>454.0</v>
+        <v>1138.0</v>
       </c>
       <c r="K36" t="n">
-        <v>5.0</v>
+        <v>9.0</v>
       </c>
       <c r="L36" t="n">
         <v>0.0</v>
       </c>
       <c r="M36" t="n">
-        <v>138.0</v>
+        <v>87.0</v>
       </c>
       <c r="N36" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="O36" t="n">
-        <v>65.0</v>
+        <v>324.0</v>
       </c>
       <c r="P36" t="n">
-        <v>40.0</v>
+        <v>640.0</v>
       </c>
       <c r="Q36" t="n">
-        <v>27998.0</v>
+        <v>29941.0</v>
       </c>
       <c r="R36" t="n">
-        <v>59.0</v>
+        <v>99.0</v>
       </c>
       <c r="S36" t="n">
-        <v>181225.0</v>
+        <v>138678.0</v>
       </c>
       <c r="T36" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="U36" t="n" s="2">
-        <v>43280.0</v>
+        <v>43519.0</v>
       </c>
       <c r="V36" t="n">
-        <v>306.0</v>
+        <v>78.0</v>
       </c>
     </row>
     <row r="37">
@@ -2915,61 +2915,61 @@
         <v>11.0</v>
       </c>
       <c r="D37" t="n">
-        <v>4731.0</v>
+        <v>4912.0</v>
       </c>
       <c r="E37" t="n">
-        <v>4731.0</v>
+        <v>5100.0</v>
       </c>
       <c r="F37" t="n">
-        <v>1313.0</v>
+        <v>5006.0</v>
       </c>
       <c r="G37" t="n">
-        <v>1269.0</v>
+        <v>5791.0</v>
       </c>
       <c r="H37" t="n">
-        <v>5958.0</v>
+        <v>13758.0</v>
       </c>
       <c r="I37" t="n">
-        <v>1358.0</v>
+        <v>2475.0</v>
       </c>
       <c r="J37" t="n">
-        <v>571.0</v>
+        <v>454.0</v>
       </c>
       <c r="K37" t="n">
-        <v>7.0</v>
+        <v>5.0</v>
       </c>
       <c r="L37" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="M37" t="n">
-        <v>730.0</v>
+        <v>150.0</v>
       </c>
       <c r="N37" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O37" t="n">
-        <v>304.0</v>
+        <v>452.0</v>
       </c>
       <c r="P37" t="n">
-        <v>280.0</v>
+        <v>200.0</v>
       </c>
       <c r="Q37" t="n">
-        <v>34614.0</v>
+        <v>28722.0</v>
       </c>
       <c r="R37" t="n">
-        <v>51.0</v>
+        <v>62.0</v>
       </c>
       <c r="S37" t="n">
-        <v>156906.0</v>
+        <v>190169.0</v>
       </c>
       <c r="T37" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="U37" t="n" s="2">
-        <v>43551.0</v>
+        <v>43280.0</v>
       </c>
       <c r="V37" t="n">
-        <v>35.0</v>
+        <v>317.0</v>
       </c>
     </row>
     <row r="38">
@@ -2980,64 +2980,64 @@
         <v>108</v>
       </c>
       <c r="C38" t="n">
-        <v>12.0</v>
+        <v>11.0</v>
       </c>
       <c r="D38" t="n">
-        <v>5159.0</v>
+        <v>4845.0</v>
       </c>
       <c r="E38" t="n">
-        <v>5159.0</v>
+        <v>5024.0</v>
       </c>
       <c r="F38" t="n">
-        <v>4636.0</v>
+        <v>1347.0</v>
       </c>
       <c r="G38" t="n">
-        <v>4459.0</v>
+        <v>1285.0</v>
       </c>
       <c r="H38" t="n">
-        <v>10733.0</v>
+        <v>6209.0</v>
       </c>
       <c r="I38" t="n">
-        <v>956.0</v>
+        <v>1415.0</v>
       </c>
       <c r="J38" t="n">
-        <v>1932.0</v>
+        <v>571.0</v>
       </c>
       <c r="K38" t="n">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="L38" t="n">
-        <v>53.0</v>
+        <v>4.0</v>
       </c>
       <c r="M38" t="n">
-        <v>206.0</v>
+        <v>738.0</v>
       </c>
       <c r="N38" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="O38" t="n">
-        <v>300.0</v>
+        <v>789.0</v>
       </c>
       <c r="P38" t="n">
-        <v>200.0</v>
+        <v>680.0</v>
       </c>
       <c r="Q38" t="n">
-        <v>72805.0</v>
+        <v>35807.0</v>
       </c>
       <c r="R38" t="n">
-        <v>94.0</v>
+        <v>52.0</v>
       </c>
       <c r="S38" t="n">
-        <v>160856.0</v>
+        <v>165237.0</v>
       </c>
       <c r="T38" t="s">
         <v>126</v>
       </c>
       <c r="U38" t="n" s="2">
-        <v>43549.0</v>
+        <v>43551.0</v>
       </c>
       <c r="V38" t="n">
-        <v>37.0</v>
+        <v>46.0</v>
       </c>
     </row>
     <row r="39">
@@ -3048,64 +3048,64 @@
         <v>109</v>
       </c>
       <c r="C39" t="n">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
       <c r="D39" t="n">
-        <v>5025.0</v>
+        <v>4881.0</v>
       </c>
       <c r="E39" t="n">
-        <v>5025.0</v>
+        <v>5208.0</v>
       </c>
       <c r="F39" t="n">
-        <v>3937.0</v>
+        <v>4652.0</v>
       </c>
       <c r="G39" t="n">
-        <v>3127.0</v>
+        <v>4466.0</v>
       </c>
       <c r="H39" t="n">
-        <v>16161.0</v>
+        <v>10771.0</v>
       </c>
       <c r="I39" t="n">
-        <v>1963.0</v>
+        <v>960.0</v>
       </c>
       <c r="J39" t="n">
-        <v>8110.0</v>
+        <v>1932.0</v>
       </c>
       <c r="K39" t="n">
-        <v>12.0</v>
+        <v>8.0</v>
       </c>
       <c r="L39" t="n">
-        <v>43.0</v>
+        <v>53.0</v>
       </c>
       <c r="M39" t="n">
-        <v>116.0</v>
+        <v>206.0</v>
       </c>
       <c r="N39" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="O39" t="n">
-        <v>531.0</v>
+        <v>356.0</v>
       </c>
       <c r="P39" t="n">
-        <v>240.0</v>
+        <v>440.0</v>
       </c>
       <c r="Q39" t="n">
-        <v>109133.0</v>
+        <v>73429.0</v>
       </c>
       <c r="R39" t="n">
-        <v>68.0</v>
+        <v>96.0</v>
       </c>
       <c r="S39" t="n">
-        <v>135872.0</v>
+        <v>166850.0</v>
       </c>
       <c r="T39" t="s">
         <v>126</v>
       </c>
       <c r="U39" t="n" s="2">
-        <v>43563.0</v>
+        <v>43549.0</v>
       </c>
       <c r="V39" t="n">
-        <v>23.0</v>
+        <v>48.0</v>
       </c>
     </row>
     <row r="40">
@@ -3116,64 +3116,64 @@
         <v>110</v>
       </c>
       <c r="C40" t="n">
-        <v>11.0</v>
+        <v>13.0</v>
       </c>
       <c r="D40" t="n">
-        <v>5026.0</v>
+        <v>4802.0</v>
       </c>
       <c r="E40" t="n">
-        <v>5026.0</v>
+        <v>5224.0</v>
       </c>
       <c r="F40" t="n">
-        <v>5234.0</v>
+        <v>4008.0</v>
       </c>
       <c r="G40" t="n">
-        <v>5275.0</v>
+        <v>3176.0</v>
       </c>
       <c r="H40" t="n">
-        <v>32237.0</v>
+        <v>16400.0</v>
       </c>
       <c r="I40" t="n">
-        <v>4364.0</v>
+        <v>2001.0</v>
       </c>
       <c r="J40" t="n">
-        <v>2288.0</v>
+        <v>8254.0</v>
       </c>
       <c r="K40" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="L40" t="n">
-        <v>0.0</v>
+        <v>43.0</v>
       </c>
       <c r="M40" t="n">
-        <v>97.0</v>
+        <v>116.0</v>
       </c>
       <c r="N40" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="O40" t="n">
-        <v>0.0</v>
+        <v>1348.0</v>
       </c>
       <c r="P40" t="n">
-        <v>80.0</v>
+        <v>640.0</v>
       </c>
       <c r="Q40" t="n">
-        <v>7558.0</v>
+        <v>111673.0</v>
       </c>
       <c r="R40" t="n">
-        <v>98.0</v>
+        <v>72.0</v>
       </c>
       <c r="S40" t="n">
-        <v>174035.0</v>
+        <v>143075.0</v>
       </c>
       <c r="T40" t="s">
         <v>126</v>
       </c>
       <c r="U40" t="n" s="2">
-        <v>43252.0</v>
+        <v>43563.0</v>
       </c>
       <c r="V40" t="n">
-        <v>334.0</v>
+        <v>34.0</v>
       </c>
     </row>
     <row r="41">
@@ -3187,25 +3187,25 @@
         <v>11.0</v>
       </c>
       <c r="D41" t="n">
-        <v>4417.0</v>
+        <v>4772.0</v>
       </c>
       <c r="E41" t="n">
-        <v>4431.0</v>
+        <v>5215.0</v>
       </c>
       <c r="F41" t="n">
-        <v>2747.0</v>
+        <v>5264.0</v>
       </c>
       <c r="G41" t="n">
-        <v>2693.0</v>
+        <v>5298.0</v>
       </c>
       <c r="H41" t="n">
-        <v>7298.0</v>
+        <v>32562.0</v>
       </c>
       <c r="I41" t="n">
-        <v>1415.0</v>
+        <v>4426.0</v>
       </c>
       <c r="J41" t="n">
-        <v>2904.0</v>
+        <v>2288.0</v>
       </c>
       <c r="K41" t="n">
         <v>11.0</v>
@@ -3214,34 +3214,34 @@
         <v>0.0</v>
       </c>
       <c r="M41" t="n">
-        <v>80.0</v>
+        <v>98.0</v>
       </c>
       <c r="N41" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O41" t="n">
-        <v>10.0</v>
+        <v>50.0</v>
       </c>
       <c r="P41" t="n">
-        <v>160.0</v>
+        <v>320.0</v>
       </c>
       <c r="Q41" t="n">
-        <v>29463.0</v>
+        <v>7630.0</v>
       </c>
       <c r="R41" t="n">
-        <v>63.0</v>
+        <v>100.0</v>
       </c>
       <c r="S41" t="n">
-        <v>129612.0</v>
+        <v>181780.0</v>
       </c>
       <c r="T41" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="U41" t="n" s="2">
-        <v>43370.0</v>
+        <v>43252.0</v>
       </c>
       <c r="V41" t="n">
-        <v>216.0</v>
+        <v>345.0</v>
       </c>
     </row>
     <row r="42">
@@ -3252,64 +3252,64 @@
         <v>112</v>
       </c>
       <c r="C42" t="n">
-        <v>12.0</v>
+        <v>11.0</v>
       </c>
       <c r="D42" t="n">
-        <v>4389.0</v>
+        <v>4739.0</v>
       </c>
       <c r="E42" t="n">
-        <v>4389.0</v>
+        <v>4785.0</v>
       </c>
       <c r="F42" t="n">
-        <v>4748.0</v>
+        <v>2788.0</v>
       </c>
       <c r="G42" t="n">
-        <v>5239.0</v>
+        <v>2718.0</v>
       </c>
       <c r="H42" t="n">
-        <v>17873.0</v>
+        <v>7380.0</v>
       </c>
       <c r="I42" t="n">
-        <v>3094.0</v>
+        <v>1442.0</v>
       </c>
       <c r="J42" t="n">
-        <v>3776.0</v>
+        <v>2904.0</v>
       </c>
       <c r="K42" t="n">
-        <v>9.0</v>
+        <v>11.0</v>
       </c>
       <c r="L42" t="n">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
       <c r="M42" t="n">
-        <v>215.0</v>
+        <v>81.0</v>
       </c>
       <c r="N42" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="O42" t="n">
-        <v>86.0</v>
+        <v>182.0</v>
       </c>
       <c r="P42" t="n">
-        <v>200.0</v>
+        <v>400.0</v>
       </c>
       <c r="Q42" t="n">
-        <v>44116.0</v>
+        <v>29751.0</v>
       </c>
       <c r="R42" t="n">
-        <v>76.0</v>
+        <v>64.0</v>
       </c>
       <c r="S42" t="n">
-        <v>170876.0</v>
+        <v>137172.0</v>
       </c>
       <c r="T42" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="U42" t="n" s="2">
-        <v>43578.0</v>
+        <v>43370.0</v>
       </c>
       <c r="V42" t="n">
-        <v>8.0</v>
+        <v>227.0</v>
       </c>
     </row>
     <row r="43">
@@ -3323,61 +3323,61 @@
         <v>12.0</v>
       </c>
       <c r="D43" t="n">
-        <v>4603.0</v>
+        <v>4803.0</v>
       </c>
       <c r="E43" t="n">
-        <v>4606.0</v>
+        <v>4803.0</v>
       </c>
       <c r="F43" t="n">
-        <v>3041.0</v>
+        <v>4782.0</v>
       </c>
       <c r="G43" t="n">
-        <v>2957.0</v>
+        <v>5249.0</v>
       </c>
       <c r="H43" t="n">
-        <v>9160.0</v>
+        <v>18010.0</v>
       </c>
       <c r="I43" t="n">
-        <v>2707.0</v>
+        <v>3143.0</v>
       </c>
       <c r="J43" t="n">
-        <v>2656.0</v>
+        <v>3776.0</v>
       </c>
       <c r="K43" t="n">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="L43" t="n">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="M43" t="n">
-        <v>118.0</v>
+        <v>224.0</v>
       </c>
       <c r="N43" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="O43" t="n">
-        <v>90.0</v>
+        <v>251.0</v>
       </c>
       <c r="P43" t="n">
-        <v>130.0</v>
+        <v>520.0</v>
       </c>
       <c r="Q43" t="n">
-        <v>37024.0</v>
+        <v>44548.0</v>
       </c>
       <c r="R43" t="n">
-        <v>63.0</v>
+        <v>78.0</v>
       </c>
       <c r="S43" t="n">
-        <v>127055.0</v>
+        <v>179036.0</v>
       </c>
       <c r="T43" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="U43" t="n" s="2">
-        <v>43382.0</v>
+        <v>43578.0</v>
       </c>
       <c r="V43" t="n">
-        <v>204.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="44">
@@ -3385,67 +3385,67 @@
         <v>64</v>
       </c>
       <c r="B44" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="C44" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="D44" t="n">
-        <v>4814.0</v>
+        <v>4652.0</v>
       </c>
       <c r="E44" t="n">
-        <v>4814.0</v>
+        <v>4903.0</v>
       </c>
       <c r="F44" t="n">
-        <v>4314.0</v>
+        <v>3067.0</v>
       </c>
       <c r="G44" t="n">
-        <v>4593.0</v>
+        <v>2967.0</v>
       </c>
       <c r="H44" t="n">
-        <v>9972.0</v>
+        <v>9237.0</v>
       </c>
       <c r="I44" t="n">
-        <v>2345.0</v>
+        <v>2735.0</v>
       </c>
       <c r="J44" t="n">
-        <v>1635.0</v>
+        <v>2656.0</v>
       </c>
       <c r="K44" t="n">
         <v>10.0</v>
       </c>
       <c r="L44" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="M44" t="n">
-        <v>120.0</v>
+        <v>119.0</v>
       </c>
       <c r="N44" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O44" t="n">
-        <v>40.0</v>
+        <v>182.0</v>
       </c>
       <c r="P44" t="n">
-        <v>80.0</v>
+        <v>280.0</v>
       </c>
       <c r="Q44" t="n">
-        <v>31055.0</v>
+        <v>37552.0</v>
       </c>
       <c r="R44" t="n">
-        <v>39.0</v>
+        <v>65.0</v>
       </c>
       <c r="S44" t="n">
-        <v>169572.0</v>
+        <v>134535.0</v>
       </c>
       <c r="T44" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="U44" t="n" s="2">
-        <v>43390.0</v>
+        <v>43382.0</v>
       </c>
       <c r="V44" t="n">
-        <v>196.0</v>
+        <v>215.0</v>
       </c>
     </row>
     <row r="45">
@@ -3453,31 +3453,31 @@
         <v>65</v>
       </c>
       <c r="B45" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C45" t="n">
         <v>12.0</v>
       </c>
       <c r="D45" t="n">
-        <v>5051.0</v>
+        <v>5034.0</v>
       </c>
       <c r="E45" t="n">
-        <v>5070.0</v>
+        <v>5317.0</v>
       </c>
       <c r="F45" t="n">
-        <v>3056.0</v>
+        <v>3110.0</v>
       </c>
       <c r="G45" t="n">
-        <v>2951.0</v>
+        <v>2992.0</v>
       </c>
       <c r="H45" t="n">
-        <v>8544.0</v>
+        <v>8687.0</v>
       </c>
       <c r="I45" t="n">
-        <v>1687.0</v>
+        <v>1725.0</v>
       </c>
       <c r="J45" t="n">
-        <v>4026.0</v>
+        <v>4070.0</v>
       </c>
       <c r="K45" t="n">
         <v>10.0</v>
@@ -3486,34 +3486,34 @@
         <v>106.0</v>
       </c>
       <c r="M45" t="n">
-        <v>298.0</v>
+        <v>311.0</v>
       </c>
       <c r="N45" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="O45" t="n">
-        <v>228.0</v>
+        <v>1178.0</v>
       </c>
       <c r="P45" t="n">
-        <v>240.0</v>
+        <v>640.0</v>
       </c>
       <c r="Q45" t="n">
-        <v>65206.0</v>
+        <v>66899.0</v>
       </c>
       <c r="R45" t="n">
-        <v>73.0</v>
+        <v>79.0</v>
       </c>
       <c r="S45" t="n">
-        <v>123790.0</v>
+        <v>133602.0</v>
       </c>
       <c r="T45" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="U45" t="n" s="2">
         <v>43390.0</v>
       </c>
       <c r="V45" t="n">
-        <v>196.0</v>
+        <v>207.0</v>
       </c>
     </row>
     <row r="46">
@@ -3521,28 +3521,28 @@
         <v>66</v>
       </c>
       <c r="B46" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C46" t="n">
         <v>10.0</v>
       </c>
       <c r="D46" t="n">
-        <v>4620.0</v>
+        <v>4425.0</v>
       </c>
       <c r="E46" t="n">
         <v>4638.0</v>
       </c>
       <c r="F46" t="n">
-        <v>735.0</v>
+        <v>749.0</v>
       </c>
       <c r="G46" t="n">
-        <v>708.0</v>
+        <v>717.0</v>
       </c>
       <c r="H46" t="n">
-        <v>3986.0</v>
+        <v>4165.0</v>
       </c>
       <c r="I46" t="n">
-        <v>798.0</v>
+        <v>832.0</v>
       </c>
       <c r="J46" t="n">
         <v>899.0</v>
@@ -3554,34 +3554,34 @@
         <v>0.0</v>
       </c>
       <c r="M46" t="n">
-        <v>89.0</v>
+        <v>101.0</v>
       </c>
       <c r="N46" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="O46" t="n">
-        <v>86.0</v>
+        <v>442.0</v>
       </c>
       <c r="P46" t="n">
-        <v>280.0</v>
+        <v>640.0</v>
       </c>
       <c r="Q46" t="n">
-        <v>8021.0</v>
+        <v>8575.0</v>
       </c>
       <c r="R46" t="n">
-        <v>31.0</v>
+        <v>33.0</v>
       </c>
       <c r="S46" t="n">
-        <v>68070.0</v>
+        <v>76630.0</v>
       </c>
       <c r="T46" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="U46" t="n" s="2">
         <v>43529.0</v>
       </c>
       <c r="V46" t="n">
-        <v>57.0</v>
+        <v>68.0</v>
       </c>
     </row>
     <row r="47">
@@ -3589,28 +3589,28 @@
         <v>67</v>
       </c>
       <c r="B47" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C47" t="n">
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
       <c r="D47" t="n">
-        <v>5345.0</v>
+        <v>5151.0</v>
       </c>
       <c r="E47" t="n">
-        <v>5535.0</v>
+        <v>5714.0</v>
       </c>
       <c r="F47" t="n">
-        <v>13598.0</v>
+        <v>13791.0</v>
       </c>
       <c r="G47" t="n">
-        <v>14458.0</v>
+        <v>14674.0</v>
       </c>
       <c r="H47" t="n">
-        <v>32822.0</v>
+        <v>33328.0</v>
       </c>
       <c r="I47" t="n">
-        <v>11411.0</v>
+        <v>11589.0</v>
       </c>
       <c r="J47" t="n">
         <v>2419.0</v>
@@ -3622,25 +3622,25 @@
         <v>0.0</v>
       </c>
       <c r="M47" t="n">
-        <v>196.0</v>
+        <v>210.0</v>
       </c>
       <c r="N47" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="O47" t="n">
-        <v>443.0</v>
+        <v>1456.0</v>
       </c>
       <c r="P47" t="n">
-        <v>200.0</v>
+        <v>680.0</v>
       </c>
       <c r="Q47" t="n">
-        <v>110926.0</v>
+        <v>113041.0</v>
       </c>
       <c r="R47" t="n">
-        <v>59.0</v>
+        <v>63.0</v>
       </c>
       <c r="S47" t="n">
-        <v>199305.0</v>
+        <v>208062.0</v>
       </c>
       <c r="T47" t="s">
         <v>127</v>
@@ -3649,7 +3649,7 @@
         <v>43390.0</v>
       </c>
       <c r="V47" t="n">
-        <v>196.0</v>
+        <v>207.0</v>
       </c>
     </row>
     <row r="48">
@@ -3657,28 +3657,28 @@
         <v>68</v>
       </c>
       <c r="B48" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C48" t="n">
         <v>13.0</v>
       </c>
       <c r="D48" t="n">
-        <v>5155.0</v>
+        <v>4980.0</v>
       </c>
       <c r="E48" t="n">
-        <v>5165.0</v>
+        <v>5406.0</v>
       </c>
       <c r="F48" t="n">
-        <v>8851.0</v>
+        <v>8914.0</v>
       </c>
       <c r="G48" t="n">
-        <v>8390.0</v>
+        <v>8450.0</v>
       </c>
       <c r="H48" t="n">
-        <v>19044.0</v>
+        <v>19184.0</v>
       </c>
       <c r="I48" t="n">
-        <v>6253.0</v>
+        <v>6289.0</v>
       </c>
       <c r="J48" t="n">
         <v>4308.0</v>
@@ -3690,25 +3690,25 @@
         <v>48.0</v>
       </c>
       <c r="M48" t="n">
-        <v>417.0</v>
+        <v>423.0</v>
       </c>
       <c r="N48" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="O48" t="n">
-        <v>118.0</v>
+        <v>278.0</v>
       </c>
       <c r="P48" t="n">
-        <v>40.0</v>
+        <v>120.0</v>
       </c>
       <c r="Q48" t="n">
-        <v>133390.0</v>
+        <v>133813.0</v>
       </c>
       <c r="R48" t="n">
-        <v>27.0</v>
+        <v>28.0</v>
       </c>
       <c r="S48" t="n">
-        <v>173434.0</v>
+        <v>181857.0</v>
       </c>
       <c r="T48" t="s">
         <v>126</v>
@@ -3717,7 +3717,7 @@
         <v>43483.0</v>
       </c>
       <c r="V48" t="n">
-        <v>103.0</v>
+        <v>114.0</v>
       </c>
     </row>
     <row r="49">
@@ -3725,28 +3725,28 @@
         <v>69</v>
       </c>
       <c r="B49" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C49" t="n">
         <v>12.0</v>
       </c>
       <c r="D49" t="n">
-        <v>4607.0</v>
+        <v>4457.0</v>
       </c>
       <c r="E49" t="n">
-        <v>4607.0</v>
+        <v>4915.0</v>
       </c>
       <c r="F49" t="n">
-        <v>3190.0</v>
+        <v>3216.0</v>
       </c>
       <c r="G49" t="n">
-        <v>3211.0</v>
+        <v>3234.0</v>
       </c>
       <c r="H49" t="n">
-        <v>18727.0</v>
+        <v>18947.0</v>
       </c>
       <c r="I49" t="n">
-        <v>3793.0</v>
+        <v>3835.0</v>
       </c>
       <c r="J49" t="n">
         <v>1927.0</v>
@@ -3761,31 +3761,31 @@
         <v>57.0</v>
       </c>
       <c r="N49" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="O49" t="n">
-        <v>121.0</v>
+        <v>514.0</v>
       </c>
       <c r="P49" t="n">
-        <v>240.0</v>
+        <v>680.0</v>
       </c>
       <c r="Q49" t="n">
-        <v>47621.0</v>
+        <v>48531.0</v>
       </c>
       <c r="R49" t="n">
-        <v>77.0</v>
+        <v>79.0</v>
       </c>
       <c r="S49" t="n">
-        <v>170335.0</v>
+        <v>177495.0</v>
       </c>
       <c r="T49" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="U49" t="n" s="2">
         <v>43230.0</v>
       </c>
       <c r="V49" t="n">
-        <v>356.0</v>
+        <v>367.0</v>
       </c>
     </row>
     <row r="50">
@@ -3793,28 +3793,28 @@
         <v>70</v>
       </c>
       <c r="B50" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C50" t="n">
         <v>12.0</v>
       </c>
       <c r="D50" t="n">
-        <v>5047.0</v>
+        <v>5016.0</v>
       </c>
       <c r="E50" t="n">
-        <v>5110.0</v>
+        <v>5251.0</v>
       </c>
       <c r="F50" t="n">
-        <v>7717.0</v>
+        <v>7790.0</v>
       </c>
       <c r="G50" t="n">
-        <v>8067.0</v>
+        <v>8137.0</v>
       </c>
       <c r="H50" t="n">
-        <v>22026.0</v>
+        <v>22206.0</v>
       </c>
       <c r="I50" t="n">
-        <v>4486.0</v>
+        <v>4529.0</v>
       </c>
       <c r="J50" t="n">
         <v>4810.0</v>
@@ -3826,34 +3826,34 @@
         <v>47.0</v>
       </c>
       <c r="M50" t="n">
-        <v>901.0</v>
+        <v>912.0</v>
       </c>
       <c r="N50" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O50" t="n">
-        <v>136.0</v>
+        <v>394.0</v>
       </c>
       <c r="P50" t="n">
-        <v>200.0</v>
+        <v>440.0</v>
       </c>
       <c r="Q50" t="n">
-        <v>27997.0</v>
+        <v>28499.0</v>
       </c>
       <c r="R50" t="n">
-        <v>112.0</v>
+        <v>115.0</v>
       </c>
       <c r="S50" t="n">
-        <v>190502.0</v>
+        <v>199257.0</v>
       </c>
       <c r="T50" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="U50" t="n" s="2">
         <v>43184.0</v>
       </c>
       <c r="V50" t="n">
-        <v>402.0</v>
+        <v>413.0</v>
       </c>
     </row>
     <row r="51">
@@ -3861,28 +3861,28 @@
         <v>71</v>
       </c>
       <c r="B51" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C51" t="n">
         <v>13.0</v>
       </c>
       <c r="D51" t="n">
-        <v>5305.0</v>
+        <v>5060.0</v>
       </c>
       <c r="E51" t="n">
-        <v>5353.0</v>
+        <v>5586.0</v>
       </c>
       <c r="F51" t="n">
-        <v>6338.0</v>
+        <v>6419.0</v>
       </c>
       <c r="G51" t="n">
-        <v>6193.0</v>
+        <v>6283.0</v>
       </c>
       <c r="H51" t="n">
-        <v>20484.0</v>
+        <v>20697.0</v>
       </c>
       <c r="I51" t="n">
-        <v>3404.0</v>
+        <v>3434.0</v>
       </c>
       <c r="J51" t="n">
         <v>3170.0</v>
@@ -3894,25 +3894,25 @@
         <v>4.0</v>
       </c>
       <c r="M51" t="n">
-        <v>178.0</v>
+        <v>187.0</v>
       </c>
       <c r="N51" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="O51" t="n">
-        <v>176.0</v>
+        <v>758.0</v>
       </c>
       <c r="P51" t="n">
-        <v>240.0</v>
+        <v>560.0</v>
       </c>
       <c r="Q51" t="n">
-        <v>109064.0</v>
+        <v>110295.0</v>
       </c>
       <c r="R51" t="n">
-        <v>85.0</v>
+        <v>87.0</v>
       </c>
       <c r="S51" t="n">
-        <v>225288.0</v>
+        <v>234340.0</v>
       </c>
       <c r="T51" t="s">
         <v>127</v>
@@ -3921,7 +3921,7 @@
         <v>43501.0</v>
       </c>
       <c r="V51" t="n">
-        <v>85.0</v>
+        <v>96.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change to 75 wars; score formula update (less points for total victories
</commit_message>
<xml_diff>
--- a/docs/data/memberstats.xlsx
+++ b/docs/data/memberstats.xlsx
@@ -704,13 +704,13 @@
         <v>120</v>
       </c>
       <c r="O4" t="n">
-        <v>646.0</v>
+        <v>662.0</v>
       </c>
       <c r="P4" t="n">
-        <v>560.0</v>
+        <v>568.0</v>
       </c>
       <c r="Q4" t="n">
-        <v>99711.0</v>
+        <v>99727.0</v>
       </c>
       <c r="R4" t="n">
         <v>114.0</v>
@@ -1591,7 +1591,7 @@
         <v>1424.0</v>
       </c>
       <c r="P17" t="n">
-        <v>749.0</v>
+        <v>757.0</v>
       </c>
       <c r="Q17" t="n">
         <v>169199.0</v>
@@ -1659,7 +1659,7 @@
         <v>588.0</v>
       </c>
       <c r="P18" t="n">
-        <v>709.0</v>
+        <v>717.0</v>
       </c>
       <c r="Q18" t="n">
         <v>53553.0</v>
@@ -2031,7 +2031,7 @@
         <v>13.0</v>
       </c>
       <c r="D24" t="n">
-        <v>5365.0</v>
+        <v>5342.0</v>
       </c>
       <c r="E24" t="n">
         <v>6024.0</v>
@@ -2040,10 +2040,10 @@
         <v>13008.0</v>
       </c>
       <c r="G24" t="n">
-        <v>13523.0</v>
+        <v>13524.0</v>
       </c>
       <c r="H24" t="n">
-        <v>43060.0</v>
+        <v>43061.0</v>
       </c>
       <c r="I24" t="n">
         <v>5303.0</v>
@@ -3193,16 +3193,16 @@
         <v>5609.0</v>
       </c>
       <c r="F41" t="n">
-        <v>4470.0</v>
+        <v>4471.0</v>
       </c>
       <c r="G41" t="n">
         <v>4612.0</v>
       </c>
       <c r="H41" t="n">
-        <v>13472.0</v>
+        <v>13473.0</v>
       </c>
       <c r="I41" t="n">
-        <v>3968.0</v>
+        <v>3969.0</v>
       </c>
       <c r="J41" t="n">
         <v>2702.0</v>
@@ -3764,13 +3764,13 @@
         <v>120</v>
       </c>
       <c r="O49" t="n">
-        <v>758.0</v>
+        <v>766.0</v>
       </c>
       <c r="P49" t="n">
         <v>520.0</v>
       </c>
       <c r="Q49" t="n">
-        <v>37596.0</v>
+        <v>37604.0</v>
       </c>
       <c r="R49" t="n">
         <v>51.0</v>

</xml_diff>

<commit_message>
Score formula changed - slower progression for battle misses (3 >> 2.5)
</commit_message>
<xml_diff>
--- a/docs/data/memberstats.xlsx
+++ b/docs/data/memberstats.xlsx
@@ -819,7 +819,7 @@
         <v>6660.0</v>
       </c>
       <c r="H6" t="n">
-        <v>17634.0</v>
+        <v>17637.0</v>
       </c>
       <c r="I6" t="n">
         <v>1986.0</v>
@@ -852,7 +852,7 @@
         <v>145.0</v>
       </c>
       <c r="S6" t="n">
-        <v>400342.0</v>
+        <v>402211.0</v>
       </c>
       <c r="T6" t="s">
         <v>125</v>
@@ -955,10 +955,10 @@
         <v>7500.0</v>
       </c>
       <c r="H8" t="n">
-        <v>20825.0</v>
+        <v>20828.0</v>
       </c>
       <c r="I8" t="n">
-        <v>4508.0</v>
+        <v>4509.0</v>
       </c>
       <c r="J8" t="n">
         <v>2328.0</v>
@@ -988,7 +988,7 @@
         <v>203.0</v>
       </c>
       <c r="S8" t="n">
-        <v>561038.0</v>
+        <v>563375.0</v>
       </c>
       <c r="T8" t="s">
         <v>124</v>
@@ -1588,13 +1588,13 @@
         <v>123</v>
       </c>
       <c r="O17" t="n">
-        <v>256.0</v>
+        <v>266.0</v>
       </c>
       <c r="P17" t="n">
-        <v>80.0</v>
+        <v>88.0</v>
       </c>
       <c r="Q17" t="n">
-        <v>171337.0</v>
+        <v>171347.0</v>
       </c>
       <c r="R17" t="n">
         <v>307.0</v>
@@ -1638,7 +1638,7 @@
         <v>32017.0</v>
       </c>
       <c r="I18" t="n">
-        <v>5949.0</v>
+        <v>5950.0</v>
       </c>
       <c r="J18" t="n">
         <v>3076.0</v>
@@ -1656,13 +1656,13 @@
         <v>121</v>
       </c>
       <c r="O18" t="n">
-        <v>108.0</v>
+        <v>118.0</v>
       </c>
       <c r="P18" t="n">
-        <v>80.0</v>
+        <v>88.0</v>
       </c>
       <c r="Q18" t="n">
-        <v>54443.0</v>
+        <v>54453.0</v>
       </c>
       <c r="R18" t="n">
         <v>282.0</v>
@@ -2475,7 +2475,7 @@
         <v>10.0</v>
       </c>
       <c r="P30" t="n">
-        <v>40.0</v>
+        <v>80.0</v>
       </c>
       <c r="Q30" t="n">
         <v>41251.0</v>
@@ -2519,7 +2519,7 @@
         <v>1717.0</v>
       </c>
       <c r="H31" t="n">
-        <v>7507.0</v>
+        <v>7508.0</v>
       </c>
       <c r="I31" t="n">
         <v>1661.0</v>
@@ -2540,19 +2540,19 @@
         <v>121</v>
       </c>
       <c r="O31" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="P31" t="n">
         <v>0.0</v>
       </c>
       <c r="Q31" t="n">
-        <v>19310.0</v>
+        <v>19320.0</v>
       </c>
       <c r="R31" t="n">
         <v>162.0</v>
       </c>
       <c r="S31" t="n">
-        <v>493345.0</v>
+        <v>494225.0</v>
       </c>
       <c r="T31" t="s">
         <v>127</v>
@@ -2575,7 +2575,7 @@
         <v>12.0</v>
       </c>
       <c r="D32" t="n">
-        <v>5364.0</v>
+        <v>5340.0</v>
       </c>
       <c r="E32" t="n">
         <v>5778.0</v>
@@ -2584,13 +2584,13 @@
         <v>9378.0</v>
       </c>
       <c r="G32" t="n">
-        <v>11376.0</v>
+        <v>11377.0</v>
       </c>
       <c r="H32" t="n">
-        <v>24926.0</v>
+        <v>24928.0</v>
       </c>
       <c r="I32" t="n">
-        <v>4485.0</v>
+        <v>4486.0</v>
       </c>
       <c r="J32" t="n">
         <v>467.0</v>
@@ -2620,7 +2620,7 @@
         <v>139.0</v>
       </c>
       <c r="S32" t="n">
-        <v>553706.0</v>
+        <v>554641.0</v>
       </c>
       <c r="T32" t="s">
         <v>125</v>
@@ -2791,7 +2791,7 @@
         <v>2024.0</v>
       </c>
       <c r="H35" t="n">
-        <v>10634.0</v>
+        <v>10635.0</v>
       </c>
       <c r="I35" t="n">
         <v>2381.0</v>
@@ -2930,7 +2930,7 @@
         <v>10275.0</v>
       </c>
       <c r="I37" t="n">
-        <v>2894.0</v>
+        <v>2895.0</v>
       </c>
       <c r="J37" t="n">
         <v>1128.0</v>
@@ -3799,19 +3799,19 @@
         <v>13.0</v>
       </c>
       <c r="D50" t="n">
-        <v>5411.0</v>
+        <v>5368.0</v>
       </c>
       <c r="E50" t="n">
         <v>5878.0</v>
       </c>
       <c r="F50" t="n">
-        <v>9212.0</v>
+        <v>9213.0</v>
       </c>
       <c r="G50" t="n">
-        <v>9198.0</v>
+        <v>9201.0</v>
       </c>
       <c r="H50" t="n">
-        <v>27741.0</v>
+        <v>27745.0</v>
       </c>
       <c r="I50" t="n">
         <v>4387.0</v>
@@ -3832,13 +3832,13 @@
         <v>121</v>
       </c>
       <c r="O50" t="n">
-        <v>46.0</v>
+        <v>72.0</v>
       </c>
       <c r="P50" t="n">
         <v>80.0</v>
       </c>
       <c r="Q50" t="n">
-        <v>143486.0</v>
+        <v>143512.0</v>
       </c>
       <c r="R50" t="n">
         <v>202.0</v>

</xml_diff>